<commit_message>
Update Excel files from OneDrive - Thu May 22 13:45:59 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8361E43E-1CBE-43B2-B112-0982E7117FD0}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{220EF934-265D-4081-A7CB-6C68BF0F0DC0}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,9 +120,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,15 +458,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,6 +517,10 @@
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" s="2">
+        <f ca="1">TODAY()</f>
+        <v>45799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May 22 16:30:33 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{220EF934-265D-4081-A7CB-6C68BF0F0DC0}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0B24D94-D915-454F-A041-27B3AEFB0563}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Module ID</t>
   </si>
@@ -79,12 +79,21 @@
   </si>
   <si>
     <t>Actual End Date</t>
+  </si>
+  <si>
+    <t>encapsulant</t>
+  </si>
+  <si>
+    <t>DH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -123,7 +132,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,14 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -523,6 +533,29 @@
         <v>45799</v>
       </c>
     </row>
+    <row r="2" spans="1:17">
+      <c r="A2">
+        <v>123</v>
+      </c>
+      <c r="B2">
+        <v>456</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45749</v>
+      </c>
+      <c r="Q2">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May 22 16:36:38 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0B24D94-D915-454F-A041-27B3AEFB0563}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8074C94E-BFCC-4FC2-9D37-A5ECAA604179}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
     <t>encapsulant</t>
   </si>
   <si>
-    <t>DH</t>
+    <t>TC</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri May 23 04:55:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45C13EC3-7B90-47F2-B862-F54B0618B474}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="109">
   <si>
     <t>Module ID</t>
   </si>
@@ -86,10 +86,283 @@
     <t>Actual End Date</t>
   </si>
   <si>
-    <t>encapsulant</t>
+    <t>VSL202425316</t>
+  </si>
+  <si>
+    <t>M10R HYPERSOL (AMPIN)</t>
+  </si>
+  <si>
+    <t>PID</t>
+  </si>
+  <si>
+    <t>VSL202425317</t>
+  </si>
+  <si>
+    <t>VSL202425318</t>
   </si>
   <si>
     <t>TC</t>
+  </si>
+  <si>
+    <t>VSL202425319</t>
+  </si>
+  <si>
+    <t>VSL202425320</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>VSL202425321</t>
+  </si>
+  <si>
+    <t>VSL202425322</t>
+  </si>
+  <si>
+    <t>DH</t>
+  </si>
+  <si>
+    <t>VSL202425323</t>
+  </si>
+  <si>
+    <t>VSL202425324</t>
+  </si>
+  <si>
+    <t>LID</t>
+  </si>
+  <si>
+    <t>VSL202425325</t>
+  </si>
+  <si>
+    <t>VSL202425326</t>
+  </si>
+  <si>
+    <t>VSL202425280</t>
+  </si>
+  <si>
+    <t>QC Solar Blocking Diode Reliability testing</t>
+  </si>
+  <si>
+    <t>VSL202425283</t>
+  </si>
+  <si>
+    <t>UKTR Blocking Diode Reliability testing</t>
+  </si>
+  <si>
+    <t>VSL202425289</t>
+  </si>
+  <si>
+    <t>Solarspace 8.4 Wp TOPCon + HTARC</t>
+  </si>
+  <si>
+    <t>VSL202425290</t>
+  </si>
+  <si>
+    <t>VSL202425330</t>
+  </si>
+  <si>
+    <t>Valeo 0.24mm INTC ribbon trial (For TOPCon)</t>
+  </si>
+  <si>
+    <t>VSL202425331</t>
+  </si>
+  <si>
+    <t>VSL202425327</t>
+  </si>
+  <si>
+    <t>Glass rainbow/visual damage inspection test (FAB 3 module)</t>
+  </si>
+  <si>
+    <t>VSL202425328</t>
+  </si>
+  <si>
+    <t>VSL202425329</t>
+  </si>
+  <si>
+    <t>VSL202425309</t>
+  </si>
+  <si>
+    <t>VSL202425310</t>
+  </si>
+  <si>
+    <t>VSL202425342</t>
+  </si>
+  <si>
+    <t>Module from UDAY PH-II line (From IPQC)</t>
+  </si>
+  <si>
+    <t>VSL202425343</t>
+  </si>
+  <si>
+    <t>G12R TOPCon (PVEL BOM)</t>
+  </si>
+  <si>
+    <t>VSL202425344</t>
+  </si>
+  <si>
+    <t>VSL202425345</t>
+  </si>
+  <si>
+    <t>VSL202425351</t>
+  </si>
+  <si>
+    <t>Renewsys EPE+EVA evaluation</t>
+  </si>
+  <si>
+    <t>VSL202425348</t>
+  </si>
+  <si>
+    <t>Alishan EPE+EVA evaluation</t>
+  </si>
+  <si>
+    <t>VSL202425346</t>
+  </si>
+  <si>
+    <t>ESun Solar EPE+EVA evaluation</t>
+  </si>
+  <si>
+    <t>VSL202425350</t>
+  </si>
+  <si>
+    <t>VSL202425347</t>
+  </si>
+  <si>
+    <t>VSL202425352</t>
+  </si>
+  <si>
+    <t>Stringer 8, Lam 11 UDAY PH-II line (IPQC)</t>
+  </si>
+  <si>
+    <t>VSL202425354</t>
+  </si>
+  <si>
+    <t>Stringer 8, Lam 8 UDAY PH-II line (IPQC)</t>
+  </si>
+  <si>
+    <t>VSL202425355</t>
+  </si>
+  <si>
+    <t>Stringer 12, Lam 8 UDAY PH-II line (IPQC)</t>
+  </si>
+  <si>
+    <t>VSL202425356</t>
+  </si>
+  <si>
+    <t>Stringer 7, Lam 7 UDAY PH-II line (IPQC)</t>
+  </si>
+  <si>
+    <t>VSL202425357</t>
+  </si>
+  <si>
+    <t>Stringer 10, Lam 8 UDAY PH-II line (IPQC)</t>
+  </si>
+  <si>
+    <t>VSL202425358</t>
+  </si>
+  <si>
+    <t>UDAY PH-II line (IPQC)</t>
+  </si>
+  <si>
+    <t>VSL202425359</t>
+  </si>
+  <si>
+    <t>Stringer 9, Lam 6 UDAY PH-II line (IPQC)</t>
+  </si>
+  <si>
+    <t>VSL202425360</t>
+  </si>
+  <si>
+    <t>VSL202425266</t>
+  </si>
+  <si>
+    <t>G12R Extended Reliability</t>
+  </si>
+  <si>
+    <t>VSL202425268</t>
+  </si>
+  <si>
+    <t>VSL202425367</t>
+  </si>
+  <si>
+    <t>M10R HYPERSOL (ENERPARC)</t>
+  </si>
+  <si>
+    <t>VSL202425369</t>
+  </si>
+  <si>
+    <t>M10R HYPERSOL (GA INFRA)</t>
+  </si>
+  <si>
+    <t>VSL202425371</t>
+  </si>
+  <si>
+    <t>VSL202425372</t>
+  </si>
+  <si>
+    <t>VSL202425381</t>
+  </si>
+  <si>
+    <t>Tongwei M10R Hypersol cell trial</t>
+  </si>
+  <si>
+    <t>VSL202425382</t>
+  </si>
+  <si>
+    <t>VSL202425383</t>
+  </si>
+  <si>
+    <t>VSL202425384</t>
+  </si>
+  <si>
+    <t>DMEGC M10R Hypersol cell trial</t>
+  </si>
+  <si>
+    <t>VSL202425385</t>
+  </si>
+  <si>
+    <t>VSL202425386</t>
+  </si>
+  <si>
+    <t>VSL202425373</t>
+  </si>
+  <si>
+    <t>QC SOLAR BLK DIODE 2.0</t>
+  </si>
+  <si>
+    <t>VSL202425377</t>
+  </si>
+  <si>
+    <t>UKT BLK DIODE (Modified)</t>
+  </si>
+  <si>
+    <t>VSL202526006</t>
+  </si>
+  <si>
+    <t>ACME M10R HYPERSOL</t>
+  </si>
+  <si>
+    <t>Anti PID</t>
+  </si>
+  <si>
+    <t>VSL202526007</t>
+  </si>
+  <si>
+    <t>VSL202526008</t>
+  </si>
+  <si>
+    <t>LETID</t>
+  </si>
+  <si>
+    <t>VSL202425379</t>
+  </si>
+  <si>
+    <t>Fasto White Sealant trial</t>
+  </si>
+  <si>
+    <t>VSL202425380</t>
+  </si>
+  <si>
+    <t>VSL202425376</t>
   </si>
 </sst>
 </file>
@@ -97,9 +370,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="164" formatCode="dd/mmm/yy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +386,30 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -122,7 +419,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,14 +427,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,433 +789,574 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD2"/>
+  <dimension ref="A1:XFD90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" topLeftCell="AL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
+      <pane xSplit="16" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" customWidth="1"/>
-    <col min="10" max="10" width="16.36328125" customWidth="1"/>
-    <col min="11" max="11" width="17.1796875" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="16.90625" customWidth="1"/>
-    <col min="16" max="16" width="14.26953125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="47" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="75" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="76" max="106" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="107" max="136" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="137" max="167" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="168" max="228" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="229" max="320" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="321" max="350" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="351" max="381" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="382" max="412" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="413" max="440" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="441" max="471" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="472" max="501" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="502" max="532" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="533" max="593" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="594" max="685" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="686" max="715" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="716" max="746" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="747" max="777" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="778" max="805" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="806" max="836" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="837" max="866" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="867" max="897" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="898" max="958" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="959" max="1050" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="1051" max="1080" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="1081" max="1111" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="1112" max="1142" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="1143" max="1171" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="1172" max="1202" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="1203" max="1232" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="1233" max="1263" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="1264" max="1324" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="1325" max="1416" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="1417" max="1446" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="1447" max="1477" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="1478" max="1508" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="1509" max="1536" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1567" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="1568" max="1597" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="1598" max="1628" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="1629" max="1689" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="1690" max="1781" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="1782" max="1811" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="1812" max="1842" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="1843" max="1873" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="1874" max="1901" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="1902" max="1932" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="1933" max="1962" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="1963" max="1993" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="1994" max="2054" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2055" max="2146" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2147" max="2176" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2177" max="2207" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2208" max="2238" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2239" max="2266" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2267" max="2297" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2298" max="2327" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2328" max="2358" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2359" max="2419" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2420" max="2511" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2512" max="2541" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2542" max="2572" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2573" max="2603" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2604" max="2632" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2633" max="2663" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2664" max="2693" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2694" max="2724" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2725" max="2785" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2786" max="2877" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2878" max="2907" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2908" max="2938" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2939" max="2969" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2970" max="2997" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2998" max="3028" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3029" max="3058" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3059" max="3089" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3090" max="3150" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3151" max="3242" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3243" max="3272" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3273" max="3303" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3304" max="3334" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3335" max="3362" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3363" max="3393" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3394" max="3423" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3424" max="3454" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3455" max="3515" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3516" max="3607" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3608" max="3637" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3638" max="3668" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3669" max="3699" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3700" max="3727" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3728" max="3758" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3759" max="3788" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3789" max="3819" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3820" max="3880" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3881" max="3972" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3973" max="4002" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4003" max="4033" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4034" max="4064" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4065" max="4093" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4094" max="4124" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4125" max="4154" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4155" max="4185" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4186" max="4246" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4247" max="4338" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4339" max="4368" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4369" max="4399" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4400" max="4430" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4431" max="4458" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4459" max="4489" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4490" max="4519" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4520" max="4550" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4551" max="4611" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4703" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4704" max="4733" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4734" max="4764" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4765" max="4795" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4796" max="4823" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4824" max="4854" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4855" max="4884" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4885" max="4915" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4916" max="4976" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4977" max="5068" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5069" max="5098" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5099" max="5129" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5130" max="5160" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5161" max="5188" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5189" max="5219" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5220" max="5249" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5250" max="5280" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5281" max="5341" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5342" max="5433" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5434" max="5463" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5464" max="5494" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5495" max="5525" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5526" max="5554" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5555" max="5585" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5586" max="5615" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5616" max="5646" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5647" max="5707" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5708" max="5799" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5800" max="5829" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5830" max="5860" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5861" max="5891" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5919" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5920" max="5950" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="5951" max="5980" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5981" max="6011" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6012" max="6072" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6073" max="6164" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="6165" max="6194" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6195" max="6225" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6226" max="6256" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6257" max="6284" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="6285" max="6315" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6316" max="6345" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6346" max="6376" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6377" max="6437" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6438" max="6529" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="6530" max="6559" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6560" max="6590" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6591" max="6621" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6622" max="6649" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="6650" max="6680" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6710" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6711" max="6741" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6742" max="6802" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6803" max="6894" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="6895" max="6924" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6925" max="6955" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6956" max="6986" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6987" max="7015" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7016" max="7046" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7047" max="7076" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7077" max="7107" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="7108" max="7168" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7260" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7261" max="7290" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7291" max="7321" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="7322" max="7352" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7353" max="7380" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7381" max="7411" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7412" max="7441" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7442" max="7472" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="7473" max="7533" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7534" max="7625" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7626" max="7655" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7656" max="7686" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="7687" max="7717" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7718" max="7745" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7746" max="7776" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7777" max="7806" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7807" max="7837" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="7838" max="7898" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7899" max="7990" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7991" max="8020" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8021" max="8051" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="8052" max="8082" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8083" max="8110" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8111" max="8141" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8142" max="8171" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8172" max="8202" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="8203" max="8263" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8264" max="8355" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8356" max="8385" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8386" max="8416" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="8417" max="8447" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8448" max="8476" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8477" max="8507" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8508" max="8537" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8538" max="8568" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="8569" max="8629" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8630" max="8721" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8722" max="8751" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8752" max="8782" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="8783" max="8813" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8814" max="8841" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8842" max="8872" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8873" max="8902" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8903" max="8933" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="8934" max="8994" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8995" max="9086" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9087" max="9116" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9117" max="9147" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="9148" max="9178" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9179" max="9206" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9207" max="9237" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9238" max="9267" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9268" max="9298" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="9299" max="9359" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9360" max="9451" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9452" max="9481" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9482" max="9512" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="9513" max="9543" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9544" max="9571" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9572" max="9602" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9603" max="9632" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9633" max="9663" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="9664" max="9724" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9725" max="9816" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9817" max="9846" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9847" max="9877" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="9878" max="9908" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9909" max="9937" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9938" max="9968" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9969" max="9998" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9999" max="10029" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="10030" max="10090" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10091" max="10182" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="10183" max="10212" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="10213" max="10243" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10274" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10275" max="10302" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="10303" max="10333" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="10334" max="10363" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10364" max="10394" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="10395" max="10455" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10456" max="10547" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="10548" max="10577" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="10578" max="10608" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="10609" max="10639" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10640" max="10667" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="10668" max="10698" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="10699" max="10728" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10729" max="10759" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10820" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10821" max="10912" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="10913" max="10942" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="10943" max="10973" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="10974" max="11004" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11005" max="11032" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11063" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="11064" max="11093" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11094" max="11124" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="11125" max="11185" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11186" max="11277" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="11278" max="11307" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="11308" max="11338" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="11339" max="11369" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11370" max="11398" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="11399" max="11429" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="11430" max="11459" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11460" max="11490" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="11491" max="11551" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11552" max="11643" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="11644" max="11673" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="11674" max="11704" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="11705" max="11735" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11736" max="11763" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="11764" max="11794" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="11795" max="11824" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11825" max="11855" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="11856" max="11916" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="11917" max="12008" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12009" max="12038" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12039" max="12069" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="12070" max="12100" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12101" max="12128" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12129" max="12159" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12160" max="12189" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12190" max="12220" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="12221" max="12281" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12282" max="12373" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12374" max="12403" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12404" max="12434" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="12435" max="12465" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12466" max="12493" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12494" max="12524" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12525" max="12554" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12555" max="12585" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="12586" max="12646" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12647" max="12738" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12739" max="12768" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12769" max="12799" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="12800" max="12830" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12831" max="12859" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12860" max="12890" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12891" max="12920" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="12921" max="12951" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="12952" max="13012" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13013" max="13104" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="13105" max="13134" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="13135" max="13165" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13166" max="13196" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13197" max="13224" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="13225" max="13255" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="13256" max="13285" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13286" max="13316" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13377" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13378" max="13469" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="13470" max="13499" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="13500" max="13530" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13531" max="13561" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13562" max="13589" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="13590" max="13620" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="13621" max="13650" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13651" max="13681" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13682" max="13742" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13743" max="13834" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="13835" max="13864" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="13865" max="13895" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="13896" max="13926" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="13927" max="13954" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="13955" max="13985" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="13986" max="14015" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14016" max="14046" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="14047" max="14107" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14108" max="14199" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="14200" max="14229" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="14230" max="14260" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="14261" max="14291" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14292" max="14320" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="14321" max="14351" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="14352" max="14381" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14382" max="14412" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="14413" max="14473" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14474" max="14565" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="14566" max="14595" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14626" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="14627" max="14657" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14658" max="14685" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="14686" max="14716" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="14717" max="14746" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14747" max="14777" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="14778" max="14838" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14839" max="14930" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="14931" max="14960" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="14961" max="14991" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="14992" max="15022" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15023" max="15050" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15051" max="15081" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="15082" max="15111" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15142" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="15143" max="15203" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15204" max="15295" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15296" max="15325" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="15326" max="15356" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="15357" max="15387" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15388" max="15415" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15416" max="15446" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="15447" max="15476" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15477" max="15507" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="15508" max="15568" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15569" max="15660" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15661" max="15690" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="15691" max="15721" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="15722" max="15752" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15753" max="15781" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="15782" max="15812" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="15813" max="15842" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15843" max="15873" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15934" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="15935" max="16026" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="16027" max="16056" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="16057" max="16087" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="16088" max="16118" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="16119" max="16146" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="16147" max="16177" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="16178" max="16207" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="16208" max="16238" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="16239" max="16299" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="16300" max="16384" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" style="2" customWidth="1"/>
+    <col min="17" max="47" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="66" width="10" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10" customWidth="1"/>
+    <col min="68" max="75" width="10" bestFit="1" customWidth="1"/>
+    <col min="76" max="106" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="107" max="136" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="137" max="167" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="168" max="197" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="198" max="228" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="229" max="259" width="10" bestFit="1" customWidth="1"/>
+    <col min="260" max="289" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="290" max="320" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="321" max="350" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="351" max="381" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="382" max="412" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="413" max="440" width="10" bestFit="1" customWidth="1"/>
+    <col min="441" max="471" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="472" max="501" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="502" max="532" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="533" max="562" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="563" max="593" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="594" max="624" width="10" bestFit="1" customWidth="1"/>
+    <col min="625" max="654" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="655" max="685" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="686" max="715" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="716" max="746" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="747" max="777" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="778" max="805" width="10" bestFit="1" customWidth="1"/>
+    <col min="806" max="836" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="837" max="866" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="867" max="897" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="898" max="927" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="928" max="958" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="959" max="989" width="10" bestFit="1" customWidth="1"/>
+    <col min="990" max="1019" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1020" max="1050" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1051" max="1080" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1081" max="1111" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1112" max="1142" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1143" max="1171" width="10" bestFit="1" customWidth="1"/>
+    <col min="1172" max="1202" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1203" max="1232" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1233" max="1263" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1264" max="1293" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1294" max="1324" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1325" max="1355" width="10" bestFit="1" customWidth="1"/>
+    <col min="1356" max="1385" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1386" max="1416" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1417" max="1446" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1447" max="1477" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1478" max="1508" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1509" max="1536" width="10" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1567" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1568" max="1597" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1598" max="1628" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1629" max="1658" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1659" max="1689" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1690" max="1720" width="10" bestFit="1" customWidth="1"/>
+    <col min="1721" max="1750" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1751" max="1781" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1782" max="1811" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1812" max="1842" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1843" max="1873" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1874" max="1901" width="10" bestFit="1" customWidth="1"/>
+    <col min="1902" max="1932" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1933" max="1962" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1963" max="1993" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1994" max="2023" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2024" max="2054" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2085" width="10" bestFit="1" customWidth="1"/>
+    <col min="2086" max="2115" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2116" max="2146" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2147" max="2176" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2177" max="2207" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2208" max="2238" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2239" max="2266" width="10" bestFit="1" customWidth="1"/>
+    <col min="2267" max="2297" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2298" max="2327" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2358" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2359" max="2388" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2389" max="2419" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2420" max="2450" width="10" bestFit="1" customWidth="1"/>
+    <col min="2451" max="2480" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2481" max="2511" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2512" max="2541" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2542" max="2572" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2573" max="2603" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2604" max="2632" width="10" bestFit="1" customWidth="1"/>
+    <col min="2633" max="2663" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2664" max="2693" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2694" max="2724" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2725" max="2754" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2755" max="2785" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2786" max="2816" width="10" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2846" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2847" max="2877" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2878" max="2907" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2908" max="2938" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2939" max="2969" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2970" max="2997" width="10" bestFit="1" customWidth="1"/>
+    <col min="2998" max="3028" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3029" max="3058" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3059" max="3089" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3090" max="3119" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3120" max="3150" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3151" max="3181" width="10" bestFit="1" customWidth="1"/>
+    <col min="3182" max="3211" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3212" max="3242" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3243" max="3272" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3273" max="3303" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3304" max="3334" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3362" width="10" bestFit="1" customWidth="1"/>
+    <col min="3363" max="3393" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3394" max="3423" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3424" max="3454" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3455" max="3484" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3485" max="3515" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3516" max="3546" width="10" bestFit="1" customWidth="1"/>
+    <col min="3547" max="3576" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3577" max="3607" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3637" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3638" max="3668" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3669" max="3699" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3700" max="3727" width="10" bestFit="1" customWidth="1"/>
+    <col min="3728" max="3758" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3759" max="3788" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3789" max="3819" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3820" max="3849" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3850" max="3880" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3881" max="3911" width="10" bestFit="1" customWidth="1"/>
+    <col min="3912" max="3941" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3942" max="3972" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3973" max="4002" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4003" max="4033" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4034" max="4064" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4065" max="4093" width="10" bestFit="1" customWidth="1"/>
+    <col min="4094" max="4124" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4125" max="4154" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4155" max="4185" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4186" max="4215" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4216" max="4246" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4247" max="4277" width="10" bestFit="1" customWidth="1"/>
+    <col min="4278" max="4307" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4308" max="4338" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4339" max="4368" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4369" max="4399" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4400" max="4430" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4431" max="4458" width="10" bestFit="1" customWidth="1"/>
+    <col min="4459" max="4489" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4490" max="4519" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4520" max="4550" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4551" max="4580" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4581" max="4611" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4642" width="10" bestFit="1" customWidth="1"/>
+    <col min="4643" max="4672" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4673" max="4703" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4704" max="4733" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4734" max="4764" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4765" max="4795" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4796" max="4823" width="10" bestFit="1" customWidth="1"/>
+    <col min="4824" max="4854" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4855" max="4884" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4885" max="4915" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4916" max="4945" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4946" max="4976" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4977" max="5007" width="10" bestFit="1" customWidth="1"/>
+    <col min="5008" max="5037" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5038" max="5068" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5069" max="5098" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5099" max="5129" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5130" max="5160" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5161" max="5188" width="10" bestFit="1" customWidth="1"/>
+    <col min="5189" max="5219" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5220" max="5249" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5250" max="5280" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5281" max="5310" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5311" max="5341" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5342" max="5372" width="10" bestFit="1" customWidth="1"/>
+    <col min="5373" max="5402" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5403" max="5433" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5434" max="5463" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5464" max="5494" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5495" max="5525" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5526" max="5554" width="10" bestFit="1" customWidth="1"/>
+    <col min="5555" max="5585" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5586" max="5615" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5616" max="5646" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5647" max="5676" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5677" max="5707" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5708" max="5738" width="10" bestFit="1" customWidth="1"/>
+    <col min="5739" max="5768" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5769" max="5799" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5800" max="5829" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5830" max="5860" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5861" max="5891" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5892" max="5919" width="10" bestFit="1" customWidth="1"/>
+    <col min="5920" max="5950" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5951" max="5980" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5981" max="6011" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6012" max="6041" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6042" max="6072" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6073" max="6103" width="10" bestFit="1" customWidth="1"/>
+    <col min="6104" max="6133" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6134" max="6164" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6165" max="6194" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6195" max="6225" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6226" max="6256" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6257" max="6284" width="10" bestFit="1" customWidth="1"/>
+    <col min="6285" max="6315" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6316" max="6345" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6346" max="6376" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6377" max="6406" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6437" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6438" max="6468" width="10" bestFit="1" customWidth="1"/>
+    <col min="6469" max="6498" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6499" max="6529" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6530" max="6559" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6560" max="6590" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6591" max="6621" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6622" max="6649" width="10" bestFit="1" customWidth="1"/>
+    <col min="6650" max="6680" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6710" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6711" max="6741" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6742" max="6771" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6772" max="6802" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6803" max="6833" width="10" bestFit="1" customWidth="1"/>
+    <col min="6834" max="6863" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6864" max="6894" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6895" max="6924" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6925" max="6955" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6956" max="6986" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6987" max="7015" width="10" bestFit="1" customWidth="1"/>
+    <col min="7016" max="7046" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7047" max="7076" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7077" max="7107" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7108" max="7137" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7138" max="7168" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7199" width="10" bestFit="1" customWidth="1"/>
+    <col min="7200" max="7229" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7230" max="7260" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7261" max="7290" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7291" max="7321" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7322" max="7352" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7353" max="7380" width="10" bestFit="1" customWidth="1"/>
+    <col min="7381" max="7411" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7412" max="7441" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7442" max="7472" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7473" max="7502" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7503" max="7533" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7534" max="7564" width="10" bestFit="1" customWidth="1"/>
+    <col min="7565" max="7594" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7595" max="7625" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7626" max="7655" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7656" max="7686" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7717" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7718" max="7745" width="10" bestFit="1" customWidth="1"/>
+    <col min="7746" max="7776" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7777" max="7806" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7807" max="7837" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7838" max="7867" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7868" max="7898" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7899" max="7929" width="10" bestFit="1" customWidth="1"/>
+    <col min="7930" max="7959" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7990" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7991" max="8020" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8021" max="8051" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8052" max="8082" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8083" max="8110" width="10" bestFit="1" customWidth="1"/>
+    <col min="8111" max="8141" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8142" max="8171" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8172" max="8202" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8203" max="8232" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8233" max="8263" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8264" max="8294" width="10" bestFit="1" customWidth="1"/>
+    <col min="8295" max="8324" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8325" max="8355" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8356" max="8385" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8386" max="8416" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8417" max="8447" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8448" max="8476" width="10" bestFit="1" customWidth="1"/>
+    <col min="8477" max="8507" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8508" max="8537" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8538" max="8568" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8569" max="8598" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8599" max="8629" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8630" max="8660" width="10" bestFit="1" customWidth="1"/>
+    <col min="8661" max="8690" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8691" max="8721" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8722" max="8751" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8752" max="8782" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8783" max="8813" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8814" max="8841" width="10" bestFit="1" customWidth="1"/>
+    <col min="8842" max="8872" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8873" max="8902" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8903" max="8933" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8934" max="8963" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8964" max="8994" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8995" max="9025" width="10" bestFit="1" customWidth="1"/>
+    <col min="9026" max="9055" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9056" max="9086" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9087" max="9116" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9117" max="9147" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9148" max="9178" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9179" max="9206" width="10" bestFit="1" customWidth="1"/>
+    <col min="9207" max="9237" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9238" max="9267" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9268" max="9298" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9299" max="9328" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9329" max="9359" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9360" max="9390" width="10" bestFit="1" customWidth="1"/>
+    <col min="9391" max="9420" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9421" max="9451" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9452" max="9481" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9482" max="9512" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9513" max="9543" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9544" max="9571" width="10" bestFit="1" customWidth="1"/>
+    <col min="9572" max="9602" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9603" max="9632" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9633" max="9663" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9664" max="9693" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9694" max="9724" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9725" max="9755" width="10" bestFit="1" customWidth="1"/>
+    <col min="9756" max="9785" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9786" max="9816" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9817" max="9846" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9847" max="9877" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9878" max="9908" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9909" max="9937" width="10" bestFit="1" customWidth="1"/>
+    <col min="9938" max="9968" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9969" max="9998" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9999" max="10029" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10030" max="10059" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10060" max="10090" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10091" max="10121" width="10" bestFit="1" customWidth="1"/>
+    <col min="10122" max="10151" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10152" max="10182" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10183" max="10212" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10213" max="10243" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10274" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10275" max="10302" width="10" bestFit="1" customWidth="1"/>
+    <col min="10303" max="10333" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10334" max="10363" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10364" max="10394" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10395" max="10424" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10425" max="10455" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10456" max="10486" width="10" bestFit="1" customWidth="1"/>
+    <col min="10487" max="10516" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10517" max="10547" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10548" max="10577" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10578" max="10608" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10609" max="10639" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10640" max="10667" width="10" bestFit="1" customWidth="1"/>
+    <col min="10668" max="10698" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10699" max="10728" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10729" max="10759" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10789" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10790" max="10820" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10821" max="10851" width="10" bestFit="1" customWidth="1"/>
+    <col min="10852" max="10881" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10882" max="10912" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10913" max="10942" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10943" max="10973" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10974" max="11004" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11005" max="11032" width="10" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11063" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11064" max="11093" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11094" max="11124" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11125" max="11154" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11155" max="11185" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11186" max="11216" width="10" bestFit="1" customWidth="1"/>
+    <col min="11217" max="11246" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11247" max="11277" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11278" max="11307" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11308" max="11338" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11339" max="11369" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11370" max="11398" width="10" bestFit="1" customWidth="1"/>
+    <col min="11399" max="11429" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11430" max="11459" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11460" max="11490" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11491" max="11520" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11551" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11552" max="11582" width="10" bestFit="1" customWidth="1"/>
+    <col min="11583" max="11612" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11613" max="11643" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11644" max="11673" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11674" max="11704" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11705" max="11735" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11736" max="11763" width="10" bestFit="1" customWidth="1"/>
+    <col min="11764" max="11794" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11795" max="11824" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11825" max="11855" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11856" max="11885" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11886" max="11916" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11917" max="11947" width="10" bestFit="1" customWidth="1"/>
+    <col min="11948" max="11977" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11978" max="12008" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12009" max="12038" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12069" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12070" max="12100" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12101" max="12128" width="10" bestFit="1" customWidth="1"/>
+    <col min="12129" max="12159" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12160" max="12189" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12190" max="12220" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12221" max="12250" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12251" max="12281" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12282" max="12312" width="10" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12342" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12343" max="12373" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12374" max="12403" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12404" max="12434" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12435" max="12465" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12466" max="12493" width="10" bestFit="1" customWidth="1"/>
+    <col min="12494" max="12524" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12525" max="12554" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12555" max="12585" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12586" max="12615" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12616" max="12646" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12647" max="12677" width="10" bestFit="1" customWidth="1"/>
+    <col min="12678" max="12707" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12708" max="12738" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12739" max="12768" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12769" max="12799" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12800" max="12830" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12831" max="12859" width="10" bestFit="1" customWidth="1"/>
+    <col min="12860" max="12890" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12891" max="12920" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12921" max="12951" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12952" max="12981" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12982" max="13012" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13013" max="13043" width="10" bestFit="1" customWidth="1"/>
+    <col min="13044" max="13073" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13074" max="13104" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13105" max="13134" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13135" max="13165" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13166" max="13196" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13197" max="13224" width="10" bestFit="1" customWidth="1"/>
+    <col min="13225" max="13255" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13256" max="13285" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13286" max="13316" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13317" max="13346" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13347" max="13377" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13378" max="13408" width="10" bestFit="1" customWidth="1"/>
+    <col min="13409" max="13438" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13439" max="13469" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13470" max="13499" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13500" max="13530" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13531" max="13561" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13562" max="13589" width="10" bestFit="1" customWidth="1"/>
+    <col min="13590" max="13620" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13621" max="13650" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13651" max="13681" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13682" max="13711" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13712" max="13742" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13743" max="13773" width="10" bestFit="1" customWidth="1"/>
+    <col min="13774" max="13803" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13804" max="13834" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13835" max="13864" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13865" max="13895" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13896" max="13926" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13927" max="13954" width="10" bestFit="1" customWidth="1"/>
+    <col min="13955" max="13985" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13986" max="14015" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14016" max="14046" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14047" max="14076" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14077" max="14107" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14108" max="14138" width="10" bestFit="1" customWidth="1"/>
+    <col min="14139" max="14168" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14169" max="14199" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14200" max="14229" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14230" max="14260" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14261" max="14291" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14292" max="14320" width="10" bestFit="1" customWidth="1"/>
+    <col min="14321" max="14351" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14352" max="14381" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14382" max="14412" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14413" max="14442" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14443" max="14473" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14474" max="14504" width="10" bestFit="1" customWidth="1"/>
+    <col min="14505" max="14534" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14535" max="14565" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14566" max="14595" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14626" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14627" max="14657" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14658" max="14685" width="10" bestFit="1" customWidth="1"/>
+    <col min="14686" max="14716" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14717" max="14746" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14747" max="14777" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14778" max="14807" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14808" max="14838" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14839" max="14869" width="10" bestFit="1" customWidth="1"/>
+    <col min="14870" max="14899" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14900" max="14930" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14931" max="14960" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14961" max="14991" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14992" max="15022" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15023" max="15050" width="10" bestFit="1" customWidth="1"/>
+    <col min="15051" max="15081" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15082" max="15111" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15142" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15143" max="15172" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15173" max="15203" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15204" max="15234" width="10" bestFit="1" customWidth="1"/>
+    <col min="15235" max="15264" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15265" max="15295" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15296" max="15325" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15326" max="15356" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15357" max="15387" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15388" max="15415" width="10" bestFit="1" customWidth="1"/>
+    <col min="15416" max="15446" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15447" max="15476" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15477" max="15507" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15508" max="15537" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15538" max="15568" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15569" max="15599" width="10" bestFit="1" customWidth="1"/>
+    <col min="15600" max="15629" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15630" max="15660" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15661" max="15690" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15691" max="15721" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15722" max="15752" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15753" max="15781" width="10" bestFit="1" customWidth="1"/>
+    <col min="15782" max="15812" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15813" max="15842" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15843" max="15873" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15903" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15904" max="15934" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15935" max="15965" width="10" bestFit="1" customWidth="1"/>
+    <col min="15966" max="15995" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15996" max="16026" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16027" max="16056" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16057" max="16087" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16088" max="16118" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16119" max="16146" width="10" bestFit="1" customWidth="1"/>
+    <col min="16147" max="16177" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16178" max="16207" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16208" max="16238" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16239" max="16268" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16269" max="16299" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="16300" max="16330" width="10" bestFit="1" customWidth="1"/>
+    <col min="16331" max="16360" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16361" max="16384" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1071,39 +1529,39 @@
         <v>45688</v>
       </c>
       <c r="AV1" s="2">
-        <f t="shared" si="0"/>
+        <f>AU1+1</f>
         <v>45689</v>
       </c>
       <c r="AW1" s="2">
-        <f t="shared" si="0"/>
+        <f>AV1+1</f>
         <v>45690</v>
       </c>
       <c r="AX1" s="2">
-        <f t="shared" si="0"/>
+        <f>AW1+1</f>
         <v>45691</v>
       </c>
       <c r="AY1" s="2">
-        <f t="shared" si="0"/>
+        <f>AX1+1</f>
         <v>45692</v>
       </c>
       <c r="AZ1" s="2">
-        <f t="shared" si="0"/>
+        <f>AY1+1</f>
         <v>45693</v>
       </c>
       <c r="BA1" s="2">
-        <f t="shared" si="0"/>
+        <f>AZ1+1</f>
         <v>45694</v>
       </c>
       <c r="BB1" s="2">
-        <f t="shared" si="0"/>
+        <f>BA1+1</f>
         <v>45695</v>
       </c>
       <c r="BC1" s="2">
-        <f t="shared" si="0"/>
+        <f>BB1+1</f>
         <v>45696</v>
       </c>
       <c r="BD1" s="2">
-        <f t="shared" si="0"/>
+        <f>BC1+1</f>
         <v>45697</v>
       </c>
       <c r="BE1" s="2">
@@ -66419,28 +66877,1717 @@
         <v>62025</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>123</v>
-      </c>
-      <c r="B2">
-        <v>456</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:16384" ht="15">
+      <c r="A2" s="3">
+        <v>24166832</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2">
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3">
+        <v>288</v>
+      </c>
+      <c r="F2" s="7">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16384" ht="15">
+      <c r="A3" s="3">
+        <v>24166841</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3">
+        <v>288</v>
+      </c>
+      <c r="F3" s="7">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16384" ht="15">
+      <c r="A4" s="3">
+        <v>24166861</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <v>600</v>
+      </c>
+      <c r="F4" s="7">
+        <v>45692</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16384" ht="15">
+      <c r="A5" s="3">
+        <v>24166862</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3">
+        <v>600</v>
+      </c>
+      <c r="F5" s="7">
+        <v>45692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16384" ht="15">
+      <c r="A6" s="3">
+        <v>24166863</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:16384" ht="15">
+      <c r="A7" s="3">
+        <v>24166864</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:16384" ht="15">
+      <c r="A8" s="3">
+        <v>24166865</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3000</v>
+      </c>
+      <c r="F8" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16384" ht="15">
+      <c r="A9" s="3">
+        <v>24166867</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3000</v>
+      </c>
+      <c r="F9" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16384" ht="15">
+      <c r="A10" s="3">
+        <v>24166869</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3">
+        <v>60</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:16384" ht="15">
+      <c r="A11" s="3">
+        <v>24166889</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3">
+        <v>60</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:16384" ht="15">
+      <c r="A12" s="3">
+        <v>24166896</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="3">
+        <v>60</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:16384" ht="15">
+      <c r="A13" s="3">
+        <v>24306368</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="3">
+        <v>60</v>
+      </c>
+      <c r="F13" s="7">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16384" ht="15">
+      <c r="A14" s="3">
+        <v>24308189</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3">
+        <v>60</v>
+      </c>
+      <c r="F14" s="7">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16384" ht="15">
+      <c r="A15" s="3">
+        <v>24303936</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F15" s="7">
+        <v>45698</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16384" ht="15">
+      <c r="A16" s="3">
+        <v>24303937</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3">
         <v>200</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F16" s="7">
+        <v>45698</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15">
+      <c r="A17" s="3">
+        <v>24401571</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="7">
+        <v>45698</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15">
+      <c r="A18" s="3">
+        <v>24401574</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3">
+        <v>200</v>
+      </c>
+      <c r="F18" s="7">
+        <v>45720</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15">
+      <c r="A19" s="3">
+        <v>51816376</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F19" s="7">
+        <v>45704</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15">
+      <c r="A20" s="3">
+        <v>51817126</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="7">
+        <v>45704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15">
+      <c r="A21" s="3">
+        <v>51814914</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F21" s="7">
+        <v>45698</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15">
+      <c r="A22" s="3">
+        <v>24166740</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="3">
+        <v>50</v>
+      </c>
+      <c r="F22" s="7">
+        <v>45707</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15">
+      <c r="A23" s="3">
+        <v>24166738</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="3">
+        <v>50</v>
+      </c>
+      <c r="F23" s="7">
+        <v>45707</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15">
+      <c r="A24" s="3">
+        <v>24166740</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="3">
+        <v>50</v>
+      </c>
+      <c r="F24" s="7">
+        <v>45712</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15">
+      <c r="A25" s="3">
+        <v>24166738</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="3">
+        <v>50</v>
+      </c>
+      <c r="F25" s="7">
+        <v>45712</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15">
+      <c r="A26" s="3">
+        <v>24471120</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="3">
+        <v>200</v>
+      </c>
+      <c r="F26" s="7">
+        <v>45720</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15">
+      <c r="A27" s="3">
+        <v>24395952</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="3">
+        <v>60</v>
+      </c>
+      <c r="F27" s="7">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15">
+      <c r="A28" s="3">
+        <v>24395977</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="3">
+        <v>60</v>
+      </c>
+      <c r="F28" s="7">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15">
+      <c r="A29" s="3">
+        <v>24395942</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="3">
+        <v>60</v>
+      </c>
+      <c r="F29" s="7">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15">
+      <c r="A30" s="6">
+        <v>24636087</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="3">
+        <v>60</v>
+      </c>
+      <c r="F30" s="7">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15">
+      <c r="A31" s="3">
+        <v>24636090</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="3">
+        <v>60</v>
+      </c>
+      <c r="F31" s="7">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15">
+      <c r="A32" s="3">
+        <v>24636091</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="3">
+        <v>60</v>
+      </c>
+      <c r="F32" s="7">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15">
+      <c r="A33" s="3">
+        <v>24636088</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="3">
+        <v>96</v>
+      </c>
+      <c r="F33" s="7">
+        <v>45721</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15">
+      <c r="A34" s="3">
+        <v>24636089</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="3">
+        <v>96</v>
+      </c>
+      <c r="F34" s="7">
+        <v>45721</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15">
+      <c r="A35" s="3">
+        <v>24636092</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="3">
+        <v>96</v>
+      </c>
+      <c r="F35" s="7">
+        <v>45721</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15">
+      <c r="A36" s="3">
+        <v>24395952</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" ht="15">
+      <c r="A37" s="3">
+        <v>24395977</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="3">
+        <v>400</v>
+      </c>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" ht="15">
+      <c r="A38" s="3">
+        <v>24395942</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="3">
+        <v>288</v>
+      </c>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" ht="15">
+      <c r="A39" s="6">
+        <v>24567303</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="3">
+        <v>60</v>
+      </c>
+      <c r="F39" s="7">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15">
+      <c r="A40" s="6">
+        <v>24567296</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="3">
+        <v>60</v>
+      </c>
+      <c r="F40" s="7">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15">
+      <c r="A41" s="6">
+        <v>24567289</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="3">
+        <v>60</v>
+      </c>
+      <c r="F41" s="7">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15">
+      <c r="A42" s="6">
+        <v>24567319</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="3">
+        <v>60</v>
+      </c>
+      <c r="F42" s="7">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15">
+      <c r="A43" s="6">
+        <v>24567277</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="3">
+        <v>60</v>
+      </c>
+      <c r="F43" s="7">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15">
+      <c r="A44" s="6">
+        <v>24567774</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="3">
+        <v>60</v>
+      </c>
+      <c r="F44" s="7">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15">
+      <c r="A45" s="6">
+        <v>24567851</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="3">
+        <v>60</v>
+      </c>
+      <c r="F45" s="7">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15">
+      <c r="A46" s="6">
+        <v>24559501</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="3">
+        <v>60</v>
+      </c>
+      <c r="F46" s="7">
+        <v>45722</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15">
+      <c r="A47" s="6">
+        <v>24567303</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" ht="15">
+      <c r="A48" s="6">
+        <v>24567296</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F48" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15">
+      <c r="A49" s="6">
+        <v>24567289</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" ht="15">
+      <c r="A50" s="6">
+        <v>24567319</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F50" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15">
+      <c r="A51" s="6">
+        <v>24567277</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F51" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15">
+      <c r="A52" s="6">
+        <v>24567774</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F52" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15">
+      <c r="A53" s="6">
+        <v>24567851</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6" ht="15">
+      <c r="A54" s="6">
+        <v>24559501</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" ht="15">
+      <c r="A55" s="3">
+        <v>24079686</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F55" s="7">
+        <v>45733</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15">
+      <c r="A56" s="3">
+        <v>24079692</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="3">
+        <v>200</v>
+      </c>
+      <c r="F56" s="7">
+        <v>45733</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15">
+      <c r="A57" s="3">
+        <v>24636092</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="3">
+        <v>96</v>
+      </c>
+      <c r="F57" s="7">
+        <v>45733</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15">
+      <c r="A58" s="3">
+        <v>24793376</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="3">
+        <v>10</v>
+      </c>
+      <c r="F58" s="7">
         <v>45749</v>
       </c>
-      <c r="Q2">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15">
+      <c r="A59" s="3">
+        <v>24713456</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="3">
+        <v>200</v>
+      </c>
+      <c r="F59" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15">
+      <c r="A60" s="3">
+        <v>24713371</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="3">
+        <v>96</v>
+      </c>
+      <c r="F60" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15">
+      <c r="A61" s="3">
+        <v>24713222</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="3">
+        <v>200</v>
+      </c>
+      <c r="F61" s="7">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15">
+      <c r="A62" s="6">
+        <v>24636087</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F62" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15">
+      <c r="A63" s="3">
+        <v>24636090</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F63" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15">
+      <c r="A64" s="3">
+        <v>24636091</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F64" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15">
+      <c r="A65" s="3">
+        <v>24636089</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="3">
+        <v>96</v>
+      </c>
+      <c r="F65" s="7">
+        <v>45755</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15">
+      <c r="A66" s="3">
+        <v>24636088</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="3">
+        <v>96</v>
+      </c>
+      <c r="F66" s="7">
+        <v>45755</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15">
+      <c r="A67" s="3">
+        <v>25017935</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E67" s="3">
+        <v>60</v>
+      </c>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="1:6" ht="15">
+      <c r="A68" s="3">
+        <v>25017936</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E68" s="3">
+        <v>96</v>
+      </c>
+      <c r="F68" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15">
+      <c r="A69" s="3">
+        <v>25017937</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:6" ht="15">
+      <c r="A70" s="3">
+        <v>25019644</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E70" s="3">
+        <v>60</v>
+      </c>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:6" ht="15">
+      <c r="A71" s="3">
+        <v>25019645</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="3">
+        <v>96</v>
+      </c>
+      <c r="F71" s="7">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15">
+      <c r="A72" s="3">
+        <v>25019646</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:6" ht="15">
+      <c r="A73" s="3">
+        <v>24948800</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" s="3">
+        <v>500</v>
+      </c>
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="1:6" ht="15">
+      <c r="A74" s="3">
+        <v>24859051</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" s="3">
+        <v>500</v>
+      </c>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="1:6" ht="15">
+      <c r="A75" s="3">
+        <v>24948800</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" s="3">
+        <v>500</v>
+      </c>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="1:6" ht="15">
+      <c r="A76" s="3">
+        <v>24859051</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E76" s="3">
+        <v>500</v>
+      </c>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:6" ht="15">
+      <c r="A77" s="3">
+        <v>24948800</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E77" s="3">
+        <v>500</v>
+      </c>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:6" ht="15">
+      <c r="A78" s="3">
+        <v>24859051</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E78" s="3">
+        <v>500</v>
+      </c>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:6" ht="15">
+      <c r="A79" s="3">
+        <v>24948800</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E79" s="3">
+        <v>500</v>
+      </c>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:6" ht="15">
+      <c r="A80" s="3">
+        <v>24859051</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E80" s="3">
+        <v>500</v>
+      </c>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="1:6" ht="15">
+      <c r="A81" s="3">
+        <v>24948800</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E81" s="3">
+        <v>500</v>
+      </c>
+      <c r="F81" s="7"/>
+    </row>
+    <row r="82" spans="1:6" ht="15">
+      <c r="A82" s="3">
+        <v>24859051</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" s="3">
+        <v>500</v>
+      </c>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="83" spans="1:6" ht="15">
+      <c r="A83" s="3">
+        <v>24948800</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" s="3">
+        <v>500</v>
+      </c>
+      <c r="F83" s="7"/>
+    </row>
+    <row r="84" spans="1:6" ht="15">
+      <c r="A84" s="3">
+        <v>24859051</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E84" s="3">
+        <v>500</v>
+      </c>
+      <c r="F84" s="7"/>
+    </row>
+    <row r="85" spans="1:6" ht="15">
+      <c r="A85" s="3">
+        <v>24988445</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" s="3">
+        <v>96</v>
+      </c>
+      <c r="F85" s="7"/>
+    </row>
+    <row r="86" spans="1:6" ht="15">
+      <c r="A86" s="3">
+        <v>24988559</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E86" s="3">
+        <v>96</v>
+      </c>
+      <c r="F86" s="7"/>
+    </row>
+    <row r="87" spans="1:6" ht="15">
+      <c r="A87" s="3">
+        <v>24988692</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" s="3">
+        <v>162</v>
+      </c>
+      <c r="F87" s="7"/>
+    </row>
+    <row r="88" spans="1:6" ht="15">
+      <c r="A88" s="3">
+        <v>24923318</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E88" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F88" s="7"/>
+    </row>
+    <row r="89" spans="1:6" ht="15">
+      <c r="A89" s="3">
+        <v>24925212</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F89" s="7"/>
+    </row>
+    <row r="90" spans="1:6" ht="15">
+      <c r="A90" s="3">
+        <v>24857462</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90" s="3">
+        <v>50</v>
+      </c>
+      <c r="F90" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon May 26 05:37:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28922"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C5D0EF-4725-439E-AC0A-7C5CB483F8B3}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF024B2-BDAE-42F3-BD1D-9431A3C2E7B1}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -449,16 +449,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,8 +795,10 @@
   <dimension ref="A1:XFD90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" topLeftCell="XEU1048542" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AX2" sqref="AX2:XFD1048576"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FG2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FK2" sqref="FK2:FK8"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -808,557 +809,556 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
-    <col min="12" max="12" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="18" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="4.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" style="2" customWidth="1"/>
     <col min="17" max="47" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="10" bestFit="1" customWidth="1"/>
-    <col min="50" max="66" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10" style="8" customWidth="1"/>
-    <col min="68" max="75" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="76" max="106" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="107" max="136" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="137" max="167" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="168" max="197" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="198" max="228" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="229" max="259" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="260" max="289" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="290" max="320" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="321" max="350" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="351" max="381" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="382" max="412" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="413" max="440" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="441" max="471" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="472" max="501" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="502" max="532" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="533" max="562" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="563" max="593" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="594" max="624" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="625" max="654" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="655" max="685" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="686" max="715" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="716" max="746" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="747" max="777" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="778" max="805" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="806" max="836" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="837" max="866" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="867" max="897" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="898" max="927" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="928" max="958" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="959" max="989" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="990" max="1019" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1020" max="1050" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="1051" max="1080" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1081" max="1111" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1112" max="1142" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="1143" max="1171" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="1172" max="1202" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1203" max="1232" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="1233" max="1263" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1264" max="1293" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="1294" max="1324" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1325" max="1355" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="1356" max="1385" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1386" max="1416" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="1417" max="1446" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1447" max="1477" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1478" max="1508" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="1509" max="1536" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1567" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1568" max="1597" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="1598" max="1628" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1629" max="1658" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="1659" max="1689" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1690" max="1720" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="1721" max="1750" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1751" max="1781" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="1782" max="1811" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1812" max="1842" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1843" max="1873" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="1874" max="1901" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="1902" max="1932" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1933" max="1962" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="1963" max="1993" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="1994" max="2023" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2024" max="2054" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2055" max="2085" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="2086" max="2115" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2116" max="2146" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2147" max="2176" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2177" max="2207" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2208" max="2238" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2239" max="2266" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="2267" max="2297" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2298" max="2327" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2328" max="2358" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2359" max="2388" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2389" max="2419" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2420" max="2450" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="2451" max="2480" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2481" max="2511" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2512" max="2541" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2542" max="2572" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2573" max="2603" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2604" max="2632" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="2633" max="2663" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2664" max="2693" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2694" max="2724" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2725" max="2754" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2755" max="2785" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2786" max="2816" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2846" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2847" max="2877" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2878" max="2907" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2908" max="2938" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2939" max="2969" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2970" max="2997" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="2998" max="3028" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3029" max="3058" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3059" max="3089" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3090" max="3119" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3120" max="3150" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3151" max="3181" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="3182" max="3211" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3212" max="3242" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3243" max="3272" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3273" max="3303" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3304" max="3334" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3335" max="3362" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="3363" max="3393" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3394" max="3423" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3424" max="3454" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3455" max="3484" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3485" max="3515" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3516" max="3546" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="3547" max="3576" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3577" max="3607" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3608" max="3637" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3638" max="3668" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3669" max="3699" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3700" max="3727" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="3728" max="3758" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3759" max="3788" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3789" max="3819" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3820" max="3849" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3850" max="3880" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3881" max="3911" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="3912" max="3941" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3942" max="3972" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3973" max="4002" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4003" max="4033" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4034" max="4064" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4065" max="4093" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="4094" max="4124" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4125" max="4154" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4155" max="4185" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4186" max="4215" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4216" max="4246" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4247" max="4277" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="4278" max="4307" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4308" max="4338" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4339" max="4368" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4369" max="4399" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4400" max="4430" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4431" max="4458" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="4459" max="4489" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4490" max="4519" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4520" max="4550" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4551" max="4580" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4581" max="4611" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4642" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="4643" max="4672" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4673" max="4703" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4704" max="4733" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4734" max="4764" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4765" max="4795" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4796" max="4823" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="4824" max="4854" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4855" max="4884" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4885" max="4915" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4916" max="4945" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4946" max="4976" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4977" max="5007" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5008" max="5037" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5038" max="5068" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5069" max="5098" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5099" max="5129" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5130" max="5160" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5161" max="5188" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5189" max="5219" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5220" max="5249" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5250" max="5280" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5281" max="5310" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5311" max="5341" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5342" max="5372" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5373" max="5402" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5403" max="5433" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5434" max="5463" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5464" max="5494" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5495" max="5525" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5526" max="5554" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5555" max="5585" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5586" max="5615" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5616" max="5646" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5647" max="5676" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5677" max="5707" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5708" max="5738" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5739" max="5768" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5769" max="5799" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5800" max="5829" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5830" max="5860" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5861" max="5891" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5919" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5920" max="5950" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5951" max="5980" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5981" max="6011" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6012" max="6041" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6042" max="6072" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6073" max="6103" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="6104" max="6133" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6134" max="6164" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6165" max="6194" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6195" max="6225" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6226" max="6256" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6257" max="6284" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="6285" max="6315" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6316" max="6345" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6346" max="6376" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6377" max="6406" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6407" max="6437" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6438" max="6468" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="6469" max="6498" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6499" max="6529" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6530" max="6559" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6560" max="6590" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6591" max="6621" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6622" max="6649" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="6650" max="6680" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6710" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6711" max="6741" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6742" max="6771" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6772" max="6802" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6803" max="6833" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="6834" max="6863" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6864" max="6894" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6895" max="6924" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6925" max="6955" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6956" max="6986" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6987" max="7015" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="7016" max="7046" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7047" max="7076" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7077" max="7107" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7108" max="7137" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7138" max="7168" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7199" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="7200" max="7229" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7230" max="7260" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7261" max="7290" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7291" max="7321" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7322" max="7352" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7353" max="7380" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="7381" max="7411" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7412" max="7441" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7442" max="7472" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7473" max="7502" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7503" max="7533" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7534" max="7564" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="7565" max="7594" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7595" max="7625" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7626" max="7655" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7656" max="7686" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7687" max="7717" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7718" max="7745" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="7746" max="7776" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7777" max="7806" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7807" max="7837" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7838" max="7867" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7868" max="7898" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7899" max="7929" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="7930" max="7959" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7960" max="7990" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7991" max="8020" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8021" max="8051" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8052" max="8082" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8083" max="8110" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="8111" max="8141" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8142" max="8171" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8172" max="8202" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8203" max="8232" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8233" max="8263" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8264" max="8294" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="8295" max="8324" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8325" max="8355" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8356" max="8385" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8386" max="8416" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8417" max="8447" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8448" max="8476" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="8477" max="8507" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8508" max="8537" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8538" max="8568" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8569" max="8598" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8599" max="8629" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8630" max="8660" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="8661" max="8690" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8691" max="8721" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8722" max="8751" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8752" max="8782" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8783" max="8813" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8814" max="8841" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="8842" max="8872" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8873" max="8902" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8903" max="8933" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8934" max="8963" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8994" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8995" max="9025" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="9026" max="9055" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9056" max="9086" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9087" max="9116" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9117" max="9147" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9148" max="9178" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9179" max="9206" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="9207" max="9237" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9238" max="9267" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9268" max="9298" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9299" max="9328" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9329" max="9359" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9360" max="9390" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="9391" max="9420" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9421" max="9451" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9452" max="9481" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9482" max="9512" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9513" max="9543" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9544" max="9571" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="9572" max="9602" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9603" max="9632" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9633" max="9663" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9664" max="9693" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9694" max="9724" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9725" max="9755" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="9756" max="9785" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9786" max="9816" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9817" max="9846" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9847" max="9877" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9878" max="9908" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9909" max="9937" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="9938" max="9968" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9969" max="9998" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="9999" max="10029" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10030" max="10059" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10060" max="10090" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10091" max="10121" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="10122" max="10151" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10152" max="10182" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10183" max="10212" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10213" max="10243" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10274" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10275" max="10302" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="10303" max="10333" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10334" max="10363" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10364" max="10394" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10395" max="10424" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10425" max="10455" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10456" max="10486" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="10487" max="10516" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10517" max="10547" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10548" max="10577" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10578" max="10608" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10609" max="10639" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10640" max="10667" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="10668" max="10698" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10699" max="10728" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10729" max="10759" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10789" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10790" max="10820" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10821" max="10851" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="10852" max="10881" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10882" max="10912" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10913" max="10942" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10943" max="10973" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10974" max="11004" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11005" max="11032" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11063" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11064" max="11093" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11094" max="11124" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11125" max="11154" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11155" max="11185" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11186" max="11216" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="11217" max="11246" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11247" max="11277" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11278" max="11307" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11308" max="11338" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11339" max="11369" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11370" max="11398" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="11399" max="11429" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11430" max="11459" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11460" max="11490" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11491" max="11520" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11551" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11552" max="11582" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="11583" max="11612" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11613" max="11643" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11644" max="11673" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11674" max="11704" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11705" max="11735" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11736" max="11763" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="11764" max="11794" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11795" max="11824" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11825" max="11855" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11856" max="11885" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11886" max="11916" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11917" max="11947" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="11948" max="11977" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11978" max="12008" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12009" max="12038" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12039" max="12069" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12070" max="12100" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12101" max="12128" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="12129" max="12159" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12160" max="12189" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12190" max="12220" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12221" max="12250" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12251" max="12281" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12282" max="12312" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="12313" max="12342" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12343" max="12373" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12374" max="12403" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12404" max="12434" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12435" max="12465" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12466" max="12493" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="12494" max="12524" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12525" max="12554" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12555" max="12585" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12586" max="12615" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12616" max="12646" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12647" max="12677" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="12678" max="12707" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12708" max="12738" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12739" max="12768" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12769" max="12799" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12800" max="12830" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12831" max="12859" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="12860" max="12890" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12891" max="12920" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12921" max="12951" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12952" max="12981" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12982" max="13012" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13013" max="13043" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="13044" max="13073" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13074" max="13104" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13105" max="13134" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13135" max="13165" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13166" max="13196" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13197" max="13224" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="13225" max="13255" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13256" max="13285" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13286" max="13316" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13317" max="13346" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13347" max="13377" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13378" max="13408" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="13409" max="13438" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13439" max="13469" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13470" max="13499" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13500" max="13530" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13531" max="13561" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13562" max="13589" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="13590" max="13620" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13621" max="13650" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13651" max="13681" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13682" max="13711" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="13712" max="13742" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13743" max="13773" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="13774" max="13803" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13804" max="13834" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13835" max="13864" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13865" max="13895" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13896" max="13926" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13927" max="13954" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="13955" max="13985" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13986" max="14015" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14016" max="14046" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14047" max="14076" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14077" max="14107" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14108" max="14138" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="14139" max="14168" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14169" max="14199" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="14200" max="14229" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14230" max="14260" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14261" max="14291" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14292" max="14320" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="14321" max="14351" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14352" max="14381" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14382" max="14412" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14413" max="14442" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14443" max="14473" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14474" max="14504" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="14505" max="14534" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14535" max="14565" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="14566" max="14595" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14626" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14627" max="14657" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14658" max="14685" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="14686" max="14716" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14717" max="14746" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14747" max="14777" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14778" max="14807" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="14808" max="14838" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14839" max="14869" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="14870" max="14899" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14900" max="14930" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="14931" max="14960" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14961" max="14991" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14992" max="15022" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15023" max="15050" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="15051" max="15081" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15082" max="15111" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15142" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15143" max="15172" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15173" max="15203" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15204" max="15234" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="15235" max="15264" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15265" max="15295" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="15296" max="15325" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15326" max="15356" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15357" max="15387" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15388" max="15415" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="15416" max="15446" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15447" max="15476" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15477" max="15507" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15508" max="15537" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15538" max="15568" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15569" max="15599" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="15600" max="15629" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15630" max="15660" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="15661" max="15690" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15691" max="15721" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15722" max="15752" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15753" max="15781" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="15782" max="15812" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15813" max="15842" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15843" max="15873" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15903" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15904" max="15934" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15935" max="15965" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="15966" max="15995" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15996" max="16026" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="16027" max="16056" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16057" max="16087" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16088" max="16118" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16119" max="16146" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="16147" max="16177" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16178" max="16207" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="16208" max="16238" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16239" max="16268" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="16269" max="16299" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16300" max="16330" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="16331" max="16360" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16361" max="16384" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="48" max="66" width="10" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10" customWidth="1"/>
+    <col min="68" max="75" width="10" bestFit="1" customWidth="1"/>
+    <col min="76" max="106" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="107" max="136" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="137" max="167" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="168" max="197" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="198" max="228" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="229" max="259" width="10" bestFit="1" customWidth="1"/>
+    <col min="260" max="289" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="290" max="320" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="321" max="350" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="351" max="381" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="382" max="412" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="413" max="440" width="10" bestFit="1" customWidth="1"/>
+    <col min="441" max="471" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="472" max="501" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="502" max="532" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="533" max="562" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="563" max="593" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="594" max="624" width="10" bestFit="1" customWidth="1"/>
+    <col min="625" max="654" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="655" max="685" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="686" max="715" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="716" max="746" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="747" max="777" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="778" max="805" width="10" bestFit="1" customWidth="1"/>
+    <col min="806" max="836" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="837" max="866" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="867" max="897" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="898" max="927" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="928" max="958" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="959" max="989" width="10" bestFit="1" customWidth="1"/>
+    <col min="990" max="1019" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1020" max="1050" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1051" max="1080" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1081" max="1111" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1112" max="1142" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1143" max="1171" width="10" bestFit="1" customWidth="1"/>
+    <col min="1172" max="1202" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1203" max="1232" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1233" max="1263" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1264" max="1293" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1294" max="1324" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1325" max="1355" width="10" bestFit="1" customWidth="1"/>
+    <col min="1356" max="1385" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1386" max="1416" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1417" max="1446" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1447" max="1477" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1478" max="1508" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1509" max="1536" width="10" bestFit="1" customWidth="1"/>
+    <col min="1537" max="1567" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1568" max="1597" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1598" max="1628" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1629" max="1658" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1659" max="1689" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1690" max="1720" width="10" bestFit="1" customWidth="1"/>
+    <col min="1721" max="1750" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1751" max="1781" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1782" max="1811" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1812" max="1842" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1843" max="1873" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1874" max="1901" width="10" bestFit="1" customWidth="1"/>
+    <col min="1902" max="1932" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1933" max="1962" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1963" max="1993" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1994" max="2023" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2024" max="2054" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2085" width="10" bestFit="1" customWidth="1"/>
+    <col min="2086" max="2115" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2116" max="2146" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2147" max="2176" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2177" max="2207" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2208" max="2238" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2239" max="2266" width="10" bestFit="1" customWidth="1"/>
+    <col min="2267" max="2297" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2298" max="2327" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2328" max="2358" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2359" max="2388" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2389" max="2419" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2420" max="2450" width="10" bestFit="1" customWidth="1"/>
+    <col min="2451" max="2480" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2481" max="2511" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2512" max="2541" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2542" max="2572" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2573" max="2603" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2604" max="2632" width="10" bestFit="1" customWidth="1"/>
+    <col min="2633" max="2663" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2664" max="2693" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2694" max="2724" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2725" max="2754" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2755" max="2785" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2786" max="2816" width="10" bestFit="1" customWidth="1"/>
+    <col min="2817" max="2846" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2847" max="2877" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2878" max="2907" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2908" max="2938" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2939" max="2969" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2970" max="2997" width="10" bestFit="1" customWidth="1"/>
+    <col min="2998" max="3028" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3029" max="3058" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3059" max="3089" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3090" max="3119" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3120" max="3150" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3151" max="3181" width="10" bestFit="1" customWidth="1"/>
+    <col min="3182" max="3211" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3212" max="3242" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3243" max="3272" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3273" max="3303" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3304" max="3334" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3362" width="10" bestFit="1" customWidth="1"/>
+    <col min="3363" max="3393" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3394" max="3423" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3424" max="3454" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3455" max="3484" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3485" max="3515" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3516" max="3546" width="10" bestFit="1" customWidth="1"/>
+    <col min="3547" max="3576" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3577" max="3607" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3608" max="3637" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3638" max="3668" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3669" max="3699" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3700" max="3727" width="10" bestFit="1" customWidth="1"/>
+    <col min="3728" max="3758" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3759" max="3788" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3789" max="3819" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3820" max="3849" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3850" max="3880" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3881" max="3911" width="10" bestFit="1" customWidth="1"/>
+    <col min="3912" max="3941" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3942" max="3972" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3973" max="4002" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4003" max="4033" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4034" max="4064" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4065" max="4093" width="10" bestFit="1" customWidth="1"/>
+    <col min="4094" max="4124" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4125" max="4154" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4155" max="4185" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4186" max="4215" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4216" max="4246" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4247" max="4277" width="10" bestFit="1" customWidth="1"/>
+    <col min="4278" max="4307" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4308" max="4338" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4339" max="4368" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4369" max="4399" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4400" max="4430" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4431" max="4458" width="10" bestFit="1" customWidth="1"/>
+    <col min="4459" max="4489" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4490" max="4519" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4520" max="4550" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4551" max="4580" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4581" max="4611" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4642" width="10" bestFit="1" customWidth="1"/>
+    <col min="4643" max="4672" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4673" max="4703" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4704" max="4733" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4734" max="4764" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4765" max="4795" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4796" max="4823" width="10" bestFit="1" customWidth="1"/>
+    <col min="4824" max="4854" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4855" max="4884" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4885" max="4915" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4916" max="4945" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4946" max="4976" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4977" max="5007" width="10" bestFit="1" customWidth="1"/>
+    <col min="5008" max="5037" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5038" max="5068" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5069" max="5098" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5099" max="5129" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5130" max="5160" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5161" max="5188" width="10" bestFit="1" customWidth="1"/>
+    <col min="5189" max="5219" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5220" max="5249" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5250" max="5280" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5281" max="5310" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5311" max="5341" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5342" max="5372" width="10" bestFit="1" customWidth="1"/>
+    <col min="5373" max="5402" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5403" max="5433" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5434" max="5463" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5464" max="5494" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5495" max="5525" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5526" max="5554" width="10" bestFit="1" customWidth="1"/>
+    <col min="5555" max="5585" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5586" max="5615" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5616" max="5646" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5647" max="5676" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5677" max="5707" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5708" max="5738" width="10" bestFit="1" customWidth="1"/>
+    <col min="5739" max="5768" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5769" max="5799" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5800" max="5829" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5830" max="5860" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5861" max="5891" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5892" max="5919" width="10" bestFit="1" customWidth="1"/>
+    <col min="5920" max="5950" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5951" max="5980" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5981" max="6011" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6012" max="6041" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6042" max="6072" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6073" max="6103" width="10" bestFit="1" customWidth="1"/>
+    <col min="6104" max="6133" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6134" max="6164" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6165" max="6194" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6195" max="6225" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6226" max="6256" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6257" max="6284" width="10" bestFit="1" customWidth="1"/>
+    <col min="6285" max="6315" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6316" max="6345" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6346" max="6376" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6377" max="6406" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6437" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6438" max="6468" width="10" bestFit="1" customWidth="1"/>
+    <col min="6469" max="6498" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6499" max="6529" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6530" max="6559" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6560" max="6590" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6591" max="6621" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6622" max="6649" width="10" bestFit="1" customWidth="1"/>
+    <col min="6650" max="6680" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6710" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6711" max="6741" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6742" max="6771" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6772" max="6802" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6803" max="6833" width="10" bestFit="1" customWidth="1"/>
+    <col min="6834" max="6863" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6864" max="6894" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6895" max="6924" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6925" max="6955" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6956" max="6986" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6987" max="7015" width="10" bestFit="1" customWidth="1"/>
+    <col min="7016" max="7046" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7047" max="7076" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7077" max="7107" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7108" max="7137" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7138" max="7168" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7169" max="7199" width="10" bestFit="1" customWidth="1"/>
+    <col min="7200" max="7229" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7230" max="7260" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7261" max="7290" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7291" max="7321" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7322" max="7352" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7353" max="7380" width="10" bestFit="1" customWidth="1"/>
+    <col min="7381" max="7411" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7412" max="7441" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7442" max="7472" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7473" max="7502" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7503" max="7533" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7534" max="7564" width="10" bestFit="1" customWidth="1"/>
+    <col min="7565" max="7594" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7595" max="7625" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7626" max="7655" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7656" max="7686" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7717" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7718" max="7745" width="10" bestFit="1" customWidth="1"/>
+    <col min="7746" max="7776" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7777" max="7806" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7807" max="7837" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7838" max="7867" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7868" max="7898" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7899" max="7929" width="10" bestFit="1" customWidth="1"/>
+    <col min="7930" max="7959" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7960" max="7990" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7991" max="8020" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8021" max="8051" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8052" max="8082" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8083" max="8110" width="10" bestFit="1" customWidth="1"/>
+    <col min="8111" max="8141" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8142" max="8171" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8172" max="8202" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8203" max="8232" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8233" max="8263" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8264" max="8294" width="10" bestFit="1" customWidth="1"/>
+    <col min="8295" max="8324" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8325" max="8355" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8356" max="8385" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8386" max="8416" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8417" max="8447" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8448" max="8476" width="10" bestFit="1" customWidth="1"/>
+    <col min="8477" max="8507" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8508" max="8537" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8538" max="8568" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8569" max="8598" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8599" max="8629" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8630" max="8660" width="10" bestFit="1" customWidth="1"/>
+    <col min="8661" max="8690" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8691" max="8721" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8722" max="8751" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8752" max="8782" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8783" max="8813" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8814" max="8841" width="10" bestFit="1" customWidth="1"/>
+    <col min="8842" max="8872" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8873" max="8902" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8903" max="8933" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8934" max="8963" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8964" max="8994" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8995" max="9025" width="10" bestFit="1" customWidth="1"/>
+    <col min="9026" max="9055" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9056" max="9086" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9087" max="9116" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9117" max="9147" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9148" max="9178" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9179" max="9206" width="10" bestFit="1" customWidth="1"/>
+    <col min="9207" max="9237" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9238" max="9267" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9268" max="9298" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9299" max="9328" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9329" max="9359" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9360" max="9390" width="10" bestFit="1" customWidth="1"/>
+    <col min="9391" max="9420" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9421" max="9451" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9452" max="9481" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9482" max="9512" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9513" max="9543" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9544" max="9571" width="10" bestFit="1" customWidth="1"/>
+    <col min="9572" max="9602" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9603" max="9632" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9633" max="9663" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9664" max="9693" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9694" max="9724" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9725" max="9755" width="10" bestFit="1" customWidth="1"/>
+    <col min="9756" max="9785" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9786" max="9816" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9817" max="9846" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9847" max="9877" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9878" max="9908" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9909" max="9937" width="10" bestFit="1" customWidth="1"/>
+    <col min="9938" max="9968" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9969" max="9998" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9999" max="10029" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10030" max="10059" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10060" max="10090" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10091" max="10121" width="10" bestFit="1" customWidth="1"/>
+    <col min="10122" max="10151" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10152" max="10182" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10183" max="10212" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10213" max="10243" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10274" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10275" max="10302" width="10" bestFit="1" customWidth="1"/>
+    <col min="10303" max="10333" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10334" max="10363" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10364" max="10394" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10395" max="10424" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10425" max="10455" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10456" max="10486" width="10" bestFit="1" customWidth="1"/>
+    <col min="10487" max="10516" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10517" max="10547" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10548" max="10577" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10578" max="10608" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10609" max="10639" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10640" max="10667" width="10" bestFit="1" customWidth="1"/>
+    <col min="10668" max="10698" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10699" max="10728" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10729" max="10759" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10789" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10790" max="10820" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10821" max="10851" width="10" bestFit="1" customWidth="1"/>
+    <col min="10852" max="10881" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10882" max="10912" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10913" max="10942" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10943" max="10973" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10974" max="11004" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11005" max="11032" width="10" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11063" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11064" max="11093" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11094" max="11124" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11125" max="11154" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11155" max="11185" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11186" max="11216" width="10" bestFit="1" customWidth="1"/>
+    <col min="11217" max="11246" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11247" max="11277" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11278" max="11307" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11308" max="11338" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11339" max="11369" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11370" max="11398" width="10" bestFit="1" customWidth="1"/>
+    <col min="11399" max="11429" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11430" max="11459" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11460" max="11490" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11491" max="11520" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11521" max="11551" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11552" max="11582" width="10" bestFit="1" customWidth="1"/>
+    <col min="11583" max="11612" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11613" max="11643" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11644" max="11673" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11674" max="11704" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11705" max="11735" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11736" max="11763" width="10" bestFit="1" customWidth="1"/>
+    <col min="11764" max="11794" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11795" max="11824" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11825" max="11855" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11856" max="11885" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11886" max="11916" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11917" max="11947" width="10" bestFit="1" customWidth="1"/>
+    <col min="11948" max="11977" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11978" max="12008" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12009" max="12038" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12069" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12070" max="12100" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12101" max="12128" width="10" bestFit="1" customWidth="1"/>
+    <col min="12129" max="12159" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12160" max="12189" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12190" max="12220" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12221" max="12250" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12251" max="12281" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12282" max="12312" width="10" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12342" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12343" max="12373" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12374" max="12403" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12404" max="12434" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12435" max="12465" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12466" max="12493" width="10" bestFit="1" customWidth="1"/>
+    <col min="12494" max="12524" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12525" max="12554" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12555" max="12585" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12586" max="12615" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12616" max="12646" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12647" max="12677" width="10" bestFit="1" customWidth="1"/>
+    <col min="12678" max="12707" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12708" max="12738" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12739" max="12768" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12769" max="12799" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12800" max="12830" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12831" max="12859" width="10" bestFit="1" customWidth="1"/>
+    <col min="12860" max="12890" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12891" max="12920" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12921" max="12951" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12952" max="12981" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12982" max="13012" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13013" max="13043" width="10" bestFit="1" customWidth="1"/>
+    <col min="13044" max="13073" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13074" max="13104" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13105" max="13134" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13135" max="13165" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13166" max="13196" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13197" max="13224" width="10" bestFit="1" customWidth="1"/>
+    <col min="13225" max="13255" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13256" max="13285" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13286" max="13316" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13317" max="13346" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13347" max="13377" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13378" max="13408" width="10" bestFit="1" customWidth="1"/>
+    <col min="13409" max="13438" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13439" max="13469" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13470" max="13499" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13500" max="13530" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13531" max="13561" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13562" max="13589" width="10" bestFit="1" customWidth="1"/>
+    <col min="13590" max="13620" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13621" max="13650" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13651" max="13681" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13682" max="13711" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13712" max="13742" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13743" max="13773" width="10" bestFit="1" customWidth="1"/>
+    <col min="13774" max="13803" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13804" max="13834" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13835" max="13864" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13865" max="13895" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13896" max="13926" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13927" max="13954" width="10" bestFit="1" customWidth="1"/>
+    <col min="13955" max="13985" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13986" max="14015" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14016" max="14046" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14047" max="14076" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14077" max="14107" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14108" max="14138" width="10" bestFit="1" customWidth="1"/>
+    <col min="14139" max="14168" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14169" max="14199" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14200" max="14229" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14230" max="14260" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14261" max="14291" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14292" max="14320" width="10" bestFit="1" customWidth="1"/>
+    <col min="14321" max="14351" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14352" max="14381" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14382" max="14412" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14413" max="14442" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14443" max="14473" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14474" max="14504" width="10" bestFit="1" customWidth="1"/>
+    <col min="14505" max="14534" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14535" max="14565" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14566" max="14595" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14626" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14627" max="14657" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14658" max="14685" width="10" bestFit="1" customWidth="1"/>
+    <col min="14686" max="14716" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14717" max="14746" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14747" max="14777" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14778" max="14807" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14808" max="14838" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="14839" max="14869" width="10" bestFit="1" customWidth="1"/>
+    <col min="14870" max="14899" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14900" max="14930" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14931" max="14960" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14961" max="14991" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14992" max="15022" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15023" max="15050" width="10" bestFit="1" customWidth="1"/>
+    <col min="15051" max="15081" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15082" max="15111" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15142" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15143" max="15172" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15173" max="15203" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15204" max="15234" width="10" bestFit="1" customWidth="1"/>
+    <col min="15235" max="15264" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15265" max="15295" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15296" max="15325" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15326" max="15356" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15357" max="15387" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15388" max="15415" width="10" bestFit="1" customWidth="1"/>
+    <col min="15416" max="15446" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15447" max="15476" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15477" max="15507" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15508" max="15537" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15538" max="15568" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15569" max="15599" width="10" bestFit="1" customWidth="1"/>
+    <col min="15600" max="15629" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15630" max="15660" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15661" max="15690" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15691" max="15721" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15722" max="15752" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15753" max="15781" width="10" bestFit="1" customWidth="1"/>
+    <col min="15782" max="15812" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15813" max="15842" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15843" max="15873" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15903" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15904" max="15934" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15935" max="15965" width="10" bestFit="1" customWidth="1"/>
+    <col min="15966" max="15995" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15996" max="16026" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16027" max="16056" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16057" max="16087" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16088" max="16118" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16119" max="16146" width="10" bestFit="1" customWidth="1"/>
+    <col min="16147" max="16177" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16178" max="16207" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16208" max="16238" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16239" max="16268" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16269" max="16299" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="16300" max="16330" width="10" bestFit="1" customWidth="1"/>
+    <col min="16331" max="16360" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16361" max="16384" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" customFormat="1">
@@ -66882,7 +66882,7 @@
         <v>62025</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="2" spans="1:16384" customFormat="1" ht="15">
       <c r="A2" s="3">
         <v>24166832</v>
       </c>
@@ -66901,49 +66901,7 @@
       <c r="F2" s="7">
         <v>45693</v>
       </c>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
       <c r="P2" s="2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
-      <c r="AB2"/>
-      <c r="AC2"/>
-      <c r="AD2"/>
-      <c r="AE2"/>
-      <c r="AF2"/>
-      <c r="AG2"/>
-      <c r="AH2"/>
-      <c r="AI2"/>
-      <c r="AJ2"/>
-      <c r="AK2"/>
-      <c r="AL2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
-      <c r="AP2"/>
-      <c r="AQ2"/>
-      <c r="AR2"/>
-      <c r="AS2"/>
-      <c r="AT2"/>
-      <c r="AU2"/>
-      <c r="AV2"/>
-      <c r="AW2"/>
       <c r="AY2" s="3"/>
       <c r="AZ2" s="3">
         <v>12</v>
@@ -67087,7 +67045,7 @@
       <c r="FI2" s="3"/>
       <c r="FJ2" s="3"/>
     </row>
-    <row r="3" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="3" spans="1:16384" customFormat="1" ht="15">
       <c r="A3" s="3">
         <v>24166841</v>
       </c>
@@ -67106,49 +67064,7 @@
       <c r="F3" s="7">
         <v>45693</v>
       </c>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
       <c r="P3" s="2"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3"/>
-      <c r="AD3"/>
-      <c r="AE3"/>
-      <c r="AF3"/>
-      <c r="AG3"/>
-      <c r="AH3"/>
-      <c r="AI3"/>
-      <c r="AJ3"/>
-      <c r="AK3"/>
-      <c r="AL3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3"/>
-      <c r="AS3"/>
-      <c r="AT3"/>
-      <c r="AU3"/>
-      <c r="AV3"/>
-      <c r="AW3"/>
       <c r="AY3" s="3"/>
       <c r="AZ3" s="3">
         <v>12</v>
@@ -67292,7 +67208,7 @@
       <c r="FI3" s="3"/>
       <c r="FJ3" s="3"/>
     </row>
-    <row r="4" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="4" spans="1:16384" customFormat="1" ht="15">
       <c r="A4" s="3">
         <v>24166861</v>
       </c>
@@ -67311,49 +67227,7 @@
       <c r="F4" s="7">
         <v>45692</v>
       </c>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
       <c r="P4" s="2"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-      <c r="AC4"/>
-      <c r="AD4"/>
-      <c r="AE4"/>
-      <c r="AF4"/>
-      <c r="AG4"/>
-      <c r="AH4"/>
-      <c r="AI4"/>
-      <c r="AJ4"/>
-      <c r="AK4"/>
-      <c r="AL4"/>
-      <c r="AM4"/>
-      <c r="AN4"/>
-      <c r="AO4"/>
-      <c r="AP4"/>
-      <c r="AQ4"/>
-      <c r="AR4"/>
-      <c r="AS4"/>
-      <c r="AT4"/>
-      <c r="AU4"/>
-      <c r="AV4"/>
-      <c r="AW4"/>
       <c r="AY4" s="3">
         <v>18</v>
       </c>
@@ -67579,7 +67453,7 @@
       <c r="FI4" s="3"/>
       <c r="FJ4" s="3"/>
     </row>
-    <row r="5" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="5" spans="1:16384" customFormat="1" ht="15">
       <c r="A5" s="3">
         <v>24166862</v>
       </c>
@@ -67598,49 +67472,7 @@
       <c r="F5" s="7">
         <v>45692</v>
       </c>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
       <c r="P5" s="2"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-      <c r="AE5"/>
-      <c r="AF5"/>
-      <c r="AG5"/>
-      <c r="AH5"/>
-      <c r="AI5"/>
-      <c r="AJ5"/>
-      <c r="AK5"/>
-      <c r="AL5"/>
-      <c r="AM5"/>
-      <c r="AN5"/>
-      <c r="AO5"/>
-      <c r="AP5"/>
-      <c r="AQ5"/>
-      <c r="AR5"/>
-      <c r="AS5"/>
-      <c r="AT5"/>
-      <c r="AU5"/>
-      <c r="AV5"/>
-      <c r="AW5"/>
       <c r="AY5" s="3">
         <v>18</v>
       </c>
@@ -67866,7 +67698,7 @@
       <c r="FI5" s="3"/>
       <c r="FJ5" s="3"/>
     </row>
-    <row r="6" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="6" spans="1:16384" customFormat="1" ht="15">
       <c r="A6" s="3">
         <v>24166863</v>
       </c>
@@ -67883,49 +67715,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="7"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
       <c r="P6" s="2"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-      <c r="AF6"/>
-      <c r="AG6"/>
-      <c r="AH6"/>
-      <c r="AI6"/>
-      <c r="AJ6"/>
-      <c r="AK6"/>
-      <c r="AL6"/>
-      <c r="AM6"/>
-      <c r="AN6"/>
-      <c r="AO6"/>
-      <c r="AP6"/>
-      <c r="AQ6"/>
-      <c r="AR6"/>
-      <c r="AS6"/>
-      <c r="AT6"/>
-      <c r="AU6"/>
-      <c r="AV6"/>
-      <c r="AW6"/>
       <c r="AY6" s="3"/>
       <c r="AZ6" s="3"/>
       <c r="BA6" s="3"/>
@@ -68043,7 +67833,7 @@
       <c r="FI6" s="3"/>
       <c r="FJ6" s="3"/>
     </row>
-    <row r="7" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="7" spans="1:16384" customFormat="1" ht="15">
       <c r="A7" s="3">
         <v>24166864</v>
       </c>
@@ -68060,49 +67850,7 @@
         <v>30</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
       <c r="P7" s="2"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-      <c r="AC7"/>
-      <c r="AD7"/>
-      <c r="AE7"/>
-      <c r="AF7"/>
-      <c r="AG7"/>
-      <c r="AH7"/>
-      <c r="AI7"/>
-      <c r="AJ7"/>
-      <c r="AK7"/>
-      <c r="AL7"/>
-      <c r="AM7"/>
-      <c r="AN7"/>
-      <c r="AO7"/>
-      <c r="AP7"/>
-      <c r="AQ7"/>
-      <c r="AR7"/>
-      <c r="AS7"/>
-      <c r="AT7"/>
-      <c r="AU7"/>
-      <c r="AV7"/>
-      <c r="AW7"/>
       <c r="AY7" s="3"/>
       <c r="AZ7" s="3"/>
       <c r="BA7" s="3"/>
@@ -68220,7 +67968,7 @@
       <c r="FI7" s="3"/>
       <c r="FJ7" s="3"/>
     </row>
-    <row r="8" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="8" spans="1:16384" customFormat="1" ht="15">
       <c r="A8" s="3">
         <v>24166865</v>
       </c>
@@ -68239,49 +67987,7 @@
       <c r="F8" s="7">
         <v>45749</v>
       </c>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
       <c r="P8" s="2"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="S8"/>
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="Z8"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8"/>
-      <c r="AD8"/>
-      <c r="AE8"/>
-      <c r="AF8"/>
-      <c r="AG8"/>
-      <c r="AH8"/>
-      <c r="AI8"/>
-      <c r="AJ8"/>
-      <c r="AK8"/>
-      <c r="AL8"/>
-      <c r="AM8"/>
-      <c r="AN8"/>
-      <c r="AO8"/>
-      <c r="AP8"/>
-      <c r="AQ8"/>
-      <c r="AR8"/>
-      <c r="AS8"/>
-      <c r="AT8"/>
-      <c r="AU8"/>
-      <c r="AV8"/>
-      <c r="AW8"/>
       <c r="AY8" s="3"/>
       <c r="AZ8" s="3"/>
       <c r="BA8" s="3"/>
@@ -68421,7 +68127,7 @@
       <c r="FI8" s="3"/>
       <c r="FJ8" s="3"/>
     </row>
-    <row r="9" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="9" spans="1:16384" customFormat="1" ht="15">
       <c r="A9" s="3">
         <v>24166867</v>
       </c>
@@ -68440,49 +68146,7 @@
       <c r="F9" s="7">
         <v>45749</v>
       </c>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
       <c r="P9" s="2"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-      <c r="AC9"/>
-      <c r="AD9"/>
-      <c r="AE9"/>
-      <c r="AF9"/>
-      <c r="AG9"/>
-      <c r="AH9"/>
-      <c r="AI9"/>
-      <c r="AJ9"/>
-      <c r="AK9"/>
-      <c r="AL9"/>
-      <c r="AM9"/>
-      <c r="AN9"/>
-      <c r="AO9"/>
-      <c r="AP9"/>
-      <c r="AQ9"/>
-      <c r="AR9"/>
-      <c r="AS9"/>
-      <c r="AT9"/>
-      <c r="AU9"/>
-      <c r="AV9"/>
-      <c r="AW9"/>
       <c r="AY9" s="3"/>
       <c r="AZ9" s="3"/>
       <c r="BA9" s="3"/>
@@ -68620,7 +68284,7 @@
       <c r="FI9" s="3"/>
       <c r="FJ9" s="3"/>
     </row>
-    <row r="10" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="10" spans="1:16384" customFormat="1" ht="15">
       <c r="A10" s="3">
         <v>24166869</v>
       </c>
@@ -68637,49 +68301,7 @@
         <v>60</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
       <c r="P10" s="2"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
-      <c r="AE10"/>
-      <c r="AF10"/>
-      <c r="AG10"/>
-      <c r="AH10"/>
-      <c r="AI10"/>
-      <c r="AJ10"/>
-      <c r="AK10"/>
-      <c r="AL10"/>
-      <c r="AM10"/>
-      <c r="AN10"/>
-      <c r="AO10"/>
-      <c r="AP10"/>
-      <c r="AQ10"/>
-      <c r="AR10"/>
-      <c r="AS10"/>
-      <c r="AT10"/>
-      <c r="AU10"/>
-      <c r="AV10"/>
-      <c r="AW10"/>
       <c r="AY10" s="3"/>
       <c r="AZ10" s="3"/>
       <c r="BA10" s="3"/>
@@ -68797,7 +68419,7 @@
       <c r="FI10" s="3"/>
       <c r="FJ10" s="3"/>
     </row>
-    <row r="11" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="11" spans="1:16384" customFormat="1" ht="15">
       <c r="A11" s="3">
         <v>24166889</v>
       </c>
@@ -68814,49 +68436,7 @@
         <v>60</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
       <c r="P11" s="2"/>
-      <c r="Q11"/>
-      <c r="R11"/>
-      <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-      <c r="Z11"/>
-      <c r="AA11"/>
-      <c r="AB11"/>
-      <c r="AC11"/>
-      <c r="AD11"/>
-      <c r="AE11"/>
-      <c r="AF11"/>
-      <c r="AG11"/>
-      <c r="AH11"/>
-      <c r="AI11"/>
-      <c r="AJ11"/>
-      <c r="AK11"/>
-      <c r="AL11"/>
-      <c r="AM11"/>
-      <c r="AN11"/>
-      <c r="AO11"/>
-      <c r="AP11"/>
-      <c r="AQ11"/>
-      <c r="AR11"/>
-      <c r="AS11"/>
-      <c r="AT11"/>
-      <c r="AU11"/>
-      <c r="AV11"/>
-      <c r="AW11"/>
       <c r="AY11" s="3"/>
       <c r="AZ11" s="3"/>
       <c r="BA11" s="3"/>
@@ -68974,7 +68554,7 @@
       <c r="FI11" s="3"/>
       <c r="FJ11" s="3"/>
     </row>
-    <row r="12" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="12" spans="1:16384" customFormat="1" ht="15">
       <c r="A12" s="3">
         <v>24166896</v>
       </c>
@@ -68991,49 +68571,7 @@
         <v>60</v>
       </c>
       <c r="F12" s="7"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
       <c r="P12" s="2"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-      <c r="AE12"/>
-      <c r="AF12"/>
-      <c r="AG12"/>
-      <c r="AH12"/>
-      <c r="AI12"/>
-      <c r="AJ12"/>
-      <c r="AK12"/>
-      <c r="AL12"/>
-      <c r="AM12"/>
-      <c r="AN12"/>
-      <c r="AO12"/>
-      <c r="AP12"/>
-      <c r="AQ12"/>
-      <c r="AR12"/>
-      <c r="AS12"/>
-      <c r="AT12"/>
-      <c r="AU12"/>
-      <c r="AV12"/>
-      <c r="AW12"/>
       <c r="AY12" s="3"/>
       <c r="AZ12" s="3"/>
       <c r="BA12" s="3"/>
@@ -69151,7 +68689,7 @@
       <c r="FI12" s="3"/>
       <c r="FJ12" s="3"/>
     </row>
-    <row r="13" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="13" spans="1:16384" customFormat="1" ht="15">
       <c r="A13" s="3">
         <v>24306368</v>
       </c>
@@ -69170,49 +68708,7 @@
       <c r="F13" s="7">
         <v>45677</v>
       </c>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
       <c r="P13" s="2"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="S13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-      <c r="AB13"/>
-      <c r="AC13"/>
-      <c r="AD13"/>
-      <c r="AE13"/>
-      <c r="AF13"/>
-      <c r="AG13"/>
-      <c r="AH13"/>
-      <c r="AI13"/>
-      <c r="AJ13"/>
-      <c r="AK13"/>
-      <c r="AL13"/>
-      <c r="AM13"/>
-      <c r="AN13"/>
-      <c r="AO13"/>
-      <c r="AP13"/>
-      <c r="AQ13"/>
-      <c r="AR13"/>
-      <c r="AS13"/>
-      <c r="AT13"/>
-      <c r="AU13"/>
-      <c r="AV13"/>
-      <c r="AW13"/>
       <c r="AY13" s="3"/>
       <c r="AZ13" s="3"/>
       <c r="BA13" s="3"/>
@@ -69330,7 +68826,7 @@
       <c r="FI13" s="3"/>
       <c r="FJ13" s="3"/>
     </row>
-    <row r="14" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="14" spans="1:16384" customFormat="1" ht="15">
       <c r="A14" s="3">
         <v>24308189</v>
       </c>
@@ -69349,49 +68845,7 @@
       <c r="F14" s="7">
         <v>45677</v>
       </c>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14"/>
-      <c r="O14"/>
       <c r="P14" s="2"/>
-      <c r="Q14"/>
-      <c r="R14"/>
-      <c r="S14"/>
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
-      <c r="Y14"/>
-      <c r="Z14"/>
-      <c r="AA14"/>
-      <c r="AB14"/>
-      <c r="AC14"/>
-      <c r="AD14"/>
-      <c r="AE14"/>
-      <c r="AF14"/>
-      <c r="AG14"/>
-      <c r="AH14"/>
-      <c r="AI14"/>
-      <c r="AJ14"/>
-      <c r="AK14"/>
-      <c r="AL14"/>
-      <c r="AM14"/>
-      <c r="AN14"/>
-      <c r="AO14"/>
-      <c r="AP14"/>
-      <c r="AQ14"/>
-      <c r="AR14"/>
-      <c r="AS14"/>
-      <c r="AT14"/>
-      <c r="AU14"/>
-      <c r="AV14"/>
-      <c r="AW14"/>
       <c r="AY14" s="3"/>
       <c r="AZ14" s="3"/>
       <c r="BA14" s="3"/>
@@ -69509,7 +68963,7 @@
       <c r="FI14" s="3"/>
       <c r="FJ14" s="3"/>
     </row>
-    <row r="15" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="15" spans="1:16384" customFormat="1" ht="15">
       <c r="A15" s="3">
         <v>24303936</v>
       </c>
@@ -69528,49 +68982,7 @@
       <c r="F15" s="7">
         <v>45698</v>
       </c>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
       <c r="P15" s="2"/>
-      <c r="Q15"/>
-      <c r="R15"/>
-      <c r="S15"/>
-      <c r="T15"/>
-      <c r="U15"/>
-      <c r="V15"/>
-      <c r="W15"/>
-      <c r="X15"/>
-      <c r="Y15"/>
-      <c r="Z15"/>
-      <c r="AA15"/>
-      <c r="AB15"/>
-      <c r="AC15"/>
-      <c r="AD15"/>
-      <c r="AE15"/>
-      <c r="AF15"/>
-      <c r="AG15"/>
-      <c r="AH15"/>
-      <c r="AI15"/>
-      <c r="AJ15"/>
-      <c r="AK15"/>
-      <c r="AL15"/>
-      <c r="AM15"/>
-      <c r="AN15"/>
-      <c r="AO15"/>
-      <c r="AP15"/>
-      <c r="AQ15"/>
-      <c r="AR15"/>
-      <c r="AS15"/>
-      <c r="AT15"/>
-      <c r="AU15"/>
-      <c r="AV15"/>
-      <c r="AW15"/>
       <c r="AY15" s="3"/>
       <c r="AZ15" s="3"/>
       <c r="BA15" s="3"/>
@@ -69796,7 +69208,7 @@
       <c r="FI15" s="3"/>
       <c r="FJ15" s="3"/>
     </row>
-    <row r="16" spans="1:16384" s="8" customFormat="1" ht="15">
+    <row r="16" spans="1:16384" customFormat="1" ht="15">
       <c r="A16" s="3">
         <v>24303937</v>
       </c>
@@ -69815,49 +69227,7 @@
       <c r="F16" s="7">
         <v>45698</v>
       </c>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
       <c r="P16" s="2"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-      <c r="Y16"/>
-      <c r="Z16"/>
-      <c r="AA16"/>
-      <c r="AB16"/>
-      <c r="AC16"/>
-      <c r="AD16"/>
-      <c r="AE16"/>
-      <c r="AF16"/>
-      <c r="AG16"/>
-      <c r="AH16"/>
-      <c r="AI16"/>
-      <c r="AJ16"/>
-      <c r="AK16"/>
-      <c r="AL16"/>
-      <c r="AM16"/>
-      <c r="AN16"/>
-      <c r="AO16"/>
-      <c r="AP16"/>
-      <c r="AQ16"/>
-      <c r="AR16"/>
-      <c r="AS16"/>
-      <c r="AT16"/>
-      <c r="AU16"/>
-      <c r="AV16"/>
-      <c r="AW16"/>
       <c r="AY16" s="3"/>
       <c r="AZ16" s="3"/>
       <c r="BA16" s="3"/>
@@ -81280,6 +80650,11 @@
       <c r="FJ90" s="3"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="e2d0evjMEKqaOD1xezl+l+Zg/EXqY9/tEh7JbBBiF49VTU+DQpT98U/vlJBHilgiDUz56i3BYMwAJr53+jvz/g==" saltValue="P6LFFuhE9p5aChpX4hfvVg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <protectedRanges>
+    <protectedRange sqref="A1:O1048576" name="Range1"/>
+    <protectedRange sqref="Q1:XFD1048576" name="Range2"/>
+  </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon May 26 06:20:53 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF024B2-BDAE-42F3-BD1D-9431A3C2E7B1}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{955DEF1F-E370-460F-8D4B-1EB999A6C08D}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -795,8 +795,8 @@
   <dimension ref="A1:XFD90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FG2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FK2" sqref="FK2:FK8"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="XDG2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="XEY15" sqref="XEY15"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -80650,10 +80650,11 @@
       <c r="FJ90" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="e2d0evjMEKqaOD1xezl+l+Zg/EXqY9/tEh7JbBBiF49VTU+DQpT98U/vlJBHilgiDUz56i3BYMwAJr53+jvz/g==" saltValue="P6LFFuhE9p5aChpX4hfvVg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="A1:O1048576" name="Range1"/>
-    <protectedRange sqref="Q1:XFD1048576" name="Range2"/>
+    <protectedRange sqref="F1:F1048576" name="Range1"/>
+    <protectedRange sqref="P1:P1048576" name="Range2"/>
+    <protectedRange sqref="Q1:XFD1048576" name="Range3"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon May 26 06:26:00 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{955DEF1F-E370-460F-8D4B-1EB999A6C08D}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22846581-03A8-4D54-A3C7-09AB69352775}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -795,8 +795,8 @@
   <dimension ref="A1:XFD90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="XDG2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="XEY15" sqref="XEY15"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="DJ55" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="DN62" sqref="DN62"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -76673,7 +76673,9 @@
       <c r="DM61" s="3">
         <v>24</v>
       </c>
-      <c r="DN61" s="3"/>
+      <c r="DN61" s="3">
+        <v>196</v>
+      </c>
       <c r="DO61" s="3"/>
       <c r="DP61" s="3"/>
       <c r="DQ61" s="3"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue May 27 13:46:50 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F5410F4-91DD-4F91-BFE8-CE5C675E7262}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{812ED599-ACEC-471A-92A9-A4D2CC4992C4}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="116">
   <si>
     <t>Module ID</t>
   </si>
@@ -366,6 +366,24 @@
   </si>
   <si>
     <t>VSL202425376</t>
+  </si>
+  <si>
+    <t>VSL202526033</t>
+  </si>
+  <si>
+    <t>Toyo Cell (TOPCon) evaluation</t>
+  </si>
+  <si>
+    <t>VSL202526032</t>
+  </si>
+  <si>
+    <t>VSL202526010</t>
+  </si>
+  <si>
+    <t>PT Bintan Cell Reliability Test</t>
+  </si>
+  <si>
+    <t>VSL202526009</t>
   </si>
 </sst>
 </file>
@@ -834,8 +852,8 @@
   <dimension ref="A1:XFD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FF87" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B94" sqref="B94"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FG43" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F94" sqref="F94"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -80690,8 +80708,73 @@
       <c r="FI90" s="1"/>
       <c r="FJ90" s="1"/>
     </row>
-    <row r="94" spans="1:166">
-      <c r="B94" s="15"/>
+    <row r="91" spans="1:166" ht="15">
+      <c r="A91" s="10">
+        <v>25112301</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E91" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="1:166" ht="15">
+      <c r="A92" s="10">
+        <v>25112300</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" s="10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:166" ht="15">
+      <c r="A93" s="10">
+        <v>25087863</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E93" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="94" spans="1:166" ht="15">
+      <c r="A94" s="10">
+        <v>25087787</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" s="10">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May 29 05:04:05 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28922"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28926"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{812ED599-ACEC-471A-92A9-A4D2CC4992C4}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A478A42-6CBD-4386-ADEC-604EA17C220B}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="117">
   <si>
     <t>Module ID</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>QC SOLAR BLK DIODE 2.0</t>
+  </si>
+  <si>
+    <t>off</t>
   </si>
   <si>
     <t>VSL202425377</t>
@@ -852,8 +855,8 @@
   <dimension ref="A1:XFD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FG43" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F94" sqref="F94"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FG82" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F93" sqref="F93"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -71491,6 +71494,9 @@
       <c r="F27" s="13">
         <v>45719</v>
       </c>
+      <c r="P27" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY27" s="1"/>
       <c r="AZ27" s="1"/>
       <c r="BA27" s="1"/>
@@ -71651,6 +71657,9 @@
       <c r="F28" s="13">
         <v>45719</v>
       </c>
+      <c r="P28" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY28" s="1"/>
       <c r="AZ28" s="1"/>
       <c r="BA28" s="1"/>
@@ -71811,6 +71820,9 @@
       <c r="F29" s="13">
         <v>45719</v>
       </c>
+      <c r="P29" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY29" s="1"/>
       <c r="AZ29" s="1"/>
       <c r="BA29" s="1"/>
@@ -71971,6 +71983,9 @@
       <c r="F30" s="13">
         <v>45719</v>
       </c>
+      <c r="P30" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY30" s="1"/>
       <c r="AZ30" s="1"/>
       <c r="BA30" s="1"/>
@@ -72131,6 +72146,9 @@
       <c r="F31" s="13">
         <v>45719</v>
       </c>
+      <c r="P31" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY31" s="1"/>
       <c r="AZ31" s="1"/>
       <c r="BA31" s="1"/>
@@ -72291,6 +72309,9 @@
       <c r="F32" s="13">
         <v>45719</v>
       </c>
+      <c r="P32" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY32" s="1"/>
       <c r="AZ32" s="1"/>
       <c r="BA32" s="1"/>
@@ -72405,9 +72426,7 @@
       <c r="EH32" s="1"/>
       <c r="EI32" s="1"/>
       <c r="EJ32" s="1"/>
-      <c r="EK32" s="1">
-        <v>6</v>
-      </c>
+      <c r="EK32" s="1"/>
       <c r="EL32" s="1"/>
       <c r="EM32" s="1"/>
       <c r="EN32" s="1"/>
@@ -72451,7 +72470,10 @@
         <v>96</v>
       </c>
       <c r="F33" s="13">
-        <v>45721</v>
+        <v>45755</v>
+      </c>
+      <c r="P33" s="3">
+        <v>45758</v>
       </c>
       <c r="AY33" s="1"/>
       <c r="AZ33" s="1"/>
@@ -72482,21 +72504,11 @@
       <c r="BY33" s="1"/>
       <c r="BZ33" s="1"/>
       <c r="CA33" s="1"/>
-      <c r="CB33" s="1">
-        <v>6</v>
-      </c>
-      <c r="CC33" s="1">
-        <v>24</v>
-      </c>
-      <c r="CD33" s="1">
-        <v>24</v>
-      </c>
-      <c r="CE33" s="1">
-        <v>24</v>
-      </c>
-      <c r="CF33" s="1">
-        <v>18</v>
-      </c>
+      <c r="CB33" s="1"/>
+      <c r="CC33" s="1"/>
+      <c r="CD33" s="1"/>
+      <c r="CE33" s="1"/>
+      <c r="CF33" s="1"/>
       <c r="CG33" s="1"/>
       <c r="CH33" s="1"/>
       <c r="CI33" s="1"/>
@@ -72526,11 +72538,21 @@
       <c r="DG33" s="1"/>
       <c r="DH33" s="1"/>
       <c r="DI33" s="1"/>
-      <c r="DJ33" s="1"/>
-      <c r="DK33" s="1"/>
-      <c r="DL33" s="1"/>
-      <c r="DM33" s="1"/>
-      <c r="DN33" s="1"/>
+      <c r="DJ33" s="1">
+        <v>6</v>
+      </c>
+      <c r="DK33" s="1">
+        <v>24</v>
+      </c>
+      <c r="DL33" s="1">
+        <v>24</v>
+      </c>
+      <c r="DM33" s="1">
+        <v>24</v>
+      </c>
+      <c r="DN33" s="1">
+        <v>18</v>
+      </c>
       <c r="DO33" s="1"/>
       <c r="DP33" s="1"/>
       <c r="DQ33" s="1"/>
@@ -72553,9 +72575,7 @@
       <c r="EH33" s="1"/>
       <c r="EI33" s="1"/>
       <c r="EJ33" s="1"/>
-      <c r="EK33" s="1">
-        <v>6</v>
-      </c>
+      <c r="EK33" s="1"/>
       <c r="EL33" s="1"/>
       <c r="EM33" s="1"/>
       <c r="EN33" s="1"/>
@@ -72599,7 +72619,10 @@
         <v>96</v>
       </c>
       <c r="F34" s="13">
-        <v>45721</v>
+        <v>45755</v>
+      </c>
+      <c r="P34" s="3">
+        <v>45758</v>
       </c>
       <c r="AY34" s="1"/>
       <c r="AZ34" s="1"/>
@@ -72630,21 +72653,11 @@
       <c r="BY34" s="1"/>
       <c r="BZ34" s="1"/>
       <c r="CA34" s="1"/>
-      <c r="CB34" s="1">
-        <v>6</v>
-      </c>
-      <c r="CC34" s="1">
-        <v>24</v>
-      </c>
-      <c r="CD34" s="1">
-        <v>24</v>
-      </c>
-      <c r="CE34" s="1">
-        <v>24</v>
-      </c>
-      <c r="CF34" s="1">
-        <v>18</v>
-      </c>
+      <c r="CB34" s="1"/>
+      <c r="CC34" s="1"/>
+      <c r="CD34" s="1"/>
+      <c r="CE34" s="1"/>
+      <c r="CF34" s="1"/>
       <c r="CG34" s="1"/>
       <c r="CH34" s="1"/>
       <c r="CI34" s="1"/>
@@ -72674,11 +72687,21 @@
       <c r="DG34" s="1"/>
       <c r="DH34" s="1"/>
       <c r="DI34" s="1"/>
-      <c r="DJ34" s="1"/>
-      <c r="DK34" s="1"/>
-      <c r="DL34" s="1"/>
-      <c r="DM34" s="1"/>
-      <c r="DN34" s="1"/>
+      <c r="DJ34" s="1">
+        <v>6</v>
+      </c>
+      <c r="DK34" s="1">
+        <v>24</v>
+      </c>
+      <c r="DL34" s="1">
+        <v>24</v>
+      </c>
+      <c r="DM34" s="1">
+        <v>24</v>
+      </c>
+      <c r="DN34" s="1">
+        <v>18</v>
+      </c>
       <c r="DO34" s="1"/>
       <c r="DP34" s="1"/>
       <c r="DQ34" s="1"/>
@@ -72701,9 +72724,7 @@
       <c r="EH34" s="1"/>
       <c r="EI34" s="1"/>
       <c r="EJ34" s="1"/>
-      <c r="EK34" s="1">
-        <v>6</v>
-      </c>
+      <c r="EK34" s="1"/>
       <c r="EL34" s="1"/>
       <c r="EM34" s="1"/>
       <c r="EN34" s="1"/>
@@ -72778,21 +72799,11 @@
       <c r="BY35" s="1"/>
       <c r="BZ35" s="1"/>
       <c r="CA35" s="1"/>
-      <c r="CB35" s="1">
-        <v>6</v>
-      </c>
-      <c r="CC35" s="1">
-        <v>24</v>
-      </c>
-      <c r="CD35" s="1">
-        <v>24</v>
-      </c>
-      <c r="CE35" s="1">
-        <v>24</v>
-      </c>
-      <c r="CF35" s="1">
-        <v>18</v>
-      </c>
+      <c r="CB35" s="1"/>
+      <c r="CC35" s="1"/>
+      <c r="CD35" s="1"/>
+      <c r="CE35" s="1"/>
+      <c r="CF35" s="1"/>
       <c r="CG35" s="1"/>
       <c r="CH35" s="1"/>
       <c r="CI35" s="1"/>
@@ -73297,6 +73308,9 @@
       <c r="F39" s="13">
         <v>45722</v>
       </c>
+      <c r="P39" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY39" s="1"/>
       <c r="AZ39" s="1"/>
       <c r="BA39" s="1"/>
@@ -73457,6 +73471,9 @@
       <c r="F40" s="13">
         <v>45722</v>
       </c>
+      <c r="P40" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY40" s="1"/>
       <c r="AZ40" s="1"/>
       <c r="BA40" s="1"/>
@@ -73617,6 +73634,9 @@
       <c r="F41" s="13">
         <v>45722</v>
       </c>
+      <c r="P41" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY41" s="1"/>
       <c r="AZ41" s="1"/>
       <c r="BA41" s="1"/>
@@ -73777,6 +73797,9 @@
       <c r="F42" s="13">
         <v>45722</v>
       </c>
+      <c r="P42" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY42" s="1"/>
       <c r="AZ42" s="1"/>
       <c r="BA42" s="1"/>
@@ -73937,6 +73960,9 @@
       <c r="F43" s="13">
         <v>45722</v>
       </c>
+      <c r="P43" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY43" s="1"/>
       <c r="AZ43" s="1"/>
       <c r="BA43" s="1"/>
@@ -74097,6 +74123,9 @@
       <c r="F44" s="13">
         <v>45722</v>
       </c>
+      <c r="P44" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY44" s="1"/>
       <c r="AZ44" s="1"/>
       <c r="BA44" s="1"/>
@@ -74257,6 +74286,9 @@
       <c r="F45" s="13">
         <v>45722</v>
       </c>
+      <c r="P45" s="3">
+        <v>45730</v>
+      </c>
       <c r="AY45" s="1"/>
       <c r="AZ45" s="1"/>
       <c r="BA45" s="1"/>
@@ -74416,6 +74448,9 @@
       </c>
       <c r="F46" s="13">
         <v>45722</v>
+      </c>
+      <c r="P46" s="3">
+        <v>45730</v>
       </c>
       <c r="AY46" s="1"/>
       <c r="AZ46" s="1"/>
@@ -77631,6 +77666,9 @@
       <c r="F68" s="13">
         <v>45773</v>
       </c>
+      <c r="P68" s="3">
+        <v>45776</v>
+      </c>
       <c r="AY68" s="1"/>
       <c r="AZ68" s="1"/>
       <c r="BA68" s="1"/>
@@ -77712,10 +77750,18 @@
       <c r="DY68" s="1"/>
       <c r="DZ68" s="1"/>
       <c r="EA68" s="1"/>
-      <c r="EB68" s="1"/>
-      <c r="EC68" s="1"/>
-      <c r="ED68" s="1"/>
-      <c r="EE68" s="1"/>
+      <c r="EB68" s="1">
+        <v>24</v>
+      </c>
+      <c r="EC68" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED68" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE68" s="1">
+        <v>24</v>
+      </c>
       <c r="EF68" s="1"/>
       <c r="EG68" s="1"/>
       <c r="EH68" s="1"/>
@@ -78035,6 +78081,9 @@
       <c r="F71" s="13">
         <v>45773</v>
       </c>
+      <c r="P71" s="3">
+        <v>45776</v>
+      </c>
       <c r="AY71" s="1"/>
       <c r="AZ71" s="1"/>
       <c r="BA71" s="1"/>
@@ -78117,20 +78166,18 @@
       <c r="DZ71" s="1"/>
       <c r="EA71" s="1"/>
       <c r="EB71" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="EC71" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="ED71" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="EE71" s="1">
-        <v>20</v>
-      </c>
-      <c r="EF71" s="1">
-        <v>20</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="EF71" s="1"/>
       <c r="EG71" s="1"/>
       <c r="EH71" s="1"/>
       <c r="EI71" s="1"/>
@@ -78312,7 +78359,9 @@
       <c r="E73" s="9">
         <v>500</v>
       </c>
-      <c r="F73" s="13"/>
+      <c r="F73" s="13">
+        <v>45763</v>
+      </c>
       <c r="AY73" s="1"/>
       <c r="AZ73" s="1"/>
       <c r="BA73" s="1"/>
@@ -78384,49 +78433,135 @@
       <c r="DO73" s="1"/>
       <c r="DP73" s="1"/>
       <c r="DQ73" s="1"/>
-      <c r="DR73" s="1"/>
-      <c r="DS73" s="1"/>
-      <c r="DT73" s="1"/>
-      <c r="DU73" s="1"/>
-      <c r="DV73" s="1"/>
-      <c r="DW73" s="1"/>
-      <c r="DX73" s="1"/>
-      <c r="DY73" s="1"/>
-      <c r="DZ73" s="1"/>
-      <c r="EA73" s="1"/>
-      <c r="EB73" s="1"/>
-      <c r="EC73" s="1"/>
-      <c r="ED73" s="1"/>
-      <c r="EE73" s="1"/>
-      <c r="EF73" s="1"/>
-      <c r="EG73" s="1"/>
-      <c r="EH73" s="1"/>
-      <c r="EI73" s="1"/>
-      <c r="EJ73" s="1"/>
-      <c r="EK73" s="1"/>
-      <c r="EL73" s="1"/>
-      <c r="EM73" s="1"/>
-      <c r="EN73" s="1"/>
-      <c r="EO73" s="1"/>
-      <c r="EP73" s="1"/>
-      <c r="EQ73" s="1"/>
-      <c r="ER73" s="1"/>
-      <c r="ES73" s="1"/>
-      <c r="ET73" s="1"/>
-      <c r="EU73" s="1"/>
-      <c r="EV73" s="1"/>
-      <c r="EW73" s="1"/>
-      <c r="EX73" s="1"/>
-      <c r="EY73" s="1"/>
-      <c r="EZ73" s="1"/>
-      <c r="FA73" s="1"/>
-      <c r="FB73" s="1"/>
-      <c r="FC73" s="1"/>
-      <c r="FD73" s="1"/>
-      <c r="FE73" s="1"/>
-      <c r="FF73" s="1"/>
-      <c r="FG73" s="1"/>
-      <c r="FH73" s="1"/>
+      <c r="DR73" s="1">
+        <v>12</v>
+      </c>
+      <c r="DS73" s="1">
+        <v>24</v>
+      </c>
+      <c r="DT73" s="1">
+        <v>9</v>
+      </c>
+      <c r="DU73" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DV73" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DW73" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DX73" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DY73" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DZ73" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="EA73" s="1">
+        <v>6</v>
+      </c>
+      <c r="EB73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EC73" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG73" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="EH73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ73" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER73" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES73" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY73" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH73" s="1">
+        <v>24</v>
+      </c>
       <c r="FI73" s="1"/>
       <c r="FJ73" s="1"/>
     </row>
@@ -78435,10 +78570,10 @@
         <v>24859051</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>28</v>
@@ -78446,7 +78581,9 @@
       <c r="E74" s="9">
         <v>500</v>
       </c>
-      <c r="F74" s="13"/>
+      <c r="F74" s="13">
+        <v>45763</v>
+      </c>
       <c r="AY74" s="1"/>
       <c r="AZ74" s="1"/>
       <c r="BA74" s="1"/>
@@ -78518,49 +78655,135 @@
       <c r="DO74" s="1"/>
       <c r="DP74" s="1"/>
       <c r="DQ74" s="1"/>
-      <c r="DR74" s="1"/>
-      <c r="DS74" s="1"/>
-      <c r="DT74" s="1"/>
-      <c r="DU74" s="1"/>
-      <c r="DV74" s="1"/>
-      <c r="DW74" s="1"/>
-      <c r="DX74" s="1"/>
-      <c r="DY74" s="1"/>
-      <c r="DZ74" s="1"/>
-      <c r="EA74" s="1"/>
-      <c r="EB74" s="1"/>
-      <c r="EC74" s="1"/>
-      <c r="ED74" s="1"/>
-      <c r="EE74" s="1"/>
-      <c r="EF74" s="1"/>
-      <c r="EG74" s="1"/>
-      <c r="EH74" s="1"/>
-      <c r="EI74" s="1"/>
-      <c r="EJ74" s="1"/>
-      <c r="EK74" s="1"/>
-      <c r="EL74" s="1"/>
-      <c r="EM74" s="1"/>
-      <c r="EN74" s="1"/>
-      <c r="EO74" s="1"/>
-      <c r="EP74" s="1"/>
-      <c r="EQ74" s="1"/>
-      <c r="ER74" s="1"/>
-      <c r="ES74" s="1"/>
-      <c r="ET74" s="1"/>
-      <c r="EU74" s="1"/>
-      <c r="EV74" s="1"/>
-      <c r="EW74" s="1"/>
-      <c r="EX74" s="1"/>
-      <c r="EY74" s="1"/>
-      <c r="EZ74" s="1"/>
-      <c r="FA74" s="1"/>
-      <c r="FB74" s="1"/>
-      <c r="FC74" s="1"/>
-      <c r="FD74" s="1"/>
-      <c r="FE74" s="1"/>
-      <c r="FF74" s="1"/>
-      <c r="FG74" s="1"/>
-      <c r="FH74" s="1"/>
+      <c r="DR74" s="1">
+        <v>12</v>
+      </c>
+      <c r="DS74" s="1">
+        <v>24</v>
+      </c>
+      <c r="DT74" s="1">
+        <v>9</v>
+      </c>
+      <c r="DU74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DV74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DW74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DX74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DY74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DZ74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="EA74" s="1">
+        <v>6</v>
+      </c>
+      <c r="EB74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EC74" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="EH74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ74" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER74" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES74" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY74" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH74" s="1">
+        <v>24</v>
+      </c>
       <c r="FI74" s="1"/>
       <c r="FJ74" s="1"/>
     </row>
@@ -78703,10 +78926,10 @@
         <v>24859051</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>28</v>
@@ -78971,10 +79194,10 @@
         <v>24859051</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>28</v>
@@ -79239,10 +79462,10 @@
         <v>24859051</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>28</v>
@@ -79507,10 +79730,10 @@
         <v>24859051</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>28</v>
@@ -79775,10 +79998,10 @@
         <v>24859051</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>28</v>
@@ -79909,13 +80132,13 @@
         <v>24988445</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E85" s="9">
         <v>96</v>
@@ -80043,10 +80266,10 @@
         <v>24988559</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>18</v>
@@ -80177,13 +80400,13 @@
         <v>24988692</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E87" s="9">
         <v>162</v>
@@ -80311,10 +80534,10 @@
         <v>24923318</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>28</v>
@@ -80322,7 +80545,9 @@
       <c r="E88" s="9">
         <v>1000</v>
       </c>
-      <c r="F88" s="13"/>
+      <c r="F88" s="13">
+        <v>45793</v>
+      </c>
       <c r="AY88" s="1"/>
       <c r="AZ88" s="1"/>
       <c r="BA88" s="1"/>
@@ -80427,16 +80652,36 @@
       <c r="EV88" s="1"/>
       <c r="EW88" s="1"/>
       <c r="EX88" s="1"/>
-      <c r="EY88" s="1"/>
-      <c r="EZ88" s="1"/>
-      <c r="FA88" s="1"/>
-      <c r="FB88" s="1"/>
-      <c r="FC88" s="1"/>
-      <c r="FD88" s="1"/>
-      <c r="FE88" s="1"/>
-      <c r="FF88" s="1"/>
-      <c r="FG88" s="1"/>
-      <c r="FH88" s="1"/>
+      <c r="EY88" s="1">
+        <v>12</v>
+      </c>
+      <c r="EZ88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH88" s="1">
+        <v>24</v>
+      </c>
       <c r="FI88" s="1"/>
       <c r="FJ88" s="1"/>
     </row>
@@ -80445,10 +80690,10 @@
         <v>24925212</v>
       </c>
       <c r="B89" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>28</v>
@@ -80579,10 +80824,10 @@
         <v>24857462</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>21</v>
@@ -80713,16 +80958,19 @@
         <v>25112301</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D91" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E91" s="10">
         <v>96</v>
+      </c>
+      <c r="F91" s="14">
+        <v>45806</v>
       </c>
     </row>
     <row r="92" spans="1:166" ht="15">
@@ -80730,10 +80978,10 @@
         <v>25112300</v>
       </c>
       <c r="B92" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="D92" s="10" t="s">
         <v>28</v>
@@ -80747,16 +80995,19 @@
         <v>25087863</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D93" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E93" s="10">
         <v>96</v>
+      </c>
+      <c r="F93" s="14">
+        <v>45806</v>
       </c>
     </row>
     <row r="94" spans="1:166" ht="15">
@@ -80764,10 +81015,10 @@
         <v>25087787</v>
       </c>
       <c r="B94" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="D94" s="10" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May 29 09:38:54 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A478A42-6CBD-4386-ADEC-604EA17C220B}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0569F5A1-02D7-4659-8447-5BED2044ABD5}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -855,8 +855,8 @@
   <dimension ref="A1:XFD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FG82" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F93" sqref="F93"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FE43" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="EC48" sqref="EC48:FH48"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -74746,6 +74746,9 @@
       <c r="F48" s="13">
         <v>45773</v>
       </c>
+      <c r="P48" s="3">
+        <v>45806</v>
+      </c>
       <c r="AY48" s="1"/>
       <c r="AZ48" s="1"/>
       <c r="BA48" s="1"/>
@@ -74828,39 +74831,105 @@
       <c r="DZ48" s="1"/>
       <c r="EA48" s="1"/>
       <c r="EB48" s="1"/>
-      <c r="EC48" s="1"/>
-      <c r="ED48" s="1"/>
-      <c r="EE48" s="1"/>
-      <c r="EF48" s="1"/>
-      <c r="EG48" s="1"/>
-      <c r="EH48" s="1"/>
-      <c r="EI48" s="1"/>
-      <c r="EJ48" s="1"/>
-      <c r="EK48" s="1"/>
-      <c r="EL48" s="1"/>
-      <c r="EM48" s="1"/>
-      <c r="EN48" s="1"/>
-      <c r="EO48" s="1"/>
-      <c r="EP48" s="1"/>
-      <c r="EQ48" s="1"/>
-      <c r="ER48" s="1"/>
-      <c r="ES48" s="1"/>
-      <c r="ET48" s="1"/>
-      <c r="EU48" s="1"/>
-      <c r="EV48" s="1"/>
-      <c r="EW48" s="1"/>
-      <c r="EX48" s="1"/>
-      <c r="EY48" s="1"/>
-      <c r="EZ48" s="1"/>
-      <c r="FA48" s="1"/>
-      <c r="FB48" s="1"/>
-      <c r="FC48" s="1"/>
-      <c r="FD48" s="1"/>
-      <c r="FE48" s="1"/>
-      <c r="FF48" s="1"/>
-      <c r="FG48" s="1"/>
-      <c r="FH48" s="1"/>
-      <c r="FI48" s="1"/>
+      <c r="EC48" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EH48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ48" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER48" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES48" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY48" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH48" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI48" s="1">
+        <v>10</v>
+      </c>
       <c r="FJ48" s="1"/>
     </row>
     <row r="49" spans="1:166" ht="15">
@@ -75016,6 +75085,9 @@
       <c r="F50" s="13">
         <v>45773</v>
       </c>
+      <c r="P50" s="3">
+        <v>45806</v>
+      </c>
       <c r="AY50" s="1"/>
       <c r="AZ50" s="1"/>
       <c r="BA50" s="1"/>
@@ -75098,39 +75170,105 @@
       <c r="DZ50" s="1"/>
       <c r="EA50" s="1"/>
       <c r="EB50" s="1"/>
-      <c r="EC50" s="1"/>
-      <c r="ED50" s="1"/>
-      <c r="EE50" s="1"/>
-      <c r="EF50" s="1"/>
-      <c r="EG50" s="1"/>
-      <c r="EH50" s="1"/>
-      <c r="EI50" s="1"/>
-      <c r="EJ50" s="1"/>
-      <c r="EK50" s="1"/>
-      <c r="EL50" s="1"/>
-      <c r="EM50" s="1"/>
-      <c r="EN50" s="1"/>
-      <c r="EO50" s="1"/>
-      <c r="EP50" s="1"/>
-      <c r="EQ50" s="1"/>
-      <c r="ER50" s="1"/>
-      <c r="ES50" s="1"/>
-      <c r="ET50" s="1"/>
-      <c r="EU50" s="1"/>
-      <c r="EV50" s="1"/>
-      <c r="EW50" s="1"/>
-      <c r="EX50" s="1"/>
-      <c r="EY50" s="1"/>
-      <c r="EZ50" s="1"/>
-      <c r="FA50" s="1"/>
-      <c r="FB50" s="1"/>
-      <c r="FC50" s="1"/>
-      <c r="FD50" s="1"/>
-      <c r="FE50" s="1"/>
-      <c r="FF50" s="1"/>
-      <c r="FG50" s="1"/>
-      <c r="FH50" s="1"/>
-      <c r="FI50" s="1"/>
+      <c r="EC50" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EH50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ50" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER50" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES50" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY50" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH50" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI50" s="1">
+        <v>10</v>
+      </c>
       <c r="FJ50" s="1"/>
     </row>
     <row r="51" spans="1:166" ht="15">
@@ -75151,6 +75289,9 @@
       </c>
       <c r="F51" s="13">
         <v>45773</v>
+      </c>
+      <c r="P51" s="3">
+        <v>45806</v>
       </c>
       <c r="AY51" s="1"/>
       <c r="AZ51" s="1"/>
@@ -75234,39 +75375,105 @@
       <c r="DZ51" s="1"/>
       <c r="EA51" s="1"/>
       <c r="EB51" s="1"/>
-      <c r="EC51" s="1"/>
-      <c r="ED51" s="1"/>
-      <c r="EE51" s="1"/>
-      <c r="EF51" s="1"/>
-      <c r="EG51" s="1"/>
-      <c r="EH51" s="1"/>
-      <c r="EI51" s="1"/>
-      <c r="EJ51" s="1"/>
-      <c r="EK51" s="1"/>
-      <c r="EL51" s="1"/>
-      <c r="EM51" s="1"/>
-      <c r="EN51" s="1"/>
-      <c r="EO51" s="1"/>
-      <c r="EP51" s="1"/>
-      <c r="EQ51" s="1"/>
-      <c r="ER51" s="1"/>
-      <c r="ES51" s="1"/>
-      <c r="ET51" s="1"/>
-      <c r="EU51" s="1"/>
-      <c r="EV51" s="1"/>
-      <c r="EW51" s="1"/>
-      <c r="EX51" s="1"/>
-      <c r="EY51" s="1"/>
-      <c r="EZ51" s="1"/>
-      <c r="FA51" s="1"/>
-      <c r="FB51" s="1"/>
-      <c r="FC51" s="1"/>
-      <c r="FD51" s="1"/>
-      <c r="FE51" s="1"/>
-      <c r="FF51" s="1"/>
-      <c r="FG51" s="1"/>
-      <c r="FH51" s="1"/>
-      <c r="FI51" s="1"/>
+      <c r="EC51" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EH51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ51" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER51" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES51" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY51" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH51" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI51" s="1">
+        <v>10</v>
+      </c>
       <c r="FJ51" s="1"/>
     </row>
     <row r="52" spans="1:166" ht="15">
@@ -75287,6 +75494,9 @@
       </c>
       <c r="F52" s="13">
         <v>45773</v>
+      </c>
+      <c r="P52" s="3">
+        <v>45806</v>
       </c>
       <c r="AY52" s="1"/>
       <c r="AZ52" s="1"/>
@@ -75370,39 +75580,105 @@
       <c r="DZ52" s="1"/>
       <c r="EA52" s="1"/>
       <c r="EB52" s="1"/>
-      <c r="EC52" s="1"/>
-      <c r="ED52" s="1"/>
-      <c r="EE52" s="1"/>
-      <c r="EF52" s="1"/>
-      <c r="EG52" s="1"/>
-      <c r="EH52" s="1"/>
-      <c r="EI52" s="1"/>
-      <c r="EJ52" s="1"/>
-      <c r="EK52" s="1"/>
-      <c r="EL52" s="1"/>
-      <c r="EM52" s="1"/>
-      <c r="EN52" s="1"/>
-      <c r="EO52" s="1"/>
-      <c r="EP52" s="1"/>
-      <c r="EQ52" s="1"/>
-      <c r="ER52" s="1"/>
-      <c r="ES52" s="1"/>
-      <c r="ET52" s="1"/>
-      <c r="EU52" s="1"/>
-      <c r="EV52" s="1"/>
-      <c r="EW52" s="1"/>
-      <c r="EX52" s="1"/>
-      <c r="EY52" s="1"/>
-      <c r="EZ52" s="1"/>
-      <c r="FA52" s="1"/>
-      <c r="FB52" s="1"/>
-      <c r="FC52" s="1"/>
-      <c r="FD52" s="1"/>
-      <c r="FE52" s="1"/>
-      <c r="FF52" s="1"/>
-      <c r="FG52" s="1"/>
-      <c r="FH52" s="1"/>
-      <c r="FI52" s="1"/>
+      <c r="EC52" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EH52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ52" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER52" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES52" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY52" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH52" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI52" s="1">
+        <v>10</v>
+      </c>
       <c r="FJ52" s="1"/>
     </row>
     <row r="53" spans="1:166" ht="15">
@@ -78562,7 +78838,9 @@
       <c r="FH73" s="1">
         <v>24</v>
       </c>
-      <c r="FI73" s="1"/>
+      <c r="FI73" s="1">
+        <v>24</v>
+      </c>
       <c r="FJ73" s="1"/>
     </row>
     <row r="74" spans="1:166" ht="15">
@@ -78784,7 +79062,9 @@
       <c r="FH74" s="1">
         <v>24</v>
       </c>
-      <c r="FI74" s="1"/>
+      <c r="FI74" s="1">
+        <v>24</v>
+      </c>
       <c r="FJ74" s="1"/>
     </row>
     <row r="75" spans="1:166" ht="15">
@@ -80682,7 +80962,9 @@
       <c r="FH88" s="1">
         <v>24</v>
       </c>
-      <c r="FI88" s="1"/>
+      <c r="FI88" s="1">
+        <v>24</v>
+      </c>
       <c r="FJ88" s="1"/>
     </row>
     <row r="89" spans="1:166" ht="15">
@@ -80972,6 +81254,9 @@
       <c r="F91" s="14">
         <v>45806</v>
       </c>
+      <c r="FI91" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="92" spans="1:166" ht="15">
       <c r="A92" s="10">
@@ -80989,6 +81274,12 @@
       <c r="E92" s="10">
         <v>1000</v>
       </c>
+      <c r="F92" s="14">
+        <v>45806</v>
+      </c>
+      <c r="FI92" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="93" spans="1:166" ht="15">
       <c r="A93" s="10">
@@ -81008,6 +81299,9 @@
       </c>
       <c r="F93" s="14">
         <v>45806</v>
+      </c>
+      <c r="FI93" s="4">
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:166" ht="15">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May 29 11:33:30 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -855,8 +855,8 @@
   <dimension ref="A1:XFD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FE43" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="EC48" sqref="EC48:FH48"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="ER43" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="ES54" sqref="ES54"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri May 30 13:43:45 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0569F5A1-02D7-4659-8447-5BED2044ABD5}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BB5119E-B7BF-4A42-997E-035CB28E24A5}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -855,8 +855,8 @@
   <dimension ref="A1:XFD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="ER43" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="ES54" sqref="ES54"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FG67" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FJ73" sqref="FJ73"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -78621,7 +78621,7 @@
     </row>
     <row r="73" spans="1:166" ht="15">
       <c r="A73" s="9">
-        <v>24948800</v>
+        <v>24848800</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>96</v>
@@ -79069,7 +79069,7 @@
     </row>
     <row r="75" spans="1:166" ht="15">
       <c r="A75" s="9">
-        <v>24948800</v>
+        <v>24848800</v>
       </c>
       <c r="B75" s="9" t="s">
         <v>96</v>
@@ -79337,7 +79337,7 @@
     </row>
     <row r="77" spans="1:166" ht="15">
       <c r="A77" s="9">
-        <v>24948800</v>
+        <v>24848800</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>96</v>
@@ -79605,7 +79605,7 @@
     </row>
     <row r="79" spans="1:166" ht="15">
       <c r="A79" s="9">
-        <v>24948800</v>
+        <v>24848800</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>96</v>
@@ -79873,7 +79873,7 @@
     </row>
     <row r="81" spans="1:166" ht="15">
       <c r="A81" s="9">
-        <v>24948800</v>
+        <v>24848800</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>96</v>
@@ -80141,7 +80141,7 @@
     </row>
     <row r="83" spans="1:166" ht="15">
       <c r="A83" s="9">
-        <v>24948800</v>
+        <v>24848800</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun  2 09:39:43 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BB5119E-B7BF-4A42-997E-035CB28E24A5}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C41E3173-2EE3-4D88-9F4A-2FD057296C21}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -855,8 +855,8 @@
   <dimension ref="A1:XFD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FG67" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FJ73" sqref="FJ73"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FG42" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FL52" sqref="FL52"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -72453,7 +72453,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:166" ht="15">
+    <row r="33" spans="1:168" ht="15">
       <c r="A33" s="9">
         <v>24636088</v>
       </c>
@@ -72602,7 +72602,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:166" ht="15">
+    <row r="34" spans="1:168" ht="15">
       <c r="A34" s="9">
         <v>24636089</v>
       </c>
@@ -72751,7 +72751,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:166" ht="15">
+    <row r="35" spans="1:168" ht="15">
       <c r="A35" s="9">
         <v>24636092</v>
       </c>
@@ -72887,7 +72887,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:166" ht="15">
+    <row r="36" spans="1:168" ht="15">
       <c r="A36" s="9">
         <v>24395952</v>
       </c>
@@ -73021,7 +73021,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:166" ht="15">
+    <row r="37" spans="1:168" ht="15">
       <c r="A37" s="9">
         <v>24395977</v>
       </c>
@@ -73155,7 +73155,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:166" ht="15">
+    <row r="38" spans="1:168" ht="15">
       <c r="A38" s="9">
         <v>24395942</v>
       </c>
@@ -73289,7 +73289,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:166" ht="15">
+    <row r="39" spans="1:168" ht="15">
       <c r="A39" s="12">
         <v>24567303</v>
       </c>
@@ -73452,7 +73452,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:166" ht="15">
+    <row r="40" spans="1:168" ht="15">
       <c r="A40" s="12">
         <v>24567296</v>
       </c>
@@ -73615,7 +73615,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:166" ht="15">
+    <row r="41" spans="1:168" ht="15">
       <c r="A41" s="12">
         <v>24567289</v>
       </c>
@@ -73778,7 +73778,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:166" ht="15">
+    <row r="42" spans="1:168" ht="15">
       <c r="A42" s="12">
         <v>24567319</v>
       </c>
@@ -73941,7 +73941,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:166" ht="15">
+    <row r="43" spans="1:168" ht="15">
       <c r="A43" s="12">
         <v>24567277</v>
       </c>
@@ -74104,7 +74104,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:166" ht="15">
+    <row r="44" spans="1:168" ht="15">
       <c r="A44" s="12">
         <v>24567774</v>
       </c>
@@ -74267,7 +74267,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:166" ht="15">
+    <row r="45" spans="1:168" ht="15">
       <c r="A45" s="12">
         <v>24567851</v>
       </c>
@@ -74430,7 +74430,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:166" ht="15">
+    <row r="46" spans="1:168" ht="15">
       <c r="A46" s="12">
         <v>24559501</v>
       </c>
@@ -74593,7 +74593,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:166" ht="15">
+    <row r="47" spans="1:168" ht="15">
       <c r="A47" s="12">
         <v>24567303</v>
       </c>
@@ -74727,7 +74727,7 @@
       <c r="FI47" s="1"/>
       <c r="FJ47" s="1"/>
     </row>
-    <row r="48" spans="1:166" ht="15">
+    <row r="48" spans="1:168" ht="15">
       <c r="A48" s="12">
         <v>24567296</v>
       </c>
@@ -74931,8 +74931,11 @@
         <v>10</v>
       </c>
       <c r="FJ48" s="1"/>
+      <c r="FL48" s="4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="49" spans="1:166" ht="15">
+    <row r="49" spans="1:168" ht="15">
       <c r="A49" s="12">
         <v>24567289</v>
       </c>
@@ -75066,7 +75069,7 @@
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
     </row>
-    <row r="50" spans="1:166" ht="15">
+    <row r="50" spans="1:168" ht="15">
       <c r="A50" s="12">
         <v>24567319</v>
       </c>
@@ -75270,8 +75273,11 @@
         <v>10</v>
       </c>
       <c r="FJ50" s="1"/>
+      <c r="FL50" s="4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="51" spans="1:166" ht="15">
+    <row r="51" spans="1:168" ht="15">
       <c r="A51" s="12">
         <v>24567277</v>
       </c>
@@ -75475,8 +75481,11 @@
         <v>10</v>
       </c>
       <c r="FJ51" s="1"/>
+      <c r="FL51" s="4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="52" spans="1:166" ht="15">
+    <row r="52" spans="1:168" ht="15">
       <c r="A52" s="12">
         <v>24567774</v>
       </c>
@@ -75680,8 +75689,11 @@
         <v>10</v>
       </c>
       <c r="FJ52" s="1"/>
+      <c r="FL52" s="4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="53" spans="1:166" ht="15">
+    <row r="53" spans="1:168" ht="15">
       <c r="A53" s="12">
         <v>24567851</v>
       </c>
@@ -75815,7 +75827,7 @@
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
     </row>
-    <row r="54" spans="1:166" ht="15">
+    <row r="54" spans="1:168" ht="15">
       <c r="A54" s="12">
         <v>24559501</v>
       </c>
@@ -75949,7 +75961,7 @@
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
     </row>
-    <row r="55" spans="1:166" ht="15">
+    <row r="55" spans="1:168" ht="15">
       <c r="A55" s="9">
         <v>24079686</v>
       </c>
@@ -76137,7 +76149,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:166" ht="15">
+    <row r="56" spans="1:168" ht="15">
       <c r="A56" s="9">
         <v>24079692</v>
       </c>
@@ -76325,7 +76337,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:166" ht="15">
+    <row r="57" spans="1:168" ht="15">
       <c r="A57" s="9">
         <v>24636092</v>
       </c>
@@ -76479,7 +76491,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:166" ht="15">
+    <row r="58" spans="1:168" ht="15">
       <c r="A58" s="9">
         <v>24793376</v>
       </c>
@@ -76635,7 +76647,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:166" ht="15">
+    <row r="59" spans="1:168" ht="15">
       <c r="A59" s="9">
         <v>24713456</v>
       </c>
@@ -76789,7 +76801,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:166" ht="15">
+    <row r="60" spans="1:168" ht="15">
       <c r="A60" s="9">
         <v>24713371</v>
       </c>
@@ -76935,7 +76947,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:166" ht="15">
+    <row r="61" spans="1:168" ht="15">
       <c r="A61" s="9">
         <v>24713222</v>
       </c>
@@ -77093,7 +77105,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:166" ht="15">
+    <row r="62" spans="1:168" ht="15">
       <c r="A62" s="12">
         <v>24636087</v>
       </c>
@@ -77229,7 +77241,7 @@
       <c r="FI62" s="1"/>
       <c r="FJ62" s="1"/>
     </row>
-    <row r="63" spans="1:166" ht="15">
+    <row r="63" spans="1:168" ht="15">
       <c r="A63" s="9">
         <v>24636090</v>
       </c>
@@ -77365,7 +77377,7 @@
       <c r="FI63" s="1"/>
       <c r="FJ63" s="1"/>
     </row>
-    <row r="64" spans="1:166" ht="15">
+    <row r="64" spans="1:168" ht="15">
       <c r="A64" s="9">
         <v>24636091</v>
       </c>
@@ -79871,7 +79883,7 @@
       <c r="FI80" s="1"/>
       <c r="FJ80" s="1"/>
     </row>
-    <row r="81" spans="1:166" ht="15">
+    <row r="81" spans="1:168" ht="15">
       <c r="A81" s="9">
         <v>24848800</v>
       </c>
@@ -80005,7 +80017,7 @@
       <c r="FI81" s="1"/>
       <c r="FJ81" s="1"/>
     </row>
-    <row r="82" spans="1:166" ht="15">
+    <row r="82" spans="1:168" ht="15">
       <c r="A82" s="9">
         <v>24859051</v>
       </c>
@@ -80139,7 +80151,7 @@
       <c r="FI82" s="1"/>
       <c r="FJ82" s="1"/>
     </row>
-    <row r="83" spans="1:166" ht="15">
+    <row r="83" spans="1:168" ht="15">
       <c r="A83" s="9">
         <v>24848800</v>
       </c>
@@ -80273,7 +80285,7 @@
       <c r="FI83" s="1"/>
       <c r="FJ83" s="1"/>
     </row>
-    <row r="84" spans="1:166" ht="15">
+    <row r="84" spans="1:168" ht="15">
       <c r="A84" s="9">
         <v>24859051</v>
       </c>
@@ -80407,7 +80419,7 @@
       <c r="FI84" s="1"/>
       <c r="FJ84" s="1"/>
     </row>
-    <row r="85" spans="1:166" ht="15">
+    <row r="85" spans="1:168" ht="15">
       <c r="A85" s="9">
         <v>24988445</v>
       </c>
@@ -80541,7 +80553,7 @@
       <c r="FI85" s="1"/>
       <c r="FJ85" s="1"/>
     </row>
-    <row r="86" spans="1:166" ht="15">
+    <row r="86" spans="1:168" ht="15">
       <c r="A86" s="9">
         <v>24988559</v>
       </c>
@@ -80675,7 +80687,7 @@
       <c r="FI86" s="1"/>
       <c r="FJ86" s="1"/>
     </row>
-    <row r="87" spans="1:166" ht="15">
+    <row r="87" spans="1:168" ht="15">
       <c r="A87" s="9">
         <v>24988692</v>
       </c>
@@ -80809,7 +80821,7 @@
       <c r="FI87" s="1"/>
       <c r="FJ87" s="1"/>
     </row>
-    <row r="88" spans="1:166" ht="15">
+    <row r="88" spans="1:168" ht="15">
       <c r="A88" s="9">
         <v>24923318</v>
       </c>
@@ -80966,8 +80978,11 @@
         <v>24</v>
       </c>
       <c r="FJ88" s="1"/>
+      <c r="FL88" s="4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="89" spans="1:166" ht="15">
+    <row r="89" spans="1:168" ht="15">
       <c r="A89" s="9">
         <v>24925212</v>
       </c>
@@ -81101,7 +81116,7 @@
       <c r="FI89" s="1"/>
       <c r="FJ89" s="1"/>
     </row>
-    <row r="90" spans="1:166" ht="15">
+    <row r="90" spans="1:168" ht="15">
       <c r="A90" s="9">
         <v>24857462</v>
       </c>
@@ -81235,7 +81250,7 @@
       <c r="FI90" s="1"/>
       <c r="FJ90" s="1"/>
     </row>
-    <row r="91" spans="1:166" ht="15">
+    <row r="91" spans="1:168" ht="15">
       <c r="A91" s="10">
         <v>25112301</v>
       </c>
@@ -81257,8 +81272,11 @@
       <c r="FI91" s="4">
         <v>11</v>
       </c>
+      <c r="FL91" s="4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="92" spans="1:166" ht="15">
+    <row r="92" spans="1:168" ht="15">
       <c r="A92" s="10">
         <v>25112300</v>
       </c>
@@ -81280,8 +81298,11 @@
       <c r="FI92" s="4">
         <v>11</v>
       </c>
+      <c r="FL92" s="4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="93" spans="1:166" ht="15">
+    <row r="93" spans="1:168" ht="15">
       <c r="A93" s="10">
         <v>25087863</v>
       </c>
@@ -81303,8 +81324,11 @@
       <c r="FI93" s="4">
         <v>11</v>
       </c>
+      <c r="FL93" s="4">
+        <v>14</v>
+      </c>
     </row>
-    <row r="94" spans="1:166" ht="15">
+    <row r="94" spans="1:168" ht="15">
       <c r="A94" s="10">
         <v>25087787</v>
       </c>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun  4 09:39:52 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C41E3173-2EE3-4D88-9F4A-2FD057296C21}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3446F075-04C5-4BF2-A518-5E43CF2FF986}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -855,8 +855,8 @@
   <dimension ref="A1:XFD94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FG42" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FL52" sqref="FL52"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FH82" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FO91" sqref="FO91"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -72453,7 +72453,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:168" ht="15">
+    <row r="33" spans="1:169" ht="15">
       <c r="A33" s="9">
         <v>24636088</v>
       </c>
@@ -72602,7 +72602,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:168" ht="15">
+    <row r="34" spans="1:169" ht="15">
       <c r="A34" s="9">
         <v>24636089</v>
       </c>
@@ -72751,7 +72751,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:168" ht="15">
+    <row r="35" spans="1:169" ht="15">
       <c r="A35" s="9">
         <v>24636092</v>
       </c>
@@ -72887,7 +72887,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:168" ht="15">
+    <row r="36" spans="1:169" ht="15">
       <c r="A36" s="9">
         <v>24395952</v>
       </c>
@@ -73021,7 +73021,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:168" ht="15">
+    <row r="37" spans="1:169" ht="15">
       <c r="A37" s="9">
         <v>24395977</v>
       </c>
@@ -73155,7 +73155,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:168" ht="15">
+    <row r="38" spans="1:169" ht="15">
       <c r="A38" s="9">
         <v>24395942</v>
       </c>
@@ -73289,7 +73289,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:168" ht="15">
+    <row r="39" spans="1:169" ht="15">
       <c r="A39" s="12">
         <v>24567303</v>
       </c>
@@ -73452,7 +73452,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:168" ht="15">
+    <row r="40" spans="1:169" ht="15">
       <c r="A40" s="12">
         <v>24567296</v>
       </c>
@@ -73615,7 +73615,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:168" ht="15">
+    <row r="41" spans="1:169" ht="15">
       <c r="A41" s="12">
         <v>24567289</v>
       </c>
@@ -73778,7 +73778,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:168" ht="15">
+    <row r="42" spans="1:169" ht="15">
       <c r="A42" s="12">
         <v>24567319</v>
       </c>
@@ -73941,7 +73941,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:168" ht="15">
+    <row r="43" spans="1:169" ht="15">
       <c r="A43" s="12">
         <v>24567277</v>
       </c>
@@ -74104,7 +74104,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:168" ht="15">
+    <row r="44" spans="1:169" ht="15">
       <c r="A44" s="12">
         <v>24567774</v>
       </c>
@@ -74267,7 +74267,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:168" ht="15">
+    <row r="45" spans="1:169" ht="15">
       <c r="A45" s="12">
         <v>24567851</v>
       </c>
@@ -74430,7 +74430,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:168" ht="15">
+    <row r="46" spans="1:169" ht="15">
       <c r="A46" s="12">
         <v>24559501</v>
       </c>
@@ -74593,7 +74593,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:168" ht="15">
+    <row r="47" spans="1:169" ht="15">
       <c r="A47" s="12">
         <v>24567303</v>
       </c>
@@ -74727,7 +74727,7 @@
       <c r="FI47" s="1"/>
       <c r="FJ47" s="1"/>
     </row>
-    <row r="48" spans="1:168" ht="15">
+    <row r="48" spans="1:169" ht="15">
       <c r="A48" s="12">
         <v>24567296</v>
       </c>
@@ -74928,14 +74928,22 @@
         <v>24</v>
       </c>
       <c r="FI48" s="1">
-        <v>10</v>
-      </c>
-      <c r="FJ48" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="FJ48" s="1">
+        <v>8</v>
+      </c>
+      <c r="FK48" s="4">
+        <v>14</v>
+      </c>
       <c r="FL48" s="4">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="FM48" s="4">
+        <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:168" ht="15">
+    <row r="49" spans="1:169" ht="15">
       <c r="A49" s="12">
         <v>24567289</v>
       </c>
@@ -75069,7 +75077,7 @@
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
     </row>
-    <row r="50" spans="1:168" ht="15">
+    <row r="50" spans="1:169" ht="15">
       <c r="A50" s="12">
         <v>24567319</v>
       </c>
@@ -75270,14 +75278,22 @@
         <v>24</v>
       </c>
       <c r="FI50" s="1">
-        <v>10</v>
-      </c>
-      <c r="FJ50" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="FJ50" s="1">
+        <v>8</v>
+      </c>
+      <c r="FK50" s="4">
+        <v>14</v>
+      </c>
       <c r="FL50" s="4">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="FM50" s="4">
+        <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:168" ht="15">
+    <row r="51" spans="1:169" ht="15">
       <c r="A51" s="12">
         <v>24567277</v>
       </c>
@@ -75478,14 +75494,22 @@
         <v>24</v>
       </c>
       <c r="FI51" s="1">
-        <v>10</v>
-      </c>
-      <c r="FJ51" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="FJ51" s="1">
+        <v>8</v>
+      </c>
+      <c r="FK51" s="4">
+        <v>14</v>
+      </c>
       <c r="FL51" s="4">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="FM51" s="4">
+        <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:168" ht="15">
+    <row r="52" spans="1:169" ht="15">
       <c r="A52" s="12">
         <v>24567774</v>
       </c>
@@ -75686,14 +75710,22 @@
         <v>24</v>
       </c>
       <c r="FI52" s="1">
-        <v>10</v>
-      </c>
-      <c r="FJ52" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="FJ52" s="1">
+        <v>8</v>
+      </c>
+      <c r="FK52" s="4">
+        <v>14</v>
+      </c>
       <c r="FL52" s="4">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="FM52" s="4">
+        <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:168" ht="15">
+    <row r="53" spans="1:169" ht="15">
       <c r="A53" s="12">
         <v>24567851</v>
       </c>
@@ -75827,7 +75859,7 @@
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
     </row>
-    <row r="54" spans="1:168" ht="15">
+    <row r="54" spans="1:169" ht="15">
       <c r="A54" s="12">
         <v>24559501</v>
       </c>
@@ -75961,7 +75993,7 @@
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
     </row>
-    <row r="55" spans="1:168" ht="15">
+    <row r="55" spans="1:169" ht="15">
       <c r="A55" s="9">
         <v>24079686</v>
       </c>
@@ -76149,7 +76181,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:168" ht="15">
+    <row r="56" spans="1:169" ht="15">
       <c r="A56" s="9">
         <v>24079692</v>
       </c>
@@ -76337,7 +76369,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:168" ht="15">
+    <row r="57" spans="1:169" ht="15">
       <c r="A57" s="9">
         <v>24636092</v>
       </c>
@@ -76491,7 +76523,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:168" ht="15">
+    <row r="58" spans="1:169" ht="15">
       <c r="A58" s="9">
         <v>24793376</v>
       </c>
@@ -76647,7 +76679,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:168" ht="15">
+    <row r="59" spans="1:169" ht="15">
       <c r="A59" s="9">
         <v>24713456</v>
       </c>
@@ -76801,7 +76833,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:168" ht="15">
+    <row r="60" spans="1:169" ht="15">
       <c r="A60" s="9">
         <v>24713371</v>
       </c>
@@ -76947,7 +76979,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:168" ht="15">
+    <row r="61" spans="1:169" ht="15">
       <c r="A61" s="9">
         <v>24713222</v>
       </c>
@@ -77105,7 +77137,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:168" ht="15">
+    <row r="62" spans="1:169" ht="15">
       <c r="A62" s="12">
         <v>24636087</v>
       </c>
@@ -77241,7 +77273,7 @@
       <c r="FI62" s="1"/>
       <c r="FJ62" s="1"/>
     </row>
-    <row r="63" spans="1:168" ht="15">
+    <row r="63" spans="1:169" ht="15">
       <c r="A63" s="9">
         <v>24636090</v>
       </c>
@@ -77377,7 +77409,7 @@
       <c r="FI63" s="1"/>
       <c r="FJ63" s="1"/>
     </row>
-    <row r="64" spans="1:168" ht="15">
+    <row r="64" spans="1:169" ht="15">
       <c r="A64" s="9">
         <v>24636091</v>
       </c>
@@ -77513,7 +77545,7 @@
       <c r="FI64" s="1"/>
       <c r="FJ64" s="1"/>
     </row>
-    <row r="65" spans="1:166" ht="15">
+    <row r="65" spans="1:170" ht="15">
       <c r="A65" s="9">
         <v>24636089</v>
       </c>
@@ -77657,7 +77689,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:166" ht="15">
+    <row r="66" spans="1:170" ht="15">
       <c r="A66" s="9">
         <v>24636088</v>
       </c>
@@ -77801,7 +77833,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:166" ht="15">
+    <row r="67" spans="1:170" ht="15">
       <c r="A67" s="9">
         <v>25017935</v>
       </c>
@@ -77935,7 +77967,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:166" ht="15">
+    <row r="68" spans="1:170" ht="15">
       <c r="A68" s="9">
         <v>25017936</v>
       </c>
@@ -78082,7 +78114,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:166" ht="15">
+    <row r="69" spans="1:170" ht="15">
       <c r="A69" s="9">
         <v>25017937</v>
       </c>
@@ -78216,7 +78248,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:166" ht="15">
+    <row r="70" spans="1:170" ht="15">
       <c r="A70" s="9">
         <v>25019644</v>
       </c>
@@ -78350,7 +78382,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:166" ht="15">
+    <row r="71" spans="1:170" ht="15">
       <c r="A71" s="9">
         <v>25019645</v>
       </c>
@@ -78497,7 +78529,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:166" ht="15">
+    <row r="72" spans="1:170" ht="15">
       <c r="A72" s="9">
         <v>25019646</v>
       </c>
@@ -78631,7 +78663,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:166" ht="15">
+    <row r="73" spans="1:170" ht="15">
       <c r="A73" s="9">
         <v>24848800</v>
       </c>
@@ -78853,9 +78885,23 @@
       <c r="FI73" s="1">
         <v>24</v>
       </c>
-      <c r="FJ73" s="1"/>
+      <c r="FJ73" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK73" s="4">
+        <v>8</v>
+      </c>
+      <c r="FL73" s="4">
+        <v>14</v>
+      </c>
+      <c r="FM73" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN73" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="74" spans="1:166" ht="15">
+    <row r="74" spans="1:170" ht="15">
       <c r="A74" s="9">
         <v>24859051</v>
       </c>
@@ -79077,9 +79123,23 @@
       <c r="FI74" s="1">
         <v>24</v>
       </c>
-      <c r="FJ74" s="1"/>
+      <c r="FJ74" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK74" s="4">
+        <v>8</v>
+      </c>
+      <c r="FL74" s="4">
+        <v>14</v>
+      </c>
+      <c r="FM74" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN74" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="75" spans="1:166" ht="15">
+    <row r="75" spans="1:170" ht="15">
       <c r="A75" s="9">
         <v>24848800</v>
       </c>
@@ -79213,7 +79273,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:166" ht="15">
+    <row r="76" spans="1:170" ht="15">
       <c r="A76" s="9">
         <v>24859051</v>
       </c>
@@ -79347,7 +79407,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:166" ht="15">
+    <row r="77" spans="1:170" ht="15">
       <c r="A77" s="9">
         <v>24848800</v>
       </c>
@@ -79481,7 +79541,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:166" ht="15">
+    <row r="78" spans="1:170" ht="15">
       <c r="A78" s="9">
         <v>24859051</v>
       </c>
@@ -79615,7 +79675,7 @@
       <c r="FI78" s="1"/>
       <c r="FJ78" s="1"/>
     </row>
-    <row r="79" spans="1:166" ht="15">
+    <row r="79" spans="1:170" ht="15">
       <c r="A79" s="9">
         <v>24848800</v>
       </c>
@@ -79749,7 +79809,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:166" ht="15">
+    <row r="80" spans="1:170" ht="15">
       <c r="A80" s="9">
         <v>24859051</v>
       </c>
@@ -79883,7 +79943,7 @@
       <c r="FI80" s="1"/>
       <c r="FJ80" s="1"/>
     </row>
-    <row r="81" spans="1:168" ht="15">
+    <row r="81" spans="1:170" ht="15">
       <c r="A81" s="9">
         <v>24848800</v>
       </c>
@@ -80017,7 +80077,7 @@
       <c r="FI81" s="1"/>
       <c r="FJ81" s="1"/>
     </row>
-    <row r="82" spans="1:168" ht="15">
+    <row r="82" spans="1:170" ht="15">
       <c r="A82" s="9">
         <v>24859051</v>
       </c>
@@ -80151,7 +80211,7 @@
       <c r="FI82" s="1"/>
       <c r="FJ82" s="1"/>
     </row>
-    <row r="83" spans="1:168" ht="15">
+    <row r="83" spans="1:170" ht="15">
       <c r="A83" s="9">
         <v>24848800</v>
       </c>
@@ -80285,7 +80345,7 @@
       <c r="FI83" s="1"/>
       <c r="FJ83" s="1"/>
     </row>
-    <row r="84" spans="1:168" ht="15">
+    <row r="84" spans="1:170" ht="15">
       <c r="A84" s="9">
         <v>24859051</v>
       </c>
@@ -80419,7 +80479,7 @@
       <c r="FI84" s="1"/>
       <c r="FJ84" s="1"/>
     </row>
-    <row r="85" spans="1:168" ht="15">
+    <row r="85" spans="1:170" ht="15">
       <c r="A85" s="9">
         <v>24988445</v>
       </c>
@@ -80553,7 +80613,7 @@
       <c r="FI85" s="1"/>
       <c r="FJ85" s="1"/>
     </row>
-    <row r="86" spans="1:168" ht="15">
+    <row r="86" spans="1:170" ht="15">
       <c r="A86" s="9">
         <v>24988559</v>
       </c>
@@ -80687,7 +80747,7 @@
       <c r="FI86" s="1"/>
       <c r="FJ86" s="1"/>
     </row>
-    <row r="87" spans="1:168" ht="15">
+    <row r="87" spans="1:170" ht="15">
       <c r="A87" s="9">
         <v>24988692</v>
       </c>
@@ -80821,7 +80881,7 @@
       <c r="FI87" s="1"/>
       <c r="FJ87" s="1"/>
     </row>
-    <row r="88" spans="1:168" ht="15">
+    <row r="88" spans="1:170" ht="15">
       <c r="A88" s="9">
         <v>24923318</v>
       </c>
@@ -80977,12 +81037,23 @@
       <c r="FI88" s="1">
         <v>24</v>
       </c>
-      <c r="FJ88" s="1"/>
+      <c r="FJ88" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK88" s="4">
+        <v>8</v>
+      </c>
       <c r="FL88" s="4">
         <v>14</v>
       </c>
+      <c r="FM88" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN88" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="89" spans="1:168" ht="15">
+    <row r="89" spans="1:170" ht="15">
       <c r="A89" s="9">
         <v>24925212</v>
       </c>
@@ -81116,7 +81187,7 @@
       <c r="FI89" s="1"/>
       <c r="FJ89" s="1"/>
     </row>
-    <row r="90" spans="1:168" ht="15">
+    <row r="90" spans="1:170" ht="15">
       <c r="A90" s="9">
         <v>24857462</v>
       </c>
@@ -81250,7 +81321,7 @@
       <c r="FI90" s="1"/>
       <c r="FJ90" s="1"/>
     </row>
-    <row r="91" spans="1:168" ht="15">
+    <row r="91" spans="1:170" ht="15">
       <c r="A91" s="10">
         <v>25112301</v>
       </c>
@@ -81272,11 +81343,23 @@
       <c r="FI91" s="4">
         <v>11</v>
       </c>
+      <c r="FJ91" s="4">
+        <v>24</v>
+      </c>
+      <c r="FK91" s="4">
+        <v>8</v>
+      </c>
       <c r="FL91" s="4">
         <v>14</v>
       </c>
+      <c r="FM91" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN91" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="92" spans="1:168" ht="15">
+    <row r="92" spans="1:170" ht="15">
       <c r="A92" s="10">
         <v>25112300</v>
       </c>
@@ -81298,11 +81381,23 @@
       <c r="FI92" s="4">
         <v>11</v>
       </c>
+      <c r="FJ92" s="4">
+        <v>24</v>
+      </c>
+      <c r="FK92" s="4">
+        <v>8</v>
+      </c>
       <c r="FL92" s="4">
         <v>14</v>
       </c>
+      <c r="FM92" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN92" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="93" spans="1:168" ht="15">
+    <row r="93" spans="1:170" ht="15">
       <c r="A93" s="10">
         <v>25087863</v>
       </c>
@@ -81324,11 +81419,23 @@
       <c r="FI93" s="4">
         <v>11</v>
       </c>
+      <c r="FJ93" s="4">
+        <v>24</v>
+      </c>
+      <c r="FK93" s="4">
+        <v>8</v>
+      </c>
       <c r="FL93" s="4">
         <v>14</v>
       </c>
+      <c r="FM93" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN93" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="94" spans="1:168" ht="15">
+    <row r="94" spans="1:170" ht="15">
       <c r="A94" s="10">
         <v>25087787</v>
       </c>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun  4 11:36:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3446F075-04C5-4BF2-A518-5E43CF2FF986}"/>
+  <xr:revisionPtr revIDLastSave="354" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5FADF30-1555-4C46-8169-0E6823772994}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="132">
   <si>
     <t>Module ID</t>
   </si>
@@ -374,10 +374,13 @@
     <t>VSL202526033</t>
   </si>
   <si>
-    <t>Toyo Cell (TOPCon) evaluation</t>
+    <t>Toyo Cell (TOPCon) evaluation : 2 times</t>
   </si>
   <si>
     <t>VSL202526032</t>
+  </si>
+  <si>
+    <t>Toyo Cell (TOPCon) evaluation</t>
   </si>
   <si>
     <t>VSL202526010</t>
@@ -388,15 +391,59 @@
   <si>
     <t>VSL202526009</t>
   </si>
+  <si>
+    <t>VSL202425374</t>
+  </si>
+  <si>
+    <t>VSL202526035</t>
+  </si>
+  <si>
+    <t>SemCorp G2B Module Failure Analysis</t>
+  </si>
+  <si>
+    <t>VSL202526030</t>
+  </si>
+  <si>
+    <t>Bbetter Low GSM Trial (420F,400B)</t>
+  </si>
+  <si>
+    <t>VSL202526023</t>
+  </si>
+  <si>
+    <t>Cybrid Low GSM Trial (420F,400B)</t>
+  </si>
+  <si>
+    <t>VSL202526021</t>
+  </si>
+  <si>
+    <t>VSL202526028</t>
+  </si>
+  <si>
+    <t>VSL202526031</t>
+  </si>
+  <si>
+    <t>VSL202526016</t>
+  </si>
+  <si>
+    <t>IPQC Module (SML+DML+TC50+HF10)</t>
+  </si>
+  <si>
+    <t>VSL202526015</t>
+  </si>
+  <si>
+    <t>IPQC Yellow Spot on Ribbon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="165" formatCode="&quot;VSL&quot;#"/>
+    <numFmt numFmtId="166" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,6 +490,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -458,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -481,11 +534,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -518,11 +586,48 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -852,11 +957,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD94"/>
+  <dimension ref="A1:XFD113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FH82" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FO91" sqref="FO91"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FI89" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FK105" sqref="FK105"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -67287,7 +67392,9 @@
       <c r="F4" s="13">
         <v>45692</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="P4" s="3">
+        <v>45745</v>
+      </c>
       <c r="AY4" s="1">
         <v>18</v>
       </c>
@@ -67532,7 +67639,9 @@
       <c r="F5" s="13">
         <v>45692</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="3">
+        <v>45745</v>
+      </c>
       <c r="AY5" s="1">
         <v>18</v>
       </c>
@@ -72453,7 +72562,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:169" ht="15">
+    <row r="33" spans="1:170" ht="15">
       <c r="A33" s="9">
         <v>24636088</v>
       </c>
@@ -72602,7 +72711,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:169" ht="15">
+    <row r="34" spans="1:170" ht="15">
       <c r="A34" s="9">
         <v>24636089</v>
       </c>
@@ -72751,7 +72860,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:169" ht="15">
+    <row r="35" spans="1:170" ht="15">
       <c r="A35" s="9">
         <v>24636092</v>
       </c>
@@ -72887,7 +72996,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:169" ht="15">
+    <row r="36" spans="1:170" ht="15">
       <c r="A36" s="9">
         <v>24395952</v>
       </c>
@@ -73021,7 +73130,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:169" ht="15">
+    <row r="37" spans="1:170" ht="15">
       <c r="A37" s="9">
         <v>24395977</v>
       </c>
@@ -73155,7 +73264,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:169" ht="15">
+    <row r="38" spans="1:170" ht="15">
       <c r="A38" s="9">
         <v>24395942</v>
       </c>
@@ -73289,7 +73398,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:169" ht="15">
+    <row r="39" spans="1:170" ht="15">
       <c r="A39" s="12">
         <v>24567303</v>
       </c>
@@ -73452,7 +73561,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:169" ht="15">
+    <row r="40" spans="1:170" ht="15">
       <c r="A40" s="12">
         <v>24567296</v>
       </c>
@@ -73615,7 +73724,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:169" ht="15">
+    <row r="41" spans="1:170" ht="15">
       <c r="A41" s="12">
         <v>24567289</v>
       </c>
@@ -73778,7 +73887,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:169" ht="15">
+    <row r="42" spans="1:170" ht="15">
       <c r="A42" s="12">
         <v>24567319</v>
       </c>
@@ -73941,7 +74050,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:169" ht="15">
+    <row r="43" spans="1:170" ht="15">
       <c r="A43" s="12">
         <v>24567277</v>
       </c>
@@ -74104,7 +74213,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:169" ht="15">
+    <row r="44" spans="1:170" ht="15">
       <c r="A44" s="12">
         <v>24567774</v>
       </c>
@@ -74267,7 +74376,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:169" ht="15">
+    <row r="45" spans="1:170" ht="15">
       <c r="A45" s="12">
         <v>24567851</v>
       </c>
@@ -74430,7 +74539,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:169" ht="15">
+    <row r="46" spans="1:170" ht="15">
       <c r="A46" s="12">
         <v>24559501</v>
       </c>
@@ -74593,7 +74702,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:169" ht="15">
+    <row r="47" spans="1:170" ht="15">
       <c r="A47" s="12">
         <v>24567303</v>
       </c>
@@ -74727,7 +74836,7 @@
       <c r="FI47" s="1"/>
       <c r="FJ47" s="1"/>
     </row>
-    <row r="48" spans="1:169" ht="15">
+    <row r="48" spans="1:170" ht="15">
       <c r="A48" s="12">
         <v>24567296</v>
       </c>
@@ -74942,8 +75051,11 @@
       <c r="FM48" s="4">
         <v>24</v>
       </c>
+      <c r="FN48" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="49" spans="1:169" ht="15">
+    <row r="49" spans="1:170" ht="15">
       <c r="A49" s="12">
         <v>24567289</v>
       </c>
@@ -75077,7 +75189,7 @@
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
     </row>
-    <row r="50" spans="1:169" ht="15">
+    <row r="50" spans="1:170" ht="15">
       <c r="A50" s="12">
         <v>24567319</v>
       </c>
@@ -75292,8 +75404,11 @@
       <c r="FM50" s="4">
         <v>24</v>
       </c>
+      <c r="FN50" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="51" spans="1:169" ht="15">
+    <row r="51" spans="1:170" ht="15">
       <c r="A51" s="12">
         <v>24567277</v>
       </c>
@@ -75508,8 +75623,11 @@
       <c r="FM51" s="4">
         <v>24</v>
       </c>
+      <c r="FN51" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="52" spans="1:169" ht="15">
+    <row r="52" spans="1:170" ht="15">
       <c r="A52" s="12">
         <v>24567774</v>
       </c>
@@ -75724,8 +75842,11 @@
       <c r="FM52" s="4">
         <v>24</v>
       </c>
+      <c r="FN52" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="53" spans="1:169" ht="15">
+    <row r="53" spans="1:170" ht="15">
       <c r="A53" s="12">
         <v>24567851</v>
       </c>
@@ -75859,7 +75980,7 @@
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
     </row>
-    <row r="54" spans="1:169" ht="15">
+    <row r="54" spans="1:170" ht="15">
       <c r="A54" s="12">
         <v>24559501</v>
       </c>
@@ -75993,7 +76114,7 @@
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
     </row>
-    <row r="55" spans="1:169" ht="15">
+    <row r="55" spans="1:170" ht="15">
       <c r="A55" s="9">
         <v>24079686</v>
       </c>
@@ -76181,7 +76302,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:169" ht="15">
+    <row r="56" spans="1:170" ht="15">
       <c r="A56" s="9">
         <v>24079692</v>
       </c>
@@ -76369,7 +76490,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:169" ht="15">
+    <row r="57" spans="1:170" ht="15">
       <c r="A57" s="9">
         <v>24636092</v>
       </c>
@@ -76523,7 +76644,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:169" ht="15">
+    <row r="58" spans="1:170" ht="15">
       <c r="A58" s="9">
         <v>24793376</v>
       </c>
@@ -76679,7 +76800,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:169" ht="15">
+    <row r="59" spans="1:170" ht="15">
       <c r="A59" s="9">
         <v>24713456</v>
       </c>
@@ -76833,7 +76954,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:169" ht="15">
+    <row r="60" spans="1:170" ht="15">
       <c r="A60" s="9">
         <v>24713371</v>
       </c>
@@ -76979,7 +77100,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:169" ht="15">
+    <row r="61" spans="1:170" ht="15">
       <c r="A61" s="9">
         <v>24713222</v>
       </c>
@@ -77137,7 +77258,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:169" ht="15">
+    <row r="62" spans="1:170" ht="15">
       <c r="A62" s="12">
         <v>24636087</v>
       </c>
@@ -77273,7 +77394,7 @@
       <c r="FI62" s="1"/>
       <c r="FJ62" s="1"/>
     </row>
-    <row r="63" spans="1:169" ht="15">
+    <row r="63" spans="1:170" ht="15">
       <c r="A63" s="9">
         <v>24636090</v>
       </c>
@@ -77409,7 +77530,7 @@
       <c r="FI63" s="1"/>
       <c r="FJ63" s="1"/>
     </row>
-    <row r="64" spans="1:169" ht="15">
+    <row r="64" spans="1:170" ht="15">
       <c r="A64" s="9">
         <v>24636091</v>
       </c>
@@ -81201,9 +81322,11 @@
         <v>21</v>
       </c>
       <c r="E90" s="9">
-        <v>50</v>
-      </c>
-      <c r="F90" s="13"/>
+        <v>200</v>
+      </c>
+      <c r="F90" s="13">
+        <v>45792</v>
+      </c>
       <c r="AY90" s="1"/>
       <c r="AZ90" s="1"/>
       <c r="BA90" s="1"/>
@@ -81304,22 +81427,66 @@
       <c r="ER90" s="1"/>
       <c r="ES90" s="1"/>
       <c r="ET90" s="1"/>
-      <c r="EU90" s="1"/>
-      <c r="EV90" s="1"/>
-      <c r="EW90" s="1"/>
-      <c r="EX90" s="1"/>
-      <c r="EY90" s="1"/>
-      <c r="EZ90" s="1"/>
-      <c r="FA90" s="1"/>
-      <c r="FB90" s="1"/>
-      <c r="FC90" s="1"/>
-      <c r="FD90" s="1"/>
-      <c r="FE90" s="1"/>
-      <c r="FF90" s="1"/>
-      <c r="FG90" s="1"/>
-      <c r="FH90" s="1"/>
-      <c r="FI90" s="1"/>
-      <c r="FJ90" s="1"/>
+      <c r="EU90" s="1">
+        <v>8</v>
+      </c>
+      <c r="EV90" s="1">
+        <v>12</v>
+      </c>
+      <c r="EW90" s="1">
+        <v>12</v>
+      </c>
+      <c r="EX90" s="1">
+        <v>12</v>
+      </c>
+      <c r="EY90" s="1">
+        <v>12</v>
+      </c>
+      <c r="EZ90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FA90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FB90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FC90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FD90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FE90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FF90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FG90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FH90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FI90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FJ90" s="1">
+        <v>12</v>
+      </c>
+      <c r="FK90" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FL90" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FM90" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FN90" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="91" spans="1:170" ht="15">
       <c r="A91" s="10">
@@ -81328,7 +81495,7 @@
       <c r="B91" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="18" t="s">
         <v>112</v>
       </c>
       <c r="D91" s="10" t="s">
@@ -81339,6 +81506,9 @@
       </c>
       <c r="F91" s="14">
         <v>45806</v>
+      </c>
+      <c r="P91" s="3">
+        <v>45811</v>
       </c>
       <c r="FI91" s="4">
         <v>11</v>
@@ -81367,7 +81537,7 @@
         <v>113</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D92" s="10" t="s">
         <v>28</v>
@@ -81402,10 +81572,10 @@
         <v>25087863</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D93" s="10" t="s">
         <v>18</v>
@@ -81415,6 +81585,9 @@
       </c>
       <c r="F93" s="14">
         <v>45806</v>
+      </c>
+      <c r="P93" s="3">
+        <v>45811</v>
       </c>
       <c r="FI93" s="4">
         <v>11</v>
@@ -81440,10 +81613,10 @@
         <v>25087787</v>
       </c>
       <c r="B94" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="D94" s="10" t="s">
         <v>28</v>
@@ -81451,14 +81624,634 @@
       <c r="E94" s="10">
         <v>1000</v>
       </c>
+    </row>
+    <row r="95" spans="1:170" ht="15">
+      <c r="A95" s="10">
+        <v>24848184</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E95" s="9">
+        <v>200</v>
+      </c>
+      <c r="F95" s="13">
+        <v>45792</v>
+      </c>
+      <c r="EU95" s="4">
+        <v>8</v>
+      </c>
+      <c r="EV95" s="4">
+        <v>12</v>
+      </c>
+      <c r="EW95" s="4">
+        <v>12</v>
+      </c>
+      <c r="EX95" s="4">
+        <v>12</v>
+      </c>
+      <c r="EY95" s="4">
+        <v>12</v>
+      </c>
+      <c r="EZ95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FA95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FB95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FC95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FD95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FE95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FF95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FG95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FH95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FI95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FJ95" s="4">
+        <v>12</v>
+      </c>
+      <c r="FK95" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FL95" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FM95" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FN95" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:170" s="4" customFormat="1" ht="15">
+      <c r="A96" s="16">
+        <v>50872159</v>
+      </c>
+      <c r="B96" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E96" s="16">
+        <v>192</v>
+      </c>
+      <c r="F96" s="19">
+        <v>45793</v>
+      </c>
+      <c r="P96" s="3"/>
+    </row>
+    <row r="97" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A97" s="16">
+        <v>25019645</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" s="16">
+        <v>96</v>
+      </c>
+      <c r="F97" s="19"/>
+      <c r="P97" s="3"/>
+    </row>
+    <row r="98" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A98" s="16">
+        <v>25017936</v>
+      </c>
+      <c r="B98" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" s="16">
+        <v>96</v>
+      </c>
+      <c r="F98" s="19"/>
+      <c r="P98" s="3"/>
+    </row>
+    <row r="99" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A99" s="16">
+        <v>25089372</v>
+      </c>
+      <c r="B99" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E99" s="16">
+        <v>60</v>
+      </c>
+      <c r="F99" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P99" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ99" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK99" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A100" s="16">
+        <v>25089365</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E100" s="16">
+        <v>60</v>
+      </c>
+      <c r="F100" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P100" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ100" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK100" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A101" s="16">
+        <v>25089363</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E101" s="16">
+        <v>60</v>
+      </c>
+      <c r="F101" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P101" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ101" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK101" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A102" s="16">
+        <v>25089370</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D102" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E102" s="16">
+        <v>60</v>
+      </c>
+      <c r="F102" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P102" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ102" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK102" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A103" s="16">
+        <v>25112299</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E103" s="16">
+        <v>60</v>
+      </c>
+      <c r="F103" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P103" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ103" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK103" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A104" s="16">
+        <v>72149637</v>
+      </c>
+      <c r="B104" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E104" s="16">
+        <v>50</v>
+      </c>
+      <c r="F104" s="19">
+        <v>45796</v>
+      </c>
+      <c r="P104" s="3">
+        <v>45806</v>
+      </c>
+      <c r="FI104" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A105" s="16">
+        <v>72238923</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E105" s="16">
+        <v>1000</v>
+      </c>
+      <c r="F105" s="19"/>
+      <c r="P105" s="3"/>
+    </row>
+    <row r="106" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A106" s="16">
+        <v>25089372</v>
+      </c>
+      <c r="B106" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D106" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" s="16">
+        <v>96</v>
+      </c>
+      <c r="F106" s="19"/>
+      <c r="P106" s="3"/>
+    </row>
+    <row r="107" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A107" s="16">
+        <v>25089365</v>
+      </c>
+      <c r="B107" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E107" s="16">
+        <v>96</v>
+      </c>
+      <c r="F107" s="19"/>
+      <c r="P107" s="3"/>
+    </row>
+    <row r="108" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A108" s="16">
+        <v>25089363</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108" s="16">
+        <v>1000</v>
+      </c>
+      <c r="F108" s="19"/>
+      <c r="P108" s="3"/>
+    </row>
+    <row r="109" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A109" s="16">
+        <v>25089370</v>
+      </c>
+      <c r="B109" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E109" s="16">
+        <v>1000</v>
+      </c>
+      <c r="F109" s="19"/>
+      <c r="P109" s="3"/>
+    </row>
+    <row r="110" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A110" s="16">
+        <v>25112301</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C110" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" s="16">
+        <v>96</v>
+      </c>
+      <c r="F110" s="19"/>
+      <c r="P110" s="3"/>
+    </row>
+    <row r="111" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A111" s="16">
+        <v>25112300</v>
+      </c>
+      <c r="B111" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C111" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E111" s="16">
+        <v>1000</v>
+      </c>
+      <c r="F111" s="19"/>
+      <c r="P111" s="3"/>
+    </row>
+    <row r="112" spans="1:167" s="4" customFormat="1" ht="15">
+      <c r="A112" s="10"/>
+      <c r="B112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="14"/>
+      <c r="P112" s="3"/>
+    </row>
+    <row r="113" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A113" s="10"/>
+      <c r="B113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="14"/>
+      <c r="P113" s="3"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="F1:F1048576" name="Range1"/>
     <protectedRange sqref="P1:P1048576" name="Range2"/>
-    <protectedRange sqref="Q1:XFD1048576" name="Range3"/>
+    <protectedRange sqref="A95 Q1:XFD1048576" name="Range3"/>
   </protectedRanges>
+  <conditionalFormatting sqref="A96:A100 A102:A111">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A101">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D96:D111" xr:uid="{AE741107-2DDE-448F-B66D-3CC4D6043D49}">
+      <formula1>"LID,PID,TC,DH,HF,LETID,"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun  4 13:48:55 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="354" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5FADF30-1555-4C46-8169-0E6823772994}"/>
+  <xr:revisionPtr revIDLastSave="422" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62CB8486-5111-4AF7-BEFF-BFDE278027F4}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="132">
   <si>
     <t>Module ID</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>DH</t>
+  </si>
+  <si>
+    <t>off</t>
   </si>
   <si>
     <t>VSL202425323</t>
@@ -330,9 +333,6 @@
   </si>
   <si>
     <t>QC SOLAR BLK DIODE 2.0</t>
-  </si>
-  <si>
-    <t>off</t>
   </si>
   <si>
     <t>VSL202425377</t>
@@ -960,8 +960,8 @@
   <dimension ref="A1:XFD113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FI89" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FK105" sqref="FK105"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="EA6" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="EG8" sqref="EG8:EG9"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -68247,61 +68247,259 @@
       <c r="DN8" s="1">
         <v>24</v>
       </c>
-      <c r="DO8" s="1"/>
-      <c r="DP8" s="1"/>
-      <c r="DQ8" s="1"/>
-      <c r="DR8" s="1"/>
-      <c r="DS8" s="1"/>
-      <c r="DT8" s="1"/>
-      <c r="DU8" s="1"/>
-      <c r="DV8" s="1"/>
-      <c r="DW8" s="1"/>
-      <c r="DX8" s="1"/>
-      <c r="DY8" s="1"/>
-      <c r="DZ8" s="1"/>
-      <c r="EA8" s="1"/>
-      <c r="EB8" s="1"/>
-      <c r="EC8" s="1"/>
-      <c r="ED8" s="1"/>
-      <c r="EE8" s="1"/>
-      <c r="EF8" s="1"/>
-      <c r="EG8" s="1"/>
-      <c r="EH8" s="1"/>
-      <c r="EI8" s="1"/>
-      <c r="EJ8" s="1"/>
-      <c r="EK8" s="1"/>
-      <c r="EL8" s="1"/>
-      <c r="EM8" s="1"/>
-      <c r="EN8" s="1"/>
-      <c r="EO8" s="1"/>
-      <c r="EP8" s="1"/>
-      <c r="EQ8" s="1"/>
-      <c r="ER8" s="1"/>
-      <c r="ES8" s="1"/>
-      <c r="ET8" s="1"/>
-      <c r="EU8" s="1"/>
-      <c r="EV8" s="1"/>
-      <c r="EW8" s="1"/>
-      <c r="EX8" s="1"/>
-      <c r="EY8" s="1"/>
-      <c r="EZ8" s="1"/>
-      <c r="FA8" s="1"/>
-      <c r="FB8" s="1"/>
-      <c r="FC8" s="1"/>
-      <c r="FD8" s="1"/>
-      <c r="FE8" s="1"/>
-      <c r="FF8" s="1"/>
-      <c r="FG8" s="1"/>
-      <c r="FH8" s="1"/>
-      <c r="FI8" s="1"/>
-      <c r="FJ8" s="1"/>
+      <c r="DO8" s="1">
+        <v>24</v>
+      </c>
+      <c r="DP8" s="1">
+        <v>24</v>
+      </c>
+      <c r="DQ8" s="1">
+        <v>24</v>
+      </c>
+      <c r="DR8" s="1">
+        <v>12</v>
+      </c>
+      <c r="DS8" s="1">
+        <v>24</v>
+      </c>
+      <c r="DT8" s="1">
+        <v>9</v>
+      </c>
+      <c r="DU8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DV8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DW8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DX8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DY8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DZ8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="EA8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EB8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EC8" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="EH8" s="1">
+        <v>12</v>
+      </c>
+      <c r="EI8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ8" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER8" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES8" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW8" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX8" s="1">
+        <v>9</v>
+      </c>
+      <c r="EY8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="EZ8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FA8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FB8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FC8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FD8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FE8" s="1">
+        <v>6</v>
+      </c>
+      <c r="FF8" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG8" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH8" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI8" s="1">
+        <v>24</v>
+      </c>
+      <c r="FJ8" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="FL8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FM8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FO8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FP8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FQ8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FR8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FS8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FT8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FU8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FV8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FW8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FX8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FY8" s="4">
+        <v>24</v>
+      </c>
+      <c r="FZ8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GA8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GB8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GC8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GD8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GE8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GF8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GG8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GH8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GI8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GJ8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GK8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GL8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GM8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GN8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GO8" s="4">
+        <v>8</v>
+      </c>
+      <c r="GP8" s="4">
+        <v>14</v>
+      </c>
+      <c r="GQ8" s="4">
+        <v>24</v>
+      </c>
+      <c r="GR8" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:16384" s="4" customFormat="1" ht="15">
       <c r="A9" s="9">
         <v>24166867</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
@@ -68403,68 +68601,262 @@
       <c r="DM9" s="1">
         <v>24</v>
       </c>
-      <c r="DN9" s="1"/>
+      <c r="DN9" s="1">
+        <v>24</v>
+      </c>
       <c r="DO9" s="1"/>
       <c r="DP9" s="1"/>
       <c r="DQ9" s="1"/>
-      <c r="DR9" s="1"/>
-      <c r="DS9" s="1"/>
-      <c r="DT9" s="1"/>
-      <c r="DU9" s="1"/>
-      <c r="DV9" s="1"/>
-      <c r="DW9" s="1"/>
-      <c r="DX9" s="1"/>
-      <c r="DY9" s="1"/>
-      <c r="DZ9" s="1"/>
-      <c r="EA9" s="1"/>
-      <c r="EB9" s="1"/>
-      <c r="EC9" s="1"/>
-      <c r="ED9" s="1"/>
-      <c r="EE9" s="1"/>
-      <c r="EF9" s="1"/>
-      <c r="EG9" s="1"/>
-      <c r="EH9" s="1"/>
-      <c r="EI9" s="1"/>
-      <c r="EJ9" s="1"/>
-      <c r="EK9" s="1"/>
-      <c r="EL9" s="1"/>
-      <c r="EM9" s="1"/>
-      <c r="EN9" s="1"/>
-      <c r="EO9" s="1"/>
-      <c r="EP9" s="1"/>
-      <c r="EQ9" s="1"/>
-      <c r="ER9" s="1"/>
-      <c r="ES9" s="1"/>
-      <c r="ET9" s="1"/>
-      <c r="EU9" s="1"/>
-      <c r="EV9" s="1"/>
-      <c r="EW9" s="1"/>
-      <c r="EX9" s="1"/>
-      <c r="EY9" s="1"/>
-      <c r="EZ9" s="1"/>
-      <c r="FA9" s="1"/>
-      <c r="FB9" s="1"/>
-      <c r="FC9" s="1"/>
-      <c r="FD9" s="1"/>
-      <c r="FE9" s="1"/>
-      <c r="FF9" s="1"/>
-      <c r="FG9" s="1"/>
-      <c r="FH9" s="1"/>
-      <c r="FI9" s="1"/>
-      <c r="FJ9" s="1"/>
+      <c r="DR9" s="1">
+        <v>12</v>
+      </c>
+      <c r="DS9" s="1">
+        <v>24</v>
+      </c>
+      <c r="DT9" s="1">
+        <v>9</v>
+      </c>
+      <c r="DU9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DV9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DW9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DX9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DY9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DZ9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="EA9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EB9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EC9" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="EH9" s="1">
+        <v>12</v>
+      </c>
+      <c r="EI9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ9" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER9" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES9" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW9" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX9" s="1">
+        <v>9</v>
+      </c>
+      <c r="EY9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="EZ9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FA9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FB9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FC9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FD9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="FE9" s="1">
+        <v>6</v>
+      </c>
+      <c r="FF9" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG9" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH9" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI9" s="1">
+        <v>24</v>
+      </c>
+      <c r="FJ9" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="FL9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FM9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FO9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FP9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FQ9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FR9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FS9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FT9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FU9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FV9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FW9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FX9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FY9" s="4">
+        <v>24</v>
+      </c>
+      <c r="FZ9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GA9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GB9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GC9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GD9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GE9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GF9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GG9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GH9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GI9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GJ9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GK9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GL9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GM9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GN9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GO9" s="4">
+        <v>8</v>
+      </c>
+      <c r="GP9" s="4">
+        <v>14</v>
+      </c>
+      <c r="GQ9" s="4">
+        <v>24</v>
+      </c>
+      <c r="GR9" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:16384" s="4" customFormat="1" ht="15">
       <c r="A10" s="9">
         <v>24166869</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="9">
         <v>60</v>
@@ -68593,13 +68985,13 @@
         <v>24166889</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" s="9">
         <v>60</v>
@@ -68728,13 +69120,13 @@
         <v>24166896</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="9">
         <v>60</v>
@@ -68863,13 +69255,13 @@
         <v>24306368</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="9">
         <v>60</v>
@@ -69000,13 +69392,13 @@
         <v>24308189</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" s="9">
         <v>60</v>
@@ -69137,10 +69529,10 @@
         <v>24303936</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>28</v>
@@ -69382,10 +69774,10 @@
         <v>24303937</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>21</v>
@@ -69605,10 +69997,10 @@
         <v>24401571</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>28</v>
@@ -69849,10 +70241,10 @@
         <v>24401574</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>21</v>
@@ -70063,10 +70455,10 @@
         <v>51816376</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>28</v>
@@ -70307,10 +70699,10 @@
         <v>51817126</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>28</v>
@@ -70551,10 +70943,10 @@
         <v>51814914</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>28</v>
@@ -70795,7 +71187,7 @@
         <v>24166740</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>17</v>
@@ -70943,7 +71335,7 @@
         <v>24166738</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
@@ -71091,7 +71483,7 @@
         <v>24166740</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>17</v>
@@ -71233,7 +71625,7 @@
         <v>24166738</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>17</v>
@@ -71375,10 +71767,10 @@
         <v>24471120</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>21</v>
@@ -71589,13 +71981,13 @@
         <v>24395952</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E27" s="9">
         <v>60</v>
@@ -71752,13 +72144,13 @@
         <v>24395977</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D28" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E28" s="9">
         <v>60</v>
@@ -71915,13 +72307,13 @@
         <v>24395942</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E29" s="9">
         <v>60</v>
@@ -72078,13 +72470,13 @@
         <v>24636087</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E30" s="9">
         <v>60</v>
@@ -72241,13 +72633,13 @@
         <v>24636090</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E31" s="9">
         <v>60</v>
@@ -72404,13 +72796,13 @@
         <v>24636091</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E32" s="9">
         <v>60</v>
@@ -72562,15 +72954,15 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:170" ht="15">
+    <row r="33" spans="1:166" ht="15">
       <c r="A33" s="9">
         <v>24636088</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>18</v>
@@ -72711,15 +73103,15 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:170" ht="15">
+    <row r="34" spans="1:166" ht="15">
       <c r="A34" s="9">
         <v>24636089</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>18</v>
@@ -72860,15 +73252,15 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:170" ht="15">
+    <row r="35" spans="1:166" ht="15">
       <c r="A35" s="9">
         <v>24636092</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>18</v>
@@ -72996,15 +73388,15 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:170" ht="15">
+    <row r="36" spans="1:166" ht="15">
       <c r="A36" s="9">
         <v>24395952</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>28</v>
@@ -73130,15 +73522,15 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:170" ht="15">
+    <row r="37" spans="1:166" ht="15">
       <c r="A37" s="9">
         <v>24395977</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>21</v>
@@ -73264,15 +73656,15 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:170" ht="15">
+    <row r="38" spans="1:166" ht="15">
       <c r="A38" s="9">
         <v>24395942</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>18</v>
@@ -73398,18 +73790,18 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:170" ht="15">
+    <row r="39" spans="1:166" ht="15">
       <c r="A39" s="12">
         <v>24567303</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E39" s="9">
         <v>60</v>
@@ -73561,18 +73953,18 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:170" ht="15">
+    <row r="40" spans="1:166" ht="15">
       <c r="A40" s="12">
         <v>24567296</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E40" s="9">
         <v>60</v>
@@ -73724,18 +74116,18 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:170" ht="15">
+    <row r="41" spans="1:166" ht="15">
       <c r="A41" s="12">
         <v>24567289</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E41" s="9">
         <v>60</v>
@@ -73887,18 +74279,18 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:170" ht="15">
+    <row r="42" spans="1:166" ht="15">
       <c r="A42" s="12">
         <v>24567319</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E42" s="9">
         <v>60</v>
@@ -74050,18 +74442,18 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:170" ht="15">
+    <row r="43" spans="1:166" ht="15">
       <c r="A43" s="12">
         <v>24567277</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E43" s="9">
         <v>60</v>
@@ -74213,18 +74605,18 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:170" ht="15">
+    <row r="44" spans="1:166" ht="15">
       <c r="A44" s="12">
         <v>24567774</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E44" s="9">
         <v>60</v>
@@ -74376,18 +74768,18 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:170" ht="15">
+    <row r="45" spans="1:166" ht="15">
       <c r="A45" s="12">
         <v>24567851</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E45" s="9">
         <v>60</v>
@@ -74539,18 +74931,18 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:170" ht="15">
+    <row r="46" spans="1:166" ht="15">
       <c r="A46" s="12">
         <v>24559501</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E46" s="9">
         <v>60</v>
@@ -74702,15 +75094,15 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:170" ht="15">
+    <row r="47" spans="1:166" ht="15">
       <c r="A47" s="12">
         <v>24567303</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>28</v>
@@ -74836,15 +75228,15 @@
       <c r="FI47" s="1"/>
       <c r="FJ47" s="1"/>
     </row>
-    <row r="48" spans="1:170" ht="15">
+    <row r="48" spans="1:166" ht="15">
       <c r="A48" s="12">
         <v>24567296</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>28</v>
@@ -74938,8 +75330,12 @@
       <c r="DX48" s="1"/>
       <c r="DY48" s="1"/>
       <c r="DZ48" s="1"/>
-      <c r="EA48" s="1"/>
-      <c r="EB48" s="1"/>
+      <c r="EA48" s="1">
+        <v>6</v>
+      </c>
+      <c r="EB48" s="1">
+        <v>24</v>
+      </c>
       <c r="EC48" s="1">
         <v>24</v>
       </c>
@@ -74952,8 +75348,8 @@
       <c r="EF48" s="1">
         <v>24</v>
       </c>
-      <c r="EG48" s="1">
-        <v>24</v>
+      <c r="EG48" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="EH48" s="1">
         <v>24</v>
@@ -75039,31 +75435,17 @@
       <c r="FI48" s="1">
         <v>24</v>
       </c>
-      <c r="FJ48" s="1">
-        <v>8</v>
-      </c>
-      <c r="FK48" s="4">
-        <v>14</v>
-      </c>
-      <c r="FL48" s="4">
-        <v>24</v>
-      </c>
-      <c r="FM48" s="4">
-        <v>24</v>
-      </c>
-      <c r="FN48" s="4">
-        <v>24</v>
-      </c>
+      <c r="FJ48" s="1"/>
     </row>
     <row r="49" spans="1:170" ht="15">
       <c r="A49" s="12">
         <v>24567289</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>28</v>
@@ -75194,10 +75576,10 @@
         <v>24567319</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>28</v>
@@ -75291,8 +75673,12 @@
       <c r="DX50" s="1"/>
       <c r="DY50" s="1"/>
       <c r="DZ50" s="1"/>
-      <c r="EA50" s="1"/>
-      <c r="EB50" s="1"/>
+      <c r="EA50" s="1">
+        <v>6</v>
+      </c>
+      <c r="EB50" s="1">
+        <v>24</v>
+      </c>
       <c r="EC50" s="1">
         <v>24</v>
       </c>
@@ -75305,8 +75691,8 @@
       <c r="EF50" s="1">
         <v>24</v>
       </c>
-      <c r="EG50" s="1">
-        <v>24</v>
+      <c r="EG50" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="EH50" s="1">
         <v>24</v>
@@ -75392,31 +75778,17 @@
       <c r="FI50" s="1">
         <v>24</v>
       </c>
-      <c r="FJ50" s="1">
-        <v>8</v>
-      </c>
-      <c r="FK50" s="4">
-        <v>14</v>
-      </c>
-      <c r="FL50" s="4">
-        <v>24</v>
-      </c>
-      <c r="FM50" s="4">
-        <v>24</v>
-      </c>
-      <c r="FN50" s="4">
-        <v>24</v>
-      </c>
+      <c r="FJ50" s="1"/>
     </row>
     <row r="51" spans="1:170" ht="15">
       <c r="A51" s="12">
         <v>24567277</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>28</v>
@@ -75510,8 +75882,12 @@
       <c r="DX51" s="1"/>
       <c r="DY51" s="1"/>
       <c r="DZ51" s="1"/>
-      <c r="EA51" s="1"/>
-      <c r="EB51" s="1"/>
+      <c r="EA51" s="1">
+        <v>6</v>
+      </c>
+      <c r="EB51" s="1">
+        <v>24</v>
+      </c>
       <c r="EC51" s="1">
         <v>24</v>
       </c>
@@ -75524,8 +75900,8 @@
       <c r="EF51" s="1">
         <v>24</v>
       </c>
-      <c r="EG51" s="1">
-        <v>24</v>
+      <c r="EG51" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="EH51" s="1">
         <v>24</v>
@@ -75611,31 +75987,17 @@
       <c r="FI51" s="1">
         <v>24</v>
       </c>
-      <c r="FJ51" s="1">
-        <v>8</v>
-      </c>
-      <c r="FK51" s="4">
-        <v>14</v>
-      </c>
-      <c r="FL51" s="4">
-        <v>24</v>
-      </c>
-      <c r="FM51" s="4">
-        <v>24</v>
-      </c>
-      <c r="FN51" s="4">
-        <v>24</v>
-      </c>
+      <c r="FJ51" s="1"/>
     </row>
     <row r="52" spans="1:170" ht="15">
       <c r="A52" s="12">
         <v>24567774</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>28</v>
@@ -75729,8 +76091,12 @@
       <c r="DX52" s="1"/>
       <c r="DY52" s="1"/>
       <c r="DZ52" s="1"/>
-      <c r="EA52" s="1"/>
-      <c r="EB52" s="1"/>
+      <c r="EA52" s="1">
+        <v>6</v>
+      </c>
+      <c r="EB52" s="1">
+        <v>24</v>
+      </c>
       <c r="EC52" s="1">
         <v>24</v>
       </c>
@@ -75743,8 +76109,8 @@
       <c r="EF52" s="1">
         <v>24</v>
       </c>
-      <c r="EG52" s="1">
-        <v>24</v>
+      <c r="EG52" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="EH52" s="1">
         <v>24</v>
@@ -75830,31 +76196,17 @@
       <c r="FI52" s="1">
         <v>24</v>
       </c>
-      <c r="FJ52" s="1">
-        <v>8</v>
-      </c>
-      <c r="FK52" s="4">
-        <v>14</v>
-      </c>
-      <c r="FL52" s="4">
-        <v>24</v>
-      </c>
-      <c r="FM52" s="4">
-        <v>24</v>
-      </c>
-      <c r="FN52" s="4">
-        <v>24</v>
-      </c>
+      <c r="FJ52" s="1"/>
     </row>
     <row r="53" spans="1:170" ht="15">
       <c r="A53" s="12">
         <v>24567851</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>28</v>
@@ -75985,10 +76337,10 @@
         <v>24559501</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>28</v>
@@ -76119,10 +76471,10 @@
         <v>24079686</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>28</v>
@@ -76307,10 +76659,10 @@
         <v>24079692</v>
       </c>
       <c r="B56" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>21</v>
@@ -76495,10 +76847,10 @@
         <v>24636092</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>18</v>
@@ -76649,10 +77001,10 @@
         <v>24793376</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>25</v>
@@ -76805,10 +77157,10 @@
         <v>24713456</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>28</v>
@@ -76959,10 +77311,10 @@
         <v>24713371</v>
       </c>
       <c r="B60" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>18</v>
@@ -77105,10 +77457,10 @@
         <v>24713222</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>21</v>
@@ -77263,10 +77615,10 @@
         <v>24636087</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>28</v>
@@ -77358,51 +77710,133 @@
       <c r="DY62" s="1"/>
       <c r="DZ62" s="1"/>
       <c r="EA62" s="1"/>
-      <c r="EB62" s="1"/>
-      <c r="EC62" s="1"/>
-      <c r="ED62" s="1"/>
-      <c r="EE62" s="1"/>
-      <c r="EF62" s="1"/>
-      <c r="EG62" s="1"/>
-      <c r="EH62" s="1"/>
-      <c r="EI62" s="1"/>
-      <c r="EJ62" s="1"/>
-      <c r="EK62" s="1"/>
-      <c r="EL62" s="1"/>
-      <c r="EM62" s="1"/>
-      <c r="EN62" s="1"/>
-      <c r="EO62" s="1"/>
-      <c r="EP62" s="1"/>
-      <c r="EQ62" s="1"/>
-      <c r="ER62" s="1"/>
-      <c r="ES62" s="1"/>
-      <c r="ET62" s="1"/>
-      <c r="EU62" s="1"/>
-      <c r="EV62" s="1"/>
-      <c r="EW62" s="1"/>
-      <c r="EX62" s="1"/>
-      <c r="EY62" s="1"/>
-      <c r="EZ62" s="1"/>
-      <c r="FA62" s="1"/>
-      <c r="FB62" s="1"/>
-      <c r="FC62" s="1"/>
-      <c r="FD62" s="1"/>
-      <c r="FE62" s="1"/>
-      <c r="FF62" s="1"/>
-      <c r="FG62" s="1"/>
-      <c r="FH62" s="1"/>
-      <c r="FI62" s="1"/>
-      <c r="FJ62" s="1"/>
+      <c r="EB62" s="1">
+        <v>16</v>
+      </c>
+      <c r="EC62" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="EH62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ62" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER62" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES62" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY62" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FJ62" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK62" s="4">
+        <v>24</v>
+      </c>
+      <c r="FL62" s="4">
+        <v>24</v>
+      </c>
+      <c r="FM62" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN62" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="63" spans="1:170" ht="15">
       <c r="A63" s="9">
         <v>24636090</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>28</v>
@@ -77494,51 +77928,133 @@
       <c r="DY63" s="1"/>
       <c r="DZ63" s="1"/>
       <c r="EA63" s="1"/>
-      <c r="EB63" s="1"/>
-      <c r="EC63" s="1"/>
-      <c r="ED63" s="1"/>
-      <c r="EE63" s="1"/>
-      <c r="EF63" s="1"/>
-      <c r="EG63" s="1"/>
-      <c r="EH63" s="1"/>
-      <c r="EI63" s="1"/>
-      <c r="EJ63" s="1"/>
-      <c r="EK63" s="1"/>
-      <c r="EL63" s="1"/>
-      <c r="EM63" s="1"/>
-      <c r="EN63" s="1"/>
-      <c r="EO63" s="1"/>
-      <c r="EP63" s="1"/>
-      <c r="EQ63" s="1"/>
-      <c r="ER63" s="1"/>
-      <c r="ES63" s="1"/>
-      <c r="ET63" s="1"/>
-      <c r="EU63" s="1"/>
-      <c r="EV63" s="1"/>
-      <c r="EW63" s="1"/>
-      <c r="EX63" s="1"/>
-      <c r="EY63" s="1"/>
-      <c r="EZ63" s="1"/>
-      <c r="FA63" s="1"/>
-      <c r="FB63" s="1"/>
-      <c r="FC63" s="1"/>
-      <c r="FD63" s="1"/>
-      <c r="FE63" s="1"/>
-      <c r="FF63" s="1"/>
-      <c r="FG63" s="1"/>
-      <c r="FH63" s="1"/>
-      <c r="FI63" s="1"/>
-      <c r="FJ63" s="1"/>
+      <c r="EB63" s="1">
+        <v>16</v>
+      </c>
+      <c r="EC63" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG63" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="EH63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ63" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER63" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES63" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY63" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FJ63" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK63" s="4">
+        <v>24</v>
+      </c>
+      <c r="FL63" s="4">
+        <v>24</v>
+      </c>
+      <c r="FM63" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN63" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="64" spans="1:170" ht="15">
       <c r="A64" s="9">
         <v>24636091</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>28</v>
@@ -77630,51 +78146,133 @@
       <c r="DY64" s="1"/>
       <c r="DZ64" s="1"/>
       <c r="EA64" s="1"/>
-      <c r="EB64" s="1"/>
-      <c r="EC64" s="1"/>
-      <c r="ED64" s="1"/>
-      <c r="EE64" s="1"/>
-      <c r="EF64" s="1"/>
-      <c r="EG64" s="1"/>
-      <c r="EH64" s="1"/>
-      <c r="EI64" s="1"/>
-      <c r="EJ64" s="1"/>
-      <c r="EK64" s="1"/>
-      <c r="EL64" s="1"/>
-      <c r="EM64" s="1"/>
-      <c r="EN64" s="1"/>
-      <c r="EO64" s="1"/>
-      <c r="EP64" s="1"/>
-      <c r="EQ64" s="1"/>
-      <c r="ER64" s="1"/>
-      <c r="ES64" s="1"/>
-      <c r="ET64" s="1"/>
-      <c r="EU64" s="1"/>
-      <c r="EV64" s="1"/>
-      <c r="EW64" s="1"/>
-      <c r="EX64" s="1"/>
-      <c r="EY64" s="1"/>
-      <c r="EZ64" s="1"/>
-      <c r="FA64" s="1"/>
-      <c r="FB64" s="1"/>
-      <c r="FC64" s="1"/>
-      <c r="FD64" s="1"/>
-      <c r="FE64" s="1"/>
-      <c r="FF64" s="1"/>
-      <c r="FG64" s="1"/>
-      <c r="FH64" s="1"/>
-      <c r="FI64" s="1"/>
-      <c r="FJ64" s="1"/>
+      <c r="EB64" s="1">
+        <v>16</v>
+      </c>
+      <c r="EC64" s="1">
+        <v>24</v>
+      </c>
+      <c r="ED64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EE64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EF64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EG64" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="EH64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EI64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EJ64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EK64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EL64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EM64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EN64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EO64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EP64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EQ64" s="1">
+        <v>24</v>
+      </c>
+      <c r="ER64" s="1">
+        <v>24</v>
+      </c>
+      <c r="ES64" s="1">
+        <v>24</v>
+      </c>
+      <c r="ET64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EU64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EV64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EW64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY64" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FJ64" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK64" s="4">
+        <v>24</v>
+      </c>
+      <c r="FL64" s="4">
+        <v>24</v>
+      </c>
+      <c r="FM64" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN64" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="65" spans="1:170" ht="15">
       <c r="A65" s="9">
         <v>24636089</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>18</v>
@@ -77815,10 +78413,10 @@
         <v>24636088</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>18</v>
@@ -77959,13 +78557,13 @@
         <v>25017935</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E67" s="9">
         <v>60</v>
@@ -78093,10 +78691,10 @@
         <v>25017936</v>
       </c>
       <c r="B68" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>18</v>
@@ -78240,10 +78838,10 @@
         <v>25017937</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>28</v>
@@ -78374,13 +78972,13 @@
         <v>25019644</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E70" s="9">
         <v>60</v>
@@ -78508,10 +79106,10 @@
         <v>25019645</v>
       </c>
       <c r="B71" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>18</v>
@@ -78655,10 +79253,10 @@
         <v>25019646</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>28</v>
@@ -78789,10 +79387,10 @@
         <v>24848800</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>28</v>
@@ -78884,22 +79482,22 @@
         <v>9</v>
       </c>
       <c r="DU73" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DV73" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DW73" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DX73" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DY73" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DZ73" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="EA73" s="1">
         <v>6</v>
@@ -78920,7 +79518,7 @@
         <v>24</v>
       </c>
       <c r="EG73" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="EH73" s="1">
         <v>24</v>
@@ -79122,22 +79720,22 @@
         <v>9</v>
       </c>
       <c r="DU74" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DV74" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DW74" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DX74" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DY74" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="DZ74" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="EA74" s="1">
         <v>6</v>
@@ -79158,7 +79756,7 @@
         <v>24</v>
       </c>
       <c r="EG74" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="EH74" s="1">
         <v>24</v>
@@ -79265,10 +79863,10 @@
         <v>24848800</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>28</v>
@@ -79533,10 +80131,10 @@
         <v>24848800</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>28</v>
@@ -79801,10 +80399,10 @@
         <v>24848800</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>28</v>
@@ -80069,10 +80667,10 @@
         <v>24848800</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>28</v>
@@ -80337,10 +80935,10 @@
         <v>24848800</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>28</v>
@@ -81122,11 +81720,17 @@
       <c r="ES88" s="1"/>
       <c r="ET88" s="1"/>
       <c r="EU88" s="1"/>
-      <c r="EV88" s="1"/>
-      <c r="EW88" s="1"/>
-      <c r="EX88" s="1"/>
+      <c r="EV88" s="1">
+        <v>12</v>
+      </c>
+      <c r="EW88" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX88" s="1">
+        <v>24</v>
+      </c>
       <c r="EY88" s="1">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="EZ88" s="1">
         <v>24</v>
@@ -81705,7 +82309,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:170" s="4" customFormat="1" ht="15">
+    <row r="96" spans="1:170" ht="15">
       <c r="A96" s="16">
         <v>50872159</v>
       </c>
@@ -81724,17 +82328,16 @@
       <c r="F96" s="19">
         <v>45793</v>
       </c>
-      <c r="P96" s="3"/>
     </row>
-    <row r="97" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="97" spans="1:167" ht="15">
       <c r="A97" s="16">
         <v>25019645</v>
       </c>
       <c r="B97" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C97" s="18" t="s">
         <v>94</v>
-      </c>
-      <c r="C97" s="18" t="s">
-        <v>93</v>
       </c>
       <c r="D97" s="16" t="s">
         <v>18</v>
@@ -81743,17 +82346,16 @@
         <v>96</v>
       </c>
       <c r="F97" s="19"/>
-      <c r="P97" s="3"/>
     </row>
-    <row r="98" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="98" spans="1:167" ht="15">
       <c r="A98" s="16">
         <v>25017936</v>
       </c>
       <c r="B98" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C98" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="C98" s="18" t="s">
-        <v>89</v>
       </c>
       <c r="D98" s="16" t="s">
         <v>18</v>
@@ -81762,9 +82364,8 @@
         <v>96</v>
       </c>
       <c r="F98" s="19"/>
-      <c r="P98" s="3"/>
     </row>
-    <row r="99" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="99" spans="1:167" ht="15">
       <c r="A99" s="16">
         <v>25089372</v>
       </c>
@@ -81775,7 +82376,7 @@
         <v>122</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E99" s="16">
         <v>60</v>
@@ -81823,7 +82424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="100" spans="1:167" ht="15">
       <c r="A100" s="16">
         <v>25089365</v>
       </c>
@@ -81834,7 +82435,7 @@
         <v>124</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E100" s="16">
         <v>60</v>
@@ -81882,7 +82483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="101" spans="1:167" ht="15">
       <c r="A101" s="16">
         <v>25089363</v>
       </c>
@@ -81893,7 +82494,7 @@
         <v>124</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E101" s="16">
         <v>60</v>
@@ -81941,7 +82542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="102" spans="1:167" ht="15">
       <c r="A102" s="16">
         <v>25089370</v>
       </c>
@@ -81952,7 +82553,7 @@
         <v>122</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E102" s="16">
         <v>60</v>
@@ -82000,7 +82601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="103" spans="1:167" ht="15">
       <c r="A103" s="16">
         <v>25112299</v>
       </c>
@@ -82011,7 +82612,7 @@
         <v>114</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E103" s="16">
         <v>60</v>
@@ -82059,7 +82660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="104" spans="1:167" ht="15">
       <c r="A104" s="16">
         <v>72149637</v>
       </c>
@@ -82081,11 +82682,41 @@
       <c r="P104" s="3">
         <v>45806</v>
       </c>
+      <c r="EY104" s="4">
+        <v>8</v>
+      </c>
+      <c r="EZ104" s="4">
+        <v>12</v>
+      </c>
+      <c r="FA104" s="4">
+        <v>12</v>
+      </c>
+      <c r="FB104" s="4">
+        <v>12</v>
+      </c>
+      <c r="FC104" s="4">
+        <v>12</v>
+      </c>
+      <c r="FD104" s="4">
+        <v>12</v>
+      </c>
+      <c r="FE104" s="4">
+        <v>12</v>
+      </c>
+      <c r="FF104" s="4">
+        <v>12</v>
+      </c>
+      <c r="FG104" s="4">
+        <v>12</v>
+      </c>
+      <c r="FH104" s="4">
+        <v>12</v>
+      </c>
       <c r="FI104" s="4">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="105" spans="1:167" ht="15">
       <c r="A105" s="16">
         <v>72238923</v>
       </c>
@@ -82102,9 +82733,8 @@
         <v>1000</v>
       </c>
       <c r="F105" s="19"/>
-      <c r="P105" s="3"/>
     </row>
-    <row r="106" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="106" spans="1:167" ht="15">
       <c r="A106" s="16">
         <v>25089372</v>
       </c>
@@ -82121,9 +82751,8 @@
         <v>96</v>
       </c>
       <c r="F106" s="19"/>
-      <c r="P106" s="3"/>
     </row>
-    <row r="107" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="107" spans="1:167" ht="15">
       <c r="A107" s="16">
         <v>25089365</v>
       </c>
@@ -82140,9 +82769,8 @@
         <v>96</v>
       </c>
       <c r="F107" s="19"/>
-      <c r="P107" s="3"/>
     </row>
-    <row r="108" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="108" spans="1:167" ht="15">
       <c r="A108" s="16">
         <v>25089363</v>
       </c>
@@ -82159,9 +82787,8 @@
         <v>1000</v>
       </c>
       <c r="F108" s="19"/>
-      <c r="P108" s="3"/>
     </row>
-    <row r="109" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="109" spans="1:167" ht="15">
       <c r="A109" s="16">
         <v>25089370</v>
       </c>
@@ -82178,9 +82805,8 @@
         <v>1000</v>
       </c>
       <c r="F109" s="19"/>
-      <c r="P109" s="3"/>
     </row>
-    <row r="110" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="110" spans="1:167" ht="15">
       <c r="A110" s="16">
         <v>25112301</v>
       </c>
@@ -82197,9 +82823,8 @@
         <v>96</v>
       </c>
       <c r="F110" s="19"/>
-      <c r="P110" s="3"/>
     </row>
-    <row r="111" spans="1:167" s="4" customFormat="1" ht="15">
+    <row r="111" spans="1:167" ht="15">
       <c r="A111" s="16">
         <v>25112300</v>
       </c>
@@ -82216,24 +82841,9 @@
         <v>1000</v>
       </c>
       <c r="F111" s="19"/>
-      <c r="P111" s="3"/>
     </row>
-    <row r="112" spans="1:167" s="4" customFormat="1" ht="15">
-      <c r="A112" s="10"/>
-      <c r="B112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="10"/>
-      <c r="F112" s="14"/>
-      <c r="P112" s="3"/>
-    </row>
-    <row r="113" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A113" s="10"/>
-      <c r="B113" s="10"/>
-      <c r="D113" s="10"/>
-      <c r="E113" s="10"/>
-      <c r="F113" s="14"/>
-      <c r="P113" s="3"/>
-    </row>
+    <row r="112" spans="1:167" ht="15"/>
+    <row r="113" ht="15"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun  5 09:39:34 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="422" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62CB8486-5111-4AF7-BEFF-BFDE278027F4}"/>
+  <xr:revisionPtr revIDLastSave="455" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15BF28A8-7951-4C66-81B4-4CC648525F03}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="137">
   <si>
     <t>Module ID</t>
   </si>
@@ -432,6 +432,21 @@
   </si>
   <si>
     <t>IPQC Yellow Spot on Ribbon</t>
+  </si>
+  <si>
+    <t>VSL202526114</t>
+  </si>
+  <si>
+    <t>IPQC PID Test Modules : Jun '25</t>
+  </si>
+  <si>
+    <t>VSL202526115</t>
+  </si>
+  <si>
+    <t>VSL202526116</t>
+  </si>
+  <si>
+    <t>VSL202526117</t>
   </si>
 </sst>
 </file>
@@ -957,11 +972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD113"/>
+  <dimension ref="A1:XFD115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="EA6" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="EG8" sqref="EG8:EG9"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FL82" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FO91" sqref="FO91"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -68406,93 +68421,6 @@
       <c r="FO8" s="4">
         <v>24</v>
       </c>
-      <c r="FP8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FQ8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FR8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FS8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FT8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FU8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FV8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FW8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FX8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FY8" s="4">
-        <v>24</v>
-      </c>
-      <c r="FZ8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GA8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GB8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GC8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GD8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GE8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GF8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GG8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GH8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GI8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GJ8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GK8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GL8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GM8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GN8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GO8" s="4">
-        <v>8</v>
-      </c>
-      <c r="GP8" s="4">
-        <v>14</v>
-      </c>
-      <c r="GQ8" s="4">
-        <v>24</v>
-      </c>
-      <c r="GR8" s="4">
-        <v>24</v>
-      </c>
     </row>
     <row r="9" spans="1:16384" s="4" customFormat="1" ht="15">
       <c r="A9" s="9">
@@ -68755,93 +68683,6 @@
         <v>24</v>
       </c>
       <c r="FO9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FP9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FQ9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FR9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FS9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FT9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FU9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FV9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FW9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FX9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FY9" s="4">
-        <v>24</v>
-      </c>
-      <c r="FZ9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GA9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GB9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GC9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GD9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GE9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GF9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GG9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GH9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GI9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GJ9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GK9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GL9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GM9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GN9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GO9" s="4">
-        <v>8</v>
-      </c>
-      <c r="GP9" s="4">
-        <v>14</v>
-      </c>
-      <c r="GQ9" s="4">
-        <v>24</v>
-      </c>
-      <c r="GR9" s="4">
         <v>24</v>
       </c>
     </row>
@@ -75248,7 +75089,7 @@
         <v>45773</v>
       </c>
       <c r="P48" s="3">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="AY48" s="1"/>
       <c r="AZ48" s="1"/>
@@ -75435,9 +75276,11 @@
       <c r="FI48" s="1">
         <v>24</v>
       </c>
-      <c r="FJ48" s="1"/>
+      <c r="FJ48" s="1">
+        <v>202</v>
+      </c>
     </row>
-    <row r="49" spans="1:170" ht="15">
+    <row r="49" spans="1:171" ht="15">
       <c r="A49" s="12">
         <v>24567289</v>
       </c>
@@ -75571,7 +75414,7 @@
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
     </row>
-    <row r="50" spans="1:170" ht="15">
+    <row r="50" spans="1:171" ht="15">
       <c r="A50" s="12">
         <v>24567319</v>
       </c>
@@ -75591,7 +75434,7 @@
         <v>45773</v>
       </c>
       <c r="P50" s="3">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="AY50" s="1"/>
       <c r="AZ50" s="1"/>
@@ -75778,9 +75621,11 @@
       <c r="FI50" s="1">
         <v>24</v>
       </c>
-      <c r="FJ50" s="1"/>
+      <c r="FJ50" s="1">
+        <v>202</v>
+      </c>
     </row>
-    <row r="51" spans="1:170" ht="15">
+    <row r="51" spans="1:171" ht="15">
       <c r="A51" s="12">
         <v>24567277</v>
       </c>
@@ -75800,7 +75645,7 @@
         <v>45773</v>
       </c>
       <c r="P51" s="3">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="AY51" s="1"/>
       <c r="AZ51" s="1"/>
@@ -75987,9 +75832,11 @@
       <c r="FI51" s="1">
         <v>24</v>
       </c>
-      <c r="FJ51" s="1"/>
+      <c r="FJ51" s="1">
+        <v>202</v>
+      </c>
     </row>
-    <row r="52" spans="1:170" ht="15">
+    <row r="52" spans="1:171" ht="15">
       <c r="A52" s="12">
         <v>24567774</v>
       </c>
@@ -76009,7 +75856,7 @@
         <v>45773</v>
       </c>
       <c r="P52" s="3">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="AY52" s="1"/>
       <c r="AZ52" s="1"/>
@@ -76196,9 +76043,11 @@
       <c r="FI52" s="1">
         <v>24</v>
       </c>
-      <c r="FJ52" s="1"/>
+      <c r="FJ52" s="1">
+        <v>202</v>
+      </c>
     </row>
-    <row r="53" spans="1:170" ht="15">
+    <row r="53" spans="1:171" ht="15">
       <c r="A53" s="12">
         <v>24567851</v>
       </c>
@@ -76332,7 +76181,7 @@
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
     </row>
-    <row r="54" spans="1:170" ht="15">
+    <row r="54" spans="1:171" ht="15">
       <c r="A54" s="12">
         <v>24559501</v>
       </c>
@@ -76466,7 +76315,7 @@
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
     </row>
-    <row r="55" spans="1:170" ht="15">
+    <row r="55" spans="1:171" ht="15">
       <c r="A55" s="9">
         <v>24079686</v>
       </c>
@@ -76654,7 +76503,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:170" ht="15">
+    <row r="56" spans="1:171" ht="15">
       <c r="A56" s="9">
         <v>24079692</v>
       </c>
@@ -76842,7 +76691,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:170" ht="15">
+    <row r="57" spans="1:171" ht="15">
       <c r="A57" s="9">
         <v>24636092</v>
       </c>
@@ -76996,7 +76845,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:170" ht="15">
+    <row r="58" spans="1:171" ht="15">
       <c r="A58" s="9">
         <v>24793376</v>
       </c>
@@ -77152,7 +77001,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:170" ht="15">
+    <row r="59" spans="1:171" ht="15">
       <c r="A59" s="9">
         <v>24713456</v>
       </c>
@@ -77306,7 +77155,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:170" ht="15">
+    <row r="60" spans="1:171" ht="15">
       <c r="A60" s="9">
         <v>24713371</v>
       </c>
@@ -77452,7 +77301,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:170" ht="15">
+    <row r="61" spans="1:171" ht="15">
       <c r="A61" s="9">
         <v>24713222</v>
       </c>
@@ -77610,7 +77459,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:170" ht="15">
+    <row r="62" spans="1:171" ht="15">
       <c r="A62" s="12">
         <v>24636087</v>
       </c>
@@ -77827,8 +77676,11 @@
       <c r="FN62" s="4">
         <v>24</v>
       </c>
+      <c r="FO62" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="63" spans="1:170" ht="15">
+    <row r="63" spans="1:171" ht="15">
       <c r="A63" s="9">
         <v>24636090</v>
       </c>
@@ -78045,8 +77897,11 @@
       <c r="FN63" s="4">
         <v>24</v>
       </c>
+      <c r="FO63" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="64" spans="1:170" ht="15">
+    <row r="64" spans="1:171" ht="15">
       <c r="A64" s="9">
         <v>24636091</v>
       </c>
@@ -78263,8 +78118,11 @@
       <c r="FN64" s="4">
         <v>24</v>
       </c>
+      <c r="FO64" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="65" spans="1:170" ht="15">
+    <row r="65" spans="1:171" ht="15">
       <c r="A65" s="9">
         <v>24636089</v>
       </c>
@@ -78408,7 +78266,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:170" ht="15">
+    <row r="66" spans="1:171" ht="15">
       <c r="A66" s="9">
         <v>24636088</v>
       </c>
@@ -78552,7 +78410,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:170" ht="15">
+    <row r="67" spans="1:171" ht="15">
       <c r="A67" s="9">
         <v>25017935</v>
       </c>
@@ -78686,7 +78544,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:170" ht="15">
+    <row r="68" spans="1:171" ht="15">
       <c r="A68" s="9">
         <v>25017936</v>
       </c>
@@ -78833,7 +78691,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:170" ht="15">
+    <row r="69" spans="1:171" ht="15">
       <c r="A69" s="9">
         <v>25017937</v>
       </c>
@@ -78967,7 +78825,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:170" ht="15">
+    <row r="70" spans="1:171" ht="15">
       <c r="A70" s="9">
         <v>25019644</v>
       </c>
@@ -79101,7 +78959,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:170" ht="15">
+    <row r="71" spans="1:171" ht="15">
       <c r="A71" s="9">
         <v>25019645</v>
       </c>
@@ -79248,7 +79106,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:170" ht="15">
+    <row r="72" spans="1:171" ht="15">
       <c r="A72" s="9">
         <v>25019646</v>
       </c>
@@ -79382,7 +79240,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:170" ht="15">
+    <row r="73" spans="1:171" ht="15">
       <c r="A73" s="9">
         <v>24848800</v>
       </c>
@@ -79619,8 +79477,11 @@
       <c r="FN73" s="4">
         <v>24</v>
       </c>
+      <c r="FO73" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="74" spans="1:170" ht="15">
+    <row r="74" spans="1:171" ht="15">
       <c r="A74" s="9">
         <v>24859051</v>
       </c>
@@ -79857,8 +79718,11 @@
       <c r="FN74" s="4">
         <v>24</v>
       </c>
+      <c r="FO74" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="75" spans="1:170" ht="15">
+    <row r="75" spans="1:171" ht="15">
       <c r="A75" s="9">
         <v>24848800</v>
       </c>
@@ -79992,7 +79856,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:170" ht="15">
+    <row r="76" spans="1:171" ht="15">
       <c r="A76" s="9">
         <v>24859051</v>
       </c>
@@ -80126,7 +79990,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:170" ht="15">
+    <row r="77" spans="1:171" ht="15">
       <c r="A77" s="9">
         <v>24848800</v>
       </c>
@@ -80260,7 +80124,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:170" ht="15">
+    <row r="78" spans="1:171" ht="15">
       <c r="A78" s="9">
         <v>24859051</v>
       </c>
@@ -80394,7 +80258,7 @@
       <c r="FI78" s="1"/>
       <c r="FJ78" s="1"/>
     </row>
-    <row r="79" spans="1:170" ht="15">
+    <row r="79" spans="1:171" ht="15">
       <c r="A79" s="9">
         <v>24848800</v>
       </c>
@@ -80528,7 +80392,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:170" ht="15">
+    <row r="80" spans="1:171" ht="15">
       <c r="A80" s="9">
         <v>24859051</v>
       </c>
@@ -80662,7 +80526,7 @@
       <c r="FI80" s="1"/>
       <c r="FJ80" s="1"/>
     </row>
-    <row r="81" spans="1:170" ht="15">
+    <row r="81" spans="1:171" ht="15">
       <c r="A81" s="9">
         <v>24848800</v>
       </c>
@@ -80796,7 +80660,7 @@
       <c r="FI81" s="1"/>
       <c r="FJ81" s="1"/>
     </row>
-    <row r="82" spans="1:170" ht="15">
+    <row r="82" spans="1:171" ht="15">
       <c r="A82" s="9">
         <v>24859051</v>
       </c>
@@ -80930,7 +80794,7 @@
       <c r="FI82" s="1"/>
       <c r="FJ82" s="1"/>
     </row>
-    <row r="83" spans="1:170" ht="15">
+    <row r="83" spans="1:171" ht="15">
       <c r="A83" s="9">
         <v>24848800</v>
       </c>
@@ -81064,7 +80928,7 @@
       <c r="FI83" s="1"/>
       <c r="FJ83" s="1"/>
     </row>
-    <row r="84" spans="1:170" ht="15">
+    <row r="84" spans="1:171" ht="15">
       <c r="A84" s="9">
         <v>24859051</v>
       </c>
@@ -81198,7 +81062,7 @@
       <c r="FI84" s="1"/>
       <c r="FJ84" s="1"/>
     </row>
-    <row r="85" spans="1:170" ht="15">
+    <row r="85" spans="1:171" ht="15">
       <c r="A85" s="9">
         <v>24988445</v>
       </c>
@@ -81332,7 +81196,7 @@
       <c r="FI85" s="1"/>
       <c r="FJ85" s="1"/>
     </row>
-    <row r="86" spans="1:170" ht="15">
+    <row r="86" spans="1:171" ht="15">
       <c r="A86" s="9">
         <v>24988559</v>
       </c>
@@ -81466,7 +81330,7 @@
       <c r="FI86" s="1"/>
       <c r="FJ86" s="1"/>
     </row>
-    <row r="87" spans="1:170" ht="15">
+    <row r="87" spans="1:171" ht="15">
       <c r="A87" s="9">
         <v>24988692</v>
       </c>
@@ -81600,7 +81464,7 @@
       <c r="FI87" s="1"/>
       <c r="FJ87" s="1"/>
     </row>
-    <row r="88" spans="1:170" ht="15">
+    <row r="88" spans="1:171" ht="15">
       <c r="A88" s="9">
         <v>24923318</v>
       </c>
@@ -81777,8 +81641,11 @@
       <c r="FN88" s="4">
         <v>24</v>
       </c>
+      <c r="FO88" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="89" spans="1:170" ht="15">
+    <row r="89" spans="1:171" ht="15">
       <c r="A89" s="9">
         <v>24925212</v>
       </c>
@@ -81912,7 +81779,7 @@
       <c r="FI89" s="1"/>
       <c r="FJ89" s="1"/>
     </row>
-    <row r="90" spans="1:170" ht="15">
+    <row r="90" spans="1:171" ht="15">
       <c r="A90" s="9">
         <v>24857462</v>
       </c>
@@ -82091,8 +81958,11 @@
       <c r="FN90" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="FO90" s="4">
+        <v>12</v>
+      </c>
     </row>
-    <row r="91" spans="1:170" ht="15">
+    <row r="91" spans="1:171" ht="15">
       <c r="A91" s="10">
         <v>25112301</v>
       </c>
@@ -82132,8 +82002,11 @@
       <c r="FN91" s="4">
         <v>24</v>
       </c>
+      <c r="FO91" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="92" spans="1:170" ht="15">
+    <row r="92" spans="1:171" ht="15">
       <c r="A92" s="10">
         <v>25112300</v>
       </c>
@@ -82170,8 +82043,11 @@
       <c r="FN92" s="4">
         <v>24</v>
       </c>
+      <c r="FO92" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="93" spans="1:170" ht="15">
+    <row r="93" spans="1:171" ht="15">
       <c r="A93" s="10">
         <v>25087863</v>
       </c>
@@ -82211,8 +82087,11 @@
       <c r="FN93" s="4">
         <v>24</v>
       </c>
+      <c r="FO93" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="94" spans="1:170" ht="15">
+    <row r="94" spans="1:171" ht="15">
       <c r="A94" s="10">
         <v>25087787</v>
       </c>
@@ -82229,7 +82108,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="95" spans="1:170" ht="15">
+    <row r="95" spans="1:171" ht="15">
       <c r="A95" s="10">
         <v>24848184</v>
       </c>
@@ -82308,8 +82187,11 @@
       <c r="FN95" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="FO95" s="4">
+        <v>12</v>
+      </c>
     </row>
-    <row r="96" spans="1:170" ht="15">
+    <row r="96" spans="1:171" ht="15">
       <c r="A96" s="16">
         <v>50872159</v>
       </c>
@@ -82842,8 +82724,74 @@
       </c>
       <c r="F111" s="19"/>
     </row>
-    <row r="112" spans="1:167" ht="15"/>
-    <row r="113" ht="15"/>
+    <row r="112" spans="1:167" ht="15">
+      <c r="A112" s="10">
+        <v>72309509</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C112" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D112" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E112" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="15">
+      <c r="A113" s="10">
+        <v>72304210</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C113" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E113" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="15">
+      <c r="A114" s="10">
+        <v>25263837</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C114" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E114" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15">
+      <c r="A115" s="10">
+        <v>25264958</v>
+      </c>
+      <c r="B115" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C115" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D115" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" s="10">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun  5 11:34:58 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="455" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15BF28A8-7951-4C66-81B4-4CC648525F03}"/>
+  <xr:revisionPtr revIDLastSave="458" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15D03372-6191-4E5A-A244-EB58EB75B900}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="137">
   <si>
     <t>Module ID</t>
   </si>
@@ -975,8 +975,8 @@
   <dimension ref="A1:XFD115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FL82" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FO91" sqref="FO91"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="ES90" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A101" sqref="A101:XFD101"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -79722,23 +79722,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:171" ht="15">
+    <row r="75" spans="1:171" s="4" customFormat="1" ht="15">
       <c r="A75" s="9">
-        <v>24848800</v>
+        <v>24988445</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>28</v>
+        <v>102</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="E75" s="9">
-        <v>500</v>
+        <v>96</v>
       </c>
       <c r="F75" s="13"/>
+      <c r="P75" s="3"/>
       <c r="AY75" s="1"/>
       <c r="AZ75" s="1"/>
       <c r="BA75" s="1"/>
@@ -79856,23 +79857,24 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:171" ht="15">
+    <row r="76" spans="1:171" s="4" customFormat="1" ht="15">
       <c r="A76" s="9">
-        <v>24859051</v>
+        <v>24988559</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E76" s="9">
-        <v>500</v>
+        <v>96</v>
       </c>
       <c r="F76" s="13"/>
+      <c r="P76" s="3"/>
       <c r="AY76" s="1"/>
       <c r="AZ76" s="1"/>
       <c r="BA76" s="1"/>
@@ -79990,23 +79992,24 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:171" ht="15">
+    <row r="77" spans="1:171" s="4" customFormat="1" ht="15">
       <c r="A77" s="9">
-        <v>24848800</v>
+        <v>24988692</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="E77" s="9">
-        <v>500</v>
+        <v>162</v>
       </c>
       <c r="F77" s="13"/>
+      <c r="P77" s="3"/>
       <c r="AY77" s="1"/>
       <c r="AZ77" s="1"/>
       <c r="BA77" s="1"/>
@@ -80124,23 +80127,26 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:171" ht="15">
+    <row r="78" spans="1:171" s="4" customFormat="1" ht="15">
       <c r="A78" s="9">
-        <v>24859051</v>
+        <v>24923318</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E78" s="9">
-        <v>500</v>
-      </c>
-      <c r="F78" s="13"/>
+        <v>1000</v>
+      </c>
+      <c r="F78" s="13">
+        <v>45793</v>
+      </c>
+      <c r="P78" s="3"/>
       <c r="AY78" s="1"/>
       <c r="AZ78" s="1"/>
       <c r="BA78" s="1"/>
@@ -80242,39 +80248,85 @@
       <c r="ES78" s="1"/>
       <c r="ET78" s="1"/>
       <c r="EU78" s="1"/>
-      <c r="EV78" s="1"/>
-      <c r="EW78" s="1"/>
-      <c r="EX78" s="1"/>
-      <c r="EY78" s="1"/>
-      <c r="EZ78" s="1"/>
-      <c r="FA78" s="1"/>
-      <c r="FB78" s="1"/>
-      <c r="FC78" s="1"/>
-      <c r="FD78" s="1"/>
-      <c r="FE78" s="1"/>
-      <c r="FF78" s="1"/>
-      <c r="FG78" s="1"/>
-      <c r="FH78" s="1"/>
-      <c r="FI78" s="1"/>
-      <c r="FJ78" s="1"/>
+      <c r="EV78" s="1">
+        <v>12</v>
+      </c>
+      <c r="EW78" s="1">
+        <v>24</v>
+      </c>
+      <c r="EX78" s="1">
+        <v>24</v>
+      </c>
+      <c r="EY78" s="1">
+        <v>24</v>
+      </c>
+      <c r="EZ78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FA78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FB78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FC78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FD78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FE78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FF78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FG78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FH78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FI78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FJ78" s="1">
+        <v>24</v>
+      </c>
+      <c r="FK78" s="4">
+        <v>8</v>
+      </c>
+      <c r="FL78" s="4">
+        <v>14</v>
+      </c>
+      <c r="FM78" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN78" s="4">
+        <v>24</v>
+      </c>
+      <c r="FO78" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:171" ht="15">
+    <row r="79" spans="1:171" s="4" customFormat="1" ht="15">
       <c r="A79" s="9">
-        <v>24848800</v>
+        <v>24925212</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E79" s="9">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="F79" s="13"/>
+      <c r="P79" s="3"/>
       <c r="AY79" s="1"/>
       <c r="AZ79" s="1"/>
       <c r="BA79" s="1"/>
@@ -80392,23 +80444,26 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:171" ht="15">
+    <row r="80" spans="1:171" s="4" customFormat="1" ht="15">
       <c r="A80" s="9">
-        <v>24859051</v>
+        <v>24857462</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E80" s="9">
-        <v>500</v>
-      </c>
-      <c r="F80" s="13"/>
+        <v>200</v>
+      </c>
+      <c r="F80" s="13">
+        <v>45792</v>
+      </c>
+      <c r="P80" s="3"/>
       <c r="AY80" s="1"/>
       <c r="AZ80" s="1"/>
       <c r="BA80" s="1"/>
@@ -80509,1717 +80564,760 @@
       <c r="ER80" s="1"/>
       <c r="ES80" s="1"/>
       <c r="ET80" s="1"/>
-      <c r="EU80" s="1"/>
-      <c r="EV80" s="1"/>
-      <c r="EW80" s="1"/>
-      <c r="EX80" s="1"/>
-      <c r="EY80" s="1"/>
-      <c r="EZ80" s="1"/>
-      <c r="FA80" s="1"/>
-      <c r="FB80" s="1"/>
-      <c r="FC80" s="1"/>
-      <c r="FD80" s="1"/>
-      <c r="FE80" s="1"/>
-      <c r="FF80" s="1"/>
-      <c r="FG80" s="1"/>
-      <c r="FH80" s="1"/>
-      <c r="FI80" s="1"/>
-      <c r="FJ80" s="1"/>
+      <c r="EU80" s="1">
+        <v>8</v>
+      </c>
+      <c r="EV80" s="1">
+        <v>12</v>
+      </c>
+      <c r="EW80" s="1">
+        <v>12</v>
+      </c>
+      <c r="EX80" s="1">
+        <v>12</v>
+      </c>
+      <c r="EY80" s="1">
+        <v>12</v>
+      </c>
+      <c r="EZ80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FA80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FB80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FC80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FD80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FE80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FF80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FG80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FH80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FI80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FJ80" s="1">
+        <v>12</v>
+      </c>
+      <c r="FK80" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FL80" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FM80" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FN80" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FO80" s="4">
+        <v>12</v>
+      </c>
     </row>
-    <row r="81" spans="1:171" ht="15">
-      <c r="A81" s="9">
-        <v>24848800</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D81" s="9" t="s">
+    <row r="81" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A81" s="10">
+        <v>25112301</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E81" s="10">
+        <v>96</v>
+      </c>
+      <c r="F81" s="14">
+        <v>45806</v>
+      </c>
+      <c r="P81" s="3">
+        <v>45811</v>
+      </c>
+      <c r="FI81" s="4">
+        <v>11</v>
+      </c>
+      <c r="FJ81" s="4">
+        <v>24</v>
+      </c>
+      <c r="FK81" s="4">
+        <v>8</v>
+      </c>
+      <c r="FL81" s="4">
+        <v>14</v>
+      </c>
+      <c r="FM81" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN81" s="4">
+        <v>24</v>
+      </c>
+      <c r="FO81" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A82" s="10">
+        <v>25112300</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D82" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E81" s="9">
-        <v>500</v>
-      </c>
-      <c r="F81" s="13"/>
-      <c r="AY81" s="1"/>
-      <c r="AZ81" s="1"/>
-      <c r="BA81" s="1"/>
-      <c r="BB81" s="1"/>
-      <c r="BC81" s="1"/>
-      <c r="BD81" s="1"/>
-      <c r="BE81" s="1"/>
-      <c r="BF81" s="1"/>
-      <c r="BG81" s="1"/>
-      <c r="BH81" s="1"/>
-      <c r="BI81" s="1"/>
-      <c r="BJ81" s="1"/>
-      <c r="BK81" s="1"/>
-      <c r="BL81" s="1"/>
-      <c r="BM81" s="1"/>
-      <c r="BN81" s="1"/>
-      <c r="BO81" s="1"/>
-      <c r="BP81" s="1"/>
-      <c r="BQ81" s="1"/>
-      <c r="BR81" s="1"/>
-      <c r="BS81" s="1"/>
-      <c r="BT81" s="1"/>
-      <c r="BU81" s="1"/>
-      <c r="BV81" s="1"/>
-      <c r="BW81" s="1"/>
-      <c r="BX81" s="1"/>
-      <c r="BY81" s="1"/>
-      <c r="BZ81" s="1"/>
-      <c r="CA81" s="1"/>
-      <c r="CB81" s="1"/>
-      <c r="CC81" s="1"/>
-      <c r="CD81" s="1"/>
-      <c r="CE81" s="1"/>
-      <c r="CF81" s="1"/>
-      <c r="CG81" s="1"/>
-      <c r="CH81" s="1"/>
-      <c r="CI81" s="1"/>
-      <c r="CJ81" s="1"/>
-      <c r="CK81" s="1"/>
-      <c r="CL81" s="1"/>
-      <c r="CM81" s="1"/>
-      <c r="CN81" s="1"/>
-      <c r="CO81" s="1"/>
-      <c r="CP81" s="1"/>
-      <c r="CQ81" s="1"/>
-      <c r="CR81" s="1"/>
-      <c r="CS81" s="1"/>
-      <c r="CT81" s="1"/>
-      <c r="CU81" s="1"/>
-      <c r="CV81" s="1"/>
-      <c r="CW81" s="1"/>
-      <c r="CX81" s="1"/>
-      <c r="CY81" s="1"/>
-      <c r="CZ81" s="1"/>
-      <c r="DA81" s="1"/>
-      <c r="DB81" s="1"/>
-      <c r="DC81" s="1"/>
-      <c r="DD81" s="1"/>
-      <c r="DE81" s="1"/>
-      <c r="DF81" s="1"/>
-      <c r="DG81" s="1"/>
-      <c r="DH81" s="1"/>
-      <c r="DI81" s="1"/>
-      <c r="DJ81" s="1"/>
-      <c r="DK81" s="1"/>
-      <c r="DL81" s="1"/>
-      <c r="DM81" s="1"/>
-      <c r="DN81" s="1"/>
-      <c r="DO81" s="1"/>
-      <c r="DP81" s="1"/>
-      <c r="DQ81" s="1"/>
-      <c r="DR81" s="1"/>
-      <c r="DS81" s="1"/>
-      <c r="DT81" s="1"/>
-      <c r="DU81" s="1"/>
-      <c r="DV81" s="1"/>
-      <c r="DW81" s="1"/>
-      <c r="DX81" s="1"/>
-      <c r="DY81" s="1"/>
-      <c r="DZ81" s="1"/>
-      <c r="EA81" s="1"/>
-      <c r="EB81" s="1"/>
-      <c r="EC81" s="1"/>
-      <c r="ED81" s="1"/>
-      <c r="EE81" s="1"/>
-      <c r="EF81" s="1"/>
-      <c r="EG81" s="1"/>
-      <c r="EH81" s="1"/>
-      <c r="EI81" s="1"/>
-      <c r="EJ81" s="1"/>
-      <c r="EK81" s="1"/>
-      <c r="EL81" s="1"/>
-      <c r="EM81" s="1"/>
-      <c r="EN81" s="1"/>
-      <c r="EO81" s="1"/>
-      <c r="EP81" s="1"/>
-      <c r="EQ81" s="1"/>
-      <c r="ER81" s="1"/>
-      <c r="ES81" s="1"/>
-      <c r="ET81" s="1"/>
-      <c r="EU81" s="1"/>
-      <c r="EV81" s="1"/>
-      <c r="EW81" s="1"/>
-      <c r="EX81" s="1"/>
-      <c r="EY81" s="1"/>
-      <c r="EZ81" s="1"/>
-      <c r="FA81" s="1"/>
-      <c r="FB81" s="1"/>
-      <c r="FC81" s="1"/>
-      <c r="FD81" s="1"/>
-      <c r="FE81" s="1"/>
-      <c r="FF81" s="1"/>
-      <c r="FG81" s="1"/>
-      <c r="FH81" s="1"/>
-      <c r="FI81" s="1"/>
-      <c r="FJ81" s="1"/>
+      <c r="E82" s="10">
+        <v>1000</v>
+      </c>
+      <c r="F82" s="14">
+        <v>45806</v>
+      </c>
+      <c r="P82" s="3"/>
+      <c r="FI82" s="4">
+        <v>11</v>
+      </c>
+      <c r="FJ82" s="4">
+        <v>24</v>
+      </c>
+      <c r="FK82" s="4">
+        <v>8</v>
+      </c>
+      <c r="FL82" s="4">
+        <v>14</v>
+      </c>
+      <c r="FM82" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN82" s="4">
+        <v>24</v>
+      </c>
+      <c r="FO82" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="82" spans="1:171" ht="15">
-      <c r="A82" s="9">
-        <v>24859051</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C82" s="2" t="s">
+    <row r="83" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A83" s="10">
+        <v>25087863</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83" s="10">
+        <v>96</v>
+      </c>
+      <c r="F83" s="14">
+        <v>45806</v>
+      </c>
+      <c r="P83" s="3">
+        <v>45811</v>
+      </c>
+      <c r="FI83" s="4">
+        <v>11</v>
+      </c>
+      <c r="FJ83" s="4">
+        <v>24</v>
+      </c>
+      <c r="FK83" s="4">
+        <v>8</v>
+      </c>
+      <c r="FL83" s="4">
+        <v>14</v>
+      </c>
+      <c r="FM83" s="4">
+        <v>24</v>
+      </c>
+      <c r="FN83" s="4">
+        <v>24</v>
+      </c>
+      <c r="FO83" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A84" s="10">
+        <v>25087787</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" s="10">
+        <v>1000</v>
+      </c>
+      <c r="F84" s="14"/>
+      <c r="P84" s="3"/>
+    </row>
+    <row r="85" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A85" s="10">
+        <v>24848184</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="D85" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="9">
+        <v>200</v>
+      </c>
+      <c r="F85" s="13">
+        <v>45792</v>
+      </c>
+      <c r="P85" s="3"/>
+      <c r="EU85" s="4">
+        <v>8</v>
+      </c>
+      <c r="EV85" s="4">
+        <v>12</v>
+      </c>
+      <c r="EW85" s="4">
+        <v>12</v>
+      </c>
+      <c r="EX85" s="4">
+        <v>12</v>
+      </c>
+      <c r="EY85" s="4">
+        <v>12</v>
+      </c>
+      <c r="EZ85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FA85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FB85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FC85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FD85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FE85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FF85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FG85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FH85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FI85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FJ85" s="4">
+        <v>12</v>
+      </c>
+      <c r="FK85" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FL85" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FM85" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FN85" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="FO85" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A86" s="16">
+        <v>50872159</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E86" s="16">
+        <v>192</v>
+      </c>
+      <c r="F86" s="19">
+        <v>45793</v>
+      </c>
+      <c r="P86" s="3"/>
+    </row>
+    <row r="87" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A87" s="16">
+        <v>25019645</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D87" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E87" s="16">
+        <v>96</v>
+      </c>
+      <c r="F87" s="19"/>
+      <c r="P87" s="3"/>
+    </row>
+    <row r="88" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A88" s="16">
+        <v>25017936</v>
+      </c>
+      <c r="B88" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E88" s="16">
+        <v>96</v>
+      </c>
+      <c r="F88" s="19"/>
+      <c r="P88" s="3"/>
+    </row>
+    <row r="89" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A89" s="16">
+        <v>25089372</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E89" s="16">
+        <v>60</v>
+      </c>
+      <c r="F89" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P89" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ89" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK89" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A90" s="16">
+        <v>25089365</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D90" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E90" s="16">
+        <v>60</v>
+      </c>
+      <c r="F90" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P90" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ90" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK90" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A91" s="16">
+        <v>25089363</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E91" s="16">
+        <v>60</v>
+      </c>
+      <c r="F91" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P91" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ91" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK91" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A92" s="16">
+        <v>25089370</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E92" s="16">
+        <v>60</v>
+      </c>
+      <c r="F92" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P92" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ92" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK92" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A93" s="16">
+        <v>25112299</v>
+      </c>
+      <c r="B93" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E93" s="16">
+        <v>60</v>
+      </c>
+      <c r="F93" s="19">
+        <v>45797</v>
+      </c>
+      <c r="P93" s="3">
+        <v>45808</v>
+      </c>
+      <c r="EZ93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FA93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FB93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FC93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FD93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FE93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FF93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FG93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FH93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FI93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FJ93" s="4">
+        <v>5</v>
+      </c>
+      <c r="FK93" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A94" s="16">
+        <v>72149637</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E94" s="16">
+        <v>50</v>
+      </c>
+      <c r="F94" s="19">
+        <v>45796</v>
+      </c>
+      <c r="P94" s="3">
+        <v>45806</v>
+      </c>
+      <c r="EY94" s="4">
+        <v>8</v>
+      </c>
+      <c r="EZ94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FA94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FB94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FC94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FD94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FE94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FF94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FG94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FH94" s="4">
+        <v>12</v>
+      </c>
+      <c r="FI94" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:171" s="4" customFormat="1" ht="15">
+      <c r="A95" s="16">
+        <v>72238923</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D95" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E82" s="9">
-        <v>500</v>
-      </c>
-      <c r="F82" s="13"/>
-      <c r="AY82" s="1"/>
-      <c r="AZ82" s="1"/>
-      <c r="BA82" s="1"/>
-      <c r="BB82" s="1"/>
-      <c r="BC82" s="1"/>
-      <c r="BD82" s="1"/>
-      <c r="BE82" s="1"/>
-      <c r="BF82" s="1"/>
-      <c r="BG82" s="1"/>
-      <c r="BH82" s="1"/>
-      <c r="BI82" s="1"/>
-      <c r="BJ82" s="1"/>
-      <c r="BK82" s="1"/>
-      <c r="BL82" s="1"/>
-      <c r="BM82" s="1"/>
-      <c r="BN82" s="1"/>
-      <c r="BO82" s="1"/>
-      <c r="BP82" s="1"/>
-      <c r="BQ82" s="1"/>
-      <c r="BR82" s="1"/>
-      <c r="BS82" s="1"/>
-      <c r="BT82" s="1"/>
-      <c r="BU82" s="1"/>
-      <c r="BV82" s="1"/>
-      <c r="BW82" s="1"/>
-      <c r="BX82" s="1"/>
-      <c r="BY82" s="1"/>
-      <c r="BZ82" s="1"/>
-      <c r="CA82" s="1"/>
-      <c r="CB82" s="1"/>
-      <c r="CC82" s="1"/>
-      <c r="CD82" s="1"/>
-      <c r="CE82" s="1"/>
-      <c r="CF82" s="1"/>
-      <c r="CG82" s="1"/>
-      <c r="CH82" s="1"/>
-      <c r="CI82" s="1"/>
-      <c r="CJ82" s="1"/>
-      <c r="CK82" s="1"/>
-      <c r="CL82" s="1"/>
-      <c r="CM82" s="1"/>
-      <c r="CN82" s="1"/>
-      <c r="CO82" s="1"/>
-      <c r="CP82" s="1"/>
-      <c r="CQ82" s="1"/>
-      <c r="CR82" s="1"/>
-      <c r="CS82" s="1"/>
-      <c r="CT82" s="1"/>
-      <c r="CU82" s="1"/>
-      <c r="CV82" s="1"/>
-      <c r="CW82" s="1"/>
-      <c r="CX82" s="1"/>
-      <c r="CY82" s="1"/>
-      <c r="CZ82" s="1"/>
-      <c r="DA82" s="1"/>
-      <c r="DB82" s="1"/>
-      <c r="DC82" s="1"/>
-      <c r="DD82" s="1"/>
-      <c r="DE82" s="1"/>
-      <c r="DF82" s="1"/>
-      <c r="DG82" s="1"/>
-      <c r="DH82" s="1"/>
-      <c r="DI82" s="1"/>
-      <c r="DJ82" s="1"/>
-      <c r="DK82" s="1"/>
-      <c r="DL82" s="1"/>
-      <c r="DM82" s="1"/>
-      <c r="DN82" s="1"/>
-      <c r="DO82" s="1"/>
-      <c r="DP82" s="1"/>
-      <c r="DQ82" s="1"/>
-      <c r="DR82" s="1"/>
-      <c r="DS82" s="1"/>
-      <c r="DT82" s="1"/>
-      <c r="DU82" s="1"/>
-      <c r="DV82" s="1"/>
-      <c r="DW82" s="1"/>
-      <c r="DX82" s="1"/>
-      <c r="DY82" s="1"/>
-      <c r="DZ82" s="1"/>
-      <c r="EA82" s="1"/>
-      <c r="EB82" s="1"/>
-      <c r="EC82" s="1"/>
-      <c r="ED82" s="1"/>
-      <c r="EE82" s="1"/>
-      <c r="EF82" s="1"/>
-      <c r="EG82" s="1"/>
-      <c r="EH82" s="1"/>
-      <c r="EI82" s="1"/>
-      <c r="EJ82" s="1"/>
-      <c r="EK82" s="1"/>
-      <c r="EL82" s="1"/>
-      <c r="EM82" s="1"/>
-      <c r="EN82" s="1"/>
-      <c r="EO82" s="1"/>
-      <c r="EP82" s="1"/>
-      <c r="EQ82" s="1"/>
-      <c r="ER82" s="1"/>
-      <c r="ES82" s="1"/>
-      <c r="ET82" s="1"/>
-      <c r="EU82" s="1"/>
-      <c r="EV82" s="1"/>
-      <c r="EW82" s="1"/>
-      <c r="EX82" s="1"/>
-      <c r="EY82" s="1"/>
-      <c r="EZ82" s="1"/>
-      <c r="FA82" s="1"/>
-      <c r="FB82" s="1"/>
-      <c r="FC82" s="1"/>
-      <c r="FD82" s="1"/>
-      <c r="FE82" s="1"/>
-      <c r="FF82" s="1"/>
-      <c r="FG82" s="1"/>
-      <c r="FH82" s="1"/>
-      <c r="FI82" s="1"/>
-      <c r="FJ82" s="1"/>
+      <c r="E95" s="16">
+        <v>1000</v>
+      </c>
+      <c r="F95" s="19"/>
+      <c r="P95" s="3"/>
     </row>
-    <row r="83" spans="1:171" ht="15">
-      <c r="A83" s="9">
-        <v>24848800</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E83" s="9">
-        <v>500</v>
-      </c>
-      <c r="F83" s="13"/>
-      <c r="AY83" s="1"/>
-      <c r="AZ83" s="1"/>
-      <c r="BA83" s="1"/>
-      <c r="BB83" s="1"/>
-      <c r="BC83" s="1"/>
-      <c r="BD83" s="1"/>
-      <c r="BE83" s="1"/>
-      <c r="BF83" s="1"/>
-      <c r="BG83" s="1"/>
-      <c r="BH83" s="1"/>
-      <c r="BI83" s="1"/>
-      <c r="BJ83" s="1"/>
-      <c r="BK83" s="1"/>
-      <c r="BL83" s="1"/>
-      <c r="BM83" s="1"/>
-      <c r="BN83" s="1"/>
-      <c r="BO83" s="1"/>
-      <c r="BP83" s="1"/>
-      <c r="BQ83" s="1"/>
-      <c r="BR83" s="1"/>
-      <c r="BS83" s="1"/>
-      <c r="BT83" s="1"/>
-      <c r="BU83" s="1"/>
-      <c r="BV83" s="1"/>
-      <c r="BW83" s="1"/>
-      <c r="BX83" s="1"/>
-      <c r="BY83" s="1"/>
-      <c r="BZ83" s="1"/>
-      <c r="CA83" s="1"/>
-      <c r="CB83" s="1"/>
-      <c r="CC83" s="1"/>
-      <c r="CD83" s="1"/>
-      <c r="CE83" s="1"/>
-      <c r="CF83" s="1"/>
-      <c r="CG83" s="1"/>
-      <c r="CH83" s="1"/>
-      <c r="CI83" s="1"/>
-      <c r="CJ83" s="1"/>
-      <c r="CK83" s="1"/>
-      <c r="CL83" s="1"/>
-      <c r="CM83" s="1"/>
-      <c r="CN83" s="1"/>
-      <c r="CO83" s="1"/>
-      <c r="CP83" s="1"/>
-      <c r="CQ83" s="1"/>
-      <c r="CR83" s="1"/>
-      <c r="CS83" s="1"/>
-      <c r="CT83" s="1"/>
-      <c r="CU83" s="1"/>
-      <c r="CV83" s="1"/>
-      <c r="CW83" s="1"/>
-      <c r="CX83" s="1"/>
-      <c r="CY83" s="1"/>
-      <c r="CZ83" s="1"/>
-      <c r="DA83" s="1"/>
-      <c r="DB83" s="1"/>
-      <c r="DC83" s="1"/>
-      <c r="DD83" s="1"/>
-      <c r="DE83" s="1"/>
-      <c r="DF83" s="1"/>
-      <c r="DG83" s="1"/>
-      <c r="DH83" s="1"/>
-      <c r="DI83" s="1"/>
-      <c r="DJ83" s="1"/>
-      <c r="DK83" s="1"/>
-      <c r="DL83" s="1"/>
-      <c r="DM83" s="1"/>
-      <c r="DN83" s="1"/>
-      <c r="DO83" s="1"/>
-      <c r="DP83" s="1"/>
-      <c r="DQ83" s="1"/>
-      <c r="DR83" s="1"/>
-      <c r="DS83" s="1"/>
-      <c r="DT83" s="1"/>
-      <c r="DU83" s="1"/>
-      <c r="DV83" s="1"/>
-      <c r="DW83" s="1"/>
-      <c r="DX83" s="1"/>
-      <c r="DY83" s="1"/>
-      <c r="DZ83" s="1"/>
-      <c r="EA83" s="1"/>
-      <c r="EB83" s="1"/>
-      <c r="EC83" s="1"/>
-      <c r="ED83" s="1"/>
-      <c r="EE83" s="1"/>
-      <c r="EF83" s="1"/>
-      <c r="EG83" s="1"/>
-      <c r="EH83" s="1"/>
-      <c r="EI83" s="1"/>
-      <c r="EJ83" s="1"/>
-      <c r="EK83" s="1"/>
-      <c r="EL83" s="1"/>
-      <c r="EM83" s="1"/>
-      <c r="EN83" s="1"/>
-      <c r="EO83" s="1"/>
-      <c r="EP83" s="1"/>
-      <c r="EQ83" s="1"/>
-      <c r="ER83" s="1"/>
-      <c r="ES83" s="1"/>
-      <c r="ET83" s="1"/>
-      <c r="EU83" s="1"/>
-      <c r="EV83" s="1"/>
-      <c r="EW83" s="1"/>
-      <c r="EX83" s="1"/>
-      <c r="EY83" s="1"/>
-      <c r="EZ83" s="1"/>
-      <c r="FA83" s="1"/>
-      <c r="FB83" s="1"/>
-      <c r="FC83" s="1"/>
-      <c r="FD83" s="1"/>
-      <c r="FE83" s="1"/>
-      <c r="FF83" s="1"/>
-      <c r="FG83" s="1"/>
-      <c r="FH83" s="1"/>
-      <c r="FI83" s="1"/>
-      <c r="FJ83" s="1"/>
-    </row>
-    <row r="84" spans="1:171" ht="15">
-      <c r="A84" s="9">
-        <v>24859051</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E84" s="9">
-        <v>500</v>
-      </c>
-      <c r="F84" s="13"/>
-      <c r="AY84" s="1"/>
-      <c r="AZ84" s="1"/>
-      <c r="BA84" s="1"/>
-      <c r="BB84" s="1"/>
-      <c r="BC84" s="1"/>
-      <c r="BD84" s="1"/>
-      <c r="BE84" s="1"/>
-      <c r="BF84" s="1"/>
-      <c r="BG84" s="1"/>
-      <c r="BH84" s="1"/>
-      <c r="BI84" s="1"/>
-      <c r="BJ84" s="1"/>
-      <c r="BK84" s="1"/>
-      <c r="BL84" s="1"/>
-      <c r="BM84" s="1"/>
-      <c r="BN84" s="1"/>
-      <c r="BO84" s="1"/>
-      <c r="BP84" s="1"/>
-      <c r="BQ84" s="1"/>
-      <c r="BR84" s="1"/>
-      <c r="BS84" s="1"/>
-      <c r="BT84" s="1"/>
-      <c r="BU84" s="1"/>
-      <c r="BV84" s="1"/>
-      <c r="BW84" s="1"/>
-      <c r="BX84" s="1"/>
-      <c r="BY84" s="1"/>
-      <c r="BZ84" s="1"/>
-      <c r="CA84" s="1"/>
-      <c r="CB84" s="1"/>
-      <c r="CC84" s="1"/>
-      <c r="CD84" s="1"/>
-      <c r="CE84" s="1"/>
-      <c r="CF84" s="1"/>
-      <c r="CG84" s="1"/>
-      <c r="CH84" s="1"/>
-      <c r="CI84" s="1"/>
-      <c r="CJ84" s="1"/>
-      <c r="CK84" s="1"/>
-      <c r="CL84" s="1"/>
-      <c r="CM84" s="1"/>
-      <c r="CN84" s="1"/>
-      <c r="CO84" s="1"/>
-      <c r="CP84" s="1"/>
-      <c r="CQ84" s="1"/>
-      <c r="CR84" s="1"/>
-      <c r="CS84" s="1"/>
-      <c r="CT84" s="1"/>
-      <c r="CU84" s="1"/>
-      <c r="CV84" s="1"/>
-      <c r="CW84" s="1"/>
-      <c r="CX84" s="1"/>
-      <c r="CY84" s="1"/>
-      <c r="CZ84" s="1"/>
-      <c r="DA84" s="1"/>
-      <c r="DB84" s="1"/>
-      <c r="DC84" s="1"/>
-      <c r="DD84" s="1"/>
-      <c r="DE84" s="1"/>
-      <c r="DF84" s="1"/>
-      <c r="DG84" s="1"/>
-      <c r="DH84" s="1"/>
-      <c r="DI84" s="1"/>
-      <c r="DJ84" s="1"/>
-      <c r="DK84" s="1"/>
-      <c r="DL84" s="1"/>
-      <c r="DM84" s="1"/>
-      <c r="DN84" s="1"/>
-      <c r="DO84" s="1"/>
-      <c r="DP84" s="1"/>
-      <c r="DQ84" s="1"/>
-      <c r="DR84" s="1"/>
-      <c r="DS84" s="1"/>
-      <c r="DT84" s="1"/>
-      <c r="DU84" s="1"/>
-      <c r="DV84" s="1"/>
-      <c r="DW84" s="1"/>
-      <c r="DX84" s="1"/>
-      <c r="DY84" s="1"/>
-      <c r="DZ84" s="1"/>
-      <c r="EA84" s="1"/>
-      <c r="EB84" s="1"/>
-      <c r="EC84" s="1"/>
-      <c r="ED84" s="1"/>
-      <c r="EE84" s="1"/>
-      <c r="EF84" s="1"/>
-      <c r="EG84" s="1"/>
-      <c r="EH84" s="1"/>
-      <c r="EI84" s="1"/>
-      <c r="EJ84" s="1"/>
-      <c r="EK84" s="1"/>
-      <c r="EL84" s="1"/>
-      <c r="EM84" s="1"/>
-      <c r="EN84" s="1"/>
-      <c r="EO84" s="1"/>
-      <c r="EP84" s="1"/>
-      <c r="EQ84" s="1"/>
-      <c r="ER84" s="1"/>
-      <c r="ES84" s="1"/>
-      <c r="ET84" s="1"/>
-      <c r="EU84" s="1"/>
-      <c r="EV84" s="1"/>
-      <c r="EW84" s="1"/>
-      <c r="EX84" s="1"/>
-      <c r="EY84" s="1"/>
-      <c r="EZ84" s="1"/>
-      <c r="FA84" s="1"/>
-      <c r="FB84" s="1"/>
-      <c r="FC84" s="1"/>
-      <c r="FD84" s="1"/>
-      <c r="FE84" s="1"/>
-      <c r="FF84" s="1"/>
-      <c r="FG84" s="1"/>
-      <c r="FH84" s="1"/>
-      <c r="FI84" s="1"/>
-      <c r="FJ84" s="1"/>
-    </row>
-    <row r="85" spans="1:171" ht="15">
-      <c r="A85" s="9">
-        <v>24988445</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E85" s="9">
-        <v>96</v>
-      </c>
-      <c r="F85" s="13"/>
-      <c r="AY85" s="1"/>
-      <c r="AZ85" s="1"/>
-      <c r="BA85" s="1"/>
-      <c r="BB85" s="1"/>
-      <c r="BC85" s="1"/>
-      <c r="BD85" s="1"/>
-      <c r="BE85" s="1"/>
-      <c r="BF85" s="1"/>
-      <c r="BG85" s="1"/>
-      <c r="BH85" s="1"/>
-      <c r="BI85" s="1"/>
-      <c r="BJ85" s="1"/>
-      <c r="BK85" s="1"/>
-      <c r="BL85" s="1"/>
-      <c r="BM85" s="1"/>
-      <c r="BN85" s="1"/>
-      <c r="BO85" s="1"/>
-      <c r="BP85" s="1"/>
-      <c r="BQ85" s="1"/>
-      <c r="BR85" s="1"/>
-      <c r="BS85" s="1"/>
-      <c r="BT85" s="1"/>
-      <c r="BU85" s="1"/>
-      <c r="BV85" s="1"/>
-      <c r="BW85" s="1"/>
-      <c r="BX85" s="1"/>
-      <c r="BY85" s="1"/>
-      <c r="BZ85" s="1"/>
-      <c r="CA85" s="1"/>
-      <c r="CB85" s="1"/>
-      <c r="CC85" s="1"/>
-      <c r="CD85" s="1"/>
-      <c r="CE85" s="1"/>
-      <c r="CF85" s="1"/>
-      <c r="CG85" s="1"/>
-      <c r="CH85" s="1"/>
-      <c r="CI85" s="1"/>
-      <c r="CJ85" s="1"/>
-      <c r="CK85" s="1"/>
-      <c r="CL85" s="1"/>
-      <c r="CM85" s="1"/>
-      <c r="CN85" s="1"/>
-      <c r="CO85" s="1"/>
-      <c r="CP85" s="1"/>
-      <c r="CQ85" s="1"/>
-      <c r="CR85" s="1"/>
-      <c r="CS85" s="1"/>
-      <c r="CT85" s="1"/>
-      <c r="CU85" s="1"/>
-      <c r="CV85" s="1"/>
-      <c r="CW85" s="1"/>
-      <c r="CX85" s="1"/>
-      <c r="CY85" s="1"/>
-      <c r="CZ85" s="1"/>
-      <c r="DA85" s="1"/>
-      <c r="DB85" s="1"/>
-      <c r="DC85" s="1"/>
-      <c r="DD85" s="1"/>
-      <c r="DE85" s="1"/>
-      <c r="DF85" s="1"/>
-      <c r="DG85" s="1"/>
-      <c r="DH85" s="1"/>
-      <c r="DI85" s="1"/>
-      <c r="DJ85" s="1"/>
-      <c r="DK85" s="1"/>
-      <c r="DL85" s="1"/>
-      <c r="DM85" s="1"/>
-      <c r="DN85" s="1"/>
-      <c r="DO85" s="1"/>
-      <c r="DP85" s="1"/>
-      <c r="DQ85" s="1"/>
-      <c r="DR85" s="1"/>
-      <c r="DS85" s="1"/>
-      <c r="DT85" s="1"/>
-      <c r="DU85" s="1"/>
-      <c r="DV85" s="1"/>
-      <c r="DW85" s="1"/>
-      <c r="DX85" s="1"/>
-      <c r="DY85" s="1"/>
-      <c r="DZ85" s="1"/>
-      <c r="EA85" s="1"/>
-      <c r="EB85" s="1"/>
-      <c r="EC85" s="1"/>
-      <c r="ED85" s="1"/>
-      <c r="EE85" s="1"/>
-      <c r="EF85" s="1"/>
-      <c r="EG85" s="1"/>
-      <c r="EH85" s="1"/>
-      <c r="EI85" s="1"/>
-      <c r="EJ85" s="1"/>
-      <c r="EK85" s="1"/>
-      <c r="EL85" s="1"/>
-      <c r="EM85" s="1"/>
-      <c r="EN85" s="1"/>
-      <c r="EO85" s="1"/>
-      <c r="EP85" s="1"/>
-      <c r="EQ85" s="1"/>
-      <c r="ER85" s="1"/>
-      <c r="ES85" s="1"/>
-      <c r="ET85" s="1"/>
-      <c r="EU85" s="1"/>
-      <c r="EV85" s="1"/>
-      <c r="EW85" s="1"/>
-      <c r="EX85" s="1"/>
-      <c r="EY85" s="1"/>
-      <c r="EZ85" s="1"/>
-      <c r="FA85" s="1"/>
-      <c r="FB85" s="1"/>
-      <c r="FC85" s="1"/>
-      <c r="FD85" s="1"/>
-      <c r="FE85" s="1"/>
-      <c r="FF85" s="1"/>
-      <c r="FG85" s="1"/>
-      <c r="FH85" s="1"/>
-      <c r="FI85" s="1"/>
-      <c r="FJ85" s="1"/>
-    </row>
-    <row r="86" spans="1:171" ht="15">
-      <c r="A86" s="9">
-        <v>24988559</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E86" s="9">
-        <v>96</v>
-      </c>
-      <c r="F86" s="13"/>
-      <c r="AY86" s="1"/>
-      <c r="AZ86" s="1"/>
-      <c r="BA86" s="1"/>
-      <c r="BB86" s="1"/>
-      <c r="BC86" s="1"/>
-      <c r="BD86" s="1"/>
-      <c r="BE86" s="1"/>
-      <c r="BF86" s="1"/>
-      <c r="BG86" s="1"/>
-      <c r="BH86" s="1"/>
-      <c r="BI86" s="1"/>
-      <c r="BJ86" s="1"/>
-      <c r="BK86" s="1"/>
-      <c r="BL86" s="1"/>
-      <c r="BM86" s="1"/>
-      <c r="BN86" s="1"/>
-      <c r="BO86" s="1"/>
-      <c r="BP86" s="1"/>
-      <c r="BQ86" s="1"/>
-      <c r="BR86" s="1"/>
-      <c r="BS86" s="1"/>
-      <c r="BT86" s="1"/>
-      <c r="BU86" s="1"/>
-      <c r="BV86" s="1"/>
-      <c r="BW86" s="1"/>
-      <c r="BX86" s="1"/>
-      <c r="BY86" s="1"/>
-      <c r="BZ86" s="1"/>
-      <c r="CA86" s="1"/>
-      <c r="CB86" s="1"/>
-      <c r="CC86" s="1"/>
-      <c r="CD86" s="1"/>
-      <c r="CE86" s="1"/>
-      <c r="CF86" s="1"/>
-      <c r="CG86" s="1"/>
-      <c r="CH86" s="1"/>
-      <c r="CI86" s="1"/>
-      <c r="CJ86" s="1"/>
-      <c r="CK86" s="1"/>
-      <c r="CL86" s="1"/>
-      <c r="CM86" s="1"/>
-      <c r="CN86" s="1"/>
-      <c r="CO86" s="1"/>
-      <c r="CP86" s="1"/>
-      <c r="CQ86" s="1"/>
-      <c r="CR86" s="1"/>
-      <c r="CS86" s="1"/>
-      <c r="CT86" s="1"/>
-      <c r="CU86" s="1"/>
-      <c r="CV86" s="1"/>
-      <c r="CW86" s="1"/>
-      <c r="CX86" s="1"/>
-      <c r="CY86" s="1"/>
-      <c r="CZ86" s="1"/>
-      <c r="DA86" s="1"/>
-      <c r="DB86" s="1"/>
-      <c r="DC86" s="1"/>
-      <c r="DD86" s="1"/>
-      <c r="DE86" s="1"/>
-      <c r="DF86" s="1"/>
-      <c r="DG86" s="1"/>
-      <c r="DH86" s="1"/>
-      <c r="DI86" s="1"/>
-      <c r="DJ86" s="1"/>
-      <c r="DK86" s="1"/>
-      <c r="DL86" s="1"/>
-      <c r="DM86" s="1"/>
-      <c r="DN86" s="1"/>
-      <c r="DO86" s="1"/>
-      <c r="DP86" s="1"/>
-      <c r="DQ86" s="1"/>
-      <c r="DR86" s="1"/>
-      <c r="DS86" s="1"/>
-      <c r="DT86" s="1"/>
-      <c r="DU86" s="1"/>
-      <c r="DV86" s="1"/>
-      <c r="DW86" s="1"/>
-      <c r="DX86" s="1"/>
-      <c r="DY86" s="1"/>
-      <c r="DZ86" s="1"/>
-      <c r="EA86" s="1"/>
-      <c r="EB86" s="1"/>
-      <c r="EC86" s="1"/>
-      <c r="ED86" s="1"/>
-      <c r="EE86" s="1"/>
-      <c r="EF86" s="1"/>
-      <c r="EG86" s="1"/>
-      <c r="EH86" s="1"/>
-      <c r="EI86" s="1"/>
-      <c r="EJ86" s="1"/>
-      <c r="EK86" s="1"/>
-      <c r="EL86" s="1"/>
-      <c r="EM86" s="1"/>
-      <c r="EN86" s="1"/>
-      <c r="EO86" s="1"/>
-      <c r="EP86" s="1"/>
-      <c r="EQ86" s="1"/>
-      <c r="ER86" s="1"/>
-      <c r="ES86" s="1"/>
-      <c r="ET86" s="1"/>
-      <c r="EU86" s="1"/>
-      <c r="EV86" s="1"/>
-      <c r="EW86" s="1"/>
-      <c r="EX86" s="1"/>
-      <c r="EY86" s="1"/>
-      <c r="EZ86" s="1"/>
-      <c r="FA86" s="1"/>
-      <c r="FB86" s="1"/>
-      <c r="FC86" s="1"/>
-      <c r="FD86" s="1"/>
-      <c r="FE86" s="1"/>
-      <c r="FF86" s="1"/>
-      <c r="FG86" s="1"/>
-      <c r="FH86" s="1"/>
-      <c r="FI86" s="1"/>
-      <c r="FJ86" s="1"/>
-    </row>
-    <row r="87" spans="1:171" ht="15">
-      <c r="A87" s="9">
-        <v>24988692</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E87" s="9">
-        <v>162</v>
-      </c>
-      <c r="F87" s="13"/>
-      <c r="AY87" s="1"/>
-      <c r="AZ87" s="1"/>
-      <c r="BA87" s="1"/>
-      <c r="BB87" s="1"/>
-      <c r="BC87" s="1"/>
-      <c r="BD87" s="1"/>
-      <c r="BE87" s="1"/>
-      <c r="BF87" s="1"/>
-      <c r="BG87" s="1"/>
-      <c r="BH87" s="1"/>
-      <c r="BI87" s="1"/>
-      <c r="BJ87" s="1"/>
-      <c r="BK87" s="1"/>
-      <c r="BL87" s="1"/>
-      <c r="BM87" s="1"/>
-      <c r="BN87" s="1"/>
-      <c r="BO87" s="1"/>
-      <c r="BP87" s="1"/>
-      <c r="BQ87" s="1"/>
-      <c r="BR87" s="1"/>
-      <c r="BS87" s="1"/>
-      <c r="BT87" s="1"/>
-      <c r="BU87" s="1"/>
-      <c r="BV87" s="1"/>
-      <c r="BW87" s="1"/>
-      <c r="BX87" s="1"/>
-      <c r="BY87" s="1"/>
-      <c r="BZ87" s="1"/>
-      <c r="CA87" s="1"/>
-      <c r="CB87" s="1"/>
-      <c r="CC87" s="1"/>
-      <c r="CD87" s="1"/>
-      <c r="CE87" s="1"/>
-      <c r="CF87" s="1"/>
-      <c r="CG87" s="1"/>
-      <c r="CH87" s="1"/>
-      <c r="CI87" s="1"/>
-      <c r="CJ87" s="1"/>
-      <c r="CK87" s="1"/>
-      <c r="CL87" s="1"/>
-      <c r="CM87" s="1"/>
-      <c r="CN87" s="1"/>
-      <c r="CO87" s="1"/>
-      <c r="CP87" s="1"/>
-      <c r="CQ87" s="1"/>
-      <c r="CR87" s="1"/>
-      <c r="CS87" s="1"/>
-      <c r="CT87" s="1"/>
-      <c r="CU87" s="1"/>
-      <c r="CV87" s="1"/>
-      <c r="CW87" s="1"/>
-      <c r="CX87" s="1"/>
-      <c r="CY87" s="1"/>
-      <c r="CZ87" s="1"/>
-      <c r="DA87" s="1"/>
-      <c r="DB87" s="1"/>
-      <c r="DC87" s="1"/>
-      <c r="DD87" s="1"/>
-      <c r="DE87" s="1"/>
-      <c r="DF87" s="1"/>
-      <c r="DG87" s="1"/>
-      <c r="DH87" s="1"/>
-      <c r="DI87" s="1"/>
-      <c r="DJ87" s="1"/>
-      <c r="DK87" s="1"/>
-      <c r="DL87" s="1"/>
-      <c r="DM87" s="1"/>
-      <c r="DN87" s="1"/>
-      <c r="DO87" s="1"/>
-      <c r="DP87" s="1"/>
-      <c r="DQ87" s="1"/>
-      <c r="DR87" s="1"/>
-      <c r="DS87" s="1"/>
-      <c r="DT87" s="1"/>
-      <c r="DU87" s="1"/>
-      <c r="DV87" s="1"/>
-      <c r="DW87" s="1"/>
-      <c r="DX87" s="1"/>
-      <c r="DY87" s="1"/>
-      <c r="DZ87" s="1"/>
-      <c r="EA87" s="1"/>
-      <c r="EB87" s="1"/>
-      <c r="EC87" s="1"/>
-      <c r="ED87" s="1"/>
-      <c r="EE87" s="1"/>
-      <c r="EF87" s="1"/>
-      <c r="EG87" s="1"/>
-      <c r="EH87" s="1"/>
-      <c r="EI87" s="1"/>
-      <c r="EJ87" s="1"/>
-      <c r="EK87" s="1"/>
-      <c r="EL87" s="1"/>
-      <c r="EM87" s="1"/>
-      <c r="EN87" s="1"/>
-      <c r="EO87" s="1"/>
-      <c r="EP87" s="1"/>
-      <c r="EQ87" s="1"/>
-      <c r="ER87" s="1"/>
-      <c r="ES87" s="1"/>
-      <c r="ET87" s="1"/>
-      <c r="EU87" s="1"/>
-      <c r="EV87" s="1"/>
-      <c r="EW87" s="1"/>
-      <c r="EX87" s="1"/>
-      <c r="EY87" s="1"/>
-      <c r="EZ87" s="1"/>
-      <c r="FA87" s="1"/>
-      <c r="FB87" s="1"/>
-      <c r="FC87" s="1"/>
-      <c r="FD87" s="1"/>
-      <c r="FE87" s="1"/>
-      <c r="FF87" s="1"/>
-      <c r="FG87" s="1"/>
-      <c r="FH87" s="1"/>
-      <c r="FI87" s="1"/>
-      <c r="FJ87" s="1"/>
-    </row>
-    <row r="88" spans="1:171" ht="15">
-      <c r="A88" s="9">
-        <v>24923318</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E88" s="9">
-        <v>1000</v>
-      </c>
-      <c r="F88" s="13">
-        <v>45793</v>
-      </c>
-      <c r="AY88" s="1"/>
-      <c r="AZ88" s="1"/>
-      <c r="BA88" s="1"/>
-      <c r="BB88" s="1"/>
-      <c r="BC88" s="1"/>
-      <c r="BD88" s="1"/>
-      <c r="BE88" s="1"/>
-      <c r="BF88" s="1"/>
-      <c r="BG88" s="1"/>
-      <c r="BH88" s="1"/>
-      <c r="BI88" s="1"/>
-      <c r="BJ88" s="1"/>
-      <c r="BK88" s="1"/>
-      <c r="BL88" s="1"/>
-      <c r="BM88" s="1"/>
-      <c r="BN88" s="1"/>
-      <c r="BO88" s="1"/>
-      <c r="BP88" s="1"/>
-      <c r="BQ88" s="1"/>
-      <c r="BR88" s="1"/>
-      <c r="BS88" s="1"/>
-      <c r="BT88" s="1"/>
-      <c r="BU88" s="1"/>
-      <c r="BV88" s="1"/>
-      <c r="BW88" s="1"/>
-      <c r="BX88" s="1"/>
-      <c r="BY88" s="1"/>
-      <c r="BZ88" s="1"/>
-      <c r="CA88" s="1"/>
-      <c r="CB88" s="1"/>
-      <c r="CC88" s="1"/>
-      <c r="CD88" s="1"/>
-      <c r="CE88" s="1"/>
-      <c r="CF88" s="1"/>
-      <c r="CG88" s="1"/>
-      <c r="CH88" s="1"/>
-      <c r="CI88" s="1"/>
-      <c r="CJ88" s="1"/>
-      <c r="CK88" s="1"/>
-      <c r="CL88" s="1"/>
-      <c r="CM88" s="1"/>
-      <c r="CN88" s="1"/>
-      <c r="CO88" s="1"/>
-      <c r="CP88" s="1"/>
-      <c r="CQ88" s="1"/>
-      <c r="CR88" s="1"/>
-      <c r="CS88" s="1"/>
-      <c r="CT88" s="1"/>
-      <c r="CU88" s="1"/>
-      <c r="CV88" s="1"/>
-      <c r="CW88" s="1"/>
-      <c r="CX88" s="1"/>
-      <c r="CY88" s="1"/>
-      <c r="CZ88" s="1"/>
-      <c r="DA88" s="1"/>
-      <c r="DB88" s="1"/>
-      <c r="DC88" s="1"/>
-      <c r="DD88" s="1"/>
-      <c r="DE88" s="1"/>
-      <c r="DF88" s="1"/>
-      <c r="DG88" s="1"/>
-      <c r="DH88" s="1"/>
-      <c r="DI88" s="1"/>
-      <c r="DJ88" s="1"/>
-      <c r="DK88" s="1"/>
-      <c r="DL88" s="1"/>
-      <c r="DM88" s="1"/>
-      <c r="DN88" s="1"/>
-      <c r="DO88" s="1"/>
-      <c r="DP88" s="1"/>
-      <c r="DQ88" s="1"/>
-      <c r="DR88" s="1"/>
-      <c r="DS88" s="1"/>
-      <c r="DT88" s="1"/>
-      <c r="DU88" s="1"/>
-      <c r="DV88" s="1"/>
-      <c r="DW88" s="1"/>
-      <c r="DX88" s="1"/>
-      <c r="DY88" s="1"/>
-      <c r="DZ88" s="1"/>
-      <c r="EA88" s="1"/>
-      <c r="EB88" s="1"/>
-      <c r="EC88" s="1"/>
-      <c r="ED88" s="1"/>
-      <c r="EE88" s="1"/>
-      <c r="EF88" s="1"/>
-      <c r="EG88" s="1"/>
-      <c r="EH88" s="1"/>
-      <c r="EI88" s="1"/>
-      <c r="EJ88" s="1"/>
-      <c r="EK88" s="1"/>
-      <c r="EL88" s="1"/>
-      <c r="EM88" s="1"/>
-      <c r="EN88" s="1"/>
-      <c r="EO88" s="1"/>
-      <c r="EP88" s="1"/>
-      <c r="EQ88" s="1"/>
-      <c r="ER88" s="1"/>
-      <c r="ES88" s="1"/>
-      <c r="ET88" s="1"/>
-      <c r="EU88" s="1"/>
-      <c r="EV88" s="1">
-        <v>12</v>
-      </c>
-      <c r="EW88" s="1">
-        <v>24</v>
-      </c>
-      <c r="EX88" s="1">
-        <v>24</v>
-      </c>
-      <c r="EY88" s="1">
-        <v>24</v>
-      </c>
-      <c r="EZ88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FA88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FB88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FC88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FD88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FE88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FF88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FG88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FH88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FI88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FJ88" s="1">
-        <v>24</v>
-      </c>
-      <c r="FK88" s="4">
-        <v>8</v>
-      </c>
-      <c r="FL88" s="4">
-        <v>14</v>
-      </c>
-      <c r="FM88" s="4">
-        <v>24</v>
-      </c>
-      <c r="FN88" s="4">
-        <v>24</v>
-      </c>
-      <c r="FO88" s="4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="89" spans="1:171" ht="15">
-      <c r="A89" s="9">
-        <v>24925212</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E89" s="9">
-        <v>1000</v>
-      </c>
-      <c r="F89" s="13"/>
-      <c r="AY89" s="1"/>
-      <c r="AZ89" s="1"/>
-      <c r="BA89" s="1"/>
-      <c r="BB89" s="1"/>
-      <c r="BC89" s="1"/>
-      <c r="BD89" s="1"/>
-      <c r="BE89" s="1"/>
-      <c r="BF89" s="1"/>
-      <c r="BG89" s="1"/>
-      <c r="BH89" s="1"/>
-      <c r="BI89" s="1"/>
-      <c r="BJ89" s="1"/>
-      <c r="BK89" s="1"/>
-      <c r="BL89" s="1"/>
-      <c r="BM89" s="1"/>
-      <c r="BN89" s="1"/>
-      <c r="BO89" s="1"/>
-      <c r="BP89" s="1"/>
-      <c r="BQ89" s="1"/>
-      <c r="BR89" s="1"/>
-      <c r="BS89" s="1"/>
-      <c r="BT89" s="1"/>
-      <c r="BU89" s="1"/>
-      <c r="BV89" s="1"/>
-      <c r="BW89" s="1"/>
-      <c r="BX89" s="1"/>
-      <c r="BY89" s="1"/>
-      <c r="BZ89" s="1"/>
-      <c r="CA89" s="1"/>
-      <c r="CB89" s="1"/>
-      <c r="CC89" s="1"/>
-      <c r="CD89" s="1"/>
-      <c r="CE89" s="1"/>
-      <c r="CF89" s="1"/>
-      <c r="CG89" s="1"/>
-      <c r="CH89" s="1"/>
-      <c r="CI89" s="1"/>
-      <c r="CJ89" s="1"/>
-      <c r="CK89" s="1"/>
-      <c r="CL89" s="1"/>
-      <c r="CM89" s="1"/>
-      <c r="CN89" s="1"/>
-      <c r="CO89" s="1"/>
-      <c r="CP89" s="1"/>
-      <c r="CQ89" s="1"/>
-      <c r="CR89" s="1"/>
-      <c r="CS89" s="1"/>
-      <c r="CT89" s="1"/>
-      <c r="CU89" s="1"/>
-      <c r="CV89" s="1"/>
-      <c r="CW89" s="1"/>
-      <c r="CX89" s="1"/>
-      <c r="CY89" s="1"/>
-      <c r="CZ89" s="1"/>
-      <c r="DA89" s="1"/>
-      <c r="DB89" s="1"/>
-      <c r="DC89" s="1"/>
-      <c r="DD89" s="1"/>
-      <c r="DE89" s="1"/>
-      <c r="DF89" s="1"/>
-      <c r="DG89" s="1"/>
-      <c r="DH89" s="1"/>
-      <c r="DI89" s="1"/>
-      <c r="DJ89" s="1"/>
-      <c r="DK89" s="1"/>
-      <c r="DL89" s="1"/>
-      <c r="DM89" s="1"/>
-      <c r="DN89" s="1"/>
-      <c r="DO89" s="1"/>
-      <c r="DP89" s="1"/>
-      <c r="DQ89" s="1"/>
-      <c r="DR89" s="1"/>
-      <c r="DS89" s="1"/>
-      <c r="DT89" s="1"/>
-      <c r="DU89" s="1"/>
-      <c r="DV89" s="1"/>
-      <c r="DW89" s="1"/>
-      <c r="DX89" s="1"/>
-      <c r="DY89" s="1"/>
-      <c r="DZ89" s="1"/>
-      <c r="EA89" s="1"/>
-      <c r="EB89" s="1"/>
-      <c r="EC89" s="1"/>
-      <c r="ED89" s="1"/>
-      <c r="EE89" s="1"/>
-      <c r="EF89" s="1"/>
-      <c r="EG89" s="1"/>
-      <c r="EH89" s="1"/>
-      <c r="EI89" s="1"/>
-      <c r="EJ89" s="1"/>
-      <c r="EK89" s="1"/>
-      <c r="EL89" s="1"/>
-      <c r="EM89" s="1"/>
-      <c r="EN89" s="1"/>
-      <c r="EO89" s="1"/>
-      <c r="EP89" s="1"/>
-      <c r="EQ89" s="1"/>
-      <c r="ER89" s="1"/>
-      <c r="ES89" s="1"/>
-      <c r="ET89" s="1"/>
-      <c r="EU89" s="1"/>
-      <c r="EV89" s="1"/>
-      <c r="EW89" s="1"/>
-      <c r="EX89" s="1"/>
-      <c r="EY89" s="1"/>
-      <c r="EZ89" s="1"/>
-      <c r="FA89" s="1"/>
-      <c r="FB89" s="1"/>
-      <c r="FC89" s="1"/>
-      <c r="FD89" s="1"/>
-      <c r="FE89" s="1"/>
-      <c r="FF89" s="1"/>
-      <c r="FG89" s="1"/>
-      <c r="FH89" s="1"/>
-      <c r="FI89" s="1"/>
-      <c r="FJ89" s="1"/>
-    </row>
-    <row r="90" spans="1:171" ht="15">
-      <c r="A90" s="9">
-        <v>24857462</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D90" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E90" s="9">
-        <v>200</v>
-      </c>
-      <c r="F90" s="13">
-        <v>45792</v>
-      </c>
-      <c r="AY90" s="1"/>
-      <c r="AZ90" s="1"/>
-      <c r="BA90" s="1"/>
-      <c r="BB90" s="1"/>
-      <c r="BC90" s="1"/>
-      <c r="BD90" s="1"/>
-      <c r="BE90" s="1"/>
-      <c r="BF90" s="1"/>
-      <c r="BG90" s="1"/>
-      <c r="BH90" s="1"/>
-      <c r="BI90" s="1"/>
-      <c r="BJ90" s="1"/>
-      <c r="BK90" s="1"/>
-      <c r="BL90" s="1"/>
-      <c r="BM90" s="1"/>
-      <c r="BN90" s="1"/>
-      <c r="BO90" s="1"/>
-      <c r="BP90" s="1"/>
-      <c r="BQ90" s="1"/>
-      <c r="BR90" s="1"/>
-      <c r="BS90" s="1"/>
-      <c r="BT90" s="1"/>
-      <c r="BU90" s="1"/>
-      <c r="BV90" s="1"/>
-      <c r="BW90" s="1"/>
-      <c r="BX90" s="1"/>
-      <c r="BY90" s="1"/>
-      <c r="BZ90" s="1"/>
-      <c r="CA90" s="1"/>
-      <c r="CB90" s="1"/>
-      <c r="CC90" s="1"/>
-      <c r="CD90" s="1"/>
-      <c r="CE90" s="1"/>
-      <c r="CF90" s="1"/>
-      <c r="CG90" s="1"/>
-      <c r="CH90" s="1"/>
-      <c r="CI90" s="1"/>
-      <c r="CJ90" s="1"/>
-      <c r="CK90" s="1"/>
-      <c r="CL90" s="1"/>
-      <c r="CM90" s="1"/>
-      <c r="CN90" s="1"/>
-      <c r="CO90" s="1"/>
-      <c r="CP90" s="1"/>
-      <c r="CQ90" s="1"/>
-      <c r="CR90" s="1"/>
-      <c r="CS90" s="1"/>
-      <c r="CT90" s="1"/>
-      <c r="CU90" s="1"/>
-      <c r="CV90" s="1"/>
-      <c r="CW90" s="1"/>
-      <c r="CX90" s="1"/>
-      <c r="CY90" s="1"/>
-      <c r="CZ90" s="1"/>
-      <c r="DA90" s="1"/>
-      <c r="DB90" s="1"/>
-      <c r="DC90" s="1"/>
-      <c r="DD90" s="1"/>
-      <c r="DE90" s="1"/>
-      <c r="DF90" s="1"/>
-      <c r="DG90" s="1"/>
-      <c r="DH90" s="1"/>
-      <c r="DI90" s="1"/>
-      <c r="DJ90" s="1"/>
-      <c r="DK90" s="1"/>
-      <c r="DL90" s="1"/>
-      <c r="DM90" s="1"/>
-      <c r="DN90" s="1"/>
-      <c r="DO90" s="1"/>
-      <c r="DP90" s="1"/>
-      <c r="DQ90" s="1"/>
-      <c r="DR90" s="1"/>
-      <c r="DS90" s="1"/>
-      <c r="DT90" s="1"/>
-      <c r="DU90" s="1"/>
-      <c r="DV90" s="1"/>
-      <c r="DW90" s="1"/>
-      <c r="DX90" s="1"/>
-      <c r="DY90" s="1"/>
-      <c r="DZ90" s="1"/>
-      <c r="EA90" s="1"/>
-      <c r="EB90" s="1"/>
-      <c r="EC90" s="1"/>
-      <c r="ED90" s="1"/>
-      <c r="EE90" s="1"/>
-      <c r="EF90" s="1"/>
-      <c r="EG90" s="1"/>
-      <c r="EH90" s="1"/>
-      <c r="EI90" s="1"/>
-      <c r="EJ90" s="1"/>
-      <c r="EK90" s="1"/>
-      <c r="EL90" s="1"/>
-      <c r="EM90" s="1"/>
-      <c r="EN90" s="1"/>
-      <c r="EO90" s="1"/>
-      <c r="EP90" s="1"/>
-      <c r="EQ90" s="1"/>
-      <c r="ER90" s="1"/>
-      <c r="ES90" s="1"/>
-      <c r="ET90" s="1"/>
-      <c r="EU90" s="1">
-        <v>8</v>
-      </c>
-      <c r="EV90" s="1">
-        <v>12</v>
-      </c>
-      <c r="EW90" s="1">
-        <v>12</v>
-      </c>
-      <c r="EX90" s="1">
-        <v>12</v>
-      </c>
-      <c r="EY90" s="1">
-        <v>12</v>
-      </c>
-      <c r="EZ90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FA90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FB90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FC90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FD90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FE90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FF90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FG90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FH90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FI90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FJ90" s="1">
-        <v>12</v>
-      </c>
-      <c r="FK90" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="FL90" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="FM90" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="FN90" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="FO90" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="91" spans="1:171" ht="15">
-      <c r="A91" s="10">
-        <v>25112301</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C91" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D91" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E91" s="10">
-        <v>96</v>
-      </c>
-      <c r="F91" s="14">
-        <v>45806</v>
-      </c>
-      <c r="P91" s="3">
-        <v>45811</v>
-      </c>
-      <c r="FI91" s="4">
-        <v>11</v>
-      </c>
-      <c r="FJ91" s="4">
-        <v>24</v>
-      </c>
-      <c r="FK91" s="4">
-        <v>8</v>
-      </c>
-      <c r="FL91" s="4">
-        <v>14</v>
-      </c>
-      <c r="FM91" s="4">
-        <v>24</v>
-      </c>
-      <c r="FN91" s="4">
-        <v>24</v>
-      </c>
-      <c r="FO91" s="4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="92" spans="1:171" ht="15">
-      <c r="A92" s="10">
-        <v>25112300</v>
-      </c>
-      <c r="B92" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D92" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E92" s="10">
-        <v>1000</v>
-      </c>
-      <c r="F92" s="14">
-        <v>45806</v>
-      </c>
-      <c r="FI92" s="4">
-        <v>11</v>
-      </c>
-      <c r="FJ92" s="4">
-        <v>24</v>
-      </c>
-      <c r="FK92" s="4">
-        <v>8</v>
-      </c>
-      <c r="FL92" s="4">
-        <v>14</v>
-      </c>
-      <c r="FM92" s="4">
-        <v>24</v>
-      </c>
-      <c r="FN92" s="4">
-        <v>24</v>
-      </c>
-      <c r="FO92" s="4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="93" spans="1:171" ht="15">
-      <c r="A93" s="10">
-        <v>25087863</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D93" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E93" s="10">
-        <v>96</v>
-      </c>
-      <c r="F93" s="14">
-        <v>45806</v>
-      </c>
-      <c r="P93" s="3">
-        <v>45811</v>
-      </c>
-      <c r="FI93" s="4">
-        <v>11</v>
-      </c>
-      <c r="FJ93" s="4">
-        <v>24</v>
-      </c>
-      <c r="FK93" s="4">
-        <v>8</v>
-      </c>
-      <c r="FL93" s="4">
-        <v>14</v>
-      </c>
-      <c r="FM93" s="4">
-        <v>24</v>
-      </c>
-      <c r="FN93" s="4">
-        <v>24</v>
-      </c>
-      <c r="FO93" s="4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="94" spans="1:171" ht="15">
-      <c r="A94" s="10">
-        <v>25087787</v>
-      </c>
-      <c r="B94" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D94" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E94" s="10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:171" ht="15">
-      <c r="A95" s="10">
-        <v>24848184</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E95" s="9">
-        <v>200</v>
-      </c>
-      <c r="F95" s="13">
-        <v>45792</v>
-      </c>
-      <c r="EU95" s="4">
-        <v>8</v>
-      </c>
-      <c r="EV95" s="4">
-        <v>12</v>
-      </c>
-      <c r="EW95" s="4">
-        <v>12</v>
-      </c>
-      <c r="EX95" s="4">
-        <v>12</v>
-      </c>
-      <c r="EY95" s="4">
-        <v>12</v>
-      </c>
-      <c r="EZ95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FA95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FB95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FC95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FD95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FE95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FF95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FG95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FH95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FI95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FJ95" s="4">
-        <v>12</v>
-      </c>
-      <c r="FK95" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="FL95" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="FM95" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="FN95" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="FO95" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="96" spans="1:171" ht="15">
+    <row r="96" spans="1:171" s="4" customFormat="1" ht="15">
       <c r="A96" s="16">
-        <v>50872159</v>
+        <v>25089372</v>
       </c>
       <c r="B96" s="17" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D96" s="16" t="s">
         <v>18</v>
       </c>
       <c r="E96" s="16">
-        <v>192</v>
-      </c>
-      <c r="F96" s="19">
-        <v>45793</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="F96" s="19"/>
+      <c r="P96" s="3"/>
     </row>
-    <row r="97" spans="1:167" ht="15">
+    <row r="97" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A97" s="16">
-        <v>25019645</v>
+        <v>25089365</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C97" s="18" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="D97" s="16" t="s">
         <v>18</v>
@@ -82228,585 +81326,244 @@
         <v>96</v>
       </c>
       <c r="F97" s="19"/>
+      <c r="P97" s="3"/>
     </row>
-    <row r="98" spans="1:167" ht="15">
+    <row r="98" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A98" s="16">
-        <v>25017936</v>
+        <v>25089363</v>
       </c>
       <c r="B98" s="17" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E98" s="16">
-        <v>96</v>
+        <v>1000</v>
       </c>
       <c r="F98" s="19"/>
+      <c r="P98" s="3"/>
     </row>
-    <row r="99" spans="1:167" ht="15">
+    <row r="99" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A99" s="16">
-        <v>25089372</v>
+        <v>25089370</v>
       </c>
       <c r="B99" s="17" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C99" s="18" t="s">
         <v>122</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E99" s="16">
-        <v>60</v>
-      </c>
-      <c r="F99" s="19">
-        <v>45797</v>
-      </c>
-      <c r="P99" s="3">
-        <v>45808</v>
-      </c>
-      <c r="EZ99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FA99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FB99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FC99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FD99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FE99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FF99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FG99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FH99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FI99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FJ99" s="4">
-        <v>5</v>
-      </c>
-      <c r="FK99" s="4">
-        <v>5</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="F99" s="19"/>
+      <c r="P99" s="3"/>
     </row>
-    <row r="100" spans="1:167" ht="15">
+    <row r="100" spans="1:16" s="4" customFormat="1" ht="15">
       <c r="A100" s="16">
-        <v>25089365</v>
+        <v>25112301</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E100" s="16">
-        <v>60</v>
-      </c>
-      <c r="F100" s="19">
-        <v>45797</v>
-      </c>
-      <c r="P100" s="3">
-        <v>45808</v>
-      </c>
-      <c r="EZ100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FA100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FB100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FC100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FD100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FE100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FF100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FG100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FH100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FI100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FJ100" s="4">
-        <v>5</v>
-      </c>
-      <c r="FK100" s="4">
-        <v>5</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="F100" s="19"/>
+      <c r="P100" s="3"/>
     </row>
-    <row r="101" spans="1:167" ht="15">
-      <c r="A101" s="16">
-        <v>25089363</v>
-      </c>
-      <c r="B101" s="17" t="s">
-        <v>125</v>
+    <row r="101" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A101" s="10">
+        <v>72309509</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D101" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E101" s="16">
-        <v>60</v>
-      </c>
-      <c r="F101" s="19">
-        <v>45797</v>
-      </c>
-      <c r="P101" s="3">
-        <v>45808</v>
-      </c>
-      <c r="EZ101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FA101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FB101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FC101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FD101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FE101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FF101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FG101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FH101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FI101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FJ101" s="4">
-        <v>5</v>
-      </c>
-      <c r="FK101" s="4">
-        <v>5</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E101" s="10">
+        <v>96</v>
+      </c>
+      <c r="F101" s="14"/>
+      <c r="P101" s="3"/>
     </row>
-    <row r="102" spans="1:167" ht="15">
-      <c r="A102" s="16">
-        <v>25089370</v>
-      </c>
-      <c r="B102" s="17" t="s">
-        <v>126</v>
+    <row r="102" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A102" s="10">
+        <v>72304210</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E102" s="16">
-        <v>60</v>
-      </c>
-      <c r="F102" s="19">
-        <v>45797</v>
-      </c>
-      <c r="P102" s="3">
-        <v>45808</v>
-      </c>
-      <c r="EZ102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FA102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FB102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FC102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FD102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FE102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FF102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FG102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FH102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FI102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FJ102" s="4">
-        <v>5</v>
-      </c>
-      <c r="FK102" s="4">
-        <v>5</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" s="10">
+        <v>96</v>
+      </c>
+      <c r="F102" s="14"/>
+      <c r="P102" s="3"/>
     </row>
-    <row r="103" spans="1:167" ht="15">
-      <c r="A103" s="16">
-        <v>25112299</v>
-      </c>
-      <c r="B103" s="17" t="s">
-        <v>127</v>
+    <row r="103" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A103" s="10">
+        <v>25263837</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="C103" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="D103" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E103" s="16">
-        <v>60</v>
-      </c>
-      <c r="F103" s="19">
-        <v>45797</v>
-      </c>
-      <c r="P103" s="3">
-        <v>45808</v>
-      </c>
-      <c r="EZ103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FA103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FB103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FC103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FD103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FE103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FF103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FG103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FH103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FI103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FJ103" s="4">
-        <v>5</v>
-      </c>
-      <c r="FK103" s="4">
-        <v>5</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D103" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E103" s="10">
+        <v>96</v>
+      </c>
+      <c r="F103" s="14"/>
+      <c r="P103" s="3"/>
     </row>
-    <row r="104" spans="1:167" ht="15">
-      <c r="A104" s="16">
-        <v>72149637</v>
-      </c>
-      <c r="B104" s="17" t="s">
-        <v>128</v>
+    <row r="104" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A104" s="10">
+        <v>25264958</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>136</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D104" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E104" s="16">
-        <v>50</v>
-      </c>
-      <c r="F104" s="19">
-        <v>45796</v>
-      </c>
-      <c r="P104" s="3">
-        <v>45806</v>
-      </c>
-      <c r="EY104" s="4">
-        <v>8</v>
-      </c>
-      <c r="EZ104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FA104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FB104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FC104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FD104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FE104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FF104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FG104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FH104" s="4">
-        <v>12</v>
-      </c>
-      <c r="FI104" s="4">
-        <v>12</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D104" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E104" s="10">
+        <v>96</v>
+      </c>
+      <c r="F104" s="14"/>
+      <c r="P104" s="3"/>
     </row>
-    <row r="105" spans="1:167" ht="15">
-      <c r="A105" s="16">
-        <v>72238923</v>
-      </c>
-      <c r="B105" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C105" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D105" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E105" s="16">
-        <v>1000</v>
-      </c>
-      <c r="F105" s="19"/>
+    <row r="105" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A105" s="10"/>
+      <c r="B105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="14"/>
+      <c r="P105" s="3"/>
     </row>
-    <row r="106" spans="1:167" ht="15">
-      <c r="A106" s="16">
-        <v>25089372</v>
-      </c>
-      <c r="B106" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C106" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D106" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E106" s="16">
-        <v>96</v>
-      </c>
-      <c r="F106" s="19"/>
+    <row r="106" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A106" s="10"/>
+      <c r="B106" s="10"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="14"/>
+      <c r="P106" s="3"/>
     </row>
-    <row r="107" spans="1:167" ht="15">
-      <c r="A107" s="16">
-        <v>25089365</v>
-      </c>
-      <c r="B107" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C107" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E107" s="16">
-        <v>96</v>
-      </c>
-      <c r="F107" s="19"/>
+    <row r="107" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A107" s="10"/>
+      <c r="B107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="14"/>
+      <c r="P107" s="3"/>
     </row>
-    <row r="108" spans="1:167" ht="15">
-      <c r="A108" s="16">
-        <v>25089363</v>
-      </c>
-      <c r="B108" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C108" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D108" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E108" s="16">
-        <v>1000</v>
-      </c>
-      <c r="F108" s="19"/>
+    <row r="108" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A108" s="10"/>
+      <c r="B108" s="10"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="14"/>
+      <c r="P108" s="3"/>
     </row>
-    <row r="109" spans="1:167" ht="15">
-      <c r="A109" s="16">
-        <v>25089370</v>
-      </c>
-      <c r="B109" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C109" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D109" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E109" s="16">
-        <v>1000</v>
-      </c>
-      <c r="F109" s="19"/>
+    <row r="109" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A109" s="10"/>
+      <c r="B109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="14"/>
+      <c r="P109" s="3"/>
     </row>
-    <row r="110" spans="1:167" ht="15">
-      <c r="A110" s="16">
-        <v>25112301</v>
-      </c>
-      <c r="B110" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C110" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D110" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E110" s="16">
-        <v>96</v>
-      </c>
-      <c r="F110" s="19"/>
+    <row r="110" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A110" s="10"/>
+      <c r="B110" s="10"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="14"/>
+      <c r="P110" s="3"/>
     </row>
-    <row r="111" spans="1:167" ht="15">
-      <c r="A111" s="16">
-        <v>25112300</v>
-      </c>
-      <c r="B111" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C111" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="D111" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E111" s="16">
-        <v>1000</v>
-      </c>
-      <c r="F111" s="19"/>
+    <row r="111" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A111" s="10"/>
+      <c r="B111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="14"/>
+      <c r="P111" s="3"/>
     </row>
-    <row r="112" spans="1:167" ht="15">
-      <c r="A112" s="10">
-        <v>72309509</v>
-      </c>
-      <c r="B112" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C112" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E112" s="10">
-        <v>96</v>
-      </c>
+    <row r="112" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A112" s="10"/>
+      <c r="B112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="14"/>
+      <c r="P112" s="3"/>
     </row>
-    <row r="113" spans="1:5" ht="15">
-      <c r="A113" s="10">
-        <v>72304210</v>
-      </c>
-      <c r="B113" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C113" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D113" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E113" s="10">
-        <v>96</v>
-      </c>
+    <row r="113" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A113" s="10"/>
+      <c r="B113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="14"/>
+      <c r="P113" s="3"/>
     </row>
-    <row r="114" spans="1:5" ht="15">
-      <c r="A114" s="10">
-        <v>25263837</v>
-      </c>
-      <c r="B114" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C114" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D114" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E114" s="10">
-        <v>96</v>
-      </c>
+    <row r="114" spans="1:16" s="4" customFormat="1" ht="15">
+      <c r="A114" s="10"/>
+      <c r="B114" s="10"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="14"/>
+      <c r="P114" s="3"/>
     </row>
-    <row r="115" spans="1:5" ht="15">
-      <c r="A115" s="10">
-        <v>25264958</v>
-      </c>
-      <c r="B115" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C115" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D115" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E115" s="10">
-        <v>96</v>
-      </c>
+    <row r="115" spans="1:16" s="4" customFormat="1">
+      <c r="A115" s="10"/>
+      <c r="B115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="14"/>
+      <c r="P115" s="3"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="F1:F1048576" name="Range1"/>
     <protectedRange sqref="P1:P1048576" name="Range2"/>
-    <protectedRange sqref="A95 Q1:XFD1048576" name="Range3"/>
+    <protectedRange sqref="A85 Q1:XFD1048576" name="Range3"/>
   </protectedRanges>
-  <conditionalFormatting sqref="A96:A100 A102:A111">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A101">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A86:A90 A92:A100">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D96:D111" xr:uid="{AE741107-2DDE-448F-B66D-3CC4D6043D49}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D86:D100" xr:uid="{AE741107-2DDE-448F-B66D-3CC4D6043D49}">
       <formula1>"LID,PID,TC,DH,HF,LETID,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun  5 17:32:46 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="458" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15D03372-6191-4E5A-A244-EB58EB75B900}"/>
+  <xr:revisionPtr revIDLastSave="504" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F878D522-C5BD-4795-ADEE-D75CF3555C9E}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -972,11 +972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD115"/>
+  <dimension ref="A1:XFD114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="ES90" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A101" sqref="A101:XFD101"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="CO40" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="CU47" sqref="CU47"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -70096,6 +70096,9 @@
       <c r="F18" s="13">
         <v>45720</v>
       </c>
+      <c r="P18" s="3">
+        <v>45803</v>
+      </c>
       <c r="AY18" s="1"/>
       <c r="AZ18" s="1"/>
       <c r="BA18" s="1"/>
@@ -70255,7 +70258,9 @@
       <c r="DY18" s="1"/>
       <c r="DZ18" s="1"/>
       <c r="EA18" s="1"/>
-      <c r="EB18" s="1"/>
+      <c r="EB18" s="1">
+        <v>355</v>
+      </c>
       <c r="EC18" s="1"/>
       <c r="ED18" s="1"/>
       <c r="EE18" s="1"/>
@@ -71042,6 +71047,9 @@
       <c r="F22" s="13">
         <v>45707</v>
       </c>
+      <c r="P22" s="3">
+        <v>45721</v>
+      </c>
       <c r="AY22" s="1"/>
       <c r="AZ22" s="1"/>
       <c r="BA22" s="1"/>
@@ -71083,7 +71091,9 @@
       <c r="BY22" s="1"/>
       <c r="BZ22" s="1"/>
       <c r="CA22" s="1"/>
-      <c r="CB22" s="1"/>
+      <c r="CB22" s="1">
+        <v>51</v>
+      </c>
       <c r="CC22" s="1"/>
       <c r="CD22" s="1"/>
       <c r="CE22" s="1"/>
@@ -71338,6 +71348,9 @@
       <c r="F24" s="13">
         <v>45712</v>
       </c>
+      <c r="P24" s="3">
+        <v>45813</v>
+      </c>
       <c r="AY24" s="1"/>
       <c r="AZ24" s="1"/>
       <c r="BA24" s="1"/>
@@ -71373,7 +71386,9 @@
       <c r="BY24" s="1"/>
       <c r="BZ24" s="1"/>
       <c r="CA24" s="1"/>
-      <c r="CB24" s="1"/>
+      <c r="CB24" s="1">
+        <v>51</v>
+      </c>
       <c r="CC24" s="1"/>
       <c r="CD24" s="1"/>
       <c r="CE24" s="1"/>
@@ -71622,6 +71637,9 @@
       <c r="F26" s="13">
         <v>45720</v>
       </c>
+      <c r="P26" s="3">
+        <v>45803</v>
+      </c>
       <c r="AY26" s="1"/>
       <c r="AZ26" s="1"/>
       <c r="BA26" s="1"/>
@@ -71781,7 +71799,9 @@
       <c r="DY26" s="1"/>
       <c r="DZ26" s="1"/>
       <c r="EA26" s="1"/>
-      <c r="EB26" s="1"/>
+      <c r="EB26" s="1">
+        <v>355</v>
+      </c>
       <c r="EC26" s="1"/>
       <c r="ED26" s="1"/>
       <c r="EE26" s="1"/>
@@ -73112,6 +73132,9 @@
       <c r="F35" s="13">
         <v>45721</v>
       </c>
+      <c r="P35" s="3">
+        <v>45725</v>
+      </c>
       <c r="AY35" s="1"/>
       <c r="AZ35" s="1"/>
       <c r="BA35" s="1"/>
@@ -73141,11 +73164,21 @@
       <c r="BY35" s="1"/>
       <c r="BZ35" s="1"/>
       <c r="CA35" s="1"/>
-      <c r="CB35" s="1"/>
-      <c r="CC35" s="1"/>
-      <c r="CD35" s="1"/>
-      <c r="CE35" s="1"/>
-      <c r="CF35" s="1"/>
+      <c r="CB35" s="1">
+        <v>12</v>
+      </c>
+      <c r="CC35" s="1">
+        <v>24</v>
+      </c>
+      <c r="CD35" s="1">
+        <v>24</v>
+      </c>
+      <c r="CE35" s="1">
+        <v>24</v>
+      </c>
+      <c r="CF35" s="1">
+        <v>14</v>
+      </c>
       <c r="CG35" s="1"/>
       <c r="CH35" s="1"/>
       <c r="CI35" s="1"/>
@@ -75280,7 +75313,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:171" ht="15">
+    <row r="49" spans="1:172" ht="15">
       <c r="A49" s="12">
         <v>24567289</v>
       </c>
@@ -75414,7 +75447,7 @@
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
     </row>
-    <row r="50" spans="1:171" ht="15">
+    <row r="50" spans="1:172" ht="15">
       <c r="A50" s="12">
         <v>24567319</v>
       </c>
@@ -75625,7 +75658,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:171" ht="15">
+    <row r="51" spans="1:172" ht="15">
       <c r="A51" s="12">
         <v>24567277</v>
       </c>
@@ -75836,7 +75869,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:171" ht="15">
+    <row r="52" spans="1:172" ht="15">
       <c r="A52" s="12">
         <v>24567774</v>
       </c>
@@ -76047,7 +76080,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:171" ht="15">
+    <row r="53" spans="1:172" ht="15">
       <c r="A53" s="12">
         <v>24567851</v>
       </c>
@@ -76181,7 +76214,7 @@
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
     </row>
-    <row r="54" spans="1:171" ht="15">
+    <row r="54" spans="1:172" ht="15">
       <c r="A54" s="12">
         <v>24559501</v>
       </c>
@@ -76315,7 +76348,7 @@
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
     </row>
-    <row r="55" spans="1:171" ht="15">
+    <row r="55" spans="1:172" ht="15">
       <c r="A55" s="9">
         <v>24079686</v>
       </c>
@@ -76503,7 +76536,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:171" ht="15">
+    <row r="56" spans="1:172" ht="15">
       <c r="A56" s="9">
         <v>24079692</v>
       </c>
@@ -76521,6 +76554,9 @@
       </c>
       <c r="F56" s="13">
         <v>45733</v>
+      </c>
+      <c r="P56" s="3">
+        <v>45803</v>
       </c>
       <c r="AY56" s="1"/>
       <c r="AZ56" s="1"/>
@@ -76630,16 +76666,16 @@
         <v>22</v>
       </c>
       <c r="DJ56" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="DK56" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="DL56" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="DM56" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="DN56" s="1"/>
       <c r="DO56" s="1"/>
@@ -76655,7 +76691,9 @@
       <c r="DY56" s="1"/>
       <c r="DZ56" s="1"/>
       <c r="EA56" s="1"/>
-      <c r="EB56" s="1"/>
+      <c r="EB56" s="1">
+        <v>408</v>
+      </c>
       <c r="EC56" s="1"/>
       <c r="ED56" s="1"/>
       <c r="EE56" s="1"/>
@@ -76691,7 +76729,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:171" ht="15">
+    <row r="57" spans="1:172" ht="15">
       <c r="A57" s="9">
         <v>24636092</v>
       </c>
@@ -76709,6 +76747,9 @@
       </c>
       <c r="F57" s="13">
         <v>45733</v>
+      </c>
+      <c r="P57" s="3">
+        <v>45741</v>
       </c>
       <c r="AY57" s="1"/>
       <c r="AZ57" s="1"/>
@@ -76776,7 +76817,7 @@
         <v>24</v>
       </c>
       <c r="CV57" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="CW57" s="1"/>
       <c r="CX57" s="1"/>
@@ -76845,7 +76886,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:171" ht="15">
+    <row r="58" spans="1:172" ht="15">
       <c r="A58" s="9">
         <v>24793376</v>
       </c>
@@ -77001,7 +77042,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:171" ht="15">
+    <row r="59" spans="1:172" ht="15">
       <c r="A59" s="9">
         <v>24713456</v>
       </c>
@@ -77155,7 +77196,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:171" ht="15">
+    <row r="60" spans="1:172" ht="15">
       <c r="A60" s="9">
         <v>24713371</v>
       </c>
@@ -77301,7 +77342,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:171" ht="15">
+    <row r="61" spans="1:172" ht="15">
       <c r="A61" s="9">
         <v>24713222</v>
       </c>
@@ -77459,7 +77500,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:171" ht="15">
+    <row r="62" spans="1:172" ht="15">
       <c r="A62" s="12">
         <v>24636087</v>
       </c>
@@ -77679,8 +77720,11 @@
       <c r="FO62" s="4">
         <v>24</v>
       </c>
+      <c r="FP62" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="63" spans="1:171" ht="15">
+    <row r="63" spans="1:172" ht="15">
       <c r="A63" s="9">
         <v>24636090</v>
       </c>
@@ -77900,8 +77944,11 @@
       <c r="FO63" s="4">
         <v>24</v>
       </c>
+      <c r="FP63" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="64" spans="1:171" ht="15">
+    <row r="64" spans="1:172" ht="15">
       <c r="A64" s="9">
         <v>24636091</v>
       </c>
@@ -78121,8 +78168,11 @@
       <c r="FO64" s="4">
         <v>24</v>
       </c>
+      <c r="FP64" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="65" spans="1:171" ht="15">
+    <row r="65" spans="1:172" ht="15">
       <c r="A65" s="9">
         <v>24636089</v>
       </c>
@@ -78140,6 +78190,9 @@
       </c>
       <c r="F65" s="13">
         <v>45755</v>
+      </c>
+      <c r="P65" s="3">
+        <v>45759</v>
       </c>
       <c r="AY65" s="1"/>
       <c r="AZ65" s="1"/>
@@ -78216,7 +78269,9 @@
       <c r="DM65" s="1">
         <v>24</v>
       </c>
-      <c r="DN65" s="1"/>
+      <c r="DN65" s="1">
+        <v>22</v>
+      </c>
       <c r="DO65" s="1"/>
       <c r="DP65" s="1"/>
       <c r="DQ65" s="1"/>
@@ -78266,7 +78321,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:171" ht="15">
+    <row r="66" spans="1:172" ht="15">
       <c r="A66" s="9">
         <v>24636088</v>
       </c>
@@ -78284,6 +78339,9 @@
       </c>
       <c r="F66" s="13">
         <v>45755</v>
+      </c>
+      <c r="P66" s="3">
+        <v>45759</v>
       </c>
       <c r="AY66" s="1"/>
       <c r="AZ66" s="1"/>
@@ -78360,7 +78418,9 @@
       <c r="DM66" s="1">
         <v>24</v>
       </c>
-      <c r="DN66" s="1"/>
+      <c r="DN66" s="1">
+        <v>22</v>
+      </c>
       <c r="DO66" s="1"/>
       <c r="DP66" s="1"/>
       <c r="DQ66" s="1"/>
@@ -78410,7 +78470,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:171" ht="15">
+    <row r="67" spans="1:172" ht="15">
       <c r="A67" s="9">
         <v>25017935</v>
       </c>
@@ -78544,7 +78604,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:171" ht="15">
+    <row r="68" spans="1:172" ht="15">
       <c r="A68" s="9">
         <v>25017936</v>
       </c>
@@ -78691,7 +78751,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:171" ht="15">
+    <row r="69" spans="1:172" ht="15">
       <c r="A69" s="9">
         <v>25017937</v>
       </c>
@@ -78825,7 +78885,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:171" ht="15">
+    <row r="70" spans="1:172" ht="15">
       <c r="A70" s="9">
         <v>25019644</v>
       </c>
@@ -78959,7 +79019,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:171" ht="15">
+    <row r="71" spans="1:172" ht="15">
       <c r="A71" s="9">
         <v>25019645</v>
       </c>
@@ -79106,7 +79166,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:171" ht="15">
+    <row r="72" spans="1:172" ht="15">
       <c r="A72" s="9">
         <v>25019646</v>
       </c>
@@ -79240,7 +79300,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:171" ht="15">
+    <row r="73" spans="1:172" ht="15">
       <c r="A73" s="9">
         <v>24848800</v>
       </c>
@@ -79480,8 +79540,11 @@
       <c r="FO73" s="4">
         <v>24</v>
       </c>
+      <c r="FP73" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="74" spans="1:171" ht="15">
+    <row r="74" spans="1:172" ht="15">
       <c r="A74" s="9">
         <v>24859051</v>
       </c>
@@ -79721,8 +79784,11 @@
       <c r="FO74" s="4">
         <v>24</v>
       </c>
+      <c r="FP74" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="75" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="75" spans="1:172" ht="15">
       <c r="A75" s="9">
         <v>24988445</v>
       </c>
@@ -79739,7 +79805,6 @@
         <v>96</v>
       </c>
       <c r="F75" s="13"/>
-      <c r="P75" s="3"/>
       <c r="AY75" s="1"/>
       <c r="AZ75" s="1"/>
       <c r="BA75" s="1"/>
@@ -79857,7 +79922,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="76" spans="1:172" ht="15">
       <c r="A76" s="9">
         <v>24988559</v>
       </c>
@@ -79874,7 +79939,6 @@
         <v>96</v>
       </c>
       <c r="F76" s="13"/>
-      <c r="P76" s="3"/>
       <c r="AY76" s="1"/>
       <c r="AZ76" s="1"/>
       <c r="BA76" s="1"/>
@@ -79992,7 +80056,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="77" spans="1:172" ht="15">
       <c r="A77" s="9">
         <v>24988692</v>
       </c>
@@ -80009,7 +80073,6 @@
         <v>162</v>
       </c>
       <c r="F77" s="13"/>
-      <c r="P77" s="3"/>
       <c r="AY77" s="1"/>
       <c r="AZ77" s="1"/>
       <c r="BA77" s="1"/>
@@ -80127,7 +80190,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="78" spans="1:172" ht="15">
       <c r="A78" s="9">
         <v>24923318</v>
       </c>
@@ -80146,7 +80209,6 @@
       <c r="F78" s="13">
         <v>45793</v>
       </c>
-      <c r="P78" s="3"/>
       <c r="AY78" s="1"/>
       <c r="AZ78" s="1"/>
       <c r="BA78" s="1"/>
@@ -80308,8 +80370,11 @@
       <c r="FO78" s="4">
         <v>24</v>
       </c>
+      <c r="FP78" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="79" spans="1:172" ht="15">
       <c r="A79" s="9">
         <v>24925212</v>
       </c>
@@ -80326,7 +80391,6 @@
         <v>1000</v>
       </c>
       <c r="F79" s="13"/>
-      <c r="P79" s="3"/>
       <c r="AY79" s="1"/>
       <c r="AZ79" s="1"/>
       <c r="BA79" s="1"/>
@@ -80444,7 +80508,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="80" spans="1:172" ht="15">
       <c r="A80" s="9">
         <v>24857462</v>
       </c>
@@ -80463,7 +80527,6 @@
       <c r="F80" s="13">
         <v>45792</v>
       </c>
-      <c r="P80" s="3"/>
       <c r="AY80" s="1"/>
       <c r="AZ80" s="1"/>
       <c r="BA80" s="1"/>
@@ -80627,8 +80690,11 @@
       <c r="FO80" s="4">
         <v>12</v>
       </c>
+      <c r="FP80" s="4">
+        <v>12</v>
+      </c>
     </row>
-    <row r="81" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="81" spans="1:172" ht="15">
       <c r="A81" s="10">
         <v>25112301</v>
       </c>
@@ -80668,11 +80734,8 @@
       <c r="FN81" s="4">
         <v>24</v>
       </c>
-      <c r="FO81" s="4">
-        <v>24</v>
-      </c>
     </row>
-    <row r="82" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="82" spans="1:172" ht="15">
       <c r="A82" s="10">
         <v>25112300</v>
       </c>
@@ -80691,7 +80754,6 @@
       <c r="F82" s="14">
         <v>45806</v>
       </c>
-      <c r="P82" s="3"/>
       <c r="FI82" s="4">
         <v>11</v>
       </c>
@@ -80713,8 +80775,11 @@
       <c r="FO82" s="4">
         <v>24</v>
       </c>
+      <c r="FP82" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="83" spans="1:172" ht="15">
       <c r="A83" s="10">
         <v>25087863</v>
       </c>
@@ -80754,11 +80819,8 @@
       <c r="FN83" s="4">
         <v>24</v>
       </c>
-      <c r="FO83" s="4">
-        <v>24</v>
-      </c>
     </row>
-    <row r="84" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="84" spans="1:172" ht="15">
       <c r="A84" s="10">
         <v>25087787</v>
       </c>
@@ -80774,10 +80836,8 @@
       <c r="E84" s="10">
         <v>1000</v>
       </c>
-      <c r="F84" s="14"/>
-      <c r="P84" s="3"/>
     </row>
-    <row r="85" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="85" spans="1:172" ht="15">
       <c r="A85" s="10">
         <v>24848184</v>
       </c>
@@ -80796,7 +80856,6 @@
       <c r="F85" s="13">
         <v>45792</v>
       </c>
-      <c r="P85" s="3"/>
       <c r="EU85" s="4">
         <v>8</v>
       </c>
@@ -80860,8 +80919,11 @@
       <c r="FO85" s="4">
         <v>12</v>
       </c>
+      <c r="FP85" s="4">
+        <v>12</v>
+      </c>
     </row>
-    <row r="86" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="86" spans="1:172" ht="15">
       <c r="A86" s="16">
         <v>50872159</v>
       </c>
@@ -80880,9 +80942,8 @@
       <c r="F86" s="19">
         <v>45793</v>
       </c>
-      <c r="P86" s="3"/>
     </row>
-    <row r="87" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="87" spans="1:172" ht="15">
       <c r="A87" s="16">
         <v>25019645</v>
       </c>
@@ -80899,9 +80960,8 @@
         <v>96</v>
       </c>
       <c r="F87" s="19"/>
-      <c r="P87" s="3"/>
     </row>
-    <row r="88" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="88" spans="1:172" ht="15">
       <c r="A88" s="16">
         <v>25017936</v>
       </c>
@@ -80918,9 +80978,8 @@
         <v>96</v>
       </c>
       <c r="F88" s="19"/>
-      <c r="P88" s="3"/>
     </row>
-    <row r="89" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="89" spans="1:172" ht="15">
       <c r="A89" s="16">
         <v>25089372</v>
       </c>
@@ -80979,7 +81038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="90" spans="1:172" ht="15">
       <c r="A90" s="16">
         <v>25089365</v>
       </c>
@@ -81038,7 +81097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="91" spans="1:172" ht="15">
       <c r="A91" s="16">
         <v>25089363</v>
       </c>
@@ -81097,7 +81156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="92" spans="1:172" ht="15">
       <c r="A92" s="16">
         <v>25089370</v>
       </c>
@@ -81156,7 +81215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="93" spans="1:172" ht="15">
       <c r="A93" s="16">
         <v>25112299</v>
       </c>
@@ -81215,7 +81274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="94" spans="1:172" ht="15">
       <c r="A94" s="16">
         <v>72149637</v>
       </c>
@@ -81271,7 +81330,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="95" spans="1:172" ht="15">
       <c r="A95" s="16">
         <v>72238923</v>
       </c>
@@ -81288,9 +81347,8 @@
         <v>1000</v>
       </c>
       <c r="F95" s="19"/>
-      <c r="P95" s="3"/>
     </row>
-    <row r="96" spans="1:171" s="4" customFormat="1" ht="15">
+    <row r="96" spans="1:172" ht="15">
       <c r="A96" s="16">
         <v>25089372</v>
       </c>
@@ -81307,9 +81365,8 @@
         <v>96</v>
       </c>
       <c r="F96" s="19"/>
-      <c r="P96" s="3"/>
     </row>
-    <row r="97" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="97" spans="1:6" ht="15">
       <c r="A97" s="16">
         <v>25089365</v>
       </c>
@@ -81326,9 +81383,8 @@
         <v>96</v>
       </c>
       <c r="F97" s="19"/>
-      <c r="P97" s="3"/>
     </row>
-    <row r="98" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="98" spans="1:6" ht="15">
       <c r="A98" s="16">
         <v>25089363</v>
       </c>
@@ -81345,9 +81401,8 @@
         <v>1000</v>
       </c>
       <c r="F98" s="19"/>
-      <c r="P98" s="3"/>
     </row>
-    <row r="99" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="99" spans="1:6" ht="15">
       <c r="A99" s="16">
         <v>25089370</v>
       </c>
@@ -81364,9 +81419,8 @@
         <v>1000</v>
       </c>
       <c r="F99" s="19"/>
-      <c r="P99" s="3"/>
     </row>
-    <row r="100" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="100" spans="1:6" ht="15">
       <c r="A100" s="16">
         <v>25112301</v>
       </c>
@@ -81383,9 +81437,8 @@
         <v>96</v>
       </c>
       <c r="F100" s="19"/>
-      <c r="P100" s="3"/>
     </row>
-    <row r="101" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="101" spans="1:6" ht="15">
       <c r="A101" s="10">
         <v>72309509</v>
       </c>
@@ -81401,10 +81454,8 @@
       <c r="E101" s="10">
         <v>96</v>
       </c>
-      <c r="F101" s="14"/>
-      <c r="P101" s="3"/>
     </row>
-    <row r="102" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="102" spans="1:6" ht="15">
       <c r="A102" s="10">
         <v>72304210</v>
       </c>
@@ -81420,10 +81471,8 @@
       <c r="E102" s="10">
         <v>96</v>
       </c>
-      <c r="F102" s="14"/>
-      <c r="P102" s="3"/>
     </row>
-    <row r="103" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="103" spans="1:6" ht="15">
       <c r="A103" s="10">
         <v>25263837</v>
       </c>
@@ -81439,10 +81488,8 @@
       <c r="E103" s="10">
         <v>96</v>
       </c>
-      <c r="F103" s="14"/>
-      <c r="P103" s="3"/>
     </row>
-    <row r="104" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="104" spans="1:6" ht="15">
       <c r="A104" s="10">
         <v>25264958</v>
       </c>
@@ -81458,97 +81505,17 @@
       <c r="E104" s="10">
         <v>96</v>
       </c>
-      <c r="F104" s="14"/>
-      <c r="P104" s="3"/>
     </row>
-    <row r="105" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A105" s="10"/>
-      <c r="B105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10"/>
-      <c r="F105" s="14"/>
-      <c r="P105" s="3"/>
-    </row>
-    <row r="106" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A106" s="10"/>
-      <c r="B106" s="10"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="10"/>
-      <c r="F106" s="14"/>
-      <c r="P106" s="3"/>
-    </row>
-    <row r="107" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A107" s="10"/>
-      <c r="B107" s="10"/>
-      <c r="D107" s="10"/>
-      <c r="E107" s="10"/>
-      <c r="F107" s="14"/>
-      <c r="P107" s="3"/>
-    </row>
-    <row r="108" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10"/>
-      <c r="F108" s="14"/>
-      <c r="P108" s="3"/>
-    </row>
-    <row r="109" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A109" s="10"/>
-      <c r="B109" s="10"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="10"/>
-      <c r="F109" s="14"/>
-      <c r="P109" s="3"/>
-    </row>
-    <row r="110" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A110" s="10"/>
-      <c r="B110" s="10"/>
-      <c r="D110" s="10"/>
-      <c r="E110" s="10"/>
-      <c r="F110" s="14"/>
-      <c r="P110" s="3"/>
-    </row>
-    <row r="111" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A111" s="10"/>
-      <c r="B111" s="10"/>
-      <c r="D111" s="10"/>
-      <c r="E111" s="10"/>
-      <c r="F111" s="14"/>
-      <c r="P111" s="3"/>
-    </row>
-    <row r="112" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A112" s="10"/>
-      <c r="B112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="10"/>
-      <c r="F112" s="14"/>
-      <c r="P112" s="3"/>
-    </row>
-    <row r="113" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A113" s="10"/>
-      <c r="B113" s="10"/>
-      <c r="D113" s="10"/>
-      <c r="E113" s="10"/>
-      <c r="F113" s="14"/>
-      <c r="P113" s="3"/>
-    </row>
-    <row r="114" spans="1:16" s="4" customFormat="1" ht="15">
-      <c r="A114" s="10"/>
-      <c r="B114" s="10"/>
-      <c r="D114" s="10"/>
-      <c r="E114" s="10"/>
-      <c r="F114" s="14"/>
-      <c r="P114" s="3"/>
-    </row>
-    <row r="115" spans="1:16" s="4" customFormat="1">
-      <c r="A115" s="10"/>
-      <c r="B115" s="10"/>
-      <c r="D115" s="10"/>
-      <c r="E115" s="10"/>
-      <c r="F115" s="14"/>
-      <c r="P115" s="3"/>
-    </row>
+    <row r="105" spans="1:6" ht="15"/>
+    <row r="106" spans="1:6" ht="15"/>
+    <row r="107" spans="1:6" ht="15"/>
+    <row r="108" spans="1:6" ht="15"/>
+    <row r="109" spans="1:6" ht="15"/>
+    <row r="110" spans="1:6" ht="15"/>
+    <row r="111" spans="1:6" ht="15"/>
+    <row r="112" spans="1:6" ht="15"/>
+    <row r="113" ht="15"/>
+    <row r="114" ht="15"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun  6 09:30:22 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="504" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F878D522-C5BD-4795-ADEE-D75CF3555C9E}"/>
+  <xr:revisionPtr revIDLastSave="509" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63DF047F-C777-4E7A-9466-09ED94033F79}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -975,8 +975,8 @@
   <dimension ref="A1:XFD114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="CO40" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="CU47" sqref="CU47"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FA54" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="P55" sqref="P55"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -71349,7 +71349,7 @@
         <v>45712</v>
       </c>
       <c r="P24" s="3">
-        <v>45813</v>
+        <v>45721</v>
       </c>
       <c r="AY24" s="1"/>
       <c r="AZ24" s="1"/>
@@ -71495,6 +71495,9 @@
       <c r="F25" s="13">
         <v>45712</v>
       </c>
+      <c r="P25" s="3">
+        <v>45721</v>
+      </c>
       <c r="AY25" s="1"/>
       <c r="AZ25" s="1"/>
       <c r="BA25" s="1"/>
@@ -71530,7 +71533,9 @@
       <c r="BY25" s="1"/>
       <c r="BZ25" s="1"/>
       <c r="CA25" s="1"/>
-      <c r="CB25" s="1"/>
+      <c r="CB25" s="1">
+        <v>51</v>
+      </c>
       <c r="CC25" s="1"/>
       <c r="CD25" s="1"/>
       <c r="CE25" s="1"/>
@@ -76367,6 +76372,9 @@
       <c r="F55" s="13">
         <v>45733</v>
       </c>
+      <c r="P55" s="3">
+        <v>45799</v>
+      </c>
       <c r="AY55" s="1"/>
       <c r="AZ55" s="1"/>
       <c r="BA55" s="1"/>
@@ -76526,7 +76534,9 @@
       <c r="EY55" s="1"/>
       <c r="EZ55" s="1"/>
       <c r="FA55" s="1"/>
-      <c r="FB55" s="1"/>
+      <c r="FB55" s="1">
+        <v>502</v>
+      </c>
       <c r="FC55" s="1"/>
       <c r="FD55" s="1"/>
       <c r="FE55" s="1"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun  6 09:38:51 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="509" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63DF047F-C777-4E7A-9466-09ED94033F79}"/>
+  <xr:revisionPtr revIDLastSave="511" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EB15155-E614-4FFD-96B8-CFBEBF1B614C}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -975,8 +975,8 @@
   <dimension ref="A1:XFD114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FA54" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="P55" sqref="P55"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="Q70" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E75" sqref="E75"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -79324,7 +79324,7 @@
         <v>28</v>
       </c>
       <c r="E73" s="9">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="F73" s="13">
         <v>45763</v>
@@ -79568,7 +79568,7 @@
         <v>28</v>
       </c>
       <c r="E74" s="9">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="F74" s="13">
         <v>45763</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun  6 11:34:24 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EB15155-E614-4FFD-96B8-CFBEBF1B614C}"/>
+  <xr:revisionPtr revIDLastSave="534" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B192C712-2E46-47F3-B1A8-E55F5D4B305A}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="143">
   <si>
     <t>Module ID</t>
   </si>
@@ -447,6 +447,24 @@
   </si>
   <si>
     <t>VSL202526117</t>
+  </si>
+  <si>
+    <t>VSL202526118</t>
+  </si>
+  <si>
+    <t>Hangzhou First Low GSM Trial (420F,400B)</t>
+  </si>
+  <si>
+    <t>VSL202526119</t>
+  </si>
+  <si>
+    <t>VSL202526120</t>
+  </si>
+  <si>
+    <t>VSL202526121</t>
+  </si>
+  <si>
+    <t>VSL202526122</t>
   </si>
 </sst>
 </file>
@@ -975,8 +993,8 @@
   <dimension ref="A1:XFD114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="Q70" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E75" sqref="E75"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FP95" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FR104" sqref="FR104"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -81376,7 +81394,7 @@
       </c>
       <c r="F96" s="19"/>
     </row>
-    <row r="97" spans="1:6" ht="15">
+    <row r="97" spans="1:173" ht="15">
       <c r="A97" s="16">
         <v>25089365</v>
       </c>
@@ -81394,7 +81412,7 @@
       </c>
       <c r="F97" s="19"/>
     </row>
-    <row r="98" spans="1:6" ht="15">
+    <row r="98" spans="1:173" ht="15">
       <c r="A98" s="16">
         <v>25089363</v>
       </c>
@@ -81412,7 +81430,7 @@
       </c>
       <c r="F98" s="19"/>
     </row>
-    <row r="99" spans="1:6" ht="15">
+    <row r="99" spans="1:173" ht="15">
       <c r="A99" s="16">
         <v>25089370</v>
       </c>
@@ -81430,7 +81448,7 @@
       </c>
       <c r="F99" s="19"/>
     </row>
-    <row r="100" spans="1:6" ht="15">
+    <row r="100" spans="1:173" ht="15">
       <c r="A100" s="16">
         <v>25112301</v>
       </c>
@@ -81448,7 +81466,7 @@
       </c>
       <c r="F100" s="19"/>
     </row>
-    <row r="101" spans="1:6" ht="15">
+    <row r="101" spans="1:173" ht="15">
       <c r="A101" s="10">
         <v>72309509</v>
       </c>
@@ -81464,8 +81482,14 @@
       <c r="E101" s="10">
         <v>96</v>
       </c>
+      <c r="F101" s="14">
+        <v>45814</v>
+      </c>
+      <c r="FQ101" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="102" spans="1:6" ht="15">
+    <row r="102" spans="1:173" ht="15">
       <c r="A102" s="10">
         <v>72304210</v>
       </c>
@@ -81481,8 +81505,14 @@
       <c r="E102" s="10">
         <v>96</v>
       </c>
+      <c r="F102" s="14">
+        <v>45814</v>
+      </c>
+      <c r="FQ102" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="103" spans="1:6" ht="15">
+    <row r="103" spans="1:173" ht="15">
       <c r="A103" s="10">
         <v>25263837</v>
       </c>
@@ -81498,8 +81528,14 @@
       <c r="E103" s="10">
         <v>96</v>
       </c>
+      <c r="F103" s="14">
+        <v>45814</v>
+      </c>
+      <c r="FQ103" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="104" spans="1:6" ht="15">
+    <row r="104" spans="1:173" ht="15">
       <c r="A104" s="10">
         <v>25264958</v>
       </c>
@@ -81515,15 +81551,101 @@
       <c r="E104" s="10">
         <v>96</v>
       </c>
+      <c r="F104" s="14">
+        <v>45814</v>
+      </c>
+      <c r="FQ104" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="105" spans="1:6" ht="15"/>
-    <row r="106" spans="1:6" ht="15"/>
-    <row r="107" spans="1:6" ht="15"/>
-    <row r="108" spans="1:6" ht="15"/>
-    <row r="109" spans="1:6" ht="15"/>
-    <row r="110" spans="1:6" ht="15"/>
-    <row r="111" spans="1:6" ht="15"/>
-    <row r="112" spans="1:6" ht="15"/>
+    <row r="105" spans="1:173" ht="15">
+      <c r="A105" s="10">
+        <v>25273922</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D105" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E105" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:173" ht="15">
+      <c r="A106" s="10">
+        <v>25273923</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D106" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="107" spans="1:173" ht="15">
+      <c r="A107" s="10">
+        <v>25273924</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E107" s="10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:173" ht="15">
+      <c r="A108" s="10">
+        <v>25273925</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D108" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E108" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:173" ht="15">
+      <c r="A109" s="10">
+        <v>25273926</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D109" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E109" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:173" ht="15"/>
+    <row r="111" spans="1:173" ht="15"/>
+    <row r="112" spans="1:173" ht="15"/>
     <row r="113" ht="15"/>
     <row r="114" ht="15"/>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun  9 09:39:50 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="542" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C4C88DC-341B-4F8E-BB5D-1F362692136B}"/>
+  <xr:revisionPtr revIDLastSave="554" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A0FB4DE-CE92-4EDA-B034-ACFCDCF30C54}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="143">
   <si>
     <t>Module ID</t>
   </si>
@@ -992,8 +992,8 @@
   <dimension ref="A1:XFD114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="DA77" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F81" sqref="F81"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FR71" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GF64" sqref="GF64"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -68438,6 +68438,12 @@
       <c r="FO8" s="3">
         <v>24</v>
       </c>
+      <c r="FP8" s="3">
+        <v>24</v>
+      </c>
+      <c r="FQ8" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:16384" s="3" customFormat="1" ht="15">
       <c r="A9" s="8">
@@ -68701,6 +68707,12 @@
       </c>
       <c r="FO9" s="3">
         <v>24</v>
+      </c>
+      <c r="FP9" s="3">
+        <v>24</v>
+      </c>
+      <c r="FQ9" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:16384" s="3" customFormat="1" ht="15">
@@ -75335,7 +75347,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:172" ht="15">
+    <row r="49" spans="1:173" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75469,7 +75481,7 @@
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
     </row>
-    <row r="50" spans="1:172" ht="15">
+    <row r="50" spans="1:173" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75680,7 +75692,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:172" ht="15">
+    <row r="51" spans="1:173" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -75891,7 +75903,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:172" ht="15">
+    <row r="52" spans="1:173" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76102,7 +76114,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:172" ht="15">
+    <row r="53" spans="1:173" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76236,7 +76248,7 @@
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
     </row>
-    <row r="54" spans="1:172" ht="15">
+    <row r="54" spans="1:173" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76370,7 +76382,7 @@
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
     </row>
-    <row r="55" spans="1:172" ht="15">
+    <row r="55" spans="1:173" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76563,7 +76575,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:172" ht="15">
+    <row r="56" spans="1:173" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76756,7 +76768,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:172" ht="15">
+    <row r="57" spans="1:173" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -76913,7 +76925,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:172" ht="15">
+    <row r="58" spans="1:173" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77069,7 +77081,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:172" ht="15">
+    <row r="59" spans="1:173" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77223,7 +77235,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:172" ht="15">
+    <row r="60" spans="1:173" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77369,7 +77381,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:172" ht="15">
+    <row r="61" spans="1:173" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77527,7 +77539,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:172" ht="15">
+    <row r="62" spans="1:173" ht="15">
       <c r="A62" s="11">
         <v>24636087</v>
       </c>
@@ -77750,8 +77762,11 @@
       <c r="FP62" s="3">
         <v>24</v>
       </c>
+      <c r="FQ62" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="63" spans="1:172" ht="15">
+    <row r="63" spans="1:173" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -77974,8 +77989,11 @@
       <c r="FP63" s="3">
         <v>24</v>
       </c>
+      <c r="FQ63" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="64" spans="1:172" ht="15">
+    <row r="64" spans="1:173" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78198,8 +78216,11 @@
       <c r="FP64" s="3">
         <v>24</v>
       </c>
+      <c r="FQ64" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="65" spans="1:172" ht="15">
+    <row r="65" spans="1:173" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78348,7 +78369,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:172" ht="15">
+    <row r="66" spans="1:173" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78497,7 +78518,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:172" ht="15">
+    <row r="67" spans="1:173" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78631,7 +78652,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:172" ht="15">
+    <row r="68" spans="1:173" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -78778,7 +78799,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:172" ht="15">
+    <row r="69" spans="1:173" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -78912,7 +78933,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:172" ht="15">
+    <row r="70" spans="1:173" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79046,7 +79067,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:172" ht="15">
+    <row r="71" spans="1:173" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79193,7 +79214,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:172" ht="15">
+    <row r="72" spans="1:173" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79327,7 +79348,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:172" ht="15">
+    <row r="73" spans="1:173" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79570,8 +79591,11 @@
       <c r="FP73" s="3">
         <v>24</v>
       </c>
+      <c r="FQ73" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="74" spans="1:172" ht="15">
+    <row r="74" spans="1:173" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -79814,8 +79838,11 @@
       <c r="FP74" s="3">
         <v>24</v>
       </c>
+      <c r="FQ74" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="75" spans="1:172" ht="15">
+    <row r="75" spans="1:173" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -79949,7 +79976,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:172" ht="15">
+    <row r="76" spans="1:173" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80083,7 +80110,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:172" ht="15">
+    <row r="77" spans="1:173" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80217,7 +80244,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:172" ht="15">
+    <row r="78" spans="1:173" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80400,8 +80427,11 @@
       <c r="FP78" s="3">
         <v>24</v>
       </c>
+      <c r="FQ78" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="79" spans="1:172" ht="15">
+    <row r="79" spans="1:173" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80535,7 +80565,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:172" ht="15">
+    <row r="80" spans="1:173" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -80720,6 +80750,9 @@
       <c r="FP80" s="3">
         <v>12</v>
       </c>
+      <c r="FQ80" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="81" spans="1:173" ht="15">
       <c r="A81" s="9">
@@ -80804,6 +80837,9 @@
       </c>
       <c r="FP82" s="3">
         <v>24</v>
+      </c>
+      <c r="FQ82" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:173" ht="15">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun  9 13:47:06 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="554" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A0FB4DE-CE92-4EDA-B034-ACFCDCF30C54}"/>
+  <xr:revisionPtr revIDLastSave="606" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08588BFD-4144-4938-979F-CDE7E90A62E9}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="155">
   <si>
     <t>Module ID</t>
   </si>
@@ -465,6 +465,42 @@
   </si>
   <si>
     <t>VSL202526122</t>
+  </si>
+  <si>
+    <t>VSL202526091</t>
+  </si>
+  <si>
+    <t>Sunsure HYPERSOL Internal Reliability Tests</t>
+  </si>
+  <si>
+    <t>VSL202526090</t>
+  </si>
+  <si>
+    <t>VSL202526084</t>
+  </si>
+  <si>
+    <t>VSL202526089</t>
+  </si>
+  <si>
+    <t>VSL202526092</t>
+  </si>
+  <si>
+    <t>VSL202526093</t>
+  </si>
+  <si>
+    <t>VSL202526094</t>
+  </si>
+  <si>
+    <t>Sunsure HYPERSOL Internal Reliability Tests (DH 1000+SML)</t>
+  </si>
+  <si>
+    <t>VSL202526085</t>
+  </si>
+  <si>
+    <t>VSL202526101</t>
+  </si>
+  <si>
+    <t>VSL202526103</t>
   </si>
 </sst>
 </file>
@@ -989,11 +1025,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD114"/>
+  <dimension ref="A1:XFD119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FR71" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GF64" sqref="GF64"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FR106" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="D112" sqref="D112"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -81684,11 +81720,194 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:173" ht="15"/>
-    <row r="111" spans="1:173" ht="15"/>
-    <row r="112" spans="1:173" ht="15"/>
-    <row r="113" ht="15"/>
-    <row r="114" ht="15"/>
+    <row r="110" spans="1:173" ht="15">
+      <c r="A110" s="9">
+        <v>25119247</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" s="9">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="111" spans="1:173" ht="15">
+      <c r="A111" s="9">
+        <v>25121350</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C111" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E111" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="112" spans="1:173" ht="15">
+      <c r="A112" s="9">
+        <v>25121029</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C112" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E112" s="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:176" ht="15">
+      <c r="A113" s="9">
+        <v>25120989</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C113" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E113" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="114" spans="1:176" ht="15">
+      <c r="A114" s="9">
+        <v>25129692</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D114" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E114" s="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:176" ht="15">
+      <c r="A115" s="9">
+        <v>25129767</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:176" ht="15">
+      <c r="A116" s="9">
+        <v>25129647</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D116" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E116" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:176" ht="15">
+      <c r="A117" s="9">
+        <v>25129669</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C117" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D117" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E117" s="9">
+        <v>60</v>
+      </c>
+      <c r="F117" s="13">
+        <v>45817</v>
+      </c>
+      <c r="FT117" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:176" ht="15">
+      <c r="A118" s="9">
+        <v>25173191</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D118" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E118" s="9">
+        <v>20</v>
+      </c>
+      <c r="F118" s="13">
+        <v>45817</v>
+      </c>
+      <c r="FT118" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:176" ht="15">
+      <c r="A119" s="9">
+        <v>25170488</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C119" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D119" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E119" s="9">
+        <v>60</v>
+      </c>
+      <c r="F119" s="13">
+        <v>45817</v>
+      </c>
+      <c r="FT119" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun 10 09:39:49 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="606" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08588BFD-4144-4938-979F-CDE7E90A62E9}"/>
+  <xr:revisionPtr revIDLastSave="666" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F537380-773B-4078-A0A6-1292FE862226}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="156">
   <si>
     <t>Module ID</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>VSL202526103</t>
+  </si>
+  <si>
+    <t>VSL202526108</t>
   </si>
 </sst>
 </file>
@@ -1025,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD119"/>
+  <dimension ref="A1:XFD120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FR106" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D112" sqref="D112"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FO92" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FU105" sqref="FU105"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -68480,6 +68483,15 @@
       <c r="FQ8" s="3">
         <v>9</v>
       </c>
+      <c r="FR8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS8" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT8" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:16384" s="3" customFormat="1" ht="15">
       <c r="A9" s="8">
@@ -68749,6 +68761,15 @@
       </c>
       <c r="FQ9" s="3">
         <v>9</v>
+      </c>
+      <c r="FR9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS9" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT9" s="3">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:16384" s="3" customFormat="1" ht="15">
@@ -75383,7 +75404,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:173" ht="15">
+    <row r="49" spans="1:176" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75517,7 +75538,7 @@
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
     </row>
-    <row r="50" spans="1:173" ht="15">
+    <row r="50" spans="1:176" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75728,7 +75749,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:173" ht="15">
+    <row r="51" spans="1:176" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -75939,7 +75960,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:173" ht="15">
+    <row r="52" spans="1:176" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76150,7 +76171,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:173" ht="15">
+    <row r="53" spans="1:176" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76284,7 +76305,7 @@
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
     </row>
-    <row r="54" spans="1:173" ht="15">
+    <row r="54" spans="1:176" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76418,7 +76439,7 @@
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
     </row>
-    <row r="55" spans="1:173" ht="15">
+    <row r="55" spans="1:176" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76611,7 +76632,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:173" ht="15">
+    <row r="56" spans="1:176" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76804,7 +76825,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:173" ht="15">
+    <row r="57" spans="1:176" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -76961,7 +76982,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:173" ht="15">
+    <row r="58" spans="1:176" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77117,7 +77138,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:173" ht="15">
+    <row r="59" spans="1:176" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77271,7 +77292,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:173" ht="15">
+    <row r="60" spans="1:176" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77417,7 +77438,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:173" ht="15">
+    <row r="61" spans="1:176" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77575,7 +77596,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:173" ht="15">
+    <row r="62" spans="1:176" ht="15">
       <c r="A62" s="11">
         <v>24636087</v>
       </c>
@@ -77801,8 +77822,17 @@
       <c r="FQ62" s="3">
         <v>9</v>
       </c>
+      <c r="FR62" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS62" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT62" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="63" spans="1:173" ht="15">
+    <row r="63" spans="1:176" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78028,8 +78058,17 @@
       <c r="FQ63" s="3">
         <v>9</v>
       </c>
+      <c r="FR63" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS63" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT63" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="64" spans="1:173" ht="15">
+    <row r="64" spans="1:176" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78255,8 +78294,17 @@
       <c r="FQ64" s="3">
         <v>9</v>
       </c>
+      <c r="FR64" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS64" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT64" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="65" spans="1:173" ht="15">
+    <row r="65" spans="1:176" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78405,7 +78453,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:173" ht="15">
+    <row r="66" spans="1:176" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78554,7 +78602,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:173" ht="15">
+    <row r="67" spans="1:176" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78688,7 +78736,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:173" ht="15">
+    <row r="68" spans="1:176" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -78835,7 +78883,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:173" ht="15">
+    <row r="69" spans="1:176" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -78969,7 +79017,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:173" ht="15">
+    <row r="70" spans="1:176" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79103,7 +79151,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:173" ht="15">
+    <row r="71" spans="1:176" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79250,7 +79298,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:173" ht="15">
+    <row r="72" spans="1:176" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79384,7 +79432,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:173" ht="15">
+    <row r="73" spans="1:176" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79630,8 +79678,17 @@
       <c r="FQ73" s="3">
         <v>9</v>
       </c>
+      <c r="FR73" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS73" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT73" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="74" spans="1:173" ht="15">
+    <row r="74" spans="1:176" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -79877,8 +79934,17 @@
       <c r="FQ74" s="3">
         <v>9</v>
       </c>
+      <c r="FR74" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS74" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT74" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="75" spans="1:173" ht="15">
+    <row r="75" spans="1:176" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80012,7 +80078,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:173" ht="15">
+    <row r="76" spans="1:176" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80146,7 +80212,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:173" ht="15">
+    <row r="77" spans="1:176" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80280,7 +80346,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:173" ht="15">
+    <row r="78" spans="1:176" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80466,8 +80532,17 @@
       <c r="FQ78" s="3">
         <v>9</v>
       </c>
+      <c r="FR78" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS78" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:173" ht="15">
+    <row r="79" spans="1:176" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80601,7 +80676,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:173" ht="15">
+    <row r="80" spans="1:176" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81471,7 +81546,7 @@
       </c>
       <c r="F96" s="18"/>
     </row>
-    <row r="97" spans="1:173" ht="15">
+    <row r="97" spans="1:176" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81489,7 +81564,7 @@
       </c>
       <c r="F97" s="18"/>
     </row>
-    <row r="98" spans="1:173" ht="15">
+    <row r="98" spans="1:176" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81507,7 +81582,7 @@
       </c>
       <c r="F98" s="18"/>
     </row>
-    <row r="99" spans="1:173" ht="15">
+    <row r="99" spans="1:176" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81525,7 +81600,7 @@
       </c>
       <c r="F99" s="18"/>
     </row>
-    <row r="100" spans="1:173" ht="15">
+    <row r="100" spans="1:176" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -81543,7 +81618,7 @@
       </c>
       <c r="F100" s="18"/>
     </row>
-    <row r="101" spans="1:173" ht="15">
+    <row r="101" spans="1:176" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -81565,8 +81640,17 @@
       <c r="FQ101" s="3">
         <v>24</v>
       </c>
+      <c r="FR101" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS101" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT101" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="102" spans="1:173" ht="15">
+    <row r="102" spans="1:176" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -81588,8 +81672,17 @@
       <c r="FQ102" s="3">
         <v>24</v>
       </c>
+      <c r="FR102" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS102" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT102" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="103" spans="1:173" ht="15">
+    <row r="103" spans="1:176" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -81611,8 +81704,17 @@
       <c r="FQ103" s="3">
         <v>24</v>
       </c>
+      <c r="FR103" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS103" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT103" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="104" spans="1:173" ht="15">
+    <row r="104" spans="1:176" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -81634,8 +81736,17 @@
       <c r="FQ104" s="3">
         <v>24</v>
       </c>
+      <c r="FR104" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS104" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT104" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="105" spans="1:173" ht="15">
+    <row r="105" spans="1:176" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -81652,7 +81763,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:173" ht="15">
+    <row r="106" spans="1:176" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -81669,7 +81780,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="107" spans="1:173" ht="15">
+    <row r="107" spans="1:176" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -81686,7 +81797,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="108" spans="1:173" ht="15">
+    <row r="108" spans="1:176" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -81703,7 +81814,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:173" ht="15">
+    <row r="109" spans="1:176" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -81720,7 +81831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:173" ht="15">
+    <row r="110" spans="1:176" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -81736,8 +81847,11 @@
       <c r="E110" s="9">
         <v>288</v>
       </c>
+      <c r="F110" s="13">
+        <v>45818</v>
+      </c>
     </row>
-    <row r="111" spans="1:173" ht="15">
+    <row r="111" spans="1:176" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -81753,8 +81867,11 @@
       <c r="E111" s="9">
         <v>96</v>
       </c>
+      <c r="F111" s="13">
+        <v>45818</v>
+      </c>
     </row>
-    <row r="112" spans="1:173" ht="15">
+    <row r="112" spans="1:176" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -81765,13 +81882,16 @@
         <v>144</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E112" s="9">
-        <v>200</v>
+        <v>60</v>
+      </c>
+      <c r="F112" s="13">
+        <v>45818</v>
       </c>
     </row>
-    <row r="113" spans="1:176" ht="15">
+    <row r="113" spans="1:177" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -81787,8 +81907,11 @@
       <c r="E113" s="9">
         <v>96</v>
       </c>
+      <c r="F113" s="13">
+        <v>45818</v>
+      </c>
     </row>
-    <row r="114" spans="1:176" ht="15">
+    <row r="114" spans="1:177" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -81804,8 +81927,11 @@
       <c r="E114" s="9">
         <v>200</v>
       </c>
+      <c r="F114" s="13">
+        <v>45818</v>
+      </c>
     </row>
-    <row r="115" spans="1:176" ht="15">
+    <row r="115" spans="1:177" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -81821,8 +81947,11 @@
       <c r="E115" s="9">
         <v>1000</v>
       </c>
+      <c r="F115" s="13">
+        <v>45818</v>
+      </c>
     </row>
-    <row r="116" spans="1:176" ht="15">
+    <row r="116" spans="1:177" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -81838,8 +81967,11 @@
       <c r="E116" s="9">
         <v>1000</v>
       </c>
+      <c r="F116" s="13">
+        <v>45818</v>
+      </c>
     </row>
-    <row r="117" spans="1:176" ht="15">
+    <row r="117" spans="1:177" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -81856,13 +81988,13 @@
         <v>60</v>
       </c>
       <c r="F117" s="13">
-        <v>45817</v>
-      </c>
-      <c r="FT117" s="3">
-        <v>1</v>
+        <v>45818</v>
+      </c>
+      <c r="FU117" s="3">
+        <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:176" ht="15">
+    <row r="118" spans="1:177" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -81884,8 +82016,11 @@
       <c r="FT118" s="3">
         <v>1</v>
       </c>
+      <c r="FU118" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="119" spans="1:176" ht="15">
+    <row r="119" spans="1:177" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -81906,6 +82041,35 @@
       </c>
       <c r="FT119" s="3">
         <v>1</v>
+      </c>
+      <c r="FU119" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:177" ht="15">
+      <c r="A120" s="9">
+        <v>25176404</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D120" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E120" s="9">
+        <v>60</v>
+      </c>
+      <c r="F120" s="13">
+        <v>45817</v>
+      </c>
+      <c r="FT120" s="3">
+        <v>1</v>
+      </c>
+      <c r="FU120" s="3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun 10 11:34:39 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="666" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F537380-773B-4078-A0A6-1292FE862226}"/>
+  <xr:revisionPtr revIDLastSave="674" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE2F6DC7-C327-4FCC-9385-28D24E7407F7}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1031,8 +1031,8 @@
   <dimension ref="A1:XFD120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FO92" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FU105" sqref="FU105"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FR72" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A73" sqref="A73:XFD73"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -81546,7 +81546,7 @@
       </c>
       <c r="F96" s="18"/>
     </row>
-    <row r="97" spans="1:176" ht="15">
+    <row r="97" spans="1:177" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81564,7 +81564,7 @@
       </c>
       <c r="F97" s="18"/>
     </row>
-    <row r="98" spans="1:176" ht="15">
+    <row r="98" spans="1:177" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81582,7 +81582,7 @@
       </c>
       <c r="F98" s="18"/>
     </row>
-    <row r="99" spans="1:176" ht="15">
+    <row r="99" spans="1:177" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81600,7 +81600,7 @@
       </c>
       <c r="F99" s="18"/>
     </row>
-    <row r="100" spans="1:176" ht="15">
+    <row r="100" spans="1:177" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -81618,7 +81618,7 @@
       </c>
       <c r="F100" s="18"/>
     </row>
-    <row r="101" spans="1:176" ht="15">
+    <row r="101" spans="1:177" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -81650,7 +81650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:176" ht="15">
+    <row r="102" spans="1:177" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -81682,7 +81682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:176" ht="15">
+    <row r="103" spans="1:177" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -81714,7 +81714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:176" ht="15">
+    <row r="104" spans="1:177" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -81746,7 +81746,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:176" ht="15">
+    <row r="105" spans="1:177" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -81763,7 +81763,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:176" ht="15">
+    <row r="106" spans="1:177" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -81780,7 +81780,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="107" spans="1:176" ht="15">
+    <row r="107" spans="1:177" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -81797,7 +81797,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="108" spans="1:176" ht="15">
+    <row r="108" spans="1:177" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -81814,7 +81814,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:176" ht="15">
+    <row r="109" spans="1:177" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -81831,7 +81831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:176" ht="15">
+    <row r="110" spans="1:177" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -81850,8 +81850,11 @@
       <c r="F110" s="13">
         <v>45818</v>
       </c>
+      <c r="FU110" s="3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="111" spans="1:176" ht="15">
+    <row r="111" spans="1:177" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -81870,8 +81873,11 @@
       <c r="F111" s="13">
         <v>45818</v>
       </c>
+      <c r="FU111" s="3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="112" spans="1:176" ht="15">
+    <row r="112" spans="1:177" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -81910,6 +81916,9 @@
       <c r="F113" s="13">
         <v>45818</v>
       </c>
+      <c r="FU113" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="114" spans="1:177" ht="15">
       <c r="A114" s="9">
@@ -81930,6 +81939,9 @@
       <c r="F114" s="13">
         <v>45818</v>
       </c>
+      <c r="FU114" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="115" spans="1:177" ht="15">
       <c r="A115" s="9">
@@ -81950,6 +81962,9 @@
       <c r="F115" s="13">
         <v>45818</v>
       </c>
+      <c r="FU115" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="116" spans="1:177" ht="15">
       <c r="A116" s="9">
@@ -81969,6 +81984,9 @@
       </c>
       <c r="F116" s="13">
         <v>45818</v>
+      </c>
+      <c r="FU116" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:177" ht="15">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 11 09:40:05 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="674" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE2F6DC7-C327-4FCC-9385-28D24E7407F7}"/>
+  <xr:revisionPtr revIDLastSave="676" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4BFFF58-538B-4B34-9CA8-70F81D067290}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1031,8 +1031,8 @@
   <dimension ref="A1:XFD120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FR72" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A73" sqref="A73:XFD73"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FQ107" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FU115" sqref="FU115"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -81896,6 +81896,9 @@
       <c r="F112" s="13">
         <v>45818</v>
       </c>
+      <c r="FU112" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="113" spans="1:177" ht="15">
       <c r="A113" s="9">
@@ -81940,7 +81943,7 @@
         <v>45818</v>
       </c>
       <c r="FU114" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:177" ht="15">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 11 11:34:44 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1031,8 +1031,8 @@
   <dimension ref="A1:XFD120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FQ107" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FU115" sqref="FU115"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FM91" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FS107" sqref="FS107"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 11 13:47:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="676" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4BFFF58-538B-4B34-9CA8-70F81D067290}"/>
+  <xr:revisionPtr revIDLastSave="683" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C5DD8F7-D5FF-466C-8D69-133924C03CBC}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="156">
   <si>
     <t>Module ID</t>
   </si>
@@ -677,7 +677,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1028,11 +1038,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD120"/>
+  <dimension ref="A1:XFD122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FM91" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FS107" sqref="FS107"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FT108" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F122" sqref="F122"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -81005,10 +81015,10 @@
         <v>116</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E84" s="9">
-        <v>1000</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:173" ht="15">
@@ -82091,6 +82101,40 @@
       </c>
       <c r="FU120" s="3">
         <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:177" ht="15">
+      <c r="A121" s="9">
+        <v>25087863</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E121" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:177" ht="15">
+      <c r="A122" s="15">
+        <v>72149637</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C122" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E122" s="9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -82101,10 +82145,13 @@
     <protectedRange sqref="A85 Q1:XFD1048576" name="Range3"/>
   </protectedRanges>
   <conditionalFormatting sqref="A91">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86:A90 A92:A100">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A122">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D86:D100" xr:uid="{AE741107-2DDE-448F-B66D-3CC4D6043D49}">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 11 15:40:12 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C5DD8F7-D5FF-466C-8D69-133924C03CBC}"/>
+  <xr:revisionPtr revIDLastSave="695" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C61CBF1E-BCFD-4800-AA6B-5954811A638C}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="156">
   <si>
     <t>Module ID</t>
   </si>
@@ -1041,8 +1041,8 @@
   <dimension ref="A1:XFD122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FT108" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F122" sqref="F122"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FQ107" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FV74" sqref="FV74"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -78314,7 +78314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:176" ht="15">
+    <row r="65" spans="1:178" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78463,7 +78463,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:176" ht="15">
+    <row r="66" spans="1:178" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78612,7 +78612,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:176" ht="15">
+    <row r="67" spans="1:178" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78746,7 +78746,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:176" ht="15">
+    <row r="68" spans="1:178" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -78893,7 +78893,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:176" ht="15">
+    <row r="69" spans="1:178" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79027,7 +79027,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:176" ht="15">
+    <row r="70" spans="1:178" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79161,7 +79161,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:176" ht="15">
+    <row r="71" spans="1:178" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79308,7 +79308,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:176" ht="15">
+    <row r="72" spans="1:178" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79442,7 +79442,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:176" ht="15">
+    <row r="73" spans="1:178" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79460,6 +79460,9 @@
       </c>
       <c r="F73" s="12">
         <v>45763</v>
+      </c>
+      <c r="P73" s="13">
+        <v>45819</v>
       </c>
       <c r="AY73" s="1"/>
       <c r="AZ73" s="1"/>
@@ -79697,8 +79700,14 @@
       <c r="FT73" s="3">
         <v>24</v>
       </c>
+      <c r="FU73" s="3">
+        <v>5</v>
+      </c>
+      <c r="FV73" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="74" spans="1:176" ht="15">
+    <row r="74" spans="1:178" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -79716,6 +79725,9 @@
       </c>
       <c r="F74" s="12">
         <v>45763</v>
+      </c>
+      <c r="P74" s="13">
+        <v>45819</v>
       </c>
       <c r="AY74" s="1"/>
       <c r="AZ74" s="1"/>
@@ -79953,8 +79965,14 @@
       <c r="FT74" s="3">
         <v>24</v>
       </c>
+      <c r="FU74" s="3">
+        <v>5</v>
+      </c>
+      <c r="FV74" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="75" spans="1:176" ht="15">
+    <row r="75" spans="1:178" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80088,7 +80106,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:176" ht="15">
+    <row r="76" spans="1:178" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80222,7 +80240,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:176" ht="15">
+    <row r="77" spans="1:178" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80356,7 +80374,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:176" ht="15">
+    <row r="78" spans="1:178" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80552,7 +80570,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:176" ht="15">
+    <row r="79" spans="1:178" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80686,7 +80704,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:176" ht="15">
+    <row r="80" spans="1:178" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81659,6 +81677,9 @@
       <c r="FT101" s="3">
         <v>24</v>
       </c>
+      <c r="FU101" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="102" spans="1:177" ht="15">
       <c r="A102" s="9">
@@ -81691,6 +81712,9 @@
       <c r="FT102" s="3">
         <v>24</v>
       </c>
+      <c r="FU102" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="103" spans="1:177" ht="15">
       <c r="A103" s="9">
@@ -81723,6 +81747,9 @@
       <c r="FT103" s="3">
         <v>24</v>
       </c>
+      <c r="FU103" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="104" spans="1:177" ht="15">
       <c r="A104" s="9">
@@ -81754,6 +81781,9 @@
       </c>
       <c r="FT104" s="3">
         <v>24</v>
+      </c>
+      <c r="FU104" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:177" ht="15">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun 12 09:39:48 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="695" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C61CBF1E-BCFD-4800-AA6B-5954811A638C}"/>
+  <xr:revisionPtr revIDLastSave="703" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5098FEEE-A7F6-4F0D-A81C-C832D4B432EA}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1041,8 +1041,8 @@
   <dimension ref="A1:XFD122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FQ107" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FV74" sqref="FV74"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FT115" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C125" sqref="C125"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun 12 11:34:48 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="703" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5098FEEE-A7F6-4F0D-A81C-C832D4B432EA}"/>
+  <xr:revisionPtr revIDLastSave="710" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10AEB6C5-3E55-40C7-B945-003FAC93EE18}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1041,8 +1041,8 @@
   <dimension ref="A1:XFD122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FT115" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C125" sqref="C125"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FR94" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F107" sqref="F107"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -81572,7 +81572,9 @@
       <c r="E96" s="15">
         <v>96</v>
       </c>
-      <c r="F96" s="18"/>
+      <c r="F96" s="18">
+        <v>45820</v>
+      </c>
     </row>
     <row r="97" spans="1:177" ht="15">
       <c r="A97" s="15">
@@ -81590,7 +81592,9 @@
       <c r="E97" s="15">
         <v>96</v>
       </c>
-      <c r="F97" s="18"/>
+      <c r="F97" s="18">
+        <v>45820</v>
+      </c>
     </row>
     <row r="98" spans="1:177" ht="15">
       <c r="A98" s="15">
@@ -81608,7 +81612,9 @@
       <c r="E98" s="15">
         <v>1000</v>
       </c>
-      <c r="F98" s="18"/>
+      <c r="F98" s="18">
+        <v>45820</v>
+      </c>
     </row>
     <row r="99" spans="1:177" ht="15">
       <c r="A99" s="15">
@@ -81626,7 +81632,9 @@
       <c r="E99" s="15">
         <v>1000</v>
       </c>
-      <c r="F99" s="18"/>
+      <c r="F99" s="18">
+        <v>45820</v>
+      </c>
     </row>
     <row r="100" spans="1:177" ht="15">
       <c r="A100" s="15">
@@ -81819,6 +81827,9 @@
       <c r="E106" s="9">
         <v>96</v>
       </c>
+      <c r="F106" s="13">
+        <v>45820</v>
+      </c>
     </row>
     <row r="107" spans="1:177" ht="15">
       <c r="A107" s="9">
@@ -81836,6 +81847,9 @@
       <c r="E107" s="9">
         <v>1000</v>
       </c>
+      <c r="F107" s="13">
+        <v>45820</v>
+      </c>
     </row>
     <row r="108" spans="1:177" ht="15">
       <c r="A108" s="9">
@@ -82165,6 +82179,9 @@
       </c>
       <c r="E122" s="9">
         <v>10</v>
+      </c>
+      <c r="F122" s="13">
+        <v>45820</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun 13 09:39:14 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="710" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10AEB6C5-3E55-40C7-B945-003FAC93EE18}"/>
+  <xr:revisionPtr revIDLastSave="770" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15A39452-60D0-4280-B52E-6AEDF24A3B86}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="160">
   <si>
     <t>Module ID</t>
   </si>
@@ -504,6 +504,18 @@
   </si>
   <si>
     <t>VSL202526108</t>
+  </si>
+  <si>
+    <t>VSL202526123</t>
+  </si>
+  <si>
+    <t>HIUV EPE+EVA encapsulant trial</t>
+  </si>
+  <si>
+    <t>VSL202526124</t>
+  </si>
+  <si>
+    <t>VSL202526125</t>
   </si>
 </sst>
 </file>
@@ -1038,11 +1050,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD122"/>
+  <dimension ref="A1:XFD125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FR94" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F107" sqref="F107"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FR106" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FX109" sqref="FX109"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -78314,7 +78326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:178" ht="15">
+    <row r="65" spans="1:179" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78463,7 +78475,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:178" ht="15">
+    <row r="66" spans="1:179" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78612,7 +78624,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:178" ht="15">
+    <row r="67" spans="1:179" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78746,7 +78758,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:178" ht="15">
+    <row r="68" spans="1:179" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -78893,7 +78905,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:178" ht="15">
+    <row r="69" spans="1:179" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79027,7 +79039,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:178" ht="15">
+    <row r="70" spans="1:179" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79161,7 +79173,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:178" ht="15">
+    <row r="71" spans="1:179" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79308,7 +79320,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:178" ht="15">
+    <row r="72" spans="1:179" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79442,7 +79454,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:178" ht="15">
+    <row r="73" spans="1:179" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79707,7 +79719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:178" ht="15">
+    <row r="74" spans="1:179" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -79972,7 +79984,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:178" ht="15">
+    <row r="75" spans="1:179" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80106,7 +80118,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:178" ht="15">
+    <row r="76" spans="1:179" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80240,7 +80252,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:178" ht="15">
+    <row r="77" spans="1:179" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80374,7 +80386,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:178" ht="15">
+    <row r="78" spans="1:179" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80569,8 +80581,17 @@
       <c r="FT78" s="3">
         <v>24</v>
       </c>
+      <c r="FU78" s="3">
+        <v>24</v>
+      </c>
+      <c r="FV78" s="3">
+        <v>24</v>
+      </c>
+      <c r="FW78" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="79" spans="1:178" ht="15">
+    <row r="79" spans="1:179" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80704,7 +80725,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:178" ht="15">
+    <row r="80" spans="1:179" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -80893,7 +80914,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:173" ht="15">
+    <row r="81" spans="1:179" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -80934,7 +80955,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:173" ht="15">
+    <row r="82" spans="1:179" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -80980,8 +81001,26 @@
       <c r="FQ82" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="FR82" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="FS82" s="3">
+        <v>8</v>
+      </c>
+      <c r="FT82" s="3">
+        <v>24</v>
+      </c>
+      <c r="FU82" s="3">
+        <v>24</v>
+      </c>
+      <c r="FV82" s="3">
+        <v>24</v>
+      </c>
+      <c r="FW82" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="83" spans="1:173" ht="15">
+    <row r="83" spans="1:179" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81022,7 +81061,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:173" ht="15">
+    <row r="84" spans="1:179" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81038,8 +81077,11 @@
       <c r="E84" s="9">
         <v>60</v>
       </c>
+      <c r="F84" s="13">
+        <v>45821</v>
+      </c>
     </row>
-    <row r="85" spans="1:173" ht="15">
+    <row r="85" spans="1:179" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81131,7 +81173,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:173" ht="15">
+    <row r="86" spans="1:179" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81151,7 +81193,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:173" ht="15">
+    <row r="87" spans="1:179" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81169,7 +81211,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:173" ht="15">
+    <row r="88" spans="1:179" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81187,7 +81229,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:173" ht="15">
+    <row r="89" spans="1:179" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81246,7 +81288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:173" ht="15">
+    <row r="90" spans="1:179" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81305,7 +81347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:173" ht="15">
+    <row r="91" spans="1:179" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81364,7 +81406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:173" ht="15">
+    <row r="92" spans="1:179" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81423,7 +81465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:173" ht="15">
+    <row r="93" spans="1:179" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81482,7 +81524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:173" ht="15">
+    <row r="94" spans="1:179" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -81538,7 +81580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:173" ht="15">
+    <row r="95" spans="1:179" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -81556,7 +81598,7 @@
       </c>
       <c r="F95" s="18"/>
     </row>
-    <row r="96" spans="1:173" ht="15">
+    <row r="96" spans="1:179" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -81575,8 +81617,11 @@
       <c r="F96" s="18">
         <v>45820</v>
       </c>
+      <c r="FW96" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="97" spans="1:177" ht="15">
+    <row r="97" spans="1:179" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81595,8 +81640,11 @@
       <c r="F97" s="18">
         <v>45820</v>
       </c>
+      <c r="FW97" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="98" spans="1:177" ht="15">
+    <row r="98" spans="1:179" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81615,8 +81663,11 @@
       <c r="F98" s="18">
         <v>45820</v>
       </c>
+      <c r="FW98" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="99" spans="1:177" ht="15">
+    <row r="99" spans="1:179" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81636,7 +81687,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:177" ht="15">
+    <row r="100" spans="1:179" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -81654,7 +81705,7 @@
       </c>
       <c r="F100" s="18"/>
     </row>
-    <row r="101" spans="1:177" ht="15">
+    <row r="101" spans="1:179" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -81689,7 +81740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:177" ht="15">
+    <row r="102" spans="1:179" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -81724,7 +81775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:177" ht="15">
+    <row r="103" spans="1:179" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -81759,7 +81810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:177" ht="15">
+    <row r="104" spans="1:179" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -81794,7 +81845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:177" ht="15">
+    <row r="105" spans="1:179" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -81810,8 +81861,14 @@
       <c r="E105" s="9">
         <v>60</v>
       </c>
+      <c r="F105" s="13">
+        <v>45821</v>
+      </c>
+      <c r="FW105" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="106" spans="1:177" ht="15">
+    <row r="106" spans="1:179" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -81830,8 +81887,11 @@
       <c r="F106" s="13">
         <v>45820</v>
       </c>
+      <c r="FW106" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="107" spans="1:177" ht="15">
+    <row r="107" spans="1:179" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -81850,8 +81910,11 @@
       <c r="F107" s="13">
         <v>45820</v>
       </c>
+      <c r="FW107" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="108" spans="1:177" ht="15">
+    <row r="108" spans="1:179" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -81867,8 +81930,11 @@
       <c r="E108" s="9">
         <v>60</v>
       </c>
+      <c r="F108" s="13">
+        <v>45821</v>
+      </c>
     </row>
-    <row r="109" spans="1:177" ht="15">
+    <row r="109" spans="1:179" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -81885,7 +81951,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:177" ht="15">
+    <row r="110" spans="1:179" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -81907,8 +81973,14 @@
       <c r="FU110" s="3">
         <v>12</v>
       </c>
+      <c r="FV110" s="3">
+        <v>24</v>
+      </c>
+      <c r="FW110" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="111" spans="1:177" ht="15">
+    <row r="111" spans="1:179" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -81930,8 +82002,14 @@
       <c r="FU111" s="3">
         <v>12</v>
       </c>
+      <c r="FV111" s="3">
+        <v>24</v>
+      </c>
+      <c r="FW111" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="112" spans="1:177" ht="15">
+    <row r="112" spans="1:179" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -81953,8 +82031,14 @@
       <c r="FU112" s="3">
         <v>5</v>
       </c>
+      <c r="FV112" s="3">
+        <v>5</v>
+      </c>
+      <c r="FW112" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="113" spans="1:177" ht="15">
+    <row r="113" spans="1:179" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -81976,8 +82060,14 @@
       <c r="FU113" s="3">
         <v>12</v>
       </c>
+      <c r="FV113" s="3">
+        <v>24</v>
+      </c>
+      <c r="FW113" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="114" spans="1:177" ht="15">
+    <row r="114" spans="1:179" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -81999,8 +82089,14 @@
       <c r="FU114" s="3">
         <v>10</v>
       </c>
+      <c r="FV114" s="3">
+        <v>16</v>
+      </c>
+      <c r="FW114" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="115" spans="1:177" ht="15">
+    <row r="115" spans="1:179" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -82022,8 +82118,14 @@
       <c r="FU115" s="3">
         <v>12</v>
       </c>
+      <c r="FV115" s="3">
+        <v>24</v>
+      </c>
+      <c r="FW115" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="116" spans="1:177" ht="15">
+    <row r="116" spans="1:179" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -82045,8 +82147,14 @@
       <c r="FU116" s="3">
         <v>12</v>
       </c>
+      <c r="FV116" s="3">
+        <v>24</v>
+      </c>
+      <c r="FW116" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="117" spans="1:177" ht="15">
+    <row r="117" spans="1:179" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -82068,8 +82176,14 @@
       <c r="FU117" s="3">
         <v>5</v>
       </c>
+      <c r="FV117" s="3">
+        <v>5</v>
+      </c>
+      <c r="FW117" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:177" ht="15">
+    <row r="118" spans="1:179" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -82094,8 +82208,14 @@
       <c r="FU118" s="3">
         <v>5</v>
       </c>
+      <c r="FV118" s="3">
+        <v>5</v>
+      </c>
+      <c r="FW118" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="119" spans="1:177" ht="15">
+    <row r="119" spans="1:179" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -82120,8 +82240,14 @@
       <c r="FU119" s="3">
         <v>5</v>
       </c>
+      <c r="FV119" s="3">
+        <v>5</v>
+      </c>
+      <c r="FW119" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:177" ht="15">
+    <row r="120" spans="1:179" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -82146,8 +82272,14 @@
       <c r="FU120" s="3">
         <v>5</v>
       </c>
+      <c r="FV120" s="3">
+        <v>5</v>
+      </c>
+      <c r="FW120" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="121" spans="1:177" ht="15">
+    <row r="121" spans="1:179" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -82164,7 +82296,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="122" spans="1:177" ht="15">
+    <row r="122" spans="1:179" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -82182,6 +82314,57 @@
       </c>
       <c r="F122" s="13">
         <v>45820</v>
+      </c>
+    </row>
+    <row r="123" spans="1:179" ht="15">
+      <c r="A123" s="9">
+        <v>25321818</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C123" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E123" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:179" ht="15">
+      <c r="A124" s="9">
+        <v>25321819</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C124" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E124" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="125" spans="1:179" ht="15">
+      <c r="A125" s="9">
+        <v>25321820</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C125" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D125" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E125" s="9">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 16 07:52:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="770" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15A39452-60D0-4280-B52E-6AEDF24A3B86}"/>
+  <xr:revisionPtr revIDLastSave="919" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01F93DB7-3391-4375-918B-CDB535C17C28}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="165">
   <si>
     <t>Module ID</t>
   </si>
@@ -305,6 +305,9 @@
     <t>VSL202425372</t>
   </si>
   <si>
+    <t>hold</t>
+  </si>
+  <si>
     <t>VSL202425381</t>
   </si>
   <si>
@@ -516,6 +519,18 @@
   </si>
   <si>
     <t>VSL202526125</t>
+  </si>
+  <si>
+    <t>VSL202526109</t>
+  </si>
+  <si>
+    <t>VSL202526112</t>
+  </si>
+  <si>
+    <t>VSL202526102</t>
+  </si>
+  <si>
+    <t>VSL202526106</t>
   </si>
 </sst>
 </file>
@@ -1050,11 +1065,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD125"/>
+  <dimension ref="A1:XFD129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FR106" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FX109" sqref="FX109"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FV87" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GA96" sqref="GA96"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -75426,7 +75441,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:176" ht="15">
+    <row r="49" spans="1:177" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75560,7 +75575,7 @@
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
     </row>
-    <row r="50" spans="1:176" ht="15">
+    <row r="50" spans="1:177" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75771,7 +75786,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:176" ht="15">
+    <row r="51" spans="1:177" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -75982,7 +75997,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:176" ht="15">
+    <row r="52" spans="1:177" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76193,7 +76208,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:176" ht="15">
+    <row r="53" spans="1:177" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76327,7 +76342,7 @@
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
     </row>
-    <row r="54" spans="1:176" ht="15">
+    <row r="54" spans="1:177" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76461,7 +76476,7 @@
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
     </row>
-    <row r="55" spans="1:176" ht="15">
+    <row r="55" spans="1:177" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76654,7 +76669,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:176" ht="15">
+    <row r="56" spans="1:177" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76847,7 +76862,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:176" ht="15">
+    <row r="57" spans="1:177" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77004,7 +77019,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:176" ht="15">
+    <row r="58" spans="1:177" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77160,7 +77175,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:176" ht="15">
+    <row r="59" spans="1:177" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77314,7 +77329,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:176" ht="15">
+    <row r="60" spans="1:177" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77460,7 +77475,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:176" ht="15">
+    <row r="61" spans="1:177" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77618,8 +77633,8 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:176" ht="15">
-      <c r="A62" s="11">
+    <row r="62" spans="1:177" ht="15">
+      <c r="A62" s="8">
         <v>24636087</v>
       </c>
       <c r="B62" s="8" t="s">
@@ -77853,8 +77868,11 @@
       <c r="FT62" s="3">
         <v>24</v>
       </c>
+      <c r="FU62" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="63" spans="1:176" ht="15">
+    <row r="63" spans="1:177" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78089,8 +78107,11 @@
       <c r="FT63" s="3">
         <v>24</v>
       </c>
+      <c r="FU63" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="64" spans="1:176" ht="15">
+    <row r="64" spans="1:177" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78325,8 +78346,11 @@
       <c r="FT64" s="3">
         <v>24</v>
       </c>
+      <c r="FU64" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="65" spans="1:179" ht="15">
+    <row r="65" spans="1:182" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78475,7 +78499,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:179" ht="15">
+    <row r="66" spans="1:182" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78624,15 +78648,15 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:179" ht="15">
+    <row r="67" spans="1:182" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>32</v>
@@ -78640,7 +78664,12 @@
       <c r="E67" s="8">
         <v>60</v>
       </c>
-      <c r="F67" s="12"/>
+      <c r="F67" s="12">
+        <v>45764</v>
+      </c>
+      <c r="P67" s="13">
+        <v>45775</v>
+      </c>
       <c r="AY67" s="1"/>
       <c r="AZ67" s="1"/>
       <c r="BA67" s="1"/>
@@ -78758,15 +78787,15 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:179" ht="15">
+    <row r="68" spans="1:182" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
       <c r="B68" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>18</v>
@@ -78905,15 +78934,15 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:179" ht="15">
+    <row r="69" spans="1:182" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>28</v>
@@ -79039,15 +79068,15 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:179" ht="15">
+    <row r="70" spans="1:182" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>32</v>
@@ -79055,7 +79084,12 @@
       <c r="E70" s="8">
         <v>60</v>
       </c>
-      <c r="F70" s="12"/>
+      <c r="F70" s="12">
+        <v>45764</v>
+      </c>
+      <c r="P70" s="13">
+        <v>45775</v>
+      </c>
       <c r="AY70" s="1"/>
       <c r="AZ70" s="1"/>
       <c r="BA70" s="1"/>
@@ -79128,18 +79162,42 @@
       <c r="DP70" s="1"/>
       <c r="DQ70" s="1"/>
       <c r="DR70" s="1"/>
-      <c r="DS70" s="1"/>
-      <c r="DT70" s="1"/>
-      <c r="DU70" s="1"/>
-      <c r="DV70" s="1"/>
-      <c r="DW70" s="1"/>
-      <c r="DX70" s="1"/>
-      <c r="DY70" s="1"/>
-      <c r="DZ70" s="1"/>
-      <c r="EA70" s="1"/>
-      <c r="EB70" s="1"/>
-      <c r="EC70" s="1"/>
-      <c r="ED70" s="1"/>
+      <c r="DS70" s="1">
+        <v>5</v>
+      </c>
+      <c r="DT70" s="1">
+        <v>5</v>
+      </c>
+      <c r="DU70" s="1">
+        <v>5</v>
+      </c>
+      <c r="DV70" s="1">
+        <v>5</v>
+      </c>
+      <c r="DW70" s="1">
+        <v>5</v>
+      </c>
+      <c r="DX70" s="1">
+        <v>5</v>
+      </c>
+      <c r="DY70" s="1">
+        <v>5</v>
+      </c>
+      <c r="DZ70" s="1">
+        <v>5</v>
+      </c>
+      <c r="EA70" s="1">
+        <v>5</v>
+      </c>
+      <c r="EB70" s="1">
+        <v>5</v>
+      </c>
+      <c r="EC70" s="1">
+        <v>5</v>
+      </c>
+      <c r="ED70" s="1">
+        <v>5</v>
+      </c>
       <c r="EE70" s="1"/>
       <c r="EF70" s="1"/>
       <c r="EG70" s="1"/>
@@ -79173,15 +79231,15 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:179" ht="15">
+    <row r="71" spans="1:182" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
       <c r="B71" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>18</v>
@@ -79320,15 +79378,15 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:179" ht="15">
+    <row r="72" spans="1:182" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>28</v>
@@ -79454,15 +79512,15 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:179" ht="15">
+    <row r="73" spans="1:182" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>28</v>
@@ -79716,18 +79774,18 @@
         <v>5</v>
       </c>
       <c r="FV73" s="3" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:179" ht="15">
+    <row r="74" spans="1:182" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>28</v>
@@ -79981,21 +80039,21 @@
         <v>5</v>
       </c>
       <c r="FV74" s="3" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:179" ht="15">
+    <row r="75" spans="1:182" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E75" s="8">
         <v>96</v>
@@ -80118,15 +80176,15 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:179" ht="15">
+    <row r="76" spans="1:182" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>18</v>
@@ -80252,18 +80310,18 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:179" ht="15">
+    <row r="77" spans="1:182" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E77" s="8">
         <v>162</v>
@@ -80386,15 +80444,15 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:179" ht="15">
+    <row r="78" spans="1:182" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>28</v>
@@ -80590,16 +80648,25 @@
       <c r="FW78" s="3">
         <v>19</v>
       </c>
+      <c r="FX78" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY78" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:179" ht="15">
+    <row r="79" spans="1:182" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
       <c r="B79" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>28</v>
@@ -80725,15 +80792,15 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:179" ht="15">
+    <row r="80" spans="1:182" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>21</v>
@@ -80914,15 +80981,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:179" ht="15">
+    <row r="81" spans="1:182" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>18</v>
@@ -80955,15 +81022,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:179" ht="15">
+    <row r="82" spans="1:182" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>28</v>
@@ -81019,16 +81086,25 @@
       <c r="FW82" s="3">
         <v>19</v>
       </c>
+      <c r="FX82" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY82" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:179" ht="15">
+    <row r="83" spans="1:182" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>18</v>
@@ -81061,15 +81137,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:179" ht="15">
+    <row r="84" spans="1:182" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
       <c r="B84" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>32</v>
@@ -81080,16 +81156,25 @@
       <c r="F84" s="13">
         <v>45821</v>
       </c>
+      <c r="FX84" s="3">
+        <v>5</v>
+      </c>
+      <c r="FY84" s="3">
+        <v>5</v>
+      </c>
+      <c r="FZ84" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:179" ht="15">
+    <row r="85" spans="1:182" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>21</v>
@@ -81173,15 +81258,15 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:179" ht="15">
+    <row r="86" spans="1:182" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>18</v>
@@ -81193,15 +81278,15 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:179" ht="15">
+    <row r="87" spans="1:182" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
       <c r="B87" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C87" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="C87" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>18</v>
@@ -81211,15 +81296,15 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:179" ht="15">
+    <row r="88" spans="1:182" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
       <c r="B88" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>18</v>
@@ -81229,15 +81314,15 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:179" ht="15">
+    <row r="89" spans="1:182" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>32</v>
@@ -81288,15 +81373,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:179" ht="15">
+    <row r="90" spans="1:182" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>32</v>
@@ -81347,15 +81432,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:179" ht="15">
+    <row r="91" spans="1:182" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
       <c r="B91" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C91" s="17" t="s">
         <v>125</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>124</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>32</v>
@@ -81406,15 +81491,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:179" ht="15">
+    <row r="92" spans="1:182" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>32</v>
@@ -81465,15 +81550,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:179" ht="15">
+    <row r="93" spans="1:182" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>32</v>
@@ -81524,15 +81609,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:179" ht="15">
+    <row r="94" spans="1:182" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>21</v>
@@ -81580,15 +81665,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:179" ht="15">
+    <row r="95" spans="1:182" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>28</v>
@@ -81598,15 +81683,15 @@
       </c>
       <c r="F95" s="18"/>
     </row>
-    <row r="96" spans="1:179" ht="15">
+    <row r="96" spans="1:182" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>18</v>
@@ -81620,16 +81705,25 @@
       <c r="FW96" s="3">
         <v>7</v>
       </c>
+      <c r="FX96" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY96" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ96" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="97" spans="1:179" ht="15">
+    <row r="97" spans="1:182" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>18</v>
@@ -81643,16 +81737,25 @@
       <c r="FW97" s="3">
         <v>7</v>
       </c>
+      <c r="FX97" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY97" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ97" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="98" spans="1:179" ht="15">
+    <row r="98" spans="1:182" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
       <c r="B98" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C98" s="17" t="s">
         <v>125</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>124</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>28</v>
@@ -81666,16 +81769,25 @@
       <c r="FW98" s="3">
         <v>7</v>
       </c>
+      <c r="FX98" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY98" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:179" ht="15">
+    <row r="99" spans="1:182" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>28</v>
@@ -81687,15 +81799,15 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:179" ht="15">
+    <row r="100" spans="1:182" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D100" s="15" t="s">
         <v>18</v>
@@ -81705,15 +81817,15 @@
       </c>
       <c r="F100" s="18"/>
     </row>
-    <row r="101" spans="1:179" ht="15">
+    <row r="101" spans="1:182" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>18</v>
@@ -81737,18 +81849,18 @@
         <v>24</v>
       </c>
       <c r="FU101" s="3">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:179" ht="15">
+    <row r="102" spans="1:182" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
       <c r="B102" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C102" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="C102" s="17" t="s">
-        <v>133</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>18</v>
@@ -81772,18 +81884,18 @@
         <v>24</v>
       </c>
       <c r="FU102" s="3">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:179" ht="15">
+    <row r="103" spans="1:182" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>18</v>
@@ -81810,15 +81922,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:179" ht="15">
+    <row r="104" spans="1:182" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>18</v>
@@ -81842,18 +81954,18 @@
         <v>24</v>
       </c>
       <c r="FU104" s="3">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:179" ht="15">
+    <row r="105" spans="1:182" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>32</v>
@@ -81865,18 +81977,27 @@
         <v>45821</v>
       </c>
       <c r="FW105" s="3">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="FX105" s="3">
+        <v>5</v>
+      </c>
+      <c r="FY105" s="3">
+        <v>5</v>
+      </c>
+      <c r="FZ105" s="3">
+        <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:179" ht="15">
+    <row r="106" spans="1:182" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
       <c r="B106" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C106" s="17" t="s">
         <v>139</v>
-      </c>
-      <c r="C106" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>18</v>
@@ -81890,16 +82011,25 @@
       <c r="FW106" s="3">
         <v>7</v>
       </c>
+      <c r="FX106" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY106" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ106" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="107" spans="1:179" ht="15">
+    <row r="107" spans="1:182" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>28</v>
@@ -81913,16 +82043,25 @@
       <c r="FW107" s="3">
         <v>7</v>
       </c>
+      <c r="FX107" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY107" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:179" ht="15">
+    <row r="108" spans="1:182" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>32</v>
@@ -81934,15 +82073,15 @@
         <v>45821</v>
       </c>
     </row>
-    <row r="109" spans="1:179" ht="15">
+    <row r="109" spans="1:182" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>32</v>
@@ -81951,15 +82090,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:179" ht="15">
+    <row r="110" spans="1:182" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>18</v>
@@ -81979,16 +82118,25 @@
       <c r="FW110" s="3">
         <v>19</v>
       </c>
+      <c r="FX110" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY110" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:179" ht="15">
+    <row r="111" spans="1:182" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C111" s="17" t="s">
         <v>145</v>
-      </c>
-      <c r="C111" s="17" t="s">
-        <v>144</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>18</v>
@@ -82008,16 +82156,25 @@
       <c r="FW111" s="3">
         <v>19</v>
       </c>
+      <c r="FX111" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY111" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ111" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="112" spans="1:179" ht="15">
+    <row r="112" spans="1:182" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>32</v>
@@ -82037,16 +82194,25 @@
       <c r="FW112" s="3">
         <v>5</v>
       </c>
+      <c r="FX112" s="3">
+        <v>5</v>
+      </c>
+      <c r="FY112" s="3">
+        <v>5</v>
+      </c>
+      <c r="FZ112" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="113" spans="1:179" ht="15">
+    <row r="113" spans="1:182" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>18</v>
@@ -82066,16 +82232,25 @@
       <c r="FW113" s="3">
         <v>19</v>
       </c>
+      <c r="FX113" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY113" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ113" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="114" spans="1:179" ht="15">
+    <row r="114" spans="1:182" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>21</v>
@@ -82093,18 +82268,24 @@
         <v>16</v>
       </c>
       <c r="FW114" s="3">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="FX114" s="3">
+        <v>16</v>
+      </c>
+      <c r="FY114" s="3">
+        <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:179" ht="15">
+    <row r="115" spans="1:182" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>28</v>
@@ -82124,16 +82305,25 @@
       <c r="FW115" s="3">
         <v>19</v>
       </c>
+      <c r="FX115" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY115" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:179" ht="15">
+    <row r="116" spans="1:182" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>28</v>
@@ -82153,16 +82343,25 @@
       <c r="FW116" s="3">
         <v>19</v>
       </c>
+      <c r="FX116" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY116" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:179" ht="15">
+    <row r="117" spans="1:182" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>32</v>
@@ -82182,16 +82381,25 @@
       <c r="FW117" s="3">
         <v>5</v>
       </c>
+      <c r="FX117" s="3">
+        <v>5</v>
+      </c>
+      <c r="FY117" s="3">
+        <v>5</v>
+      </c>
+      <c r="FZ117" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:179" ht="15">
+    <row r="118" spans="1:182" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>32</v>
@@ -82214,16 +82422,25 @@
       <c r="FW118" s="3">
         <v>5</v>
       </c>
+      <c r="FX118" s="3">
+        <v>5</v>
+      </c>
+      <c r="FY118" s="3">
+        <v>5</v>
+      </c>
+      <c r="FZ118" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="119" spans="1:179" ht="15">
+    <row r="119" spans="1:182" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>32</v>
@@ -82246,16 +82463,25 @@
       <c r="FW119" s="3">
         <v>5</v>
       </c>
+      <c r="FX119" s="3">
+        <v>5</v>
+      </c>
+      <c r="FY119" s="3">
+        <v>5</v>
+      </c>
+      <c r="FZ119" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:179" ht="15">
+    <row r="120" spans="1:182" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C120" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>32</v>
@@ -82278,16 +82504,25 @@
       <c r="FW120" s="3">
         <v>5</v>
       </c>
+      <c r="FX120" s="3">
+        <v>5</v>
+      </c>
+      <c r="FY120" s="3">
+        <v>5</v>
+      </c>
+      <c r="FZ120" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="121" spans="1:179" ht="15">
+    <row r="121" spans="1:182" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C121" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>18</v>
@@ -82296,15 +82531,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="122" spans="1:179" ht="15">
+    <row r="122" spans="1:182" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C122" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>25</v>
@@ -82315,16 +82550,28 @@
       <c r="F122" s="13">
         <v>45820</v>
       </c>
+      <c r="FW122" s="3">
+        <v>12</v>
+      </c>
+      <c r="FX122" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY122" s="3">
+        <v>24</v>
+      </c>
+      <c r="FZ122" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="123" spans="1:179" ht="15">
+    <row r="123" spans="1:182" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C123" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>32</v>
@@ -82333,15 +82580,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:179" ht="15">
+    <row r="124" spans="1:182" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
       <c r="B124" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C124" s="17" t="s">
         <v>158</v>
-      </c>
-      <c r="C124" s="17" t="s">
-        <v>157</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>18</v>
@@ -82350,21 +82597,125 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:179" ht="15">
+    <row r="125" spans="1:182" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C125" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E125" s="9">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:182" ht="15">
+      <c r="A126" s="9">
+        <v>25176363</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C126" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D126" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E126" s="9">
+        <v>96</v>
+      </c>
+      <c r="F126" s="13">
+        <v>45822</v>
+      </c>
+      <c r="FY126" s="3">
+        <v>12</v>
+      </c>
+      <c r="FZ126" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:182" ht="15">
+      <c r="A127" s="9">
+        <v>25179725</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C127" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E127" s="9">
+        <v>96</v>
+      </c>
+      <c r="F127" s="13">
+        <v>45822</v>
+      </c>
+      <c r="FY127" s="3">
+        <v>12</v>
+      </c>
+      <c r="FZ127" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:182" ht="15">
+      <c r="A128" s="9">
+        <v>25173127</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C128" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D128" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E128" s="9">
+        <v>96</v>
+      </c>
+      <c r="F128" s="13">
+        <v>45822</v>
+      </c>
+      <c r="FY128" s="3">
+        <v>12</v>
+      </c>
+      <c r="FZ128" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:182" ht="15">
+      <c r="A129" s="9">
+        <v>25173179</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C129" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E129" s="9">
+        <v>96</v>
+      </c>
+      <c r="F129" s="13">
+        <v>45822</v>
+      </c>
+      <c r="FY129" s="3">
+        <v>12</v>
+      </c>
+      <c r="FZ129" s="3">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 16 09:41:15 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="919" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01F93DB7-3391-4375-918B-CDB535C17C28}"/>
+  <xr:revisionPtr revIDLastSave="921" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B251671-11E7-4347-B361-59BC2826514E}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1068,8 +1068,8 @@
   <dimension ref="A1:XFD129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FV87" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GA96" sqref="GA96"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FG89" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="FJ94" sqref="FJ94"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 16 13:49:06 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="921" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B251671-11E7-4347-B361-59BC2826514E}"/>
+  <xr:revisionPtr revIDLastSave="968" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82863DDC-1144-4292-9679-C15689406722}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="166">
   <si>
     <t>Module ID</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>IPQC Yellow Spot on Ribbon</t>
+  </si>
+  <si>
+    <t>PID-2</t>
   </si>
   <si>
     <t>VSL202526114</t>
@@ -1068,8 +1071,8 @@
   <dimension ref="A1:XFD129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FG89" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="FJ94" sqref="FJ94"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FW82" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GA85" sqref="GA85"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -72943,7 +72946,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:166" ht="15">
+    <row r="33" spans="1:183" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73092,7 +73095,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:166" ht="15">
+    <row r="34" spans="1:183" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73241,7 +73244,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:166" ht="15">
+    <row r="35" spans="1:183" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73390,7 +73393,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:166" ht="15">
+    <row r="36" spans="1:183" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73524,7 +73527,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:166" ht="15">
+    <row r="37" spans="1:183" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73658,7 +73661,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:166" ht="15">
+    <row r="38" spans="1:183" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73792,7 +73795,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:166" ht="15">
+    <row r="39" spans="1:183" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -73955,7 +73958,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:166" ht="15">
+    <row r="40" spans="1:183" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74118,7 +74121,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:166" ht="15">
+    <row r="41" spans="1:183" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74281,7 +74284,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:166" ht="15">
+    <row r="42" spans="1:183" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74444,7 +74447,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:166" ht="15">
+    <row r="43" spans="1:183" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74607,7 +74610,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:166" ht="15">
+    <row r="44" spans="1:183" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74770,7 +74773,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:166" ht="15">
+    <row r="45" spans="1:183" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -74933,7 +74936,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:166" ht="15">
+    <row r="46" spans="1:183" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75096,7 +75099,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:166" ht="15">
+    <row r="47" spans="1:183" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75112,7 +75115,9 @@
       <c r="E47" s="8">
         <v>1000</v>
       </c>
-      <c r="F47" s="12"/>
+      <c r="F47" s="12">
+        <v>45824</v>
+      </c>
       <c r="AY47" s="1"/>
       <c r="AZ47" s="1"/>
       <c r="BA47" s="1"/>
@@ -75229,8 +75234,11 @@
       <c r="FH47" s="1"/>
       <c r="FI47" s="1"/>
       <c r="FJ47" s="1"/>
+      <c r="GA47" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="48" spans="1:166" ht="15">
+    <row r="48" spans="1:183" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75441,7 +75449,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:177" ht="15">
+    <row r="49" spans="1:183" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75457,7 +75465,9 @@
       <c r="E49" s="8">
         <v>1000</v>
       </c>
-      <c r="F49" s="12"/>
+      <c r="F49" s="12">
+        <v>45824</v>
+      </c>
       <c r="AY49" s="1"/>
       <c r="AZ49" s="1"/>
       <c r="BA49" s="1"/>
@@ -75574,8 +75584,11 @@
       <c r="FH49" s="1"/>
       <c r="FI49" s="1"/>
       <c r="FJ49" s="1"/>
+      <c r="GA49" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="50" spans="1:177" ht="15">
+    <row r="50" spans="1:183" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75786,7 +75799,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:177" ht="15">
+    <row r="51" spans="1:183" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -75997,7 +76010,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:177" ht="15">
+    <row r="52" spans="1:183" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76208,7 +76221,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:177" ht="15">
+    <row r="53" spans="1:183" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76224,7 +76237,9 @@
       <c r="E53" s="8">
         <v>1000</v>
       </c>
-      <c r="F53" s="12"/>
+      <c r="F53" s="12">
+        <v>45824</v>
+      </c>
       <c r="AY53" s="1"/>
       <c r="AZ53" s="1"/>
       <c r="BA53" s="1"/>
@@ -76341,8 +76356,11 @@
       <c r="FH53" s="1"/>
       <c r="FI53" s="1"/>
       <c r="FJ53" s="1"/>
+      <c r="GA53" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="54" spans="1:177" ht="15">
+    <row r="54" spans="1:183" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76358,7 +76376,9 @@
       <c r="E54" s="8">
         <v>1000</v>
       </c>
-      <c r="F54" s="12"/>
+      <c r="F54" s="12">
+        <v>45824</v>
+      </c>
       <c r="AY54" s="1"/>
       <c r="AZ54" s="1"/>
       <c r="BA54" s="1"/>
@@ -76475,8 +76495,11 @@
       <c r="FH54" s="1"/>
       <c r="FI54" s="1"/>
       <c r="FJ54" s="1"/>
+      <c r="GA54" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="55" spans="1:177" ht="15">
+    <row r="55" spans="1:183" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76669,7 +76692,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:177" ht="15">
+    <row r="56" spans="1:183" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76862,7 +76885,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:177" ht="15">
+    <row r="57" spans="1:183" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77019,7 +77042,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:177" ht="15">
+    <row r="58" spans="1:183" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77175,7 +77198,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:177" ht="15">
+    <row r="59" spans="1:183" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77329,7 +77352,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:177" ht="15">
+    <row r="60" spans="1:183" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77475,7 +77498,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:177" ht="15">
+    <row r="61" spans="1:183" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77633,7 +77656,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:177" ht="15">
+    <row r="62" spans="1:183" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -77872,7 +77895,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:177" ht="15">
+    <row r="63" spans="1:183" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78111,7 +78134,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:177" ht="15">
+    <row r="64" spans="1:183" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78350,7 +78373,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:182" ht="15">
+    <row r="65" spans="1:183" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78499,7 +78522,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:182" ht="15">
+    <row r="66" spans="1:183" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78648,7 +78671,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:182" ht="15">
+    <row r="67" spans="1:183" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78787,7 +78810,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:182" ht="15">
+    <row r="68" spans="1:183" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -78934,7 +78957,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:182" ht="15">
+    <row r="69" spans="1:183" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79068,7 +79091,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:182" ht="15">
+    <row r="70" spans="1:183" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79231,7 +79254,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:182" ht="15">
+    <row r="71" spans="1:183" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79378,7 +79401,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:182" ht="15">
+    <row r="72" spans="1:183" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79512,7 +79535,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:182" ht="15">
+    <row r="73" spans="1:183" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79777,7 +79800,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:182" ht="15">
+    <row r="74" spans="1:183" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80042,7 +80065,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:182" ht="15">
+    <row r="75" spans="1:183" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80176,7 +80199,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:182" ht="15">
+    <row r="76" spans="1:183" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80310,7 +80333,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:182" ht="15">
+    <row r="77" spans="1:183" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80444,7 +80467,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:182" ht="15">
+    <row r="78" spans="1:183" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80657,8 +80680,11 @@
       <c r="FZ78" s="3">
         <v>24</v>
       </c>
+      <c r="GA78" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="79" spans="1:182" ht="15">
+    <row r="79" spans="1:183" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80792,7 +80818,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:182" ht="15">
+    <row r="80" spans="1:183" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -80981,7 +81007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:182" ht="15">
+    <row r="81" spans="1:183" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81022,7 +81048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:182" ht="15">
+    <row r="82" spans="1:183" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81095,8 +81121,11 @@
       <c r="FZ82" s="3">
         <v>24</v>
       </c>
+      <c r="GA82" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="83" spans="1:182" ht="15">
+    <row r="83" spans="1:183" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81137,7 +81166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:182" ht="15">
+    <row r="84" spans="1:183" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81165,8 +81194,11 @@
       <c r="FZ84" s="3">
         <v>5</v>
       </c>
+      <c r="GA84" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:182" ht="15">
+    <row r="85" spans="1:183" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81258,7 +81290,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:182" ht="15">
+    <row r="86" spans="1:183" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81278,7 +81310,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:182" ht="15">
+    <row r="87" spans="1:183" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81296,7 +81328,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:182" ht="15">
+    <row r="88" spans="1:183" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81314,7 +81346,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:182" ht="15">
+    <row r="89" spans="1:183" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81373,7 +81405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:182" ht="15">
+    <row r="90" spans="1:183" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81432,7 +81464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:182" ht="15">
+    <row r="91" spans="1:183" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81491,7 +81523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:182" ht="15">
+    <row r="92" spans="1:183" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81550,7 +81582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:182" ht="15">
+    <row r="93" spans="1:183" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81609,7 +81641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:182" ht="15">
+    <row r="94" spans="1:183" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -81665,7 +81697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:182" ht="15">
+    <row r="95" spans="1:183" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -81681,9 +81713,14 @@
       <c r="E95" s="15">
         <v>1000</v>
       </c>
-      <c r="F95" s="18"/>
+      <c r="F95" s="18">
+        <v>45824</v>
+      </c>
+      <c r="GA95" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="96" spans="1:182" ht="15">
+    <row r="96" spans="1:183" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -81714,8 +81751,11 @@
       <c r="FZ96" s="3">
         <v>24</v>
       </c>
+      <c r="GA96" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="97" spans="1:182" ht="15">
+    <row r="97" spans="1:183" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81746,8 +81786,11 @@
       <c r="FZ97" s="3">
         <v>24</v>
       </c>
+      <c r="GA97" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="98" spans="1:182" ht="15">
+    <row r="98" spans="1:183" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81778,8 +81821,11 @@
       <c r="FZ98" s="3">
         <v>24</v>
       </c>
+      <c r="GA98" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="99" spans="1:182" ht="15">
+    <row r="99" spans="1:183" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81799,7 +81845,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:182" ht="15">
+    <row r="100" spans="1:183" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -81809,23 +81855,28 @@
       <c r="C100" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D100" s="15" t="s">
-        <v>18</v>
+      <c r="D100" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="E100" s="15">
         <v>96</v>
       </c>
-      <c r="F100" s="18"/>
+      <c r="F100" s="18">
+        <v>45824</v>
+      </c>
+      <c r="GA100" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="101" spans="1:182" ht="15">
+    <row r="101" spans="1:183" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>18</v>
@@ -81852,15 +81903,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:182" ht="15">
+    <row r="102" spans="1:183" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
       <c r="B102" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C102" s="17" t="s">
         <v>135</v>
-      </c>
-      <c r="C102" s="17" t="s">
-        <v>134</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>18</v>
@@ -81887,15 +81938,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:182" ht="15">
+    <row r="103" spans="1:183" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>18</v>
@@ -81922,15 +81973,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:182" ht="15">
+    <row r="104" spans="1:183" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>18</v>
@@ -81957,15 +82008,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:182" ht="15">
+    <row r="105" spans="1:183" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>32</v>
@@ -81988,16 +82039,19 @@
       <c r="FZ105" s="3">
         <v>5</v>
       </c>
+      <c r="GA105" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="106" spans="1:182" ht="15">
+    <row r="106" spans="1:183" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
       <c r="B106" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C106" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="C106" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>18</v>
@@ -82020,16 +82074,19 @@
       <c r="FZ106" s="3">
         <v>24</v>
       </c>
+      <c r="GA106" s="3">
+        <v>19</v>
+      </c>
     </row>
-    <row r="107" spans="1:182" ht="15">
+    <row r="107" spans="1:183" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>28</v>
@@ -82052,16 +82109,19 @@
       <c r="FZ107" s="3">
         <v>24</v>
       </c>
+      <c r="GA107" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="108" spans="1:182" ht="15">
+    <row r="108" spans="1:183" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>32</v>
@@ -82073,15 +82133,15 @@
         <v>45821</v>
       </c>
     </row>
-    <row r="109" spans="1:182" ht="15">
+    <row r="109" spans="1:183" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>32</v>
@@ -82090,15 +82150,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:182" ht="15">
+    <row r="110" spans="1:183" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>18</v>
@@ -82127,16 +82187,19 @@
       <c r="FZ110" s="3">
         <v>24</v>
       </c>
+      <c r="GA110" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="111" spans="1:182" ht="15">
+    <row r="111" spans="1:183" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C111" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="C111" s="17" t="s">
-        <v>145</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>18</v>
@@ -82165,16 +82228,19 @@
       <c r="FZ111" s="3">
         <v>24</v>
       </c>
+      <c r="GA111" s="3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="112" spans="1:182" ht="15">
+    <row r="112" spans="1:183" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>32</v>
@@ -82203,16 +82269,19 @@
       <c r="FZ112" s="3">
         <v>5</v>
       </c>
+      <c r="GA112" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="113" spans="1:182" ht="15">
+    <row r="113" spans="1:183" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>18</v>
@@ -82241,16 +82310,19 @@
       <c r="FZ113" s="3">
         <v>24</v>
       </c>
+      <c r="GA113" s="3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="114" spans="1:182" ht="15">
+    <row r="114" spans="1:183" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>21</v>
@@ -82277,15 +82349,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:182" ht="15">
+    <row r="115" spans="1:183" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>28</v>
@@ -82314,16 +82386,19 @@
       <c r="FZ115" s="3">
         <v>24</v>
       </c>
+      <c r="GA115" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="116" spans="1:182" ht="15">
+    <row r="116" spans="1:183" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>28</v>
@@ -82352,16 +82427,19 @@
       <c r="FZ116" s="3">
         <v>24</v>
       </c>
+      <c r="GA116" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="117" spans="1:182" ht="15">
+    <row r="117" spans="1:183" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>32</v>
@@ -82390,16 +82468,19 @@
       <c r="FZ117" s="3">
         <v>5</v>
       </c>
+      <c r="GA117" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:182" ht="15">
+    <row r="118" spans="1:183" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>32</v>
@@ -82431,16 +82512,19 @@
       <c r="FZ118" s="3">
         <v>5</v>
       </c>
+      <c r="GA118" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="119" spans="1:182" ht="15">
+    <row r="119" spans="1:183" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>32</v>
@@ -82472,16 +82556,19 @@
       <c r="FZ119" s="3">
         <v>5</v>
       </c>
+      <c r="GA119" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:182" ht="15">
+    <row r="120" spans="1:183" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C120" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>32</v>
@@ -82513,8 +82600,11 @@
       <c r="FZ120" s="3">
         <v>5</v>
       </c>
+      <c r="GA120" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="121" spans="1:182" ht="15">
+    <row r="121" spans="1:183" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -82525,13 +82615,19 @@
         <v>117</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="E121" s="9">
         <v>96</v>
       </c>
+      <c r="F121" s="13">
+        <v>45824</v>
+      </c>
+      <c r="GA121" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="122" spans="1:182" ht="15">
+    <row r="122" spans="1:183" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -82563,15 +82659,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:182" ht="15">
+    <row r="123" spans="1:183" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C123" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>32</v>
@@ -82580,15 +82676,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:182" ht="15">
+    <row r="124" spans="1:183" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
       <c r="B124" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C124" s="17" t="s">
         <v>159</v>
-      </c>
-      <c r="C124" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>18</v>
@@ -82597,15 +82693,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:182" ht="15">
+    <row r="125" spans="1:183" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C125" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>28</v>
@@ -82614,15 +82710,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="126" spans="1:182" ht="15">
+    <row r="126" spans="1:183" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C126" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>18</v>
@@ -82639,16 +82735,19 @@
       <c r="FZ126" s="3">
         <v>24</v>
       </c>
+      <c r="GA126" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="127" spans="1:182" ht="15">
+    <row r="127" spans="1:183" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C127" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>18</v>
@@ -82665,16 +82764,19 @@
       <c r="FZ127" s="3">
         <v>24</v>
       </c>
+      <c r="GA127" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="128" spans="1:182" ht="15">
+    <row r="128" spans="1:183" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>18</v>
@@ -82691,16 +82793,19 @@
       <c r="FZ128" s="3">
         <v>24</v>
       </c>
+      <c r="GA128" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="129" spans="1:182" ht="15">
+    <row r="129" spans="1:183" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>18</v>
@@ -82716,6 +82821,9 @@
       </c>
       <c r="FZ129" s="3">
         <v>24</v>
+      </c>
+      <c r="GA129" s="3">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -82735,7 +82843,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D86:D100" xr:uid="{AE741107-2DDE-448F-B66D-3CC4D6043D49}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D86:D99" xr:uid="{AE741107-2DDE-448F-B66D-3CC4D6043D49}">
       <formula1>"LID,PID,TC,DH,HF,LETID,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 18 09:40:53 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="968" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82863DDC-1144-4292-9679-C15689406722}"/>
+  <xr:revisionPtr revIDLastSave="1009" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B29BA187-9933-4C48-9BCC-B1043799E447}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="167">
   <si>
     <t>Module ID</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>VSL202526119</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
   <si>
     <t>VSL202526120</t>
@@ -1068,11 +1071,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD129"/>
+  <dimension ref="A1:XFD130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FW82" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GA85" sqref="GA85"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FW116" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F130" sqref="F130"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -72946,7 +72949,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:183" ht="15">
+    <row r="33" spans="1:184" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73095,7 +73098,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:183" ht="15">
+    <row r="34" spans="1:184" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73244,7 +73247,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:183" ht="15">
+    <row r="35" spans="1:184" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73393,7 +73396,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:183" ht="15">
+    <row r="36" spans="1:184" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73527,7 +73530,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:183" ht="15">
+    <row r="37" spans="1:184" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73661,7 +73664,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:183" ht="15">
+    <row r="38" spans="1:184" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73795,7 +73798,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:183" ht="15">
+    <row r="39" spans="1:184" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -73958,7 +73961,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:183" ht="15">
+    <row r="40" spans="1:184" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74121,7 +74124,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:183" ht="15">
+    <row r="41" spans="1:184" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74284,7 +74287,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:183" ht="15">
+    <row r="42" spans="1:184" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74447,7 +74450,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:183" ht="15">
+    <row r="43" spans="1:184" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74610,7 +74613,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:183" ht="15">
+    <row r="44" spans="1:184" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74773,7 +74776,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:183" ht="15">
+    <row r="45" spans="1:184" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -74936,7 +74939,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:183" ht="15">
+    <row r="46" spans="1:184" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75099,7 +75102,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:183" ht="15">
+    <row r="47" spans="1:184" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75237,8 +75240,11 @@
       <c r="GA47" s="3">
         <v>7</v>
       </c>
+      <c r="GB47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:183" ht="15">
+    <row r="48" spans="1:184" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75449,7 +75455,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:183" ht="15">
+    <row r="49" spans="1:184" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75587,8 +75593,11 @@
       <c r="GA49" s="3">
         <v>7</v>
       </c>
+      <c r="GB49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:183" ht="15">
+    <row r="50" spans="1:184" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75799,7 +75808,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:183" ht="15">
+    <row r="51" spans="1:184" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76010,7 +76019,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:183" ht="15">
+    <row r="52" spans="1:184" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76221,7 +76230,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:183" ht="15">
+    <row r="53" spans="1:184" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76359,8 +76368,11 @@
       <c r="GA53" s="3">
         <v>7</v>
       </c>
+      <c r="GB53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:183" ht="15">
+    <row r="54" spans="1:184" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76498,8 +76510,11 @@
       <c r="GA54" s="3">
         <v>7</v>
       </c>
+      <c r="GB54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:183" ht="15">
+    <row r="55" spans="1:184" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76692,7 +76707,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:183" ht="15">
+    <row r="56" spans="1:184" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76885,7 +76900,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:183" ht="15">
+    <row r="57" spans="1:184" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77042,7 +77057,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:183" ht="15">
+    <row r="58" spans="1:184" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77198,7 +77213,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:183" ht="15">
+    <row r="59" spans="1:184" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77352,7 +77367,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:183" ht="15">
+    <row r="60" spans="1:184" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77498,7 +77513,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:183" ht="15">
+    <row r="61" spans="1:184" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77656,7 +77671,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:183" ht="15">
+    <row r="62" spans="1:184" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -77895,7 +77910,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:183" ht="15">
+    <row r="63" spans="1:184" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78134,7 +78149,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:183" ht="15">
+    <row r="64" spans="1:184" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78373,7 +78388,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:183" ht="15">
+    <row r="65" spans="1:184" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78522,7 +78537,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:183" ht="15">
+    <row r="66" spans="1:184" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78671,7 +78686,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:183" ht="15">
+    <row r="67" spans="1:184" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78810,7 +78825,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:183" ht="15">
+    <row r="68" spans="1:184" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -78957,7 +78972,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:183" ht="15">
+    <row r="69" spans="1:184" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79091,7 +79106,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:183" ht="15">
+    <row r="70" spans="1:184" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79254,7 +79269,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:183" ht="15">
+    <row r="71" spans="1:184" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79401,7 +79416,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:183" ht="15">
+    <row r="72" spans="1:184" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79535,7 +79550,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:183" ht="15">
+    <row r="73" spans="1:184" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79800,7 +79815,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:183" ht="15">
+    <row r="74" spans="1:184" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80065,7 +80080,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:183" ht="15">
+    <row r="75" spans="1:184" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80199,7 +80214,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:183" ht="15">
+    <row r="76" spans="1:184" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80333,7 +80348,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:183" ht="15">
+    <row r="77" spans="1:184" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80467,7 +80482,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:183" ht="15">
+    <row r="78" spans="1:184" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80683,8 +80698,11 @@
       <c r="GA78" s="3">
         <v>22</v>
       </c>
+      <c r="GB78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:183" ht="15">
+    <row r="79" spans="1:184" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80818,7 +80836,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:183" ht="15">
+    <row r="80" spans="1:184" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81007,7 +81025,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:183" ht="15">
+    <row r="81" spans="1:184" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81048,7 +81066,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:183" ht="15">
+    <row r="82" spans="1:184" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81124,8 +81142,11 @@
       <c r="GA82" s="3">
         <v>22</v>
       </c>
+      <c r="GB82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:183" ht="15">
+    <row r="83" spans="1:184" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81166,7 +81187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:183" ht="15">
+    <row r="84" spans="1:184" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81197,8 +81218,11 @@
       <c r="GA84" s="3">
         <v>5</v>
       </c>
+      <c r="GB84" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:183" ht="15">
+    <row r="85" spans="1:184" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81290,7 +81314,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:183" ht="15">
+    <row r="86" spans="1:184" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81310,7 +81334,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:183" ht="15">
+    <row r="87" spans="1:184" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81328,7 +81352,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:183" ht="15">
+    <row r="88" spans="1:184" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81346,7 +81370,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:183" ht="15">
+    <row r="89" spans="1:184" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81405,7 +81429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:183" ht="15">
+    <row r="90" spans="1:184" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81464,7 +81488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:183" ht="15">
+    <row r="91" spans="1:184" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81523,7 +81547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:183" ht="15">
+    <row r="92" spans="1:184" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81582,7 +81606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:183" ht="15">
+    <row r="93" spans="1:184" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81641,7 +81665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:183" ht="15">
+    <row r="94" spans="1:184" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -81697,7 +81721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:183" ht="15">
+    <row r="95" spans="1:184" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -81719,8 +81743,11 @@
       <c r="GA95" s="3">
         <v>7</v>
       </c>
+      <c r="GB95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:183" ht="15">
+    <row r="96" spans="1:184" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -81739,6 +81766,9 @@
       <c r="F96" s="18">
         <v>45820</v>
       </c>
+      <c r="P96" s="13">
+        <v>45824</v>
+      </c>
       <c r="FW96" s="3">
         <v>7</v>
       </c>
@@ -81755,7 +81785,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:183" ht="15">
+    <row r="97" spans="1:184" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81774,6 +81804,9 @@
       <c r="F97" s="18">
         <v>45820</v>
       </c>
+      <c r="P97" s="13">
+        <v>45824</v>
+      </c>
       <c r="FW97" s="3">
         <v>7</v>
       </c>
@@ -81790,7 +81823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:183" ht="15">
+    <row r="98" spans="1:184" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81824,8 +81857,11 @@
       <c r="GA98" s="3">
         <v>22</v>
       </c>
+      <c r="GB98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:183" ht="15">
+    <row r="99" spans="1:184" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81845,7 +81881,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:183" ht="15">
+    <row r="100" spans="1:184" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -81867,8 +81903,11 @@
       <c r="GA100" s="3">
         <v>7</v>
       </c>
+      <c r="GB100" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="101" spans="1:183" ht="15">
+    <row r="101" spans="1:184" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -81903,7 +81942,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:183" ht="15">
+    <row r="102" spans="1:184" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -81938,7 +81977,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:183" ht="15">
+    <row r="103" spans="1:184" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -81973,7 +82012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:183" ht="15">
+    <row r="104" spans="1:184" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82008,7 +82047,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:183" ht="15">
+    <row r="105" spans="1:184" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82042,8 +82081,11 @@
       <c r="GA105" s="3">
         <v>5</v>
       </c>
+      <c r="GB105" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="106" spans="1:183" ht="15">
+    <row r="106" spans="1:184" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82062,6 +82104,9 @@
       <c r="F106" s="13">
         <v>45820</v>
       </c>
+      <c r="P106" s="13">
+        <v>45824</v>
+      </c>
       <c r="FW106" s="3">
         <v>7</v>
       </c>
@@ -82077,13 +82122,16 @@
       <c r="GA106" s="3">
         <v>19</v>
       </c>
+      <c r="GB106" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="107" spans="1:183" ht="15">
+    <row r="107" spans="1:184" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C107" s="17" t="s">
         <v>140</v>
@@ -82112,13 +82160,16 @@
       <c r="GA107" s="3">
         <v>22</v>
       </c>
+      <c r="GB107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:183" ht="15">
+    <row r="108" spans="1:184" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C108" s="17" t="s">
         <v>140</v>
@@ -82133,12 +82184,12 @@
         <v>45821</v>
       </c>
     </row>
-    <row r="109" spans="1:183" ht="15">
+    <row r="109" spans="1:184" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C109" s="17" t="s">
         <v>140</v>
@@ -82150,15 +82201,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:183" ht="15">
+    <row r="110" spans="1:184" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>18</v>
@@ -82190,16 +82241,19 @@
       <c r="GA110" s="3">
         <v>22</v>
       </c>
+      <c r="GB110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:183" ht="15">
+    <row r="111" spans="1:184" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C111" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="C111" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>18</v>
@@ -82210,6 +82264,9 @@
       <c r="F111" s="13">
         <v>45818</v>
       </c>
+      <c r="P111" s="13">
+        <v>45824</v>
+      </c>
       <c r="FU111" s="3">
         <v>12</v>
       </c>
@@ -82231,16 +82288,19 @@
       <c r="GA111" s="3">
         <v>10</v>
       </c>
+      <c r="GB111" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="112" spans="1:183" ht="15">
+    <row r="112" spans="1:184" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>32</v>
@@ -82273,15 +82333,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:183" ht="15">
+    <row r="113" spans="1:184" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>18</v>
@@ -82292,6 +82352,9 @@
       <c r="F113" s="13">
         <v>45818</v>
       </c>
+      <c r="P113" s="13">
+        <v>45824</v>
+      </c>
       <c r="FU113" s="3">
         <v>12</v>
       </c>
@@ -82313,16 +82376,19 @@
       <c r="GA113" s="3">
         <v>10</v>
       </c>
+      <c r="GB113" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="114" spans="1:183" ht="15">
+    <row r="114" spans="1:184" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>21</v>
@@ -82349,15 +82415,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:183" ht="15">
+    <row r="115" spans="1:184" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>28</v>
@@ -82389,16 +82455,19 @@
       <c r="GA115" s="3">
         <v>22</v>
       </c>
+      <c r="GB115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:183" ht="15">
+    <row r="116" spans="1:184" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>28</v>
@@ -82430,16 +82499,19 @@
       <c r="GA116" s="3">
         <v>22</v>
       </c>
+      <c r="GB116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:183" ht="15">
+    <row r="117" spans="1:184" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>32</v>
@@ -82471,16 +82543,19 @@
       <c r="GA117" s="3">
         <v>5</v>
       </c>
+      <c r="GB117" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:183" ht="15">
+    <row r="118" spans="1:184" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>32</v>
@@ -82515,16 +82590,19 @@
       <c r="GA118" s="3">
         <v>5</v>
       </c>
+      <c r="GB118" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="119" spans="1:183" ht="15">
+    <row r="119" spans="1:184" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>32</v>
@@ -82559,16 +82637,19 @@
       <c r="GA119" s="3">
         <v>5</v>
       </c>
+      <c r="GB119" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:183" ht="15">
+    <row r="120" spans="1:184" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C120" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>32</v>
@@ -82603,8 +82684,11 @@
       <c r="GA120" s="3">
         <v>5</v>
       </c>
+      <c r="GB120" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="121" spans="1:183" ht="15">
+    <row r="121" spans="1:184" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -82626,8 +82710,11 @@
       <c r="GA121" s="3">
         <v>7</v>
       </c>
+      <c r="GB121" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="122" spans="1:183" ht="15">
+    <row r="122" spans="1:184" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -82658,16 +82745,22 @@
       <c r="FZ122" s="3">
         <v>24</v>
       </c>
+      <c r="GA122" s="3">
+        <v>24</v>
+      </c>
+      <c r="GB122" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="123" spans="1:183" ht="15">
+    <row r="123" spans="1:184" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C123" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>32</v>
@@ -82676,15 +82769,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:183" ht="15">
+    <row r="124" spans="1:184" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
       <c r="B124" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C124" s="17" t="s">
         <v>160</v>
-      </c>
-      <c r="C124" s="17" t="s">
-        <v>159</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>18</v>
@@ -82693,15 +82786,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:183" ht="15">
+    <row r="125" spans="1:184" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C125" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>28</v>
@@ -82710,15 +82803,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="126" spans="1:183" ht="15">
+    <row r="126" spans="1:184" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C126" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>18</v>
@@ -82738,16 +82831,19 @@
       <c r="GA126" s="3">
         <v>22</v>
       </c>
+      <c r="GB126" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="127" spans="1:183" ht="15">
+    <row r="127" spans="1:184" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C127" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>18</v>
@@ -82767,16 +82863,19 @@
       <c r="GA127" s="3">
         <v>22</v>
       </c>
+      <c r="GB127" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="128" spans="1:183" ht="15">
+    <row r="128" spans="1:184" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>18</v>
@@ -82796,16 +82895,19 @@
       <c r="GA128" s="3">
         <v>22</v>
       </c>
+      <c r="GB128" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="129" spans="1:183" ht="15">
+    <row r="129" spans="1:184" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>18</v>
@@ -82824,6 +82926,29 @@
       </c>
       <c r="GA129" s="3">
         <v>22</v>
+      </c>
+      <c r="GB129" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:184" ht="15">
+      <c r="A130" s="8">
+        <v>24859051</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D130" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E130" s="9">
+        <v>10</v>
+      </c>
+      <c r="F130" s="13">
+        <v>45826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 18 13:48:32 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1009" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B29BA187-9933-4C48-9BCC-B1043799E447}"/>
+  <xr:revisionPtr revIDLastSave="1044" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D773AEDF-78D1-4F3D-AEE6-CCBE0ED6EDD1}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="167">
   <si>
     <t>Module ID</t>
   </si>
@@ -437,6 +437,9 @@
     <t>IPQC Yellow Spot on Ribbon</t>
   </si>
   <si>
+    <t>END</t>
+  </si>
+  <si>
     <t>PID-2</t>
   </si>
   <si>
@@ -462,9 +465,6 @@
   </si>
   <si>
     <t>VSL202526119</t>
-  </si>
-  <si>
-    <t>END</t>
   </si>
   <si>
     <t>VSL202526120</t>
@@ -1074,8 +1074,8 @@
   <dimension ref="A1:XFD130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FW116" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F130" sqref="F130"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GA109" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GH110" sqref="GH110"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -72949,7 +72949,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:184" ht="15">
+    <row r="33" spans="1:185" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73098,7 +73098,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:184" ht="15">
+    <row r="34" spans="1:185" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73247,7 +73247,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:184" ht="15">
+    <row r="35" spans="1:185" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73396,7 +73396,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:184" ht="15">
+    <row r="36" spans="1:185" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73530,7 +73530,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:184" ht="15">
+    <row r="37" spans="1:185" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73664,7 +73664,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:184" ht="15">
+    <row r="38" spans="1:185" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73798,7 +73798,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:184" ht="15">
+    <row r="39" spans="1:185" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -73961,7 +73961,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:184" ht="15">
+    <row r="40" spans="1:185" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74124,7 +74124,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:184" ht="15">
+    <row r="41" spans="1:185" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74287,7 +74287,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:184" ht="15">
+    <row r="42" spans="1:185" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74450,7 +74450,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:184" ht="15">
+    <row r="43" spans="1:185" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74613,7 +74613,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:184" ht="15">
+    <row r="44" spans="1:185" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74776,7 +74776,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:184" ht="15">
+    <row r="45" spans="1:185" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -74939,7 +74939,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:184" ht="15">
+    <row r="46" spans="1:185" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75102,7 +75102,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:184" ht="15">
+    <row r="47" spans="1:185" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75243,8 +75243,11 @@
       <c r="GB47" s="3">
         <v>24</v>
       </c>
+      <c r="GC47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:184" ht="15">
+    <row r="48" spans="1:185" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75455,7 +75458,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:184" ht="15">
+    <row r="49" spans="1:185" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75596,8 +75599,11 @@
       <c r="GB49" s="3">
         <v>24</v>
       </c>
+      <c r="GC49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:184" ht="15">
+    <row r="50" spans="1:185" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75808,7 +75814,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:184" ht="15">
+    <row r="51" spans="1:185" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76019,7 +76025,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:184" ht="15">
+    <row r="52" spans="1:185" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76230,7 +76236,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:184" ht="15">
+    <row r="53" spans="1:185" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76371,8 +76377,11 @@
       <c r="GB53" s="3">
         <v>24</v>
       </c>
+      <c r="GC53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:184" ht="15">
+    <row r="54" spans="1:185" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76513,8 +76522,11 @@
       <c r="GB54" s="3">
         <v>24</v>
       </c>
+      <c r="GC54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:184" ht="15">
+    <row r="55" spans="1:185" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76707,7 +76719,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:184" ht="15">
+    <row r="56" spans="1:185" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76900,7 +76912,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:184" ht="15">
+    <row r="57" spans="1:185" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77057,7 +77069,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:184" ht="15">
+    <row r="58" spans="1:185" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77213,7 +77225,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:184" ht="15">
+    <row r="59" spans="1:185" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77367,7 +77379,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:184" ht="15">
+    <row r="60" spans="1:185" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77513,7 +77525,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:184" ht="15">
+    <row r="61" spans="1:185" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77671,7 +77683,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:184" ht="15">
+    <row r="62" spans="1:185" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -77910,7 +77922,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:184" ht="15">
+    <row r="63" spans="1:185" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78149,7 +78161,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:184" ht="15">
+    <row r="64" spans="1:185" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78388,7 +78400,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:184" ht="15">
+    <row r="65" spans="1:185" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78537,7 +78549,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:184" ht="15">
+    <row r="66" spans="1:185" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78686,7 +78698,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:184" ht="15">
+    <row r="67" spans="1:185" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78825,7 +78837,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:184" ht="15">
+    <row r="68" spans="1:185" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -78972,7 +78984,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:184" ht="15">
+    <row r="69" spans="1:185" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79106,7 +79118,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:184" ht="15">
+    <row r="70" spans="1:185" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79269,7 +79281,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:184" ht="15">
+    <row r="71" spans="1:185" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79416,7 +79428,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:184" ht="15">
+    <row r="72" spans="1:185" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79550,7 +79562,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:184" ht="15">
+    <row r="73" spans="1:185" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79815,7 +79827,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:184" ht="15">
+    <row r="74" spans="1:185" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80080,7 +80092,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:184" ht="15">
+    <row r="75" spans="1:185" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80214,7 +80226,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:184" ht="15">
+    <row r="76" spans="1:185" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80348,7 +80360,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:184" ht="15">
+    <row r="77" spans="1:185" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80482,7 +80494,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:184" ht="15">
+    <row r="78" spans="1:185" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80701,8 +80713,11 @@
       <c r="GB78" s="3">
         <v>24</v>
       </c>
+      <c r="GC78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:184" ht="15">
+    <row r="79" spans="1:185" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80836,7 +80851,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:184" ht="15">
+    <row r="80" spans="1:185" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81025,7 +81040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:184" ht="15">
+    <row r="81" spans="1:185" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81066,7 +81081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:184" ht="15">
+    <row r="82" spans="1:185" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81145,8 +81160,11 @@
       <c r="GB82" s="3">
         <v>24</v>
       </c>
+      <c r="GC82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:184" ht="15">
+    <row r="83" spans="1:185" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81187,7 +81205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:184" ht="15">
+    <row r="84" spans="1:185" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81221,8 +81239,11 @@
       <c r="GB84" s="3">
         <v>5</v>
       </c>
+      <c r="GC84" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:184" ht="15">
+    <row r="85" spans="1:185" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81314,7 +81335,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:184" ht="15">
+    <row r="86" spans="1:185" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81334,7 +81355,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:184" ht="15">
+    <row r="87" spans="1:185" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81352,7 +81373,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:184" ht="15">
+    <row r="88" spans="1:185" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81370,7 +81391,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:184" ht="15">
+    <row r="89" spans="1:185" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81429,7 +81450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:184" ht="15">
+    <row r="90" spans="1:185" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81488,7 +81509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:184" ht="15">
+    <row r="91" spans="1:185" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81547,7 +81568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:184" ht="15">
+    <row r="92" spans="1:185" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81606,7 +81627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:184" ht="15">
+    <row r="93" spans="1:185" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81665,7 +81686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:184" ht="15">
+    <row r="94" spans="1:185" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -81721,7 +81742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:184" ht="15">
+    <row r="95" spans="1:185" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -81746,8 +81767,11 @@
       <c r="GB95" s="3">
         <v>24</v>
       </c>
+      <c r="GC95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:184" ht="15">
+    <row r="96" spans="1:185" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -81784,8 +81808,11 @@
       <c r="GA96" s="3">
         <v>19</v>
       </c>
+      <c r="GB96" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="97" spans="1:184" ht="15">
+    <row r="97" spans="1:185" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81822,8 +81849,11 @@
       <c r="GA97" s="3">
         <v>19</v>
       </c>
+      <c r="GB97" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="98" spans="1:184" ht="15">
+    <row r="98" spans="1:185" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81860,8 +81890,11 @@
       <c r="GB98" s="3">
         <v>24</v>
       </c>
+      <c r="GC98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:184" ht="15">
+    <row r="99" spans="1:185" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81881,7 +81914,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:184" ht="15">
+    <row r="100" spans="1:185" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -81892,7 +81925,7 @@
         <v>113</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E100" s="15">
         <v>96</v>
@@ -81906,16 +81939,19 @@
       <c r="GB100" s="3">
         <v>24</v>
       </c>
+      <c r="GC100" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="101" spans="1:184" ht="15">
+    <row r="101" spans="1:185" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>18</v>
@@ -81942,15 +81978,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:184" ht="15">
+    <row r="102" spans="1:185" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
       <c r="B102" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C102" s="17" t="s">
         <v>136</v>
-      </c>
-      <c r="C102" s="17" t="s">
-        <v>135</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>18</v>
@@ -81977,15 +82013,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:184" ht="15">
+    <row r="103" spans="1:185" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>18</v>
@@ -82012,15 +82048,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:184" ht="15">
+    <row r="104" spans="1:185" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>18</v>
@@ -82047,15 +82083,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:184" ht="15">
+    <row r="105" spans="1:185" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>32</v>
@@ -82084,16 +82120,19 @@
       <c r="GB105" s="3">
         <v>5</v>
       </c>
+      <c r="GC105" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="106" spans="1:184" ht="15">
+    <row r="106" spans="1:185" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
       <c r="B106" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C106" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="C106" s="17" t="s">
-        <v>140</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>18</v>
@@ -82123,10 +82162,10 @@
         <v>19</v>
       </c>
       <c r="GB106" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="107" spans="1:184" ht="15">
+    <row r="107" spans="1:185" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82134,7 +82173,7 @@
         <v>143</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>28</v>
@@ -82163,8 +82202,11 @@
       <c r="GB107" s="3">
         <v>24</v>
       </c>
+      <c r="GC107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:184" ht="15">
+    <row r="108" spans="1:185" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82172,7 +82214,7 @@
         <v>144</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>32</v>
@@ -82184,7 +82226,7 @@
         <v>45821</v>
       </c>
     </row>
-    <row r="109" spans="1:184" ht="15">
+    <row r="109" spans="1:185" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82192,7 +82234,7 @@
         <v>145</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>32</v>
@@ -82201,7 +82243,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:184" ht="15">
+    <row r="110" spans="1:185" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -82244,8 +82286,11 @@
       <c r="GB110" s="3">
         <v>24</v>
       </c>
+      <c r="GC110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:184" ht="15">
+    <row r="111" spans="1:185" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -82289,10 +82334,10 @@
         <v>10</v>
       </c>
       <c r="GB111" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="112" spans="1:184" ht="15">
+    <row r="112" spans="1:185" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -82332,8 +82377,11 @@
       <c r="GA112" s="3">
         <v>5</v>
       </c>
+      <c r="GC112" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="113" spans="1:184" ht="15">
+    <row r="113" spans="1:185" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -82377,10 +82425,10 @@
         <v>10</v>
       </c>
       <c r="GB113" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="114" spans="1:184" ht="15">
+    <row r="114" spans="1:185" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -82415,7 +82463,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:184" ht="15">
+    <row r="115" spans="1:185" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -82458,8 +82506,11 @@
       <c r="GB115" s="3">
         <v>24</v>
       </c>
+      <c r="GC115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:184" ht="15">
+    <row r="116" spans="1:185" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -82502,8 +82553,11 @@
       <c r="GB116" s="3">
         <v>24</v>
       </c>
+      <c r="GC116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:184" ht="15">
+    <row r="117" spans="1:185" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -82546,8 +82600,11 @@
       <c r="GB117" s="3">
         <v>5</v>
       </c>
+      <c r="GC117" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:184" ht="15">
+    <row r="118" spans="1:185" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -82593,8 +82650,11 @@
       <c r="GB118" s="3">
         <v>5</v>
       </c>
+      <c r="GC118" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="119" spans="1:184" ht="15">
+    <row r="119" spans="1:185" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -82640,8 +82700,11 @@
       <c r="GB119" s="3">
         <v>5</v>
       </c>
+      <c r="GC119" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:184" ht="15">
+    <row r="120" spans="1:185" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -82687,8 +82750,11 @@
       <c r="GB120" s="3">
         <v>5</v>
       </c>
+      <c r="GC120" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="121" spans="1:184" ht="15">
+    <row r="121" spans="1:185" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -82699,7 +82765,7 @@
         <v>117</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E121" s="9">
         <v>96</v>
@@ -82713,8 +82779,11 @@
       <c r="GB121" s="3">
         <v>24</v>
       </c>
+      <c r="GC121" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="122" spans="1:184" ht="15">
+    <row r="122" spans="1:185" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -82751,8 +82820,11 @@
       <c r="GB122" s="3">
         <v>24</v>
       </c>
+      <c r="GC122" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="123" spans="1:184" ht="15">
+    <row r="123" spans="1:185" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -82769,7 +82841,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:184" ht="15">
+    <row r="124" spans="1:185" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -82786,7 +82858,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:184" ht="15">
+    <row r="125" spans="1:185" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -82803,7 +82875,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="126" spans="1:184" ht="15">
+    <row r="126" spans="1:185" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -82822,6 +82894,9 @@
       <c r="F126" s="13">
         <v>45822</v>
       </c>
+      <c r="P126" s="13">
+        <v>45826</v>
+      </c>
       <c r="FY126" s="3">
         <v>12</v>
       </c>
@@ -82834,8 +82909,11 @@
       <c r="GB126" s="3">
         <v>24</v>
       </c>
+      <c r="GC126" s="3">
+        <v>14</v>
+      </c>
     </row>
-    <row r="127" spans="1:184" ht="15">
+    <row r="127" spans="1:185" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -82854,6 +82932,9 @@
       <c r="F127" s="13">
         <v>45822</v>
       </c>
+      <c r="P127" s="13">
+        <v>45826</v>
+      </c>
       <c r="FY127" s="3">
         <v>12</v>
       </c>
@@ -82866,8 +82947,11 @@
       <c r="GB127" s="3">
         <v>24</v>
       </c>
+      <c r="GC127" s="3">
+        <v>14</v>
+      </c>
     </row>
-    <row r="128" spans="1:184" ht="15">
+    <row r="128" spans="1:185" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -82886,6 +82970,9 @@
       <c r="F128" s="13">
         <v>45822</v>
       </c>
+      <c r="P128" s="13">
+        <v>45826</v>
+      </c>
       <c r="FY128" s="3">
         <v>12</v>
       </c>
@@ -82898,8 +82985,11 @@
       <c r="GB128" s="3">
         <v>24</v>
       </c>
+      <c r="GC128" s="3">
+        <v>14</v>
+      </c>
     </row>
-    <row r="129" spans="1:184" ht="15">
+    <row r="129" spans="1:185" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -82918,6 +83008,9 @@
       <c r="F129" s="13">
         <v>45822</v>
       </c>
+      <c r="P129" s="13">
+        <v>45826</v>
+      </c>
       <c r="FY129" s="3">
         <v>12</v>
       </c>
@@ -82930,8 +83023,11 @@
       <c r="GB129" s="3">
         <v>24</v>
       </c>
+      <c r="GC129" s="3">
+        <v>14</v>
+      </c>
     </row>
-    <row r="130" spans="1:184" ht="15">
+    <row r="130" spans="1:185" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -82949,6 +83045,9 @@
       </c>
       <c r="F130" s="13">
         <v>45826</v>
+      </c>
+      <c r="GC130" s="3">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun 19 09:40:00 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1044" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D773AEDF-78D1-4F3D-AEE6-CCBE0ED6EDD1}"/>
+  <xr:revisionPtr revIDLastSave="1074" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678B9FFC-CDA9-4C16-A97B-A750A47839A5}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="178">
   <si>
     <t>Module ID</t>
   </si>
@@ -537,6 +537,39 @@
   </si>
   <si>
     <t>VSL202526106</t>
+  </si>
+  <si>
+    <t>VSL202526126</t>
+  </si>
+  <si>
+    <t>IPQC Lower Lam Cycle module</t>
+  </si>
+  <si>
+    <t>VSL202526127</t>
+  </si>
+  <si>
+    <t>VSL202526132</t>
+  </si>
+  <si>
+    <t>Cybrid Raybo UV Down Conversion Film Line Trial (1)</t>
+  </si>
+  <si>
+    <t>VSL202526128</t>
+  </si>
+  <si>
+    <t>Cybrid Raybo UV Down Conversion Film Line Trial (2)</t>
+  </si>
+  <si>
+    <t>VSL202526129</t>
+  </si>
+  <si>
+    <t>Sunbez EPE+EVA encapsulant trial</t>
+  </si>
+  <si>
+    <t>VSL202526130</t>
+  </si>
+  <si>
+    <t>VSL202526131</t>
   </si>
 </sst>
 </file>
@@ -1071,11 +1104,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD130"/>
+  <dimension ref="A1:XFD138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GA109" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GH110" sqref="GH110"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GA125" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C131" sqref="C131:C132"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -83050,6 +83083,141 @@
         <v>13</v>
       </c>
     </row>
+    <row r="131" spans="1:185" ht="15">
+      <c r="A131" s="9">
+        <v>72369597</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D131" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E131" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:185" ht="15">
+      <c r="A132" s="9">
+        <v>72369575</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D132" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E132" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:185" ht="15">
+      <c r="A133" s="9">
+        <v>25151639</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D133" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E133" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:185" s="3" customFormat="1" ht="15">
+      <c r="A134" s="9">
+        <v>25353591</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D134" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E134" s="9">
+        <v>1000</v>
+      </c>
+      <c r="F134" s="13"/>
+      <c r="P134" s="13"/>
+    </row>
+    <row r="135" spans="1:185" s="3" customFormat="1" ht="15">
+      <c r="A135" s="9">
+        <v>25353593</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D135" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E135" s="9">
+        <v>60</v>
+      </c>
+      <c r="F135" s="13"/>
+      <c r="P135" s="13"/>
+    </row>
+    <row r="136" spans="1:185" s="3" customFormat="1" ht="15">
+      <c r="A136" s="9">
+        <v>25353594</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D136" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E136" s="9">
+        <v>96</v>
+      </c>
+      <c r="F136" s="13"/>
+      <c r="P136" s="13"/>
+    </row>
+    <row r="137" spans="1:185" s="3" customFormat="1" ht="15">
+      <c r="A137" s="9">
+        <v>25353595</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D137" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E137" s="9">
+        <v>1000</v>
+      </c>
+      <c r="F137" s="13"/>
+      <c r="P137" s="13"/>
+    </row>
+    <row r="138" spans="1:185" s="3" customFormat="1" ht="15">
+      <c r="A138" s="9"/>
+      <c r="B138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="13"/>
+      <c r="P138" s="13"/>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun 19 13:46:09 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1074" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678B9FFC-CDA9-4C16-A97B-A750A47839A5}"/>
+  <xr:revisionPtr revIDLastSave="1106" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A708C0E-52B7-4AE9-903B-72CB129609E2}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="178">
   <si>
     <t>Module ID</t>
   </si>
@@ -440,9 +440,6 @@
     <t>END</t>
   </si>
   <si>
-    <t>PID-2</t>
-  </si>
-  <si>
     <t>VSL202526114</t>
   </si>
   <si>
@@ -513,6 +510,9 @@
   </si>
   <si>
     <t>VSL202526108</t>
+  </si>
+  <si>
+    <t>PT Bintan Cell Reliability Test (2 times)</t>
   </si>
   <si>
     <t>VSL202526123</t>
@@ -1107,8 +1107,8 @@
   <dimension ref="A1:XFD138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GA125" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C131" sqref="C131:C132"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GA117" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GE47" sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -72982,7 +72982,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:185" ht="15">
+    <row r="33" spans="1:186" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73131,7 +73131,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:185" ht="15">
+    <row r="34" spans="1:186" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73280,7 +73280,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:185" ht="15">
+    <row r="35" spans="1:186" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73429,7 +73429,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:185" ht="15">
+    <row r="36" spans="1:186" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73563,7 +73563,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:185" ht="15">
+    <row r="37" spans="1:186" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73697,7 +73697,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:185" ht="15">
+    <row r="38" spans="1:186" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73831,7 +73831,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:185" ht="15">
+    <row r="39" spans="1:186" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -73994,7 +73994,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:185" ht="15">
+    <row r="40" spans="1:186" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74157,7 +74157,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:185" ht="15">
+    <row r="41" spans="1:186" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74320,7 +74320,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:185" ht="15">
+    <row r="42" spans="1:186" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74483,7 +74483,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:185" ht="15">
+    <row r="43" spans="1:186" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74646,7 +74646,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:185" ht="15">
+    <row r="44" spans="1:186" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74809,7 +74809,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:185" ht="15">
+    <row r="45" spans="1:186" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -74972,7 +74972,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:185" ht="15">
+    <row r="46" spans="1:186" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75135,7 +75135,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:185" ht="15">
+    <row r="47" spans="1:186" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75279,8 +75279,11 @@
       <c r="GC47" s="3">
         <v>24</v>
       </c>
+      <c r="GD47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:185" ht="15">
+    <row r="48" spans="1:186" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75491,7 +75494,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:185" ht="15">
+    <row r="49" spans="1:186" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75635,8 +75638,11 @@
       <c r="GC49" s="3">
         <v>24</v>
       </c>
+      <c r="GD49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:185" ht="15">
+    <row r="50" spans="1:186" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75847,7 +75853,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:185" ht="15">
+    <row r="51" spans="1:186" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76058,7 +76064,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:185" ht="15">
+    <row r="52" spans="1:186" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76269,7 +76275,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:185" ht="15">
+    <row r="53" spans="1:186" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76413,8 +76419,11 @@
       <c r="GC53" s="3">
         <v>24</v>
       </c>
+      <c r="GD53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:185" ht="15">
+    <row r="54" spans="1:186" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76558,8 +76567,11 @@
       <c r="GC54" s="3">
         <v>24</v>
       </c>
+      <c r="GD54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:185" ht="15">
+    <row r="55" spans="1:186" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76752,7 +76764,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:185" ht="15">
+    <row r="56" spans="1:186" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76945,7 +76957,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:185" ht="15">
+    <row r="57" spans="1:186" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77102,7 +77114,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:185" ht="15">
+    <row r="58" spans="1:186" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77258,7 +77270,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:185" ht="15">
+    <row r="59" spans="1:186" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77412,7 +77424,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:185" ht="15">
+    <row r="60" spans="1:186" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77558,7 +77570,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:185" ht="15">
+    <row r="61" spans="1:186" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77716,7 +77728,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:185" ht="15">
+    <row r="62" spans="1:186" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -77955,7 +77967,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:185" ht="15">
+    <row r="63" spans="1:186" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78194,7 +78206,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:185" ht="15">
+    <row r="64" spans="1:186" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78433,7 +78445,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:185" ht="15">
+    <row r="65" spans="1:186" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78582,7 +78594,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:185" ht="15">
+    <row r="66" spans="1:186" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78731,7 +78743,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:185" ht="15">
+    <row r="67" spans="1:186" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78870,7 +78882,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:185" ht="15">
+    <row r="68" spans="1:186" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79017,7 +79029,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:185" ht="15">
+    <row r="69" spans="1:186" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79151,7 +79163,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:185" ht="15">
+    <row r="70" spans="1:186" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79314,7 +79326,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:185" ht="15">
+    <row r="71" spans="1:186" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79461,7 +79473,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:185" ht="15">
+    <row r="72" spans="1:186" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79595,7 +79607,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:185" ht="15">
+    <row r="73" spans="1:186" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79860,7 +79872,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:185" ht="15">
+    <row r="74" spans="1:186" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80125,7 +80137,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:185" ht="15">
+    <row r="75" spans="1:186" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80259,7 +80271,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:185" ht="15">
+    <row r="76" spans="1:186" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80393,7 +80405,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:185" ht="15">
+    <row r="77" spans="1:186" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80527,7 +80539,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:185" ht="15">
+    <row r="78" spans="1:186" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80749,8 +80761,11 @@
       <c r="GC78" s="3">
         <v>24</v>
       </c>
+      <c r="GD78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:185" ht="15">
+    <row r="79" spans="1:186" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80884,7 +80899,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:185" ht="15">
+    <row r="80" spans="1:186" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81073,7 +81088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:185" ht="15">
+    <row r="81" spans="1:186" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81114,7 +81129,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:185" ht="15">
+    <row r="82" spans="1:186" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81196,8 +81211,11 @@
       <c r="GC82" s="3">
         <v>24</v>
       </c>
+      <c r="GD82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:185" ht="15">
+    <row r="83" spans="1:186" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81238,7 +81256,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:185" ht="15">
+    <row r="84" spans="1:186" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81275,8 +81293,11 @@
       <c r="GC84" s="3">
         <v>5</v>
       </c>
+      <c r="GD84" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:185" ht="15">
+    <row r="85" spans="1:186" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81368,7 +81389,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:185" ht="15">
+    <row r="86" spans="1:186" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81388,7 +81409,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:185" ht="15">
+    <row r="87" spans="1:186" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81406,7 +81427,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:185" ht="15">
+    <row r="88" spans="1:186" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81424,7 +81445,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:185" ht="15">
+    <row r="89" spans="1:186" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81483,7 +81504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:185" ht="15">
+    <row r="90" spans="1:186" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81542,7 +81563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:185" ht="15">
+    <row r="91" spans="1:186" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81601,7 +81622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:185" ht="15">
+    <row r="92" spans="1:186" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81660,7 +81681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:185" ht="15">
+    <row r="93" spans="1:186" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81719,7 +81740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:185" ht="15">
+    <row r="94" spans="1:186" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -81775,7 +81796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:185" ht="15">
+    <row r="95" spans="1:186" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -81803,8 +81824,11 @@
       <c r="GC95" s="3">
         <v>24</v>
       </c>
+      <c r="GD95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:185" ht="15">
+    <row r="96" spans="1:186" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -81845,7 +81869,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:185" ht="15">
+    <row r="97" spans="1:186" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81886,7 +81910,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" spans="1:185" ht="15">
+    <row r="98" spans="1:186" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81926,8 +81950,11 @@
       <c r="GC98" s="3">
         <v>24</v>
       </c>
+      <c r="GD98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:185" ht="15">
+    <row r="99" spans="1:186" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81947,7 +81974,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:185" ht="15">
+    <row r="100" spans="1:186" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -81958,7 +81985,7 @@
         <v>113</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="E100" s="15">
         <v>96</v>
@@ -81975,16 +82002,19 @@
       <c r="GC100" s="3">
         <v>24</v>
       </c>
+      <c r="GD100" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="101" spans="1:185" ht="15">
+    <row r="101" spans="1:186" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
       <c r="B101" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C101" s="17" t="s">
         <v>135</v>
-      </c>
-      <c r="C101" s="17" t="s">
-        <v>136</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>18</v>
@@ -82011,15 +82041,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:185" ht="15">
+    <row r="102" spans="1:186" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>18</v>
@@ -82046,15 +82076,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:185" ht="15">
+    <row r="103" spans="1:186" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>18</v>
@@ -82081,15 +82111,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:185" ht="15">
+    <row r="104" spans="1:186" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>18</v>
@@ -82116,15 +82146,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:185" ht="15">
+    <row r="105" spans="1:186" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
       <c r="B105" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C105" s="17" t="s">
         <v>140</v>
-      </c>
-      <c r="C105" s="17" t="s">
-        <v>141</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>32</v>
@@ -82156,16 +82186,19 @@
       <c r="GC105" s="3">
         <v>5</v>
       </c>
+      <c r="GD105" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="106" spans="1:185" ht="15">
+    <row r="106" spans="1:186" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>18</v>
@@ -82198,15 +82231,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="107" spans="1:185" ht="15">
+    <row r="107" spans="1:186" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>28</v>
@@ -82238,16 +82271,19 @@
       <c r="GC107" s="3">
         <v>24</v>
       </c>
+      <c r="GD107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:185" ht="15">
+    <row r="108" spans="1:186" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>32</v>
@@ -82259,15 +82295,15 @@
         <v>45821</v>
       </c>
     </row>
-    <row r="109" spans="1:185" ht="15">
+    <row r="109" spans="1:186" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>32</v>
@@ -82276,15 +82312,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:185" ht="15">
+    <row r="110" spans="1:186" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
       <c r="B110" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C110" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="C110" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>18</v>
@@ -82322,16 +82358,19 @@
       <c r="GC110" s="3">
         <v>24</v>
       </c>
+      <c r="GD110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:185" ht="15">
+    <row r="111" spans="1:186" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>18</v>
@@ -82370,15 +82409,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="112" spans="1:185" ht="15">
+    <row r="112" spans="1:186" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>32</v>
@@ -82413,16 +82452,19 @@
       <c r="GC112" s="3">
         <v>5</v>
       </c>
+      <c r="GD112" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="113" spans="1:185" ht="15">
+    <row r="113" spans="1:186" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>18</v>
@@ -82461,15 +82503,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="114" spans="1:185" ht="15">
+    <row r="114" spans="1:186" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>21</v>
@@ -82496,15 +82538,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:185" ht="15">
+    <row r="115" spans="1:186" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>28</v>
@@ -82542,16 +82584,19 @@
       <c r="GC115" s="3">
         <v>24</v>
       </c>
+      <c r="GD115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:185" ht="15">
+    <row r="116" spans="1:186" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
       <c r="B116" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C116" s="17" t="s">
         <v>153</v>
-      </c>
-      <c r="C116" s="17" t="s">
-        <v>154</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>28</v>
@@ -82589,16 +82634,19 @@
       <c r="GC116" s="3">
         <v>24</v>
       </c>
+      <c r="GD116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:185" ht="15">
+    <row r="117" spans="1:186" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>32</v>
@@ -82636,16 +82684,19 @@
       <c r="GC117" s="3">
         <v>5</v>
       </c>
+      <c r="GD117" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:185" ht="15">
+    <row r="118" spans="1:186" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>32</v>
@@ -82686,16 +82737,19 @@
       <c r="GC118" s="3">
         <v>5</v>
       </c>
+      <c r="GD118" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="119" spans="1:185" ht="15">
+    <row r="119" spans="1:186" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>32</v>
@@ -82736,16 +82790,19 @@
       <c r="GC119" s="3">
         <v>5</v>
       </c>
+      <c r="GD119" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:185" ht="15">
+    <row r="120" spans="1:186" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C120" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>32</v>
@@ -82786,8 +82843,11 @@
       <c r="GC120" s="3">
         <v>5</v>
       </c>
+      <c r="GD120" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="121" spans="1:185" ht="15">
+    <row r="121" spans="1:186" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -82795,10 +82855,10 @@
         <v>116</v>
       </c>
       <c r="C121" s="17" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="E121" s="9">
         <v>96</v>
@@ -82815,8 +82875,11 @@
       <c r="GC121" s="3">
         <v>24</v>
       </c>
+      <c r="GD121" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="122" spans="1:185" ht="15">
+    <row r="122" spans="1:186" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -82856,8 +82919,11 @@
       <c r="GC122" s="3">
         <v>23</v>
       </c>
+      <c r="GD122" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="123" spans="1:185" ht="15">
+    <row r="123" spans="1:186" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -82874,7 +82940,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:185" ht="15">
+    <row r="124" spans="1:186" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -82891,7 +82957,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:185" ht="15">
+    <row r="125" spans="1:186" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -82908,7 +82974,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="126" spans="1:185" ht="15">
+    <row r="126" spans="1:186" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -82916,7 +82982,7 @@
         <v>163</v>
       </c>
       <c r="C126" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>18</v>
@@ -82945,8 +83011,11 @@
       <c r="GC126" s="3">
         <v>14</v>
       </c>
+      <c r="GD126" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="127" spans="1:185" ht="15">
+    <row r="127" spans="1:186" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -82954,7 +83023,7 @@
         <v>164</v>
       </c>
       <c r="C127" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>18</v>
@@ -82983,8 +83052,11 @@
       <c r="GC127" s="3">
         <v>14</v>
       </c>
+      <c r="GD127" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="128" spans="1:185" ht="15">
+    <row r="128" spans="1:186" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -82992,7 +83064,7 @@
         <v>165</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>18</v>
@@ -83021,8 +83093,11 @@
       <c r="GC128" s="3">
         <v>14</v>
       </c>
+      <c r="GD128" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="129" spans="1:185" ht="15">
+    <row r="129" spans="1:186" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -83030,7 +83105,7 @@
         <v>166</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>18</v>
@@ -83059,8 +83134,11 @@
       <c r="GC129" s="3">
         <v>14</v>
       </c>
+      <c r="GD129" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="130" spans="1:185" ht="15">
+    <row r="130" spans="1:186" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -83082,8 +83160,11 @@
       <c r="GC130" s="3">
         <v>13</v>
       </c>
+      <c r="GD130" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="131" spans="1:185" ht="15">
+    <row r="131" spans="1:186" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -83100,7 +83181,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="132" spans="1:185" ht="15">
+    <row r="132" spans="1:186" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -83117,7 +83198,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="133" spans="1:185" ht="15">
+    <row r="133" spans="1:186" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -83134,7 +83215,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:185" s="3" customFormat="1" ht="15">
+    <row r="134" spans="1:186" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -83150,10 +83231,8 @@
       <c r="E134" s="9">
         <v>1000</v>
       </c>
-      <c r="F134" s="13"/>
-      <c r="P134" s="13"/>
     </row>
-    <row r="135" spans="1:185" s="3" customFormat="1" ht="15">
+    <row r="135" spans="1:186" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -83169,10 +83248,8 @@
       <c r="E135" s="9">
         <v>60</v>
       </c>
-      <c r="F135" s="13"/>
-      <c r="P135" s="13"/>
     </row>
-    <row r="136" spans="1:185" s="3" customFormat="1" ht="15">
+    <row r="136" spans="1:186" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -83188,10 +83265,8 @@
       <c r="E136" s="9">
         <v>96</v>
       </c>
-      <c r="F136" s="13"/>
-      <c r="P136" s="13"/>
     </row>
-    <row r="137" spans="1:185" s="3" customFormat="1" ht="15">
+    <row r="137" spans="1:186" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -83207,17 +83282,8 @@
       <c r="E137" s="9">
         <v>1000</v>
       </c>
-      <c r="F137" s="13"/>
-      <c r="P137" s="13"/>
     </row>
-    <row r="138" spans="1:185" s="3" customFormat="1" ht="15">
-      <c r="A138" s="9"/>
-      <c r="B138" s="9"/>
-      <c r="D138" s="9"/>
-      <c r="E138" s="9"/>
-      <c r="F138" s="13"/>
-      <c r="P138" s="13"/>
-    </row>
+    <row r="138" spans="1:186" ht="15"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun 20 09:39:52 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1106" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A708C0E-52B7-4AE9-903B-72CB129609E2}"/>
+  <xr:revisionPtr revIDLastSave="1109" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F32B7F7-BBE4-4FD8-B5B4-51B9F2EB97BE}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1107,8 +1107,8 @@
   <dimension ref="A1:XFD138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GA117" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GE47" sqref="A1:XFD1048576"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GA112" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GE123" sqref="GE123"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -81869,7 +81869,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:186" ht="15">
+    <row r="97" spans="1:187" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81910,7 +81910,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" spans="1:186" ht="15">
+    <row r="98" spans="1:187" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81954,7 +81954,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:186" ht="15">
+    <row r="99" spans="1:187" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81974,7 +81974,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:186" ht="15">
+    <row r="100" spans="1:187" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82005,8 +82005,11 @@
       <c r="GD100" s="3">
         <v>24</v>
       </c>
+      <c r="GE100" s="3">
+        <v>17</v>
+      </c>
     </row>
-    <row r="101" spans="1:186" ht="15">
+    <row r="101" spans="1:187" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82041,7 +82044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:186" ht="15">
+    <row r="102" spans="1:187" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82076,7 +82079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:186" ht="15">
+    <row r="103" spans="1:187" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82111,7 +82114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:186" ht="15">
+    <row r="104" spans="1:187" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82146,7 +82149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:186" ht="15">
+    <row r="105" spans="1:187" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82190,7 +82193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:186" ht="15">
+    <row r="106" spans="1:187" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82231,7 +82234,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="107" spans="1:186" ht="15">
+    <row r="107" spans="1:187" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82275,7 +82278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:186" ht="15">
+    <row r="108" spans="1:187" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82295,7 +82298,7 @@
         <v>45821</v>
       </c>
     </row>
-    <row r="109" spans="1:186" ht="15">
+    <row r="109" spans="1:187" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82312,7 +82315,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:186" ht="15">
+    <row r="110" spans="1:187" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -82362,7 +82365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:186" ht="15">
+    <row r="111" spans="1:187" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -82409,7 +82412,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="112" spans="1:186" ht="15">
+    <row r="112" spans="1:187" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -82456,7 +82459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:186" ht="15">
+    <row r="113" spans="1:187" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -82503,7 +82506,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="114" spans="1:186" ht="15">
+    <row r="114" spans="1:187" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -82538,7 +82541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:186" ht="15">
+    <row r="115" spans="1:187" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -82588,7 +82591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="1:186" ht="15">
+    <row r="116" spans="1:187" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -82638,7 +82641,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:186" ht="15">
+    <row r="117" spans="1:187" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -82688,7 +82691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:186" ht="15">
+    <row r="118" spans="1:187" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -82741,7 +82744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:186" ht="15">
+    <row r="119" spans="1:187" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -82794,7 +82797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:186" ht="15">
+    <row r="120" spans="1:187" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -82847,7 +82850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:186" ht="15">
+    <row r="121" spans="1:187" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -82878,8 +82881,11 @@
       <c r="GD121" s="3">
         <v>24</v>
       </c>
+      <c r="GE121" s="3">
+        <v>17</v>
+      </c>
     </row>
-    <row r="122" spans="1:186" ht="15">
+    <row r="122" spans="1:187" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -82923,7 +82929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:186" ht="15">
+    <row r="123" spans="1:187" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -82940,7 +82946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:186" ht="15">
+    <row r="124" spans="1:187" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -82957,7 +82963,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:186" ht="15">
+    <row r="125" spans="1:187" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -82974,7 +82980,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="126" spans="1:186" ht="15">
+    <row r="126" spans="1:187" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -83015,7 +83021,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="127" spans="1:186" ht="15">
+    <row r="127" spans="1:187" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -83056,7 +83062,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:186" ht="15">
+    <row r="128" spans="1:187" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Fri Jun 20 11:35:48 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1109" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F32B7F7-BBE4-4FD8-B5B4-51B9F2EB97BE}"/>
+  <xr:revisionPtr revIDLastSave="1123" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9AF0CB0-2EF7-4185-B1B7-104F395C3D54}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1107,8 +1107,8 @@
   <dimension ref="A1:XFD138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GA112" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GE123" sqref="GE123"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GA84" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GA95" sqref="GA95:GD95"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -82028,6 +82028,9 @@
       <c r="F101" s="13">
         <v>45814</v>
       </c>
+      <c r="P101" s="13">
+        <v>45819</v>
+      </c>
       <c r="FQ101" s="3">
         <v>24</v>
       </c>
@@ -82042,6 +82045,9 @@
       </c>
       <c r="FU101" s="3">
         <v>16</v>
+      </c>
+      <c r="FV101" s="3">
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:187" ht="15">
@@ -82063,6 +82069,9 @@
       <c r="F102" s="13">
         <v>45814</v>
       </c>
+      <c r="P102" s="13">
+        <v>45819</v>
+      </c>
       <c r="FQ102" s="3">
         <v>24</v>
       </c>
@@ -82077,6 +82086,9 @@
       </c>
       <c r="FU102" s="3">
         <v>16</v>
+      </c>
+      <c r="FV102" s="3">
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:187" ht="15">
@@ -82098,6 +82110,9 @@
       <c r="F103" s="13">
         <v>45814</v>
       </c>
+      <c r="P103" s="13">
+        <v>45819</v>
+      </c>
       <c r="FQ103" s="3">
         <v>24</v>
       </c>
@@ -82111,7 +82126,10 @@
         <v>24</v>
       </c>
       <c r="FU103" s="3">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="FV103" s="3">
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:187" ht="15">
@@ -82133,6 +82151,9 @@
       <c r="F104" s="13">
         <v>45814</v>
       </c>
+      <c r="P104" s="13">
+        <v>45819</v>
+      </c>
       <c r="FQ104" s="3">
         <v>24</v>
       </c>
@@ -82147,6 +82168,9 @@
       </c>
       <c r="FU104" s="3">
         <v>16</v>
+      </c>
+      <c r="FV104" s="3">
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:187" ht="15">
@@ -82452,6 +82476,9 @@
       <c r="GA112" s="3">
         <v>5</v>
       </c>
+      <c r="GB112" s="3">
+        <v>5</v>
+      </c>
       <c r="GC112" s="3">
         <v>5</v>
       </c>
@@ -82660,6 +82687,9 @@
       <c r="F117" s="13">
         <v>45818</v>
       </c>
+      <c r="FT117" s="3">
+        <v>5</v>
+      </c>
       <c r="FU117" s="3">
         <v>5</v>
       </c>
@@ -82711,7 +82741,7 @@
         <v>45817</v>
       </c>
       <c r="FT118" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="FU118" s="3">
         <v>5</v>
@@ -82764,7 +82794,7 @@
         <v>45817</v>
       </c>
       <c r="FT119" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="FU119" s="3">
         <v>5</v>
@@ -82817,7 +82847,7 @@
         <v>45817</v>
       </c>
       <c r="FT120" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="FU120" s="3">
         <v>5</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 23 09:41:29 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1123" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9AF0CB0-2EF7-4185-B1B7-104F395C3D54}"/>
+  <xr:revisionPtr revIDLastSave="1220" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D94E3B3-4214-4CAA-88E9-80617145F967}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="179">
   <si>
     <t>Module ID</t>
   </si>
@@ -471,6 +471,9 @@
   </si>
   <si>
     <t>VSL202526122</t>
+  </si>
+  <si>
+    <t>controle</t>
   </si>
   <si>
     <t>VSL202526091</t>
@@ -1107,8 +1110,8 @@
   <dimension ref="A1:XFD138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GA84" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GA95" sqref="GA95:GD95"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GD52" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GG130" sqref="GG130"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -72982,7 +72985,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:186" ht="15">
+    <row r="33" spans="1:189" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73131,7 +73134,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:186" ht="15">
+    <row r="34" spans="1:189" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73280,7 +73283,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:186" ht="15">
+    <row r="35" spans="1:189" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73429,7 +73432,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:186" ht="15">
+    <row r="36" spans="1:189" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73563,7 +73566,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:186" ht="15">
+    <row r="37" spans="1:189" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73697,7 +73700,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:186" ht="15">
+    <row r="38" spans="1:189" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73831,7 +73834,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:186" ht="15">
+    <row r="39" spans="1:189" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -73994,7 +73997,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:186" ht="15">
+    <row r="40" spans="1:189" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74157,7 +74160,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:186" ht="15">
+    <row r="41" spans="1:189" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74320,7 +74323,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:186" ht="15">
+    <row r="42" spans="1:189" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74483,7 +74486,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:186" ht="15">
+    <row r="43" spans="1:189" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74646,7 +74649,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:186" ht="15">
+    <row r="44" spans="1:189" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74809,7 +74812,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:186" ht="15">
+    <row r="45" spans="1:189" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -74972,7 +74975,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:186" ht="15">
+    <row r="46" spans="1:189" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75135,7 +75138,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:186" ht="15">
+    <row r="47" spans="1:189" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75282,8 +75285,17 @@
       <c r="GD47" s="3">
         <v>24</v>
       </c>
+      <c r="GE47" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF47" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:186" ht="15">
+    <row r="48" spans="1:189" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75494,7 +75506,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:186" ht="15">
+    <row r="49" spans="1:189" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75641,8 +75653,17 @@
       <c r="GD49" s="3">
         <v>24</v>
       </c>
+      <c r="GE49" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF49" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:186" ht="15">
+    <row r="50" spans="1:189" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75853,7 +75874,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:186" ht="15">
+    <row r="51" spans="1:189" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76064,7 +76085,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:186" ht="15">
+    <row r="52" spans="1:189" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76275,7 +76296,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:186" ht="15">
+    <row r="53" spans="1:189" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76422,8 +76443,17 @@
       <c r="GD53" s="3">
         <v>24</v>
       </c>
+      <c r="GE53" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF53" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:186" ht="15">
+    <row r="54" spans="1:189" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76570,8 +76600,17 @@
       <c r="GD54" s="3">
         <v>24</v>
       </c>
+      <c r="GE54" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF54" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:186" ht="15">
+    <row r="55" spans="1:189" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76764,7 +76803,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:186" ht="15">
+    <row r="56" spans="1:189" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76957,7 +76996,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:186" ht="15">
+    <row r="57" spans="1:189" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77114,7 +77153,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:186" ht="15">
+    <row r="58" spans="1:189" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77270,7 +77309,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:186" ht="15">
+    <row r="59" spans="1:189" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77424,7 +77463,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:186" ht="15">
+    <row r="60" spans="1:189" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77570,7 +77609,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:186" ht="15">
+    <row r="61" spans="1:189" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77728,7 +77767,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:186" ht="15">
+    <row r="62" spans="1:189" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -77967,7 +78006,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:186" ht="15">
+    <row r="63" spans="1:189" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78206,7 +78245,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:186" ht="15">
+    <row r="64" spans="1:189" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78445,7 +78484,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:186" ht="15">
+    <row r="65" spans="1:189" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78594,7 +78633,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:186" ht="15">
+    <row r="66" spans="1:189" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78743,7 +78782,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:186" ht="15">
+    <row r="67" spans="1:189" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78882,7 +78921,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:186" ht="15">
+    <row r="68" spans="1:189" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79029,7 +79068,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:186" ht="15">
+    <row r="69" spans="1:189" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79163,7 +79202,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:186" ht="15">
+    <row r="70" spans="1:189" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79326,7 +79365,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:186" ht="15">
+    <row r="71" spans="1:189" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79473,7 +79512,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:186" ht="15">
+    <row r="72" spans="1:189" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79607,7 +79646,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:186" ht="15">
+    <row r="73" spans="1:189" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79872,7 +79911,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:186" ht="15">
+    <row r="74" spans="1:189" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80137,7 +80176,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:186" ht="15">
+    <row r="75" spans="1:189" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80271,7 +80310,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:186" ht="15">
+    <row r="76" spans="1:189" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80405,7 +80444,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:186" ht="15">
+    <row r="77" spans="1:189" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80539,7 +80578,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:186" ht="15">
+    <row r="78" spans="1:189" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80764,8 +80803,17 @@
       <c r="GD78" s="3">
         <v>24</v>
       </c>
+      <c r="GE78" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF78" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:186" ht="15">
+    <row r="79" spans="1:189" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80899,7 +80947,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:186" ht="15">
+    <row r="80" spans="1:189" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81088,7 +81136,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:186" ht="15">
+    <row r="81" spans="1:189" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81129,7 +81177,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:186" ht="15">
+    <row r="82" spans="1:189" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81214,8 +81262,17 @@
       <c r="GD82" s="3">
         <v>24</v>
       </c>
+      <c r="GE82" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF82" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:186" ht="15">
+    <row r="83" spans="1:189" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81256,7 +81313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:186" ht="15">
+    <row r="84" spans="1:189" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81296,8 +81353,17 @@
       <c r="GD84" s="3">
         <v>5</v>
       </c>
+      <c r="GE84" s="3">
+        <v>5</v>
+      </c>
+      <c r="GF84" s="3">
+        <v>5</v>
+      </c>
+      <c r="GG84" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:186" ht="15">
+    <row r="85" spans="1:189" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81389,7 +81455,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:186" ht="15">
+    <row r="86" spans="1:189" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81409,7 +81475,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:186" ht="15">
+    <row r="87" spans="1:189" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81427,7 +81493,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:186" ht="15">
+    <row r="88" spans="1:189" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81445,7 +81511,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:186" ht="15">
+    <row r="89" spans="1:189" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81504,7 +81570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:186" ht="15">
+    <row r="90" spans="1:189" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81563,7 +81629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:186" ht="15">
+    <row r="91" spans="1:189" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81622,7 +81688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:186" ht="15">
+    <row r="92" spans="1:189" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81681,7 +81747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:186" ht="15">
+    <row r="93" spans="1:189" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81740,7 +81806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:186" ht="15">
+    <row r="94" spans="1:189" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -81796,7 +81862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:186" ht="15">
+    <row r="95" spans="1:189" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -81827,8 +81893,17 @@
       <c r="GD95" s="3">
         <v>24</v>
       </c>
+      <c r="GE95" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF95" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:186" ht="15">
+    <row r="96" spans="1:189" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -81869,7 +81944,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:187" ht="15">
+    <row r="97" spans="1:189" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81910,7 +81985,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" spans="1:187" ht="15">
+    <row r="98" spans="1:189" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -81953,8 +82028,17 @@
       <c r="GD98" s="3">
         <v>24</v>
       </c>
+      <c r="GE98" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF98" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:187" ht="15">
+    <row r="99" spans="1:189" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -81974,7 +82058,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:187" ht="15">
+    <row r="100" spans="1:189" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82008,8 +82092,11 @@
       <c r="GE100" s="3">
         <v>17</v>
       </c>
+      <c r="GF100" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="101" spans="1:187" ht="15">
+    <row r="101" spans="1:189" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82050,7 +82137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:187" ht="15">
+    <row r="102" spans="1:189" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82091,7 +82178,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:187" ht="15">
+    <row r="103" spans="1:189" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82132,7 +82219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:187" ht="15">
+    <row r="104" spans="1:189" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82173,7 +82260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:187" ht="15">
+    <row r="105" spans="1:189" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82192,9 +82279,6 @@
       <c r="F105" s="13">
         <v>45821</v>
       </c>
-      <c r="FW105" s="3">
-        <v>5</v>
-      </c>
       <c r="FX105" s="3">
         <v>5</v>
       </c>
@@ -82216,8 +82300,17 @@
       <c r="GD105" s="3">
         <v>5</v>
       </c>
+      <c r="GE105" s="3">
+        <v>5</v>
+      </c>
+      <c r="GF105" s="3">
+        <v>5</v>
+      </c>
+      <c r="GG105" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="106" spans="1:187" ht="15">
+    <row r="106" spans="1:189" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82258,7 +82351,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="107" spans="1:187" ht="15">
+    <row r="107" spans="1:189" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82301,8 +82394,17 @@
       <c r="GD107" s="3">
         <v>24</v>
       </c>
+      <c r="GE107" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF107" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:187" ht="15">
+    <row r="108" spans="1:189" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82321,8 +82423,38 @@
       <c r="F108" s="13">
         <v>45821</v>
       </c>
+      <c r="FX108" s="3">
+        <v>5</v>
+      </c>
+      <c r="FY108" s="3">
+        <v>5</v>
+      </c>
+      <c r="FZ108" s="3">
+        <v>5</v>
+      </c>
+      <c r="GA108" s="3">
+        <v>5</v>
+      </c>
+      <c r="GB108" s="3">
+        <v>5</v>
+      </c>
+      <c r="GC108" s="3">
+        <v>5</v>
+      </c>
+      <c r="GD108" s="3">
+        <v>5</v>
+      </c>
+      <c r="GE108" s="3">
+        <v>5</v>
+      </c>
+      <c r="GF108" s="3">
+        <v>5</v>
+      </c>
+      <c r="GG108" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="109" spans="1:187" ht="15">
+    <row r="109" spans="1:189" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82338,16 +82470,19 @@
       <c r="E109" s="9">
         <v>60</v>
       </c>
+      <c r="F109" s="13" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="110" spans="1:187" ht="15">
+    <row r="110" spans="1:189" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>18</v>
@@ -82388,16 +82523,25 @@
       <c r="GD110" s="3">
         <v>24</v>
       </c>
+      <c r="GE110" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF110" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:187" ht="15">
+    <row r="111" spans="1:189" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C111" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="C111" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>18</v>
@@ -82436,15 +82580,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="112" spans="1:187" ht="15">
+    <row r="112" spans="1:189" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>32</v>
@@ -82485,16 +82629,25 @@
       <c r="GD112" s="3">
         <v>5</v>
       </c>
+      <c r="GE112" s="3">
+        <v>5</v>
+      </c>
+      <c r="GF112" s="3">
+        <v>5</v>
+      </c>
+      <c r="GG112" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="113" spans="1:187" ht="15">
+    <row r="113" spans="1:189" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>18</v>
@@ -82533,15 +82686,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="114" spans="1:187" ht="15">
+    <row r="114" spans="1:189" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>21</v>
@@ -82567,16 +82720,37 @@
       <c r="FY114" s="3">
         <v>16</v>
       </c>
+      <c r="FZ114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GA114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GB114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GC114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GD114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GE114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GF114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:187" ht="15">
+    <row r="115" spans="1:189" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>28</v>
@@ -82617,16 +82791,25 @@
       <c r="GD115" s="3">
         <v>24</v>
       </c>
+      <c r="GE115" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF115" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:187" ht="15">
+    <row r="116" spans="1:189" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>28</v>
@@ -82667,16 +82850,25 @@
       <c r="GD116" s="3">
         <v>24</v>
       </c>
+      <c r="GE116" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF116" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:187" ht="15">
+    <row r="117" spans="1:189" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>32</v>
@@ -82685,7 +82877,7 @@
         <v>60</v>
       </c>
       <c r="F117" s="13">
-        <v>45818</v>
+        <v>45817</v>
       </c>
       <c r="FT117" s="3">
         <v>5</v>
@@ -82720,16 +82912,25 @@
       <c r="GD117" s="3">
         <v>5</v>
       </c>
+      <c r="GE117" s="3">
+        <v>5</v>
+      </c>
+      <c r="GF117" s="3">
+        <v>5</v>
+      </c>
+      <c r="GG117" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="118" spans="1:187" ht="15">
+    <row r="118" spans="1:189" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>32</v>
@@ -82773,16 +82974,25 @@
       <c r="GD118" s="3">
         <v>5</v>
       </c>
+      <c r="GE118" s="3">
+        <v>5</v>
+      </c>
+      <c r="GF118" s="3">
+        <v>5</v>
+      </c>
+      <c r="GG118" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="119" spans="1:187" ht="15">
+    <row r="119" spans="1:189" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>32</v>
@@ -82826,16 +83036,25 @@
       <c r="GD119" s="3">
         <v>5</v>
       </c>
+      <c r="GE119" s="3">
+        <v>5</v>
+      </c>
+      <c r="GF119" s="3">
+        <v>5</v>
+      </c>
+      <c r="GG119" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="120" spans="1:187" ht="15">
+    <row r="120" spans="1:189" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C120" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>32</v>
@@ -82879,8 +83098,17 @@
       <c r="GD120" s="3">
         <v>5</v>
       </c>
+      <c r="GE120" s="3">
+        <v>5</v>
+      </c>
+      <c r="GF120" s="3">
+        <v>5</v>
+      </c>
+      <c r="GG120" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="121" spans="1:187" ht="15">
+    <row r="121" spans="1:189" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -82888,7 +83116,7 @@
         <v>116</v>
       </c>
       <c r="C121" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>18</v>
@@ -82914,8 +83142,11 @@
       <c r="GE121" s="3">
         <v>17</v>
       </c>
+      <c r="GF121" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="122" spans="1:187" ht="15">
+    <row r="122" spans="1:189" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -82958,16 +83189,25 @@
       <c r="GD122" s="3">
         <v>24</v>
       </c>
+      <c r="GE122" s="3">
+        <v>24</v>
+      </c>
+      <c r="GF122" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG122" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="123" spans="1:187" ht="15">
+    <row r="123" spans="1:189" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C123" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>32</v>
@@ -82975,16 +83215,19 @@
       <c r="E123" s="9">
         <v>60</v>
       </c>
+      <c r="F123" s="13">
+        <v>45830</v>
+      </c>
     </row>
-    <row r="124" spans="1:187" ht="15">
+    <row r="124" spans="1:189" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
       <c r="B124" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C124" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="C124" s="17" t="s">
-        <v>160</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>18</v>
@@ -82992,16 +83235,28 @@
       <c r="E124" s="9">
         <v>96</v>
       </c>
+      <c r="F124" s="13">
+        <v>45828</v>
+      </c>
+      <c r="GE124" s="3">
+        <v>6</v>
+      </c>
+      <c r="GF124" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG124" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="125" spans="1:187" ht="15">
+    <row r="125" spans="1:189" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C125" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>28</v>
@@ -83009,16 +83264,28 @@
       <c r="E125" s="9">
         <v>1000</v>
       </c>
+      <c r="F125" s="13">
+        <v>45828</v>
+      </c>
+      <c r="GE125" s="3">
+        <v>6</v>
+      </c>
+      <c r="GF125" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:187" ht="15">
+    <row r="126" spans="1:189" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C126" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>18</v>
@@ -83051,15 +83318,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="127" spans="1:187" ht="15">
+    <row r="127" spans="1:189" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C127" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>18</v>
@@ -83092,15 +83359,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:187" ht="15">
+    <row r="128" spans="1:189" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>18</v>
@@ -83133,15 +83400,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="1:186" ht="15">
+    <row r="129" spans="1:189" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>18</v>
@@ -83174,7 +83441,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:186" ht="15">
+    <row r="130" spans="1:189" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -83199,16 +83466,25 @@
       <c r="GD130" s="3">
         <v>24</v>
       </c>
+      <c r="GE130" s="3">
+        <v>24</v>
+      </c>
+      <c r="GF130" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG130" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="131" spans="1:186" ht="15">
+    <row r="131" spans="1:189" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D131" s="9" t="s">
         <v>28</v>
@@ -83217,15 +83493,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="132" spans="1:186" ht="15">
+    <row r="132" spans="1:189" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
       <c r="B132" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>28</v>
@@ -83234,15 +83510,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="133" spans="1:186" ht="15">
+    <row r="133" spans="1:189" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>28</v>
@@ -83251,15 +83527,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:186" ht="15">
+    <row r="134" spans="1:189" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D134" s="9" t="s">
         <v>28</v>
@@ -83268,15 +83544,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:186" ht="15">
+    <row r="135" spans="1:189" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D135" s="9" t="s">
         <v>32</v>
@@ -83285,15 +83561,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:186" ht="15">
+    <row r="136" spans="1:189" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
       <c r="B136" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C136" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="D136" s="9" t="s">
         <v>18</v>
@@ -83302,15 +83578,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:186" ht="15">
+    <row r="137" spans="1:189" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D137" s="9" t="s">
         <v>28</v>
@@ -83319,7 +83595,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:186" ht="15"/>
+    <row r="138" spans="1:189" ht="15"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 23 11:35:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1220" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D94E3B3-4214-4CAA-88E9-80617145F967}"/>
+  <xr:revisionPtr revIDLastSave="1224" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2B820E7-E97B-4819-B924-53DA3AEB74FC}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="179">
   <si>
     <t>Module ID</t>
   </si>
@@ -1110,8 +1110,8 @@
   <dimension ref="A1:XFD138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GD52" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GG130" sqref="GG130"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GA111" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="P122" sqref="P122"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -82639,7 +82639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:189" ht="15">
+    <row r="113" spans="1:190" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -82686,7 +82686,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="114" spans="1:189" ht="15">
+    <row r="114" spans="1:190" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -82741,8 +82741,11 @@
       <c r="GF114" s="3">
         <v>16</v>
       </c>
+      <c r="GG114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:189" ht="15">
+    <row r="115" spans="1:190" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -82801,7 +82804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="1:189" ht="15">
+    <row r="116" spans="1:190" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -82860,7 +82863,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:189" ht="15">
+    <row r="117" spans="1:190" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -82922,7 +82925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:189" ht="15">
+    <row r="118" spans="1:190" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -82984,7 +82987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:189" ht="15">
+    <row r="119" spans="1:190" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83046,7 +83049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:189" ht="15">
+    <row r="120" spans="1:190" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83108,7 +83111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:189" ht="15">
+    <row r="121" spans="1:190" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83146,7 +83149,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="122" spans="1:189" ht="15">
+    <row r="122" spans="1:190" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -83165,6 +83168,9 @@
       <c r="F122" s="13">
         <v>45820</v>
       </c>
+      <c r="P122" s="13">
+        <v>45830</v>
+      </c>
       <c r="FW122" s="3">
         <v>12</v>
       </c>
@@ -83198,8 +83204,11 @@
       <c r="GG122" s="3">
         <v>24</v>
       </c>
+      <c r="GH122" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="123" spans="1:189" ht="15">
+    <row r="123" spans="1:190" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -83218,8 +83227,11 @@
       <c r="F123" s="13">
         <v>45830</v>
       </c>
+      <c r="GG123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:189" ht="15">
+    <row r="124" spans="1:190" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -83248,7 +83260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:189" ht="15">
+    <row r="125" spans="1:190" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -83277,7 +83289,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:189" ht="15">
+    <row r="126" spans="1:190" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -83318,7 +83330,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="127" spans="1:189" ht="15">
+    <row r="127" spans="1:190" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -83359,7 +83371,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:189" ht="15">
+    <row r="128" spans="1:190" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon Jun 23 17:40:18 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1224" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2B820E7-E97B-4819-B924-53DA3AEB74FC}"/>
+  <xr:revisionPtr revIDLastSave="1255" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B18050AF-45CE-4320-B860-6257D8611782}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1110,8 +1110,8 @@
   <dimension ref="A1:XFD138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GA111" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="P122" sqref="P122"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GB113" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GG136" sqref="GG136"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -72985,7 +72985,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:189" ht="15">
+    <row r="33" spans="1:190" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73134,7 +73134,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:189" ht="15">
+    <row r="34" spans="1:190" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73283,7 +73283,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:189" ht="15">
+    <row r="35" spans="1:190" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73432,7 +73432,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:189" ht="15">
+    <row r="36" spans="1:190" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73566,7 +73566,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:189" ht="15">
+    <row r="37" spans="1:190" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73700,7 +73700,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:189" ht="15">
+    <row r="38" spans="1:190" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73834,7 +73834,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:189" ht="15">
+    <row r="39" spans="1:190" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -73997,7 +73997,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:189" ht="15">
+    <row r="40" spans="1:190" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74160,7 +74160,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:189" ht="15">
+    <row r="41" spans="1:190" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74323,7 +74323,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:189" ht="15">
+    <row r="42" spans="1:190" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74486,7 +74486,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:189" ht="15">
+    <row r="43" spans="1:190" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74649,7 +74649,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:189" ht="15">
+    <row r="44" spans="1:190" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74812,7 +74812,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:189" ht="15">
+    <row r="45" spans="1:190" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -74975,7 +74975,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:189" ht="15">
+    <row r="46" spans="1:190" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75138,7 +75138,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:189" ht="15">
+    <row r="47" spans="1:190" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75294,8 +75294,11 @@
       <c r="GG47" s="3">
         <v>24</v>
       </c>
+      <c r="GH47" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="48" spans="1:189" ht="15">
+    <row r="48" spans="1:190" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75506,7 +75509,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:189" ht="15">
+    <row r="49" spans="1:190" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75662,8 +75665,11 @@
       <c r="GG49" s="3">
         <v>24</v>
       </c>
+      <c r="GH49" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="50" spans="1:189" ht="15">
+    <row r="50" spans="1:190" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75874,7 +75880,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:189" ht="15">
+    <row r="51" spans="1:190" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76085,7 +76091,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:189" ht="15">
+    <row r="52" spans="1:190" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76296,7 +76302,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:189" ht="15">
+    <row r="53" spans="1:190" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76452,8 +76458,11 @@
       <c r="GG53" s="3">
         <v>24</v>
       </c>
+      <c r="GH53" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="54" spans="1:189" ht="15">
+    <row r="54" spans="1:190" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76609,8 +76618,11 @@
       <c r="GG54" s="3">
         <v>24</v>
       </c>
+      <c r="GH54" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="55" spans="1:189" ht="15">
+    <row r="55" spans="1:190" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76803,7 +76815,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:189" ht="15">
+    <row r="56" spans="1:190" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -76996,7 +77008,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:189" ht="15">
+    <row r="57" spans="1:190" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77153,7 +77165,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:189" ht="15">
+    <row r="58" spans="1:190" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77309,7 +77321,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:189" ht="15">
+    <row r="59" spans="1:190" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77463,7 +77475,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:189" ht="15">
+    <row r="60" spans="1:190" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77609,7 +77621,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:189" ht="15">
+    <row r="61" spans="1:190" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77767,7 +77779,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:189" ht="15">
+    <row r="62" spans="1:190" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78006,7 +78018,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:189" ht="15">
+    <row r="63" spans="1:190" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78245,7 +78257,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:189" ht="15">
+    <row r="64" spans="1:190" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78484,7 +78496,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:189" ht="15">
+    <row r="65" spans="1:190" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78633,7 +78645,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:189" ht="15">
+    <row r="66" spans="1:190" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78782,7 +78794,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:189" ht="15">
+    <row r="67" spans="1:190" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78921,7 +78933,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:189" ht="15">
+    <row r="68" spans="1:190" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79068,7 +79080,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:189" ht="15">
+    <row r="69" spans="1:190" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79202,7 +79214,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:189" ht="15">
+    <row r="70" spans="1:190" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79365,7 +79377,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:189" ht="15">
+    <row r="71" spans="1:190" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79512,7 +79524,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:189" ht="15">
+    <row r="72" spans="1:190" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79646,7 +79658,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:189" ht="15">
+    <row r="73" spans="1:190" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79911,7 +79923,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:189" ht="15">
+    <row r="74" spans="1:190" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80176,7 +80188,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:189" ht="15">
+    <row r="75" spans="1:190" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80310,7 +80322,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:189" ht="15">
+    <row r="76" spans="1:190" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80444,7 +80456,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:189" ht="15">
+    <row r="77" spans="1:190" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80578,7 +80590,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:189" ht="15">
+    <row r="78" spans="1:190" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80812,8 +80824,11 @@
       <c r="GG78" s="3">
         <v>24</v>
       </c>
+      <c r="GH78" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="79" spans="1:189" ht="15">
+    <row r="79" spans="1:190" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -80947,7 +80962,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:189" ht="15">
+    <row r="80" spans="1:190" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81136,7 +81151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:189" ht="15">
+    <row r="81" spans="1:190" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81177,7 +81192,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:189" ht="15">
+    <row r="82" spans="1:190" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81271,8 +81286,11 @@
       <c r="GG82" s="3">
         <v>24</v>
       </c>
+      <c r="GH82" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="83" spans="1:189" ht="15">
+    <row r="83" spans="1:190" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81313,7 +81331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:189" ht="15">
+    <row r="84" spans="1:190" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81362,8 +81380,11 @@
       <c r="GG84" s="3">
         <v>5</v>
       </c>
+      <c r="GH84" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="85" spans="1:189" ht="15">
+    <row r="85" spans="1:190" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81455,7 +81476,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:189" ht="15">
+    <row r="86" spans="1:190" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81475,7 +81496,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:189" ht="15">
+    <row r="87" spans="1:190" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81493,7 +81514,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:189" ht="15">
+    <row r="88" spans="1:190" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81511,7 +81532,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:189" ht="15">
+    <row r="89" spans="1:190" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81570,7 +81591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:189" ht="15">
+    <row r="90" spans="1:190" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81629,7 +81650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:189" ht="15">
+    <row r="91" spans="1:190" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81688,7 +81709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:189" ht="15">
+    <row r="92" spans="1:190" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81747,7 +81768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:189" ht="15">
+    <row r="93" spans="1:190" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81806,7 +81827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:189" ht="15">
+    <row r="94" spans="1:190" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -81862,7 +81883,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:189" ht="15">
+    <row r="95" spans="1:190" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -81902,8 +81923,11 @@
       <c r="GG95" s="3">
         <v>24</v>
       </c>
+      <c r="GH95" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="96" spans="1:189" ht="15">
+    <row r="96" spans="1:190" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -81944,7 +81968,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:189" ht="15">
+    <row r="97" spans="1:190" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -81985,7 +82009,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" spans="1:189" ht="15">
+    <row r="98" spans="1:190" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82037,8 +82061,11 @@
       <c r="GG98" s="3">
         <v>24</v>
       </c>
+      <c r="GH98" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="99" spans="1:189" ht="15">
+    <row r="99" spans="1:190" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82058,7 +82085,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:189" ht="15">
+    <row r="100" spans="1:190" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82096,7 +82123,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="101" spans="1:189" ht="15">
+    <row r="101" spans="1:190" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82137,7 +82164,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:189" ht="15">
+    <row r="102" spans="1:190" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82178,7 +82205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:189" ht="15">
+    <row r="103" spans="1:190" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82219,7 +82246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:189" ht="15">
+    <row r="104" spans="1:190" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82260,7 +82287,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:189" ht="15">
+    <row r="105" spans="1:190" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82309,8 +82336,11 @@
       <c r="GG105" s="3">
         <v>5</v>
       </c>
+      <c r="GH105" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="106" spans="1:189" ht="15">
+    <row r="106" spans="1:190" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82351,7 +82381,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="107" spans="1:189" ht="15">
+    <row r="107" spans="1:190" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82403,8 +82433,11 @@
       <c r="GG107" s="3">
         <v>24</v>
       </c>
+      <c r="GH107" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="108" spans="1:189" ht="15">
+    <row r="108" spans="1:190" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82453,8 +82486,11 @@
       <c r="GG108" s="3">
         <v>5</v>
       </c>
+      <c r="GH108" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="109" spans="1:189" ht="15">
+    <row r="109" spans="1:190" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82474,7 +82510,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:189" ht="15">
+    <row r="110" spans="1:190" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -82532,8 +82568,11 @@
       <c r="GG110" s="3">
         <v>24</v>
       </c>
+      <c r="GH110" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="111" spans="1:189" ht="15">
+    <row r="111" spans="1:190" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -82580,7 +82619,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="112" spans="1:189" ht="15">
+    <row r="112" spans="1:190" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -82636,6 +82675,9 @@
         <v>5</v>
       </c>
       <c r="GG112" s="3">
+        <v>5</v>
+      </c>
+      <c r="GH112" s="3">
         <v>5</v>
       </c>
     </row>
@@ -82744,6 +82786,9 @@
       <c r="GG114" s="3">
         <v>16</v>
       </c>
+      <c r="GH114" s="3">
+        <v>16</v>
+      </c>
     </row>
     <row r="115" spans="1:190" ht="15">
       <c r="A115" s="9">
@@ -82803,6 +82848,9 @@
       <c r="GG115" s="3">
         <v>24</v>
       </c>
+      <c r="GH115" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="116" spans="1:190" ht="15">
       <c r="A116" s="9">
@@ -82862,6 +82910,9 @@
       <c r="GG116" s="3">
         <v>24</v>
       </c>
+      <c r="GH116" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="117" spans="1:190" ht="15">
       <c r="A117" s="9">
@@ -82924,6 +82975,9 @@
       <c r="GG117" s="3">
         <v>5</v>
       </c>
+      <c r="GH117" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="118" spans="1:190" ht="15">
       <c r="A118" s="9">
@@ -82986,6 +83040,9 @@
       <c r="GG118" s="3">
         <v>5</v>
       </c>
+      <c r="GH118" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="119" spans="1:190" ht="15">
       <c r="A119" s="9">
@@ -83048,6 +83105,9 @@
       <c r="GG119" s="3">
         <v>5</v>
       </c>
+      <c r="GH119" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="120" spans="1:190" ht="15">
       <c r="A120" s="9">
@@ -83110,6 +83170,9 @@
       <c r="GG120" s="3">
         <v>5</v>
       </c>
+      <c r="GH120" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="121" spans="1:190" ht="15">
       <c r="A121" s="9">
@@ -83230,6 +83293,9 @@
       <c r="GG123" s="3">
         <v>5</v>
       </c>
+      <c r="GH123" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="124" spans="1:190" ht="15">
       <c r="A124" s="9">
@@ -83259,6 +83325,9 @@
       <c r="GG124" s="3">
         <v>24</v>
       </c>
+      <c r="GH124" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="125" spans="1:190" ht="15">
       <c r="A125" s="9">
@@ -83288,6 +83357,9 @@
       <c r="GG125" s="3">
         <v>24</v>
       </c>
+      <c r="GH125" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="126" spans="1:190" ht="15">
       <c r="A126" s="9">
@@ -83412,7 +83484,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="1:189" ht="15">
+    <row r="129" spans="1:190" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -83453,7 +83525,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:189" ht="15">
+    <row r="130" spans="1:190" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -83487,8 +83559,11 @@
       <c r="GG130" s="3">
         <v>24</v>
       </c>
+      <c r="GH130" s="3">
+        <v>18</v>
+      </c>
     </row>
-    <row r="131" spans="1:189" ht="15">
+    <row r="131" spans="1:190" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -83504,8 +83579,14 @@
       <c r="E131" s="9">
         <v>1000</v>
       </c>
+      <c r="F131" s="13">
+        <v>45831</v>
+      </c>
+      <c r="GH131" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="132" spans="1:189" ht="15">
+    <row r="132" spans="1:190" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -83521,8 +83602,14 @@
       <c r="E132" s="9">
         <v>1000</v>
       </c>
+      <c r="F132" s="13">
+        <v>45831</v>
+      </c>
+      <c r="GH132" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="133" spans="1:189" ht="15">
+    <row r="133" spans="1:190" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -83539,7 +83626,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:189" ht="15">
+    <row r="134" spans="1:190" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -83556,7 +83643,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:189" ht="15">
+    <row r="135" spans="1:190" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -83573,7 +83660,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:189" ht="15">
+    <row r="136" spans="1:190" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -83590,7 +83677,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:189" ht="15">
+    <row r="137" spans="1:190" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -83607,7 +83694,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:189" ht="15"/>
+    <row r="138" spans="1:190" ht="15"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue Jun 24 09:41:01 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29019"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1255" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B18050AF-45CE-4320-B860-6257D8611782}"/>
+  <xr:revisionPtr revIDLastSave="1295" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7869A843-6630-4F1C-827C-D05D2A500F48}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="200">
   <si>
     <t>Module ID</t>
   </si>
@@ -554,13 +554,13 @@
     <t>VSL202526132</t>
   </si>
   <si>
-    <t>Cybrid Raybo UV Down Conversion Film Line Trial (1)</t>
+    <t>Cybrid Raybo UV Down Conversion Film Line Trial (Aiko cell)</t>
   </si>
   <si>
     <t>VSL202526128</t>
   </si>
   <si>
-    <t>Cybrid Raybo UV Down Conversion Film Line Trial (2)</t>
+    <t>Cybrid Raybo UV Down Conversion Film Line Trial (Solarspace cell)</t>
   </si>
   <si>
     <t>VSL202526129</t>
@@ -573,6 +573,69 @@
   </si>
   <si>
     <t>VSL202526131</t>
+  </si>
+  <si>
+    <t>VSL202526149</t>
+  </si>
+  <si>
+    <t>VSL202526150</t>
+  </si>
+  <si>
+    <t>VSL202526151</t>
+  </si>
+  <si>
+    <t>VSL202526152</t>
+  </si>
+  <si>
+    <t>VSL202526133</t>
+  </si>
+  <si>
+    <t>Cleanmax HYPERSOL Internal Reliability Tests</t>
+  </si>
+  <si>
+    <t>VSL202526134</t>
+  </si>
+  <si>
+    <t>VSL202526135</t>
+  </si>
+  <si>
+    <t>VSL202526136</t>
+  </si>
+  <si>
+    <t>VSL202526137</t>
+  </si>
+  <si>
+    <t>VSL202526138</t>
+  </si>
+  <si>
+    <t>VSL202526139</t>
+  </si>
+  <si>
+    <t>VSL202526140</t>
+  </si>
+  <si>
+    <t>VSL202526141</t>
+  </si>
+  <si>
+    <t>VSL202526142</t>
+  </si>
+  <si>
+    <t>VSL202526143</t>
+  </si>
+  <si>
+    <t>VSL202526144</t>
+  </si>
+  <si>
+    <t>VSL202526145</t>
+  </si>
+  <si>
+    <t>VSL202526146</t>
+  </si>
+  <si>
+    <t>VSL202526147</t>
+  </si>
+  <si>
+    <t>VSL202526148</t>
   </si>
 </sst>
 </file>
@@ -1107,11 +1170,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD138"/>
+  <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GB113" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GG136" sqref="GG136"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GB143" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="D156" activeCellId="8" sqref="D136 D143 D146 D148 D150 D151 D154 D155 D156"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -83694,7 +83757,346 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:190" ht="15"/>
+    <row r="138" spans="1:190" ht="15">
+      <c r="A138" s="9">
+        <v>25357620</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D138" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E138" s="9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="139" spans="1:190" ht="15">
+      <c r="A139" s="9">
+        <v>25359186</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D139" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E139" s="9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="140" spans="1:190" ht="15">
+      <c r="A140" s="9">
+        <v>25357399</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D140" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E140" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:190" ht="15">
+      <c r="A141" s="9">
+        <v>25358777</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D141" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E141" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="142" spans="1:190" ht="15">
+      <c r="A142" s="9">
+        <v>25238843</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C142" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D142" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E142" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:190" ht="15">
+      <c r="A143" s="9">
+        <v>25239166</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C143" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D143" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E143" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="144" spans="1:190" ht="15">
+      <c r="A144" s="9">
+        <v>25248252</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C144" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D144" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E144" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15">
+      <c r="A145" s="9">
+        <v>25313260</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C145" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D145" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E145" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="15">
+      <c r="A146" s="9">
+        <v>25313310</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C146" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E146" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15">
+      <c r="A147" s="9">
+        <v>25270829</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C147" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D147" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E147" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="15">
+      <c r="A148" s="9">
+        <v>25310847</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C148" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D148" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E148" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="15">
+      <c r="A149" s="9">
+        <v>25249419</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C149" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D149" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E149" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="15">
+      <c r="A150" s="9">
+        <v>25249424</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C150" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D150" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E150" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="15">
+      <c r="A151" s="9">
+        <v>25249390</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C151" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E151" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="15">
+      <c r="A152" s="9">
+        <v>25338380</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C152" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E152" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="15">
+      <c r="A153" s="9">
+        <v>25336519</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C153" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D153" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E153" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="15">
+      <c r="A154" s="9">
+        <v>25338967</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C154" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D154" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E154" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="15">
+      <c r="A155" s="9">
+        <v>25338894</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C155" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D155" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E155" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="15">
+      <c r="A156" s="9">
+        <v>25344642</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C156" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D156" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E156" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="15">
+      <c r="A157" s="9">
+        <v>25344659</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C157" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E157" s="9">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 25 09:41:36 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1295" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7869A843-6630-4F1C-827C-D05D2A500F48}"/>
+  <xr:revisionPtr revIDLastSave="1307" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45D717D3-9801-45C8-9794-0003C4228A99}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,7 +473,7 @@
     <t>VSL202526122</t>
   </si>
   <si>
-    <t>controle</t>
+    <t>Reference</t>
   </si>
   <si>
     <t>VSL202526091</t>
@@ -1173,8 +1173,8 @@
   <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GB143" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D156" activeCellId="8" sqref="D136 D143 D146 D148 D150 D151 D154 D155 D156"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FZ118" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GF128" sqref="GF128"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -78559,7 +78559,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:190" ht="15">
+    <row r="65" spans="1:191" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78708,7 +78708,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:190" ht="15">
+    <row r="66" spans="1:191" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78857,7 +78857,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:190" ht="15">
+    <row r="67" spans="1:191" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78996,7 +78996,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:190" ht="15">
+    <row r="68" spans="1:191" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79143,7 +79143,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:190" ht="15">
+    <row r="69" spans="1:191" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79277,7 +79277,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:190" ht="15">
+    <row r="70" spans="1:191" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79440,7 +79440,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:190" ht="15">
+    <row r="71" spans="1:191" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79587,7 +79587,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:190" ht="15">
+    <row r="72" spans="1:191" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79721,7 +79721,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:190" ht="15">
+    <row r="73" spans="1:191" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79986,7 +79986,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:190" ht="15">
+    <row r="74" spans="1:191" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80251,7 +80251,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:190" ht="15">
+    <row r="75" spans="1:191" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80385,7 +80385,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:190" ht="15">
+    <row r="76" spans="1:191" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80519,7 +80519,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:190" ht="15">
+    <row r="77" spans="1:191" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80653,7 +80653,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:190" ht="15">
+    <row r="78" spans="1:191" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80890,8 +80890,11 @@
       <c r="GH78" s="3">
         <v>23</v>
       </c>
+      <c r="GI78" s="3">
+        <v>22</v>
+      </c>
     </row>
-    <row r="79" spans="1:190" ht="15">
+    <row r="79" spans="1:191" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81025,7 +81028,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:190" ht="15">
+    <row r="80" spans="1:191" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -82167,6 +82170,9 @@
       <c r="F100" s="18">
         <v>45824</v>
       </c>
+      <c r="P100" s="13">
+        <v>45828</v>
+      </c>
       <c r="GA100" s="3">
         <v>7</v>
       </c>
@@ -83256,6 +83262,9 @@
       <c r="F121" s="13">
         <v>45824</v>
       </c>
+      <c r="P121" s="13">
+        <v>45828</v>
+      </c>
       <c r="GA121" s="3">
         <v>7</v>
       </c>
@@ -83841,6 +83850,9 @@
       <c r="E142" s="9">
         <v>60</v>
       </c>
+      <c r="F142" s="13">
+        <v>45833</v>
+      </c>
     </row>
     <row r="143" spans="1:190" ht="15">
       <c r="A143" s="9">
@@ -83858,6 +83870,9 @@
       <c r="E143" s="9">
         <v>96</v>
       </c>
+      <c r="F143" s="13">
+        <v>45833</v>
+      </c>
     </row>
     <row r="144" spans="1:190" ht="15">
       <c r="A144" s="9">
@@ -83875,8 +83890,11 @@
       <c r="E144" s="9">
         <v>60</v>
       </c>
+      <c r="F144" s="13">
+        <v>45833</v>
+      </c>
     </row>
-    <row r="145" spans="1:5" ht="15">
+    <row r="145" spans="1:6" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -83892,8 +83910,11 @@
       <c r="E145" s="9">
         <v>60</v>
       </c>
+      <c r="F145" s="13">
+        <v>45833</v>
+      </c>
     </row>
-    <row r="146" spans="1:5" ht="15">
+    <row r="146" spans="1:6" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -83909,8 +83930,11 @@
       <c r="E146" s="9">
         <v>96</v>
       </c>
+      <c r="F146" s="13">
+        <v>45833</v>
+      </c>
     </row>
-    <row r="147" spans="1:5" ht="15">
+    <row r="147" spans="1:6" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -83926,8 +83950,11 @@
       <c r="E147" s="9">
         <v>60</v>
       </c>
+      <c r="F147" s="13">
+        <v>45833</v>
+      </c>
     </row>
-    <row r="148" spans="1:5" ht="15">
+    <row r="148" spans="1:6" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -83943,8 +83970,11 @@
       <c r="E148" s="9">
         <v>96</v>
       </c>
+      <c r="F148" s="13">
+        <v>45833</v>
+      </c>
     </row>
-    <row r="149" spans="1:5" ht="15">
+    <row r="149" spans="1:6" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -83961,7 +83991,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="15">
+    <row r="150" spans="1:6" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -83977,8 +84007,11 @@
       <c r="E150" s="9">
         <v>96</v>
       </c>
+      <c r="F150" s="13">
+        <v>45833</v>
+      </c>
     </row>
-    <row r="151" spans="1:5" ht="15">
+    <row r="151" spans="1:6" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -83995,7 +84028,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="15">
+    <row r="152" spans="1:6" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -84012,7 +84045,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="15">
+    <row r="153" spans="1:6" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -84029,7 +84062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="15">
+    <row r="154" spans="1:6" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -84046,7 +84079,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="15">
+    <row r="155" spans="1:6" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -84063,7 +84096,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="15">
+    <row r="156" spans="1:6" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -84080,7 +84113,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="15">
+    <row r="157" spans="1:6" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 25 15:41:39 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1307" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45D717D3-9801-45C8-9794-0003C4228A99}"/>
+  <xr:revisionPtr revIDLastSave="1327" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CE5C124-3324-416A-B9D0-C872BF340B7D}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="200">
   <si>
     <t>Module ID</t>
   </si>
@@ -395,6 +395,9 @@
     <t>VSL202526009</t>
   </si>
   <si>
+    <t>END</t>
+  </si>
+  <si>
     <t>VSL202425378</t>
   </si>
   <si>
@@ -435,9 +438,6 @@
   </si>
   <si>
     <t>IPQC Yellow Spot on Ribbon</t>
-  </si>
-  <si>
-    <t>END</t>
   </si>
   <si>
     <t>VSL202526114</t>
@@ -1173,8 +1173,8 @@
   <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FZ118" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GF128" sqref="GF128"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GD101" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GJ112" sqref="GJ112"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -80891,7 +80891,7 @@
         <v>23</v>
       </c>
       <c r="GI78" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:191" ht="15">
@@ -81217,7 +81217,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:190" ht="15">
+    <row r="81" spans="1:192" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81258,7 +81258,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:190" ht="15">
+    <row r="82" spans="1:192" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81355,8 +81355,11 @@
       <c r="GH82" s="3">
         <v>23</v>
       </c>
+      <c r="GI82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:190" ht="15">
+    <row r="83" spans="1:192" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81397,7 +81400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:190" ht="15">
+    <row r="84" spans="1:192" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81416,6 +81419,9 @@
       <c r="F84" s="13">
         <v>45821</v>
       </c>
+      <c r="P84" s="13">
+        <v>45832</v>
+      </c>
       <c r="FX84" s="3">
         <v>5</v>
       </c>
@@ -81449,13 +81455,19 @@
       <c r="GH84" s="3">
         <v>5</v>
       </c>
+      <c r="GI84" s="3">
+        <v>5</v>
+      </c>
+      <c r="GJ84" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="85" spans="1:190" ht="15">
+    <row r="85" spans="1:192" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>101</v>
@@ -81542,15 +81554,15 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:190" ht="15">
+    <row r="86" spans="1:192" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>18</v>
@@ -81562,7 +81574,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:190" ht="15">
+    <row r="87" spans="1:192" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81580,7 +81592,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:190" ht="15">
+    <row r="88" spans="1:192" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81598,15 +81610,15 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:190" ht="15">
+    <row r="89" spans="1:192" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>32</v>
@@ -81657,15 +81669,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:190" ht="15">
+    <row r="90" spans="1:192" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>32</v>
@@ -81716,15 +81728,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:190" ht="15">
+    <row r="91" spans="1:192" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
       <c r="B91" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C91" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>125</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>32</v>
@@ -81775,15 +81787,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:190" ht="15">
+    <row r="92" spans="1:192" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>32</v>
@@ -81834,12 +81846,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:190" ht="15">
+    <row r="93" spans="1:192" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C93" s="17" t="s">
         <v>115</v>
@@ -81893,15 +81905,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:190" ht="15">
+    <row r="94" spans="1:192" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>21</v>
@@ -81949,15 +81961,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:190" ht="15">
+    <row r="95" spans="1:192" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>28</v>
@@ -81992,16 +82004,19 @@
       <c r="GH95" s="3">
         <v>23</v>
       </c>
+      <c r="GI95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:190" ht="15">
+    <row r="96" spans="1:192" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>18</v>
@@ -82031,18 +82046,18 @@
         <v>19</v>
       </c>
       <c r="GB96" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="97" spans="1:190" ht="15">
+    <row r="97" spans="1:192" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>18</v>
@@ -82072,18 +82087,18 @@
         <v>19</v>
       </c>
       <c r="GB97" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="98" spans="1:190" ht="15">
+    <row r="98" spans="1:192" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
       <c r="B98" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C98" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>125</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>28</v>
@@ -82130,16 +82145,19 @@
       <c r="GH98" s="3">
         <v>23</v>
       </c>
+      <c r="GI98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:190" ht="15">
+    <row r="99" spans="1:192" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>28</v>
@@ -82151,7 +82169,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:190" ht="15">
+    <row r="100" spans="1:192" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82189,10 +82207,10 @@
         <v>17</v>
       </c>
       <c r="GF100" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="101" spans="1:190" ht="15">
+    <row r="101" spans="1:192" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82233,7 +82251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:190" ht="15">
+    <row r="102" spans="1:192" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82274,7 +82292,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:190" ht="15">
+    <row r="103" spans="1:192" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82315,7 +82333,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:190" ht="15">
+    <row r="104" spans="1:192" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82356,7 +82374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:190" ht="15">
+    <row r="105" spans="1:192" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82408,8 +82426,14 @@
       <c r="GH105" s="3">
         <v>5</v>
       </c>
+      <c r="GI105" s="3">
+        <v>5</v>
+      </c>
+      <c r="GJ105" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="106" spans="1:190" ht="15">
+    <row r="106" spans="1:192" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82447,10 +82471,10 @@
         <v>19</v>
       </c>
       <c r="GB106" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="107" spans="1:190" ht="15">
+    <row r="107" spans="1:192" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82505,8 +82529,11 @@
       <c r="GH107" s="3">
         <v>23</v>
       </c>
+      <c r="GI107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:190" ht="15">
+    <row r="108" spans="1:192" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82525,6 +82552,9 @@
       <c r="F108" s="13">
         <v>45821</v>
       </c>
+      <c r="P108" s="13">
+        <v>45832</v>
+      </c>
       <c r="FX108" s="3">
         <v>5</v>
       </c>
@@ -82558,8 +82588,14 @@
       <c r="GH108" s="3">
         <v>5</v>
       </c>
+      <c r="GI108" s="3">
+        <v>5</v>
+      </c>
+      <c r="GJ108" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="109" spans="1:190" ht="15">
+    <row r="109" spans="1:192" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82579,7 +82615,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:190" ht="15">
+    <row r="110" spans="1:192" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -82641,7 +82677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:190" ht="15">
+    <row r="111" spans="1:192" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -82685,10 +82721,10 @@
         <v>10</v>
       </c>
       <c r="GB111" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="112" spans="1:190" ht="15">
+    <row r="112" spans="1:192" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -82794,7 +82830,7 @@
         <v>10</v>
       </c>
       <c r="GB113" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:190" ht="15">
@@ -83281,7 +83317,7 @@
         <v>17</v>
       </c>
       <c r="GF121" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:190" ht="15">
@@ -83289,10 +83325,10 @@
         <v>72149637</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C122" s="17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>25</v>
@@ -83340,7 +83376,7 @@
         <v>24</v>
       </c>
       <c r="GH122" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:190" ht="15">
@@ -83471,7 +83507,7 @@
         <v>14</v>
       </c>
       <c r="GD126" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="1:190" ht="15">
@@ -83512,7 +83548,7 @@
         <v>14</v>
       </c>
       <c r="GD127" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="128" spans="1:190" ht="15">
@@ -83553,10 +83589,10 @@
         <v>14</v>
       </c>
       <c r="GD128" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:190" ht="15">
+    <row r="129" spans="1:192" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -83594,10 +83630,10 @@
         <v>14</v>
       </c>
       <c r="GD129" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
-    <row r="130" spans="1:190" ht="15">
+    <row r="130" spans="1:192" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -83634,8 +83670,14 @@
       <c r="GH130" s="3">
         <v>18</v>
       </c>
+      <c r="GI130" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ130" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="131" spans="1:190" ht="15">
+    <row r="131" spans="1:192" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -83657,8 +83699,14 @@
       <c r="GH131" s="3">
         <v>5</v>
       </c>
+      <c r="GI131" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:190" ht="15">
+    <row r="132" spans="1:192" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -83680,8 +83728,14 @@
       <c r="GH132" s="3">
         <v>5</v>
       </c>
+      <c r="GI132" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:190" ht="15">
+    <row r="133" spans="1:192" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -83698,7 +83752,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:190" ht="15">
+    <row r="134" spans="1:192" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -83715,7 +83769,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:190" ht="15">
+    <row r="135" spans="1:192" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -83732,7 +83786,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:190" ht="15">
+    <row r="136" spans="1:192" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -83749,7 +83803,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:190" ht="15">
+    <row r="137" spans="1:192" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -83766,7 +83820,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:190" ht="15">
+    <row r="138" spans="1:192" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -83783,7 +83837,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="139" spans="1:190" ht="15">
+    <row r="139" spans="1:192" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -83800,7 +83854,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="140" spans="1:190" ht="15">
+    <row r="140" spans="1:192" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -83817,7 +83871,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="141" spans="1:190" ht="15">
+    <row r="141" spans="1:192" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -83834,7 +83888,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="142" spans="1:190" ht="15">
+    <row r="142" spans="1:192" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -83854,7 +83908,7 @@
         <v>45833</v>
       </c>
     </row>
-    <row r="143" spans="1:190" ht="15">
+    <row r="143" spans="1:192" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -83874,7 +83928,7 @@
         <v>45833</v>
       </c>
     </row>
-    <row r="144" spans="1:190" ht="15">
+    <row r="144" spans="1:192" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed Jun 25 17:40:34 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1327" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CE5C124-3324-416A-B9D0-C872BF340B7D}"/>
+  <xr:revisionPtr revIDLastSave="1389" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B44C9A-2E87-4522-AAC1-D9ECD754AFE2}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="200">
   <si>
     <t>Module ID</t>
   </si>
@@ -1173,8 +1173,8 @@
   <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GD101" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GJ112" sqref="GJ112"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GC117" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GJ127" sqref="GJ127"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73048,7 +73048,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:190" ht="15">
+    <row r="33" spans="1:192" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73197,7 +73197,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:190" ht="15">
+    <row r="34" spans="1:192" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73346,7 +73346,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:190" ht="15">
+    <row r="35" spans="1:192" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73495,7 +73495,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:190" ht="15">
+    <row r="36" spans="1:192" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73629,7 +73629,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:190" ht="15">
+    <row r="37" spans="1:192" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73763,7 +73763,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:190" ht="15">
+    <row r="38" spans="1:192" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73897,7 +73897,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:190" ht="15">
+    <row r="39" spans="1:192" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74060,7 +74060,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:190" ht="15">
+    <row r="40" spans="1:192" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74223,7 +74223,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:190" ht="15">
+    <row r="41" spans="1:192" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74386,7 +74386,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:190" ht="15">
+    <row r="42" spans="1:192" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74549,7 +74549,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:190" ht="15">
+    <row r="43" spans="1:192" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74712,7 +74712,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:190" ht="15">
+    <row r="44" spans="1:192" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74875,7 +74875,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:190" ht="15">
+    <row r="45" spans="1:192" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75038,7 +75038,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:190" ht="15">
+    <row r="46" spans="1:192" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75201,7 +75201,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:190" ht="15">
+    <row r="47" spans="1:192" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75360,8 +75360,14 @@
       <c r="GH47" s="3">
         <v>23</v>
       </c>
+      <c r="GI47" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ47" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="48" spans="1:190" ht="15">
+    <row r="48" spans="1:192" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75572,7 +75578,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:190" ht="15">
+    <row r="49" spans="1:192" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75731,8 +75737,14 @@
       <c r="GH49" s="3">
         <v>23</v>
       </c>
+      <c r="GI49" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ49" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="50" spans="1:190" ht="15">
+    <row r="50" spans="1:192" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75943,7 +75955,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:190" ht="15">
+    <row r="51" spans="1:192" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76154,7 +76166,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:190" ht="15">
+    <row r="52" spans="1:192" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76365,7 +76377,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:190" ht="15">
+    <row r="53" spans="1:192" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76524,8 +76536,14 @@
       <c r="GH53" s="3">
         <v>23</v>
       </c>
+      <c r="GI53" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ53" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="54" spans="1:190" ht="15">
+    <row r="54" spans="1:192" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76684,8 +76702,14 @@
       <c r="GH54" s="3">
         <v>23</v>
       </c>
+      <c r="GI54" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ54" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="55" spans="1:190" ht="15">
+    <row r="55" spans="1:192" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76878,7 +76902,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:190" ht="15">
+    <row r="56" spans="1:192" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77071,7 +77095,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:190" ht="15">
+    <row r="57" spans="1:192" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77228,7 +77252,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:190" ht="15">
+    <row r="58" spans="1:192" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77384,7 +77408,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:190" ht="15">
+    <row r="59" spans="1:192" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77538,7 +77562,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:190" ht="15">
+    <row r="60" spans="1:192" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77684,7 +77708,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:190" ht="15">
+    <row r="61" spans="1:192" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77842,7 +77866,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:190" ht="15">
+    <row r="62" spans="1:192" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78081,7 +78105,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:190" ht="15">
+    <row r="63" spans="1:192" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78320,7 +78344,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:190" ht="15">
+    <row r="64" spans="1:192" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78559,7 +78583,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:191" ht="15">
+    <row r="65" spans="1:192" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78708,7 +78732,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:191" ht="15">
+    <row r="66" spans="1:192" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78857,7 +78881,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:191" ht="15">
+    <row r="67" spans="1:192" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -78996,7 +79020,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:191" ht="15">
+    <row r="68" spans="1:192" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79143,7 +79167,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:191" ht="15">
+    <row r="69" spans="1:192" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79277,7 +79301,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:191" ht="15">
+    <row r="70" spans="1:192" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79440,7 +79464,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:191" ht="15">
+    <row r="71" spans="1:192" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79587,7 +79611,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:191" ht="15">
+    <row r="72" spans="1:192" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79721,7 +79745,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:191" ht="15">
+    <row r="73" spans="1:192" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -79986,7 +80010,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:191" ht="15">
+    <row r="74" spans="1:192" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80251,7 +80275,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:191" ht="15">
+    <row r="75" spans="1:192" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80385,7 +80409,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:191" ht="15">
+    <row r="76" spans="1:192" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80519,7 +80543,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:191" ht="15">
+    <row r="77" spans="1:192" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80653,7 +80677,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:191" ht="15">
+    <row r="78" spans="1:192" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80893,8 +80917,11 @@
       <c r="GI78" s="3">
         <v>24</v>
       </c>
+      <c r="GJ78" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="79" spans="1:191" ht="15">
+    <row r="79" spans="1:192" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81028,7 +81055,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:191" ht="15">
+    <row r="80" spans="1:192" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81358,6 +81385,9 @@
       <c r="GI82" s="3">
         <v>24</v>
       </c>
+      <c r="GJ82" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="83" spans="1:192" ht="15">
       <c r="A83" s="9">
@@ -82007,6 +82037,9 @@
       <c r="GI95" s="3">
         <v>24</v>
       </c>
+      <c r="GJ95" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="96" spans="1:192" ht="15">
       <c r="A96" s="15">
@@ -82148,6 +82181,9 @@
       <c r="GI98" s="3">
         <v>24</v>
       </c>
+      <c r="GJ98" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="99" spans="1:192" ht="15">
       <c r="A99" s="15">
@@ -82532,6 +82568,9 @@
       <c r="GI107" s="3">
         <v>24</v>
       </c>
+      <c r="GJ107" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="108" spans="1:192" ht="15">
       <c r="A108" s="9">
@@ -82676,6 +82715,12 @@
       <c r="GH110" s="3">
         <v>23</v>
       </c>
+      <c r="GI110" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ110" s="3">
+        <v>23</v>
+      </c>
     </row>
     <row r="111" spans="1:192" ht="15">
       <c r="A111" s="9">
@@ -82743,6 +82788,9 @@
       <c r="F112" s="13">
         <v>45818</v>
       </c>
+      <c r="P112" s="13">
+        <v>45831</v>
+      </c>
       <c r="FU112" s="3">
         <v>5</v>
       </c>
@@ -82785,8 +82833,11 @@
       <c r="GH112" s="3">
         <v>5</v>
       </c>
+      <c r="GI112" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="113" spans="1:190" ht="15">
+    <row r="113" spans="1:192" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -82833,7 +82884,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:190" ht="15">
+    <row r="114" spans="1:192" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -82894,8 +82945,14 @@
       <c r="GH114" s="3">
         <v>16</v>
       </c>
+      <c r="GI114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GJ114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:190" ht="15">
+    <row r="115" spans="1:192" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -82956,8 +83013,14 @@
       <c r="GH115" s="3">
         <v>23</v>
       </c>
+      <c r="GI115" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ115" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="116" spans="1:190" ht="15">
+    <row r="116" spans="1:192" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -82976,6 +83039,9 @@
       <c r="F116" s="13">
         <v>45818</v>
       </c>
+      <c r="P116" s="13">
+        <v>45831</v>
+      </c>
       <c r="FU116" s="3">
         <v>12</v>
       </c>
@@ -83018,8 +83084,14 @@
       <c r="GH116" s="3">
         <v>23</v>
       </c>
+      <c r="GI116" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ116" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="117" spans="1:190" ht="15">
+    <row r="117" spans="1:192" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83083,8 +83155,11 @@
       <c r="GH117" s="3">
         <v>5</v>
       </c>
+      <c r="GI117" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="118" spans="1:190" ht="15">
+    <row r="118" spans="1:192" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83103,6 +83178,9 @@
       <c r="F118" s="13">
         <v>45817</v>
       </c>
+      <c r="P118" s="13">
+        <v>45831</v>
+      </c>
       <c r="FT118" s="3">
         <v>5</v>
       </c>
@@ -83148,8 +83226,11 @@
       <c r="GH118" s="3">
         <v>5</v>
       </c>
+      <c r="GI118" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="119" spans="1:190" ht="15">
+    <row r="119" spans="1:192" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83168,6 +83249,9 @@
       <c r="F119" s="13">
         <v>45817</v>
       </c>
+      <c r="P119" s="13">
+        <v>45831</v>
+      </c>
       <c r="FT119" s="3">
         <v>5</v>
       </c>
@@ -83213,8 +83297,11 @@
       <c r="GH119" s="3">
         <v>5</v>
       </c>
+      <c r="GI119" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="120" spans="1:190" ht="15">
+    <row r="120" spans="1:192" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83233,6 +83320,9 @@
       <c r="F120" s="13">
         <v>45817</v>
       </c>
+      <c r="P120" s="13">
+        <v>45831</v>
+      </c>
       <c r="FT120" s="3">
         <v>5</v>
       </c>
@@ -83278,8 +83368,11 @@
       <c r="GH120" s="3">
         <v>5</v>
       </c>
+      <c r="GI120" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="121" spans="1:190" ht="15">
+    <row r="121" spans="1:192" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83320,7 +83413,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:190" ht="15">
+    <row r="122" spans="1:192" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -83379,7 +83472,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:190" ht="15">
+    <row r="123" spans="1:192" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -83404,8 +83497,14 @@
       <c r="GH123" s="3">
         <v>5</v>
       </c>
+      <c r="GI123" s="3">
+        <v>5</v>
+      </c>
+      <c r="GJ123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:190" ht="15">
+    <row r="124" spans="1:192" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -83424,6 +83523,9 @@
       <c r="F124" s="13">
         <v>45828</v>
       </c>
+      <c r="P124" s="13">
+        <v>45832</v>
+      </c>
       <c r="GE124" s="3">
         <v>6</v>
       </c>
@@ -83436,8 +83538,14 @@
       <c r="GH124" s="3">
         <v>23</v>
       </c>
+      <c r="GI124" s="3">
+        <v>19</v>
+      </c>
+      <c r="GJ124" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="125" spans="1:190" ht="15">
+    <row r="125" spans="1:192" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -83468,8 +83576,14 @@
       <c r="GH125" s="3">
         <v>23</v>
       </c>
+      <c r="GI125" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ125" s="3">
+        <v>23</v>
+      </c>
     </row>
-    <row r="126" spans="1:190" ht="15">
+    <row r="126" spans="1:192" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -83510,7 +83624,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:190" ht="15">
+    <row r="127" spans="1:192" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -83551,7 +83665,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="128" spans="1:190" ht="15">
+    <row r="128" spans="1:192" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -83703,7 +83817,7 @@
         <v>24</v>
       </c>
       <c r="GJ131" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="132" spans="1:192" ht="15">
@@ -83732,7 +83846,7 @@
         <v>24</v>
       </c>
       <c r="GJ132" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="133" spans="1:192" ht="15">
@@ -83907,6 +84021,9 @@
       <c r="F142" s="13">
         <v>45833</v>
       </c>
+      <c r="GJ142" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="143" spans="1:192" ht="15">
       <c r="A143" s="9">
@@ -83927,6 +84044,9 @@
       <c r="F143" s="13">
         <v>45833</v>
       </c>
+      <c r="GJ143" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="144" spans="1:192" ht="15">
       <c r="A144" s="9">
@@ -83947,8 +84067,11 @@
       <c r="F144" s="13">
         <v>45833</v>
       </c>
+      <c r="GJ144" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="145" spans="1:6" ht="15">
+    <row r="145" spans="1:192" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -83967,8 +84090,11 @@
       <c r="F145" s="13">
         <v>45833</v>
       </c>
+      <c r="GJ145" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="146" spans="1:6" ht="15">
+    <row r="146" spans="1:192" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -83987,8 +84113,11 @@
       <c r="F146" s="13">
         <v>45833</v>
       </c>
+      <c r="GJ146" s="3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="147" spans="1:6" ht="15">
+    <row r="147" spans="1:192" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -84007,8 +84136,11 @@
       <c r="F147" s="13">
         <v>45833</v>
       </c>
+      <c r="GJ147" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:6" ht="15">
+    <row r="148" spans="1:192" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -84027,8 +84159,11 @@
       <c r="F148" s="13">
         <v>45833</v>
       </c>
+      <c r="GJ148" s="3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="149" spans="1:6" ht="15">
+    <row r="149" spans="1:192" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -84045,7 +84180,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15">
+    <row r="150" spans="1:192" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -84064,8 +84199,11 @@
       <c r="F150" s="13">
         <v>45833</v>
       </c>
+      <c r="GJ150" s="3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="151" spans="1:6" ht="15">
+    <row r="151" spans="1:192" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -84082,7 +84220,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15">
+    <row r="152" spans="1:192" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -84099,7 +84237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15">
+    <row r="153" spans="1:192" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -84116,7 +84254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15">
+    <row r="154" spans="1:192" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -84133,7 +84271,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15">
+    <row r="155" spans="1:192" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -84150,7 +84288,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="15">
+    <row r="156" spans="1:192" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -84167,7 +84305,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15">
+    <row r="157" spans="1:192" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun 26 09:40:48 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1389" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B44C9A-2E87-4522-AAC1-D9ECD754AFE2}"/>
+  <xr:revisionPtr revIDLastSave="1393" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD3ECEE-6318-4C8F-AD29-6B40D18D0C20}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1173,8 +1173,8 @@
   <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GC117" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GJ127" sqref="GJ127"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GE145" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F149" sqref="F149"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -84179,6 +84179,9 @@
       <c r="E149" s="9">
         <v>60</v>
       </c>
+      <c r="F149" s="13">
+        <v>45834</v>
+      </c>
     </row>
     <row r="150" spans="1:192" ht="15">
       <c r="A150" s="9">
@@ -84236,6 +84239,9 @@
       <c r="E152" s="9">
         <v>60</v>
       </c>
+      <c r="F152" s="13">
+        <v>45834</v>
+      </c>
     </row>
     <row r="153" spans="1:192" ht="15">
       <c r="A153" s="9">
@@ -84253,6 +84259,9 @@
       <c r="E153" s="9">
         <v>60</v>
       </c>
+      <c r="F153" s="13">
+        <v>45834</v>
+      </c>
     </row>
     <row r="154" spans="1:192" ht="15">
       <c r="A154" s="9">
@@ -84320,6 +84329,9 @@
       </c>
       <c r="E157" s="9">
         <v>60</v>
+      </c>
+      <c r="F157" s="13">
+        <v>45834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun 26 11:35:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1393" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD3ECEE-6318-4C8F-AD29-6B40D18D0C20}"/>
+  <xr:revisionPtr revIDLastSave="1398" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C35902-4E99-4A1A-91CB-AB7DD6E7F3A3}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1173,8 +1173,8 @@
   <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GE145" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F149" sqref="F149"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GE2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GJ126" sqref="GJ126"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -82837,7 +82837,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="113" spans="1:192" ht="15">
+    <row r="113" spans="1:193" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -82884,7 +82884,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:192" ht="15">
+    <row r="114" spans="1:193" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -82952,7 +82952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:192" ht="15">
+    <row r="115" spans="1:193" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83020,7 +83020,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:192" ht="15">
+    <row r="116" spans="1:193" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83091,7 +83091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:192" ht="15">
+    <row r="117" spans="1:193" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83159,7 +83159,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="118" spans="1:192" ht="15">
+    <row r="118" spans="1:193" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83230,7 +83230,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="119" spans="1:192" ht="15">
+    <row r="119" spans="1:193" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83301,7 +83301,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:192" ht="15">
+    <row r="120" spans="1:193" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83372,7 +83372,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:192" ht="15">
+    <row r="121" spans="1:193" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83413,7 +83413,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:192" ht="15">
+    <row r="122" spans="1:193" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -83472,7 +83472,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:192" ht="15">
+    <row r="123" spans="1:193" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -83503,8 +83503,11 @@
       <c r="GJ123" s="3">
         <v>5</v>
       </c>
+      <c r="GK123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:192" ht="15">
+    <row r="124" spans="1:193" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -83545,7 +83548,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="125" spans="1:192" ht="15">
+    <row r="125" spans="1:193" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -83583,7 +83586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:192" ht="15">
+    <row r="126" spans="1:193" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -83624,7 +83627,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:192" ht="15">
+    <row r="127" spans="1:193" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -83665,7 +83668,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="128" spans="1:192" ht="15">
+    <row r="128" spans="1:193" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84071,7 +84074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:192" ht="15">
+    <row r="145" spans="1:193" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -84094,7 +84097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:192" ht="15">
+    <row r="146" spans="1:193" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -84117,7 +84120,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:192" ht="15">
+    <row r="147" spans="1:193" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -84140,7 +84143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:192" ht="15">
+    <row r="148" spans="1:193" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -84163,7 +84166,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:192" ht="15">
+    <row r="149" spans="1:193" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -84182,8 +84185,11 @@
       <c r="F149" s="13">
         <v>45834</v>
       </c>
+      <c r="GK149" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="150" spans="1:192" ht="15">
+    <row r="150" spans="1:193" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -84206,7 +84212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:192" ht="15">
+    <row r="151" spans="1:193" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -84223,7 +84229,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="152" spans="1:192" ht="15">
+    <row r="152" spans="1:193" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -84242,8 +84248,11 @@
       <c r="F152" s="13">
         <v>45834</v>
       </c>
+      <c r="GK152" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:192" ht="15">
+    <row r="153" spans="1:193" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -84262,8 +84271,11 @@
       <c r="F153" s="13">
         <v>45834</v>
       </c>
+      <c r="GK153" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:192" ht="15">
+    <row r="154" spans="1:193" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -84280,7 +84292,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="155" spans="1:192" ht="15">
+    <row r="155" spans="1:193" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -84297,7 +84309,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="156" spans="1:192" ht="15">
+    <row r="156" spans="1:193" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -84314,7 +84326,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="157" spans="1:192" ht="15">
+    <row r="157" spans="1:193" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -84332,6 +84344,9 @@
       </c>
       <c r="F157" s="13">
         <v>45834</v>
+      </c>
+      <c r="GK157" s="3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu Jun 26 15:40:22 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1398" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C35902-4E99-4A1A-91CB-AB7DD6E7F3A3}"/>
+  <xr:revisionPtr revIDLastSave="1423" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E16C8E3-666D-498F-B6CF-124A19AB00A3}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1173,8 +1173,8 @@
   <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GE2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GJ126" sqref="GJ126"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GE136" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GK140" sqref="GK140"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73048,7 +73048,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:192" ht="15">
+    <row r="33" spans="1:193" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73197,7 +73197,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:192" ht="15">
+    <row r="34" spans="1:193" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73346,7 +73346,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:192" ht="15">
+    <row r="35" spans="1:193" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73495,7 +73495,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:192" ht="15">
+    <row r="36" spans="1:193" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73629,7 +73629,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:192" ht="15">
+    <row r="37" spans="1:193" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73763,7 +73763,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:192" ht="15">
+    <row r="38" spans="1:193" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73897,7 +73897,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:192" ht="15">
+    <row r="39" spans="1:193" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74060,7 +74060,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:192" ht="15">
+    <row r="40" spans="1:193" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74223,7 +74223,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:192" ht="15">
+    <row r="41" spans="1:193" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74386,7 +74386,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:192" ht="15">
+    <row r="42" spans="1:193" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74549,7 +74549,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:192" ht="15">
+    <row r="43" spans="1:193" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74712,7 +74712,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:192" ht="15">
+    <row r="44" spans="1:193" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74875,7 +74875,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:192" ht="15">
+    <row r="45" spans="1:193" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75038,7 +75038,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:192" ht="15">
+    <row r="46" spans="1:193" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75201,7 +75201,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:192" ht="15">
+    <row r="47" spans="1:193" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75366,8 +75366,11 @@
       <c r="GJ47" s="3">
         <v>23</v>
       </c>
+      <c r="GK47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:192" ht="15">
+    <row r="48" spans="1:193" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75578,7 +75581,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:192" ht="15">
+    <row r="49" spans="1:193" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75743,8 +75746,11 @@
       <c r="GJ49" s="3">
         <v>23</v>
       </c>
+      <c r="GK49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:192" ht="15">
+    <row r="50" spans="1:193" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75955,7 +75961,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:192" ht="15">
+    <row r="51" spans="1:193" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76166,7 +76172,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:192" ht="15">
+    <row r="52" spans="1:193" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76377,7 +76383,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:192" ht="15">
+    <row r="53" spans="1:193" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76542,8 +76548,11 @@
       <c r="GJ53" s="3">
         <v>23</v>
       </c>
+      <c r="GK53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:192" ht="15">
+    <row r="54" spans="1:193" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76708,8 +76717,11 @@
       <c r="GJ54" s="3">
         <v>23</v>
       </c>
+      <c r="GK54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:192" ht="15">
+    <row r="55" spans="1:193" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76902,7 +76914,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:192" ht="15">
+    <row r="56" spans="1:193" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77095,7 +77107,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:192" ht="15">
+    <row r="57" spans="1:193" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77252,7 +77264,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:192" ht="15">
+    <row r="58" spans="1:193" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77408,7 +77420,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:192" ht="15">
+    <row r="59" spans="1:193" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77562,7 +77574,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:192" ht="15">
+    <row r="60" spans="1:193" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77708,7 +77720,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:192" ht="15">
+    <row r="61" spans="1:193" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77866,7 +77878,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:192" ht="15">
+    <row r="62" spans="1:193" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78105,7 +78117,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:192" ht="15">
+    <row r="63" spans="1:193" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78344,7 +78356,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:192" ht="15">
+    <row r="64" spans="1:193" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78583,7 +78595,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:192" ht="15">
+    <row r="65" spans="1:193" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78732,7 +78744,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:192" ht="15">
+    <row r="66" spans="1:193" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78881,7 +78893,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:192" ht="15">
+    <row r="67" spans="1:193" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79020,7 +79032,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:192" ht="15">
+    <row r="68" spans="1:193" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79167,7 +79179,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:192" ht="15">
+    <row r="69" spans="1:193" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79301,7 +79313,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:192" ht="15">
+    <row r="70" spans="1:193" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79464,7 +79476,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:192" ht="15">
+    <row r="71" spans="1:193" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79611,7 +79623,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:192" ht="15">
+    <row r="72" spans="1:193" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79745,7 +79757,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:192" ht="15">
+    <row r="73" spans="1:193" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80010,7 +80022,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:192" ht="15">
+    <row r="74" spans="1:193" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80275,7 +80287,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:192" ht="15">
+    <row r="75" spans="1:193" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80409,7 +80421,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:192" ht="15">
+    <row r="76" spans="1:193" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80543,7 +80555,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:192" ht="15">
+    <row r="77" spans="1:193" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80677,7 +80689,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:192" ht="15">
+    <row r="78" spans="1:193" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80920,8 +80932,11 @@
       <c r="GJ78" s="3">
         <v>23</v>
       </c>
+      <c r="GK78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:192" ht="15">
+    <row r="79" spans="1:193" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81055,7 +81070,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:192" ht="15">
+    <row r="80" spans="1:193" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81244,7 +81259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:192" ht="15">
+    <row r="81" spans="1:193" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81285,7 +81300,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:192" ht="15">
+    <row r="82" spans="1:193" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81388,8 +81403,11 @@
       <c r="GJ82" s="3">
         <v>23</v>
       </c>
+      <c r="GK82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:192" ht="15">
+    <row r="83" spans="1:193" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81430,7 +81448,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:192" ht="15">
+    <row r="84" spans="1:193" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81492,7 +81510,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="85" spans="1:192" ht="15">
+    <row r="85" spans="1:193" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81584,7 +81602,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:192" ht="15">
+    <row r="86" spans="1:193" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81604,7 +81622,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:192" ht="15">
+    <row r="87" spans="1:193" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81622,7 +81640,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:192" ht="15">
+    <row r="88" spans="1:193" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81640,7 +81658,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:192" ht="15">
+    <row r="89" spans="1:193" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81699,7 +81717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:192" ht="15">
+    <row r="90" spans="1:193" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81758,7 +81776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:192" ht="15">
+    <row r="91" spans="1:193" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81817,7 +81835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:192" ht="15">
+    <row r="92" spans="1:193" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81876,7 +81894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:192" ht="15">
+    <row r="93" spans="1:193" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81935,7 +81953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:192" ht="15">
+    <row r="94" spans="1:193" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -81991,7 +82009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:192" ht="15">
+    <row r="95" spans="1:193" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82040,8 +82058,11 @@
       <c r="GJ95" s="3">
         <v>23</v>
       </c>
+      <c r="GK95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:192" ht="15">
+    <row r="96" spans="1:193" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82082,7 +82103,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="1:192" ht="15">
+    <row r="97" spans="1:193" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82123,7 +82144,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="98" spans="1:192" ht="15">
+    <row r="98" spans="1:193" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82184,8 +82205,11 @@
       <c r="GJ98" s="3">
         <v>23</v>
       </c>
+      <c r="GK98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:192" ht="15">
+    <row r="99" spans="1:193" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82205,7 +82229,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:192" ht="15">
+    <row r="100" spans="1:193" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82246,7 +82270,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="1:192" ht="15">
+    <row r="101" spans="1:193" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82287,7 +82311,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:192" ht="15">
+    <row r="102" spans="1:193" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82328,7 +82352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:192" ht="15">
+    <row r="103" spans="1:193" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82369,7 +82393,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:192" ht="15">
+    <row r="104" spans="1:193" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82410,7 +82434,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:192" ht="15">
+    <row r="105" spans="1:193" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82469,7 +82493,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="1:192" ht="15">
+    <row r="106" spans="1:193" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82510,7 +82534,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="107" spans="1:192" ht="15">
+    <row r="107" spans="1:193" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82571,8 +82595,11 @@
       <c r="GJ107" s="3">
         <v>23</v>
       </c>
+      <c r="GK107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:192" ht="15">
+    <row r="108" spans="1:193" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82634,7 +82661,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:192" ht="15">
+    <row r="109" spans="1:193" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82654,7 +82681,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:192" ht="15">
+    <row r="110" spans="1:193" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -82721,8 +82748,11 @@
       <c r="GJ110" s="3">
         <v>23</v>
       </c>
+      <c r="GK110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:192" ht="15">
+    <row r="111" spans="1:193" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -82769,7 +82799,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="1:192" ht="15">
+    <row r="112" spans="1:193" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -82951,6 +82981,9 @@
       <c r="GJ114" s="3">
         <v>16</v>
       </c>
+      <c r="GK114" s="3">
+        <v>16</v>
+      </c>
     </row>
     <row r="115" spans="1:193" ht="15">
       <c r="A115" s="9">
@@ -83019,6 +83052,9 @@
       <c r="GJ115" s="3">
         <v>23</v>
       </c>
+      <c r="GK115" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="116" spans="1:193" ht="15">
       <c r="A116" s="9">
@@ -83090,6 +83126,9 @@
       <c r="GJ116" s="3">
         <v>23</v>
       </c>
+      <c r="GK116" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="117" spans="1:193" ht="15">
       <c r="A117" s="9">
@@ -83585,6 +83624,9 @@
       <c r="GJ125" s="3">
         <v>23</v>
       </c>
+      <c r="GK125" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="126" spans="1:193" ht="15">
       <c r="A126" s="9">
@@ -83709,7 +83751,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:192" ht="15">
+    <row r="129" spans="1:193" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -83750,7 +83792,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="130" spans="1:192" ht="15">
+    <row r="130" spans="1:193" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -83793,8 +83835,11 @@
       <c r="GJ130" s="3">
         <v>24</v>
       </c>
+      <c r="GK130" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="131" spans="1:192" ht="15">
+    <row r="131" spans="1:193" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -83822,8 +83867,11 @@
       <c r="GJ131" s="3">
         <v>23</v>
       </c>
+      <c r="GK131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:192" ht="15">
+    <row r="132" spans="1:193" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -83851,8 +83899,11 @@
       <c r="GJ132" s="3">
         <v>23</v>
       </c>
+      <c r="GK132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:192" ht="15">
+    <row r="133" spans="1:193" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -83869,7 +83920,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:192" ht="15">
+    <row r="134" spans="1:193" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -83886,7 +83937,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:192" ht="15">
+    <row r="135" spans="1:193" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -83903,7 +83954,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:192" ht="15">
+    <row r="136" spans="1:193" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -83920,7 +83971,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:192" ht="15">
+    <row r="137" spans="1:193" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -83937,7 +83988,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:192" ht="15">
+    <row r="138" spans="1:193" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -83954,7 +84005,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="139" spans="1:192" ht="15">
+    <row r="139" spans="1:193" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -83971,7 +84022,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="140" spans="1:192" ht="15">
+    <row r="140" spans="1:193" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -83988,7 +84039,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="141" spans="1:192" ht="15">
+    <row r="141" spans="1:193" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -84005,7 +84056,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="142" spans="1:192" ht="15">
+    <row r="142" spans="1:193" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -84027,8 +84078,11 @@
       <c r="GJ142" s="3">
         <v>5</v>
       </c>
+      <c r="GK142" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="143" spans="1:192" ht="15">
+    <row r="143" spans="1:193" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -84050,8 +84104,11 @@
       <c r="GJ143" s="3">
         <v>12</v>
       </c>
+      <c r="GK143" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="144" spans="1:192" ht="15">
+    <row r="144" spans="1:193" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -84071,6 +84128,9 @@
         <v>45833</v>
       </c>
       <c r="GJ144" s="3">
+        <v>5</v>
+      </c>
+      <c r="GK144" s="3">
         <v>5</v>
       </c>
     </row>
@@ -84096,6 +84156,9 @@
       <c r="GJ145" s="3">
         <v>5</v>
       </c>
+      <c r="GK145" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="146" spans="1:193" ht="15">
       <c r="A146" s="9">
@@ -84119,6 +84182,9 @@
       <c r="GJ146" s="3">
         <v>12</v>
       </c>
+      <c r="GK146" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="147" spans="1:193" ht="15">
       <c r="A147" s="9">
@@ -84142,6 +84208,9 @@
       <c r="GJ147" s="3">
         <v>5</v>
       </c>
+      <c r="GK147" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="148" spans="1:193" ht="15">
       <c r="A148" s="9">
@@ -84165,6 +84234,9 @@
       <c r="GJ148" s="3">
         <v>12</v>
       </c>
+      <c r="GK148" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="149" spans="1:193" ht="15">
       <c r="A149" s="9">
@@ -84210,6 +84282,9 @@
       </c>
       <c r="GJ150" s="3">
         <v>12</v>
+      </c>
+      <c r="GK150" s="3">
+        <v>24</v>
       </c>
     </row>
     <row r="151" spans="1:193" ht="15">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-06-30 17:04:27
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29022"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1423" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E16C8E3-666D-498F-B6CF-124A19AB00A3}"/>
+  <xr:revisionPtr revIDLastSave="1522" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D105076-91E4-48EC-89B8-FB2049626AB8}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="200">
   <si>
     <t>Module ID</t>
   </si>
@@ -1170,11 +1170,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD157"/>
+  <dimension ref="A1:XFD158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GE136" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GK140" sqref="GK140"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GG145" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F151" sqref="F151"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73048,7 +73048,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:193" ht="15">
+    <row r="33" spans="1:196" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73197,7 +73197,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:193" ht="15">
+    <row r="34" spans="1:196" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73346,7 +73346,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:193" ht="15">
+    <row r="35" spans="1:196" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73495,7 +73495,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:193" ht="15">
+    <row r="36" spans="1:196" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73629,7 +73629,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:193" ht="15">
+    <row r="37" spans="1:196" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73763,7 +73763,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:193" ht="15">
+    <row r="38" spans="1:196" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73897,7 +73897,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:193" ht="15">
+    <row r="39" spans="1:196" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74060,7 +74060,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:193" ht="15">
+    <row r="40" spans="1:196" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74223,7 +74223,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:193" ht="15">
+    <row r="41" spans="1:196" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74386,7 +74386,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:193" ht="15">
+    <row r="42" spans="1:196" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74549,7 +74549,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:193" ht="15">
+    <row r="43" spans="1:196" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74712,7 +74712,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:193" ht="15">
+    <row r="44" spans="1:196" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74875,7 +74875,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:193" ht="15">
+    <row r="45" spans="1:196" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75038,7 +75038,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:193" ht="15">
+    <row r="46" spans="1:196" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75201,7 +75201,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:193" ht="15">
+    <row r="47" spans="1:196" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75369,8 +75369,17 @@
       <c r="GK47" s="3">
         <v>24</v>
       </c>
+      <c r="GL47" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM47" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:193" ht="15">
+    <row r="48" spans="1:196" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75581,7 +75590,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:193" ht="15">
+    <row r="49" spans="1:196" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75749,8 +75758,17 @@
       <c r="GK49" s="3">
         <v>24</v>
       </c>
+      <c r="GL49" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM49" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:193" ht="15">
+    <row r="50" spans="1:196" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75961,7 +75979,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:193" ht="15">
+    <row r="51" spans="1:196" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76172,7 +76190,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:193" ht="15">
+    <row r="52" spans="1:196" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76383,7 +76401,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:193" ht="15">
+    <row r="53" spans="1:196" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76551,8 +76569,17 @@
       <c r="GK53" s="3">
         <v>24</v>
       </c>
+      <c r="GL53" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM53" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:193" ht="15">
+    <row r="54" spans="1:196" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76720,8 +76747,17 @@
       <c r="GK54" s="3">
         <v>24</v>
       </c>
+      <c r="GL54" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM54" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:193" ht="15">
+    <row r="55" spans="1:196" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76914,7 +76950,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:193" ht="15">
+    <row r="56" spans="1:196" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77107,7 +77143,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:193" ht="15">
+    <row r="57" spans="1:196" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77264,7 +77300,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:193" ht="15">
+    <row r="58" spans="1:196" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77420,7 +77456,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:193" ht="15">
+    <row r="59" spans="1:196" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77574,7 +77610,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:193" ht="15">
+    <row r="60" spans="1:196" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77720,7 +77756,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:193" ht="15">
+    <row r="61" spans="1:196" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77878,7 +77914,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:193" ht="15">
+    <row r="62" spans="1:196" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78117,7 +78153,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:193" ht="15">
+    <row r="63" spans="1:196" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78356,7 +78392,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:193" ht="15">
+    <row r="64" spans="1:196" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78595,7 +78631,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:193" ht="15">
+    <row r="65" spans="1:196" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78744,7 +78780,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:193" ht="15">
+    <row r="66" spans="1:196" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78893,7 +78929,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:193" ht="15">
+    <row r="67" spans="1:196" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79032,7 +79068,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:193" ht="15">
+    <row r="68" spans="1:196" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79179,7 +79215,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:193" ht="15">
+    <row r="69" spans="1:196" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79313,7 +79349,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:193" ht="15">
+    <row r="70" spans="1:196" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79476,7 +79512,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:193" ht="15">
+    <row r="71" spans="1:196" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79623,7 +79659,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:193" ht="15">
+    <row r="72" spans="1:196" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79757,7 +79793,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:193" ht="15">
+    <row r="73" spans="1:196" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80022,7 +80058,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:193" ht="15">
+    <row r="74" spans="1:196" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80287,7 +80323,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:193" ht="15">
+    <row r="75" spans="1:196" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80421,7 +80457,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:193" ht="15">
+    <row r="76" spans="1:196" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80555,7 +80591,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:193" ht="15">
+    <row r="77" spans="1:196" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80689,7 +80725,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:193" ht="15">
+    <row r="78" spans="1:196" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80935,8 +80971,17 @@
       <c r="GK78" s="3">
         <v>24</v>
       </c>
+      <c r="GL78" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM78" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:193" ht="15">
+    <row r="79" spans="1:196" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81070,7 +81115,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:193" ht="15">
+    <row r="80" spans="1:196" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81259,7 +81304,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:193" ht="15">
+    <row r="81" spans="1:196" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81300,7 +81345,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:193" ht="15">
+    <row r="82" spans="1:196" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81406,8 +81451,17 @@
       <c r="GK82" s="3">
         <v>24</v>
       </c>
+      <c r="GL82" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM82" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:193" ht="15">
+    <row r="83" spans="1:196" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81448,7 +81502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:193" ht="15">
+    <row r="84" spans="1:196" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81510,7 +81564,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="85" spans="1:193" ht="15">
+    <row r="85" spans="1:196" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81602,7 +81656,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:193" ht="15">
+    <row r="86" spans="1:196" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81622,7 +81676,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:193" ht="15">
+    <row r="87" spans="1:196" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81640,7 +81694,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:193" ht="15">
+    <row r="88" spans="1:196" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81658,7 +81712,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:193" ht="15">
+    <row r="89" spans="1:196" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81717,7 +81771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:193" ht="15">
+    <row r="90" spans="1:196" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81776,7 +81830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:193" ht="15">
+    <row r="91" spans="1:196" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81835,7 +81889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:193" ht="15">
+    <row r="92" spans="1:196" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81894,7 +81948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:193" ht="15">
+    <row r="93" spans="1:196" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -81953,7 +82007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:193" ht="15">
+    <row r="94" spans="1:196" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82009,7 +82063,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:193" ht="15">
+    <row r="95" spans="1:196" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82061,8 +82115,17 @@
       <c r="GK95" s="3">
         <v>24</v>
       </c>
+      <c r="GL95" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM95" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:193" ht="15">
+    <row r="96" spans="1:196" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82103,7 +82166,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="1:193" ht="15">
+    <row r="97" spans="1:196" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82144,7 +82207,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="98" spans="1:193" ht="15">
+    <row r="98" spans="1:196" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82208,8 +82271,17 @@
       <c r="GK98" s="3">
         <v>24</v>
       </c>
+      <c r="GL98" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM98" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:193" ht="15">
+    <row r="99" spans="1:196" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82229,7 +82301,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:193" ht="15">
+    <row r="100" spans="1:196" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82270,7 +82342,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="1:193" ht="15">
+    <row r="101" spans="1:196" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82311,7 +82383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:193" ht="15">
+    <row r="102" spans="1:196" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82352,7 +82424,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:193" ht="15">
+    <row r="103" spans="1:196" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82393,7 +82465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:193" ht="15">
+    <row r="104" spans="1:196" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82434,7 +82506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:193" ht="15">
+    <row r="105" spans="1:196" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82493,7 +82565,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="1:193" ht="15">
+    <row r="106" spans="1:196" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82534,7 +82606,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="107" spans="1:193" ht="15">
+    <row r="107" spans="1:196" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82598,8 +82670,17 @@
       <c r="GK107" s="3">
         <v>24</v>
       </c>
+      <c r="GL107" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM107" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:193" ht="15">
+    <row r="108" spans="1:196" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82661,7 +82742,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:193" ht="15">
+    <row r="109" spans="1:196" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82681,7 +82762,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:193" ht="15">
+    <row r="110" spans="1:196" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -82751,8 +82832,17 @@
       <c r="GK110" s="3">
         <v>24</v>
       </c>
+      <c r="GL110" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM110" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:193" ht="15">
+    <row r="111" spans="1:196" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -82799,7 +82889,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="1:193" ht="15">
+    <row r="112" spans="1:196" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -82867,7 +82957,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="113" spans="1:193" ht="15">
+    <row r="113" spans="1:196" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -82914,7 +83004,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:193" ht="15">
+    <row r="114" spans="1:196" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -82984,8 +83074,17 @@
       <c r="GK114" s="3">
         <v>16</v>
       </c>
+      <c r="GL114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GM114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GN114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:193" ht="15">
+    <row r="115" spans="1:196" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83055,8 +83154,17 @@
       <c r="GK115" s="3">
         <v>24</v>
       </c>
+      <c r="GL115" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM115" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:193" ht="15">
+    <row r="116" spans="1:196" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83129,8 +83237,17 @@
       <c r="GK116" s="3">
         <v>24</v>
       </c>
+      <c r="GL116" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM116" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:193" ht="15">
+    <row r="117" spans="1:196" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83198,7 +83315,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="118" spans="1:193" ht="15">
+    <row r="118" spans="1:196" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83269,7 +83386,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="119" spans="1:193" ht="15">
+    <row r="119" spans="1:196" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83340,7 +83457,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:193" ht="15">
+    <row r="120" spans="1:196" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83411,7 +83528,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:193" ht="15">
+    <row r="121" spans="1:196" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83452,7 +83569,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:193" ht="15">
+    <row r="122" spans="1:196" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -83511,7 +83628,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:193" ht="15">
+    <row r="123" spans="1:196" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -83545,8 +83662,17 @@
       <c r="GK123" s="3">
         <v>5</v>
       </c>
+      <c r="GL123" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM123" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:193" ht="15">
+    <row r="124" spans="1:196" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -83587,7 +83713,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="125" spans="1:193" ht="15">
+    <row r="125" spans="1:196" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -83627,8 +83753,17 @@
       <c r="GK125" s="3">
         <v>24</v>
       </c>
+      <c r="GL125" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM125" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:193" ht="15">
+    <row r="126" spans="1:196" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -83669,7 +83804,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:193" ht="15">
+    <row r="127" spans="1:196" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -83710,7 +83845,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="128" spans="1:193" ht="15">
+    <row r="128" spans="1:196" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -83751,7 +83886,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:193" ht="15">
+    <row r="129" spans="1:196" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -83792,7 +83927,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="130" spans="1:193" ht="15">
+    <row r="130" spans="1:196" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -83838,8 +83973,17 @@
       <c r="GK130" s="3">
         <v>24</v>
       </c>
+      <c r="GL130" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM130" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN130" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="131" spans="1:193" ht="15">
+    <row r="131" spans="1:196" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -83870,8 +84014,17 @@
       <c r="GK131" s="3">
         <v>24</v>
       </c>
+      <c r="GL131" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM131" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:193" ht="15">
+    <row r="132" spans="1:196" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -83902,8 +84055,17 @@
       <c r="GK132" s="3">
         <v>24</v>
       </c>
+      <c r="GL132" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM132" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:193" ht="15">
+    <row r="133" spans="1:196" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -83920,7 +84082,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:193" ht="15">
+    <row r="134" spans="1:196" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -83937,7 +84099,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:193" ht="15">
+    <row r="135" spans="1:196" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -83954,7 +84116,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:193" ht="15">
+    <row r="136" spans="1:196" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -83971,7 +84133,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:193" ht="15">
+    <row r="137" spans="1:196" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -83988,7 +84150,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:193" ht="15">
+    <row r="138" spans="1:196" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -84005,7 +84167,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="139" spans="1:193" ht="15">
+    <row r="139" spans="1:196" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -84022,7 +84184,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="140" spans="1:193" ht="15">
+    <row r="140" spans="1:196" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -84039,7 +84201,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="141" spans="1:193" ht="15">
+    <row r="141" spans="1:196" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -84056,7 +84218,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="142" spans="1:193" ht="15">
+    <row r="142" spans="1:196" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -84081,8 +84243,17 @@
       <c r="GK142" s="3">
         <v>5</v>
       </c>
+      <c r="GL142" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM142" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN142" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="143" spans="1:193" ht="15">
+    <row r="143" spans="1:196" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -84107,8 +84278,17 @@
       <c r="GK143" s="3">
         <v>24</v>
       </c>
+      <c r="GL143" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM143" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN143" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="144" spans="1:193" ht="15">
+    <row r="144" spans="1:196" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -84133,8 +84313,17 @@
       <c r="GK144" s="3">
         <v>5</v>
       </c>
+      <c r="GL144" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM144" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN144" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="145" spans="1:193" ht="15">
+    <row r="145" spans="1:196" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -84159,8 +84348,17 @@
       <c r="GK145" s="3">
         <v>5</v>
       </c>
+      <c r="GL145" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM145" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN145" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="146" spans="1:193" ht="15">
+    <row r="146" spans="1:196" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -84185,8 +84383,17 @@
       <c r="GK146" s="3">
         <v>24</v>
       </c>
+      <c r="GL146" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM146" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN146" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="147" spans="1:193" ht="15">
+    <row r="147" spans="1:196" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -84211,8 +84418,17 @@
       <c r="GK147" s="3">
         <v>5</v>
       </c>
+      <c r="GL147" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM147" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN147" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:193" ht="15">
+    <row r="148" spans="1:196" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -84237,8 +84453,17 @@
       <c r="GK148" s="3">
         <v>24</v>
       </c>
+      <c r="GL148" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM148" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN148" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="149" spans="1:193" ht="15">
+    <row r="149" spans="1:196" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -84260,8 +84485,17 @@
       <c r="GK149" s="3">
         <v>5</v>
       </c>
+      <c r="GL149" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM149" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN149" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="150" spans="1:193" ht="15">
+    <row r="150" spans="1:196" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -84286,8 +84520,17 @@
       <c r="GK150" s="3">
         <v>24</v>
       </c>
+      <c r="GL150" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM150" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN150" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="151" spans="1:193" ht="15">
+    <row r="151" spans="1:196" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -84303,8 +84546,11 @@
       <c r="E151" s="9">
         <v>96</v>
       </c>
+      <c r="F151" s="13">
+        <v>45838</v>
+      </c>
     </row>
-    <row r="152" spans="1:193" ht="15">
+    <row r="152" spans="1:196" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -84326,8 +84572,17 @@
       <c r="GK152" s="3">
         <v>5</v>
       </c>
+      <c r="GL152" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM152" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN152" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:193" ht="15">
+    <row r="153" spans="1:196" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -84349,8 +84604,17 @@
       <c r="GK153" s="3">
         <v>5</v>
       </c>
+      <c r="GL153" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM153" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN153" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:193" ht="15">
+    <row r="154" spans="1:196" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -84366,8 +84630,11 @@
       <c r="E154" s="9">
         <v>96</v>
       </c>
+      <c r="F154" s="13">
+        <v>45838</v>
+      </c>
     </row>
-    <row r="155" spans="1:193" ht="15">
+    <row r="155" spans="1:196" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -84383,8 +84650,11 @@
       <c r="E155" s="9">
         <v>96</v>
       </c>
+      <c r="F155" s="13">
+        <v>45838</v>
+      </c>
     </row>
-    <row r="156" spans="1:193" ht="15">
+    <row r="156" spans="1:196" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -84400,8 +84670,11 @@
       <c r="E156" s="9">
         <v>96</v>
       </c>
+      <c r="F156" s="13">
+        <v>45838</v>
+      </c>
     </row>
-    <row r="157" spans="1:193" ht="15">
+    <row r="157" spans="1:196" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -84422,6 +84695,32 @@
       </c>
       <c r="GK157" s="3">
         <v>5</v>
+      </c>
+      <c r="GL157" s="3">
+        <v>5</v>
+      </c>
+      <c r="GM157" s="3">
+        <v>5</v>
+      </c>
+      <c r="GN157" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:196" ht="15">
+      <c r="A158" s="9">
+        <v>25273925</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C158" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D158" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E158" s="9">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-01 09:46:26
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1522" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D105076-91E4-48EC-89B8-FB2049626AB8}"/>
+  <xr:revisionPtr revIDLastSave="1590" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{903C3C67-352F-4D0C-8FEE-EE078B622CBE}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="208">
   <si>
     <t>Module ID</t>
   </si>
@@ -637,6 +637,30 @@
   <si>
     <t>VSL202526148</t>
   </si>
+  <si>
+    <t>VSL202425235</t>
+  </si>
+  <si>
+    <t>Ronma TOPCon Cell Trial</t>
+  </si>
+  <si>
+    <t>SAMPLE-1</t>
+  </si>
+  <si>
+    <t>EPE+EPE</t>
+  </si>
+  <si>
+    <t>SAMPLE-2</t>
+  </si>
+  <si>
+    <t>EPE+EPE+40MM POE</t>
+  </si>
+  <si>
+    <t>SAMPLE-3</t>
+  </si>
+  <si>
+    <t>EPE+EPE HIB TAPE</t>
+  </si>
 </sst>
 </file>
 
@@ -1170,11 +1194,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD158"/>
+  <dimension ref="A1:XFD162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GG145" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F151" sqref="F151"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GN155" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GO160" sqref="GO160:GO162"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73048,7 +73072,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:196" ht="15">
+    <row r="33" spans="1:197" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73197,7 +73221,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:196" ht="15">
+    <row r="34" spans="1:197" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73346,7 +73370,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:196" ht="15">
+    <row r="35" spans="1:197" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73495,7 +73519,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:196" ht="15">
+    <row r="36" spans="1:197" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73629,7 +73653,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:196" ht="15">
+    <row r="37" spans="1:197" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73763,7 +73787,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:196" ht="15">
+    <row r="38" spans="1:197" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73897,7 +73921,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:196" ht="15">
+    <row r="39" spans="1:197" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74060,7 +74084,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:196" ht="15">
+    <row r="40" spans="1:197" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74223,7 +74247,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:196" ht="15">
+    <row r="41" spans="1:197" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74386,7 +74410,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:196" ht="15">
+    <row r="42" spans="1:197" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74549,7 +74573,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:196" ht="15">
+    <row r="43" spans="1:197" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74712,7 +74736,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:196" ht="15">
+    <row r="44" spans="1:197" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74875,7 +74899,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:196" ht="15">
+    <row r="45" spans="1:197" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75038,7 +75062,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:196" ht="15">
+    <row r="46" spans="1:197" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75201,7 +75225,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:196" ht="15">
+    <row r="47" spans="1:197" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75378,8 +75402,11 @@
       <c r="GN47" s="3">
         <v>24</v>
       </c>
+      <c r="GO47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:196" ht="15">
+    <row r="48" spans="1:197" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75590,7 +75617,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:196" ht="15">
+    <row r="49" spans="1:197" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75767,8 +75794,11 @@
       <c r="GN49" s="3">
         <v>24</v>
       </c>
+      <c r="GO49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:196" ht="15">
+    <row r="50" spans="1:197" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -75979,7 +76009,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:196" ht="15">
+    <row r="51" spans="1:197" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76190,7 +76220,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:196" ht="15">
+    <row r="52" spans="1:197" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76401,7 +76431,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:196" ht="15">
+    <row r="53" spans="1:197" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76578,8 +76608,11 @@
       <c r="GN53" s="3">
         <v>24</v>
       </c>
+      <c r="GO53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:196" ht="15">
+    <row r="54" spans="1:197" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76756,8 +76789,11 @@
       <c r="GN54" s="3">
         <v>24</v>
       </c>
+      <c r="GO54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:196" ht="15">
+    <row r="55" spans="1:197" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76950,7 +76986,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:196" ht="15">
+    <row r="56" spans="1:197" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77143,7 +77179,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:196" ht="15">
+    <row r="57" spans="1:197" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77300,7 +77336,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:196" ht="15">
+    <row r="58" spans="1:197" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77456,7 +77492,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:196" ht="15">
+    <row r="59" spans="1:197" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77610,7 +77646,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:196" ht="15">
+    <row r="60" spans="1:197" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77756,7 +77792,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:196" ht="15">
+    <row r="61" spans="1:197" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77914,7 +77950,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:196" ht="15">
+    <row r="62" spans="1:197" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78153,7 +78189,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:196" ht="15">
+    <row r="63" spans="1:197" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78392,7 +78428,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:196" ht="15">
+    <row r="64" spans="1:197" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78631,7 +78667,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:196" ht="15">
+    <row r="65" spans="1:197" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78780,7 +78816,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:196" ht="15">
+    <row r="66" spans="1:197" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78929,7 +78965,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:196" ht="15">
+    <row r="67" spans="1:197" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79068,7 +79104,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:196" ht="15">
+    <row r="68" spans="1:197" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79215,7 +79251,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:196" ht="15">
+    <row r="69" spans="1:197" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79349,7 +79385,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:196" ht="15">
+    <row r="70" spans="1:197" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79512,7 +79548,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:196" ht="15">
+    <row r="71" spans="1:197" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79659,7 +79695,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:196" ht="15">
+    <row r="72" spans="1:197" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79793,7 +79829,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:196" ht="15">
+    <row r="73" spans="1:197" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80058,7 +80094,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:196" ht="15">
+    <row r="74" spans="1:197" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80323,7 +80359,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:196" ht="15">
+    <row r="75" spans="1:197" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80457,7 +80493,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:196" ht="15">
+    <row r="76" spans="1:197" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80591,7 +80627,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:196" ht="15">
+    <row r="77" spans="1:197" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80725,7 +80761,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:196" ht="15">
+    <row r="78" spans="1:197" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -80980,8 +81016,11 @@
       <c r="GN78" s="3">
         <v>24</v>
       </c>
+      <c r="GO78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:196" ht="15">
+    <row r="79" spans="1:197" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81115,7 +81154,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:196" ht="15">
+    <row r="80" spans="1:197" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81304,7 +81343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:196" ht="15">
+    <row r="81" spans="1:197" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81345,7 +81384,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:196" ht="15">
+    <row r="82" spans="1:197" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81460,8 +81499,11 @@
       <c r="GN82" s="3">
         <v>24</v>
       </c>
+      <c r="GO82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:196" ht="15">
+    <row r="83" spans="1:197" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81502,7 +81544,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:196" ht="15">
+    <row r="84" spans="1:197" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81564,7 +81606,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="85" spans="1:196" ht="15">
+    <row r="85" spans="1:197" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81655,8 +81697,11 @@
       <c r="FQ85" s="3">
         <v>208</v>
       </c>
+      <c r="FR85" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="86" spans="1:196" ht="15">
+    <row r="86" spans="1:197" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81676,7 +81721,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:196" ht="15">
+    <row r="87" spans="1:197" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81694,7 +81739,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:196" ht="15">
+    <row r="88" spans="1:197" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81712,7 +81757,7 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:196" ht="15">
+    <row r="89" spans="1:197" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81771,7 +81816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:196" ht="15">
+    <row r="90" spans="1:197" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81830,7 +81875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:196" ht="15">
+    <row r="91" spans="1:197" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -81889,7 +81934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:196" ht="15">
+    <row r="92" spans="1:197" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -81948,7 +81993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:196" ht="15">
+    <row r="93" spans="1:197" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82007,7 +82052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:196" ht="15">
+    <row r="94" spans="1:197" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82063,7 +82108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:196" ht="15">
+    <row r="95" spans="1:197" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82124,8 +82169,11 @@
       <c r="GN95" s="3">
         <v>24</v>
       </c>
+      <c r="GO95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:196" ht="15">
+    <row r="96" spans="1:197" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82166,7 +82214,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="1:196" ht="15">
+    <row r="97" spans="1:197" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82207,7 +82255,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="98" spans="1:196" ht="15">
+    <row r="98" spans="1:197" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82280,8 +82328,11 @@
       <c r="GN98" s="3">
         <v>24</v>
       </c>
+      <c r="GO98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:196" ht="15">
+    <row r="99" spans="1:197" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82301,7 +82352,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:196" ht="15">
+    <row r="100" spans="1:197" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82342,7 +82393,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="1:196" ht="15">
+    <row r="101" spans="1:197" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82383,7 +82434,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:196" ht="15">
+    <row r="102" spans="1:197" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82424,7 +82475,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:196" ht="15">
+    <row r="103" spans="1:197" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82465,7 +82516,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:196" ht="15">
+    <row r="104" spans="1:197" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82506,7 +82557,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:196" ht="15">
+    <row r="105" spans="1:197" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82565,7 +82616,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="1:196" ht="15">
+    <row r="106" spans="1:197" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82606,7 +82657,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="107" spans="1:196" ht="15">
+    <row r="107" spans="1:197" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82679,8 +82730,11 @@
       <c r="GN107" s="3">
         <v>24</v>
       </c>
+      <c r="GO107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:196" ht="15">
+    <row r="108" spans="1:197" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82742,7 +82796,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:196" ht="15">
+    <row r="109" spans="1:197" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82762,7 +82816,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:196" ht="15">
+    <row r="110" spans="1:197" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -82841,8 +82895,11 @@
       <c r="GN110" s="3">
         <v>24</v>
       </c>
+      <c r="GO110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:196" ht="15">
+    <row r="111" spans="1:197" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -82889,7 +82946,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="1:196" ht="15">
+    <row r="112" spans="1:197" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -82957,7 +83014,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="113" spans="1:196" ht="15">
+    <row r="113" spans="1:197" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83004,7 +83061,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:196" ht="15">
+    <row r="114" spans="1:197" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83083,8 +83140,11 @@
       <c r="GN114" s="3">
         <v>16</v>
       </c>
+      <c r="GO114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:196" ht="15">
+    <row r="115" spans="1:197" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83163,8 +83223,11 @@
       <c r="GN115" s="3">
         <v>24</v>
       </c>
+      <c r="GO115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:196" ht="15">
+    <row r="116" spans="1:197" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83246,8 +83309,11 @@
       <c r="GN116" s="3">
         <v>24</v>
       </c>
+      <c r="GO116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:196" ht="15">
+    <row r="117" spans="1:197" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83315,7 +83381,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="118" spans="1:196" ht="15">
+    <row r="118" spans="1:197" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83386,7 +83452,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="119" spans="1:196" ht="15">
+    <row r="119" spans="1:197" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83457,7 +83523,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:196" ht="15">
+    <row r="120" spans="1:197" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83528,7 +83594,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:196" ht="15">
+    <row r="121" spans="1:197" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83569,7 +83635,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:196" ht="15">
+    <row r="122" spans="1:197" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -83628,7 +83694,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:196" ht="15">
+    <row r="123" spans="1:197" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -83671,8 +83737,11 @@
       <c r="GN123" s="3">
         <v>5</v>
       </c>
+      <c r="GO123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:196" ht="15">
+    <row r="124" spans="1:197" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -83713,7 +83782,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="125" spans="1:196" ht="15">
+    <row r="125" spans="1:197" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -83762,8 +83831,11 @@
       <c r="GN125" s="3">
         <v>24</v>
       </c>
+      <c r="GO125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:196" ht="15">
+    <row r="126" spans="1:197" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -83804,7 +83876,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:196" ht="15">
+    <row r="127" spans="1:197" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -83845,7 +83917,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="128" spans="1:196" ht="15">
+    <row r="128" spans="1:197" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -83886,7 +83958,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:196" ht="15">
+    <row r="129" spans="1:197" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -83927,7 +83999,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="130" spans="1:196" ht="15">
+    <row r="130" spans="1:197" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -83983,7 +84055,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="131" spans="1:196" ht="15">
+    <row r="131" spans="1:197" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -84023,8 +84095,11 @@
       <c r="GN131" s="3">
         <v>24</v>
       </c>
+      <c r="GO131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:196" ht="15">
+    <row r="132" spans="1:197" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -84064,8 +84139,11 @@
       <c r="GN132" s="3">
         <v>24</v>
       </c>
+      <c r="GO132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:196" ht="15">
+    <row r="133" spans="1:197" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -84082,7 +84160,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:196" ht="15">
+    <row r="134" spans="1:197" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -84099,7 +84177,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:196" ht="15">
+    <row r="135" spans="1:197" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -84116,7 +84194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="136" spans="1:196" ht="15">
+    <row r="136" spans="1:197" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -84133,7 +84211,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:196" ht="15">
+    <row r="137" spans="1:197" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -84150,7 +84228,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:196" ht="15">
+    <row r="138" spans="1:197" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -84166,8 +84244,11 @@
       <c r="E138" s="9">
         <v>400</v>
       </c>
+      <c r="F138" s="13">
+        <v>45839</v>
+      </c>
     </row>
-    <row r="139" spans="1:196" ht="15">
+    <row r="139" spans="1:197" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -84183,8 +84264,11 @@
       <c r="E139" s="9">
         <v>400</v>
       </c>
+      <c r="F139" s="13">
+        <v>45839</v>
+      </c>
     </row>
-    <row r="140" spans="1:196" ht="15">
+    <row r="140" spans="1:197" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -84200,8 +84284,11 @@
       <c r="E140" s="9">
         <v>96</v>
       </c>
+      <c r="F140" s="13">
+        <v>45839</v>
+      </c>
     </row>
-    <row r="141" spans="1:196" ht="15">
+    <row r="141" spans="1:197" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -84217,8 +84304,11 @@
       <c r="E141" s="9">
         <v>96</v>
       </c>
+      <c r="F141" s="13">
+        <v>45839</v>
+      </c>
     </row>
-    <row r="142" spans="1:196" ht="15">
+    <row r="142" spans="1:197" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -84252,8 +84342,11 @@
       <c r="GN142" s="3">
         <v>5</v>
       </c>
+      <c r="GO142" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="143" spans="1:196" ht="15">
+    <row r="143" spans="1:197" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -84287,8 +84380,11 @@
       <c r="GN143" s="3">
         <v>24</v>
       </c>
+      <c r="GO143" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="144" spans="1:196" ht="15">
+    <row r="144" spans="1:197" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -84322,8 +84418,11 @@
       <c r="GN144" s="3">
         <v>5</v>
       </c>
+      <c r="GO144" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="145" spans="1:196" ht="15">
+    <row r="145" spans="1:197" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -84357,8 +84456,11 @@
       <c r="GN145" s="3">
         <v>5</v>
       </c>
+      <c r="GO145" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="146" spans="1:196" ht="15">
+    <row r="146" spans="1:197" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -84392,8 +84494,11 @@
       <c r="GN146" s="3">
         <v>24</v>
       </c>
+      <c r="GO146" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="147" spans="1:196" ht="15">
+    <row r="147" spans="1:197" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -84427,8 +84532,11 @@
       <c r="GN147" s="3">
         <v>5</v>
       </c>
+      <c r="GO147" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:196" ht="15">
+    <row r="148" spans="1:197" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -84462,8 +84570,11 @@
       <c r="GN148" s="3">
         <v>24</v>
       </c>
+      <c r="GO148" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="149" spans="1:196" ht="15">
+    <row r="149" spans="1:197" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -84494,8 +84605,11 @@
       <c r="GN149" s="3">
         <v>5</v>
       </c>
+      <c r="GO149" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="150" spans="1:196" ht="15">
+    <row r="150" spans="1:197" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -84529,8 +84643,11 @@
       <c r="GN150" s="3">
         <v>24</v>
       </c>
+      <c r="GO150" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="151" spans="1:196" ht="15">
+    <row r="151" spans="1:197" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -84550,7 +84667,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="152" spans="1:196" ht="15">
+    <row r="152" spans="1:197" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -84581,8 +84698,11 @@
       <c r="GN152" s="3">
         <v>5</v>
       </c>
+      <c r="GO152" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:196" ht="15">
+    <row r="153" spans="1:197" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -84613,8 +84733,11 @@
       <c r="GN153" s="3">
         <v>5</v>
       </c>
+      <c r="GO153" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:196" ht="15">
+    <row r="154" spans="1:197" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -84633,8 +84756,11 @@
       <c r="F154" s="13">
         <v>45838</v>
       </c>
+      <c r="GO154" s="3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="155" spans="1:196" ht="15">
+    <row r="155" spans="1:197" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -84653,8 +84779,11 @@
       <c r="F155" s="13">
         <v>45838</v>
       </c>
+      <c r="GO155" s="3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="156" spans="1:196" ht="15">
+    <row r="156" spans="1:197" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -84673,8 +84802,11 @@
       <c r="F156" s="13">
         <v>45838</v>
       </c>
+      <c r="GO156" s="3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="157" spans="1:196" ht="15">
+    <row r="157" spans="1:197" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -84705,8 +84837,11 @@
       <c r="GN157" s="3">
         <v>5</v>
       </c>
+      <c r="GO157" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="158" spans="1:196" ht="15">
+    <row r="158" spans="1:197" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -84721,6 +84856,173 @@
       </c>
       <c r="E158" s="9">
         <v>200</v>
+      </c>
+    </row>
+    <row r="159" spans="1:197" ht="15">
+      <c r="A159" s="9">
+        <v>23905761</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C159" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E159" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:197">
+      <c r="A160" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D160" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E160" s="9">
+        <v>1000</v>
+      </c>
+      <c r="F160" s="13">
+        <v>45828</v>
+      </c>
+      <c r="GE160" s="3">
+        <v>6</v>
+      </c>
+      <c r="GF160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GH160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GI160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GK160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GL160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GO160" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:197">
+      <c r="A161" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D161" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E161" s="9">
+        <v>1000</v>
+      </c>
+      <c r="F161" s="13">
+        <v>45829</v>
+      </c>
+      <c r="GE161" s="3">
+        <v>6</v>
+      </c>
+      <c r="GF161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GH161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GI161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GK161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GL161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GO161" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:197">
+      <c r="A162" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D162" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E162" s="9">
+        <v>1000</v>
+      </c>
+      <c r="F162" s="13">
+        <v>45830</v>
+      </c>
+      <c r="GE162" s="3">
+        <v>6</v>
+      </c>
+      <c r="GF162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GH162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GI162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GK162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GL162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GO162" s="3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-02 09:46:39
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1590" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{903C3C67-352F-4D0C-8FEE-EE078B622CBE}"/>
+  <xr:revisionPtr revIDLastSave="1685" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F312DE21-81A2-4FD4-8D8E-B23004CC262F}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="211">
   <si>
     <t>Module ID</t>
   </si>
@@ -305,7 +305,7 @@
     <t>VSL202425372</t>
   </si>
   <si>
-    <t>hold</t>
+    <t>end</t>
   </si>
   <si>
     <t>VSL202425381</t>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>QC SOLAR BLK DIODE 2.0</t>
+  </si>
+  <si>
+    <t>hold</t>
   </si>
   <si>
     <t>VSL202425377</t>
@@ -660,6 +663,12 @@
   </si>
   <si>
     <t>EPE+EPE HIB TAPE</t>
+  </si>
+  <si>
+    <t>LeTID</t>
+  </si>
+  <si>
+    <t>Sunsure HYPERSOL Internal Reliability Tests (DH1000+SML)</t>
   </si>
 </sst>
 </file>
@@ -1194,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD162"/>
+  <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GN155" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GO160" sqref="GO160:GO162"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GI171" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A133" sqref="A133"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73072,7 +73081,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:197" ht="15">
+    <row r="33" spans="1:198" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73221,7 +73230,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:197" ht="15">
+    <row r="34" spans="1:198" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73370,7 +73379,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:197" ht="15">
+    <row r="35" spans="1:198" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73519,7 +73528,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:197" ht="15">
+    <row r="36" spans="1:198" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73653,7 +73662,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:197" ht="15">
+    <row r="37" spans="1:198" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73787,7 +73796,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:197" ht="15">
+    <row r="38" spans="1:198" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73921,7 +73930,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:197" ht="15">
+    <row r="39" spans="1:198" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74084,7 +74093,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:197" ht="15">
+    <row r="40" spans="1:198" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74247,7 +74256,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:197" ht="15">
+    <row r="41" spans="1:198" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74410,7 +74419,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:197" ht="15">
+    <row r="42" spans="1:198" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74573,7 +74582,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:197" ht="15">
+    <row r="43" spans="1:198" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74736,7 +74745,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:197" ht="15">
+    <row r="44" spans="1:198" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74899,7 +74908,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:197" ht="15">
+    <row r="45" spans="1:198" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75062,7 +75071,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:197" ht="15">
+    <row r="46" spans="1:198" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75225,7 +75234,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:197" ht="15">
+    <row r="47" spans="1:198" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75405,8 +75414,11 @@
       <c r="GO47" s="3">
         <v>24</v>
       </c>
+      <c r="GP47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:197" ht="15">
+    <row r="48" spans="1:198" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75617,7 +75629,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:197" ht="15">
+    <row r="49" spans="1:198" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75797,8 +75809,11 @@
       <c r="GO49" s="3">
         <v>24</v>
       </c>
+      <c r="GP49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:197" ht="15">
+    <row r="50" spans="1:198" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -76009,7 +76024,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:197" ht="15">
+    <row r="51" spans="1:198" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76220,7 +76235,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:197" ht="15">
+    <row r="52" spans="1:198" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76431,7 +76446,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:197" ht="15">
+    <row r="53" spans="1:198" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76611,8 +76626,11 @@
       <c r="GO53" s="3">
         <v>24</v>
       </c>
+      <c r="GP53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:197" ht="15">
+    <row r="54" spans="1:198" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76792,8 +76810,11 @@
       <c r="GO54" s="3">
         <v>24</v>
       </c>
+      <c r="GP54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:197" ht="15">
+    <row r="55" spans="1:198" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -76986,7 +77007,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:197" ht="15">
+    <row r="56" spans="1:198" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77179,7 +77200,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:197" ht="15">
+    <row r="57" spans="1:198" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77336,7 +77357,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:197" ht="15">
+    <row r="58" spans="1:198" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77492,7 +77513,7 @@
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
     </row>
-    <row r="59" spans="1:197" ht="15">
+    <row r="59" spans="1:198" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77646,7 +77667,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:197" ht="15">
+    <row r="60" spans="1:198" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77792,7 +77813,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:197" ht="15">
+    <row r="61" spans="1:198" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -77950,7 +77971,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:197" ht="15">
+    <row r="62" spans="1:198" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -77968,6 +77989,9 @@
       </c>
       <c r="F62" s="12">
         <v>45773</v>
+      </c>
+      <c r="P62" s="13">
+        <v>45819</v>
       </c>
       <c r="AY62" s="1"/>
       <c r="AZ62" s="1"/>
@@ -78185,11 +78209,14 @@
       <c r="FT62" s="3">
         <v>24</v>
       </c>
-      <c r="FU62" s="3" t="s">
+      <c r="FU62" s="3">
+        <v>24</v>
+      </c>
+      <c r="FV62" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:197" ht="15">
+    <row r="63" spans="1:198" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78207,6 +78234,9 @@
       </c>
       <c r="F63" s="12">
         <v>45773</v>
+      </c>
+      <c r="P63" s="13">
+        <v>45819</v>
       </c>
       <c r="AY63" s="1"/>
       <c r="AZ63" s="1"/>
@@ -78424,11 +78454,14 @@
       <c r="FT63" s="3">
         <v>24</v>
       </c>
-      <c r="FU63" s="3" t="s">
+      <c r="FU63" s="3">
+        <v>24</v>
+      </c>
+      <c r="FV63" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:197" ht="15">
+    <row r="64" spans="1:198" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78446,6 +78479,9 @@
       </c>
       <c r="F64" s="12">
         <v>45773</v>
+      </c>
+      <c r="P64" s="13">
+        <v>45819</v>
       </c>
       <c r="AY64" s="1"/>
       <c r="AZ64" s="1"/>
@@ -78663,11 +78699,14 @@
       <c r="FT64" s="3">
         <v>24</v>
       </c>
-      <c r="FU64" s="3" t="s">
+      <c r="FU64" s="3">
+        <v>24</v>
+      </c>
+      <c r="FV64" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:197" ht="15">
+    <row r="65" spans="1:198" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78816,7 +78855,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:197" ht="15">
+    <row r="66" spans="1:198" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -78965,7 +79004,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:197" ht="15">
+    <row r="67" spans="1:198" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79104,7 +79143,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:197" ht="15">
+    <row r="68" spans="1:198" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79251,7 +79290,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:197" ht="15">
+    <row r="69" spans="1:198" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79385,7 +79424,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:197" ht="15">
+    <row r="70" spans="1:198" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79548,7 +79587,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:197" ht="15">
+    <row r="71" spans="1:198" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79695,7 +79734,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:197" ht="15">
+    <row r="72" spans="1:198" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79829,7 +79868,7 @@
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
     </row>
-    <row r="73" spans="1:197" ht="15">
+    <row r="73" spans="1:198" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80091,18 +80130,18 @@
         <v>5</v>
       </c>
       <c r="FV73" s="3" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:197" ht="15">
+    <row r="74" spans="1:198" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>28</v>
@@ -80356,21 +80395,21 @@
         <v>5</v>
       </c>
       <c r="FV74" s="3" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:197" ht="15">
+    <row r="75" spans="1:198" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E75" s="8">
         <v>96</v>
@@ -80493,15 +80532,15 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:197" ht="15">
+    <row r="76" spans="1:198" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>18</v>
@@ -80627,18 +80666,18 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:197" ht="15">
+    <row r="77" spans="1:198" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E77" s="8">
         <v>162</v>
@@ -80761,15 +80800,15 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:197" ht="15">
+    <row r="78" spans="1:198" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>28</v>
@@ -81019,16 +81058,19 @@
       <c r="GO78" s="3">
         <v>24</v>
       </c>
+      <c r="GP78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:197" ht="15">
+    <row r="79" spans="1:198" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
       <c r="B79" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>28</v>
@@ -81154,15 +81196,15 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:197" ht="15">
+    <row r="80" spans="1:198" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>21</v>
@@ -81343,15 +81385,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:197" ht="15">
+    <row r="81" spans="1:198" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>18</v>
@@ -81384,15 +81426,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:197" ht="15">
+    <row r="82" spans="1:198" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>28</v>
@@ -81502,16 +81544,19 @@
       <c r="GO82" s="3">
         <v>24</v>
       </c>
+      <c r="GP82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:197" ht="15">
+    <row r="83" spans="1:198" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>18</v>
@@ -81544,15 +81589,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:197" ht="15">
+    <row r="84" spans="1:198" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
       <c r="B84" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>32</v>
@@ -81603,18 +81648,18 @@
         <v>5</v>
       </c>
       <c r="GJ84" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:197" ht="15">
+    <row r="85" spans="1:198" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>21</v>
@@ -81698,18 +81743,18 @@
         <v>208</v>
       </c>
       <c r="FR85" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:197" ht="15">
+    <row r="86" spans="1:198" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>18</v>
@@ -81721,7 +81766,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:197" ht="15">
+    <row r="87" spans="1:198" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81739,7 +81784,7 @@
       </c>
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="1:197" ht="15">
+    <row r="88" spans="1:198" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81757,15 +81802,15 @@
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:197" ht="15">
+    <row r="89" spans="1:198" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>32</v>
@@ -81816,15 +81861,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:197" ht="15">
+    <row r="90" spans="1:198" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>32</v>
@@ -81875,15 +81920,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:197" ht="15">
+    <row r="91" spans="1:198" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
       <c r="B91" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C91" s="17" t="s">
         <v>127</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>126</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>32</v>
@@ -81934,15 +81979,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:197" ht="15">
+    <row r="92" spans="1:198" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>32</v>
@@ -81993,15 +82038,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:197" ht="15">
+    <row r="93" spans="1:198" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>32</v>
@@ -82052,15 +82097,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:197" ht="15">
+    <row r="94" spans="1:198" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>21</v>
@@ -82108,15 +82153,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:197" ht="15">
+    <row r="95" spans="1:198" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>28</v>
@@ -82172,16 +82217,19 @@
       <c r="GO95" s="3">
         <v>24</v>
       </c>
+      <c r="GP95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:197" ht="15">
+    <row r="96" spans="1:198" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>18</v>
@@ -82211,18 +82259,18 @@
         <v>19</v>
       </c>
       <c r="GB96" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:197" ht="15">
+    <row r="97" spans="1:198" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>18</v>
@@ -82252,18 +82300,18 @@
         <v>19</v>
       </c>
       <c r="GB97" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:197" ht="15">
+    <row r="98" spans="1:198" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
       <c r="B98" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C98" s="17" t="s">
         <v>127</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>126</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>28</v>
@@ -82331,16 +82379,19 @@
       <c r="GO98" s="3">
         <v>24</v>
       </c>
+      <c r="GP98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:197" ht="15">
+    <row r="99" spans="1:198" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>28</v>
@@ -82352,15 +82403,15 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:197" ht="15">
+    <row r="100" spans="1:198" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>18</v>
@@ -82390,18 +82441,18 @@
         <v>17</v>
       </c>
       <c r="GF100" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:197" ht="15">
+    <row r="101" spans="1:198" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>18</v>
@@ -82434,15 +82485,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:197" ht="15">
+    <row r="102" spans="1:198" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
       <c r="B102" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C102" s="17" t="s">
         <v>136</v>
-      </c>
-      <c r="C102" s="17" t="s">
-        <v>135</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>18</v>
@@ -82475,15 +82526,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:197" ht="15">
+    <row r="103" spans="1:198" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>18</v>
@@ -82516,15 +82567,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:197" ht="15">
+    <row r="104" spans="1:198" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>18</v>
@@ -82557,15 +82608,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:197" ht="15">
+    <row r="105" spans="1:198" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>32</v>
@@ -82613,18 +82664,18 @@
         <v>5</v>
       </c>
       <c r="GJ105" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:197" ht="15">
+    <row r="106" spans="1:198" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
       <c r="B106" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C106" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="C106" s="17" t="s">
-        <v>140</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>18</v>
@@ -82654,18 +82705,18 @@
         <v>19</v>
       </c>
       <c r="GB106" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:197" ht="15">
+    <row r="107" spans="1:198" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>28</v>
@@ -82733,16 +82784,19 @@
       <c r="GO107" s="3">
         <v>24</v>
       </c>
+      <c r="GP107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:197" ht="15">
+    <row r="108" spans="1:198" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>32</v>
@@ -82793,18 +82847,18 @@
         <v>5</v>
       </c>
       <c r="GJ108" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:197" ht="15">
+    <row r="109" spans="1:198" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>32</v>
@@ -82813,18 +82867,18 @@
         <v>60</v>
       </c>
       <c r="F109" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:197" ht="15">
+    <row r="110" spans="1:198" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>18</v>
@@ -82898,16 +82952,19 @@
       <c r="GO110" s="3">
         <v>24</v>
       </c>
+      <c r="GP110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:197" ht="15">
+    <row r="111" spans="1:198" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C111" s="17" t="s">
         <v>148</v>
-      </c>
-      <c r="C111" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>18</v>
@@ -82943,18 +83000,18 @@
         <v>10</v>
       </c>
       <c r="GB111" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:197" ht="15">
+    <row r="112" spans="1:198" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>32</v>
@@ -83011,18 +83068,18 @@
         <v>5</v>
       </c>
       <c r="GI112" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:197" ht="15">
+    <row r="113" spans="1:198" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>18</v>
@@ -83058,18 +83115,18 @@
         <v>10</v>
       </c>
       <c r="GB113" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:197" ht="15">
+    <row r="114" spans="1:198" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>21</v>
@@ -83143,16 +83200,19 @@
       <c r="GO114" s="3">
         <v>16</v>
       </c>
+      <c r="GP114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:197" ht="15">
+    <row r="115" spans="1:198" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>28</v>
@@ -83226,16 +83286,19 @@
       <c r="GO115" s="3">
         <v>24</v>
       </c>
+      <c r="GP115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:197" ht="15">
+    <row r="116" spans="1:198" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>28</v>
@@ -83312,16 +83375,19 @@
       <c r="GO116" s="3">
         <v>24</v>
       </c>
+      <c r="GP116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:197" ht="15">
+    <row r="117" spans="1:198" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>32</v>
@@ -83378,18 +83444,18 @@
         <v>5</v>
       </c>
       <c r="GI117" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:197" ht="15">
+    <row r="118" spans="1:198" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>32</v>
@@ -83449,18 +83515,18 @@
         <v>5</v>
       </c>
       <c r="GI118" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:197" ht="15">
+    <row r="119" spans="1:198" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>32</v>
@@ -83520,18 +83586,18 @@
         <v>5</v>
       </c>
       <c r="GI119" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:197" ht="15">
+    <row r="120" spans="1:198" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C120" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>32</v>
@@ -83591,18 +83657,18 @@
         <v>5</v>
       </c>
       <c r="GI120" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:197" ht="15">
+    <row r="121" spans="1:198" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C121" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>18</v>
@@ -83632,18 +83698,18 @@
         <v>17</v>
       </c>
       <c r="GF121" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:197" ht="15">
+    <row r="122" spans="1:198" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C122" s="17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>25</v>
@@ -83691,18 +83757,18 @@
         <v>24</v>
       </c>
       <c r="GH122" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:197" ht="15">
+    <row r="123" spans="1:198" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C123" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>32</v>
@@ -83740,16 +83806,19 @@
       <c r="GO123" s="3">
         <v>5</v>
       </c>
+      <c r="GP123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:197" ht="15">
+    <row r="124" spans="1:198" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
       <c r="B124" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C124" s="17" t="s">
         <v>162</v>
-      </c>
-      <c r="C124" s="17" t="s">
-        <v>161</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>18</v>
@@ -83779,18 +83848,18 @@
         <v>19</v>
       </c>
       <c r="GJ124" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:197" ht="15">
+    <row r="125" spans="1:198" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C125" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>28</v>
@@ -83834,16 +83903,19 @@
       <c r="GO125" s="3">
         <v>24</v>
       </c>
+      <c r="GP125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:197" ht="15">
+    <row r="126" spans="1:198" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C126" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>18</v>
@@ -83873,18 +83945,18 @@
         <v>14</v>
       </c>
       <c r="GD126" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:197" ht="15">
+    <row r="127" spans="1:198" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C127" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>18</v>
@@ -83914,18 +83986,18 @@
         <v>14</v>
       </c>
       <c r="GD127" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:197" ht="15">
+    <row r="128" spans="1:198" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>18</v>
@@ -83955,18 +84027,18 @@
         <v>14</v>
       </c>
       <c r="GD128" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:197" ht="15">
+    <row r="129" spans="1:198" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>18</v>
@@ -83996,18 +84068,18 @@
         <v>14</v>
       </c>
       <c r="GD129" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:197" ht="15">
+    <row r="130" spans="1:198" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D130" s="9" t="s">
         <v>25</v>
@@ -84052,18 +84124,18 @@
         <v>24</v>
       </c>
       <c r="GN130" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:197" ht="15">
+    <row r="131" spans="1:198" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D131" s="9" t="s">
         <v>28</v>
@@ -84098,16 +84170,19 @@
       <c r="GO131" s="3">
         <v>24</v>
       </c>
+      <c r="GP131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:197" ht="15">
+    <row r="132" spans="1:198" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
       <c r="B132" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>28</v>
@@ -84142,16 +84217,19 @@
       <c r="GO132" s="3">
         <v>24</v>
       </c>
+      <c r="GP132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:197" ht="15">
+    <row r="133" spans="1:198" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>28</v>
@@ -84160,15 +84238,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="134" spans="1:197" ht="15">
+    <row r="134" spans="1:198" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D134" s="9" t="s">
         <v>28</v>
@@ -84177,15 +84255,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:197" ht="15">
+    <row r="135" spans="1:198" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D135" s="9" t="s">
         <v>32</v>
@@ -84193,16 +84271,22 @@
       <c r="E135" s="9">
         <v>60</v>
       </c>
+      <c r="F135" s="13">
+        <v>45839</v>
+      </c>
+      <c r="GP135" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="136" spans="1:197" ht="15">
+    <row r="136" spans="1:198" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
       <c r="B136" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C136" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="D136" s="9" t="s">
         <v>18</v>
@@ -84211,15 +84295,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:197" ht="15">
+    <row r="137" spans="1:198" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D137" s="9" t="s">
         <v>28</v>
@@ -84228,12 +84312,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="138" spans="1:197" ht="15">
+    <row r="138" spans="1:198" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>86</v>
@@ -84248,12 +84332,12 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="139" spans="1:197" ht="15">
+    <row r="139" spans="1:198" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>86</v>
@@ -84268,12 +84352,12 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="140" spans="1:197" ht="15">
+    <row r="140" spans="1:198" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>86</v>
@@ -84288,12 +84372,12 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="141" spans="1:197" ht="15">
+    <row r="141" spans="1:198" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>86</v>
@@ -84308,15 +84392,15 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="142" spans="1:197" ht="15">
+    <row r="142" spans="1:198" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C142" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D142" s="9" t="s">
         <v>32</v>
@@ -84345,16 +84429,19 @@
       <c r="GO142" s="3">
         <v>5</v>
       </c>
+      <c r="GP142" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="143" spans="1:197" ht="15">
+    <row r="143" spans="1:198" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
       <c r="B143" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C143" s="17" t="s">
         <v>185</v>
-      </c>
-      <c r="C143" s="17" t="s">
-        <v>184</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>18</v>
@@ -84383,16 +84470,19 @@
       <c r="GO143" s="3">
         <v>24</v>
       </c>
+      <c r="GP143" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="144" spans="1:197" ht="15">
+    <row r="144" spans="1:198" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C144" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D144" s="9" t="s">
         <v>32</v>
@@ -84421,16 +84511,19 @@
       <c r="GO144" s="3">
         <v>5</v>
       </c>
+      <c r="GP144" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="145" spans="1:197" ht="15">
+    <row r="145" spans="1:198" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C145" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D145" s="9" t="s">
         <v>32</v>
@@ -84459,16 +84552,19 @@
       <c r="GO145" s="3">
         <v>5</v>
       </c>
+      <c r="GP145" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="146" spans="1:197" ht="15">
+    <row r="146" spans="1:198" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C146" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D146" s="9" t="s">
         <v>18</v>
@@ -84497,16 +84593,19 @@
       <c r="GO146" s="3">
         <v>24</v>
       </c>
+      <c r="GP146" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="147" spans="1:197" ht="15">
+    <row r="147" spans="1:198" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C147" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D147" s="9" t="s">
         <v>32</v>
@@ -84535,16 +84634,19 @@
       <c r="GO147" s="3">
         <v>5</v>
       </c>
+      <c r="GP147" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:197" ht="15">
+    <row r="148" spans="1:198" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C148" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D148" s="9" t="s">
         <v>18</v>
@@ -84573,16 +84675,19 @@
       <c r="GO148" s="3">
         <v>24</v>
       </c>
+      <c r="GP148" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="149" spans="1:197" ht="15">
+    <row r="149" spans="1:198" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C149" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>32</v>
@@ -84608,16 +84713,19 @@
       <c r="GO149" s="3">
         <v>5</v>
       </c>
+      <c r="GP149" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="150" spans="1:197" ht="15">
+    <row r="150" spans="1:198" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C150" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D150" s="9" t="s">
         <v>18</v>
@@ -84646,16 +84754,19 @@
       <c r="GO150" s="3">
         <v>24</v>
       </c>
+      <c r="GP150" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="151" spans="1:197" ht="15">
+    <row r="151" spans="1:198" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C151" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D151" s="9" t="s">
         <v>18</v>
@@ -84667,15 +84778,15 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="152" spans="1:197" ht="15">
+    <row r="152" spans="1:198" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C152" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D152" s="9" t="s">
         <v>32</v>
@@ -84701,16 +84812,19 @@
       <c r="GO152" s="3">
         <v>5</v>
       </c>
+      <c r="GP152" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:197" ht="15">
+    <row r="153" spans="1:198" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C153" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D153" s="9" t="s">
         <v>32</v>
@@ -84736,16 +84850,19 @@
       <c r="GO153" s="3">
         <v>5</v>
       </c>
+      <c r="GP153" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:197" ht="15">
+    <row r="154" spans="1:198" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C154" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D154" s="9" t="s">
         <v>18</v>
@@ -84759,16 +84876,19 @@
       <c r="GO154" s="3">
         <v>10</v>
       </c>
+      <c r="GP154" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="155" spans="1:197" ht="15">
+    <row r="155" spans="1:198" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C155" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D155" s="9" t="s">
         <v>18</v>
@@ -84782,16 +84902,19 @@
       <c r="GO155" s="3">
         <v>10</v>
       </c>
+      <c r="GP155" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="156" spans="1:197" ht="15">
+    <row r="156" spans="1:198" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C156" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D156" s="9" t="s">
         <v>18</v>
@@ -84805,16 +84928,19 @@
       <c r="GO156" s="3">
         <v>10</v>
       </c>
+      <c r="GP156" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="157" spans="1:197" ht="15">
+    <row r="157" spans="1:198" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C157" s="17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D157" s="9" t="s">
         <v>32</v>
@@ -84840,16 +84966,19 @@
       <c r="GO157" s="3">
         <v>5</v>
       </c>
+      <c r="GP157" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="158" spans="1:197" ht="15">
+    <row r="158" spans="1:198" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C158" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D158" s="9" t="s">
         <v>21</v>
@@ -84858,15 +84987,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:197" ht="15">
+    <row r="159" spans="1:198" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C159" s="17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>28</v>
@@ -84875,12 +85004,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:197">
+    <row r="160" spans="1:198">
       <c r="A160" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D160" s="9" t="s">
         <v>28</v>
@@ -84924,13 +85053,16 @@
       <c r="GO160" s="3">
         <v>12</v>
       </c>
+      <c r="GP160" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="161" spans="1:197">
+    <row r="161" spans="1:198">
       <c r="A161" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D161" s="9" t="s">
         <v>28</v>
@@ -84974,13 +85106,16 @@
       <c r="GO161" s="3">
         <v>12</v>
       </c>
+      <c r="GP161" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="162" spans="1:197">
+    <row r="162" spans="1:198">
       <c r="A162" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D162" s="9" t="s">
         <v>28</v>
@@ -85023,6 +85158,331 @@
       </c>
       <c r="GO162" s="3">
         <v>12</v>
+      </c>
+      <c r="GP162" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="163" spans="1:198" ht="15">
+      <c r="A163" s="9">
+        <v>25386587</v>
+      </c>
+      <c r="C163" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D163" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E163" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="164" spans="1:198" ht="15">
+      <c r="A164" s="9">
+        <v>25386594</v>
+      </c>
+      <c r="C164" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D164" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E164" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="165" spans="1:198" ht="15">
+      <c r="A165" s="9">
+        <v>25386583</v>
+      </c>
+      <c r="C165" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D165" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E165" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:198" ht="15">
+      <c r="A166" s="9">
+        <v>25386578</v>
+      </c>
+      <c r="C166" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D166" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E166" s="9">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="167" spans="1:198" ht="15">
+      <c r="A167" s="9">
+        <v>25386240</v>
+      </c>
+      <c r="C167" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D167" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E167" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="1:198" ht="15">
+      <c r="A168" s="9">
+        <v>25385829</v>
+      </c>
+      <c r="C168" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D168" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E168" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="169" spans="1:198" ht="15">
+      <c r="A169" s="9">
+        <v>25386238</v>
+      </c>
+      <c r="C169" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D169" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E169" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="170" spans="1:198" ht="15">
+      <c r="A170" s="9">
+        <v>25386229</v>
+      </c>
+      <c r="C170" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D170" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E170" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="171" spans="1:198" ht="15">
+      <c r="A171" s="9">
+        <v>25385835</v>
+      </c>
+      <c r="C171" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D171" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E171" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="172" spans="1:198" ht="15">
+      <c r="A172" s="9">
+        <v>25386639</v>
+      </c>
+      <c r="C172" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D172" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E172" s="9">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="173" spans="1:198" ht="15">
+      <c r="A173" s="9">
+        <v>25386618</v>
+      </c>
+      <c r="C173" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D173" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E173" s="9">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="174" spans="1:198" ht="15">
+      <c r="A174" s="9">
+        <v>25386256</v>
+      </c>
+      <c r="C174" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D174" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E174" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="175" spans="1:198" ht="15">
+      <c r="A175" s="9">
+        <v>25385821</v>
+      </c>
+      <c r="C175" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D175" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E175" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="176" spans="1:198" ht="15">
+      <c r="A176" s="9">
+        <v>25386577</v>
+      </c>
+      <c r="C176" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D176" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E176" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="15">
+      <c r="A177" s="9">
+        <v>25386584</v>
+      </c>
+      <c r="C177" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D177" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E177" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="15">
+      <c r="A178" s="9">
+        <v>25386617</v>
+      </c>
+      <c r="C178" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D178" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E178" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="15">
+      <c r="A179" s="9">
+        <v>25386605</v>
+      </c>
+      <c r="C179" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D179" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E179" s="9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="15">
+      <c r="A180" s="9">
+        <v>25438399</v>
+      </c>
+      <c r="C180" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D180" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E180" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="15">
+      <c r="A181" s="9">
+        <v>25438419</v>
+      </c>
+      <c r="C181" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D181" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E181" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="15">
+      <c r="A182" s="9">
+        <v>25445298</v>
+      </c>
+      <c r="C182" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D182" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E182" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="15">
+      <c r="A183" s="9">
+        <v>25438056</v>
+      </c>
+      <c r="C183" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D183" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E183" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="15">
+      <c r="A184" s="9">
+        <v>25438634</v>
+      </c>
+      <c r="C184" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D184" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E184" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" ht="15">
+      <c r="A185" s="9">
+        <v>25442344</v>
+      </c>
+      <c r="C185" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D185" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E185" s="9">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-02 13:50:10
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1685" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F312DE21-81A2-4FD4-8D8E-B23004CC262F}"/>
+  <xr:revisionPtr revIDLastSave="1689" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BE20C41-24F1-424E-8157-DB93855922DF}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1206,8 +1206,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GI171" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A133" sqref="A133"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GL132" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GP138" sqref="GP138"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -84237,6 +84237,9 @@
       <c r="E133" s="9">
         <v>1000</v>
       </c>
+      <c r="F133" s="13">
+        <v>45840</v>
+      </c>
     </row>
     <row r="134" spans="1:198" ht="15">
       <c r="A134" s="9">
@@ -84254,6 +84257,9 @@
       <c r="E134" s="9">
         <v>1000</v>
       </c>
+      <c r="F134" s="13">
+        <v>45840</v>
+      </c>
     </row>
     <row r="135" spans="1:198" ht="15">
       <c r="A135" s="9">
@@ -84294,6 +84300,9 @@
       <c r="E136" s="9">
         <v>96</v>
       </c>
+      <c r="F136" s="13">
+        <v>45840</v>
+      </c>
     </row>
     <row r="137" spans="1:198" ht="15">
       <c r="A137" s="9">
@@ -84310,6 +84319,9 @@
       </c>
       <c r="E137" s="9">
         <v>1000</v>
+      </c>
+      <c r="F137" s="13">
+        <v>45840</v>
       </c>
     </row>
     <row r="138" spans="1:198" ht="15">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-03 09:46:08
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29101"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1689" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BE20C41-24F1-424E-8157-DB93855922DF}"/>
+  <xr:revisionPtr revIDLastSave="1759" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C007A444-B5ED-42FF-919B-673540C6CAE0}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="213">
   <si>
     <t>Module ID</t>
   </si>
@@ -293,6 +293,9 @@
     <t>M10R HYPERSOL (ENERPARC)</t>
   </si>
   <si>
+    <t>end</t>
+  </si>
+  <si>
     <t>VSL202425369</t>
   </si>
   <si>
@@ -303,9 +306,6 @@
   </si>
   <si>
     <t>VSL202425372</t>
-  </si>
-  <si>
-    <t>end</t>
   </si>
   <si>
     <t>VSL202425381</t>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>SemCorp G2B Module Failure Analysis</t>
+  </si>
+  <si>
+    <t>DMEGC M10R Hypersol cell trial (2nd time)</t>
+  </si>
+  <si>
+    <t>Tongwei M10R Hypersol cell trial (2nd time)</t>
   </si>
   <si>
     <t>VSL202526030</t>
@@ -647,19 +653,19 @@
     <t>Ronma TOPCon Cell Trial</t>
   </si>
   <si>
-    <t>SAMPLE-1</t>
+    <t>HJT SAMPLE-1</t>
   </si>
   <si>
     <t>EPE+EPE</t>
   </si>
   <si>
-    <t>SAMPLE-2</t>
+    <t>HJT SAMPLE-2</t>
   </si>
   <si>
     <t>EPE+EPE+40MM POE</t>
   </si>
   <si>
-    <t>SAMPLE-3</t>
+    <t>HJT SAMPLE-3</t>
   </si>
   <si>
     <t>EPE+EPE HIB TAPE</t>
@@ -1206,8 +1212,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GL132" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GP138" sqref="GP138"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GR47" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73081,7 +73087,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:198" ht="15">
+    <row r="33" spans="1:199" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73230,7 +73236,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:198" ht="15">
+    <row r="34" spans="1:199" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73379,7 +73385,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:198" ht="15">
+    <row r="35" spans="1:199" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73528,7 +73534,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:198" ht="15">
+    <row r="36" spans="1:199" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73662,7 +73668,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:198" ht="15">
+    <row r="37" spans="1:199" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73796,7 +73802,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:198" ht="15">
+    <row r="38" spans="1:199" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73930,7 +73936,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:198" ht="15">
+    <row r="39" spans="1:199" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74093,7 +74099,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:198" ht="15">
+    <row r="40" spans="1:199" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74256,7 +74262,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:198" ht="15">
+    <row r="41" spans="1:199" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74419,7 +74425,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:198" ht="15">
+    <row r="42" spans="1:199" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74582,7 +74588,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:198" ht="15">
+    <row r="43" spans="1:199" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74745,7 +74751,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:198" ht="15">
+    <row r="44" spans="1:199" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74908,7 +74914,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:198" ht="15">
+    <row r="45" spans="1:199" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75071,7 +75077,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:198" ht="15">
+    <row r="46" spans="1:199" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75234,7 +75240,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:198" ht="15">
+    <row r="47" spans="1:199" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75417,8 +75423,11 @@
       <c r="GP47" s="3">
         <v>24</v>
       </c>
+      <c r="GQ47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:198" ht="15">
+    <row r="48" spans="1:199" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75629,7 +75638,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:198" ht="15">
+    <row r="49" spans="1:207" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75812,8 +75821,11 @@
       <c r="GP49" s="3">
         <v>24</v>
       </c>
+      <c r="GQ49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:198" ht="15">
+    <row r="50" spans="1:207" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -76024,7 +76036,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:198" ht="15">
+    <row r="51" spans="1:207" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76235,7 +76247,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:198" ht="15">
+    <row r="52" spans="1:207" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76446,7 +76458,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:198" ht="15">
+    <row r="53" spans="1:207" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76629,8 +76641,11 @@
       <c r="GP53" s="3">
         <v>24</v>
       </c>
+      <c r="GQ53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:198" ht="15">
+    <row r="54" spans="1:207" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76813,8 +76828,11 @@
       <c r="GP54" s="3">
         <v>24</v>
       </c>
+      <c r="GQ54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:198" ht="15">
+    <row r="55" spans="1:207" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -77007,7 +77025,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:198" ht="15">
+    <row r="56" spans="1:207" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77200,7 +77218,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:198" ht="15">
+    <row r="57" spans="1:207" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77357,7 +77375,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:198" ht="15">
+    <row r="58" spans="1:207" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77375,6 +77393,9 @@
       </c>
       <c r="F58" s="12">
         <v>45749</v>
+      </c>
+      <c r="P58" s="13">
+        <v>45847</v>
       </c>
       <c r="AY58" s="1"/>
       <c r="AZ58" s="1"/>
@@ -77512,16 +77533,22 @@
       <c r="FH58" s="1"/>
       <c r="FI58" s="1"/>
       <c r="FJ58" s="1"/>
+      <c r="GX58" s="3">
+        <v>126</v>
+      </c>
+      <c r="GY58" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="59" spans="1:198" ht="15">
+    <row r="59" spans="1:207" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>28</v>
@@ -77667,15 +77694,15 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:198" ht="15">
+    <row r="60" spans="1:207" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>18</v>
@@ -77813,15 +77840,15 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:198" ht="15">
+    <row r="61" spans="1:207" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>21</v>
@@ -77971,7 +77998,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:198" ht="15">
+    <row r="62" spans="1:207" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78213,10 +78240,10 @@
         <v>24</v>
       </c>
       <c r="FV62" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:198" ht="15">
+    <row r="63" spans="1:207" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78458,10 +78485,10 @@
         <v>24</v>
       </c>
       <c r="FV63" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:198" ht="15">
+    <row r="64" spans="1:207" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78703,10 +78730,10 @@
         <v>24</v>
       </c>
       <c r="FV64" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:198" ht="15">
+    <row r="65" spans="1:199" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78855,7 +78882,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:198" ht="15">
+    <row r="66" spans="1:199" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79004,7 +79031,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:198" ht="15">
+    <row r="67" spans="1:199" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79143,7 +79170,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:198" ht="15">
+    <row r="68" spans="1:199" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79290,7 +79317,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:198" ht="15">
+    <row r="69" spans="1:199" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79306,7 +79333,9 @@
       <c r="E69" s="8">
         <v>1000</v>
       </c>
-      <c r="F69" s="12"/>
+      <c r="F69" s="12">
+        <v>45840</v>
+      </c>
       <c r="AY69" s="1"/>
       <c r="AZ69" s="1"/>
       <c r="BA69" s="1"/>
@@ -79424,7 +79453,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:198" ht="15">
+    <row r="70" spans="1:199" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79586,8 +79615,11 @@
       <c r="FH70" s="1"/>
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
+      <c r="GQ70" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="71" spans="1:198" ht="15">
+    <row r="71" spans="1:199" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79734,7 +79766,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:198" ht="15">
+    <row r="72" spans="1:199" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79750,7 +79782,9 @@
       <c r="E72" s="8">
         <v>1000</v>
       </c>
-      <c r="F72" s="12"/>
+      <c r="F72" s="12">
+        <v>45840</v>
+      </c>
       <c r="AY72" s="1"/>
       <c r="AZ72" s="1"/>
       <c r="BA72" s="1"/>
@@ -79867,8 +79901,11 @@
       <c r="FH72" s="1"/>
       <c r="FI72" s="1"/>
       <c r="FJ72" s="1"/>
+      <c r="GQ72" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="73" spans="1:198" ht="15">
+    <row r="73" spans="1:199" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80133,7 +80170,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:198" ht="15">
+    <row r="74" spans="1:199" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80398,7 +80435,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:198" ht="15">
+    <row r="75" spans="1:199" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80532,7 +80569,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:198" ht="15">
+    <row r="76" spans="1:199" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80666,7 +80703,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:198" ht="15">
+    <row r="77" spans="1:199" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80800,7 +80837,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:198" ht="15">
+    <row r="78" spans="1:199" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81061,8 +81098,11 @@
       <c r="GP78" s="3">
         <v>24</v>
       </c>
+      <c r="GQ78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:198" ht="15">
+    <row r="79" spans="1:199" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81196,7 +81236,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:198" ht="15">
+    <row r="80" spans="1:199" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81385,7 +81425,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:198" ht="15">
+    <row r="81" spans="1:199" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81426,7 +81466,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:198" ht="15">
+    <row r="82" spans="1:199" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81547,8 +81587,11 @@
       <c r="GP82" s="3">
         <v>24</v>
       </c>
+      <c r="GQ82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:198" ht="15">
+    <row r="83" spans="1:199" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81589,7 +81632,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:198" ht="15">
+    <row r="84" spans="1:199" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81651,7 +81694,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:198" ht="15">
+    <row r="85" spans="1:199" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81746,7 +81789,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:198" ht="15">
+    <row r="86" spans="1:199" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81766,7 +81809,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:198" ht="15">
+    <row r="87" spans="1:199" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81774,7 +81817,7 @@
         <v>96</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>18</v>
@@ -81782,9 +81825,14 @@
       <c r="E87" s="15">
         <v>96</v>
       </c>
-      <c r="F87" s="18"/>
+      <c r="F87" s="18">
+        <v>45840</v>
+      </c>
+      <c r="GQ87" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="88" spans="1:198" ht="15">
+    <row r="88" spans="1:199" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81792,7 +81840,7 @@
         <v>92</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>18</v>
@@ -81800,17 +81848,22 @@
       <c r="E88" s="15">
         <v>96</v>
       </c>
-      <c r="F88" s="18"/>
+      <c r="F88" s="18">
+        <v>45840</v>
+      </c>
+      <c r="GQ88" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="89" spans="1:198" ht="15">
+    <row r="89" spans="1:199" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>32</v>
@@ -81861,15 +81914,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:198" ht="15">
+    <row r="90" spans="1:199" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>32</v>
@@ -81920,15 +81973,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:198" ht="15">
+    <row r="91" spans="1:199" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>32</v>
@@ -81979,15 +82032,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:198" ht="15">
+    <row r="92" spans="1:199" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>32</v>
@@ -82038,12 +82091,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:198" ht="15">
+    <row r="93" spans="1:199" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C93" s="17" t="s">
         <v>116</v>
@@ -82097,15 +82150,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:198" ht="15">
+    <row r="94" spans="1:199" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>21</v>
@@ -82153,15 +82206,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:198" ht="15">
+    <row r="95" spans="1:199" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D95" s="15" t="s">
         <v>28</v>
@@ -82220,16 +82273,19 @@
       <c r="GP95" s="3">
         <v>24</v>
       </c>
+      <c r="GQ95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:198" ht="15">
+    <row r="96" spans="1:199" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>18</v>
@@ -82262,15 +82318,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:198" ht="15">
+    <row r="97" spans="1:199" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>18</v>
@@ -82303,15 +82359,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:198" ht="15">
+    <row r="98" spans="1:199" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D98" s="15" t="s">
         <v>28</v>
@@ -82382,16 +82438,19 @@
       <c r="GP98" s="3">
         <v>24</v>
       </c>
+      <c r="GQ98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:198" ht="15">
+    <row r="99" spans="1:199" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D99" s="15" t="s">
         <v>28</v>
@@ -82403,7 +82462,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:198" ht="15">
+    <row r="100" spans="1:199" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82444,15 +82503,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:198" ht="15">
+    <row r="101" spans="1:199" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>18</v>
@@ -82485,15 +82544,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:198" ht="15">
+    <row r="102" spans="1:199" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>18</v>
@@ -82526,15 +82585,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:198" ht="15">
+    <row r="103" spans="1:199" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
       <c r="B103" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C103" s="17" t="s">
         <v>138</v>
-      </c>
-      <c r="C103" s="17" t="s">
-        <v>136</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>18</v>
@@ -82567,15 +82626,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:198" ht="15">
+    <row r="104" spans="1:199" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>18</v>
@@ -82608,15 +82667,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:198" ht="15">
+    <row r="105" spans="1:199" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>32</v>
@@ -82667,15 +82726,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:198" ht="15">
+    <row r="106" spans="1:199" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>18</v>
@@ -82708,15 +82767,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:198" ht="15">
+    <row r="107" spans="1:199" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
       <c r="B107" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C107" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="C107" s="17" t="s">
-        <v>141</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>28</v>
@@ -82787,16 +82846,19 @@
       <c r="GP107" s="3">
         <v>24</v>
       </c>
+      <c r="GQ107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:198" ht="15">
+    <row r="108" spans="1:199" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>32</v>
@@ -82850,15 +82912,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:198" ht="15">
+    <row r="109" spans="1:199" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>32</v>
@@ -82867,18 +82929,18 @@
         <v>60</v>
       </c>
       <c r="F109" s="13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:198" ht="15">
+    <row r="110" spans="1:199" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>18</v>
@@ -82955,16 +83017,19 @@
       <c r="GP110" s="3">
         <v>24</v>
       </c>
+      <c r="GQ110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:198" ht="15">
+    <row r="111" spans="1:199" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>18</v>
@@ -83003,15 +83068,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:198" ht="15">
+    <row r="112" spans="1:199" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
       <c r="B112" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C112" s="17" t="s">
         <v>150</v>
-      </c>
-      <c r="C112" s="17" t="s">
-        <v>148</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>32</v>
@@ -83071,15 +83136,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:198" ht="15">
+    <row r="113" spans="1:199" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>18</v>
@@ -83118,15 +83183,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:198" ht="15">
+    <row r="114" spans="1:199" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C114" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>21</v>
@@ -83203,16 +83268,19 @@
       <c r="GP114" s="3">
         <v>16</v>
       </c>
+      <c r="GQ114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:198" ht="15">
+    <row r="115" spans="1:199" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C115" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>28</v>
@@ -83289,16 +83357,19 @@
       <c r="GP115" s="3">
         <v>24</v>
       </c>
+      <c r="GQ115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:198" ht="15">
+    <row r="116" spans="1:199" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C116" s="17" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>28</v>
@@ -83378,16 +83449,19 @@
       <c r="GP116" s="3">
         <v>24</v>
       </c>
+      <c r="GQ116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:198" ht="15">
+    <row r="117" spans="1:199" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C117" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>32</v>
@@ -83447,15 +83521,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:198" ht="15">
+    <row r="118" spans="1:199" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C118" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>32</v>
@@ -83518,15 +83592,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:198" ht="15">
+    <row r="119" spans="1:199" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C119" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>32</v>
@@ -83589,15 +83663,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:198" ht="15">
+    <row r="120" spans="1:199" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C120" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>32</v>
@@ -83660,7 +83734,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:198" ht="15">
+    <row r="121" spans="1:199" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83668,7 +83742,7 @@
         <v>117</v>
       </c>
       <c r="C121" s="17" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>18</v>
@@ -83701,15 +83775,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:198" ht="15">
+    <row r="122" spans="1:199" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C122" s="17" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>25</v>
@@ -83760,15 +83834,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:198" ht="15">
+    <row r="123" spans="1:199" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C123" s="17" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>32</v>
@@ -83809,16 +83883,19 @@
       <c r="GP123" s="3">
         <v>5</v>
       </c>
+      <c r="GQ123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:198" ht="15">
+    <row r="124" spans="1:199" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C124" s="17" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>18</v>
@@ -83851,15 +83928,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:198" ht="15">
+    <row r="125" spans="1:199" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
       <c r="B125" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C125" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="C125" s="17" t="s">
-        <v>162</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>28</v>
@@ -83906,16 +83983,19 @@
       <c r="GP125" s="3">
         <v>24</v>
       </c>
+      <c r="GQ125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:198" ht="15">
+    <row r="126" spans="1:199" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C126" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>18</v>
@@ -83948,15 +84028,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:198" ht="15">
+    <row r="127" spans="1:199" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C127" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>18</v>
@@ -83989,15 +84069,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:198" ht="15">
+    <row r="128" spans="1:199" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C128" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>18</v>
@@ -84030,15 +84110,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:198" ht="15">
+    <row r="129" spans="1:199" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>18</v>
@@ -84071,7 +84151,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:198" ht="15">
+    <row r="130" spans="1:199" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -84127,15 +84207,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:198" ht="15">
+    <row r="131" spans="1:199" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D131" s="9" t="s">
         <v>28</v>
@@ -84173,16 +84253,19 @@
       <c r="GP131" s="3">
         <v>24</v>
       </c>
+      <c r="GQ131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:198" ht="15">
+    <row r="132" spans="1:199" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>28</v>
@@ -84220,16 +84303,19 @@
       <c r="GP132" s="3">
         <v>24</v>
       </c>
+      <c r="GQ132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:198" ht="15">
+    <row r="133" spans="1:199" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>28</v>
@@ -84240,16 +84326,19 @@
       <c r="F133" s="13">
         <v>45840</v>
       </c>
+      <c r="GQ133" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="134" spans="1:198" ht="15">
+    <row r="134" spans="1:199" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D134" s="9" t="s">
         <v>28</v>
@@ -84260,16 +84349,19 @@
       <c r="F134" s="13">
         <v>45840</v>
       </c>
+      <c r="GQ134" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="135" spans="1:198" ht="15">
+    <row r="135" spans="1:199" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D135" s="9" t="s">
         <v>32</v>
@@ -84283,16 +84375,19 @@
       <c r="GP135" s="3">
         <v>5</v>
       </c>
+      <c r="GQ135" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="136" spans="1:198" ht="15">
+    <row r="136" spans="1:199" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D136" s="9" t="s">
         <v>18</v>
@@ -84303,16 +84398,19 @@
       <c r="F136" s="13">
         <v>45840</v>
       </c>
+      <c r="GQ136" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="137" spans="1:198" ht="15">
+    <row r="137" spans="1:199" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
       <c r="B137" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C137" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="D137" s="9" t="s">
         <v>28</v>
@@ -84323,16 +84421,19 @@
       <c r="F137" s="13">
         <v>45840</v>
       </c>
+      <c r="GQ137" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="138" spans="1:198" ht="15">
+    <row r="138" spans="1:199" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D138" s="9" t="s">
         <v>28</v>
@@ -84343,16 +84444,22 @@
       <c r="F138" s="13">
         <v>45839</v>
       </c>
+      <c r="GP138" s="3">
+        <v>12</v>
+      </c>
+      <c r="GQ138" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="139" spans="1:198" ht="15">
+    <row r="139" spans="1:199" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D139" s="9" t="s">
         <v>28</v>
@@ -84363,16 +84470,22 @@
       <c r="F139" s="13">
         <v>45839</v>
       </c>
+      <c r="GP139" s="3">
+        <v>12</v>
+      </c>
+      <c r="GQ139" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="140" spans="1:198" ht="15">
+    <row r="140" spans="1:199" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D140" s="9" t="s">
         <v>18</v>
@@ -84383,16 +84496,22 @@
       <c r="F140" s="13">
         <v>45839</v>
       </c>
+      <c r="GP140" s="3">
+        <v>12</v>
+      </c>
+      <c r="GQ140" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="141" spans="1:198" ht="15">
+    <row r="141" spans="1:199" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D141" s="9" t="s">
         <v>18</v>
@@ -84403,16 +84522,22 @@
       <c r="F141" s="13">
         <v>45839</v>
       </c>
+      <c r="GP141" s="3">
+        <v>12</v>
+      </c>
+      <c r="GQ141" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="142" spans="1:198" ht="15">
+    <row r="142" spans="1:199" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C142" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D142" s="9" t="s">
         <v>32</v>
@@ -84444,16 +84569,19 @@
       <c r="GP142" s="3">
         <v>5</v>
       </c>
+      <c r="GQ142" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="143" spans="1:198" ht="15">
+    <row r="143" spans="1:199" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C143" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>18</v>
@@ -84485,16 +84613,19 @@
       <c r="GP143" s="3">
         <v>24</v>
       </c>
+      <c r="GQ143" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="144" spans="1:198" ht="15">
+    <row r="144" spans="1:199" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
       <c r="B144" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C144" s="17" t="s">
         <v>187</v>
-      </c>
-      <c r="C144" s="17" t="s">
-        <v>185</v>
       </c>
       <c r="D144" s="9" t="s">
         <v>32</v>
@@ -84526,16 +84657,19 @@
       <c r="GP144" s="3">
         <v>5</v>
       </c>
+      <c r="GQ144" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="145" spans="1:198" ht="15">
+    <row r="145" spans="1:199" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C145" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D145" s="9" t="s">
         <v>32</v>
@@ -84567,16 +84701,19 @@
       <c r="GP145" s="3">
         <v>5</v>
       </c>
+      <c r="GQ145" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="146" spans="1:198" ht="15">
+    <row r="146" spans="1:199" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C146" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D146" s="9" t="s">
         <v>18</v>
@@ -84608,16 +84745,19 @@
       <c r="GP146" s="3">
         <v>24</v>
       </c>
+      <c r="GQ146" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="147" spans="1:198" ht="15">
+    <row r="147" spans="1:199" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C147" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D147" s="9" t="s">
         <v>32</v>
@@ -84649,16 +84789,19 @@
       <c r="GP147" s="3">
         <v>5</v>
       </c>
+      <c r="GQ147" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:198" ht="15">
+    <row r="148" spans="1:199" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C148" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D148" s="9" t="s">
         <v>18</v>
@@ -84690,16 +84833,19 @@
       <c r="GP148" s="3">
         <v>24</v>
       </c>
+      <c r="GQ148" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="149" spans="1:198" ht="15">
+    <row r="149" spans="1:199" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C149" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>32</v>
@@ -84728,16 +84874,19 @@
       <c r="GP149" s="3">
         <v>5</v>
       </c>
+      <c r="GQ149" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="150" spans="1:198" ht="15">
+    <row r="150" spans="1:199" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C150" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D150" s="9" t="s">
         <v>18</v>
@@ -84769,16 +84918,19 @@
       <c r="GP150" s="3">
         <v>24</v>
       </c>
+      <c r="GQ150" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="151" spans="1:198" ht="15">
+    <row r="151" spans="1:199" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C151" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D151" s="9" t="s">
         <v>18</v>
@@ -84790,15 +84942,15 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="152" spans="1:198" ht="15">
+    <row r="152" spans="1:199" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C152" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D152" s="9" t="s">
         <v>32</v>
@@ -84827,16 +84979,19 @@
       <c r="GP152" s="3">
         <v>5</v>
       </c>
+      <c r="GQ152" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:198" ht="15">
+    <row r="153" spans="1:199" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C153" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D153" s="9" t="s">
         <v>32</v>
@@ -84865,16 +85020,19 @@
       <c r="GP153" s="3">
         <v>5</v>
       </c>
+      <c r="GQ153" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:198" ht="15">
+    <row r="154" spans="1:199" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C154" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D154" s="9" t="s">
         <v>18</v>
@@ -84891,16 +85049,19 @@
       <c r="GP154" s="3">
         <v>24</v>
       </c>
+      <c r="GQ154" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="155" spans="1:198" ht="15">
+    <row r="155" spans="1:199" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C155" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D155" s="9" t="s">
         <v>18</v>
@@ -84917,16 +85078,19 @@
       <c r="GP155" s="3">
         <v>24</v>
       </c>
+      <c r="GQ155" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="156" spans="1:198" ht="15">
+    <row r="156" spans="1:199" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C156" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D156" s="9" t="s">
         <v>18</v>
@@ -84943,16 +85107,19 @@
       <c r="GP156" s="3">
         <v>24</v>
       </c>
+      <c r="GQ156" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="157" spans="1:198" ht="15">
+    <row r="157" spans="1:199" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C157" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D157" s="9" t="s">
         <v>32</v>
@@ -84981,16 +85148,19 @@
       <c r="GP157" s="3">
         <v>5</v>
       </c>
+      <c r="GQ157" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="158" spans="1:198" ht="15">
+    <row r="158" spans="1:199" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C158" s="17" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D158" s="9" t="s">
         <v>21</v>
@@ -84999,15 +85169,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:198" ht="15">
+    <row r="159" spans="1:199" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C159" s="17" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>28</v>
@@ -85016,12 +85186,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:198">
+    <row r="160" spans="1:199">
       <c r="A160" s="9" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D160" s="9" t="s">
         <v>28</v>
@@ -85068,13 +85238,16 @@
       <c r="GP160" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="GQ160" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="161" spans="1:198">
+    <row r="161" spans="1:199">
       <c r="A161" s="9" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D161" s="9" t="s">
         <v>28</v>
@@ -85121,13 +85294,16 @@
       <c r="GP161" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="GQ161" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="162" spans="1:198">
+    <row r="162" spans="1:199">
       <c r="A162" s="9" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D162" s="9" t="s">
         <v>28</v>
@@ -85174,13 +85350,16 @@
       <c r="GP162" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="GQ162" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="163" spans="1:198" ht="15">
+    <row r="163" spans="1:199" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
       <c r="C163" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D163" s="9" t="s">
         <v>18</v>
@@ -85189,12 +85368,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:198" ht="15">
+    <row r="164" spans="1:199" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
       <c r="C164" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D164" s="9" t="s">
         <v>18</v>
@@ -85203,12 +85382,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:198" ht="15">
+    <row r="165" spans="1:199" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
       <c r="C165" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D165" s="9" t="s">
         <v>28</v>
@@ -85217,12 +85396,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:198" ht="15">
+    <row r="166" spans="1:199" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
       <c r="C166" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D166" s="9" t="s">
         <v>18</v>
@@ -85231,12 +85410,12 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:198" ht="15">
+    <row r="167" spans="1:199" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
       <c r="C167" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D167" s="9" t="s">
         <v>32</v>
@@ -85245,12 +85424,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:198" ht="15">
+    <row r="168" spans="1:199" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
       <c r="C168" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D168" s="9" t="s">
         <v>18</v>
@@ -85259,12 +85438,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:198" ht="15">
+    <row r="169" spans="1:199" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
       <c r="C169" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D169" s="9" t="s">
         <v>18</v>
@@ -85273,12 +85452,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:198" ht="15">
+    <row r="170" spans="1:199" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
       <c r="C170" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D170" s="9" t="s">
         <v>18</v>
@@ -85287,12 +85466,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:198" ht="15">
+    <row r="171" spans="1:199" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
       <c r="C171" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D171" s="9" t="s">
         <v>18</v>
@@ -85301,40 +85480,40 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:198" ht="15">
+    <row r="172" spans="1:199" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
       <c r="C172" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D172" s="9" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E172" s="9">
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:198" ht="15">
+    <row r="173" spans="1:199" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
       <c r="C173" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E173" s="9">
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:198" ht="15">
+    <row r="174" spans="1:199" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
       <c r="C174" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D174" s="9" t="s">
         <v>32</v>
@@ -85343,12 +85522,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:198" ht="15">
+    <row r="175" spans="1:199" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
       <c r="C175" s="17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D175" s="9" t="s">
         <v>28</v>
@@ -85357,12 +85536,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:198" ht="15">
+    <row r="176" spans="1:199" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>
       <c r="C176" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D176" s="9" t="s">
         <v>32</v>
@@ -85376,7 +85555,7 @@
         <v>25386584</v>
       </c>
       <c r="C177" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D177" s="9" t="s">
         <v>32</v>
@@ -85390,7 +85569,7 @@
         <v>25386617</v>
       </c>
       <c r="C178" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D178" s="9" t="s">
         <v>25</v>
@@ -85404,7 +85583,7 @@
         <v>25386605</v>
       </c>
       <c r="C179" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D179" s="9" t="s">
         <v>21</v>
@@ -85418,7 +85597,7 @@
         <v>25438399</v>
       </c>
       <c r="C180" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D180" s="9" t="s">
         <v>18</v>
@@ -85432,7 +85611,7 @@
         <v>25438419</v>
       </c>
       <c r="C181" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D181" s="9" t="s">
         <v>32</v>
@@ -85446,7 +85625,7 @@
         <v>25445298</v>
       </c>
       <c r="C182" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>18</v>
@@ -85460,7 +85639,7 @@
         <v>25438056</v>
       </c>
       <c r="C183" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>18</v>
@@ -85474,7 +85653,7 @@
         <v>25438634</v>
       </c>
       <c r="C184" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>32</v>
@@ -85488,7 +85667,7 @@
         <v>25442344</v>
       </c>
       <c r="C185" s="17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-04 09:45:00
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1759" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C007A444-B5ED-42FF-919B-673540C6CAE0}"/>
+  <xr:revisionPtr revIDLastSave="1808" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB6DE557-E295-4B86-B1E0-E111C0A47FDB}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GR47" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GP2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GT16" sqref="GT16"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73087,7 +73087,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:199" ht="15">
+    <row r="33" spans="1:200" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73236,7 +73236,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:199" ht="15">
+    <row r="34" spans="1:200" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73385,7 +73385,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:199" ht="15">
+    <row r="35" spans="1:200" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73534,7 +73534,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:199" ht="15">
+    <row r="36" spans="1:200" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73668,7 +73668,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:199" ht="15">
+    <row r="37" spans="1:200" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73802,7 +73802,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:199" ht="15">
+    <row r="38" spans="1:200" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73936,7 +73936,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:199" ht="15">
+    <row r="39" spans="1:200" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74099,7 +74099,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:199" ht="15">
+    <row r="40" spans="1:200" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74262,7 +74262,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:199" ht="15">
+    <row r="41" spans="1:200" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74425,7 +74425,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:199" ht="15">
+    <row r="42" spans="1:200" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74588,7 +74588,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:199" ht="15">
+    <row r="43" spans="1:200" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74751,7 +74751,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:199" ht="15">
+    <row r="44" spans="1:200" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74914,7 +74914,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:199" ht="15">
+    <row r="45" spans="1:200" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75077,7 +75077,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:199" ht="15">
+    <row r="46" spans="1:200" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75240,7 +75240,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:199" ht="15">
+    <row r="47" spans="1:200" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75426,8 +75426,11 @@
       <c r="GQ47" s="3">
         <v>24</v>
       </c>
+      <c r="GR47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:199" ht="15">
+    <row r="48" spans="1:200" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75824,6 +75827,9 @@
       <c r="GQ49" s="3">
         <v>24</v>
       </c>
+      <c r="GR49" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="1:207" ht="15">
       <c r="A50" s="11">
@@ -76644,6 +76650,9 @@
       <c r="GQ53" s="3">
         <v>24</v>
       </c>
+      <c r="GR53" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="1:207" ht="15">
       <c r="A54" s="11">
@@ -76831,6 +76840,9 @@
       <c r="GQ54" s="3">
         <v>24</v>
       </c>
+      <c r="GR54" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="55" spans="1:207" ht="15">
       <c r="A55" s="8">
@@ -78733,7 +78745,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:199" ht="15">
+    <row r="65" spans="1:200" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78882,7 +78894,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:199" ht="15">
+    <row r="66" spans="1:200" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79031,7 +79043,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:199" ht="15">
+    <row r="67" spans="1:200" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79170,7 +79182,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:199" ht="15">
+    <row r="68" spans="1:200" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79317,7 +79329,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:199" ht="15">
+    <row r="69" spans="1:200" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79453,7 +79465,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:199" ht="15">
+    <row r="70" spans="1:200" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79618,8 +79630,11 @@
       <c r="GQ70" s="3">
         <v>8</v>
       </c>
+      <c r="GR70" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="71" spans="1:199" ht="15">
+    <row r="71" spans="1:200" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79766,7 +79781,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:199" ht="15">
+    <row r="72" spans="1:200" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79904,8 +79919,11 @@
       <c r="GQ72" s="3">
         <v>8</v>
       </c>
+      <c r="GR72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:199" ht="15">
+    <row r="73" spans="1:200" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80170,7 +80188,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:199" ht="15">
+    <row r="74" spans="1:200" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80435,7 +80453,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:199" ht="15">
+    <row r="75" spans="1:200" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80569,7 +80587,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:199" ht="15">
+    <row r="76" spans="1:200" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80703,7 +80721,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:199" ht="15">
+    <row r="77" spans="1:200" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80837,7 +80855,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:199" ht="15">
+    <row r="78" spans="1:200" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81101,8 +81119,11 @@
       <c r="GQ78" s="3">
         <v>24</v>
       </c>
+      <c r="GR78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:199" ht="15">
+    <row r="79" spans="1:200" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81236,7 +81257,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:199" ht="15">
+    <row r="80" spans="1:200" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81425,7 +81446,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:199" ht="15">
+    <row r="81" spans="1:200" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81466,7 +81487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:199" ht="15">
+    <row r="82" spans="1:200" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81590,8 +81611,11 @@
       <c r="GQ82" s="3">
         <v>24</v>
       </c>
+      <c r="GR82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:199" ht="15">
+    <row r="83" spans="1:200" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81632,7 +81656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:199" ht="15">
+    <row r="84" spans="1:200" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81694,7 +81718,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:199" ht="15">
+    <row r="85" spans="1:200" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81789,7 +81813,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:199" ht="15">
+    <row r="86" spans="1:200" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81809,7 +81833,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:199" ht="15">
+    <row r="87" spans="1:200" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81831,8 +81855,11 @@
       <c r="GQ87" s="3">
         <v>8</v>
       </c>
+      <c r="GR87" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="88" spans="1:199" ht="15">
+    <row r="88" spans="1:200" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81854,8 +81881,11 @@
       <c r="GQ88" s="3">
         <v>8</v>
       </c>
+      <c r="GR88" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="89" spans="1:199" ht="15">
+    <row r="89" spans="1:200" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81914,7 +81944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:199" ht="15">
+    <row r="90" spans="1:200" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -81973,7 +82003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:199" ht="15">
+    <row r="91" spans="1:200" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82032,7 +82062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:199" ht="15">
+    <row r="92" spans="1:200" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82091,7 +82121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:199" ht="15">
+    <row r="93" spans="1:200" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82150,7 +82180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:199" ht="15">
+    <row r="94" spans="1:200" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82206,7 +82236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:199" ht="15">
+    <row r="95" spans="1:200" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82276,8 +82306,11 @@
       <c r="GQ95" s="3">
         <v>24</v>
       </c>
+      <c r="GR95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:199" ht="15">
+    <row r="96" spans="1:200" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82318,7 +82351,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:199" ht="15">
+    <row r="97" spans="1:200" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82359,7 +82392,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:199" ht="15">
+    <row r="98" spans="1:200" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82441,8 +82474,11 @@
       <c r="GQ98" s="3">
         <v>24</v>
       </c>
+      <c r="GR98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:199" ht="15">
+    <row r="99" spans="1:200" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82462,7 +82498,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:199" ht="15">
+    <row r="100" spans="1:200" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82503,7 +82539,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:199" ht="15">
+    <row r="101" spans="1:200" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82544,7 +82580,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:199" ht="15">
+    <row r="102" spans="1:200" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82585,7 +82621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:199" ht="15">
+    <row r="103" spans="1:200" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82626,7 +82662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:199" ht="15">
+    <row r="104" spans="1:200" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82667,7 +82703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:199" ht="15">
+    <row r="105" spans="1:200" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82726,7 +82762,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:199" ht="15">
+    <row r="106" spans="1:200" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82767,7 +82803,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:199" ht="15">
+    <row r="107" spans="1:200" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82849,8 +82885,11 @@
       <c r="GQ107" s="3">
         <v>24</v>
       </c>
+      <c r="GR107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:199" ht="15">
+    <row r="108" spans="1:200" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82912,7 +82951,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:199" ht="15">
+    <row r="109" spans="1:200" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82932,7 +82971,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:199" ht="15">
+    <row r="110" spans="1:200" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83020,8 +83059,11 @@
       <c r="GQ110" s="3">
         <v>24</v>
       </c>
+      <c r="GR110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:199" ht="15">
+    <row r="111" spans="1:200" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83068,7 +83110,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:199" ht="15">
+    <row r="112" spans="1:200" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83136,7 +83178,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:199" ht="15">
+    <row r="113" spans="1:200" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83183,7 +83225,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:199" ht="15">
+    <row r="114" spans="1:200" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83271,8 +83313,11 @@
       <c r="GQ114" s="3">
         <v>16</v>
       </c>
+      <c r="GR114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:199" ht="15">
+    <row r="115" spans="1:200" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83360,8 +83405,11 @@
       <c r="GQ115" s="3">
         <v>24</v>
       </c>
+      <c r="GR115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:199" ht="15">
+    <row r="116" spans="1:200" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83452,8 +83500,11 @@
       <c r="GQ116" s="3">
         <v>24</v>
       </c>
+      <c r="GR116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:199" ht="15">
+    <row r="117" spans="1:200" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83521,7 +83572,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:199" ht="15">
+    <row r="118" spans="1:200" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83592,7 +83643,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:199" ht="15">
+    <row r="119" spans="1:200" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83663,7 +83714,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:199" ht="15">
+    <row r="120" spans="1:200" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83734,7 +83785,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:199" ht="15">
+    <row r="121" spans="1:200" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83775,7 +83826,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:199" ht="15">
+    <row r="122" spans="1:200" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -83834,7 +83885,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:199" ht="15">
+    <row r="123" spans="1:200" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -83886,8 +83937,11 @@
       <c r="GQ123" s="3">
         <v>5</v>
       </c>
+      <c r="GR123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:199" ht="15">
+    <row r="124" spans="1:200" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -83928,7 +83982,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:199" ht="15">
+    <row r="125" spans="1:200" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -83986,8 +84040,11 @@
       <c r="GQ125" s="3">
         <v>24</v>
       </c>
+      <c r="GR125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:199" ht="15">
+    <row r="126" spans="1:200" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84028,7 +84085,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:199" ht="15">
+    <row r="127" spans="1:200" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84069,7 +84126,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:199" ht="15">
+    <row r="128" spans="1:200" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84110,7 +84167,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:199" ht="15">
+    <row r="129" spans="1:200" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -84151,7 +84208,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:199" ht="15">
+    <row r="130" spans="1:200" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -84207,7 +84264,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:199" ht="15">
+    <row r="131" spans="1:200" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -84256,8 +84313,11 @@
       <c r="GQ131" s="3">
         <v>24</v>
       </c>
+      <c r="GR131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:199" ht="15">
+    <row r="132" spans="1:200" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -84306,8 +84366,11 @@
       <c r="GQ132" s="3">
         <v>24</v>
       </c>
+      <c r="GR132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:199" ht="15">
+    <row r="133" spans="1:200" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -84329,8 +84392,11 @@
       <c r="GQ133" s="3">
         <v>8</v>
       </c>
+      <c r="GR133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:199" ht="15">
+    <row r="134" spans="1:200" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -84352,8 +84418,11 @@
       <c r="GQ134" s="3">
         <v>8</v>
       </c>
+      <c r="GR134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:199" ht="15">
+    <row r="135" spans="1:200" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -84378,8 +84447,11 @@
       <c r="GQ135" s="3">
         <v>5</v>
       </c>
+      <c r="GR135" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="136" spans="1:199" ht="15">
+    <row r="136" spans="1:200" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -84401,8 +84473,11 @@
       <c r="GQ136" s="3">
         <v>8</v>
       </c>
+      <c r="GR136" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="137" spans="1:199" ht="15">
+    <row r="137" spans="1:200" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -84424,8 +84499,11 @@
       <c r="GQ137" s="3">
         <v>8</v>
       </c>
+      <c r="GR137" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="138" spans="1:199" ht="15">
+    <row r="138" spans="1:200" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -84450,8 +84528,11 @@
       <c r="GQ138" s="3">
         <v>24</v>
       </c>
+      <c r="GR138" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="139" spans="1:199" ht="15">
+    <row r="139" spans="1:200" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -84476,8 +84557,11 @@
       <c r="GQ139" s="3">
         <v>24</v>
       </c>
+      <c r="GR139" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="140" spans="1:199" ht="15">
+    <row r="140" spans="1:200" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -84502,8 +84586,11 @@
       <c r="GQ140" s="3">
         <v>24</v>
       </c>
+      <c r="GR140" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="141" spans="1:199" ht="15">
+    <row r="141" spans="1:200" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -84528,8 +84615,11 @@
       <c r="GQ141" s="3">
         <v>24</v>
       </c>
+      <c r="GR141" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="142" spans="1:199" ht="15">
+    <row r="142" spans="1:200" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -84572,8 +84662,11 @@
       <c r="GQ142" s="3">
         <v>5</v>
       </c>
+      <c r="GR142" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="143" spans="1:199" ht="15">
+    <row r="143" spans="1:200" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -84616,8 +84709,11 @@
       <c r="GQ143" s="3">
         <v>24</v>
       </c>
+      <c r="GR143" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="144" spans="1:199" ht="15">
+    <row r="144" spans="1:200" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -84660,8 +84756,11 @@
       <c r="GQ144" s="3">
         <v>5</v>
       </c>
+      <c r="GR144" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="145" spans="1:199" ht="15">
+    <row r="145" spans="1:200" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -84704,8 +84803,11 @@
       <c r="GQ145" s="3">
         <v>5</v>
       </c>
+      <c r="GR145" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="146" spans="1:199" ht="15">
+    <row r="146" spans="1:200" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -84748,8 +84850,11 @@
       <c r="GQ146" s="3">
         <v>24</v>
       </c>
+      <c r="GR146" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="147" spans="1:199" ht="15">
+    <row r="147" spans="1:200" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -84792,8 +84897,11 @@
       <c r="GQ147" s="3">
         <v>5</v>
       </c>
+      <c r="GR147" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:199" ht="15">
+    <row r="148" spans="1:200" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -84836,8 +84944,11 @@
       <c r="GQ148" s="3">
         <v>24</v>
       </c>
+      <c r="GR148" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="149" spans="1:199" ht="15">
+    <row r="149" spans="1:200" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -84877,8 +84988,11 @@
       <c r="GQ149" s="3">
         <v>5</v>
       </c>
+      <c r="GR149" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="150" spans="1:199" ht="15">
+    <row r="150" spans="1:200" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -84921,8 +85035,11 @@
       <c r="GQ150" s="3">
         <v>24</v>
       </c>
+      <c r="GR150" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="151" spans="1:199" ht="15">
+    <row r="151" spans="1:200" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -84942,7 +85059,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="152" spans="1:199" ht="15">
+    <row r="152" spans="1:200" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -84982,8 +85099,11 @@
       <c r="GQ152" s="3">
         <v>5</v>
       </c>
+      <c r="GR152" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:199" ht="15">
+    <row r="153" spans="1:200" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -85023,8 +85143,11 @@
       <c r="GQ153" s="3">
         <v>5</v>
       </c>
+      <c r="GR153" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:199" ht="15">
+    <row r="154" spans="1:200" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -85052,8 +85175,11 @@
       <c r="GQ154" s="3">
         <v>24</v>
       </c>
+      <c r="GR154" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="155" spans="1:199" ht="15">
+    <row r="155" spans="1:200" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -85081,8 +85207,11 @@
       <c r="GQ155" s="3">
         <v>24</v>
       </c>
+      <c r="GR155" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="156" spans="1:199" ht="15">
+    <row r="156" spans="1:200" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -85110,8 +85239,11 @@
       <c r="GQ156" s="3">
         <v>24</v>
       </c>
+      <c r="GR156" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="157" spans="1:199" ht="15">
+    <row r="157" spans="1:200" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -85151,8 +85283,11 @@
       <c r="GQ157" s="3">
         <v>5</v>
       </c>
+      <c r="GR157" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="158" spans="1:199" ht="15">
+    <row r="158" spans="1:200" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -85169,7 +85304,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:199" ht="15">
+    <row r="159" spans="1:200" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -85186,7 +85321,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:199">
+    <row r="160" spans="1:200">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -85241,8 +85376,11 @@
       <c r="GQ160" s="3">
         <v>8</v>
       </c>
+      <c r="GR160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:199">
+    <row r="161" spans="1:200">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -85297,8 +85435,11 @@
       <c r="GQ161" s="3">
         <v>8</v>
       </c>
+      <c r="GR161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:199">
+    <row r="162" spans="1:200">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -85353,8 +85494,11 @@
       <c r="GQ162" s="3">
         <v>8</v>
       </c>
+      <c r="GR162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:199" ht="15">
+    <row r="163" spans="1:200" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -85368,7 +85512,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:199" ht="15">
+    <row r="164" spans="1:200" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -85382,7 +85526,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:199" ht="15">
+    <row r="165" spans="1:200" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -85396,7 +85540,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:199" ht="15">
+    <row r="166" spans="1:200" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -85410,7 +85554,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:199" ht="15">
+    <row r="167" spans="1:200" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -85424,7 +85568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:199" ht="15">
+    <row r="168" spans="1:200" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -85438,7 +85582,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:199" ht="15">
+    <row r="169" spans="1:200" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -85452,7 +85596,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:199" ht="15">
+    <row r="170" spans="1:200" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -85466,7 +85610,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:199" ht="15">
+    <row r="171" spans="1:200" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -85480,7 +85624,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:199" ht="15">
+    <row r="172" spans="1:200" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -85494,7 +85638,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:199" ht="15">
+    <row r="173" spans="1:200" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -85508,7 +85652,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:199" ht="15">
+    <row r="174" spans="1:200" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -85522,7 +85666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:199" ht="15">
+    <row r="175" spans="1:200" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -85536,7 +85680,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:199" ht="15">
+    <row r="176" spans="1:200" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-07 07:06:21
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1808" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB6DE557-E295-4B86-B1E0-E111C0A47FDB}"/>
+  <xr:revisionPtr revIDLastSave="1889" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22B90938-DC90-4A40-A835-67F890B806C7}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GP2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GT16" sqref="GT16"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GP142" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GU162" sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73087,7 +73087,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:200" ht="15">
+    <row r="33" spans="1:202" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73236,7 +73236,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:200" ht="15">
+    <row r="34" spans="1:202" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73385,7 +73385,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:200" ht="15">
+    <row r="35" spans="1:202" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73534,7 +73534,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:200" ht="15">
+    <row r="36" spans="1:202" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73668,7 +73668,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:200" ht="15">
+    <row r="37" spans="1:202" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73802,7 +73802,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:200" ht="15">
+    <row r="38" spans="1:202" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73936,7 +73936,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:200" ht="15">
+    <row r="39" spans="1:202" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74099,7 +74099,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:200" ht="15">
+    <row r="40" spans="1:202" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74262,7 +74262,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:200" ht="15">
+    <row r="41" spans="1:202" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74425,7 +74425,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:200" ht="15">
+    <row r="42" spans="1:202" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74588,7 +74588,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:200" ht="15">
+    <row r="43" spans="1:202" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74751,7 +74751,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:200" ht="15">
+    <row r="44" spans="1:202" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74914,7 +74914,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:200" ht="15">
+    <row r="45" spans="1:202" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75077,7 +75077,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:200" ht="15">
+    <row r="46" spans="1:202" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75240,7 +75240,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:200" ht="15">
+    <row r="47" spans="1:202" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75429,8 +75429,14 @@
       <c r="GR47" s="3">
         <v>24</v>
       </c>
+      <c r="GS47" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:200" ht="15">
+    <row r="48" spans="1:202" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75830,6 +75836,12 @@
       <c r="GR49" s="3">
         <v>24</v>
       </c>
+      <c r="GS49" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT49" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="1:207" ht="15">
       <c r="A50" s="11">
@@ -76653,6 +76665,12 @@
       <c r="GR53" s="3">
         <v>24</v>
       </c>
+      <c r="GS53" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT53" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="1:207" ht="15">
       <c r="A54" s="11">
@@ -76843,6 +76861,12 @@
       <c r="GR54" s="3">
         <v>24</v>
       </c>
+      <c r="GS54" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT54" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="55" spans="1:207" ht="15">
       <c r="A55" s="8">
@@ -78745,7 +78769,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:200" ht="15">
+    <row r="65" spans="1:202" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78894,7 +78918,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:200" ht="15">
+    <row r="66" spans="1:202" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79043,7 +79067,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:200" ht="15">
+    <row r="67" spans="1:202" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79182,7 +79206,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:200" ht="15">
+    <row r="68" spans="1:202" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79329,7 +79353,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:200" ht="15">
+    <row r="69" spans="1:202" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79465,7 +79489,7 @@
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
     </row>
-    <row r="70" spans="1:200" ht="15">
+    <row r="70" spans="1:202" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79633,8 +79657,14 @@
       <c r="GR70" s="3">
         <v>24</v>
       </c>
+      <c r="GS70" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT70" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="71" spans="1:200" ht="15">
+    <row r="71" spans="1:202" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79781,7 +79811,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:200" ht="15">
+    <row r="72" spans="1:202" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79922,8 +79952,14 @@
       <c r="GR72" s="3">
         <v>24</v>
       </c>
+      <c r="GS72" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:200" ht="15">
+    <row r="73" spans="1:202" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80188,7 +80224,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:200" ht="15">
+    <row r="74" spans="1:202" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80453,7 +80489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:200" ht="15">
+    <row r="75" spans="1:202" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80587,7 +80623,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:200" ht="15">
+    <row r="76" spans="1:202" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80721,7 +80757,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:200" ht="15">
+    <row r="77" spans="1:202" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80855,7 +80891,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:200" ht="15">
+    <row r="78" spans="1:202" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81122,8 +81158,14 @@
       <c r="GR78" s="3">
         <v>24</v>
       </c>
+      <c r="GS78" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:200" ht="15">
+    <row r="79" spans="1:202" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81257,7 +81299,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:200" ht="15">
+    <row r="80" spans="1:202" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81446,7 +81488,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:200" ht="15">
+    <row r="81" spans="1:202" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81487,7 +81529,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:200" ht="15">
+    <row r="82" spans="1:202" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81614,8 +81656,14 @@
       <c r="GR82" s="3">
         <v>24</v>
       </c>
+      <c r="GS82" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:200" ht="15">
+    <row r="83" spans="1:202" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81656,7 +81704,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:200" ht="15">
+    <row r="84" spans="1:202" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81718,7 +81766,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:200" ht="15">
+    <row r="85" spans="1:202" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81813,7 +81861,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:200" ht="15">
+    <row r="86" spans="1:202" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81833,7 +81881,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:200" ht="15">
+    <row r="87" spans="1:202" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81858,8 +81906,14 @@
       <c r="GR87" s="3">
         <v>24</v>
       </c>
+      <c r="GS87" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT87" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="88" spans="1:200" ht="15">
+    <row r="88" spans="1:202" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81884,8 +81938,14 @@
       <c r="GR88" s="3">
         <v>24</v>
       </c>
+      <c r="GS88" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT88" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="89" spans="1:200" ht="15">
+    <row r="89" spans="1:202" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -81944,7 +82004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:200" ht="15">
+    <row r="90" spans="1:202" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82003,7 +82063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:200" ht="15">
+    <row r="91" spans="1:202" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82062,7 +82122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:200" ht="15">
+    <row r="92" spans="1:202" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82121,7 +82181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:200" ht="15">
+    <row r="93" spans="1:202" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82180,7 +82240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:200" ht="15">
+    <row r="94" spans="1:202" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82236,7 +82296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:200" ht="15">
+    <row r="95" spans="1:202" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82309,8 +82369,14 @@
       <c r="GR95" s="3">
         <v>24</v>
       </c>
+      <c r="GS95" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:200" ht="15">
+    <row r="96" spans="1:202" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82351,7 +82417,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:200" ht="15">
+    <row r="97" spans="1:202" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82392,7 +82458,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:200" ht="15">
+    <row r="98" spans="1:202" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82477,8 +82543,14 @@
       <c r="GR98" s="3">
         <v>24</v>
       </c>
+      <c r="GS98" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:200" ht="15">
+    <row r="99" spans="1:202" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82498,7 +82570,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:200" ht="15">
+    <row r="100" spans="1:202" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82539,7 +82611,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:200" ht="15">
+    <row r="101" spans="1:202" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82580,7 +82652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:200" ht="15">
+    <row r="102" spans="1:202" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82621,7 +82693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:200" ht="15">
+    <row r="103" spans="1:202" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82662,7 +82734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:200" ht="15">
+    <row r="104" spans="1:202" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82703,7 +82775,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:200" ht="15">
+    <row r="105" spans="1:202" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82762,7 +82834,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:200" ht="15">
+    <row r="106" spans="1:202" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82803,7 +82875,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:200" ht="15">
+    <row r="107" spans="1:202" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82888,8 +82960,14 @@
       <c r="GR107" s="3">
         <v>24</v>
       </c>
+      <c r="GS107" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:200" ht="15">
+    <row r="108" spans="1:202" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -82951,7 +83029,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:200" ht="15">
+    <row r="109" spans="1:202" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -82971,7 +83049,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:200" ht="15">
+    <row r="110" spans="1:202" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83062,8 +83140,14 @@
       <c r="GR110" s="3">
         <v>24</v>
       </c>
+      <c r="GS110" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:200" ht="15">
+    <row r="111" spans="1:202" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83110,7 +83194,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:200" ht="15">
+    <row r="112" spans="1:202" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83178,7 +83262,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:200" ht="15">
+    <row r="113" spans="1:202" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83225,7 +83309,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:200" ht="15">
+    <row r="114" spans="1:202" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83316,8 +83400,14 @@
       <c r="GR114" s="3">
         <v>16</v>
       </c>
+      <c r="GS114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GT114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:200" ht="15">
+    <row r="115" spans="1:202" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83408,8 +83498,14 @@
       <c r="GR115" s="3">
         <v>24</v>
       </c>
+      <c r="GS115" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:200" ht="15">
+    <row r="116" spans="1:202" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83503,8 +83599,14 @@
       <c r="GR116" s="3">
         <v>24</v>
       </c>
+      <c r="GS116" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:200" ht="15">
+    <row r="117" spans="1:202" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83572,7 +83674,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:200" ht="15">
+    <row r="118" spans="1:202" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83643,7 +83745,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:200" ht="15">
+    <row r="119" spans="1:202" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83714,7 +83816,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:200" ht="15">
+    <row r="120" spans="1:202" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83785,7 +83887,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:200" ht="15">
+    <row r="121" spans="1:202" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83826,7 +83928,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:200" ht="15">
+    <row r="122" spans="1:202" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -83885,7 +83987,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:200" ht="15">
+    <row r="123" spans="1:202" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -83940,8 +84042,14 @@
       <c r="GR123" s="3">
         <v>5</v>
       </c>
+      <c r="GS123" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT123" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="124" spans="1:200" ht="15">
+    <row r="124" spans="1:202" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -83982,7 +84090,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:200" ht="15">
+    <row r="125" spans="1:202" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84043,8 +84151,14 @@
       <c r="GR125" s="3">
         <v>24</v>
       </c>
+      <c r="GS125" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:200" ht="15">
+    <row r="126" spans="1:202" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84085,7 +84199,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:200" ht="15">
+    <row r="127" spans="1:202" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84126,7 +84240,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:200" ht="15">
+    <row r="128" spans="1:202" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84167,7 +84281,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:200" ht="15">
+    <row r="129" spans="1:202" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -84208,7 +84322,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:200" ht="15">
+    <row r="130" spans="1:202" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -84264,7 +84378,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:200" ht="15">
+    <row r="131" spans="1:202" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -84316,8 +84430,14 @@
       <c r="GR131" s="3">
         <v>24</v>
       </c>
+      <c r="GS131" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:200" ht="15">
+    <row r="132" spans="1:202" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -84369,8 +84489,14 @@
       <c r="GR132" s="3">
         <v>24</v>
       </c>
+      <c r="GS132" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:200" ht="15">
+    <row r="133" spans="1:202" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -84395,8 +84521,14 @@
       <c r="GR133" s="3">
         <v>24</v>
       </c>
+      <c r="GS133" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:200" ht="15">
+    <row r="134" spans="1:202" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -84421,8 +84553,14 @@
       <c r="GR134" s="3">
         <v>24</v>
       </c>
+      <c r="GS134" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:200" ht="15">
+    <row r="135" spans="1:202" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -84450,8 +84588,14 @@
       <c r="GR135" s="3">
         <v>5</v>
       </c>
+      <c r="GS135" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT135" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="136" spans="1:200" ht="15">
+    <row r="136" spans="1:202" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -84476,8 +84620,14 @@
       <c r="GR136" s="3">
         <v>24</v>
       </c>
+      <c r="GS136" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT136" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="137" spans="1:200" ht="15">
+    <row r="137" spans="1:202" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -84502,8 +84652,14 @@
       <c r="GR137" s="3">
         <v>24</v>
       </c>
+      <c r="GS137" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT137" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="138" spans="1:200" ht="15">
+    <row r="138" spans="1:202" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -84531,8 +84687,14 @@
       <c r="GR138" s="3">
         <v>24</v>
       </c>
+      <c r="GS138" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT138" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="139" spans="1:200" ht="15">
+    <row r="139" spans="1:202" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -84560,8 +84722,14 @@
       <c r="GR139" s="3">
         <v>24</v>
       </c>
+      <c r="GS139" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT139" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="140" spans="1:200" ht="15">
+    <row r="140" spans="1:202" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -84589,8 +84757,14 @@
       <c r="GR140" s="3">
         <v>24</v>
       </c>
+      <c r="GS140" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT140" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="141" spans="1:200" ht="15">
+    <row r="141" spans="1:202" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -84618,8 +84792,14 @@
       <c r="GR141" s="3">
         <v>24</v>
       </c>
+      <c r="GS141" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT141" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="142" spans="1:200" ht="15">
+    <row r="142" spans="1:202" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -84666,7 +84846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:200" ht="15">
+    <row r="143" spans="1:202" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -84712,8 +84892,14 @@
       <c r="GR143" s="3">
         <v>24</v>
       </c>
+      <c r="GS143" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT143" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="144" spans="1:200" ht="15">
+    <row r="144" spans="1:202" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -84759,8 +84945,14 @@
       <c r="GR144" s="3">
         <v>5</v>
       </c>
+      <c r="GS144" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT144" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="145" spans="1:200" ht="15">
+    <row r="145" spans="1:202" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -84806,8 +84998,14 @@
       <c r="GR145" s="3">
         <v>5</v>
       </c>
+      <c r="GS145" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT145" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="146" spans="1:200" ht="15">
+    <row r="146" spans="1:202" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -84853,8 +85051,14 @@
       <c r="GR146" s="3">
         <v>24</v>
       </c>
+      <c r="GS146" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT146" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="147" spans="1:200" ht="15">
+    <row r="147" spans="1:202" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -84900,8 +85104,14 @@
       <c r="GR147" s="3">
         <v>5</v>
       </c>
+      <c r="GS147" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT147" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:200" ht="15">
+    <row r="148" spans="1:202" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -84947,8 +85157,14 @@
       <c r="GR148" s="3">
         <v>24</v>
       </c>
+      <c r="GS148" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT148" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="149" spans="1:200" ht="15">
+    <row r="149" spans="1:202" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -84991,8 +85207,14 @@
       <c r="GR149" s="3">
         <v>5</v>
       </c>
+      <c r="GS149" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT149" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="150" spans="1:200" ht="15">
+    <row r="150" spans="1:202" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -85038,8 +85260,14 @@
       <c r="GR150" s="3">
         <v>24</v>
       </c>
+      <c r="GS150" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT150" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="151" spans="1:200" ht="15">
+    <row r="151" spans="1:202" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -85059,7 +85287,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="152" spans="1:200" ht="15">
+    <row r="152" spans="1:202" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -85102,8 +85330,14 @@
       <c r="GR152" s="3">
         <v>5</v>
       </c>
+      <c r="GS152" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT152" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:200" ht="15">
+    <row r="153" spans="1:202" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -85146,8 +85380,14 @@
       <c r="GR153" s="3">
         <v>5</v>
       </c>
+      <c r="GS153" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT153" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:200" ht="15">
+    <row r="154" spans="1:202" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -85178,8 +85418,14 @@
       <c r="GR154" s="3">
         <v>24</v>
       </c>
+      <c r="GS154" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT154" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="155" spans="1:200" ht="15">
+    <row r="155" spans="1:202" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -85210,8 +85456,14 @@
       <c r="GR155" s="3">
         <v>24</v>
       </c>
+      <c r="GS155" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT155" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="156" spans="1:200" ht="15">
+    <row r="156" spans="1:202" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -85242,8 +85494,14 @@
       <c r="GR156" s="3">
         <v>24</v>
       </c>
+      <c r="GS156" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT156" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="157" spans="1:200" ht="15">
+    <row r="157" spans="1:202" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -85286,8 +85544,14 @@
       <c r="GR157" s="3">
         <v>5</v>
       </c>
+      <c r="GS157" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT157" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="158" spans="1:200" ht="15">
+    <row r="158" spans="1:202" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -85304,7 +85568,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:200" ht="15">
+    <row r="159" spans="1:202" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -85321,7 +85585,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:200">
+    <row r="160" spans="1:202">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -85379,8 +85643,14 @@
       <c r="GR160" s="3">
         <v>24</v>
       </c>
+      <c r="GS160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:200">
+    <row r="161" spans="1:202">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -85438,8 +85708,14 @@
       <c r="GR161" s="3">
         <v>24</v>
       </c>
+      <c r="GS161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:200">
+    <row r="162" spans="1:202">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -85497,8 +85773,14 @@
       <c r="GR162" s="3">
         <v>24</v>
       </c>
+      <c r="GS162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:200" ht="15">
+    <row r="163" spans="1:202" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -85512,7 +85794,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:200" ht="15">
+    <row r="164" spans="1:202" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -85526,7 +85808,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:200" ht="15">
+    <row r="165" spans="1:202" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -85540,7 +85822,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:200" ht="15">
+    <row r="166" spans="1:202" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -85554,7 +85836,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:200" ht="15">
+    <row r="167" spans="1:202" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -85568,7 +85850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:200" ht="15">
+    <row r="168" spans="1:202" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -85582,7 +85864,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:200" ht="15">
+    <row r="169" spans="1:202" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -85596,7 +85878,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:200" ht="15">
+    <row r="170" spans="1:202" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -85610,7 +85892,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:200" ht="15">
+    <row r="171" spans="1:202" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -85624,7 +85906,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:200" ht="15">
+    <row r="172" spans="1:202" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -85638,7 +85920,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:200" ht="15">
+    <row r="173" spans="1:202" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -85652,7 +85934,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:200" ht="15">
+    <row r="174" spans="1:202" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -85666,7 +85948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:200" ht="15">
+    <row r="175" spans="1:202" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -85680,7 +85962,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:200" ht="15">
+    <row r="176" spans="1:202" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-07 09:47:08
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1889" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22B90938-DC90-4A40-A835-67F890B806C7}"/>
+  <xr:revisionPtr revIDLastSave="1955" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39FD7CFD-2A7C-4F74-A583-E33DEFC6D68B}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="213">
   <si>
     <t>Module ID</t>
   </si>
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GP142" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GU162" sqref="A1:XFD1048576"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GQ127" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GV139" sqref="GV139"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73087,7 +73087,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:202" ht="15">
+    <row r="33" spans="1:203" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73236,7 +73236,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:202" ht="15">
+    <row r="34" spans="1:203" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73385,7 +73385,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:202" ht="15">
+    <row r="35" spans="1:203" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73534,7 +73534,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:202" ht="15">
+    <row r="36" spans="1:203" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73668,7 +73668,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:202" ht="15">
+    <row r="37" spans="1:203" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73802,7 +73802,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:202" ht="15">
+    <row r="38" spans="1:203" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73936,7 +73936,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:202" ht="15">
+    <row r="39" spans="1:203" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74099,7 +74099,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:202" ht="15">
+    <row r="40" spans="1:203" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74262,7 +74262,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:202" ht="15">
+    <row r="41" spans="1:203" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74425,7 +74425,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:202" ht="15">
+    <row r="42" spans="1:203" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74588,7 +74588,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:202" ht="15">
+    <row r="43" spans="1:203" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74751,7 +74751,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:202" ht="15">
+    <row r="44" spans="1:203" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74914,7 +74914,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:202" ht="15">
+    <row r="45" spans="1:203" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75077,7 +75077,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:202" ht="15">
+    <row r="46" spans="1:203" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75240,7 +75240,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:202" ht="15">
+    <row r="47" spans="1:203" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75435,8 +75435,11 @@
       <c r="GT47" s="3">
         <v>24</v>
       </c>
+      <c r="GU47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:202" ht="15">
+    <row r="48" spans="1:203" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75842,6 +75845,9 @@
       <c r="GT49" s="3">
         <v>24</v>
       </c>
+      <c r="GU49" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="1:207" ht="15">
       <c r="A50" s="11">
@@ -76671,6 +76677,9 @@
       <c r="GT53" s="3">
         <v>24</v>
       </c>
+      <c r="GU53" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="1:207" ht="15">
       <c r="A54" s="11">
@@ -76867,6 +76876,9 @@
       <c r="GT54" s="3">
         <v>24</v>
       </c>
+      <c r="GU54" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="55" spans="1:207" ht="15">
       <c r="A55" s="8">
@@ -78769,7 +78781,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:202" ht="15">
+    <row r="65" spans="1:203" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78918,7 +78930,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:202" ht="15">
+    <row r="66" spans="1:203" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79067,7 +79079,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:202" ht="15">
+    <row r="67" spans="1:203" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79206,7 +79218,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:202" ht="15">
+    <row r="68" spans="1:203" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79353,7 +79365,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:202" ht="15">
+    <row r="69" spans="1:203" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79488,8 +79500,23 @@
       <c r="FH69" s="1"/>
       <c r="FI69" s="1"/>
       <c r="FJ69" s="1"/>
+      <c r="GQ69" s="3">
+        <v>8</v>
+      </c>
+      <c r="GR69" s="3">
+        <v>24</v>
+      </c>
+      <c r="GS69" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT69" s="3">
+        <v>24</v>
+      </c>
+      <c r="GU69" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:202" ht="15">
+    <row r="70" spans="1:203" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79651,20 +79678,8 @@
       <c r="FH70" s="1"/>
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
-      <c r="GQ70" s="3">
-        <v>8</v>
-      </c>
-      <c r="GR70" s="3">
-        <v>24</v>
-      </c>
-      <c r="GS70" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT70" s="3">
-        <v>24</v>
-      </c>
     </row>
-    <row r="71" spans="1:202" ht="15">
+    <row r="71" spans="1:203" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79811,7 +79826,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:202" ht="15">
+    <row r="72" spans="1:203" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79958,8 +79973,11 @@
       <c r="GT72" s="3">
         <v>24</v>
       </c>
+      <c r="GU72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:202" ht="15">
+    <row r="73" spans="1:203" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80224,7 +80242,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:202" ht="15">
+    <row r="74" spans="1:203" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80489,7 +80507,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:202" ht="15">
+    <row r="75" spans="1:203" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80623,7 +80641,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:202" ht="15">
+    <row r="76" spans="1:203" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80757,7 +80775,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:202" ht="15">
+    <row r="77" spans="1:203" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80891,7 +80909,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:202" ht="15">
+    <row r="78" spans="1:203" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81164,8 +81182,11 @@
       <c r="GT78" s="3">
         <v>24</v>
       </c>
+      <c r="GU78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:202" ht="15">
+    <row r="79" spans="1:203" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81299,7 +81320,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:202" ht="15">
+    <row r="80" spans="1:203" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81488,7 +81509,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:202" ht="15">
+    <row r="81" spans="1:203" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81529,7 +81550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:202" ht="15">
+    <row r="82" spans="1:203" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81662,8 +81683,11 @@
       <c r="GT82" s="3">
         <v>24</v>
       </c>
+      <c r="GU82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:202" ht="15">
+    <row r="83" spans="1:203" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81704,7 +81728,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:202" ht="15">
+    <row r="84" spans="1:203" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81766,7 +81790,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:202" ht="15">
+    <row r="85" spans="1:203" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81861,7 +81885,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:202" ht="15">
+    <row r="86" spans="1:203" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81881,7 +81905,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:202" ht="15">
+    <row r="87" spans="1:203" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81912,8 +81936,11 @@
       <c r="GT87" s="3">
         <v>24</v>
       </c>
+      <c r="GU87" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="88" spans="1:202" ht="15">
+    <row r="88" spans="1:203" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81944,8 +81971,11 @@
       <c r="GT88" s="3">
         <v>24</v>
       </c>
+      <c r="GU88" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="89" spans="1:202" ht="15">
+    <row r="89" spans="1:203" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82004,7 +82034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:202" ht="15">
+    <row r="90" spans="1:203" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82063,7 +82093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:202" ht="15">
+    <row r="91" spans="1:203" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82122,7 +82152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:202" ht="15">
+    <row r="92" spans="1:203" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82181,7 +82211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:202" ht="15">
+    <row r="93" spans="1:203" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82240,7 +82270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:202" ht="15">
+    <row r="94" spans="1:203" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82296,7 +82326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:202" ht="15">
+    <row r="95" spans="1:203" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82375,8 +82405,11 @@
       <c r="GT95" s="3">
         <v>24</v>
       </c>
+      <c r="GU95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:202" ht="15">
+    <row r="96" spans="1:203" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82417,7 +82450,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:202" ht="15">
+    <row r="97" spans="1:203" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82458,7 +82491,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:202" ht="15">
+    <row r="98" spans="1:203" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82549,8 +82582,11 @@
       <c r="GT98" s="3">
         <v>24</v>
       </c>
+      <c r="GU98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:202" ht="15">
+    <row r="99" spans="1:203" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82570,7 +82606,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:202" ht="15">
+    <row r="100" spans="1:203" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82611,7 +82647,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:202" ht="15">
+    <row r="101" spans="1:203" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82652,7 +82688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:202" ht="15">
+    <row r="102" spans="1:203" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82693,7 +82729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:202" ht="15">
+    <row r="103" spans="1:203" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82734,7 +82770,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:202" ht="15">
+    <row r="104" spans="1:203" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82775,7 +82811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:202" ht="15">
+    <row r="105" spans="1:203" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82834,7 +82870,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:202" ht="15">
+    <row r="106" spans="1:203" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82875,7 +82911,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:202" ht="15">
+    <row r="107" spans="1:203" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -82966,8 +83002,11 @@
       <c r="GT107" s="3">
         <v>24</v>
       </c>
+      <c r="GU107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:202" ht="15">
+    <row r="108" spans="1:203" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83029,7 +83068,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:202" ht="15">
+    <row r="109" spans="1:203" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83049,7 +83088,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:202" ht="15">
+    <row r="110" spans="1:203" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83146,8 +83185,11 @@
       <c r="GT110" s="3">
         <v>24</v>
       </c>
+      <c r="GU110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:202" ht="15">
+    <row r="111" spans="1:203" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83194,7 +83236,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:202" ht="15">
+    <row r="112" spans="1:203" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83262,7 +83304,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:202" ht="15">
+    <row r="113" spans="1:204" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83309,7 +83351,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:202" ht="15">
+    <row r="114" spans="1:204" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83406,8 +83448,11 @@
       <c r="GT114" s="3">
         <v>16</v>
       </c>
+      <c r="GU114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:202" ht="15">
+    <row r="115" spans="1:204" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83504,8 +83549,11 @@
       <c r="GT115" s="3">
         <v>24</v>
       </c>
+      <c r="GU115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:202" ht="15">
+    <row r="116" spans="1:204" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83605,8 +83653,11 @@
       <c r="GT116" s="3">
         <v>24</v>
       </c>
+      <c r="GU116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:202" ht="15">
+    <row r="117" spans="1:204" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83674,7 +83725,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:202" ht="15">
+    <row r="118" spans="1:204" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83745,7 +83796,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:202" ht="15">
+    <row r="119" spans="1:204" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83816,7 +83867,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:202" ht="15">
+    <row r="120" spans="1:204" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83887,7 +83938,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:202" ht="15">
+    <row r="121" spans="1:204" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83928,7 +83979,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:202" ht="15">
+    <row r="122" spans="1:204" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -83987,7 +84038,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:202" ht="15">
+    <row r="123" spans="1:204" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -84048,8 +84099,14 @@
       <c r="GT123" s="3">
         <v>5</v>
       </c>
+      <c r="GU123" s="3">
+        <v>5</v>
+      </c>
+      <c r="GV123" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="124" spans="1:202" ht="15">
+    <row r="124" spans="1:204" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -84090,7 +84147,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:202" ht="15">
+    <row r="125" spans="1:204" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84157,8 +84214,11 @@
       <c r="GT125" s="3">
         <v>24</v>
       </c>
+      <c r="GU125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:202" ht="15">
+    <row r="126" spans="1:204" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84199,7 +84259,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:202" ht="15">
+    <row r="127" spans="1:204" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84240,7 +84300,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:202" ht="15">
+    <row r="128" spans="1:204" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84281,7 +84341,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:202" ht="15">
+    <row r="129" spans="1:204" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -84322,7 +84382,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:202" ht="15">
+    <row r="130" spans="1:204" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -84378,7 +84438,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:202" ht="15">
+    <row r="131" spans="1:204" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -84436,8 +84496,11 @@
       <c r="GT131" s="3">
         <v>24</v>
       </c>
+      <c r="GU131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:202" ht="15">
+    <row r="132" spans="1:204" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -84495,8 +84558,11 @@
       <c r="GT132" s="3">
         <v>24</v>
       </c>
+      <c r="GU132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:202" ht="15">
+    <row r="133" spans="1:204" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -84527,8 +84593,11 @@
       <c r="GT133" s="3">
         <v>24</v>
       </c>
+      <c r="GU133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:202" ht="15">
+    <row r="134" spans="1:204" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -84559,8 +84628,11 @@
       <c r="GT134" s="3">
         <v>24</v>
       </c>
+      <c r="GU134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:202" ht="15">
+    <row r="135" spans="1:204" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -84594,8 +84666,11 @@
       <c r="GT135" s="3">
         <v>5</v>
       </c>
+      <c r="GU135" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="136" spans="1:202" ht="15">
+    <row r="136" spans="1:204" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -84626,8 +84701,14 @@
       <c r="GT136" s="3">
         <v>24</v>
       </c>
+      <c r="GU136" s="3">
+        <v>16</v>
+      </c>
+      <c r="GV136" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="137" spans="1:202" ht="15">
+    <row r="137" spans="1:204" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -84658,8 +84739,14 @@
       <c r="GT137" s="3">
         <v>24</v>
       </c>
+      <c r="GU137" s="3">
+        <v>16</v>
+      </c>
+      <c r="GV137" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="138" spans="1:202" ht="15">
+    <row r="138" spans="1:204" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -84693,8 +84780,11 @@
       <c r="GT138" s="3">
         <v>24</v>
       </c>
+      <c r="GU138" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="139" spans="1:202" ht="15">
+    <row r="139" spans="1:204" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -84728,8 +84818,11 @@
       <c r="GT139" s="3">
         <v>24</v>
       </c>
+      <c r="GU139" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="140" spans="1:202" ht="15">
+    <row r="140" spans="1:204" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -84763,8 +84856,11 @@
       <c r="GT140" s="3">
         <v>24</v>
       </c>
+      <c r="GU140" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="141" spans="1:202" ht="15">
+    <row r="141" spans="1:204" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -84798,8 +84894,11 @@
       <c r="GT141" s="3">
         <v>24</v>
       </c>
+      <c r="GU141" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="142" spans="1:202" ht="15">
+    <row r="142" spans="1:204" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -84845,8 +84944,20 @@
       <c r="GR142" s="3">
         <v>5</v>
       </c>
+      <c r="GS142" s="3">
+        <v>5</v>
+      </c>
+      <c r="GT142" s="3">
+        <v>5</v>
+      </c>
+      <c r="GU142" s="3">
+        <v>5</v>
+      </c>
+      <c r="GV142" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="143" spans="1:202" ht="15">
+    <row r="143" spans="1:204" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -84898,8 +85009,11 @@
       <c r="GT143" s="3">
         <v>24</v>
       </c>
+      <c r="GU143" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="144" spans="1:202" ht="15">
+    <row r="144" spans="1:204" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -84951,8 +85065,11 @@
       <c r="GT144" s="3">
         <v>5</v>
       </c>
+      <c r="GU144" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="145" spans="1:202" ht="15">
+    <row r="145" spans="1:203" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -85004,8 +85121,11 @@
       <c r="GT145" s="3">
         <v>5</v>
       </c>
+      <c r="GU145" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="146" spans="1:202" ht="15">
+    <row r="146" spans="1:203" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -85057,8 +85177,11 @@
       <c r="GT146" s="3">
         <v>24</v>
       </c>
+      <c r="GU146" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="147" spans="1:202" ht="15">
+    <row r="147" spans="1:203" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -85110,8 +85233,11 @@
       <c r="GT147" s="3">
         <v>5</v>
       </c>
+      <c r="GU147" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:202" ht="15">
+    <row r="148" spans="1:203" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -85163,8 +85289,11 @@
       <c r="GT148" s="3">
         <v>24</v>
       </c>
+      <c r="GU148" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="149" spans="1:202" ht="15">
+    <row r="149" spans="1:203" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -85213,8 +85342,11 @@
       <c r="GT149" s="3">
         <v>5</v>
       </c>
+      <c r="GU149" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="150" spans="1:202" ht="15">
+    <row r="150" spans="1:203" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -85266,8 +85398,11 @@
       <c r="GT150" s="3">
         <v>24</v>
       </c>
+      <c r="GU150" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="151" spans="1:202" ht="15">
+    <row r="151" spans="1:203" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -85287,7 +85422,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="152" spans="1:202" ht="15">
+    <row r="152" spans="1:203" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -85336,8 +85471,11 @@
       <c r="GT152" s="3">
         <v>5</v>
       </c>
+      <c r="GU152" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="153" spans="1:202" ht="15">
+    <row r="153" spans="1:203" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -85386,8 +85524,11 @@
       <c r="GT153" s="3">
         <v>5</v>
       </c>
+      <c r="GU153" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="154" spans="1:202" ht="15">
+    <row r="154" spans="1:203" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -85406,6 +85547,9 @@
       <c r="F154" s="13">
         <v>45838</v>
       </c>
+      <c r="P154" s="13">
+        <v>45842</v>
+      </c>
       <c r="GO154" s="3">
         <v>10</v>
       </c>
@@ -85419,13 +85563,13 @@
         <v>24</v>
       </c>
       <c r="GS154" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT154" s="3">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="GT154" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:202" ht="15">
+    <row r="155" spans="1:203" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -85444,6 +85588,9 @@
       <c r="F155" s="13">
         <v>45838</v>
       </c>
+      <c r="P155" s="13">
+        <v>45842</v>
+      </c>
       <c r="GO155" s="3">
         <v>10</v>
       </c>
@@ -85457,13 +85604,13 @@
         <v>24</v>
       </c>
       <c r="GS155" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT155" s="3">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="GT155" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="156" spans="1:202" ht="15">
+    <row r="156" spans="1:203" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -85482,6 +85629,9 @@
       <c r="F156" s="13">
         <v>45838</v>
       </c>
+      <c r="P156" s="13">
+        <v>45842</v>
+      </c>
       <c r="GO156" s="3">
         <v>10</v>
       </c>
@@ -85495,13 +85645,13 @@
         <v>24</v>
       </c>
       <c r="GS156" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT156" s="3">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="GT156" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="157" spans="1:202" ht="15">
+    <row r="157" spans="1:203" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -85550,8 +85700,11 @@
       <c r="GT157" s="3">
         <v>5</v>
       </c>
+      <c r="GU157" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="158" spans="1:202" ht="15">
+    <row r="158" spans="1:203" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -85568,7 +85721,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:202" ht="15">
+    <row r="159" spans="1:203" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -85585,7 +85738,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:202">
+    <row r="160" spans="1:203">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -85649,8 +85802,11 @@
       <c r="GT160" s="3">
         <v>24</v>
       </c>
+      <c r="GU160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:202">
+    <row r="161" spans="1:203">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -85714,8 +85870,11 @@
       <c r="GT161" s="3">
         <v>24</v>
       </c>
+      <c r="GU161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:202">
+    <row r="162" spans="1:203">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -85779,8 +85938,11 @@
       <c r="GT162" s="3">
         <v>24</v>
       </c>
+      <c r="GU162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:202" ht="15">
+    <row r="163" spans="1:203" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -85794,7 +85956,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:202" ht="15">
+    <row r="164" spans="1:203" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -85808,7 +85970,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:202" ht="15">
+    <row r="165" spans="1:203" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -85822,7 +85984,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:202" ht="15">
+    <row r="166" spans="1:203" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -85836,7 +85998,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:202" ht="15">
+    <row r="167" spans="1:203" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -85850,7 +86012,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:202" ht="15">
+    <row r="168" spans="1:203" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -85864,7 +86026,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:202" ht="15">
+    <row r="169" spans="1:203" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -85878,7 +86040,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:202" ht="15">
+    <row r="170" spans="1:203" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -85892,7 +86054,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:202" ht="15">
+    <row r="171" spans="1:203" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -85906,7 +86068,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:202" ht="15">
+    <row r="172" spans="1:203" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -85920,7 +86082,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:202" ht="15">
+    <row r="173" spans="1:203" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -85934,7 +86096,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:202" ht="15">
+    <row r="174" spans="1:203" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -85948,7 +86110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:202" ht="15">
+    <row r="175" spans="1:203" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -85962,7 +86124,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:202" ht="15">
+    <row r="176" spans="1:203" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-07 11:41:33
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1955" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39FD7CFD-2A7C-4F74-A583-E33DEFC6D68B}"/>
+  <xr:revisionPtr revIDLastSave="2015" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71232AB4-D278-49DB-9B7C-DE4EE1003E43}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="213">
   <si>
     <t>Module ID</t>
   </si>
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GQ127" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GV139" sqref="GV139"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GO130" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GV140" sqref="GV140"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -81509,7 +81509,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:203" ht="15">
+    <row r="81" spans="1:204" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81550,7 +81550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:203" ht="15">
+    <row r="82" spans="1:204" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81687,7 +81687,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:203" ht="15">
+    <row r="83" spans="1:204" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81728,7 +81728,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:203" ht="15">
+    <row r="84" spans="1:204" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81790,7 +81790,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:203" ht="15">
+    <row r="85" spans="1:204" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81885,7 +81885,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:203" ht="15">
+    <row r="86" spans="1:204" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81905,7 +81905,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:203" ht="15">
+    <row r="87" spans="1:204" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81937,10 +81937,13 @@
         <v>24</v>
       </c>
       <c r="GU87" s="3">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="GV87" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:203" ht="15">
+    <row r="88" spans="1:204" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81972,10 +81975,13 @@
         <v>24</v>
       </c>
       <c r="GU88" s="3">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="GV88" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:203" ht="15">
+    <row r="89" spans="1:204" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82034,7 +82040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:203" ht="15">
+    <row r="90" spans="1:204" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82093,7 +82099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:203" ht="15">
+    <row r="91" spans="1:204" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82152,7 +82158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:203" ht="15">
+    <row r="92" spans="1:204" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82211,7 +82217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:203" ht="15">
+    <row r="93" spans="1:204" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82270,7 +82276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:203" ht="15">
+    <row r="94" spans="1:204" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82326,7 +82332,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:203" ht="15">
+    <row r="95" spans="1:204" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82409,7 +82415,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:203" ht="15">
+    <row r="96" spans="1:204" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -84057,6 +84063,9 @@
       <c r="F123" s="13">
         <v>45830</v>
       </c>
+      <c r="P123" s="13">
+        <v>45844</v>
+      </c>
       <c r="GG123" s="3">
         <v>5</v>
       </c>
@@ -84669,6 +84678,9 @@
       <c r="GU135" s="3">
         <v>5</v>
       </c>
+      <c r="GV135" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="136" spans="1:204" ht="15">
       <c r="A136" s="9">
@@ -84689,6 +84701,9 @@
       <c r="F136" s="13">
         <v>45840</v>
       </c>
+      <c r="P136" s="13">
+        <v>45844</v>
+      </c>
       <c r="GQ136" s="3">
         <v>8</v>
       </c>
@@ -84705,7 +84720,7 @@
         <v>16</v>
       </c>
       <c r="GV136" s="3" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
     </row>
     <row r="137" spans="1:204" ht="15">
@@ -84740,10 +84755,7 @@
         <v>24</v>
       </c>
       <c r="GU137" s="3">
-        <v>16</v>
-      </c>
-      <c r="GV137" s="3" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138" spans="1:204" ht="15">
@@ -84841,6 +84853,9 @@
       <c r="F140" s="13">
         <v>45839</v>
       </c>
+      <c r="P140" s="13">
+        <v>45843</v>
+      </c>
       <c r="GP140" s="3">
         <v>12</v>
       </c>
@@ -84854,10 +84869,10 @@
         <v>24</v>
       </c>
       <c r="GT140" s="3">
-        <v>24</v>
-      </c>
-      <c r="GU140" s="3">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="GU140" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="141" spans="1:204" ht="15">
@@ -84879,6 +84894,9 @@
       <c r="F141" s="13">
         <v>45839</v>
       </c>
+      <c r="P141" s="13">
+        <v>45843</v>
+      </c>
       <c r="GP141" s="3">
         <v>12</v>
       </c>
@@ -84892,10 +84910,10 @@
         <v>24</v>
       </c>
       <c r="GT141" s="3">
-        <v>24</v>
-      </c>
-      <c r="GU141" s="3">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="GU141" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="142" spans="1:204" ht="15">
@@ -84917,6 +84935,9 @@
       <c r="F142" s="13">
         <v>45833</v>
       </c>
+      <c r="P142" s="13">
+        <v>45845</v>
+      </c>
       <c r="GJ142" s="3">
         <v>5</v>
       </c>
@@ -84976,6 +84997,9 @@
       <c r="F143" s="13">
         <v>45833</v>
       </c>
+      <c r="P143" s="13">
+        <v>45837</v>
+      </c>
       <c r="GJ143" s="3">
         <v>12</v>
       </c>
@@ -84989,28 +85013,10 @@
         <v>24</v>
       </c>
       <c r="GN143" s="3">
-        <v>24</v>
-      </c>
-      <c r="GO143" s="3">
-        <v>24</v>
-      </c>
-      <c r="GP143" s="3">
-        <v>24</v>
-      </c>
-      <c r="GQ143" s="3">
-        <v>24</v>
-      </c>
-      <c r="GR143" s="3">
-        <v>24</v>
-      </c>
-      <c r="GS143" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT143" s="3">
-        <v>24</v>
-      </c>
-      <c r="GU143" s="3">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="GO143" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="144" spans="1:204" ht="15">
@@ -85032,6 +85038,9 @@
       <c r="F144" s="13">
         <v>45833</v>
       </c>
+      <c r="P144" s="13">
+        <v>45845</v>
+      </c>
       <c r="GJ144" s="3">
         <v>5</v>
       </c>
@@ -85068,8 +85077,11 @@
       <c r="GU144" s="3">
         <v>5</v>
       </c>
+      <c r="GV144" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="145" spans="1:203" ht="15">
+    <row r="145" spans="1:205" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -85088,6 +85100,9 @@
       <c r="F145" s="13">
         <v>45833</v>
       </c>
+      <c r="P145" s="13">
+        <v>45845</v>
+      </c>
       <c r="GJ145" s="3">
         <v>5</v>
       </c>
@@ -85124,8 +85139,11 @@
       <c r="GU145" s="3">
         <v>5</v>
       </c>
+      <c r="GV145" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="146" spans="1:203" ht="15">
+    <row r="146" spans="1:205" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -85144,6 +85162,9 @@
       <c r="F146" s="13">
         <v>45833</v>
       </c>
+      <c r="P146" s="13">
+        <v>45837</v>
+      </c>
       <c r="GJ146" s="3">
         <v>12</v>
       </c>
@@ -85157,31 +85178,13 @@
         <v>24</v>
       </c>
       <c r="GN146" s="3">
-        <v>24</v>
-      </c>
-      <c r="GO146" s="3">
-        <v>24</v>
-      </c>
-      <c r="GP146" s="3">
-        <v>24</v>
-      </c>
-      <c r="GQ146" s="3">
-        <v>24</v>
-      </c>
-      <c r="GR146" s="3">
-        <v>24</v>
-      </c>
-      <c r="GS146" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT146" s="3">
-        <v>24</v>
-      </c>
-      <c r="GU146" s="3">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="GO146" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="147" spans="1:203" ht="15">
+    <row r="147" spans="1:205" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -85200,6 +85203,9 @@
       <c r="F147" s="13">
         <v>45833</v>
       </c>
+      <c r="P147" s="13">
+        <v>45845</v>
+      </c>
       <c r="GJ147" s="3">
         <v>5</v>
       </c>
@@ -85236,8 +85242,11 @@
       <c r="GU147" s="3">
         <v>5</v>
       </c>
+      <c r="GV147" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="148" spans="1:203" ht="15">
+    <row r="148" spans="1:205" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -85256,6 +85265,9 @@
       <c r="F148" s="13">
         <v>45833</v>
       </c>
+      <c r="P148" s="13">
+        <v>45837</v>
+      </c>
       <c r="GJ148" s="3">
         <v>12</v>
       </c>
@@ -85269,31 +85281,13 @@
         <v>24</v>
       </c>
       <c r="GN148" s="3">
-        <v>24</v>
-      </c>
-      <c r="GO148" s="3">
-        <v>24</v>
-      </c>
-      <c r="GP148" s="3">
-        <v>24</v>
-      </c>
-      <c r="GQ148" s="3">
-        <v>24</v>
-      </c>
-      <c r="GR148" s="3">
-        <v>24</v>
-      </c>
-      <c r="GS148" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT148" s="3">
-        <v>24</v>
-      </c>
-      <c r="GU148" s="3">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="GO148" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:203" ht="15">
+    <row r="149" spans="1:205" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -85312,6 +85306,9 @@
       <c r="F149" s="13">
         <v>45834</v>
       </c>
+      <c r="P149" s="13">
+        <v>45845</v>
+      </c>
       <c r="GK149" s="3">
         <v>5</v>
       </c>
@@ -85345,8 +85342,14 @@
       <c r="GU149" s="3">
         <v>5</v>
       </c>
+      <c r="GV149" s="3">
+        <v>5</v>
+      </c>
+      <c r="GW149" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="150" spans="1:203" ht="15">
+    <row r="150" spans="1:205" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -85365,6 +85368,9 @@
       <c r="F150" s="13">
         <v>45833</v>
       </c>
+      <c r="P150" s="13">
+        <v>45837</v>
+      </c>
       <c r="GJ150" s="3">
         <v>12</v>
       </c>
@@ -85378,31 +85384,13 @@
         <v>24</v>
       </c>
       <c r="GN150" s="3">
-        <v>24</v>
-      </c>
-      <c r="GO150" s="3">
-        <v>24</v>
-      </c>
-      <c r="GP150" s="3">
-        <v>24</v>
-      </c>
-      <c r="GQ150" s="3">
-        <v>24</v>
-      </c>
-      <c r="GR150" s="3">
-        <v>24</v>
-      </c>
-      <c r="GS150" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT150" s="3">
-        <v>24</v>
-      </c>
-      <c r="GU150" s="3">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="GO150" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="151" spans="1:203" ht="15">
+    <row r="151" spans="1:205" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -85421,8 +85409,29 @@
       <c r="F151" s="13">
         <v>45838</v>
       </c>
+      <c r="P151" s="13">
+        <v>45842</v>
+      </c>
+      <c r="GO151" s="3">
+        <v>10</v>
+      </c>
+      <c r="GP151" s="3">
+        <v>24</v>
+      </c>
+      <c r="GQ151" s="3">
+        <v>24</v>
+      </c>
+      <c r="GR151" s="3">
+        <v>24</v>
+      </c>
+      <c r="GS151" s="3">
+        <v>14</v>
+      </c>
+      <c r="GT151" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="152" spans="1:203" ht="15">
+    <row r="152" spans="1:205" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -85441,6 +85450,9 @@
       <c r="F152" s="13">
         <v>45834</v>
       </c>
+      <c r="P152" s="13">
+        <v>45845</v>
+      </c>
       <c r="GK152" s="3">
         <v>5</v>
       </c>
@@ -85474,8 +85486,14 @@
       <c r="GU152" s="3">
         <v>5</v>
       </c>
+      <c r="GV152" s="3">
+        <v>5</v>
+      </c>
+      <c r="GW152" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="153" spans="1:203" ht="15">
+    <row r="153" spans="1:205" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -85494,6 +85512,9 @@
       <c r="F153" s="13">
         <v>45834</v>
       </c>
+      <c r="P153" s="13">
+        <v>45845</v>
+      </c>
       <c r="GK153" s="3">
         <v>5</v>
       </c>
@@ -85527,8 +85548,14 @@
       <c r="GU153" s="3">
         <v>5</v>
       </c>
+      <c r="GV153" s="3">
+        <v>5</v>
+      </c>
+      <c r="GW153" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="154" spans="1:203" ht="15">
+    <row r="154" spans="1:205" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -85569,7 +85596,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:203" ht="15">
+    <row r="155" spans="1:205" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -85610,7 +85637,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="156" spans="1:203" ht="15">
+    <row r="156" spans="1:205" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -85651,7 +85678,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="1:203" ht="15">
+    <row r="157" spans="1:205" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -85670,6 +85697,9 @@
       <c r="F157" s="13">
         <v>45834</v>
       </c>
+      <c r="P157" s="13">
+        <v>45845</v>
+      </c>
       <c r="GK157" s="3">
         <v>5</v>
       </c>
@@ -85703,8 +85733,14 @@
       <c r="GU157" s="3">
         <v>5</v>
       </c>
+      <c r="GV157" s="3">
+        <v>5</v>
+      </c>
+      <c r="GW157" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="158" spans="1:203" ht="15">
+    <row r="158" spans="1:205" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -85721,7 +85757,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:203" ht="15">
+    <row r="159" spans="1:205" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -85738,7 +85774,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:203">
+    <row r="160" spans="1:205">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-09 09:46:52
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29103"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2015" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71232AB4-D278-49DB-9B7C-DE4EE1003E43}"/>
+  <xr:revisionPtr revIDLastSave="2068" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7192EBE-3DA8-4A87-955F-8E39B65598A5}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GO130" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GV140" sqref="GV140"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GO46" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GW46" sqref="GW46"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73087,7 +73087,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:203" ht="15">
+    <row r="33" spans="1:205" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73236,7 +73236,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:203" ht="15">
+    <row r="34" spans="1:205" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73385,7 +73385,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:203" ht="15">
+    <row r="35" spans="1:205" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73534,7 +73534,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:203" ht="15">
+    <row r="36" spans="1:205" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73668,7 +73668,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:203" ht="15">
+    <row r="37" spans="1:205" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73802,7 +73802,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:203" ht="15">
+    <row r="38" spans="1:205" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73936,7 +73936,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:203" ht="15">
+    <row r="39" spans="1:205" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74099,7 +74099,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:203" ht="15">
+    <row r="40" spans="1:205" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74262,7 +74262,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:203" ht="15">
+    <row r="41" spans="1:205" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74425,7 +74425,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:203" ht="15">
+    <row r="42" spans="1:205" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74588,7 +74588,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:203" ht="15">
+    <row r="43" spans="1:205" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74751,7 +74751,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:203" ht="15">
+    <row r="44" spans="1:205" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74914,7 +74914,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:203" ht="15">
+    <row r="45" spans="1:205" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75077,7 +75077,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:203" ht="15">
+    <row r="46" spans="1:205" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75240,7 +75240,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:203" ht="15">
+    <row r="47" spans="1:205" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75438,8 +75438,14 @@
       <c r="GU47" s="3">
         <v>24</v>
       </c>
+      <c r="GV47" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:203" ht="15">
+    <row r="48" spans="1:205" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75848,6 +75854,12 @@
       <c r="GU49" s="3">
         <v>24</v>
       </c>
+      <c r="GV49" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW49" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="1:207" ht="15">
       <c r="A50" s="11">
@@ -76680,6 +76692,12 @@
       <c r="GU53" s="3">
         <v>24</v>
       </c>
+      <c r="GV53" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW53" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="1:207" ht="15">
       <c r="A54" s="11">
@@ -76879,6 +76897,12 @@
       <c r="GU54" s="3">
         <v>24</v>
       </c>
+      <c r="GV54" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW54" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="55" spans="1:207" ht="15">
       <c r="A55" s="8">
@@ -78781,7 +78805,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:203" ht="15">
+    <row r="65" spans="1:205" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78930,7 +78954,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:203" ht="15">
+    <row r="66" spans="1:205" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79079,7 +79103,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:203" ht="15">
+    <row r="67" spans="1:205" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79218,7 +79242,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:203" ht="15">
+    <row r="68" spans="1:205" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79365,7 +79389,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:203" ht="15">
+    <row r="69" spans="1:205" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79515,8 +79539,14 @@
       <c r="GU69" s="3">
         <v>24</v>
       </c>
+      <c r="GV69" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW69" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:203" ht="15">
+    <row r="70" spans="1:205" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79679,7 +79709,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:203" ht="15">
+    <row r="71" spans="1:205" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79826,7 +79856,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:203" ht="15">
+    <row r="72" spans="1:205" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -79976,8 +80006,14 @@
       <c r="GU72" s="3">
         <v>24</v>
       </c>
+      <c r="GV72" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:203" ht="15">
+    <row r="73" spans="1:205" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80242,7 +80278,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:203" ht="15">
+    <row r="74" spans="1:205" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80507,7 +80543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:203" ht="15">
+    <row r="75" spans="1:205" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80641,7 +80677,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:203" ht="15">
+    <row r="76" spans="1:205" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80775,7 +80811,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:203" ht="15">
+    <row r="77" spans="1:205" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80909,7 +80945,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:203" ht="15">
+    <row r="78" spans="1:205" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81185,8 +81221,14 @@
       <c r="GU78" s="3">
         <v>24</v>
       </c>
+      <c r="GV78" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:203" ht="15">
+    <row r="79" spans="1:205" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81320,7 +81362,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:203" ht="15">
+    <row r="80" spans="1:205" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81509,7 +81551,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:204" ht="15">
+    <row r="81" spans="1:205" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81550,7 +81592,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:204" ht="15">
+    <row r="82" spans="1:205" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81686,8 +81728,14 @@
       <c r="GU82" s="3">
         <v>24</v>
       </c>
+      <c r="GV82" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:204" ht="15">
+    <row r="83" spans="1:205" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81728,7 +81776,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:204" ht="15">
+    <row r="84" spans="1:205" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81790,7 +81838,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:204" ht="15">
+    <row r="85" spans="1:205" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81885,7 +81933,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:204" ht="15">
+    <row r="86" spans="1:205" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81905,7 +81953,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:204" ht="15">
+    <row r="87" spans="1:205" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81943,7 +81991,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:204" ht="15">
+    <row r="88" spans="1:205" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -81981,7 +82029,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:204" ht="15">
+    <row r="89" spans="1:205" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82040,7 +82088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:204" ht="15">
+    <row r="90" spans="1:205" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82099,7 +82147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:204" ht="15">
+    <row r="91" spans="1:205" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82158,7 +82206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:204" ht="15">
+    <row r="92" spans="1:205" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82217,7 +82265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:204" ht="15">
+    <row r="93" spans="1:205" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82276,7 +82324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:204" ht="15">
+    <row r="94" spans="1:205" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82332,7 +82380,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:204" ht="15">
+    <row r="95" spans="1:205" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82414,8 +82462,14 @@
       <c r="GU95" s="3">
         <v>24</v>
       </c>
+      <c r="GV95" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:204" ht="15">
+    <row r="96" spans="1:205" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82456,7 +82510,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:203" ht="15">
+    <row r="97" spans="1:205" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82497,7 +82551,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:203" ht="15">
+    <row r="98" spans="1:205" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82591,8 +82645,14 @@
       <c r="GU98" s="3">
         <v>24</v>
       </c>
+      <c r="GV98" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:203" ht="15">
+    <row r="99" spans="1:205" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82612,7 +82672,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:203" ht="15">
+    <row r="100" spans="1:205" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82653,7 +82713,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:203" ht="15">
+    <row r="101" spans="1:205" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82694,7 +82754,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:203" ht="15">
+    <row r="102" spans="1:205" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82735,7 +82795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:203" ht="15">
+    <row r="103" spans="1:205" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82776,7 +82836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:203" ht="15">
+    <row r="104" spans="1:205" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82817,7 +82877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:203" ht="15">
+    <row r="105" spans="1:205" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82876,7 +82936,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:203" ht="15">
+    <row r="106" spans="1:205" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82917,7 +82977,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:203" ht="15">
+    <row r="107" spans="1:205" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -83011,8 +83071,14 @@
       <c r="GU107" s="3">
         <v>24</v>
       </c>
+      <c r="GV107" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:203" ht="15">
+    <row r="108" spans="1:205" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83074,7 +83140,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:203" ht="15">
+    <row r="109" spans="1:205" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83094,7 +83160,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:203" ht="15">
+    <row r="110" spans="1:205" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83194,8 +83260,14 @@
       <c r="GU110" s="3">
         <v>24</v>
       </c>
+      <c r="GV110" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW110" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="111" spans="1:203" ht="15">
+    <row r="111" spans="1:205" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83242,7 +83314,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:203" ht="15">
+    <row r="112" spans="1:205" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83310,7 +83382,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:204" ht="15">
+    <row r="113" spans="1:205" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83357,7 +83429,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:204" ht="15">
+    <row r="114" spans="1:205" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83457,8 +83529,14 @@
       <c r="GU114" s="3">
         <v>16</v>
       </c>
+      <c r="GV114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GW114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:204" ht="15">
+    <row r="115" spans="1:205" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83558,8 +83636,14 @@
       <c r="GU115" s="3">
         <v>24</v>
       </c>
+      <c r="GV115" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:204" ht="15">
+    <row r="116" spans="1:205" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83662,8 +83746,14 @@
       <c r="GU116" s="3">
         <v>24</v>
       </c>
+      <c r="GV116" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:204" ht="15">
+    <row r="117" spans="1:205" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83731,7 +83821,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:204" ht="15">
+    <row r="118" spans="1:205" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83802,7 +83892,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:204" ht="15">
+    <row r="119" spans="1:205" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83873,7 +83963,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:204" ht="15">
+    <row r="120" spans="1:205" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -83944,7 +84034,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:204" ht="15">
+    <row r="121" spans="1:205" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -83985,7 +84075,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:204" ht="15">
+    <row r="122" spans="1:205" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -84044,7 +84134,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:204" ht="15">
+    <row r="123" spans="1:205" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -84115,7 +84205,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:204" ht="15">
+    <row r="124" spans="1:205" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -84156,7 +84246,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:204" ht="15">
+    <row r="125" spans="1:205" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84226,8 +84316,14 @@
       <c r="GU125" s="3">
         <v>24</v>
       </c>
+      <c r="GV125" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:204" ht="15">
+    <row r="126" spans="1:205" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84268,7 +84364,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:204" ht="15">
+    <row r="127" spans="1:205" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84309,7 +84405,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:204" ht="15">
+    <row r="128" spans="1:205" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84350,7 +84446,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:204" ht="15">
+    <row r="129" spans="1:205" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -84391,7 +84487,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:204" ht="15">
+    <row r="130" spans="1:205" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -84447,7 +84543,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:204" ht="15">
+    <row r="131" spans="1:205" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -84508,8 +84604,14 @@
       <c r="GU131" s="3">
         <v>24</v>
       </c>
+      <c r="GV131" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:204" ht="15">
+    <row r="132" spans="1:205" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -84570,8 +84672,14 @@
       <c r="GU132" s="3">
         <v>24</v>
       </c>
+      <c r="GV132" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:204" ht="15">
+    <row r="133" spans="1:205" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -84605,8 +84713,14 @@
       <c r="GU133" s="3">
         <v>24</v>
       </c>
+      <c r="GV133" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:204" ht="15">
+    <row r="134" spans="1:205" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -84640,8 +84754,14 @@
       <c r="GU134" s="3">
         <v>24</v>
       </c>
+      <c r="GV134" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:204" ht="15">
+    <row r="135" spans="1:205" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -84681,8 +84801,11 @@
       <c r="GV135" s="3">
         <v>5</v>
       </c>
+      <c r="GW135" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="136" spans="1:204" ht="15">
+    <row r="136" spans="1:205" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -84723,7 +84846,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:204" ht="15">
+    <row r="137" spans="1:205" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -84757,8 +84880,14 @@
       <c r="GU137" s="3">
         <v>24</v>
       </c>
+      <c r="GV137" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW137" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="138" spans="1:204" ht="15">
+    <row r="138" spans="1:205" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -84795,8 +84924,14 @@
       <c r="GU138" s="3">
         <v>24</v>
       </c>
+      <c r="GV138" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW138" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="139" spans="1:204" ht="15">
+    <row r="139" spans="1:205" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -84833,8 +84968,14 @@
       <c r="GU139" s="3">
         <v>24</v>
       </c>
+      <c r="GV139" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW139" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="140" spans="1:204" ht="15">
+    <row r="140" spans="1:205" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -84875,7 +85016,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="141" spans="1:204" ht="15">
+    <row r="141" spans="1:205" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -84916,7 +85057,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="142" spans="1:204" ht="15">
+    <row r="142" spans="1:205" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -84978,7 +85119,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="143" spans="1:204" ht="15">
+    <row r="143" spans="1:205" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -85019,7 +85160,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="144" spans="1:204" ht="15">
+    <row r="144" spans="1:205" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -85841,8 +85982,14 @@
       <c r="GU160" s="3">
         <v>24</v>
       </c>
+      <c r="GV160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:203">
+    <row r="161" spans="1:205">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -85909,8 +86056,14 @@
       <c r="GU161" s="3">
         <v>24</v>
       </c>
+      <c r="GV161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:203">
+    <row r="162" spans="1:205">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -85977,8 +86130,14 @@
       <c r="GU162" s="3">
         <v>24</v>
       </c>
+      <c r="GV162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:203" ht="15">
+    <row r="163" spans="1:205" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -85992,7 +86151,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:203" ht="15">
+    <row r="164" spans="1:205" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -86006,7 +86165,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:203" ht="15">
+    <row r="165" spans="1:205" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -86020,7 +86179,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:203" ht="15">
+    <row r="166" spans="1:205" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -86034,7 +86193,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:203" ht="15">
+    <row r="167" spans="1:205" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -86048,7 +86207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:203" ht="15">
+    <row r="168" spans="1:205" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -86062,7 +86221,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:203" ht="15">
+    <row r="169" spans="1:205" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -86076,7 +86235,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:203" ht="15">
+    <row r="170" spans="1:205" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -86090,7 +86249,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:203" ht="15">
+    <row r="171" spans="1:205" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -86104,7 +86263,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:203" ht="15">
+    <row r="172" spans="1:205" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -86118,7 +86277,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:203" ht="15">
+    <row r="173" spans="1:205" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -86132,7 +86291,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:203" ht="15">
+    <row r="174" spans="1:205" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -86146,7 +86305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:203" ht="15">
+    <row r="175" spans="1:205" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -86160,7 +86319,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:203" ht="15">
+    <row r="176" spans="1:205" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-14 09:50:36
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2068" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7192EBE-3DA8-4A87-955F-8E39B65598A5}"/>
+  <xr:revisionPtr revIDLastSave="2111" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{276A998C-6C84-4972-A6EF-55609CCC6191}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="213">
   <si>
     <t>Module ID</t>
   </si>
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GO46" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GW46" sqref="GW46"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="FS109" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="GL133" sqref="FT110:HC157"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73087,7 +73087,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:205" ht="15">
+    <row r="33" spans="1:210" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73236,7 +73236,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:205" ht="15">
+    <row r="34" spans="1:210" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73385,7 +73385,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:205" ht="15">
+    <row r="35" spans="1:210" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73534,7 +73534,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:205" ht="15">
+    <row r="36" spans="1:210" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73668,7 +73668,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:205" ht="15">
+    <row r="37" spans="1:210" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73802,7 +73802,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:205" ht="15">
+    <row r="38" spans="1:210" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73936,7 +73936,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:205" ht="15">
+    <row r="39" spans="1:210" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74099,7 +74099,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:205" ht="15">
+    <row r="40" spans="1:210" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74262,7 +74262,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:205" ht="15">
+    <row r="41" spans="1:210" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74425,7 +74425,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:205" ht="15">
+    <row r="42" spans="1:210" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74588,7 +74588,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:205" ht="15">
+    <row r="43" spans="1:210" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74751,7 +74751,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:205" ht="15">
+    <row r="44" spans="1:210" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74914,7 +74914,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:205" ht="15">
+    <row r="45" spans="1:210" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75077,7 +75077,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:205" ht="15">
+    <row r="46" spans="1:210" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75240,7 +75240,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:205" ht="15">
+    <row r="47" spans="1:210" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75444,8 +75444,23 @@
       <c r="GW47" s="3">
         <v>24</v>
       </c>
+      <c r="GX47" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY47" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ47" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA47" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:205" ht="15">
+    <row r="48" spans="1:210" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75656,7 +75671,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:207" ht="15">
+    <row r="49" spans="1:210" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75860,8 +75875,23 @@
       <c r="GW49" s="3">
         <v>24</v>
       </c>
+      <c r="GX49" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY49" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ49" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA49" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:207" ht="15">
+    <row r="50" spans="1:210" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -76072,7 +76102,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:207" ht="15">
+    <row r="51" spans="1:210" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76283,7 +76313,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:207" ht="15">
+    <row r="52" spans="1:210" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76494,7 +76524,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:207" ht="15">
+    <row r="53" spans="1:210" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76698,8 +76728,23 @@
       <c r="GW53" s="3">
         <v>24</v>
       </c>
+      <c r="GX53" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY53" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ53" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA53" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:207" ht="15">
+    <row r="54" spans="1:210" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76903,8 +76948,23 @@
       <c r="GW54" s="3">
         <v>24</v>
       </c>
+      <c r="GX54" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY54" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ54" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA54" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:207" ht="15">
+    <row r="55" spans="1:210" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -77097,7 +77157,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:207" ht="15">
+    <row r="56" spans="1:210" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77290,7 +77350,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:207" ht="15">
+    <row r="57" spans="1:210" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77447,7 +77507,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:207" ht="15">
+    <row r="58" spans="1:210" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77612,7 +77672,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:207" ht="15">
+    <row r="59" spans="1:210" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77766,7 +77826,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:207" ht="15">
+    <row r="60" spans="1:210" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77912,7 +77972,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:207" ht="15">
+    <row r="61" spans="1:210" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -78070,7 +78130,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:207" ht="15">
+    <row r="62" spans="1:210" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78315,7 +78375,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:207" ht="15">
+    <row r="63" spans="1:210" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78560,7 +78620,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:207" ht="15">
+    <row r="64" spans="1:210" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78805,7 +78865,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:205" ht="15">
+    <row r="65" spans="1:210" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -78954,7 +79014,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:205" ht="15">
+    <row r="66" spans="1:210" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79103,7 +79163,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:205" ht="15">
+    <row r="67" spans="1:210" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79242,7 +79302,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:205" ht="15">
+    <row r="68" spans="1:210" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79389,7 +79449,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:205" ht="15">
+    <row r="69" spans="1:210" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79545,8 +79605,23 @@
       <c r="GW69" s="3">
         <v>24</v>
       </c>
+      <c r="GX69" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY69" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ69" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA69" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB69" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:205" ht="15">
+    <row r="70" spans="1:210" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79709,7 +79784,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:205" ht="15">
+    <row r="71" spans="1:210" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79856,7 +79931,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:205" ht="15">
+    <row r="72" spans="1:210" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -80012,8 +80087,23 @@
       <c r="GW72" s="3">
         <v>24</v>
       </c>
+      <c r="GX72" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY72" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ72" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA72" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:205" ht="15">
+    <row r="73" spans="1:210" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80278,7 +80368,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:205" ht="15">
+    <row r="74" spans="1:210" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80543,7 +80633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:205" ht="15">
+    <row r="75" spans="1:210" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80677,7 +80767,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:205" ht="15">
+    <row r="76" spans="1:210" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80811,7 +80901,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:205" ht="15">
+    <row r="77" spans="1:210" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -80944,8 +81034,23 @@
       <c r="FH77" s="1"/>
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
+      <c r="GX77" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY77" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ77" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA77" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB77" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="78" spans="1:205" ht="15">
+    <row r="78" spans="1:210" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81227,8 +81332,23 @@
       <c r="GW78" s="3">
         <v>24</v>
       </c>
+      <c r="GX78" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY78" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ78" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA78" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:205" ht="15">
+    <row r="79" spans="1:210" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81362,7 +81482,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:205" ht="15">
+    <row r="80" spans="1:210" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81551,7 +81671,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:205" ht="15">
+    <row r="81" spans="1:210" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81592,7 +81712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:205" ht="15">
+    <row r="82" spans="1:210" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81734,8 +81854,23 @@
       <c r="GW82" s="3">
         <v>24</v>
       </c>
+      <c r="GX82" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY82" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ82" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA82" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:205" ht="15">
+    <row r="83" spans="1:210" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81776,7 +81911,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:205" ht="15">
+    <row r="84" spans="1:210" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81838,7 +81973,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:205" ht="15">
+    <row r="85" spans="1:210" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -81933,7 +82068,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:205" ht="15">
+    <row r="86" spans="1:210" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -81953,7 +82088,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:205" ht="15">
+    <row r="87" spans="1:210" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -81991,7 +82126,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:205" ht="15">
+    <row r="88" spans="1:210" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -82029,7 +82164,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:205" ht="15">
+    <row r="89" spans="1:210" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82088,7 +82223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:205" ht="15">
+    <row r="90" spans="1:210" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82147,7 +82282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:205" ht="15">
+    <row r="91" spans="1:210" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82206,7 +82341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:205" ht="15">
+    <row r="92" spans="1:210" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82265,7 +82400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:205" ht="15">
+    <row r="93" spans="1:210" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82324,7 +82459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:205" ht="15">
+    <row r="94" spans="1:210" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82380,7 +82515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:205" ht="15">
+    <row r="95" spans="1:210" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82468,8 +82603,23 @@
       <c r="GW95" s="3">
         <v>24</v>
       </c>
+      <c r="GX95" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY95" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ95" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA95" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:205" ht="15">
+    <row r="96" spans="1:210" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82510,7 +82660,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:205" ht="15">
+    <row r="97" spans="1:210" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82551,7 +82701,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:205" ht="15">
+    <row r="98" spans="1:210" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82651,8 +82801,23 @@
       <c r="GW98" s="3">
         <v>24</v>
       </c>
+      <c r="GX98" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY98" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ98" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA98" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:205" ht="15">
+    <row r="99" spans="1:210" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82672,7 +82837,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:205" ht="15">
+    <row r="100" spans="1:210" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82713,7 +82878,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:205" ht="15">
+    <row r="101" spans="1:210" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82754,7 +82919,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:205" ht="15">
+    <row r="102" spans="1:210" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82795,7 +82960,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:205" ht="15">
+    <row r="103" spans="1:210" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -82836,7 +83001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:205" ht="15">
+    <row r="104" spans="1:210" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -82877,7 +83042,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:205" ht="15">
+    <row r="105" spans="1:210" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -82936,7 +83101,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:205" ht="15">
+    <row r="106" spans="1:210" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -82977,7 +83142,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:205" ht="15">
+    <row r="107" spans="1:210" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -83077,8 +83242,23 @@
       <c r="GW107" s="3">
         <v>24</v>
       </c>
+      <c r="GX107" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY107" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ107" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA107" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:205" ht="15">
+    <row r="108" spans="1:210" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83140,7 +83320,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:205" ht="15">
+    <row r="109" spans="1:210" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83160,7 +83340,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:205" ht="15">
+    <row r="110" spans="1:210" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83179,6 +83359,9 @@
       <c r="F110" s="13">
         <v>45818</v>
       </c>
+      <c r="P110" s="13">
+        <v>45833</v>
+      </c>
       <c r="FU110" s="3">
         <v>12</v>
       </c>
@@ -83224,50 +83407,11 @@
       <c r="GI110" s="3">
         <v>24</v>
       </c>
-      <c r="GJ110" s="3">
-        <v>23</v>
-      </c>
-      <c r="GK110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GL110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GM110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GN110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GO110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GP110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GQ110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GR110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GS110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GU110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GV110" s="3">
-        <v>24</v>
-      </c>
-      <c r="GW110" s="3">
-        <v>24</v>
+      <c r="GJ110" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:205" ht="15">
+    <row r="111" spans="1:210" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83314,7 +83458,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:205" ht="15">
+    <row r="112" spans="1:210" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83382,7 +83526,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:205" ht="15">
+    <row r="113" spans="1:210" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83429,7 +83573,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:205" ht="15">
+    <row r="114" spans="1:210" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83535,8 +83679,23 @@
       <c r="GW114" s="3">
         <v>16</v>
       </c>
+      <c r="GX114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GY114" s="3">
+        <v>16</v>
+      </c>
+      <c r="GZ114" s="3">
+        <v>16</v>
+      </c>
+      <c r="HA114" s="3">
+        <v>16</v>
+      </c>
+      <c r="HB114" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="115" spans="1:205" ht="15">
+    <row r="115" spans="1:210" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83642,8 +83801,23 @@
       <c r="GW115" s="3">
         <v>24</v>
       </c>
+      <c r="GX115" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY115" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ115" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA115" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:205" ht="15">
+    <row r="116" spans="1:210" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83752,8 +83926,23 @@
       <c r="GW116" s="3">
         <v>24</v>
       </c>
+      <c r="GX116" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY116" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ116" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA116" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:205" ht="15">
+    <row r="117" spans="1:210" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -83821,7 +84010,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:205" ht="15">
+    <row r="118" spans="1:210" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -83892,7 +84081,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:205" ht="15">
+    <row r="119" spans="1:210" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -83963,7 +84152,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:205" ht="15">
+    <row r="120" spans="1:210" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -84034,7 +84223,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:205" ht="15">
+    <row r="121" spans="1:210" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -84075,7 +84264,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:205" ht="15">
+    <row r="122" spans="1:210" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -84134,7 +84323,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:205" ht="15">
+    <row r="123" spans="1:210" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -84205,7 +84394,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:205" ht="15">
+    <row r="124" spans="1:210" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -84246,7 +84435,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:205" ht="15">
+    <row r="125" spans="1:210" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84322,8 +84511,23 @@
       <c r="GW125" s="3">
         <v>24</v>
       </c>
+      <c r="GX125" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY125" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ125" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA125" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:205" ht="15">
+    <row r="126" spans="1:210" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84364,7 +84568,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:205" ht="15">
+    <row r="127" spans="1:210" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84405,7 +84609,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:205" ht="15">
+    <row r="128" spans="1:210" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84446,7 +84650,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:205" ht="15">
+    <row r="129" spans="1:211" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -84487,7 +84691,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:205" ht="15">
+    <row r="130" spans="1:211" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -84543,7 +84747,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:205" ht="15">
+    <row r="131" spans="1:211" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -84610,8 +84814,23 @@
       <c r="GW131" s="3">
         <v>24</v>
       </c>
+      <c r="GX131" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY131" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ131" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA131" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:205" ht="15">
+    <row r="132" spans="1:211" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -84678,8 +84897,23 @@
       <c r="GW132" s="3">
         <v>24</v>
       </c>
+      <c r="GX132" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY132" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ132" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA132" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:205" ht="15">
+    <row r="133" spans="1:211" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -84719,8 +84953,23 @@
       <c r="GW133" s="3">
         <v>24</v>
       </c>
+      <c r="GX133" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY133" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ133" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA133" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:205" ht="15">
+    <row r="134" spans="1:211" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -84760,8 +85009,23 @@
       <c r="GW134" s="3">
         <v>24</v>
       </c>
+      <c r="GX134" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY134" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ134" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA134" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:205" ht="15">
+    <row r="135" spans="1:211" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -84780,6 +85044,9 @@
       <c r="F135" s="13">
         <v>45839</v>
       </c>
+      <c r="P135" s="13">
+        <v>45852</v>
+      </c>
       <c r="GP135" s="3">
         <v>5</v>
       </c>
@@ -84804,8 +85071,26 @@
       <c r="GW135" s="3">
         <v>5</v>
       </c>
+      <c r="GX135" s="3">
+        <v>5</v>
+      </c>
+      <c r="GY135" s="3">
+        <v>5</v>
+      </c>
+      <c r="GZ135" s="3">
+        <v>5</v>
+      </c>
+      <c r="HA135" s="3">
+        <v>5</v>
+      </c>
+      <c r="HB135" s="3">
+        <v>5</v>
+      </c>
+      <c r="HC135" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="136" spans="1:205" ht="15">
+    <row r="136" spans="1:211" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -84846,7 +85131,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:205" ht="15">
+    <row r="137" spans="1:211" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -84886,8 +85171,23 @@
       <c r="GW137" s="3">
         <v>24</v>
       </c>
+      <c r="GX137" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY137" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ137" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA137" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB137" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="138" spans="1:205" ht="15">
+    <row r="138" spans="1:211" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -84930,8 +85230,23 @@
       <c r="GW138" s="3">
         <v>24</v>
       </c>
+      <c r="GX138" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY138" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ138" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA138" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB138" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="139" spans="1:205" ht="15">
+    <row r="139" spans="1:211" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -84974,8 +85289,23 @@
       <c r="GW139" s="3">
         <v>24</v>
       </c>
+      <c r="GX139" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY139" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ139" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA139" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB139" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="140" spans="1:205" ht="15">
+    <row r="140" spans="1:211" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -85016,7 +85346,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="141" spans="1:205" ht="15">
+    <row r="141" spans="1:211" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -85057,7 +85387,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="142" spans="1:205" ht="15">
+    <row r="142" spans="1:211" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -85119,7 +85449,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="143" spans="1:205" ht="15">
+    <row r="143" spans="1:211" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -85160,7 +85490,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="144" spans="1:205" ht="15">
+    <row r="144" spans="1:211" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -85222,7 +85552,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="145" spans="1:205" ht="15">
+    <row r="145" spans="1:210" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -85284,7 +85614,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="146" spans="1:205" ht="15">
+    <row r="146" spans="1:210" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -85325,7 +85655,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="147" spans="1:205" ht="15">
+    <row r="147" spans="1:210" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -85387,7 +85717,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:205" ht="15">
+    <row r="148" spans="1:210" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -85428,7 +85758,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:205" ht="15">
+    <row r="149" spans="1:210" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -85490,7 +85820,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:205" ht="15">
+    <row r="150" spans="1:210" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -85531,7 +85861,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="151" spans="1:205" ht="15">
+    <row r="151" spans="1:210" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -85572,7 +85902,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="152" spans="1:205" ht="15">
+    <row r="152" spans="1:210" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -85634,7 +85964,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="153" spans="1:205" ht="15">
+    <row r="153" spans="1:210" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -85696,7 +86026,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="154" spans="1:205" ht="15">
+    <row r="154" spans="1:210" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -85737,7 +86067,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:205" ht="15">
+    <row r="155" spans="1:210" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -85778,7 +86108,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="156" spans="1:205" ht="15">
+    <row r="156" spans="1:210" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -85819,7 +86149,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="1:205" ht="15">
+    <row r="157" spans="1:210" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -85881,7 +86211,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="158" spans="1:205" ht="15">
+    <row r="158" spans="1:210" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -85898,7 +86228,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:205" ht="15">
+    <row r="159" spans="1:210" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -85915,7 +86245,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:205">
+    <row r="160" spans="1:210">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -85988,8 +86318,23 @@
       <c r="GW160" s="3">
         <v>24</v>
       </c>
+      <c r="GX160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY160" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ160" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA160" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:205">
+    <row r="161" spans="1:210">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -86062,8 +86407,23 @@
       <c r="GW161" s="3">
         <v>24</v>
       </c>
+      <c r="GX161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY161" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ161" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA161" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:205">
+    <row r="162" spans="1:210">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -86136,8 +86496,23 @@
       <c r="GW162" s="3">
         <v>24</v>
       </c>
+      <c r="GX162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY162" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ162" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA162" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:205" ht="15">
+    <row r="163" spans="1:210" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -86151,7 +86526,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:205" ht="15">
+    <row r="164" spans="1:210" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -86165,7 +86540,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:205" ht="15">
+    <row r="165" spans="1:210" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -86179,7 +86554,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:205" ht="15">
+    <row r="166" spans="1:210" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -86193,7 +86568,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:205" ht="15">
+    <row r="167" spans="1:210" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -86207,7 +86582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:205" ht="15">
+    <row r="168" spans="1:210" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -86221,7 +86596,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:205" ht="15">
+    <row r="169" spans="1:210" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -86235,7 +86610,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:205" ht="15">
+    <row r="170" spans="1:210" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -86249,7 +86624,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:205" ht="15">
+    <row r="171" spans="1:210" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -86263,7 +86638,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:205" ht="15">
+    <row r="172" spans="1:210" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -86277,7 +86652,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:205" ht="15">
+    <row r="173" spans="1:210" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -86291,7 +86666,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:205" ht="15">
+    <row r="174" spans="1:210" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -86305,7 +86680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:205" ht="15">
+    <row r="175" spans="1:210" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -86319,7 +86694,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:205" ht="15">
+    <row r="176" spans="1:210" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-15 09:51:20
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2111" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{276A998C-6C84-4972-A6EF-55609CCC6191}"/>
+  <xr:revisionPtr revIDLastSave="2145" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC06B49D-37BB-4A4F-9F83-A3380E2407A1}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="213">
   <si>
     <t>Module ID</t>
   </si>
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:XFD185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="FS109" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="GL133" sqref="FT110:HC157"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GW154" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="HC154" sqref="HC154"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73087,7 +73087,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:210" ht="15">
+    <row r="33" spans="1:211" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73236,7 +73236,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:210" ht="15">
+    <row r="34" spans="1:211" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73385,7 +73385,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:210" ht="15">
+    <row r="35" spans="1:211" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73534,7 +73534,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:210" ht="15">
+    <row r="36" spans="1:211" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73668,7 +73668,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:210" ht="15">
+    <row r="37" spans="1:211" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73802,7 +73802,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:210" ht="15">
+    <row r="38" spans="1:211" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73936,7 +73936,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:210" ht="15">
+    <row r="39" spans="1:211" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74099,7 +74099,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:210" ht="15">
+    <row r="40" spans="1:211" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74262,7 +74262,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:210" ht="15">
+    <row r="41" spans="1:211" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74425,7 +74425,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:210" ht="15">
+    <row r="42" spans="1:211" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74588,7 +74588,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:210" ht="15">
+    <row r="43" spans="1:211" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74751,7 +74751,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:210" ht="15">
+    <row r="44" spans="1:211" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74914,7 +74914,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:210" ht="15">
+    <row r="45" spans="1:211" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75077,7 +75077,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:210" ht="15">
+    <row r="46" spans="1:211" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75240,7 +75240,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:210" ht="15">
+    <row r="47" spans="1:211" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75459,8 +75459,11 @@
       <c r="HB47" s="3">
         <v>24</v>
       </c>
+      <c r="HC47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:210" ht="15">
+    <row r="48" spans="1:211" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75671,7 +75674,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:210" ht="15">
+    <row r="49" spans="1:211" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75890,8 +75893,11 @@
       <c r="HB49" s="3">
         <v>24</v>
       </c>
+      <c r="HC49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:210" ht="15">
+    <row r="50" spans="1:211" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -76102,7 +76108,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:210" ht="15">
+    <row r="51" spans="1:211" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76313,7 +76319,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:210" ht="15">
+    <row r="52" spans="1:211" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76524,7 +76530,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:210" ht="15">
+    <row r="53" spans="1:211" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76743,8 +76749,11 @@
       <c r="HB53" s="3">
         <v>24</v>
       </c>
+      <c r="HC53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:210" ht="15">
+    <row r="54" spans="1:211" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -76963,8 +76972,11 @@
       <c r="HB54" s="3">
         <v>24</v>
       </c>
+      <c r="HC54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:210" ht="15">
+    <row r="55" spans="1:211" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -77157,7 +77169,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:210" ht="15">
+    <row r="56" spans="1:211" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77350,7 +77362,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:210" ht="15">
+    <row r="57" spans="1:211" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77507,7 +77519,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:210" ht="15">
+    <row r="58" spans="1:211" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77672,7 +77684,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:210" ht="15">
+    <row r="59" spans="1:211" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77826,7 +77838,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:210" ht="15">
+    <row r="60" spans="1:211" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -77972,7 +77984,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:210" ht="15">
+    <row r="61" spans="1:211" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -78130,7 +78142,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:210" ht="15">
+    <row r="62" spans="1:211" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78375,7 +78387,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:210" ht="15">
+    <row r="63" spans="1:211" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78620,7 +78632,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:210" ht="15">
+    <row r="64" spans="1:211" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78865,7 +78877,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:210" ht="15">
+    <row r="65" spans="1:211" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -79014,7 +79026,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:210" ht="15">
+    <row r="66" spans="1:211" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79163,7 +79175,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:210" ht="15">
+    <row r="67" spans="1:211" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79302,7 +79314,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:210" ht="15">
+    <row r="68" spans="1:211" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79449,7 +79461,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:210" ht="15">
+    <row r="69" spans="1:211" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79620,8 +79632,11 @@
       <c r="HB69" s="3">
         <v>24</v>
       </c>
+      <c r="HC69" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:210" ht="15">
+    <row r="70" spans="1:211" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79784,7 +79799,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:210" ht="15">
+    <row r="71" spans="1:211" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79931,7 +79946,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:210" ht="15">
+    <row r="72" spans="1:211" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -80102,8 +80117,11 @@
       <c r="HB72" s="3">
         <v>24</v>
       </c>
+      <c r="HC72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:210" ht="15">
+    <row r="73" spans="1:211" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80368,7 +80386,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:210" ht="15">
+    <row r="74" spans="1:211" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80633,7 +80651,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:210" ht="15">
+    <row r="75" spans="1:211" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80767,7 +80785,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:210" ht="15">
+    <row r="76" spans="1:211" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80901,7 +80919,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:210" ht="15">
+    <row r="77" spans="1:211" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -81049,8 +81067,11 @@
       <c r="HB77" s="3">
         <v>24</v>
       </c>
+      <c r="HC77" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="78" spans="1:210" ht="15">
+    <row r="78" spans="1:211" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81347,8 +81368,11 @@
       <c r="HB78" s="3">
         <v>24</v>
       </c>
+      <c r="HC78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:210" ht="15">
+    <row r="79" spans="1:211" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81482,7 +81506,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:210" ht="15">
+    <row r="80" spans="1:211" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81671,7 +81695,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:210" ht="15">
+    <row r="81" spans="1:211" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81712,7 +81736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:210" ht="15">
+    <row r="82" spans="1:211" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81869,8 +81893,11 @@
       <c r="HB82" s="3">
         <v>24</v>
       </c>
+      <c r="HC82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:210" ht="15">
+    <row r="83" spans="1:211" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81911,7 +81938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:210" ht="15">
+    <row r="84" spans="1:211" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -81973,7 +82000,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:210" ht="15">
+    <row r="85" spans="1:211" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -82068,7 +82095,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:210" ht="15">
+    <row r="86" spans="1:211" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -82088,7 +82115,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:210" ht="15">
+    <row r="87" spans="1:211" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -82126,7 +82153,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:210" ht="15">
+    <row r="88" spans="1:211" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -82164,7 +82191,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:210" ht="15">
+    <row r="89" spans="1:211" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82223,7 +82250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:210" ht="15">
+    <row r="90" spans="1:211" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82282,7 +82309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:210" ht="15">
+    <row r="91" spans="1:211" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82341,7 +82368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:210" ht="15">
+    <row r="92" spans="1:211" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82400,7 +82427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:210" ht="15">
+    <row r="93" spans="1:211" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82459,7 +82486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:210" ht="15">
+    <row r="94" spans="1:211" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82515,7 +82542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:210" ht="15">
+    <row r="95" spans="1:211" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82618,8 +82645,11 @@
       <c r="HB95" s="3">
         <v>24</v>
       </c>
+      <c r="HC95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:210" ht="15">
+    <row r="96" spans="1:211" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82660,7 +82690,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:210" ht="15">
+    <row r="97" spans="1:211" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82701,7 +82731,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:210" ht="15">
+    <row r="98" spans="1:211" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82816,8 +82846,11 @@
       <c r="HB98" s="3">
         <v>24</v>
       </c>
+      <c r="HC98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:210" ht="15">
+    <row r="99" spans="1:211" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82837,7 +82870,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:210" ht="15">
+    <row r="100" spans="1:211" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82878,7 +82911,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:210" ht="15">
+    <row r="101" spans="1:211" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82918,8 +82951,11 @@
       <c r="FV101" s="3">
         <v>24</v>
       </c>
+      <c r="FW101" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="102" spans="1:210" ht="15">
+    <row r="102" spans="1:211" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -82959,8 +82995,11 @@
       <c r="FV102" s="3">
         <v>24</v>
       </c>
+      <c r="FW102" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="103" spans="1:210" ht="15">
+    <row r="103" spans="1:211" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -83000,8 +83039,11 @@
       <c r="FV103" s="3">
         <v>24</v>
       </c>
+      <c r="FW103" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="104" spans="1:210" ht="15">
+    <row r="104" spans="1:211" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -83041,8 +83083,11 @@
       <c r="FV104" s="3">
         <v>24</v>
       </c>
+      <c r="FW104" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="105" spans="1:210" ht="15">
+    <row r="105" spans="1:211" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -83101,7 +83146,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:210" ht="15">
+    <row r="106" spans="1:211" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -83142,7 +83187,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:210" ht="15">
+    <row r="107" spans="1:211" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -83257,8 +83302,11 @@
       <c r="HB107" s="3">
         <v>24</v>
       </c>
+      <c r="HC107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:210" ht="15">
+    <row r="108" spans="1:211" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83320,7 +83368,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:210" ht="15">
+    <row r="109" spans="1:211" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83340,7 +83388,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:210" ht="15">
+    <row r="110" spans="1:211" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83411,7 +83459,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:210" ht="15">
+    <row r="111" spans="1:211" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83458,7 +83506,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:210" ht="15">
+    <row r="112" spans="1:211" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83526,7 +83574,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:210" ht="15">
+    <row r="113" spans="1:211" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83573,7 +83621,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:210" ht="15">
+    <row r="114" spans="1:211" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83592,6 +83640,9 @@
       <c r="F114" s="13">
         <v>45818</v>
       </c>
+      <c r="P114" s="13">
+        <v>45836</v>
+      </c>
       <c r="FU114" s="3">
         <v>10</v>
       </c>
@@ -83649,53 +83700,11 @@
       <c r="GM114" s="3">
         <v>16</v>
       </c>
-      <c r="GN114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GO114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GP114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GQ114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GR114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GS114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GT114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GU114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GV114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GW114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GX114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GY114" s="3">
-        <v>16</v>
-      </c>
-      <c r="GZ114" s="3">
-        <v>16</v>
-      </c>
-      <c r="HA114" s="3">
-        <v>16</v>
-      </c>
-      <c r="HB114" s="3">
-        <v>16</v>
+      <c r="GN114" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="115" spans="1:210" ht="15">
+    <row r="115" spans="1:211" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83816,8 +83825,11 @@
       <c r="HB115" s="3">
         <v>24</v>
       </c>
+      <c r="HC115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:210" ht="15">
+    <row r="116" spans="1:211" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83941,8 +83953,11 @@
       <c r="HB116" s="3">
         <v>24</v>
       </c>
+      <c r="HC116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:210" ht="15">
+    <row r="117" spans="1:211" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -84010,7 +84025,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:210" ht="15">
+    <row r="118" spans="1:211" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -84081,7 +84096,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:210" ht="15">
+    <row r="119" spans="1:211" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -84152,7 +84167,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:210" ht="15">
+    <row r="120" spans="1:211" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -84223,7 +84238,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:210" ht="15">
+    <row r="121" spans="1:211" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -84264,7 +84279,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:210" ht="15">
+    <row r="122" spans="1:211" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -84323,7 +84338,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:210" ht="15">
+    <row r="123" spans="1:211" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -84394,7 +84409,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:210" ht="15">
+    <row r="124" spans="1:211" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -84435,7 +84450,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:210" ht="15">
+    <row r="125" spans="1:211" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84526,8 +84541,11 @@
       <c r="HB125" s="3">
         <v>24</v>
       </c>
+      <c r="HC125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:210" ht="15">
+    <row r="126" spans="1:211" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84568,7 +84586,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:210" ht="15">
+    <row r="127" spans="1:211" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84609,7 +84627,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:210" ht="15">
+    <row r="128" spans="1:211" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84829,6 +84847,9 @@
       <c r="HB131" s="3">
         <v>24</v>
       </c>
+      <c r="HC131" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="132" spans="1:211" ht="15">
       <c r="A132" s="9">
@@ -84912,6 +84933,9 @@
       <c r="HB132" s="3">
         <v>24</v>
       </c>
+      <c r="HC132" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="133" spans="1:211" ht="15">
       <c r="A133" s="9">
@@ -84968,6 +84992,9 @@
       <c r="HB133" s="3">
         <v>24</v>
       </c>
+      <c r="HC133" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="134" spans="1:211" ht="15">
       <c r="A134" s="9">
@@ -85024,6 +85051,9 @@
       <c r="HB134" s="3">
         <v>24</v>
       </c>
+      <c r="HC134" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="135" spans="1:211" ht="15">
       <c r="A135" s="9">
@@ -85186,6 +85216,9 @@
       <c r="HB137" s="3">
         <v>24</v>
       </c>
+      <c r="HC137" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="138" spans="1:211" ht="15">
       <c r="A138" s="9">
@@ -85245,6 +85278,9 @@
       <c r="HB138" s="3">
         <v>24</v>
       </c>
+      <c r="HC138" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="139" spans="1:211" ht="15">
       <c r="A139" s="9">
@@ -85304,6 +85340,9 @@
       <c r="HB139" s="3">
         <v>24</v>
       </c>
+      <c r="HC139" s="3">
+        <v>24</v>
+      </c>
     </row>
     <row r="140" spans="1:211" ht="15">
       <c r="A140" s="9">
@@ -85552,7 +85591,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="145" spans="1:210" ht="15">
+    <row r="145" spans="1:211" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -85614,7 +85653,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="146" spans="1:210" ht="15">
+    <row r="146" spans="1:211" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -85655,7 +85694,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="147" spans="1:210" ht="15">
+    <row r="147" spans="1:211" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -85717,7 +85756,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:210" ht="15">
+    <row r="148" spans="1:211" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -85758,7 +85797,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:210" ht="15">
+    <row r="149" spans="1:211" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -85820,7 +85859,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:210" ht="15">
+    <row r="150" spans="1:211" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -85861,7 +85900,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="151" spans="1:210" ht="15">
+    <row r="151" spans="1:211" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -85902,7 +85941,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="152" spans="1:210" ht="15">
+    <row r="152" spans="1:211" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -85964,7 +86003,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="153" spans="1:210" ht="15">
+    <row r="153" spans="1:211" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -86026,7 +86065,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="154" spans="1:210" ht="15">
+    <row r="154" spans="1:211" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -86067,7 +86106,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:210" ht="15">
+    <row r="155" spans="1:211" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -86108,7 +86147,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="156" spans="1:210" ht="15">
+    <row r="156" spans="1:211" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -86149,7 +86188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="1:210" ht="15">
+    <row r="157" spans="1:211" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -86211,7 +86250,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="158" spans="1:210" ht="15">
+    <row r="158" spans="1:211" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -86228,7 +86267,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:210" ht="15">
+    <row r="159" spans="1:211" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -86245,7 +86284,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:210">
+    <row r="160" spans="1:211">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -86333,8 +86372,11 @@
       <c r="HB160" s="3">
         <v>24</v>
       </c>
+      <c r="HC160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:210">
+    <row r="161" spans="1:211">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -86422,8 +86464,11 @@
       <c r="HB161" s="3">
         <v>24</v>
       </c>
+      <c r="HC161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:210">
+    <row r="162" spans="1:211">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -86511,8 +86556,11 @@
       <c r="HB162" s="3">
         <v>24</v>
       </c>
+      <c r="HC162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:210" ht="15">
+    <row r="163" spans="1:211" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -86526,7 +86574,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:210" ht="15">
+    <row r="164" spans="1:211" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -86540,7 +86588,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:210" ht="15">
+    <row r="165" spans="1:211" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -86554,7 +86602,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:210" ht="15">
+    <row r="166" spans="1:211" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -86568,7 +86616,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:210" ht="15">
+    <row r="167" spans="1:211" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -86582,7 +86630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:210" ht="15">
+    <row r="168" spans="1:211" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -86596,7 +86644,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:210" ht="15">
+    <row r="169" spans="1:211" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -86610,7 +86658,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:210" ht="15">
+    <row r="170" spans="1:211" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -86624,7 +86672,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:210" ht="15">
+    <row r="171" spans="1:211" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -86638,7 +86686,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:210" ht="15">
+    <row r="172" spans="1:211" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -86652,7 +86700,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:210" ht="15">
+    <row r="173" spans="1:211" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -86666,7 +86714,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:210" ht="15">
+    <row r="174" spans="1:211" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -86680,7 +86728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:210" ht="15">
+    <row r="175" spans="1:211" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -86694,7 +86742,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:210" ht="15">
+    <row r="176" spans="1:211" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-16 09:49:22
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2145" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC06B49D-37BB-4A4F-9F83-A3380E2407A1}"/>
+  <xr:revisionPtr revIDLastSave="2157" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4709B61-5420-429B-979C-696B7A894F1F}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="217">
   <si>
     <t>Module ID</t>
   </si>
@@ -676,6 +676,18 @@
   <si>
     <t>Sunsure HYPERSOL Internal Reliability Tests (DH1000+SML)</t>
   </si>
+  <si>
+    <t>VSL202425229</t>
+  </si>
+  <si>
+    <t>Yingfa M10R Hypersol cell trial</t>
+  </si>
+  <si>
+    <t>VSL202425275</t>
+  </si>
+  <si>
+    <t>Aiko M10R Hypersol cell trial</t>
+  </si>
 </sst>
 </file>
 
@@ -1209,11 +1221,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD185"/>
+  <dimension ref="A1:XFD187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GW154" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="HC154" sqref="HC154"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GW179" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C187" sqref="C187"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -86882,6 +86894,40 @@
         <v>96</v>
       </c>
     </row>
+    <row r="186" spans="1:5" ht="15">
+      <c r="A186" s="9">
+        <v>23881328</v>
+      </c>
+      <c r="B186" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C186" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D186" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E186" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="15">
+      <c r="A187" s="9">
+        <v>24206642</v>
+      </c>
+      <c r="B187" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C187" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D187" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E187" s="9">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-16 10:50:27
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2157" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4709B61-5420-429B-979C-696B7A894F1F}"/>
+  <xr:revisionPtr revIDLastSave="2176" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ECEAD5A-93B2-48B3-B336-947955C7193A}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="226">
   <si>
     <t>Module ID</t>
   </si>
@@ -688,6 +688,33 @@
   <si>
     <t>Aiko M10R Hypersol cell trial</t>
   </si>
+  <si>
+    <t>VSL202526202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reflective Bus Ribbon Module (Yourbest- 5X0.4MM Moddle, 4X0.35MM Top &amp; Bottom) </t>
+  </si>
+  <si>
+    <t>VSL202526199</t>
+  </si>
+  <si>
+    <t>IPQC PID Test Modules : Jul '25</t>
+  </si>
+  <si>
+    <t>VSL202526200</t>
+  </si>
+  <si>
+    <t>VSL202526197</t>
+  </si>
+  <si>
+    <t>VSL202526198</t>
+  </si>
+  <si>
+    <t>VSL202526203</t>
+  </si>
+  <si>
+    <t>VSL202526204</t>
+  </si>
 </sst>
 </file>
 
@@ -1221,11 +1248,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD187"/>
+  <dimension ref="A1:XFD194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GW179" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C187" sqref="C187"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GQ184" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E195" sqref="E195"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -86928,6 +86955,125 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="188" spans="1:5" ht="15">
+      <c r="A188" s="9">
+        <v>25518469</v>
+      </c>
+      <c r="B188" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C188" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="D188" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E188" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="15">
+      <c r="A189" s="9">
+        <v>25523456</v>
+      </c>
+      <c r="B189" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C189" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E189" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="15">
+      <c r="A190" s="9">
+        <v>25522727</v>
+      </c>
+      <c r="B190" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C190" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D190" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E190" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="15">
+      <c r="A191" s="9">
+        <v>25507484</v>
+      </c>
+      <c r="B191" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C191" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D191" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E191" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="15">
+      <c r="A192" s="9">
+        <v>25517884</v>
+      </c>
+      <c r="B192" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C192" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D192" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E192" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="15">
+      <c r="A193" s="9">
+        <v>25394757</v>
+      </c>
+      <c r="B193" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C193" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D193" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E193" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" ht="15">
+      <c r="A194" s="9">
+        <v>25394035</v>
+      </c>
+      <c r="B194" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C194" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D194" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E194" s="9">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="xgRXRhGb3a6LEzLQv2CvT5VifmJIVP/5aJfbwcyQgzfHfKqm43h32oh3YZlrvYLfi298yVKsTO3jH53XVuIMbA==" saltValue="MRz+oK6mjgMDrxefnFfuWw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-17 05:18:06
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2176" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ECEAD5A-93B2-48B3-B336-947955C7193A}"/>
+  <xr:revisionPtr revIDLastSave="2220" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B546600D-35C7-47E2-AB88-FFE3F410D345}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1251,8 +1251,8 @@
   <dimension ref="A1:XFD194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GQ184" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E195" sqref="E195"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="GY2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="HE1" sqref="A1:XFD194"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73126,7 +73126,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:211" ht="15">
+    <row r="33" spans="1:213" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73275,7 +73275,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:211" ht="15">
+    <row r="34" spans="1:213" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73424,7 +73424,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:211" ht="15">
+    <row r="35" spans="1:213" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73573,7 +73573,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:211" ht="15">
+    <row r="36" spans="1:213" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73707,7 +73707,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:211" ht="15">
+    <row r="37" spans="1:213" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73841,7 +73841,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:211" ht="15">
+    <row r="38" spans="1:213" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73975,7 +73975,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:211" ht="15">
+    <row r="39" spans="1:213" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74138,7 +74138,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:211" ht="15">
+    <row r="40" spans="1:213" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74301,7 +74301,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:211" ht="15">
+    <row r="41" spans="1:213" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74464,7 +74464,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:211" ht="15">
+    <row r="42" spans="1:213" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74627,7 +74627,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:211" ht="15">
+    <row r="43" spans="1:213" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74790,7 +74790,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:211" ht="15">
+    <row r="44" spans="1:213" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74953,7 +74953,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:211" ht="15">
+    <row r="45" spans="1:213" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75116,7 +75116,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:211" ht="15">
+    <row r="46" spans="1:213" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75279,7 +75279,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:211" ht="15">
+    <row r="47" spans="1:213" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75501,8 +75501,14 @@
       <c r="HC47" s="3">
         <v>24</v>
       </c>
+      <c r="HD47" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:211" ht="15">
+    <row r="48" spans="1:213" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75713,7 +75719,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:211" ht="15">
+    <row r="49" spans="1:213" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75935,8 +75941,14 @@
       <c r="HC49" s="3">
         <v>24</v>
       </c>
+      <c r="HD49" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:211" ht="15">
+    <row r="50" spans="1:213" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -76147,7 +76159,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:211" ht="15">
+    <row r="51" spans="1:213" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76358,7 +76370,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:211" ht="15">
+    <row r="52" spans="1:213" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76569,7 +76581,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:211" ht="15">
+    <row r="53" spans="1:213" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76791,8 +76803,14 @@
       <c r="HC53" s="3">
         <v>24</v>
       </c>
+      <c r="HD53" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:211" ht="15">
+    <row r="54" spans="1:213" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -77014,8 +77032,14 @@
       <c r="HC54" s="3">
         <v>24</v>
       </c>
+      <c r="HD54" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:211" ht="15">
+    <row r="55" spans="1:213" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -77208,7 +77232,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:211" ht="15">
+    <row r="56" spans="1:213" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77401,7 +77425,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:211" ht="15">
+    <row r="57" spans="1:213" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77558,7 +77582,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:211" ht="15">
+    <row r="58" spans="1:213" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77723,7 +77747,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:211" ht="15">
+    <row r="59" spans="1:213" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77877,7 +77901,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:211" ht="15">
+    <row r="60" spans="1:213" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -78023,7 +78047,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:211" ht="15">
+    <row r="61" spans="1:213" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -78181,7 +78205,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:211" ht="15">
+    <row r="62" spans="1:213" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78426,7 +78450,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:211" ht="15">
+    <row r="63" spans="1:213" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78671,7 +78695,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:211" ht="15">
+    <row r="64" spans="1:213" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78916,7 +78940,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:211" ht="15">
+    <row r="65" spans="1:213" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -79065,7 +79089,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:211" ht="15">
+    <row r="66" spans="1:213" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79214,7 +79238,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:211" ht="15">
+    <row r="67" spans="1:213" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79353,7 +79377,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:211" ht="15">
+    <row r="68" spans="1:213" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79500,7 +79524,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:211" ht="15">
+    <row r="69" spans="1:213" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79674,8 +79698,14 @@
       <c r="HC69" s="3">
         <v>24</v>
       </c>
+      <c r="HD69" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE69" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:211" ht="15">
+    <row r="70" spans="1:213" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79838,7 +79868,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:211" ht="15">
+    <row r="71" spans="1:213" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -79985,7 +80015,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:211" ht="15">
+    <row r="72" spans="1:213" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -80159,8 +80189,14 @@
       <c r="HC72" s="3">
         <v>24</v>
       </c>
+      <c r="HD72" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:211" ht="15">
+    <row r="73" spans="1:213" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80425,7 +80461,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:211" ht="15">
+    <row r="74" spans="1:213" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80690,7 +80726,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:211" ht="15">
+    <row r="75" spans="1:213" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80824,7 +80860,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:211" ht="15">
+    <row r="76" spans="1:213" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -80958,7 +80994,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:211" ht="15">
+    <row r="77" spans="1:213" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -81109,8 +81145,14 @@
       <c r="HC77" s="3">
         <v>24</v>
       </c>
+      <c r="HD77" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE77" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="78" spans="1:211" ht="15">
+    <row r="78" spans="1:213" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81410,8 +81452,14 @@
       <c r="HC78" s="3">
         <v>24</v>
       </c>
+      <c r="HD78" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE78" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="79" spans="1:211" ht="15">
+    <row r="79" spans="1:213" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81545,7 +81593,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:211" ht="15">
+    <row r="80" spans="1:213" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81734,7 +81782,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:211" ht="15">
+    <row r="81" spans="1:213" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81775,7 +81823,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:211" ht="15">
+    <row r="82" spans="1:213" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -81935,8 +81983,14 @@
       <c r="HC82" s="3">
         <v>24</v>
       </c>
+      <c r="HD82" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE82" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="83" spans="1:211" ht="15">
+    <row r="83" spans="1:213" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -81977,7 +82031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:211" ht="15">
+    <row r="84" spans="1:213" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -82039,7 +82093,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:211" ht="15">
+    <row r="85" spans="1:213" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -82134,7 +82188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:211" ht="15">
+    <row r="86" spans="1:213" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -82154,7 +82208,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:211" ht="15">
+    <row r="87" spans="1:213" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -82192,7 +82246,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:211" ht="15">
+    <row r="88" spans="1:213" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -82230,7 +82284,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:211" ht="15">
+    <row r="89" spans="1:213" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82289,7 +82343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:211" ht="15">
+    <row r="90" spans="1:213" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82348,7 +82402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:211" ht="15">
+    <row r="91" spans="1:213" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82407,7 +82461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:211" ht="15">
+    <row r="92" spans="1:213" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82466,7 +82520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:211" ht="15">
+    <row r="93" spans="1:213" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82525,7 +82579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:211" ht="15">
+    <row r="94" spans="1:213" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82581,7 +82635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:211" ht="15">
+    <row r="95" spans="1:213" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82687,8 +82741,14 @@
       <c r="HC95" s="3">
         <v>24</v>
       </c>
+      <c r="HD95" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:211" ht="15">
+    <row r="96" spans="1:213" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82729,7 +82789,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:211" ht="15">
+    <row r="97" spans="1:213" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82770,7 +82830,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" spans="1:211" ht="15">
+    <row r="98" spans="1:213" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82888,8 +82948,14 @@
       <c r="HC98" s="3">
         <v>24</v>
       </c>
+      <c r="HD98" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:211" ht="15">
+    <row r="99" spans="1:213" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82909,7 +82975,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="100" spans="1:211" ht="15">
+    <row r="100" spans="1:213" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -82950,7 +83016,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:211" ht="15">
+    <row r="101" spans="1:213" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -82994,7 +83060,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="102" spans="1:211" ht="15">
+    <row r="102" spans="1:213" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -83038,7 +83104,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="103" spans="1:211" ht="15">
+    <row r="103" spans="1:213" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -83082,7 +83148,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="104" spans="1:211" ht="15">
+    <row r="104" spans="1:213" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -83126,7 +83192,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="105" spans="1:211" ht="15">
+    <row r="105" spans="1:213" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -83185,7 +83251,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:211" ht="15">
+    <row r="106" spans="1:213" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -83226,7 +83292,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:211" ht="15">
+    <row r="107" spans="1:213" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -83344,8 +83410,14 @@
       <c r="HC107" s="3">
         <v>24</v>
       </c>
+      <c r="HD107" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:211" ht="15">
+    <row r="108" spans="1:213" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83407,7 +83479,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:211" ht="15">
+    <row r="109" spans="1:213" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83427,7 +83499,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:211" ht="15">
+    <row r="110" spans="1:213" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83498,7 +83570,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" spans="1:211" ht="15">
+    <row r="111" spans="1:213" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83545,7 +83617,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" spans="1:211" ht="15">
+    <row r="112" spans="1:213" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83613,7 +83685,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:211" ht="15">
+    <row r="113" spans="1:213" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83660,7 +83732,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" spans="1:211" ht="15">
+    <row r="114" spans="1:213" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83743,7 +83815,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="115" spans="1:211" ht="15">
+    <row r="115" spans="1:213" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83867,8 +83939,14 @@
       <c r="HC115" s="3">
         <v>24</v>
       </c>
+      <c r="HD115" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:211" ht="15">
+    <row r="116" spans="1:213" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -83995,8 +84073,14 @@
       <c r="HC116" s="3">
         <v>24</v>
       </c>
+      <c r="HD116" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:211" ht="15">
+    <row r="117" spans="1:213" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -84064,7 +84148,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:211" ht="15">
+    <row r="118" spans="1:213" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -84135,7 +84219,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:211" ht="15">
+    <row r="119" spans="1:213" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -84206,7 +84290,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:211" ht="15">
+    <row r="120" spans="1:213" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -84277,7 +84361,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:211" ht="15">
+    <row r="121" spans="1:213" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -84318,7 +84402,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:211" ht="15">
+    <row r="122" spans="1:213" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -84377,7 +84461,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:211" ht="15">
+    <row r="123" spans="1:213" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -84448,7 +84532,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:211" ht="15">
+    <row r="124" spans="1:213" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -84489,7 +84573,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:211" ht="15">
+    <row r="125" spans="1:213" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84583,8 +84667,14 @@
       <c r="HC125" s="3">
         <v>24</v>
       </c>
+      <c r="HD125" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:211" ht="15">
+    <row r="126" spans="1:213" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84625,7 +84715,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:211" ht="15">
+    <row r="127" spans="1:213" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84666,7 +84756,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:211" ht="15">
+    <row r="128" spans="1:213" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84707,7 +84797,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" spans="1:211" ht="15">
+    <row r="129" spans="1:213" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -84748,7 +84838,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:211" ht="15">
+    <row r="130" spans="1:213" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -84804,7 +84894,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" spans="1:211" ht="15">
+    <row r="131" spans="1:213" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -84889,8 +84979,14 @@
       <c r="HC131" s="3">
         <v>24</v>
       </c>
+      <c r="HD131" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:211" ht="15">
+    <row r="132" spans="1:213" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -84975,8 +85071,14 @@
       <c r="HC132" s="3">
         <v>24</v>
       </c>
+      <c r="HD132" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:211" ht="15">
+    <row r="133" spans="1:213" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -85034,8 +85136,14 @@
       <c r="HC133" s="3">
         <v>24</v>
       </c>
+      <c r="HD133" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:211" ht="15">
+    <row r="134" spans="1:213" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -85093,8 +85201,14 @@
       <c r="HC134" s="3">
         <v>24</v>
       </c>
+      <c r="HD134" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:211" ht="15">
+    <row r="135" spans="1:213" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -85159,7 +85273,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="136" spans="1:211" ht="15">
+    <row r="136" spans="1:213" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -85200,7 +85314,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:211" ht="15">
+    <row r="137" spans="1:213" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -85258,8 +85372,11 @@
       <c r="HC137" s="3">
         <v>24</v>
       </c>
+      <c r="HD137" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="138" spans="1:211" ht="15">
+    <row r="138" spans="1:213" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -85320,8 +85437,11 @@
       <c r="HC138" s="3">
         <v>24</v>
       </c>
+      <c r="HD138" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="139" spans="1:211" ht="15">
+    <row r="139" spans="1:213" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -85382,8 +85502,11 @@
       <c r="HC139" s="3">
         <v>24</v>
       </c>
+      <c r="HD139" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="140" spans="1:211" ht="15">
+    <row r="140" spans="1:213" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -85424,7 +85547,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="141" spans="1:211" ht="15">
+    <row r="141" spans="1:213" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -85465,7 +85588,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="142" spans="1:211" ht="15">
+    <row r="142" spans="1:213" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -85527,7 +85650,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="143" spans="1:211" ht="15">
+    <row r="143" spans="1:213" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -85568,7 +85691,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="144" spans="1:211" ht="15">
+    <row r="144" spans="1:213" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -85630,7 +85753,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="145" spans="1:211" ht="15">
+    <row r="145" spans="1:212" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -85692,7 +85815,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="146" spans="1:211" ht="15">
+    <row r="146" spans="1:212" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -85733,7 +85856,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="147" spans="1:211" ht="15">
+    <row r="147" spans="1:212" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -85795,7 +85918,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:211" ht="15">
+    <row r="148" spans="1:212" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -85836,7 +85959,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" spans="1:211" ht="15">
+    <row r="149" spans="1:212" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -85898,7 +86021,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="150" spans="1:211" ht="15">
+    <row r="150" spans="1:212" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -85939,7 +86062,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="151" spans="1:211" ht="15">
+    <row r="151" spans="1:212" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -85980,7 +86103,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="152" spans="1:211" ht="15">
+    <row r="152" spans="1:212" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -86042,7 +86165,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="153" spans="1:211" ht="15">
+    <row r="153" spans="1:212" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -86104,7 +86227,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="154" spans="1:211" ht="15">
+    <row r="154" spans="1:212" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -86145,7 +86268,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="155" spans="1:211" ht="15">
+    <row r="155" spans="1:212" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -86186,7 +86309,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="156" spans="1:211" ht="15">
+    <row r="156" spans="1:212" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -86227,7 +86350,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="1:211" ht="15">
+    <row r="157" spans="1:212" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -86289,7 +86412,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="158" spans="1:211" ht="15">
+    <row r="158" spans="1:212" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -86306,7 +86429,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:211" ht="15">
+    <row r="159" spans="1:212" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -86323,7 +86446,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:211">
+    <row r="160" spans="1:212">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -86414,8 +86537,11 @@
       <c r="HC160" s="3">
         <v>24</v>
       </c>
+      <c r="HD160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:211">
+    <row r="161" spans="1:212">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -86506,8 +86632,11 @@
       <c r="HC161" s="3">
         <v>24</v>
       </c>
+      <c r="HD161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:211">
+    <row r="162" spans="1:212">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -86598,8 +86727,11 @@
       <c r="HC162" s="3">
         <v>24</v>
       </c>
+      <c r="HD162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:211" ht="15">
+    <row r="163" spans="1:212" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -86613,7 +86745,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:211" ht="15">
+    <row r="164" spans="1:212" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -86627,7 +86759,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:211" ht="15">
+    <row r="165" spans="1:212" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -86641,7 +86773,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:211" ht="15">
+    <row r="166" spans="1:212" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -86655,7 +86787,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:211" ht="15">
+    <row r="167" spans="1:212" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -86669,7 +86801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:211" ht="15">
+    <row r="168" spans="1:212" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -86683,7 +86815,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:211" ht="15">
+    <row r="169" spans="1:212" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -86697,7 +86829,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:211" ht="15">
+    <row r="170" spans="1:212" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -86711,7 +86843,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:211" ht="15">
+    <row r="171" spans="1:212" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -86725,7 +86857,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:211" ht="15">
+    <row r="172" spans="1:212" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -86739,7 +86871,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:211" ht="15">
+    <row r="173" spans="1:212" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -86753,7 +86885,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:211" ht="15">
+    <row r="174" spans="1:212" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -86767,7 +86899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:211" ht="15">
+    <row r="175" spans="1:212" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -86781,7 +86913,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:211" ht="15">
+    <row r="176" spans="1:212" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-21 07:04:38
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2220" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B546600D-35C7-47E2-AB88-FFE3F410D345}"/>
+  <xr:revisionPtr revIDLastSave="2277" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ADC30BE-921D-4D53-B848-BA840145C836}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="226">
   <si>
     <t>Module ID</t>
   </si>
@@ -302,6 +302,9 @@
     <t>M10R HYPERSOL (GA INFRA)</t>
   </si>
   <si>
+    <t>END</t>
+  </si>
+  <si>
     <t>VSL202425371</t>
   </si>
   <si>
@@ -396,9 +399,6 @@
   </si>
   <si>
     <t>VSL202526009</t>
-  </si>
-  <si>
-    <t>END</t>
   </si>
   <si>
     <t>VSL202425378</t>
@@ -1251,8 +1251,8 @@
   <dimension ref="A1:XFD194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="GY2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="HE1" sqref="A1:XFD194"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="HA84" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="HI98" sqref="HI98"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73126,7 +73126,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:213" ht="15">
+    <row r="33" spans="1:217" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73275,7 +73275,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:213" ht="15">
+    <row r="34" spans="1:217" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73424,7 +73424,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:213" ht="15">
+    <row r="35" spans="1:217" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73573,7 +73573,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:213" ht="15">
+    <row r="36" spans="1:217" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73707,7 +73707,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:213" ht="15">
+    <row r="37" spans="1:217" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73841,7 +73841,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:213" ht="15">
+    <row r="38" spans="1:217" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73975,7 +73975,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:213" ht="15">
+    <row r="39" spans="1:217" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74138,7 +74138,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:213" ht="15">
+    <row r="40" spans="1:217" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74301,7 +74301,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:213" ht="15">
+    <row r="41" spans="1:217" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74464,7 +74464,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:213" ht="15">
+    <row r="42" spans="1:217" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74627,7 +74627,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:213" ht="15">
+    <row r="43" spans="1:217" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74790,7 +74790,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:213" ht="15">
+    <row r="44" spans="1:217" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74953,7 +74953,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:213" ht="15">
+    <row r="45" spans="1:217" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75116,7 +75116,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:213" ht="15">
+    <row r="46" spans="1:217" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75279,7 +75279,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:213" ht="15">
+    <row r="47" spans="1:217" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75507,8 +75507,20 @@
       <c r="HE47" s="3">
         <v>24</v>
       </c>
+      <c r="HF47" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG47" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH47" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:213" ht="15">
+    <row r="48" spans="1:217" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75719,7 +75731,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:213" ht="15">
+    <row r="49" spans="1:217" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75947,8 +75959,20 @@
       <c r="HE49" s="3">
         <v>24</v>
       </c>
+      <c r="HF49" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG49" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH49" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:213" ht="15">
+    <row r="50" spans="1:217" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -76159,7 +76183,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:213" ht="15">
+    <row r="51" spans="1:217" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76370,7 +76394,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:213" ht="15">
+    <row r="52" spans="1:217" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76581,7 +76605,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:213" ht="15">
+    <row r="53" spans="1:217" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76809,8 +76833,20 @@
       <c r="HE53" s="3">
         <v>24</v>
       </c>
+      <c r="HF53" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG53" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH53" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:213" ht="15">
+    <row r="54" spans="1:217" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -77038,8 +77074,20 @@
       <c r="HE54" s="3">
         <v>24</v>
       </c>
+      <c r="HF54" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG54" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH54" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:213" ht="15">
+    <row r="55" spans="1:217" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -77232,7 +77280,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:213" ht="15">
+    <row r="56" spans="1:217" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77425,7 +77473,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:213" ht="15">
+    <row r="57" spans="1:217" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77582,7 +77630,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:213" ht="15">
+    <row r="58" spans="1:217" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77747,7 +77795,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:213" ht="15">
+    <row r="59" spans="1:217" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77765,6 +77813,9 @@
       </c>
       <c r="F59" s="12">
         <v>45749</v>
+      </c>
+      <c r="P59" s="13">
+        <v>45757</v>
       </c>
       <c r="AY59" s="1"/>
       <c r="AZ59" s="1"/>
@@ -77850,7 +77901,9 @@
       <c r="DL59" s="1">
         <v>24</v>
       </c>
-      <c r="DM59" s="1"/>
+      <c r="DM59" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="DN59" s="1"/>
       <c r="DO59" s="1"/>
       <c r="DP59" s="1"/>
@@ -77901,12 +77954,12 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:213" ht="15">
+    <row r="60" spans="1:217" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>87</v>
@@ -77919,6 +77972,9 @@
       </c>
       <c r="F60" s="12">
         <v>45749</v>
+      </c>
+      <c r="P60" s="13">
+        <v>45753</v>
       </c>
       <c r="AY60" s="1"/>
       <c r="AZ60" s="1"/>
@@ -77992,7 +78048,9 @@
       <c r="DH60" s="1">
         <v>16</v>
       </c>
-      <c r="DI60" s="1"/>
+      <c r="DI60" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="DJ60" s="1"/>
       <c r="DK60" s="1"/>
       <c r="DL60" s="1"/>
@@ -78047,12 +78105,12 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:213" ht="15">
+    <row r="61" spans="1:217" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>87</v>
@@ -78205,7 +78263,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:213" ht="15">
+    <row r="62" spans="1:217" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78450,7 +78508,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:213" ht="15">
+    <row r="63" spans="1:217" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78695,7 +78753,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:213" ht="15">
+    <row r="64" spans="1:217" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78940,7 +78998,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:213" ht="15">
+    <row r="65" spans="1:217" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -79089,7 +79147,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:213" ht="15">
+    <row r="66" spans="1:217" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79238,15 +79296,15 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:213" ht="15">
+    <row r="67" spans="1:217" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>32</v>
@@ -79377,15 +79435,15 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:213" ht="15">
+    <row r="68" spans="1:217" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
       <c r="B68" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>18</v>
@@ -79524,15 +79582,15 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:213" ht="15">
+    <row r="69" spans="1:217" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>28</v>
@@ -79704,16 +79762,28 @@
       <c r="HE69" s="3">
         <v>24</v>
       </c>
+      <c r="HF69" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG69" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH69" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI69" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:213" ht="15">
+    <row r="70" spans="1:217" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>32</v>
@@ -79868,15 +79938,15 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:213" ht="15">
+    <row r="71" spans="1:217" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
       <c r="B71" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>18</v>
@@ -80015,15 +80085,15 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:213" ht="15">
+    <row r="72" spans="1:217" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>28</v>
@@ -80195,16 +80265,28 @@
       <c r="HE72" s="3">
         <v>24</v>
       </c>
+      <c r="HF72" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG72" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH72" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:213" ht="15">
+    <row r="73" spans="1:217" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>28</v>
@@ -80458,18 +80540,18 @@
         <v>5</v>
       </c>
       <c r="FV73" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:213" ht="15">
+    <row r="74" spans="1:217" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>28</v>
@@ -80723,21 +80805,21 @@
         <v>5</v>
       </c>
       <c r="FV74" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:213" ht="15">
+    <row r="75" spans="1:217" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E75" s="8">
         <v>96</v>
@@ -80860,15 +80942,15 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:213" ht="15">
+    <row r="76" spans="1:217" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>18</v>
@@ -80994,18 +81076,18 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:213" ht="15">
+    <row r="77" spans="1:217" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E77" s="8">
         <v>162</v>
@@ -81127,40 +81209,16 @@
       <c r="FH77" s="1"/>
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
-      <c r="GX77" s="3">
-        <v>24</v>
-      </c>
-      <c r="GY77" s="3">
-        <v>24</v>
-      </c>
-      <c r="GZ77" s="3">
-        <v>24</v>
-      </c>
-      <c r="HA77" s="3">
-        <v>24</v>
-      </c>
-      <c r="HB77" s="3">
-        <v>24</v>
-      </c>
-      <c r="HC77" s="3">
-        <v>24</v>
-      </c>
-      <c r="HD77" s="3">
-        <v>24</v>
-      </c>
-      <c r="HE77" s="3">
-        <v>24</v>
-      </c>
     </row>
-    <row r="78" spans="1:213" ht="15">
+    <row r="78" spans="1:217" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>28</v>
@@ -81170,6 +81228,9 @@
       </c>
       <c r="F78" s="12">
         <v>45793</v>
+      </c>
+      <c r="P78" s="13">
+        <v>45840</v>
       </c>
       <c r="AY78" s="1"/>
       <c r="AZ78" s="1"/>
@@ -81411,63 +81472,21 @@
         <v>24</v>
       </c>
       <c r="GP78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GQ78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GR78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GS78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GT78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GU78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GV78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GW78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GX78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GY78" s="3">
-        <v>24</v>
-      </c>
-      <c r="GZ78" s="3">
-        <v>24</v>
-      </c>
-      <c r="HA78" s="3">
-        <v>24</v>
-      </c>
-      <c r="HB78" s="3">
-        <v>24</v>
-      </c>
-      <c r="HC78" s="3">
-        <v>24</v>
-      </c>
-      <c r="HD78" s="3">
-        <v>24</v>
-      </c>
-      <c r="HE78" s="3">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="GQ78" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:213" ht="15">
+    <row r="79" spans="1:217" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
       <c r="B79" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>28</v>
@@ -81593,15 +81612,15 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:213" ht="15">
+    <row r="80" spans="1:217" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>21</v>
@@ -81782,15 +81801,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:213" ht="15">
+    <row r="81" spans="1:217" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>18</v>
@@ -81823,15 +81842,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:213" ht="15">
+    <row r="82" spans="1:217" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>28</v>
@@ -81842,6 +81861,9 @@
       <c r="F82" s="13">
         <v>45806</v>
       </c>
+      <c r="P82" s="13">
+        <v>45852</v>
+      </c>
       <c r="FI82" s="3">
         <v>11</v>
       </c>
@@ -81983,22 +82005,19 @@
       <c r="HC82" s="3">
         <v>24</v>
       </c>
-      <c r="HD82" s="3">
-        <v>24</v>
-      </c>
-      <c r="HE82" s="3">
-        <v>24</v>
+      <c r="HD82" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:213" ht="15">
+    <row r="83" spans="1:217" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>18</v>
@@ -82031,15 +82050,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:213" ht="15">
+    <row r="84" spans="1:217" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
       <c r="B84" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>32</v>
@@ -82090,10 +82109,10 @@
         <v>5</v>
       </c>
       <c r="GJ84" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:213" ht="15">
+    <row r="85" spans="1:217" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -82101,7 +82120,7 @@
         <v>121</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>21</v>
@@ -82185,10 +82204,10 @@
         <v>208</v>
       </c>
       <c r="FR85" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:213" ht="15">
+    <row r="86" spans="1:217" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -82208,12 +82227,12 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:213" ht="15">
+    <row r="87" spans="1:217" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C87" s="17" t="s">
         <v>124</v>
@@ -82246,12 +82265,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:213" ht="15">
+    <row r="88" spans="1:217" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C88" s="17" t="s">
         <v>125</v>
@@ -82284,7 +82303,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:213" ht="15">
+    <row r="89" spans="1:217" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82343,7 +82362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:213" ht="15">
+    <row r="90" spans="1:217" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82402,7 +82421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:213" ht="15">
+    <row r="91" spans="1:217" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82461,7 +82480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:213" ht="15">
+    <row r="92" spans="1:217" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82520,7 +82539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:213" ht="15">
+    <row r="93" spans="1:217" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82528,7 +82547,7 @@
         <v>132</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>32</v>
@@ -82579,7 +82598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:213" ht="15">
+    <row r="94" spans="1:217" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82635,7 +82654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:213" ht="15">
+    <row r="95" spans="1:217" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82747,8 +82766,20 @@
       <c r="HE95" s="3">
         <v>24</v>
       </c>
+      <c r="HF95" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG95" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH95" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:213" ht="15">
+    <row r="96" spans="1:217" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82786,10 +82817,10 @@
         <v>19</v>
       </c>
       <c r="GB96" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:213" ht="15">
+    <row r="97" spans="1:217" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82827,10 +82858,10 @@
         <v>19</v>
       </c>
       <c r="GB97" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:213" ht="15">
+    <row r="98" spans="1:217" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82954,8 +82985,20 @@
       <c r="HE98" s="3">
         <v>24</v>
       </c>
+      <c r="HF98" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG98" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH98" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:213" ht="15">
+    <row r="99" spans="1:217" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -82974,16 +83017,133 @@
       <c r="F99" s="18">
         <v>45820</v>
       </c>
+      <c r="FW99" s="3">
+        <v>7</v>
+      </c>
+      <c r="FX99" s="3">
+        <v>24</v>
+      </c>
+      <c r="FY99" s="3">
+        <v>22</v>
+      </c>
+      <c r="FZ99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GA99" s="3">
+        <v>22</v>
+      </c>
+      <c r="GB99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GC99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GD99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GE99" s="3">
+        <v>23</v>
+      </c>
+      <c r="GF99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GG99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GH99" s="3">
+        <v>23</v>
+      </c>
+      <c r="GI99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GJ99" s="3">
+        <v>23</v>
+      </c>
+      <c r="GK99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GL99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GM99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GN99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GO99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GP99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GQ99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GR99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GS99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GT99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GU99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GV99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GW99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GX99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GY99" s="3">
+        <v>24</v>
+      </c>
+      <c r="GZ99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HA99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HB99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HC99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HD99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HE99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HF99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI99" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="100" spans="1:213" ht="15">
+    <row r="100" spans="1:217" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>18</v>
@@ -83013,10 +83173,10 @@
         <v>17</v>
       </c>
       <c r="GF100" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:213" ht="15">
+    <row r="101" spans="1:217" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -83057,10 +83217,10 @@
         <v>24</v>
       </c>
       <c r="FW101" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:213" ht="15">
+    <row r="102" spans="1:217" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -83101,10 +83261,10 @@
         <v>24</v>
       </c>
       <c r="FW102" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="103" spans="1:213" ht="15">
+    <row r="103" spans="1:217" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -83145,10 +83305,10 @@
         <v>24</v>
       </c>
       <c r="FW103" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:213" ht="15">
+    <row r="104" spans="1:217" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -83189,10 +83349,10 @@
         <v>24</v>
       </c>
       <c r="FW104" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:213" ht="15">
+    <row r="105" spans="1:217" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -83248,10 +83408,10 @@
         <v>5</v>
       </c>
       <c r="GJ105" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="106" spans="1:213" ht="15">
+    <row r="106" spans="1:217" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -83289,10 +83449,10 @@
         <v>19</v>
       </c>
       <c r="GB106" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="107" spans="1:213" ht="15">
+    <row r="107" spans="1:217" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -83416,8 +83576,20 @@
       <c r="HE107" s="3">
         <v>24</v>
       </c>
+      <c r="HF107" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG107" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH107" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:213" ht="15">
+    <row r="108" spans="1:217" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83476,10 +83648,10 @@
         <v>5</v>
       </c>
       <c r="GJ108" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:213" ht="15">
+    <row r="109" spans="1:217" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83499,7 +83671,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:213" ht="15">
+    <row r="110" spans="1:217" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83567,10 +83739,10 @@
         <v>24</v>
       </c>
       <c r="GJ110" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="111" spans="1:213" ht="15">
+    <row r="111" spans="1:217" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83614,10 +83786,10 @@
         <v>10</v>
       </c>
       <c r="GB111" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="112" spans="1:213" ht="15">
+    <row r="112" spans="1:217" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83682,10 +83854,10 @@
         <v>5</v>
       </c>
       <c r="GI112" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="113" spans="1:213" ht="15">
+    <row r="113" spans="1:217" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83729,10 +83901,10 @@
         <v>10</v>
       </c>
       <c r="GB113" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="114" spans="1:213" ht="15">
+    <row r="114" spans="1:217" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83812,10 +83984,10 @@
         <v>16</v>
       </c>
       <c r="GN114" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="115" spans="1:213" ht="15">
+    <row r="115" spans="1:217" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -83945,8 +84117,20 @@
       <c r="HE115" s="3">
         <v>24</v>
       </c>
+      <c r="HF115" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG115" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH115" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:213" ht="15">
+    <row r="116" spans="1:217" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -84079,8 +84263,20 @@
       <c r="HE116" s="3">
         <v>24</v>
       </c>
+      <c r="HF116" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG116" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH116" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:213" ht="15">
+    <row r="117" spans="1:217" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -84145,10 +84341,10 @@
         <v>5</v>
       </c>
       <c r="GI117" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:213" ht="15">
+    <row r="118" spans="1:217" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -84216,10 +84412,10 @@
         <v>5</v>
       </c>
       <c r="GI118" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:213" ht="15">
+    <row r="119" spans="1:217" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -84287,10 +84483,10 @@
         <v>5</v>
       </c>
       <c r="GI119" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="120" spans="1:213" ht="15">
+    <row r="120" spans="1:217" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -84358,15 +84554,15 @@
         <v>5</v>
       </c>
       <c r="GI120" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="121" spans="1:213" ht="15">
+    <row r="121" spans="1:217" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C121" s="17" t="s">
         <v>162</v>
@@ -84399,10 +84595,10 @@
         <v>17</v>
       </c>
       <c r="GF121" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="122" spans="1:213" ht="15">
+    <row r="122" spans="1:217" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -84458,10 +84654,10 @@
         <v>24</v>
       </c>
       <c r="GH122" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="123" spans="1:213" ht="15">
+    <row r="123" spans="1:217" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -84532,7 +84728,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:213" ht="15">
+    <row r="124" spans="1:217" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -84570,10 +84766,10 @@
         <v>19</v>
       </c>
       <c r="GJ124" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="125" spans="1:213" ht="15">
+    <row r="125" spans="1:217" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84673,8 +84869,20 @@
       <c r="HE125" s="3">
         <v>24</v>
       </c>
+      <c r="HF125" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG125" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH125" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:213" ht="15">
+    <row r="126" spans="1:217" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84712,10 +84920,10 @@
         <v>14</v>
       </c>
       <c r="GD126" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="127" spans="1:213" ht="15">
+    <row r="127" spans="1:217" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84753,10 +84961,10 @@
         <v>14</v>
       </c>
       <c r="GD127" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="128" spans="1:213" ht="15">
+    <row r="128" spans="1:217" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -84794,10 +85002,10 @@
         <v>14</v>
       </c>
       <c r="GD128" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="129" spans="1:213" ht="15">
+    <row r="129" spans="1:217" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -84835,18 +85043,18 @@
         <v>14</v>
       </c>
       <c r="GD129" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="130" spans="1:213" ht="15">
+    <row r="130" spans="1:217" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D130" s="9" t="s">
         <v>25</v>
@@ -84891,10 +85099,10 @@
         <v>24</v>
       </c>
       <c r="GN130" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="131" spans="1:213" ht="15">
+    <row r="131" spans="1:217" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -84985,8 +85193,20 @@
       <c r="HE131" s="3">
         <v>24</v>
       </c>
+      <c r="HF131" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG131" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH131" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:213" ht="15">
+    <row r="132" spans="1:217" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -85077,8 +85297,20 @@
       <c r="HE132" s="3">
         <v>24</v>
       </c>
+      <c r="HF132" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG132" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH132" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:213" ht="15">
+    <row r="133" spans="1:217" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -85142,8 +85374,20 @@
       <c r="HE133" s="3">
         <v>24</v>
       </c>
+      <c r="HF133" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG133" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH133" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:213" ht="15">
+    <row r="134" spans="1:217" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -85207,8 +85451,20 @@
       <c r="HE134" s="3">
         <v>24</v>
       </c>
+      <c r="HF134" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG134" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH134" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:213" ht="15">
+    <row r="135" spans="1:217" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -85270,10 +85526,10 @@
         <v>5</v>
       </c>
       <c r="HC135" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="136" spans="1:213" ht="15">
+    <row r="136" spans="1:217" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -85311,10 +85567,10 @@
         <v>16</v>
       </c>
       <c r="GV136" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="137" spans="1:213" ht="15">
+    <row r="137" spans="1:217" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -85375,8 +85631,23 @@
       <c r="HD137" s="3">
         <v>24</v>
       </c>
+      <c r="HE137" s="3">
+        <v>24</v>
+      </c>
+      <c r="HF137" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG137" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH137" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI137" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="138" spans="1:213" ht="15">
+    <row r="138" spans="1:217" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -85395,6 +85666,9 @@
       <c r="F138" s="13">
         <v>45839</v>
       </c>
+      <c r="P138" s="13">
+        <v>45857</v>
+      </c>
       <c r="GP138" s="3">
         <v>12</v>
       </c>
@@ -85440,8 +85714,20 @@
       <c r="HD138" s="3">
         <v>24</v>
       </c>
+      <c r="HE138" s="3">
+        <v>24</v>
+      </c>
+      <c r="HF138" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG138" s="3">
+        <v>4</v>
+      </c>
+      <c r="HH138" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="139" spans="1:213" ht="15">
+    <row r="139" spans="1:217" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -85460,6 +85746,9 @@
       <c r="F139" s="13">
         <v>45839</v>
       </c>
+      <c r="P139" s="13">
+        <v>45857</v>
+      </c>
       <c r="GP139" s="3">
         <v>12</v>
       </c>
@@ -85505,8 +85794,20 @@
       <c r="HD139" s="3">
         <v>24</v>
       </c>
+      <c r="HE139" s="3">
+        <v>24</v>
+      </c>
+      <c r="HF139" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG139" s="3">
+        <v>4</v>
+      </c>
+      <c r="HH139" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="140" spans="1:213" ht="15">
+    <row r="140" spans="1:217" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -85544,10 +85845,10 @@
         <v>12</v>
       </c>
       <c r="GU140" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="141" spans="1:213" ht="15">
+    <row r="141" spans="1:217" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -85585,10 +85886,10 @@
         <v>12</v>
       </c>
       <c r="GU141" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:213" ht="15">
+    <row r="142" spans="1:217" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -85647,10 +85948,10 @@
         <v>5</v>
       </c>
       <c r="GV142" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="143" spans="1:213" ht="15">
+    <row r="143" spans="1:217" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -85688,10 +85989,10 @@
         <v>14</v>
       </c>
       <c r="GO143" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="144" spans="1:213" ht="15">
+    <row r="144" spans="1:217" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -85750,10 +86051,10 @@
         <v>5</v>
       </c>
       <c r="GV144" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="145" spans="1:212" ht="15">
+    <row r="145" spans="1:217" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -85812,10 +86113,10 @@
         <v>5</v>
       </c>
       <c r="GV145" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="146" spans="1:212" ht="15">
+    <row r="146" spans="1:217" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -85853,10 +86154,10 @@
         <v>14</v>
       </c>
       <c r="GO146" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="147" spans="1:212" ht="15">
+    <row r="147" spans="1:217" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -85915,10 +86216,10 @@
         <v>5</v>
       </c>
       <c r="GV147" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="148" spans="1:212" ht="15">
+    <row r="148" spans="1:217" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -85956,10 +86257,10 @@
         <v>14</v>
       </c>
       <c r="GO148" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="149" spans="1:212" ht="15">
+    <row r="149" spans="1:217" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -86018,10 +86319,10 @@
         <v>5</v>
       </c>
       <c r="GW149" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="150" spans="1:212" ht="15">
+    <row r="150" spans="1:217" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -86059,10 +86360,10 @@
         <v>14</v>
       </c>
       <c r="GO150" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="151" spans="1:212" ht="15">
+    <row r="151" spans="1:217" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -86100,10 +86401,10 @@
         <v>14</v>
       </c>
       <c r="GT151" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="152" spans="1:212" ht="15">
+    <row r="152" spans="1:217" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -86162,10 +86463,10 @@
         <v>5</v>
       </c>
       <c r="GW152" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="153" spans="1:212" ht="15">
+    <row r="153" spans="1:217" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -86224,10 +86525,10 @@
         <v>5</v>
       </c>
       <c r="GW153" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="154" spans="1:212" ht="15">
+    <row r="154" spans="1:217" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -86265,10 +86566,10 @@
         <v>14</v>
       </c>
       <c r="GT154" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="155" spans="1:212" ht="15">
+    <row r="155" spans="1:217" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -86306,10 +86607,10 @@
         <v>14</v>
       </c>
       <c r="GT155" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="156" spans="1:212" ht="15">
+    <row r="156" spans="1:217" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -86347,10 +86648,10 @@
         <v>14</v>
       </c>
       <c r="GT156" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="157" spans="1:212" ht="15">
+    <row r="157" spans="1:217" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -86409,10 +86710,10 @@
         <v>5</v>
       </c>
       <c r="GW157" s="3" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="158" spans="1:212" ht="15">
+    <row r="158" spans="1:217" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -86429,7 +86730,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:212" ht="15">
+    <row r="159" spans="1:217" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -86446,7 +86747,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:212">
+    <row r="160" spans="1:217">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -86540,8 +86841,23 @@
       <c r="HD160" s="3">
         <v>24</v>
       </c>
+      <c r="HE160" s="3">
+        <v>24</v>
+      </c>
+      <c r="HF160" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG160" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH160" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:212">
+    <row r="161" spans="1:217">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -86635,8 +86951,23 @@
       <c r="HD161" s="3">
         <v>24</v>
       </c>
+      <c r="HE161" s="3">
+        <v>24</v>
+      </c>
+      <c r="HF161" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG161" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH161" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:212">
+    <row r="162" spans="1:217">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -86730,8 +87061,23 @@
       <c r="HD162" s="3">
         <v>24</v>
       </c>
+      <c r="HE162" s="3">
+        <v>24</v>
+      </c>
+      <c r="HF162" s="3">
+        <v>24</v>
+      </c>
+      <c r="HG162" s="3">
+        <v>24</v>
+      </c>
+      <c r="HH162" s="3">
+        <v>24</v>
+      </c>
+      <c r="HI162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:212" ht="15">
+    <row r="163" spans="1:217" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -86745,7 +87091,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:212" ht="15">
+    <row r="164" spans="1:217" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -86759,7 +87105,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:212" ht="15">
+    <row r="165" spans="1:217" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -86773,7 +87119,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:212" ht="15">
+    <row r="166" spans="1:217" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -86787,7 +87133,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:212" ht="15">
+    <row r="167" spans="1:217" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -86801,7 +87147,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:212" ht="15">
+    <row r="168" spans="1:217" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -86815,7 +87161,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:212" ht="15">
+    <row r="169" spans="1:217" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -86829,7 +87175,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:212" ht="15">
+    <row r="170" spans="1:217" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -86843,7 +87189,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:212" ht="15">
+    <row r="171" spans="1:217" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -86857,7 +87203,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:212" ht="15">
+    <row r="172" spans="1:217" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -86871,7 +87217,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:212" ht="15">
+    <row r="173" spans="1:217" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -86885,7 +87231,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:212" ht="15">
+    <row r="174" spans="1:217" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -86899,7 +87245,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:212" ht="15">
+    <row r="175" spans="1:217" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -86913,7 +87259,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:212" ht="15">
+    <row r="176" spans="1:217" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-22 09:49:14
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2277" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ADC30BE-921D-4D53-B848-BA840145C836}"/>
+  <xr:revisionPtr revIDLastSave="2304" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77E7FD3E-38B2-445C-A7B3-9DC5D7CAD38E}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1251,8 +1251,8 @@
   <dimension ref="A1:XFD194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="HA84" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="HI98" sqref="HI98"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="HF177" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="HJ189" sqref="HJ189"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73126,7 +73126,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:217" ht="15">
+    <row r="33" spans="1:218" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73275,7 +73275,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:217" ht="15">
+    <row r="34" spans="1:218" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73424,7 +73424,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:217" ht="15">
+    <row r="35" spans="1:218" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73573,7 +73573,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:217" ht="15">
+    <row r="36" spans="1:218" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73707,7 +73707,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:217" ht="15">
+    <row r="37" spans="1:218" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73841,7 +73841,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:217" ht="15">
+    <row r="38" spans="1:218" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73975,7 +73975,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:217" ht="15">
+    <row r="39" spans="1:218" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74138,7 +74138,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:217" ht="15">
+    <row r="40" spans="1:218" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74301,7 +74301,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:217" ht="15">
+    <row r="41" spans="1:218" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74464,7 +74464,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:217" ht="15">
+    <row r="42" spans="1:218" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74627,7 +74627,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:217" ht="15">
+    <row r="43" spans="1:218" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74790,7 +74790,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:217" ht="15">
+    <row r="44" spans="1:218" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74953,7 +74953,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:217" ht="15">
+    <row r="45" spans="1:218" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75116,7 +75116,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:217" ht="15">
+    <row r="46" spans="1:218" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75279,7 +75279,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:217" ht="15">
+    <row r="47" spans="1:218" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75519,8 +75519,11 @@
       <c r="HI47" s="3">
         <v>24</v>
       </c>
+      <c r="HJ47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:217" ht="15">
+    <row r="48" spans="1:218" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75731,7 +75734,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:217" ht="15">
+    <row r="49" spans="1:218" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75971,8 +75974,11 @@
       <c r="HI49" s="3">
         <v>24</v>
       </c>
+      <c r="HJ49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:217" ht="15">
+    <row r="50" spans="1:218" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -76183,7 +76189,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:217" ht="15">
+    <row r="51" spans="1:218" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76394,7 +76400,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:217" ht="15">
+    <row r="52" spans="1:218" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76605,7 +76611,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:217" ht="15">
+    <row r="53" spans="1:218" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76845,8 +76851,11 @@
       <c r="HI53" s="3">
         <v>24</v>
       </c>
+      <c r="HJ53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:217" ht="15">
+    <row r="54" spans="1:218" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -77086,8 +77095,11 @@
       <c r="HI54" s="3">
         <v>24</v>
       </c>
+      <c r="HJ54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:217" ht="15">
+    <row r="55" spans="1:218" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -77280,7 +77292,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:217" ht="15">
+    <row r="56" spans="1:218" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77473,7 +77485,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:217" ht="15">
+    <row r="57" spans="1:218" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77630,7 +77642,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:217" ht="15">
+    <row r="58" spans="1:218" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77795,7 +77807,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:217" ht="15">
+    <row r="59" spans="1:218" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77954,7 +77966,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:217" ht="15">
+    <row r="60" spans="1:218" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -78105,7 +78117,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:217" ht="15">
+    <row r="61" spans="1:218" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -78263,7 +78275,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:217" ht="15">
+    <row r="62" spans="1:218" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78508,7 +78520,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:217" ht="15">
+    <row r="63" spans="1:218" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78753,7 +78765,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:217" ht="15">
+    <row r="64" spans="1:218" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -78998,7 +79010,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:217" ht="15">
+    <row r="65" spans="1:218" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -79147,7 +79159,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:217" ht="15">
+    <row r="66" spans="1:218" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79296,7 +79308,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:217" ht="15">
+    <row r="67" spans="1:218" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79435,7 +79447,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:217" ht="15">
+    <row r="68" spans="1:218" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79582,7 +79594,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:217" ht="15">
+    <row r="69" spans="1:218" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79774,8 +79786,11 @@
       <c r="HI69" s="3">
         <v>24</v>
       </c>
+      <c r="HJ69" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:217" ht="15">
+    <row r="70" spans="1:218" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79938,7 +79953,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:217" ht="15">
+    <row r="71" spans="1:218" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -80085,7 +80100,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:217" ht="15">
+    <row r="72" spans="1:218" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -80277,8 +80292,11 @@
       <c r="HI72" s="3">
         <v>24</v>
       </c>
+      <c r="HJ72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:217" ht="15">
+    <row r="73" spans="1:218" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80543,7 +80561,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:217" ht="15">
+    <row r="74" spans="1:218" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80808,7 +80826,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:217" ht="15">
+    <row r="75" spans="1:218" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80942,7 +80960,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:217" ht="15">
+    <row r="76" spans="1:218" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -81076,7 +81094,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:217" ht="15">
+    <row r="77" spans="1:218" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -81210,7 +81228,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:217" ht="15">
+    <row r="78" spans="1:218" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81478,7 +81496,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:217" ht="15">
+    <row r="79" spans="1:218" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81612,7 +81630,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:217" ht="15">
+    <row r="80" spans="1:218" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81801,7 +81819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:217" ht="15">
+    <row r="81" spans="1:218" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81842,7 +81860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:217" ht="15">
+    <row r="82" spans="1:218" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -82009,7 +82027,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:217" ht="15">
+    <row r="83" spans="1:218" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -82050,7 +82068,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:217" ht="15">
+    <row r="84" spans="1:218" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -82112,7 +82130,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:217" ht="15">
+    <row r="85" spans="1:218" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -82207,7 +82225,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:217" ht="15">
+    <row r="86" spans="1:218" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -82227,7 +82245,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:217" ht="15">
+    <row r="87" spans="1:218" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -82265,7 +82283,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:217" ht="15">
+    <row r="88" spans="1:218" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -82303,7 +82321,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:217" ht="15">
+    <row r="89" spans="1:218" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82362,7 +82380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:217" ht="15">
+    <row r="90" spans="1:218" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82421,7 +82439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:217" ht="15">
+    <row r="91" spans="1:218" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82480,7 +82498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:217" ht="15">
+    <row r="92" spans="1:218" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82539,7 +82557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:217" ht="15">
+    <row r="93" spans="1:218" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82598,7 +82616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:217" ht="15">
+    <row r="94" spans="1:218" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82654,7 +82672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:217" ht="15">
+    <row r="95" spans="1:218" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82778,8 +82796,11 @@
       <c r="HI95" s="3">
         <v>24</v>
       </c>
+      <c r="HJ95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:217" ht="15">
+    <row r="96" spans="1:218" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82820,7 +82841,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:217" ht="15">
+    <row r="97" spans="1:218" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82861,7 +82882,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:217" ht="15">
+    <row r="98" spans="1:218" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82997,8 +83018,11 @@
       <c r="HI98" s="3">
         <v>24</v>
       </c>
+      <c r="HJ98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:217" ht="15">
+    <row r="99" spans="1:218" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -83134,8 +83158,11 @@
       <c r="HI99" s="3">
         <v>24</v>
       </c>
+      <c r="HJ99" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="100" spans="1:217" ht="15">
+    <row r="100" spans="1:218" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -83176,7 +83203,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:217" ht="15">
+    <row r="101" spans="1:218" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -83220,7 +83247,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:217" ht="15">
+    <row r="102" spans="1:218" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -83264,7 +83291,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="103" spans="1:217" ht="15">
+    <row r="103" spans="1:218" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -83308,7 +83335,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:217" ht="15">
+    <row r="104" spans="1:218" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -83352,7 +83379,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:217" ht="15">
+    <row r="105" spans="1:218" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -83411,7 +83438,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="106" spans="1:217" ht="15">
+    <row r="106" spans="1:218" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -83452,7 +83479,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="107" spans="1:217" ht="15">
+    <row r="107" spans="1:218" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -83588,8 +83615,11 @@
       <c r="HI107" s="3">
         <v>24</v>
       </c>
+      <c r="HJ107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:217" ht="15">
+    <row r="108" spans="1:218" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83651,7 +83681,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:217" ht="15">
+    <row r="109" spans="1:218" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83671,7 +83701,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:217" ht="15">
+    <row r="110" spans="1:218" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83742,7 +83772,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="111" spans="1:217" ht="15">
+    <row r="111" spans="1:218" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83789,7 +83819,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="112" spans="1:217" ht="15">
+    <row r="112" spans="1:218" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83857,7 +83887,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="113" spans="1:217" ht="15">
+    <row r="113" spans="1:218" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83904,7 +83934,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="114" spans="1:217" ht="15">
+    <row r="114" spans="1:218" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -83987,7 +84017,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="115" spans="1:217" ht="15">
+    <row r="115" spans="1:218" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -84129,8 +84159,11 @@
       <c r="HI115" s="3">
         <v>24</v>
       </c>
+      <c r="HJ115" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="116" spans="1:217" ht="15">
+    <row r="116" spans="1:218" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -84149,9 +84182,6 @@
       <c r="F116" s="13">
         <v>45818</v>
       </c>
-      <c r="P116" s="13">
-        <v>45831</v>
-      </c>
       <c r="FU116" s="3">
         <v>12</v>
       </c>
@@ -84275,8 +84305,11 @@
       <c r="HI116" s="3">
         <v>24</v>
       </c>
+      <c r="HJ116" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="117" spans="1:217" ht="15">
+    <row r="117" spans="1:218" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -84295,6 +84328,9 @@
       <c r="F117" s="13">
         <v>45817</v>
       </c>
+      <c r="P117" s="13">
+        <v>45831</v>
+      </c>
       <c r="FT117" s="3">
         <v>5</v>
       </c>
@@ -84344,7 +84380,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:217" ht="15">
+    <row r="118" spans="1:218" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -84415,7 +84451,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:217" ht="15">
+    <row r="119" spans="1:218" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -84486,7 +84522,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="120" spans="1:217" ht="15">
+    <row r="120" spans="1:218" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -84557,7 +84593,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="121" spans="1:217" ht="15">
+    <row r="121" spans="1:218" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -84598,7 +84634,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="122" spans="1:217" ht="15">
+    <row r="122" spans="1:218" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -84657,7 +84693,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="123" spans="1:217" ht="15">
+    <row r="123" spans="1:218" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -84728,7 +84764,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:217" ht="15">
+    <row r="124" spans="1:218" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -84769,7 +84805,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="125" spans="1:217" ht="15">
+    <row r="125" spans="1:218" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84881,8 +84917,11 @@
       <c r="HI125" s="3">
         <v>24</v>
       </c>
+      <c r="HJ125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:217" ht="15">
+    <row r="126" spans="1:218" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84923,7 +84962,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="127" spans="1:217" ht="15">
+    <row r="127" spans="1:218" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -84964,7 +85003,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="128" spans="1:217" ht="15">
+    <row r="128" spans="1:218" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -85005,7 +85044,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="129" spans="1:217" ht="15">
+    <row r="129" spans="1:218" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -85046,7 +85085,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="1:217" ht="15">
+    <row r="130" spans="1:218" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -85102,7 +85141,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="131" spans="1:217" ht="15">
+    <row r="131" spans="1:218" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -85205,8 +85244,11 @@
       <c r="HI131" s="3">
         <v>24</v>
       </c>
+      <c r="HJ131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:217" ht="15">
+    <row r="132" spans="1:218" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -85309,8 +85351,11 @@
       <c r="HI132" s="3">
         <v>24</v>
       </c>
+      <c r="HJ132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:217" ht="15">
+    <row r="133" spans="1:218" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -85386,8 +85431,11 @@
       <c r="HI133" s="3">
         <v>24</v>
       </c>
+      <c r="HJ133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:217" ht="15">
+    <row r="134" spans="1:218" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -85463,8 +85511,11 @@
       <c r="HI134" s="3">
         <v>24</v>
       </c>
+      <c r="HJ134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:217" ht="15">
+    <row r="135" spans="1:218" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -85529,7 +85580,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="136" spans="1:217" ht="15">
+    <row r="136" spans="1:218" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -85570,7 +85621,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="137" spans="1:217" ht="15">
+    <row r="137" spans="1:218" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -85646,8 +85697,11 @@
       <c r="HI137" s="3">
         <v>24</v>
       </c>
+      <c r="HJ137" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="138" spans="1:217" ht="15">
+    <row r="138" spans="1:218" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -85727,7 +85781,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="139" spans="1:217" ht="15">
+    <row r="139" spans="1:218" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -85807,7 +85861,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:217" ht="15">
+    <row r="140" spans="1:218" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -85848,7 +85902,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="141" spans="1:217" ht="15">
+    <row r="141" spans="1:218" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -85889,7 +85943,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:217" ht="15">
+    <row r="142" spans="1:218" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -85951,7 +86005,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="143" spans="1:217" ht="15">
+    <row r="143" spans="1:218" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -85992,7 +86046,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="144" spans="1:217" ht="15">
+    <row r="144" spans="1:218" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -86054,7 +86108,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="145" spans="1:217" ht="15">
+    <row r="145" spans="1:218" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -86116,7 +86170,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="146" spans="1:217" ht="15">
+    <row r="146" spans="1:218" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -86157,7 +86211,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="147" spans="1:217" ht="15">
+    <row r="147" spans="1:218" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -86219,7 +86273,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="148" spans="1:217" ht="15">
+    <row r="148" spans="1:218" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -86260,7 +86314,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="149" spans="1:217" ht="15">
+    <row r="149" spans="1:218" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -86322,7 +86376,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="150" spans="1:217" ht="15">
+    <row r="150" spans="1:218" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -86363,7 +86417,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="151" spans="1:217" ht="15">
+    <row r="151" spans="1:218" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -86404,7 +86458,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="152" spans="1:217" ht="15">
+    <row r="152" spans="1:218" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -86466,7 +86520,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="153" spans="1:217" ht="15">
+    <row r="153" spans="1:218" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -86528,7 +86582,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="154" spans="1:217" ht="15">
+    <row r="154" spans="1:218" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -86569,7 +86623,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="155" spans="1:217" ht="15">
+    <row r="155" spans="1:218" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -86610,7 +86664,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="156" spans="1:217" ht="15">
+    <row r="156" spans="1:218" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -86651,7 +86705,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="157" spans="1:217" ht="15">
+    <row r="157" spans="1:218" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -86713,7 +86767,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="158" spans="1:217" ht="15">
+    <row r="158" spans="1:218" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -86730,7 +86784,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:217" ht="15">
+    <row r="159" spans="1:218" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -86747,7 +86801,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:217">
+    <row r="160" spans="1:218">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -86856,8 +86910,11 @@
       <c r="HI160" s="3">
         <v>24</v>
       </c>
+      <c r="HJ160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:217">
+    <row r="161" spans="1:218">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -86966,8 +87023,11 @@
       <c r="HI161" s="3">
         <v>24</v>
       </c>
+      <c r="HJ161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:217">
+    <row r="162" spans="1:218">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -87076,8 +87136,11 @@
       <c r="HI162" s="3">
         <v>24</v>
       </c>
+      <c r="HJ162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:217" ht="15">
+    <row r="163" spans="1:218" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -87091,7 +87154,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:217" ht="15">
+    <row r="164" spans="1:218" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -87105,7 +87168,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:217" ht="15">
+    <row r="165" spans="1:218" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -87119,7 +87182,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:217" ht="15">
+    <row r="166" spans="1:218" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -87133,7 +87196,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:217" ht="15">
+    <row r="167" spans="1:218" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -87147,7 +87210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:217" ht="15">
+    <row r="168" spans="1:218" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -87161,7 +87224,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:217" ht="15">
+    <row r="169" spans="1:218" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -87175,7 +87238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:217" ht="15">
+    <row r="170" spans="1:218" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -87189,7 +87252,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:217" ht="15">
+    <row r="171" spans="1:218" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -87203,7 +87266,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:217" ht="15">
+    <row r="172" spans="1:218" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -87217,7 +87280,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:217" ht="15">
+    <row r="173" spans="1:218" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -87231,7 +87294,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:217" ht="15">
+    <row r="174" spans="1:218" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -87245,7 +87308,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:217" ht="15">
+    <row r="175" spans="1:218" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -87259,7 +87322,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:217" ht="15">
+    <row r="176" spans="1:218" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>
@@ -87518,7 +87581,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="15">
+    <row r="193" spans="1:218" ht="15">
       <c r="A193" s="9">
         <v>25394757</v>
       </c>
@@ -87534,8 +87597,14 @@
       <c r="E193" s="9">
         <v>60</v>
       </c>
+      <c r="F193" s="13">
+        <v>45859</v>
+      </c>
+      <c r="HJ193" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="194" spans="1:5" ht="15">
+    <row r="194" spans="1:218" ht="15">
       <c r="A194" s="9">
         <v>25394035</v>
       </c>
@@ -87550,6 +87619,12 @@
       </c>
       <c r="E194" s="9">
         <v>96</v>
+      </c>
+      <c r="F194" s="13">
+        <v>45859</v>
+      </c>
+      <c r="HJ194" s="3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-23 05:12:14
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2304" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77E7FD3E-38B2-445C-A7B3-9DC5D7CAD38E}"/>
+  <xr:revisionPtr revIDLastSave="2314" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C00324B0-B3B3-441D-995F-38D86CB378E6}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="227">
   <si>
     <t>Module ID</t>
   </si>
@@ -715,6 +715,9 @@
   <si>
     <t>VSL202526204</t>
   </si>
+  <si>
+    <t>Hangzhou First Low GSM Trial (420F,400B) : Modified Stress Sequence Test</t>
+  </si>
 </sst>
 </file>
 
@@ -1248,11 +1251,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD194"/>
+  <dimension ref="A1:XFD195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="HF177" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="HJ189" sqref="HJ189"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="HE122" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="HK135" sqref="HK135"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -85044,7 +85047,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="129" spans="1:218" ht="15">
+    <row r="129" spans="1:219" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -85085,7 +85088,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="1:218" ht="15">
+    <row r="130" spans="1:219" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -85141,7 +85144,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="131" spans="1:218" ht="15">
+    <row r="131" spans="1:219" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -85247,8 +85250,11 @@
       <c r="HJ131" s="3">
         <v>24</v>
       </c>
+      <c r="HK131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:218" ht="15">
+    <row r="132" spans="1:219" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -85354,8 +85360,11 @@
       <c r="HJ132" s="3">
         <v>24</v>
       </c>
+      <c r="HK132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:218" ht="15">
+    <row r="133" spans="1:219" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -85434,8 +85443,11 @@
       <c r="HJ133" s="3">
         <v>24</v>
       </c>
+      <c r="HK133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:218" ht="15">
+    <row r="134" spans="1:219" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -85514,8 +85526,11 @@
       <c r="HJ134" s="3">
         <v>24</v>
       </c>
+      <c r="HK134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:218" ht="15">
+    <row r="135" spans="1:219" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -85580,7 +85595,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="136" spans="1:218" ht="15">
+    <row r="136" spans="1:219" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -85621,7 +85636,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="137" spans="1:218" ht="15">
+    <row r="137" spans="1:219" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -85701,7 +85716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:218" ht="15">
+    <row r="138" spans="1:219" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -85781,7 +85796,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="139" spans="1:218" ht="15">
+    <row r="139" spans="1:219" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -85861,7 +85876,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:218" ht="15">
+    <row r="140" spans="1:219" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -85902,7 +85917,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="141" spans="1:218" ht="15">
+    <row r="141" spans="1:219" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -85943,7 +85958,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:218" ht="15">
+    <row r="142" spans="1:219" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -86005,7 +86020,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="143" spans="1:218" ht="15">
+    <row r="143" spans="1:219" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -86046,7 +86061,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="144" spans="1:218" ht="15">
+    <row r="144" spans="1:219" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -87625,6 +87640,23 @@
       </c>
       <c r="HJ194" s="3">
         <v>6</v>
+      </c>
+    </row>
+    <row r="195" spans="1:218" ht="15">
+      <c r="A195" s="9">
+        <v>25273925</v>
+      </c>
+      <c r="B195" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C195" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D195" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E195" s="9">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -87635,13 +87667,13 @@
     <protectedRange sqref="A85 Q1:XFD1048576" name="Range3"/>
   </protectedRanges>
   <conditionalFormatting sqref="A91">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86:A90 A92:A100">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A122">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D86:D99" xr:uid="{AE741107-2DDE-448F-B66D-3CC4D6043D49}">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-23 09:50:31
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2314" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C00324B0-B3B3-441D-995F-38D86CB378E6}"/>
+  <xr:revisionPtr revIDLastSave="2316" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9296065-A737-4EEF-A9EE-5D5C958487A2}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="228">
   <si>
     <t>Module ID</t>
   </si>
@@ -599,7 +599,7 @@
     <t>VSL202526133</t>
   </si>
   <si>
-    <t>Cleanmax HYPERSOL Internal Reliability Tests</t>
+    <t>Cleanmax HYPERSOL Internal Reliability Tests: Lot 1</t>
   </si>
   <si>
     <t>VSL202526134</t>
@@ -711,6 +711,9 @@
   </si>
   <si>
     <t>VSL202526203</t>
+  </si>
+  <si>
+    <t>Cleanmax HYPERSOL Internal Reliability Tests</t>
   </si>
   <si>
     <t>VSL202526204</t>
@@ -1254,8 +1257,8 @@
   <dimension ref="A1:XFD195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="HE122" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="HK135" sqref="HK135"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="HC144" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C143" sqref="C143:C157"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -87604,7 +87607,7 @@
         <v>224</v>
       </c>
       <c r="C193" s="17" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>32</v>
@@ -87624,10 +87627,10 @@
         <v>25394035</v>
       </c>
       <c r="B194" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C194" s="17" t="s">
         <v>225</v>
-      </c>
-      <c r="C194" s="17" t="s">
-        <v>187</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>18</v>
@@ -87650,7 +87653,7 @@
         <v>146</v>
       </c>
       <c r="C195" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-24 09:48:53
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2316" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9296065-A737-4EEF-A9EE-5D5C958487A2}"/>
+  <xr:revisionPtr revIDLastSave="2341" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C06C05-3EAC-4ECE-B103-05800575FA96}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="228">
   <si>
     <t>Module ID</t>
   </si>
@@ -1257,8 +1257,8 @@
   <dimension ref="A1:XFD195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="HC144" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C143" sqref="C143:C157"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="HJ189" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F195" sqref="F195"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -73132,7 +73132,7 @@
       <c r="FI32" s="1"/>
       <c r="FJ32" s="1"/>
     </row>
-    <row r="33" spans="1:218" ht="15">
+    <row r="33" spans="1:220" ht="15">
       <c r="A33" s="8">
         <v>24636088</v>
       </c>
@@ -73281,7 +73281,7 @@
       <c r="FI33" s="1"/>
       <c r="FJ33" s="1"/>
     </row>
-    <row r="34" spans="1:218" ht="15">
+    <row r="34" spans="1:220" ht="15">
       <c r="A34" s="8">
         <v>24636089</v>
       </c>
@@ -73430,7 +73430,7 @@
       <c r="FI34" s="1"/>
       <c r="FJ34" s="1"/>
     </row>
-    <row r="35" spans="1:218" ht="15">
+    <row r="35" spans="1:220" ht="15">
       <c r="A35" s="8">
         <v>24636092</v>
       </c>
@@ -73579,7 +73579,7 @@
       <c r="FI35" s="1"/>
       <c r="FJ35" s="1"/>
     </row>
-    <row r="36" spans="1:218" ht="15">
+    <row r="36" spans="1:220" ht="15">
       <c r="A36" s="8">
         <v>24395952</v>
       </c>
@@ -73713,7 +73713,7 @@
       <c r="FI36" s="1"/>
       <c r="FJ36" s="1"/>
     </row>
-    <row r="37" spans="1:218" ht="15">
+    <row r="37" spans="1:220" ht="15">
       <c r="A37" s="8">
         <v>24395977</v>
       </c>
@@ -73847,7 +73847,7 @@
       <c r="FI37" s="1"/>
       <c r="FJ37" s="1"/>
     </row>
-    <row r="38" spans="1:218" ht="15">
+    <row r="38" spans="1:220" ht="15">
       <c r="A38" s="8">
         <v>24395942</v>
       </c>
@@ -73981,7 +73981,7 @@
       <c r="FI38" s="1"/>
       <c r="FJ38" s="1"/>
     </row>
-    <row r="39" spans="1:218" ht="15">
+    <row r="39" spans="1:220" ht="15">
       <c r="A39" s="11">
         <v>24567303</v>
       </c>
@@ -74144,7 +74144,7 @@
       <c r="FI39" s="1"/>
       <c r="FJ39" s="1"/>
     </row>
-    <row r="40" spans="1:218" ht="15">
+    <row r="40" spans="1:220" ht="15">
       <c r="A40" s="11">
         <v>24567296</v>
       </c>
@@ -74307,7 +74307,7 @@
       <c r="FI40" s="1"/>
       <c r="FJ40" s="1"/>
     </row>
-    <row r="41" spans="1:218" ht="15">
+    <row r="41" spans="1:220" ht="15">
       <c r="A41" s="11">
         <v>24567289</v>
       </c>
@@ -74470,7 +74470,7 @@
       <c r="FI41" s="1"/>
       <c r="FJ41" s="1"/>
     </row>
-    <row r="42" spans="1:218" ht="15">
+    <row r="42" spans="1:220" ht="15">
       <c r="A42" s="11">
         <v>24567319</v>
       </c>
@@ -74633,7 +74633,7 @@
       <c r="FI42" s="1"/>
       <c r="FJ42" s="1"/>
     </row>
-    <row r="43" spans="1:218" ht="15">
+    <row r="43" spans="1:220" ht="15">
       <c r="A43" s="11">
         <v>24567277</v>
       </c>
@@ -74796,7 +74796,7 @@
       <c r="FI43" s="1"/>
       <c r="FJ43" s="1"/>
     </row>
-    <row r="44" spans="1:218" ht="15">
+    <row r="44" spans="1:220" ht="15">
       <c r="A44" s="11">
         <v>24567774</v>
       </c>
@@ -74959,7 +74959,7 @@
       <c r="FI44" s="1"/>
       <c r="FJ44" s="1"/>
     </row>
-    <row r="45" spans="1:218" ht="15">
+    <row r="45" spans="1:220" ht="15">
       <c r="A45" s="11">
         <v>24567851</v>
       </c>
@@ -75122,7 +75122,7 @@
       <c r="FI45" s="1"/>
       <c r="FJ45" s="1"/>
     </row>
-    <row r="46" spans="1:218" ht="15">
+    <row r="46" spans="1:220" ht="15">
       <c r="A46" s="11">
         <v>24559501</v>
       </c>
@@ -75285,7 +75285,7 @@
       <c r="FI46" s="1"/>
       <c r="FJ46" s="1"/>
     </row>
-    <row r="47" spans="1:218" ht="15">
+    <row r="47" spans="1:220" ht="15">
       <c r="A47" s="11">
         <v>24567303</v>
       </c>
@@ -75528,8 +75528,14 @@
       <c r="HJ47" s="3">
         <v>24</v>
       </c>
+      <c r="HK47" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL47" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="48" spans="1:218" ht="15">
+    <row r="48" spans="1:220" ht="15">
       <c r="A48" s="11">
         <v>24567296</v>
       </c>
@@ -75740,7 +75746,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="49" spans="1:218" ht="15">
+    <row r="49" spans="1:220" ht="15">
       <c r="A49" s="11">
         <v>24567289</v>
       </c>
@@ -75983,8 +75989,14 @@
       <c r="HJ49" s="3">
         <v>24</v>
       </c>
+      <c r="HK49" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL49" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="50" spans="1:218" ht="15">
+    <row r="50" spans="1:220" ht="15">
       <c r="A50" s="11">
         <v>24567319</v>
       </c>
@@ -76195,7 +76207,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:218" ht="15">
+    <row r="51" spans="1:220" ht="15">
       <c r="A51" s="11">
         <v>24567277</v>
       </c>
@@ -76406,7 +76418,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:218" ht="15">
+    <row r="52" spans="1:220" ht="15">
       <c r="A52" s="11">
         <v>24567774</v>
       </c>
@@ -76617,7 +76629,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:218" ht="15">
+    <row r="53" spans="1:220" ht="15">
       <c r="A53" s="11">
         <v>24567851</v>
       </c>
@@ -76860,8 +76872,14 @@
       <c r="HJ53" s="3">
         <v>24</v>
       </c>
+      <c r="HK53" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL53" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="54" spans="1:218" ht="15">
+    <row r="54" spans="1:220" ht="15">
       <c r="A54" s="11">
         <v>24559501</v>
       </c>
@@ -77104,8 +77122,14 @@
       <c r="HJ54" s="3">
         <v>24</v>
       </c>
+      <c r="HK54" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL54" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="55" spans="1:218" ht="15">
+    <row r="55" spans="1:220" ht="15">
       <c r="A55" s="8">
         <v>24079686</v>
       </c>
@@ -77298,7 +77322,7 @@
       <c r="FI55" s="1"/>
       <c r="FJ55" s="1"/>
     </row>
-    <row r="56" spans="1:218" ht="15">
+    <row r="56" spans="1:220" ht="15">
       <c r="A56" s="8">
         <v>24079692</v>
       </c>
@@ -77491,7 +77515,7 @@
       <c r="FI56" s="1"/>
       <c r="FJ56" s="1"/>
     </row>
-    <row r="57" spans="1:218" ht="15">
+    <row r="57" spans="1:220" ht="15">
       <c r="A57" s="8">
         <v>24636092</v>
       </c>
@@ -77648,7 +77672,7 @@
       <c r="FI57" s="1"/>
       <c r="FJ57" s="1"/>
     </row>
-    <row r="58" spans="1:218" ht="15">
+    <row r="58" spans="1:220" ht="15">
       <c r="A58" s="8">
         <v>24793376</v>
       </c>
@@ -77813,7 +77837,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:218" ht="15">
+    <row r="59" spans="1:220" ht="15">
       <c r="A59" s="8">
         <v>24713456</v>
       </c>
@@ -77972,7 +77996,7 @@
       <c r="FI59" s="1"/>
       <c r="FJ59" s="1"/>
     </row>
-    <row r="60" spans="1:218" ht="15">
+    <row r="60" spans="1:220" ht="15">
       <c r="A60" s="8">
         <v>24713371</v>
       </c>
@@ -78123,7 +78147,7 @@
       <c r="FI60" s="1"/>
       <c r="FJ60" s="1"/>
     </row>
-    <row r="61" spans="1:218" ht="15">
+    <row r="61" spans="1:220" ht="15">
       <c r="A61" s="8">
         <v>24713222</v>
       </c>
@@ -78281,7 +78305,7 @@
       <c r="FI61" s="1"/>
       <c r="FJ61" s="1"/>
     </row>
-    <row r="62" spans="1:218" ht="15">
+    <row r="62" spans="1:220" ht="15">
       <c r="A62" s="8">
         <v>24636087</v>
       </c>
@@ -78526,7 +78550,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:218" ht="15">
+    <row r="63" spans="1:220" ht="15">
       <c r="A63" s="8">
         <v>24636090</v>
       </c>
@@ -78771,7 +78795,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:218" ht="15">
+    <row r="64" spans="1:220" ht="15">
       <c r="A64" s="8">
         <v>24636091</v>
       </c>
@@ -79016,7 +79040,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:218" ht="15">
+    <row r="65" spans="1:220" ht="15">
       <c r="A65" s="8">
         <v>24636089</v>
       </c>
@@ -79165,7 +79189,7 @@
       <c r="FI65" s="1"/>
       <c r="FJ65" s="1"/>
     </row>
-    <row r="66" spans="1:218" ht="15">
+    <row r="66" spans="1:220" ht="15">
       <c r="A66" s="8">
         <v>24636088</v>
       </c>
@@ -79314,7 +79338,7 @@
       <c r="FI66" s="1"/>
       <c r="FJ66" s="1"/>
     </row>
-    <row r="67" spans="1:218" ht="15">
+    <row r="67" spans="1:220" ht="15">
       <c r="A67" s="8">
         <v>25017935</v>
       </c>
@@ -79453,7 +79477,7 @@
       <c r="FI67" s="1"/>
       <c r="FJ67" s="1"/>
     </row>
-    <row r="68" spans="1:218" ht="15">
+    <row r="68" spans="1:220" ht="15">
       <c r="A68" s="8">
         <v>25017936</v>
       </c>
@@ -79600,7 +79624,7 @@
       <c r="FI68" s="1"/>
       <c r="FJ68" s="1"/>
     </row>
-    <row r="69" spans="1:218" ht="15">
+    <row r="69" spans="1:220" ht="15">
       <c r="A69" s="8">
         <v>25017937</v>
       </c>
@@ -79795,8 +79819,14 @@
       <c r="HJ69" s="3">
         <v>24</v>
       </c>
+      <c r="HK69" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL69" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="70" spans="1:218" ht="15">
+    <row r="70" spans="1:220" ht="15">
       <c r="A70" s="8">
         <v>25019644</v>
       </c>
@@ -79959,7 +79989,7 @@
       <c r="FI70" s="1"/>
       <c r="FJ70" s="1"/>
     </row>
-    <row r="71" spans="1:218" ht="15">
+    <row r="71" spans="1:220" ht="15">
       <c r="A71" s="8">
         <v>25019645</v>
       </c>
@@ -80106,7 +80136,7 @@
       <c r="FI71" s="1"/>
       <c r="FJ71" s="1"/>
     </row>
-    <row r="72" spans="1:218" ht="15">
+    <row r="72" spans="1:220" ht="15">
       <c r="A72" s="8">
         <v>25019646</v>
       </c>
@@ -80301,8 +80331,14 @@
       <c r="HJ72" s="3">
         <v>24</v>
       </c>
+      <c r="HK72" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL72" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="73" spans="1:218" ht="15">
+    <row r="73" spans="1:220" ht="15">
       <c r="A73" s="8">
         <v>24848800</v>
       </c>
@@ -80567,7 +80603,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:218" ht="15">
+    <row r="74" spans="1:220" ht="15">
       <c r="A74" s="8">
         <v>24859051</v>
       </c>
@@ -80832,7 +80868,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:218" ht="15">
+    <row r="75" spans="1:220" ht="15">
       <c r="A75" s="8">
         <v>24988445</v>
       </c>
@@ -80966,7 +81002,7 @@
       <c r="FI75" s="1"/>
       <c r="FJ75" s="1"/>
     </row>
-    <row r="76" spans="1:218" ht="15">
+    <row r="76" spans="1:220" ht="15">
       <c r="A76" s="8">
         <v>24988559</v>
       </c>
@@ -81100,7 +81136,7 @@
       <c r="FI76" s="1"/>
       <c r="FJ76" s="1"/>
     </row>
-    <row r="77" spans="1:218" ht="15">
+    <row r="77" spans="1:220" ht="15">
       <c r="A77" s="8">
         <v>24988692</v>
       </c>
@@ -81234,7 +81270,7 @@
       <c r="FI77" s="1"/>
       <c r="FJ77" s="1"/>
     </row>
-    <row r="78" spans="1:218" ht="15">
+    <row r="78" spans="1:220" ht="15">
       <c r="A78" s="8">
         <v>24923318</v>
       </c>
@@ -81502,7 +81538,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:218" ht="15">
+    <row r="79" spans="1:220" ht="15">
       <c r="A79" s="8">
         <v>24925212</v>
       </c>
@@ -81636,7 +81672,7 @@
       <c r="FI79" s="1"/>
       <c r="FJ79" s="1"/>
     </row>
-    <row r="80" spans="1:218" ht="15">
+    <row r="80" spans="1:220" ht="15">
       <c r="A80" s="8">
         <v>24857462</v>
       </c>
@@ -81825,7 +81861,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:218" ht="15">
+    <row r="81" spans="1:220" ht="15">
       <c r="A81" s="9">
         <v>25112301</v>
       </c>
@@ -81866,7 +81902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:218" ht="15">
+    <row r="82" spans="1:220" ht="15">
       <c r="A82" s="9">
         <v>25112300</v>
       </c>
@@ -82033,7 +82069,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:218" ht="15">
+    <row r="83" spans="1:220" ht="15">
       <c r="A83" s="9">
         <v>25087863</v>
       </c>
@@ -82074,7 +82110,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:218" ht="15">
+    <row r="84" spans="1:220" ht="15">
       <c r="A84" s="9">
         <v>25087787</v>
       </c>
@@ -82136,7 +82172,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:218" ht="15">
+    <row r="85" spans="1:220" ht="15">
       <c r="A85" s="9">
         <v>24848547</v>
       </c>
@@ -82231,7 +82267,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:218" ht="15">
+    <row r="86" spans="1:220" ht="15">
       <c r="A86" s="15">
         <v>50872159</v>
       </c>
@@ -82251,7 +82287,7 @@
         <v>45793</v>
       </c>
     </row>
-    <row r="87" spans="1:218" ht="15">
+    <row r="87" spans="1:220" ht="15">
       <c r="A87" s="15">
         <v>25019645</v>
       </c>
@@ -82289,7 +82325,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:218" ht="15">
+    <row r="88" spans="1:220" ht="15">
       <c r="A88" s="15">
         <v>25017936</v>
       </c>
@@ -82327,7 +82363,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:218" ht="15">
+    <row r="89" spans="1:220" ht="15">
       <c r="A89" s="15">
         <v>25089372</v>
       </c>
@@ -82386,7 +82422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:218" ht="15">
+    <row r="90" spans="1:220" ht="15">
       <c r="A90" s="15">
         <v>25089365</v>
       </c>
@@ -82445,7 +82481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:218" ht="15">
+    <row r="91" spans="1:220" ht="15">
       <c r="A91" s="15">
         <v>25089363</v>
       </c>
@@ -82504,7 +82540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:218" ht="15">
+    <row r="92" spans="1:220" ht="15">
       <c r="A92" s="15">
         <v>25089370</v>
       </c>
@@ -82563,7 +82599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:218" ht="15">
+    <row r="93" spans="1:220" ht="15">
       <c r="A93" s="15">
         <v>25112299</v>
       </c>
@@ -82622,7 +82658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:218" ht="15">
+    <row r="94" spans="1:220" ht="15">
       <c r="A94" s="15">
         <v>72149637</v>
       </c>
@@ -82678,7 +82714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:218" ht="15">
+    <row r="95" spans="1:220" ht="15">
       <c r="A95" s="15">
         <v>72238923</v>
       </c>
@@ -82805,8 +82841,14 @@
       <c r="HJ95" s="3">
         <v>24</v>
       </c>
+      <c r="HK95" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL95" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="96" spans="1:218" ht="15">
+    <row r="96" spans="1:220" ht="15">
       <c r="A96" s="15">
         <v>25089372</v>
       </c>
@@ -82847,7 +82889,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:218" ht="15">
+    <row r="97" spans="1:220" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82888,7 +82930,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:218" ht="15">
+    <row r="98" spans="1:220" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -83027,8 +83069,14 @@
       <c r="HJ98" s="3">
         <v>24</v>
       </c>
+      <c r="HK98" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL98" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="99" spans="1:218" ht="15">
+    <row r="99" spans="1:220" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -83167,8 +83215,14 @@
       <c r="HJ99" s="3">
         <v>24</v>
       </c>
+      <c r="HK99" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL99" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="100" spans="1:218" ht="15">
+    <row r="100" spans="1:220" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -83209,7 +83263,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:218" ht="15">
+    <row r="101" spans="1:220" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -83253,7 +83307,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:218" ht="15">
+    <row r="102" spans="1:220" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -83297,7 +83351,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="103" spans="1:218" ht="15">
+    <row r="103" spans="1:220" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -83341,7 +83395,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:218" ht="15">
+    <row r="104" spans="1:220" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -83385,7 +83439,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:218" ht="15">
+    <row r="105" spans="1:220" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -83444,7 +83498,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="106" spans="1:218" ht="15">
+    <row r="106" spans="1:220" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -83485,7 +83539,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="107" spans="1:218" ht="15">
+    <row r="107" spans="1:220" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -83624,8 +83678,14 @@
       <c r="HJ107" s="3">
         <v>24</v>
       </c>
+      <c r="HK107" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL107" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="108" spans="1:218" ht="15">
+    <row r="108" spans="1:220" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83687,7 +83747,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:218" ht="15">
+    <row r="109" spans="1:220" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83707,7 +83767,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:218" ht="15">
+    <row r="110" spans="1:220" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83778,7 +83838,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="111" spans="1:218" ht="15">
+    <row r="111" spans="1:220" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83825,7 +83885,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="112" spans="1:218" ht="15">
+    <row r="112" spans="1:220" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -83893,7 +83953,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="113" spans="1:218" ht="15">
+    <row r="113" spans="1:220" ht="15">
       <c r="A113" s="9">
         <v>25120989</v>
       </c>
@@ -83940,7 +84000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="114" spans="1:218" ht="15">
+    <row r="114" spans="1:220" ht="15">
       <c r="A114" s="9">
         <v>25129692</v>
       </c>
@@ -84023,7 +84083,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="115" spans="1:218" ht="15">
+    <row r="115" spans="1:220" ht="15">
       <c r="A115" s="9">
         <v>25129767</v>
       </c>
@@ -84042,6 +84102,9 @@
       <c r="F115" s="13">
         <v>45818</v>
       </c>
+      <c r="P115" s="13">
+        <v>45861</v>
+      </c>
       <c r="FU115" s="3">
         <v>12</v>
       </c>
@@ -84168,8 +84231,14 @@
       <c r="HJ115" s="3">
         <v>24</v>
       </c>
+      <c r="HK115" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL115" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="116" spans="1:218" ht="15">
+    <row r="116" spans="1:220" ht="15">
       <c r="A116" s="9">
         <v>25129647</v>
       </c>
@@ -84188,6 +84257,9 @@
       <c r="F116" s="13">
         <v>45818</v>
       </c>
+      <c r="P116" s="13">
+        <v>45861</v>
+      </c>
       <c r="FU116" s="3">
         <v>12</v>
       </c>
@@ -84314,8 +84386,14 @@
       <c r="HJ116" s="3">
         <v>24</v>
       </c>
+      <c r="HK116" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL116" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="117" spans="1:218" ht="15">
+    <row r="117" spans="1:220" ht="15">
       <c r="A117" s="9">
         <v>25129669</v>
       </c>
@@ -84386,7 +84464,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:218" ht="15">
+    <row r="118" spans="1:220" ht="15">
       <c r="A118" s="9">
         <v>25173191</v>
       </c>
@@ -84457,7 +84535,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:218" ht="15">
+    <row r="119" spans="1:220" ht="15">
       <c r="A119" s="9">
         <v>25170488</v>
       </c>
@@ -84528,7 +84606,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="120" spans="1:218" ht="15">
+    <row r="120" spans="1:220" ht="15">
       <c r="A120" s="9">
         <v>25176404</v>
       </c>
@@ -84599,7 +84677,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="121" spans="1:218" ht="15">
+    <row r="121" spans="1:220" ht="15">
       <c r="A121" s="9">
         <v>25087863</v>
       </c>
@@ -84640,7 +84718,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="122" spans="1:218" ht="15">
+    <row r="122" spans="1:220" ht="15">
       <c r="A122" s="15">
         <v>72149637</v>
       </c>
@@ -84699,7 +84777,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="123" spans="1:218" ht="15">
+    <row r="123" spans="1:220" ht="15">
       <c r="A123" s="9">
         <v>25321818</v>
       </c>
@@ -84770,7 +84848,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:218" ht="15">
+    <row r="124" spans="1:220" ht="15">
       <c r="A124" s="9">
         <v>25321819</v>
       </c>
@@ -84811,7 +84889,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="125" spans="1:218" ht="15">
+    <row r="125" spans="1:220" ht="15">
       <c r="A125" s="9">
         <v>25321820</v>
       </c>
@@ -84926,8 +85004,14 @@
       <c r="HJ125" s="3">
         <v>24</v>
       </c>
+      <c r="HK125" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL125" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="126" spans="1:218" ht="15">
+    <row r="126" spans="1:220" ht="15">
       <c r="A126" s="9">
         <v>25176363</v>
       </c>
@@ -84968,7 +85052,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="127" spans="1:218" ht="15">
+    <row r="127" spans="1:220" ht="15">
       <c r="A127" s="9">
         <v>25179725</v>
       </c>
@@ -85009,7 +85093,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="128" spans="1:218" ht="15">
+    <row r="128" spans="1:220" ht="15">
       <c r="A128" s="9">
         <v>25173127</v>
       </c>
@@ -85050,7 +85134,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="129" spans="1:219" ht="15">
+    <row r="129" spans="1:220" ht="15">
       <c r="A129" s="9">
         <v>25173179</v>
       </c>
@@ -85091,7 +85175,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="130" spans="1:219" ht="15">
+    <row r="130" spans="1:220" ht="15">
       <c r="A130" s="8">
         <v>24859051</v>
       </c>
@@ -85147,7 +85231,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="131" spans="1:219" ht="15">
+    <row r="131" spans="1:220" ht="15">
       <c r="A131" s="9">
         <v>72369597</v>
       </c>
@@ -85256,8 +85340,11 @@
       <c r="HK131" s="3">
         <v>24</v>
       </c>
+      <c r="HL131" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="132" spans="1:219" ht="15">
+    <row r="132" spans="1:220" ht="15">
       <c r="A132" s="9">
         <v>72369575</v>
       </c>
@@ -85366,8 +85453,11 @@
       <c r="HK132" s="3">
         <v>24</v>
       </c>
+      <c r="HL132" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="133" spans="1:219" ht="15">
+    <row r="133" spans="1:220" ht="15">
       <c r="A133" s="9">
         <v>25151639</v>
       </c>
@@ -85449,8 +85539,11 @@
       <c r="HK133" s="3">
         <v>24</v>
       </c>
+      <c r="HL133" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="134" spans="1:219" ht="15">
+    <row r="134" spans="1:220" ht="15">
       <c r="A134" s="9">
         <v>25353591</v>
       </c>
@@ -85532,8 +85625,11 @@
       <c r="HK134" s="3">
         <v>24</v>
       </c>
+      <c r="HL134" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="135" spans="1:219" ht="15">
+    <row r="135" spans="1:220" ht="15">
       <c r="A135" s="9">
         <v>25353593</v>
       </c>
@@ -85598,7 +85694,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="136" spans="1:219" ht="15">
+    <row r="136" spans="1:220" ht="15">
       <c r="A136" s="9">
         <v>25353594</v>
       </c>
@@ -85639,7 +85735,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="137" spans="1:219" ht="15">
+    <row r="137" spans="1:220" ht="15">
       <c r="A137" s="9">
         <v>25353595</v>
       </c>
@@ -85718,8 +85814,14 @@
       <c r="HJ137" s="3">
         <v>24</v>
       </c>
+      <c r="HK137" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL137" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="138" spans="1:219" ht="15">
+    <row r="138" spans="1:220" ht="15">
       <c r="A138" s="9">
         <v>25357620</v>
       </c>
@@ -85799,7 +85901,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="139" spans="1:219" ht="15">
+    <row r="139" spans="1:220" ht="15">
       <c r="A139" s="9">
         <v>25359186</v>
       </c>
@@ -85879,7 +85981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:219" ht="15">
+    <row r="140" spans="1:220" ht="15">
       <c r="A140" s="9">
         <v>25357399</v>
       </c>
@@ -85920,7 +86022,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="141" spans="1:219" ht="15">
+    <row r="141" spans="1:220" ht="15">
       <c r="A141" s="9">
         <v>25358777</v>
       </c>
@@ -85961,7 +86063,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:219" ht="15">
+    <row r="142" spans="1:220" ht="15">
       <c r="A142" s="9">
         <v>25238843</v>
       </c>
@@ -86023,7 +86125,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="143" spans="1:219" ht="15">
+    <row r="143" spans="1:220" ht="15">
       <c r="A143" s="9">
         <v>25239166</v>
       </c>
@@ -86064,7 +86166,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="144" spans="1:219" ht="15">
+    <row r="144" spans="1:220" ht="15">
       <c r="A144" s="9">
         <v>25248252</v>
       </c>
@@ -86126,7 +86228,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="145" spans="1:218" ht="15">
+    <row r="145" spans="1:220" ht="15">
       <c r="A145" s="9">
         <v>25313260</v>
       </c>
@@ -86188,7 +86290,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="146" spans="1:218" ht="15">
+    <row r="146" spans="1:220" ht="15">
       <c r="A146" s="9">
         <v>25313310</v>
       </c>
@@ -86229,7 +86331,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="147" spans="1:218" ht="15">
+    <row r="147" spans="1:220" ht="15">
       <c r="A147" s="9">
         <v>25270829</v>
       </c>
@@ -86291,7 +86393,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="148" spans="1:218" ht="15">
+    <row r="148" spans="1:220" ht="15">
       <c r="A148" s="9">
         <v>25310847</v>
       </c>
@@ -86332,7 +86434,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="149" spans="1:218" ht="15">
+    <row r="149" spans="1:220" ht="15">
       <c r="A149" s="9">
         <v>25249419</v>
       </c>
@@ -86394,7 +86496,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="150" spans="1:218" ht="15">
+    <row r="150" spans="1:220" ht="15">
       <c r="A150" s="9">
         <v>25249424</v>
       </c>
@@ -86435,7 +86537,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="151" spans="1:218" ht="15">
+    <row r="151" spans="1:220" ht="15">
       <c r="A151" s="9">
         <v>25249390</v>
       </c>
@@ -86476,7 +86578,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="152" spans="1:218" ht="15">
+    <row r="152" spans="1:220" ht="15">
       <c r="A152" s="9">
         <v>25338380</v>
       </c>
@@ -86538,7 +86640,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="153" spans="1:218" ht="15">
+    <row r="153" spans="1:220" ht="15">
       <c r="A153" s="9">
         <v>25336519</v>
       </c>
@@ -86600,7 +86702,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="154" spans="1:218" ht="15">
+    <row r="154" spans="1:220" ht="15">
       <c r="A154" s="9">
         <v>25338967</v>
       </c>
@@ -86641,7 +86743,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="155" spans="1:218" ht="15">
+    <row r="155" spans="1:220" ht="15">
       <c r="A155" s="9">
         <v>25338894</v>
       </c>
@@ -86682,7 +86784,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="156" spans="1:218" ht="15">
+    <row r="156" spans="1:220" ht="15">
       <c r="A156" s="9">
         <v>25344642</v>
       </c>
@@ -86723,7 +86825,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="157" spans="1:218" ht="15">
+    <row r="157" spans="1:220" ht="15">
       <c r="A157" s="9">
         <v>25344659</v>
       </c>
@@ -86785,7 +86887,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="158" spans="1:218" ht="15">
+    <row r="158" spans="1:220" ht="15">
       <c r="A158" s="9">
         <v>25273925</v>
       </c>
@@ -86802,7 +86904,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:218" ht="15">
+    <row r="159" spans="1:220" ht="15">
       <c r="A159" s="9">
         <v>23905761</v>
       </c>
@@ -86819,7 +86921,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="160" spans="1:218">
+    <row r="160" spans="1:220">
       <c r="A160" s="9" t="s">
         <v>205</v>
       </c>
@@ -86931,8 +87033,14 @@
       <c r="HJ160" s="3">
         <v>24</v>
       </c>
+      <c r="HK160" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL160" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="161" spans="1:218">
+    <row r="161" spans="1:220">
       <c r="A161" s="9" t="s">
         <v>207</v>
       </c>
@@ -87044,8 +87152,14 @@
       <c r="HJ161" s="3">
         <v>24</v>
       </c>
+      <c r="HK161" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL161" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="162" spans="1:218">
+    <row r="162" spans="1:220">
       <c r="A162" s="9" t="s">
         <v>209</v>
       </c>
@@ -87157,8 +87271,14 @@
       <c r="HJ162" s="3">
         <v>24</v>
       </c>
+      <c r="HK162" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL162" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="163" spans="1:218" ht="15">
+    <row r="163" spans="1:220" ht="15">
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
@@ -87172,7 +87292,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="164" spans="1:218" ht="15">
+    <row r="164" spans="1:220" ht="15">
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
@@ -87186,7 +87306,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="165" spans="1:218" ht="15">
+    <row r="165" spans="1:220" ht="15">
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
@@ -87200,7 +87320,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="166" spans="1:218" ht="15">
+    <row r="166" spans="1:220" ht="15">
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
@@ -87214,7 +87334,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:218" ht="15">
+    <row r="167" spans="1:220" ht="15">
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
@@ -87228,7 +87348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:218" ht="15">
+    <row r="168" spans="1:220" ht="15">
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
@@ -87242,7 +87362,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="169" spans="1:218" ht="15">
+    <row r="169" spans="1:220" ht="15">
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
@@ -87256,7 +87376,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:218" ht="15">
+    <row r="170" spans="1:220" ht="15">
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
@@ -87270,7 +87390,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="171" spans="1:218" ht="15">
+    <row r="171" spans="1:220" ht="15">
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
@@ -87284,7 +87404,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="172" spans="1:218" ht="15">
+    <row r="172" spans="1:220" ht="15">
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
@@ -87298,7 +87418,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:218" ht="15">
+    <row r="173" spans="1:220" ht="15">
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
@@ -87312,7 +87432,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="174" spans="1:218" ht="15">
+    <row r="174" spans="1:220" ht="15">
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
@@ -87326,7 +87446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" spans="1:218" ht="15">
+    <row r="175" spans="1:220" ht="15">
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
@@ -87340,7 +87460,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="176" spans="1:218" ht="15">
+    <row r="176" spans="1:220" ht="15">
       <c r="A176" s="9">
         <v>25386577</v>
       </c>
@@ -87599,7 +87719,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="193" spans="1:218" ht="15">
+    <row r="193" spans="1:220" ht="15">
       <c r="A193" s="9">
         <v>25394757</v>
       </c>
@@ -87621,8 +87741,14 @@
       <c r="HJ193" s="3">
         <v>5</v>
       </c>
+      <c r="HK193" s="3">
+        <v>5</v>
+      </c>
+      <c r="HL193" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="194" spans="1:218" ht="15">
+    <row r="194" spans="1:220" ht="15">
       <c r="A194" s="9">
         <v>25394035</v>
       </c>
@@ -87644,8 +87770,14 @@
       <c r="HJ194" s="3">
         <v>6</v>
       </c>
+      <c r="HK194" s="3">
+        <v>24</v>
+      </c>
+      <c r="HL194" s="3">
+        <v>24</v>
+      </c>
     </row>
-    <row r="195" spans="1:218" ht="15">
+    <row r="195" spans="1:220" ht="15">
       <c r="A195" s="9">
         <v>25273925</v>
       </c>
@@ -87660,6 +87792,9 @@
       </c>
       <c r="E195" s="9">
         <v>50</v>
+      </c>
+      <c r="F195" s="13">
+        <v>45862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-07-25 09:49:30
</commit_message>
<xml_diff>
--- a/data/Chamber_Tests.xlsx
+++ b/data/Chamber_Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2341" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C06C05-3EAC-4ECE-B103-05800575FA96}"/>
+  <xr:revisionPtr revIDLastSave="2387" documentId="8_{A53666C7-9120-4C83-A847-C4965BAD787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC08EC58-6344-4719-B553-72029034778A}"/>
   <bookViews>
     <workbookView xWindow="-10" yWindow="-10" windowWidth="19220" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="252">
   <si>
     <t>Module ID</t>
   </si>
@@ -671,10 +671,82 @@
     <t>EPE+EPE HIB TAPE</t>
   </si>
   <si>
+    <t>VSL202526156</t>
+  </si>
+  <si>
+    <t>Sunsure HYPERSOL Internal Reliability Tests : Lot 2</t>
+  </si>
+  <si>
+    <t>VSL202526157</t>
+  </si>
+  <si>
+    <t>VSL202526158</t>
+  </si>
+  <si>
+    <t>VSL202526161</t>
+  </si>
+  <si>
+    <t>VSL202526163</t>
+  </si>
+  <si>
+    <t>VSL202526164</t>
+  </si>
+  <si>
+    <t>VSL202526166</t>
+  </si>
+  <si>
+    <t>VSL202526167</t>
+  </si>
+  <si>
+    <t>VSL202526169</t>
+  </si>
+  <si>
+    <t>VSL202526170</t>
+  </si>
+  <si>
     <t>LeTID</t>
   </si>
   <si>
-    <t>Sunsure HYPERSOL Internal Reliability Tests (DH1000+SML)</t>
+    <t>VSL202526171</t>
+  </si>
+  <si>
+    <t>VSL202526173</t>
+  </si>
+  <si>
+    <t>VSL202526175</t>
+  </si>
+  <si>
+    <t>Sunsure HYPERSOL Internal Reliability Tests (DH1000+SML) : Lot 2</t>
+  </si>
+  <si>
+    <t>VSL202526176</t>
+  </si>
+  <si>
+    <t>VSL202526178</t>
+  </si>
+  <si>
+    <t>VSL202526179</t>
+  </si>
+  <si>
+    <t>VSL202526180</t>
+  </si>
+  <si>
+    <t>VSL202526181</t>
+  </si>
+  <si>
+    <t>VSL202526182</t>
+  </si>
+  <si>
+    <t>VSL202526186</t>
+  </si>
+  <si>
+    <t>VSL202526189</t>
+  </si>
+  <si>
+    <t>VSL202526190</t>
+  </si>
+  <si>
+    <t>VSL202526192</t>
   </si>
   <si>
     <t>VSL202425229</t>
@@ -1257,8 +1329,8 @@
   <dimension ref="A1:XFD195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="16" ySplit="1" topLeftCell="HJ189" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F195" sqref="F195"/>
+      <pane xSplit="16" ySplit="1" topLeftCell="HJ90" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="HN99" sqref="HN99"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -82889,7 +82961,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="97" spans="1:220" ht="15">
+    <row r="97" spans="1:222" ht="15">
       <c r="A97" s="15">
         <v>25089365</v>
       </c>
@@ -82930,7 +83002,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:220" ht="15">
+    <row r="98" spans="1:222" ht="15">
       <c r="A98" s="15">
         <v>25089363</v>
       </c>
@@ -82949,6 +83021,9 @@
       <c r="F98" s="18">
         <v>45820</v>
       </c>
+      <c r="P98" s="13">
+        <v>45862</v>
+      </c>
       <c r="FW98" s="3">
         <v>7</v>
       </c>
@@ -83075,8 +83150,14 @@
       <c r="HL98" s="3">
         <v>24</v>
       </c>
+      <c r="HM98" s="3">
+        <v>16</v>
+      </c>
+      <c r="HN98" s="3" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="99" spans="1:220" ht="15">
+    <row r="99" spans="1:222" ht="15">
       <c r="A99" s="15">
         <v>25089370</v>
       </c>
@@ -83095,6 +83176,9 @@
       <c r="F99" s="18">
         <v>45820</v>
       </c>
+      <c r="P99" s="13">
+        <v>45862</v>
+      </c>
       <c r="FW99" s="3">
         <v>7</v>
       </c>
@@ -83221,8 +83305,11 @@
       <c r="HL99" s="3">
         <v>24</v>
       </c>
+      <c r="HM99" s="3">
+        <v>16</v>
+      </c>
     </row>
-    <row r="100" spans="1:220" ht="15">
+    <row r="100" spans="1:222" ht="15">
       <c r="A100" s="15">
         <v>25112301</v>
       </c>
@@ -83263,7 +83350,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:220" ht="15">
+    <row r="101" spans="1:222" ht="15">
       <c r="A101" s="9">
         <v>72309509</v>
       </c>
@@ -83307,7 +83394,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:220" ht="15">
+    <row r="102" spans="1:222" ht="15">
       <c r="A102" s="9">
         <v>72304210</v>
       </c>
@@ -83351,7 +83438,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="103" spans="1:220" ht="15">
+    <row r="103" spans="1:222" ht="15">
       <c r="A103" s="9">
         <v>25263837</v>
       </c>
@@ -83395,7 +83482,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:220" ht="15">
+    <row r="104" spans="1:222" ht="15">
       <c r="A104" s="9">
         <v>25264958</v>
       </c>
@@ -83439,7 +83526,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:220" ht="15">
+    <row r="105" spans="1:222" ht="15">
       <c r="A105" s="9">
         <v>25273922</v>
       </c>
@@ -83498,7 +83585,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="106" spans="1:220" ht="15">
+    <row r="106" spans="1:222" ht="15">
       <c r="A106" s="9">
         <v>25273923</v>
       </c>
@@ -83539,7 +83626,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="107" spans="1:220" ht="15">
+    <row r="107" spans="1:222" ht="15">
       <c r="A107" s="9">
         <v>25273924</v>
       </c>
@@ -83685,7 +83772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:220" ht="15">
+    <row r="108" spans="1:222" ht="15">
       <c r="A108" s="9">
         <v>25273925</v>
       </c>
@@ -83747,7 +83834,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:220" ht="15">
+    <row r="109" spans="1:222" ht="15">
       <c r="A109" s="9">
         <v>25273926</v>
       </c>
@@ -83767,7 +83854,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" spans="1:220" ht="15">
+    <row r="110" spans="1:222" ht="15">
       <c r="A110" s="9">
         <v>25119247</v>
       </c>
@@ -83838,7 +83925,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="111" spans="1:220" ht="15">
+    <row r="111" spans="1:222" ht="15">
       <c r="A111" s="9">
         <v>25121350</v>
       </c>
@@ -83885,7 +83972,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="112" spans="1:220" ht="15">
+    <row r="112" spans="1:222" ht="15">
       <c r="A112" s="9">
         <v>25121029</v>
       </c>
@@ -87282,8 +87369,11 @@
       <c r="A163" s="9">
         <v>25386587</v>
       </c>
+      <c r="B163" s="9" t="s">
+        <v>211</v>
+      </c>
       <c r="C163" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D163" s="9" t="s">
         <v>18</v>
@@ -87296,8 +87386,11 @@
       <c r="A164" s="9">
         <v>25386594</v>
       </c>
+      <c r="B164" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="C164" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D164" s="9" t="s">
         <v>18</v>
@@ -87310,8 +87403,11 @@
       <c r="A165" s="9">
         <v>25386583</v>
       </c>
+      <c r="B165" s="9" t="s">
+        <v>214</v>
+      </c>
       <c r="C165" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D165" s="9" t="s">
         <v>28</v>
@@ -87324,8 +87420,11 @@
       <c r="A166" s="9">
         <v>25386578</v>
       </c>
+      <c r="B166" s="9" t="s">
+        <v>215</v>
+      </c>
       <c r="C166" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D166" s="9" t="s">
         <v>18</v>
@@ -87338,8 +87437,11 @@
       <c r="A167" s="9">
         <v>25386240</v>
       </c>
+      <c r="B167" s="9" t="s">
+        <v>216</v>
+      </c>
       <c r="C167" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D167" s="9" t="s">
         <v>32</v>
@@ -87352,8 +87454,11 @@
       <c r="A168" s="9">
         <v>25385829</v>
       </c>
+      <c r="B168" s="9" t="s">
+        <v>217</v>
+      </c>
       <c r="C168" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D168" s="9" t="s">
         <v>18</v>
@@ -87366,8 +87471,11 @@
       <c r="A169" s="9">
         <v>25386238</v>
       </c>
+      <c r="B169" s="9" t="s">
+        <v>218</v>
+      </c>
       <c r="C169" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D169" s="9" t="s">
         <v>18</v>
@@ -87380,8 +87488,11 @@
       <c r="A170" s="9">
         <v>25386229</v>
       </c>
+      <c r="B170" s="9" t="s">
+        <v>219</v>
+      </c>
       <c r="C170" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D170" s="9" t="s">
         <v>18</v>
@@ -87394,8 +87505,11 @@
       <c r="A171" s="9">
         <v>25385835</v>
       </c>
+      <c r="B171" s="9" t="s">
+        <v>220</v>
+      </c>
       <c r="C171" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D171" s="9" t="s">
         <v>18</v>
@@ -87408,11 +87522,14 @@
       <c r="A172" s="9">
         <v>25386639</v>
       </c>
+      <c r="B172" s="9" t="s">
+        <v>221</v>
+      </c>
       <c r="C172" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D172" s="9" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="E172" s="9">
         <v>192</v>
@@ -87422,11 +87539,14 @@
       <c r="A173" s="9">
         <v>25386618</v>
       </c>
+      <c r="B173" s="9" t="s">
+        <v>223</v>
+      </c>
       <c r="C173" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="E173" s="9">
         <v>192</v>
@@ -87436,8 +87556,11 @@
       <c r="A174" s="9">
         <v>25386256</v>
       </c>
+      <c r="B174" s="9" t="s">
+        <v>224</v>
+      </c>
       <c r="C174" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D174" s="9" t="s">
         <v>32</v>
@@ -87450,8 +87573,11 @@
       <c r="A175" s="9">
         <v>25385821</v>
       </c>
+      <c r="B175" s="9" t="s">
+        <v>225</v>
+      </c>
       <c r="C175" s="17" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="D175" s="9" t="s">
         <v>28</v>
@@ -87464,8 +87590,11 @@
       <c r="A176" s="9">
         <v>25386577</v>
       </c>
+      <c r="B176" s="9" t="s">
+        <v>227</v>
+      </c>
       <c r="C176" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D176" s="9" t="s">
         <v>32</v>
@@ -87478,8 +87607,11 @@
       <c r="A177" s="9">
         <v>25386584</v>
       </c>
+      <c r="B177" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="C177" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D177" s="9" t="s">
         <v>32</v>
@@ -87492,8 +87624,11 @@
       <c r="A178" s="9">
         <v>25386617</v>
       </c>
+      <c r="B178" s="9" t="s">
+        <v>229</v>
+      </c>
       <c r="C178" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D178" s="9" t="s">
         <v>25</v>
@@ -87506,8 +87641,11 @@
       <c r="A179" s="9">
         <v>25386605</v>
       </c>
+      <c r="B179" s="9" t="s">
+        <v>230</v>
+      </c>
       <c r="C179" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D179" s="9" t="s">
         <v>21</v>
@@ -87520,8 +87658,11 @@
       <c r="A180" s="9">
         <v>25438399</v>
       </c>
+      <c r="B180" s="9" t="s">
+        <v>231</v>
+      </c>
       <c r="C180" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D180" s="9" t="s">
         <v>18</v>
@@ -87534,8 +87675,11 @@
       <c r="A181" s="9">
         <v>25438419</v>
       </c>
+      <c r="B181" s="9" t="s">
+        <v>232</v>
+      </c>
       <c r="C181" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D181" s="9" t="s">
         <v>32</v>
@@ -87548,8 +87692,11 @@
       <c r="A182" s="9">
         <v>25445298</v>
       </c>
+      <c r="B182" s="9" t="s">
+        <v>233</v>
+      </c>
       <c r="C182" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>18</v>
@@ -87562,8 +87709,11 @@
       <c r="A183" s="9">
         <v>25438056</v>
       </c>
+      <c r="B183" s="9" t="s">
+        <v>234</v>
+      </c>
       <c r="C183" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>18</v>
@@ -87576,8 +87726,11 @@
       <c r="A184" s="9">
         <v>25438634</v>
       </c>
+      <c r="B184" s="9" t="s">
+        <v>235</v>
+      </c>
       <c r="C184" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>32</v>
@@ -87590,8 +87743,11 @@
       <c r="A185" s="9">
         <v>25442344</v>
       </c>
+      <c r="B185" s="9" t="s">
+        <v>236</v>
+      </c>
       <c r="C185" s="17" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>18</v>
@@ -87605,10 +87761,10 @@
         <v>23881328</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C186" s="17" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="D186" s="9" t="s">
         <v>28</v>
@@ -87622,10 +87778,10 @@
         <v>24206642</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="C187" s="17" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>28</v>
@@ -87639,10 +87795,10 @@
         <v>25518469</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="C188" s="17" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="D188" s="9" t="s">
         <v>28</v>
@@ -87656,10 +87812,10 @@
         <v>25523456</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="C189" s="17" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>18</v>
@@ -87673,10 +87829,10 @@
         <v>25522727</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="C190" s="17" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>18</v>
@@ -87690,10 +87846,10 @@
         <v>25507484</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="C191" s="17" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>18</v>
@@ -87707,10 +87863,10 @@
         <v>25517884</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="C192" s="17" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>18</v>
@@ -87724,10 +87880,10 @@
         <v>25394757</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="C193" s="17" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="D193" s="9" t="s">
         <v>32</v>
@@ -87753,10 +87909,10 @@
         <v>25394035</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="C194" s="17" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>18</v>
@@ -87785,7 +87941,7 @@
         <v>146</v>
       </c>
       <c r="C195" s="17" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>21</v>

</xml_diff>